<commit_message>
Enhance KPI alerting and reporting functionality
- Updated .gitignore to exclude PNG files and the new JSON alert card.
- Modified 'calculated_KPIs_alerts.csv' to include an image column for critical alerts.
- Enhanced 'calculated_KPIs.ipynb' to adjust execution counts and improve output handling.
- Updated 'calculated_kpis.py' to generate and upload critical alerts, including a new adaptive card JSON for total TBS alerts.
- Added functionality to save critical alerts in both CSV and Excel formats, improving reporting capabilities.
</commit_message>
<xml_diff>
--- a/calculated_KPIs_alerts.xlsx
+++ b/calculated_KPIs_alerts.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +488,11 @@
           <t>forecast_upper</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -502,25 +507,30 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45638.66666666666</v>
+        <v>45639.5</v>
       </c>
       <c r="E2" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F2" t="n">
-        <v>47.90467600254193</v>
+        <v>38.64986855885751</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45638.66666666666</v>
+        <v>45639.5</v>
       </c>
       <c r="H2" t="n">
-        <v>32.30944750382193</v>
+        <v>22.62707112525826</v>
       </c>
       <c r="I2" t="n">
-        <v>14.86865374401928</v>
+        <v>7.137494636139678</v>
       </c>
       <c r="J2" t="n">
-        <v>47.90467600254193</v>
+        <v>38.64986855885751</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACWB0lEQVR4nOzdeXxU9fX/8fedmWyQzYREtqDsq4CyFVwAUUBErCyCFgVKf+5b1WpdWkUrqLhV/WrdvuCCXwXUKnVhEyxVEGMji0CxsgiELYRMEsg2M/f3R5xJJplJJiSZucHX8/Hoo+bMnXvPmXs/994cPnNjmKZpCgAAAAAAALAoW6QTAAAAAAAAAGpCAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwCAMDIMo87/GzZsWKTT9jn99NNlGIZ27doV6VTqxfvZonHt2rVLhmHo9NNPj3QqAACgiXNEOgEAAH5Jpk2bVi124MABLV26NOjr3bp1q9M2Vq9ereHDh2vo0KFavXr1CeXZlA0bNkxffPGFVq1aZanmXyDeJpppmo2+rQcffFCzZs3SAw88oAcffLDRtwcAANCQaGABABBG8+fPrxZbvXq1r4EV6HU0vK1bt0Y6BQAAANQBDSwAAPCLU9dZbQAAAIgsnoEFAIDF7d27VzfffLM6d+6s2NhYJSUl6eyzz9ZLL70kt9vtt+ywYcM0fPhwSdIXX3zh9yytys8hOnz4sJ599lmNGTNG7du3V1xcnBITE9W/f3899thjKi4ubrD8p0+fLsMwNH/+fG3YsEHjx49XWlqa4uLi1Lt3b/31r3+tVockFRQU6JVXXtH48ePVuXNnNW/eXM2bN9cZZ5yh++67T3l5eX7Lr169WoZh6IsvvpAkDR8+3K/+yrPbanoGlsvl0quvvqphw4YpJSVFMTExat++va6//nrt2bOn2vLe7Q4bNkxlZWV67LHH1LNnT8XFxSk1NVXjx4+vNuPrwQcf9Nt+1eeeVX7G2KJFi3TBBRcoNTVVUVFRSk1NVY8ePfT//t//08aNG2v7+H3rnzVrliRp1qxZftuaPn2637K5ubm699571bNnTzVr1kwJCQnq16+fHn/8cRUVFYW0vUBcLpcef/xx32fTokULXX755dq2bVvQ9xQVFenJJ5/Ur371KyUnJys2NlZdu3bVXXfdpSNHjtQ5hxUrVuiSSy7RqaeeqqioKJ1yyinq3Lmzpk6dqn/+858B37Ny5UqNHz9erVq1UnR0tNLT03XZZZdp7dq1DZb3/Pnzffvi2LFjuueee9SpUyfFxMSoZcuWmjZtmvbt21fnegEAOJkwAwsAAAv75ptvNHr0aOXm5qpdu3b69a9/LafTqdWrV+urr77SBx98oI8++kjR0dGSpNGjRys2NlZLly7VqaeeqtGjR/vW1aJFC99/L126VLfeeqvatGmjTp066Ve/+pUOHz6sr7/+Wn/84x/14YcfatWqVYqJiWmwWtavX6/rr79eLVu21IgRI3T06FGtXr1at912m/71r39p4cKFfk2dDRs26JprrlFaWpq6du2qfv366ejRo/r22281e/ZsLVy4UOvWrVNqaqok+X7R/+yzz3Tw4EGNGjVKLVu29K2vU6dOteZYUFCgcePGafXq1YqPj1e/fv2UlpamTZs26W9/+5sWLVqk5cuX68wzz6z23rKyMo0ZM0ZfffWVzjvvPHXv3l3r16/XBx98oFWrVikrK8vXROzbt6+mTZum119/XVL1Z5/Fx8dLkh566CE98MADcjgcGjJkiNq0aSOn06mffvpJr732mnr27KnevXvXWte0adP03XffacOGDerTp4/69u3re+2cc87x/feOHTt0/vnna/fu3UpLS9OYMWNUVlamVatW6e6779a7776rFStW6JRTTql1m1VNnjxZS5Ys0dChQ9W7d2+tX79eixYt0qeffqply5Zp8ODBfstnZ2dr9OjR2rRpk1JSUjRgwAAlJCTo3//+t+bOnatFixZp9erVOu2000La/uuvv64ZM2ZIkgYOHKjhw4erqKhIe/fu1TvvvKMWLVrovPPO83vPnXfeqSeffFI2m039+/fXueeeq59++kkffvihlixZoldeecW3zobI2+l0asiQIfrpp5907rnnqlevXlq7dq3eeOMNffHFF9qwYYOSkpLq8rEDAHDyMAEAQEStWrXKlGRWvSwXFxebp512minJvO6668zS0lLfaz/++KN5+umnm5LMe++9N+D6hg4dGnSbW7ZsMdeuXVstnpuba44cOdKUZD7++OPVXvfms3PnzpDrmzZtmq++G264wSwrK/O9tnnzZjMtLc2UZP7tb3/ze9+ePXvMFStWmG632y9+7Ngx8+qrr/atr6qhQ4eaksxVq1YFzSnQ522apnnllVeaksyxY8eaBw8e9Hvt6aefNiWZnTt3Nl0uly9eef+deeaZ5v79+32vFRUVmaNGjTIlmddcc03IeZhm+f6Pi4sz4+PjzW3btlV7fdeuXebWrVuD1ljVAw88YEoyH3jggaDLDBo0yJRkjhs3ziwsLPTFDx06ZJ511lmmJPPKK68MeZs7d+701diiRQtzw4YNvtdcLpd58803m5LM0047zSwuLva95vF4zLPPPtuUZM6cOdPMz8/3vVZWVmbecccdpiRz+PDhIefSvn17U5K5Zs2aaq8dPHjQ/Pe//+0Xe/nll01JZqdOnfzyNk3T/OKLL8yEhAQzOjra3L59e73znjdvnu9zGjVqlOl0On2v5ebmmn379jUlmbNnzw65XgAATjY0sAAAiLBgDaw333zTlGS2bt3a75d7r8WLF5uSzISEBLOoqKja+mpqYNXkP//5jynJHDBgQLXX6tPAatWqlV+eXs8995yvMRSqY8eOmQ6Hw0xLS6v22ok2sLZs2WIahmG2bt3ar/FQ2ZgxY0xJ5pIlS3wx7+dtGIb53XffVXvPunXrTElmhw4dQsrD69ChQ6Yks3fv3kHrqIvaGlhr1qwxJZnNmjUzDxw4UO31zMxMU5Jps9nMPXv2hLTNyg2sZ555ptrrxcXFZps2bUxJ5oIFC3zxTz/91JRk9u3b16/h6eV2u81evXqZksxNmzaFlEuzZs3MpKSkkJZ1u91m69atTUlmZmZmwGUef/xxU5J5xx131DtvbwOrefPmZnZ2drX3vfPOO6Yk8/zzzw8pfwAATkY8AwsAAItavXq1JGnKlCkBv8o3fvx4nXLKKSooKNC3335b5/W73W6tXLlSDz/8sG644QbNmDFD06dP1yOPPCJJ+s9//lOv/Ku6/PLLFRsbWy3u/frcDz/8oOzs7Gqvf/XVV3rsscd04403+nK84YYbFB0drcOHD+vo0aMNkt8nn3wi0zR10UUXKSEhIeAyw4YN8+VUVbt27dSnT59q8e7du0tSnZ9hlJaWptNPP10bN27UHXfcoS1bttTp/XXlPd5Gjx6tU089tdrr/fr1U58+feTxeHzPGauLql+TlKSYmBhNnjzZb/uS9PHHH0uSJkyYIIej+hMvbDab7+t+gfZFIAMHDpTT6dTVV1+tb7/9Vh6PJ+iyWVlZys7OVseOHdWvX7+AywQ6Fuqbd//+/dWqVatq8RM9hgAAOJnwDCwAACzK+8tq+/btA75uGIbat2+vo0eP1vkX2x9++EGXXXaZvv/++6DL5Ofn12mdtQlWR0JCglJTU3XkyBHt3btXrVu3liQdOnRIEyZM0L/+9a8a15ufn39Cz2SqaseOHZKk1157Ta+99lqNyx4+fLharF27dgGXTUxMlCSVlJTUOac33nhDEydO1FNPPaWnnnpKKSkpGjRokC688EJdddVVfs81q6/ajjdJ6tixozZs2FDn4y05OVnJyckBX/Nub+/evb6Yd1/86U9/0p/+9Kca1x1oXwTywgsvaOzYsXrzzTf15ptvKiEhQQMGDND555+vq666ym//ebf/448/Bn3Yf6Dt1zfv2o6hhvzjCgAANDU0sAAA+AWaOHGivv/+e40dO1Z33XWXevToocTEREVFRam0tLRBH95eF6Zp+v77d7/7nf71r39p8ODBmjVrlvr06aNTTjlFUVFRkqTWrVtr//79fu+pD++MnL59+wacSVXZoEGDqsVstoaf2H7uuedq165d+vjjj/XFF1/oq6++0tKlS/Xpp5/qgQce0AcffKARI0Y0+HYjofJ+9O6Lc845Rx07dqzxfT179gxp/d27d9d//vMfLVu2TJ9//rm++uorrVmzRp9//rkeeughvfbaa5o6darf9lu2bKlRo0bVuN7KTcT65t0YxxAAACcLGlgAAFhUmzZtJFXM6ghk586dfsuGYtu2bdq4caPS09P1wQcfVPuq0w8//HAC2dbOm2tVBQUFOnLkiCSpbdu2kqRjx47pk08+kc1m0yeffFJt9s6xY8d04MCBBs0vIyNDknT22Wfr+eefb9B110dcXJwmTpyoiRMnSiqfuXP//ffr5Zdf1m9/+1vt3r27QbYTyvHmfa0ux5sk5eXlKS8vL+AsrF27dkmq2PdSxb649NJLdeedd9ZpWzVxOBwaM2aMxowZI6l89t5TTz2lWbNm6dprr9Vll12m5s2b+7afmpqq+fPnh7z+xsobAABI/DMPAAAW5X3Gzrvvvhvwq0MffPCBjh49qoSEBL/n9ERHR0uSXC5XwPXm5uZKKp/BFOg5PW+99VZ9Uw9o0aJFAb9G9+abb0qSOnXq5GuMOJ1Oud1uJSYmBmx6vPXWW0FnXtVWfzAXXXSRJOmjjz4K21e1vLPJ6pJrWlqaHn/8cUnSTz/9FPIzwGr7XLzH22effaaDBw9Wez0rK0vfffed33Oc6sK7nysrLS3Vu+++67d9qWJfLFq0qMFm2AWSmJioBx98UMnJyTp+/Li2b98uSRowYIBatGihLVu21Pg126rClTcAAL9ENLAAALCoSZMmqV27dsrOztbtt9/u13jYuXOn7rjjDknSzTff7PdwdO9Mlh9++EFlZWXV1tulSxfZ7XZt2rTJ78HZkrRkyRI9/fTTjVCNlJ2drTvvvFNut9sX27p1qx566CFJ0u9//3tf/NRTT9Upp5yivLy8ao2PdevW6Z577gm6HW/9dWk8SNKZZ56pCRMmaM+ePRo/frxvZlBlx44d04IFCwI2eE5ETbnu3r1br776asBnkS1ZskSSdMopp/iej1SfbUnlX3sbNGiQioqKdO211+r48eO+13JycnTttddKKv+jAt6ZRnXx8MMPa/Pmzb6fPR6P7r77bu3du1cZGRmaMGGC77VLL71UAwYM0Pr16zVjxoyAz4s6evSo/va3v4XU/Dt+/LieeuqpgOtZs2aN8vLyZLfbfZ9RVFSUHnjgAZmmqcsuuyzgc9jcbrc+//xzrVu3rtHyBgAAlUTuDyACAADTNM1Vq1aZksxAl+X169ebKSkppiTztNNOMydPnmyOGTPGjI2NNSWZo0aNMktKSqq9r3///qYks2vXruZvfvMbc+bMmebdd9/te/3WW281JZk2m80cOnSoecUVV5hnnXWWKcm8//77g+Zz2mmnmZLMnTt3hlzftGnTTEnmddddZ8bGxprt27c3p0yZYo4aNcqMjo42JZmXXXaZ6fF4/N739NNP+/IYNGiQecUVV5hnn322aRiGedVVVwXN5R//+IcpyYyOjjbHjh1r/va3vzVnzpxpfvnll75lgtWXn59vjhgxwvf+AQMGmJdffrk5adIkc8CAAb58t27d6nuPd/8NHTo06GcQbHt33nmnKcls0aKFefnll5szZ840Z86caebk5JhZWVmmJDMqKsqXx+WXX26eeeaZpiTTMAzz1VdfDXEvmOaBAwfM5s2bm5LMs88+25w+fbo5c+ZM83//9399y/z444++zzU9Pd2cOHGieemll5qJiYmmJPOss84yc3NzQ97mzp07TUlmu3btzMsuu8yMiooyL7zwQnPKlClmx44dTUlm8+bNzTVr1lR77759+8y+ffv6lhkyZIg5ZcoUc/z48Wbfvn1Nu91uSjKLiopqzePo0aO+471Pnz7mxIkTzSuuuMIcPHiwaRiGKcn885//XO19f/jDH3z7rmfPnuall15qTpkyxRw2bJiZnJxsSjJffPHFeuc9b948U5I5bdq0Gj/H0047rdZaAQA4WdHAAgAgwmpqYJmmaf7000/mjTfeaHbo0MGMjo42ExISzMGDB5svvviiWVZWFvA9u3fvNq+88kqzVatWpsPhqPbLr8fjMV977TWzX79+Znx8vJmUlGSec8455jvvvGOaZvCGS30aWPPmzTP//e9/m5dccomZmppqxsTEmD179jSfeuqpoHX8/e9/N4cMGWImJyeb8fHxZv/+/c0XXnjB9Hg8NebyyiuvmGeddZbZrFkzXy3z5s3zvV7T5+12u823337bHDNmjHnqqaeaUVFRZmpqqtmrVy9zxowZ5gcffGCWlpb6lq9PA6uoqMi86667zE6dOvmaY96a8vPzzWeeeca87LLLzM6dO5vx8fFm8+bNzS5duphXX321mZmZGXR7wfzzn/80L7jgAvOUU04xbTZbwKbJkSNHzHvuucfs3r27GRsbazZr1sw888wzzUcffdQ8fvx4nbZXufFSVlZmPvLII2a3bt3MmJgYMyUlxZwwYYL5/fffB31/cXGx+be//c0cPny4mZqaajocDjM9Pd3s27eveeONN5pLly4NKY+ysjLzb3/7m3nFFVeY3bp1M5OSksy4uDizY8eO5oQJE8yVK1cGfe+XX35p/uY3vzFPO+00MyYmxkxISDC7dOli/vrXvzZfffXVgA29uuZNAwsAgNoZpskX9AEAQOOZPn26Xn/9dc2bN0/Tp0+PdDoAAABogngGFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI1nYAEAAAAAAMDSmIEFAAAAAAAAS6OBBQAAAAAAAEtz1HcF33//vR588EF9++23OnDggJo1a6YePXroD3/4gy655BLfct4/oV1V165dtW3btjpt0+PxKDs7WwkJCTIMo74lAAAAAAAAoBGZpqmCggK1bt1aNlvd51PVu4G1e/duFRQUaNq0aWrdurWOHz+u9957T+PGjdNLL72ka665xrdsTEyMXn31Vb/3JyUl1Xmb2dnZysjIqG/qAAAAAAAACKM9e/aobdu2dX5fozzE3e12q1+/fiouLvbNrpo+fboWL16swsLCeq/f6XQqOTlZe/bsUWJiYr3XBwAAAAAAgMaTn5+vjIwM5eXlndBkpnrPwArEbrcrIyND33zzTbXX3G63jh07Vq/Gk/drg4mJiTSwAAAAAAAAmogTfRRUgz3E/dixY8rJydGPP/6op59+Wp9++qlGjBjht8zx48eVmJiopKQkpaSk6MYbb2yQGVkAAAAAAAA4eTXYDKw77rhDL730kiTJZrNp/Pjxev75532vt2rVSnfddZfOOusseTweffbZZ3rhhRe0YcMGrV69Wg5H8FRKSkpUUlLi+zk/P1+S5HK55HK5fNu02WzyeDzyeDy+Zb1xt9utyt+WDBa32+0yDMO33spxqXwGWShxh8Mh0zT94oZhyG63V8sxWJyaqImaqImaqImaqImaqImaqImaqImaqOlkqKlqXXXVYA2s2267TRMnTlR2drYWLlwot9ut0tJS3+tz5szxW37KlCnq0qWL7rvvPi1evFhTpkwJuu45c+Zo1qxZ1eJZWVlq3ry5JCktLU0dO3bUzp07dfjwYd8ybdu2Vdu2bbV9+3Y5nU5fvEOHDkpPT9fmzZtVVFTki3fr1k3JycnKysry29m9e/dWdHS0MjMz/XLo37+/SktLtXHjRl/MbrdrwIABcjqdfn9hMS4uTn369FFOTo527NjhiyclJal79+7Kzs7W3r17fXFqoiZqoiZqoiZqoiZqoiZqoiZqoiZqoqaToSbvZKQT1SgPcZekkSNHKi8vT19//XXQ7zcWFRUpPj5eM2bMqPbXCSsLNAMrIyNDR44c8T0Di44nNVETNVETNVETNVETNVETNVETNVETNVGTNWvKz89XamqqnE7nCT3PvNEaWC+//LKuvfZabdu2TV27dg26XHp6us455xy9//77Ia87Pz9fSUlJJ1w0AAAAAAAAwqe+vZxG+SuEknxTxipPKauqoKBAOTk5SktLa6w0AAAAAABAA/HO7Knv84xw8nA4HL6ZVo26nfqu4NChQ0pPT/eLlZWV6Y033lBcXJx69Oih4uJilZWVKSEhwW+5hx9+WKZpavTo0fVNAwAAAAAANBLTNJWXl6fDhw9X+8oaYLfblZ6erqSkpEZrZNW7gXXttdcqPz9f5513ntq0aaMDBw5owYIF2rZtm5588knFx8dr165dOvPMM3XFFVeoW7dukqSlS5fqk08+0ejRo3XppZfWuxAAAAAAANA4Dhw4oLy8PCUmJioxMVEOh6PRZ9zA+kzT9D3fav/+/SoqKlKrVq0aZVv1bmBNnjxZr732ml588UUdOXJECQkJ6tevnx577DGNGzdOkpScnKyxY8dq+fLlev311+V2u9WpUyfNnj1bd955p2w2W70LAQAAAAAADc/tdsvpdCotLU0tWrSIdDqwoISEBMXExCgnJ0fp6em+B8w3pEZ7iHtj4iHuAAAAAACER3FxsXbu3KnTTz9dcXFxkU4HFlVUVKRdu3apffv2io2NrfZ6fXs5TH0CAAAAAAC14iuDqEljHx80sAAAAAAAAGBpNLAAAAAAAAAQ0PTp03X66adHOg0aWAAAAAAA4Jdr/vz5Mgwj6P/WrVsX6RRrtWXLFj344IPatWtXpFNpNPX+K4QAAAAAAABN3UMPPaT27dtXi3fq1CkC2dTNli1bNGvWLA0bNswSs6UaAw0sAAAAAABwwpZtjnQG0she9V/HRRddpP79+9d/RWgUfIUQAAAAAACgBg888IBsNptWrlzpF7/mmmsUHR2tDRs2SJJWr14twzD07rvv6t5771XLli3VvHlzjRs3Tnv27Km23q+//lqjR49WUlKSmjVrpqFDh+rLL7+stty+ffs0c+ZMtW7dWjExMWrfvr2uv/56lZaWav78+Zo0aZIkafjw4b6vPq5evdr3/k8//VTnnnuumjdvroSEBF188cX6/vvvq23n73//u3r16qXY2Fj16tVLH3zwQX0+tgbFDCwAAAAAAPCL53Q6lZOT4xczDEOpqam6//77tWTJEs2cOVObNm1SQkKCli5dqldeeUUPP/yw+vTp4/e+Rx55RIZh6O6779ahQ4f0zDPP6IILLtB3332nuLg4SdLnn3+uiy66SP369fM1yObNm6fzzz9fa9as0cCBAyVJ2dnZGjhwoPLy8nTNNdeoW7du2rdvnxYvXqzjx4/rvPPO0y233KJnn31W9957r7p37y5Jvv9/8803NW3aNI0aNUqPPfaYjh8/rhdffFHnnHOOsrKyfF85XLZsmSZMmKAePXpozpw5OnLkiGbMmKG2bds25sceMsM0TTPSSdRVfn6+kpKS5HQ6lZiYGOl0AAAAAAA4aRUXF2vnzp1q3769YmNjq73e1L9COH/+fM2YMSPgazExMSouLpYkbd68Wf369dPVV1+tuXPnqlevXmrVqpXWrl0rh6N8ftDq1as1fPhwtWnTRlu3blVCQoIkadGiRbr88sv117/+VbfccotM01TXrl3VoUMHffrppzIMQ5JUVFSknj17qlOnTlq2bJkkadq0aXrrrbf09ddfV/uKo2maMgxDixcv1qRJk7Rq1SoNGzbM93phYaEyMjI0adIkvfzyy774wYMH1bVrV11++eW++JlnnqmDBw9q69atSkpKkiQtX75cI0eO1GmnnVbrA+JrO07q28thBhYAAAAAAPjF+5//+R916dLFL2a3233/3atXL82aNUv33HOPNm7cqJycHC1btszXvKrs6quv9jWvJGnixIlq1aqVPvnkE91yyy367rvv9MMPP+j+++/XkSNH/N47YsQIvfnmm/J4PJLKv9Z3ySWXBHw+l7fxFczy5cuVl5enK664wm92md1u16BBg7Rq1SpJ0v79+/Xdd9/pj3/8o695JUkXXnihevTooWPHjtW4nXCggQUAAAAAAH7xBg4cWOtD3P/whz/onXfe0fr16zV79mz16NEj4HKdO3f2+9kwDHXq1Mk3i+mHH36QVD67Khin06nS0lLl5+erV68Tm2Lm3c75558f8HXvTKjdu3cHzFuSunbtqn//+98ntP2GRAMLAAAAQIOzwleKvBrir5MBgCTt2LHD1xTatGnTCa/HO7tq7ty56tu3b8Bl4uPjlZube8LbqLydN998Uy1btqz2eqDZY1bVdDIFAAAAfsFoCAFAZHk8Hk2fPl2JiYm67bbbNHv2bE2cOFHjx4+vtqy3yeVlmqb++9//qnfv3pKkjh07SiqfAXXBBRcE3WZaWpoSExO1eXPNF4FgXyX0bic9Pb3G7Zx22mkB85ak//znPzVuO1xskU4AAAAAAADA6p566il99dVXevnll/Xwww9ryJAhuv7666v95UJJeuONN1RQUOD7efHixdq/f78uuugiSVK/fv3UsWNHPfHEEyosLKz2/sOHD0uSbDabfv3rX2vJkiXKzMystpz37/I1b95ckpSXl+f3+qhRo5SYmKjZs2errKws6HZatWqlvn376vXXX5fT6fS9vnz5cm3ZsqXGzyVcmIEFAAAAAAB+8T799FNt27atWnzIkCEqKSnRn/70J02fPl2XXHKJpPK/Xti3b1/dcMMNWrhwod97UlJSdM4552jGjBk6ePCgnnnmGXXq1En/7//9P0nljalXX31VF110kXr27KkZM2aoTZs22rdvn1atWqXExEQtWbJEkjR79mwtW7ZMQ4cO1TXXXKPu3btr//79WrRokf71r38pOTlZffv2ld1u12OPPSan06mYmBidf/75Sk9P14svvqirrrpKZ511lqZMmaK0tDT99NNP+vjjj3X22Wfr+eeflyTNmTNHF198sc455xz99re/VW5urp577jn17NkzYJMt3GhgAQAAAACAX7w///nPAeOvvvqqXnrpJbVo0ULPPPOML965c2fNmTNHt956qxYuXKjLL7/c99q9996rjRs3as6cOSooKNCIESP0wgsvqFmzZr5lhg0bprVr1+rhhx/W888/r8LCQrVs2VKDBg3Stdde61uuTZs2+vrrr/WnP/1JCxYsUH5+vtq0aaOLLrrIt76WLVvqb3/7m+bMmaOZM2fK7XZr1apVSk9P15VXXqnWrVvr0Ucf1dy5c1VSUqI2bdro3HPP1YwZM3zbGT16tBYtWqT7779f99xzjzp27Kh58+bpww8/1OrVqxvoUz5xhumdb9aE5OfnKykpSU6n0/fEfAAAAOBk1tSegdXU8gUQXHFxsXbu3Kn27dsrNjY20ulY2urVqzV8+HAtWrRIEydOjHQ6YVXbcVLfXg7PwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXxEHcAAAAAAIAGMGzYMDXBR403CczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAv1jz58+XYRiKjY3Vvn37qr0+bNgw9erVKwKZoTJHpBMAAAAAAABN2GefRToDafToeq+ipKREjz76qJ577rkGSAgNjRlYAAAAAADgF69v37565ZVXlJ2dHelUEAANLAAAAAAA8It37733yu1269FHH61xOZfLpYcfflgdO3ZUTEyMTj/9dN17770qKSnxLXP77bcrNTVVpmn6YjfffLMMw9Czzz7rix08eFCGYejFF19s+IJOMnyFEAAAAMAv2rLNkc6gwkgeswNETPv27XX11VfrlVde0R//+Ee1bt064HK/+93v9Prrr2vixIm644479PXXX2vOnDnaunWrPvjgA0nSueeeq6efflrff/+97/lZa9askc1m05o1a3TLLbf4YpJ03nnnhaHCpo0ZWAAAAAAAAJLuu+8+uVwuPfbYYwFf37Bhg15//XX97ne/06JFi3TDDTfo9ddf15133qm///3vWrVqlSTpnHPOkVTRoHI6ndq0aZMmTJjgi3lfT0lJUY8ePRq5sqaPBhYAAAAAAICkDh066KqrrtLLL7+s/fv3V3v9k08+kVT+FcHK7rjjDknSxx9/LElKS0tTt27d9M9//lOS9OWXX8put+sPf/iDDh48qB9++EFSeQPrnHPOkWEYjVbTyYIGFgAAAAAAwM/uv/9+uVyugM/C2r17t2w2mzp16uQXb9mypZKTk7V7925f7Nxzz/XNtlqzZo369++v/v37KyUlRWvWrFF+fr42bNigc889t3ELOknQwAIAAAAAAPhZhw4dNHXq1KCzsCSFNGPqnHPO0b59+7Rjxw6tWbNG5557rgzD0DnnnKM1a9boq6++ksfjoYEVIhpYAAAAAAAAlXhnYVV9FtZpp50mj8fj+wqg18GDB5WXl6fTTjvNF/M2ppYvX65vvvnG9/N5552nNWvWaM2aNWrevLn69evXyNWcHGhgAQAAAAAAVNKxY0dNnTpVL730kg4cOOCLjxkzRpL0zDPP+C3/1FNPSZIuvvhiX6x9+/Zq06aNnn76aZWVlenss8+WVN7Y+vHHH7V48WL96le/ksPhaORqTg40sAAAAAAAAKq47777VFZWpv/85z++WJ8+fTRt2jS9/PLLmjx5sl544QVNnz5djz/+uH79619r+PDhfus499xz9Z///Ee9evXSKaecIkk666yz1Lx5c23fvp2vD9YBDSwAAAAAAIAqOnXqpKlTp1aLv/rqq5o1a5a++eYb3Xbbbfr88891zz336J133qm2rLdBdc455/hiDodDgwcP9nsdtTNM0zQjnURd5efnKykpSU6nU4mJiZFOBwAAAGh0yzZHOoMKI3vVvkxTyrcp5QpEQnFxsXbu3Kn27dsrNjY20unAomo7Turby2EGFgAAAAAAACyNBhYAAAAAAAAsjUfdAwAA4BeLr44BANA0MAMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAKCRGIahBx98MNJpNHn1bmB9//33mjRpkjp06KBmzZqpRYsWOu+887RkyZJqy27dulWjR49WfHy8UlJSdNVVV+nw4cP1TQEAAAAAAKDODMMI6X+rV6+OdKq/eI76rmD37t0qKCjQtGnT1Lp1ax0/flzvvfeexo0bp5deeknXXHONJGnv3r0677zzlJSUpNmzZ6uwsFBPPPGENm3apPXr1ys6OrrexQAAAAAAgDD7738jnYHUqdMJve3NN9/0+/mNN97Q8uXLq8W7d+9+wqmhYdS7gTVmzBiNGTPGL3bTTTepX79+euqpp3wNrNmzZ+vYsWP69ttv1a5dO0nSwIEDdeGFF2r+/Pm+5QAAAAAAAMJh6tSpfj+vW7dOy5cvrxZH5DXKM7DsdrsyMjKUl5fni7333nsaO3asr3klSRdccIG6dOmihQsXNkYaAAAAAAAA9XLs2DHdcccdysjIUExMjLp27aonnnhCpmn6LVdSUqLf//73SktLU0JCgsaNG6e9e/dWW9/u3bt1ww03qGvXroqLi1NqaqomTZqkXbt2+ZbZsWOHDMPQ008/Xe39X331lQzD0P/93/81eK1WVu8ZWF7Hjh1TUVGRnE6nPvroI3366aeaPHmyJGnfvn06dOiQ+vfvX+19AwcO1CeffNJQaQAAAAAAADQI0zQ1btw4rVq1SjNnzlTfvn21dOlS/eEPf9C+ffv8Gky/+93v9NZbb+nKK6/UkCFD9Pnnn+viiy+uts5vvvlGX331laZMmaK2bdtq165devHFFzVs2DBt2bJFzZo1U4cOHXT22WdrwYIF+v3vf+/3/gULFighIUGXXnppo9dvJQ3WwLrjjjv00ksvSZJsNpvGjx+v559/XpK0f/9+SVKrVq2qva9Vq1bKzc1VSUmJYmJiAq67pKREJSUlvp/z8/MlSS6XSy6Xy7dNm80mj8cjj8fjW9Ybd7vdft3RYHG73S7DMHzrrRyXJLfbHVLc4XDINE2/uGEYstvt1XIMFqcmaqImaqImaqImaqKmxq3JrFiNZJTnLtM/92Bxw1Zek3/ckGGzyzQ9qrLywHHDJsOwyTQ9crlqrsn0VFre45ZU6V/+jfKaTI//fmqsmlyu2vdT0Fqr5R6emmo69irSrH0/NXZNlYdaUxtPlZ0s5whqKo+7XK6Kc1GVWUeSZASLG0b44gFeD0XVdVf97w8//FCff/65Hn74Yd13330yDEM33HCDLr/8cv31r3/VjTfeqI4dO2rjxo166623dP311+t//ud/JEk33HCDpk6dqo0bN8o0Td+6x4wZo4kTJ/pta+zYsRoyZIjee+8939cXr7rqKl133XXaunWrunXrJkkqKyvTwoULNX78eMXFxUX+c6/CNE2/Xk3lY6/q8VdXDdbAuu222zRx4kRlZ2dr4cKFcrvdKi0tlSQVFRVJUsAGVWxsrG+ZYA2sOXPmaNasWdXiWVlZat68uSQpLS1NHTt21M6dO/3+smHbtm3Vtm1bbd++XU6n0xfv0KGD0tPTtXnzZl9+ktStWzclJycrKyvLbxD37t1b0dHRyszM9Muhf//+Ki0t1caNG30xu92uAQMGyOl0atu2bb54XFyc+vTpo5ycHO3YscMXT0pKUvfu3ZWdne03vZCaqImaqImaqImaqImaGrem0ryKmqJa9JZhj1bpQf+aok/tL9NdqrKcipoMw67olgNkljpVlltRk+GIU3RaH3mKcuRyVtRki0lSVEp3uQuz5S6sqMkelyZHcke5nTuVmVlzTaUFkiOpg+zN0lV2ZLNMV0VNUSndZMQkq+xQlkyz8WvKPF77fnI7d8pdVFGTPb6tHAlt5crbLk9JxX4KR021HXulBaHvp8auKfN4RU1NbTydjOcIaqqoyfu7u9vtVnFxsS9us9nUTJLL7VbZzz0ASbLZ7YqNiZHL5VJZWVnFZ+NwKCY6WqVlZXJXamhERUUpKipKJaWl8lTKMSo6WlEOh4pLSmRWauJFx8TIYberuLhYpmnKc+yY7zO22Ww69vPPXs2bN5fH4/H7XAzDUPPmzf1qqtxkcblc+uijj2S32zVz5kwVFxcrLi5OZWVluv7667V48WJ9+OGHuvHGG33fLPvd737n23Z0dLRuu+02vf322yorK/PFvb2PoqIilZSUKD8/X61atVJycrL+/e9/a/z48TJNUxdffLFiY2P11ltv6S9/+YuOHTumTz/9VDk5OZowYYIkhVSTbz81ayaXy+U3Qchut/tqKq20/xwOh2JjY1VSUuL3mURHRys6OlrFxcV+x5K3prKyMm3evNkXr3zseScjnSjDDNY2q6eRI0cqLy9PX3/9tb799lsNGDBAb7zxhq666iq/5e666y7NnTtXxcXFdZqBlZGRoSNHjigxMVGSdTrTXidTt52aqImaqImaqImaqOlkrWnllkpJRngG1ojuNde0ckul5SM8A2tEj9r309JN1pmBdWHPmo+9iuMg8jOwRvSoCDe18VTZyXKOoKbyeHFxsX766Sd16NAh4O/txo8/Rn4m0An+FcKq677pppv0wgsv+GZMXXTRRdqyZYt2797tt7zT6dQpp5yiO+64Q3PnztX111+vV155RcXFxXI4KuYKFRQUKCkpSX/+85/14IMPSipvXD366KOaN2+e9u3b57f9GTNm6LXXXvP9PHnyZH377bf6789/6fHKK6/UmjVrtHv3btlsgR9rHqkZWCUlJdqxY4fatWvna3hWPvby8/OVmpoqp9Pp6+XURYPNwKpq4sSJuvbaa7V9+3bfVwe9XyWsbP/+/UpJSQnavJLKO3mBXnc4HH4HhlQxYKvyDsBQ41XXeyJxwzACxoPlWNc4NVFTsDg1UZNETcFyrGucmqhJoqZgOdY1bsWajED3/kaQW+QAccMwgsRtCrTymuIOR801VX6bYQtck2ELPfdg8VBqqrwbg+2PoLUGzb1xa6rp2KuaZp33XwPWFGhINZXxVN84NVm3JofDUX5ukHz/X1XE40FeD0XldYf635U/j2CvVd2GN37LLbdo3rx5uu222zR48GAlJSXJMAxNmTJFHo/H7/1XX321Fi1apLVr1+qMM87QRx99pBtuuCHoPg6Ub7jjgXo1gWJ11WgNLO8UNqfTqa5duyotLa3atERJWr9+vfr27dtYaQAAAAAAAJyQ0047TStWrFBBQYESEhJ8ce9XQ0877TTf/3s8Hv3444/q2rWrb7n//Oc/1da5ePFiTZs2TU8++aQvVlxcrLy8vGrLjh49WmlpaVqwYIEGDRqk48ePV/tm2y9F4PlmdXDo0KFqsbKyMr3xxhuKi4tTjx7lc2AnTJigf/zjH9qzZ49vuZUrV2r79u2aNGlSfdMAAAAAAABoUGPGjJHb7fb9kTqvp59+WoZh6KKLLpIk3/8/++yzfss988wz1dZpt9urfQXvueeeq/ZVTql85tIVV1yhhQsXav78+TrjjDPUu3fv+pTUZNV7Bta1116r/Px8nXfeeWrTpo0OHDigBQsWaNu2bXryyScVHx8vSbr33nu1aNEiDR8+XLfeeqsKCws1d+5cnXHGGZoxY0a9CwEAAACAX4Jlm2tfJlxG9op0BkDjuuSSSzR8+HDdd9992rVrl/r06aNly5bpww8/1G233aaOHTtKkvr27asrrrhCL7zwgpxOp4YMGaKVK1f6nl1V2dixY/Xmm28qKSlJPXr00Nq1a7VixQqlpqYGzOHqq6/Ws88+q1WrVumxxx5r1HqtrN4NrMmTJ+u1117Tiy++qCNHjighIUH9+vXTY489pnHjxvmWy8jI0BdffKHbb79df/zjHxUdHa2LL75YTz75ZI3PvwIAAAAAAIgEm82mjz76SH/+85/17rvvat68eTr99NM1d+5c3XHHHX7L/u///q/v635///vfdf755+vjjz9WRkaG33J//etfZbfbtWDBAhUXF+vss8/WihUrNGrUqIA59OvXTz179tTWrVv1m9/8ptFqtbpG+yuEjSk/P19JSUkn/OR6AAAAQGpaM1maUq5S08q3KeUqNb180fQVFxdr586dat++ve+vyyG8zjzzTKWkpGjlypWRTiWo2o6T+vZy6v0MLAAAAAAAADSOzMxMfffdd7r66qsjnUpENdpfIQQAAAAAAMCJ2bx5s7799ls9+eSTatWqlSZPnhzplCKKGVgAAAAAAAAWs3jxYs2YMUNlZWX6v//7v1/81zdpYAEAAAAAAFjMgw8+KI/Ho61bt2ro0KGRTifiaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAgFqZphnpFGBhjX180MACAAAAAABB2e12SVJZWVmEM4GVeY8P7/HS0GhgAQAAAACAoKKiohQTEyOn08ksLARkmqacTqdiYmIUFRXVKNtwNMpaAQAAAADASaNFixbat2+f9u7dq6SkJEVFRckwjEinhQgzTVNlZWVyOp0qLCxUmzZtGm1bNLAAAAAAAECNEhMTJUk5OTnat29fhLOB1cTExKhNmza+46Qx0MACAAAAAAC1SkxMVGJiosrKyuR2uyOdDizCbrc32tcGK6OBBQAAAAAAQhYVFRWWhgVQGQ9xBwAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKU5Ip0AAAAAAODktGxzpDOoMLJXpDMAUB/MwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKU5Ip0AAAAATh7LNkc6gwoje0U6AwAA0FCYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLc0Q6AQAAAAAArGDZ5khnUGFkr0hnAFgLM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGn1bmB98803uummm9SzZ081b95c7dq10+WXX67t27f7LTd9+nQZhlHtf926datvCgAAAAAAADiJOeq7gscee0xffvmlJk2apN69e+vAgQN6/vnnddZZZ2ndunXq1avib3/GxMTo1Vdf9Xt/UlJSfVMAAAAAAADASazeDazbb79db7/9tqKjo32xyZMn64wzztCjjz6qt956q2JjDoemTp1a300CAAAAAADgF6TeXyEcMmSIX/NKkjp37qyePXtq69at1ZZ3u93Kz8+v72YBAAAAAADwC9EoD3E3TVMHDx5UixYt/OLHjx9XYmKikpKSlJKSohtvvFGFhYWNkQIAAAAAAABOEvX+CmEgCxYs0L59+/TQQw/5Yq1atdJdd92ls846Sx6PR5999pleeOEFbdiwQatXr5bDETyVkpISlZSU+H72zuByuVxyuVySJJvNJpvNJo/HI4/H41vWG3e73TJNs9a43W6XYRi+9VaOS+UzyEKJOxwOmabpFzcMQ3a7vVqOweLURE3URE3URE3URE1NrSbTtP/8H/5xw1Zek3/ckGGzyzQ9kumpPW7YZBi24HGPW1JF7h5P7TX5bzZw7sHiDV2Ty1XzfjI9wWuVUV6T6fHfT41Vk8tV+7EX6n4KV001jaeKNBvm2KtPTZWHWrBxJoV/PAWLm2bN54jy5QPX6hcOwzkilPNe+TgL73gKFne5uD5R08lVU9W66qrBG1jbtm3TjTfeqMGDB2vatGm++Jw5c/yWmzJlirp06aL77rtPixcv1pQpU4Kuc86cOZo1a1a1eFZWlpo3by5JSktLU8eOHbVz504dPnzYt0zbtm3Vtm1bbd++XU6n0xfv0KGD0tPTtXnzZhUVFfni3bp1U3JysrKysvx2du/evRUdHa3MzEy/HPr376/S0lJt3LjRF7Pb7RowYICcTqe2bdvmi8fFxalPnz7KycnRjh07fPGkpCR1795d2dnZ2rt3ry9OTdRETdRETdRETdTU1GpSs/4y3aUqy6moyTDsim45QGapU2W5FTUZjjhFp/WRpyhHLmdFTbaYJEWldJe7MFvuwoqa7HFpciR3lNu5U+6iiprs8W3lSGgrV952eUoqasppWXtNpXkVNUW16C3DHq3Sg/41RZ8anpoyM2veT6UFkiOpg+zN0lV2ZLNMV0VNUSndZMQkq+xQlkyz8WvKPF77sRfqfgpHTbWNp9KC0PdTY9eUebyipmDnCMWFfzwFq8nZruZzRKTGU6CaQjnvlRaEfzwFqynzONcnajq5aqrv46QMs3JrrJ4OHDigs88+W2VlZVq3bp1at25d4/JFRUWKj4/XjBkzqv11wsoCzcDKyMjQkSNHlJiYKImOJzVREzVREzVREzVRkxVqWrnVOjOwLuxVe00rt1TebGRnYI3oXvN+WrkleK3hnjEyokftx97STdaZgXVhz5rHU8VxEPkZWCN6VISDjbPPt1lnBtbIM2o+RyzbZJ0ZWCO6137eKx9n1piBNaIH1ydqOrlqys/PV2pqqpxOp6+XUxcNNgPL6XTqoosuUl5entasWVNr80oq7wCmpqYqNze3xuViYmIUExNTLe5wOKp99dD7oVXl3bGhxoN9pbEuccMwAsaD5VjXODVRU7A4NVGTRE3BcqxrnJqoSaKmYDkGihuG9z8C1xQ4bpOM6jnWOW7zz91bdk01BVhNwByDxRuyJoej5v1U+W1Va62Ih557sHgoNVXe7cGOsVD3U+3xhqmppvFUNc36Hnu1x4PnHmioBTtHhHM8BYt7x3ywc0Rd9l9j1xTKec9/nIVnPAWLhzLOuD5RU7C4FWuq6dFRoWiQBlZxcbEuueQSbd++XStWrFCPHj1qf5OkgoIC5eTkKC0trSHSAAAAAAAAwEmo3g0st9utyZMna+3atfrwww81ePDgassUFxerrKxMCQkJfvGHH35Ypmlq9OjR9U0DAAAAAAAAJ6l6N7DuuOMOffTRR7rkkkuUm5urt956y+/1qVOn6sCBAzrzzDN1xRVXqFu3bpKkpUuX6pNPPtHo0aN16aWX1jcNAAAAAAAAnKTq3cD67rvvJElLlizRkiVLqr0+depUJScna+zYsVq+fLlef/11ud1uderUSbNnz9add94Z8PuUAAAAAAAAgNQADazVq1fXukxycrLefPPN+m4KAAAAAAAAv0AN9lcIAQAAAABAeCzbHOkMKozsFekM8EvAd/cAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGmOSCcAAAAAAABObss2RzqDCiN7RToDnAhmYAEAAAAAAMDSmIEFAAB+ef7730hnUKFTp9qXeeONxs8jVFdfHekMAADALxAzsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpPMQdAADA4n7MiXQGFTpGOgEAAPCLxAwsAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoPcQcAAAAAAPjZss2RzqDCyF6RzsA6mIEFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6t3A+ubb77RTTfdpJ49e6p58+Zq166dLr/8cm3fvr3aslu3btXo0aMVHx+vlJQUXXXVVTp8+HB9UwAAAAAAAMBJzFHfFTz22GP68ssvNWnSJPXu3VsHDhzQ888/r7POOkvr1q1Tr169JEl79+7Veeedp6SkJM2ePVuFhYV64okntGnTJq1fv17R0dH1LgYAAAAAAAAnn3o3sG6//Xa9/fbbfg2oyZMn64wzztCjjz6qt956S5I0e/ZsHTt2TN9++63atWsnSRo4cKAuvPBCzZ8/X9dcc019UwEAAAAAAMBJqN5fIRwyZEi12VOdO3dWz549tXXrVl/svffe09ixY33NK0m64IIL1KVLFy1cuLC+aQAAAAAAAOAk1SgPcTdNUwcPHlSLFi0kSfv27dOhQ4fUv3//assOHDhQWVlZjZEGAAAAAAAATgL1/gphIAsWLNC+ffv00EMPSZL2798vSWrVqlW1ZVu1aqXc3FyVlJQoJiYm4PpKSkpUUlLi+zk/P1+S5HK55HK5JEk2m002m00ej0cej8e3rDfudrtlmmatcbvdLsMwfOutHJckt9sdUtzhcMg0Tb+4YRiy2+3VcgwWpyZqoiZqoiZqoqZGqsk05amc4895ejweeSqt22YYshmG3B6PzBDidsMor8lTeS3lcUlym2b1eJXcA9XkMX7erimZkkzDb/HAcbO8Lo8kVYobZvmPnirrCDXu3V/B9odp2n/+D/+4YSuvyT9uyLDZZZoeyfTUHjdsMgxb8LjHXV74zzye2o89/80Gzj1YvKFrcrlqHk+mJ3itMsprMj3+46mxanK5aj9HhLqfwlVTTeeIijQb5tirT02VT4nBxpkU/vEULG6aNZ/Ly5cPXKtfOAzniFCuT+XjLLzjKVjc5ar5mitFbjxVrUmq/T7CV24Yx1OweOXDNdB9hOmJzHgKVJPLdfLc71U9T9RVgzewtm3bphtvvFGDBw/WtGnTJElFRUWSFLBBFRsb61smWANrzpw5mjVrVrV4VlaWmjdvLklKS0tTx44dtXPnTr+/bNi2bVu1bdtW27dvl9Pp9MU7dOig9PR0bd682ZefJHXr1k3JycnKysry29m9e/dWdHS0MjMz/XLo37+/SktLtXHjRl/MbrdrwIABcjqd2rZtmy8eFxenPn36KCcnRzt27PDFk5KS1L17d2VnZ2vv3r2+ODVREzVREzVREzU1Uk1Op/ZWyjEtPl4dU1O18+hRHS4srKgpKUltk5O1PSdHzkq5d0hNVXp8vDYfOKCisrKKmtLTlRwXp6x9++SudLPXu1UrRTscytyzx7+mjAyVFhXVWtPxU5spyuVR65xiFcY5lJtU8fiG2BK3Tj1aImd8lJzxUb54fJFLqc5SHU2KVmFcxS1fUmGZkgvLdDg5RsUxdl88xVmqhCKXDqTGqsxRMUk/PbdYcaUe7U2Pk2kYOvLzfgm2n9Ssv0x3qcpyKmoyDLuiWw6QWepUWW7FfjIccYpO6yNPUY5czor9ZItJUlRKd7kLs+UurDj27HFpciR3lNu5U+6iimPPHt9WjoS2cuVtl6ekYr/mtKz92CvNqzj2olr0lmGPVulB/5qiTw1PTZmZNY+n0gLJkdRB9mbpKjuyWaaroqaolG4yYpJVdihLptn4NWUer/0cEep+CkdNtZ0jSgtC30+NXVPm8Yqagp33FBf+8RSsJme7ms/lkRpPgWoK5fpUWhD+8RSspszjNV9zpciMp0A1SbXfR3jHWTjHU7CavOMs2H1EWVFkxlOgmjKPnzz3e97JSCfKMM0q/xRYDwcOHNDZZ5+tsrIyrVu3Tq1bt5YkZWZmasCAAXrjjTd01VVX+b3nrrvu0ty5c1VcXFynGVgZGRk6cuSIEhMTJTX9fw1euTWy/9JT2cgzmlYXt7KTpTNNTdRETdRETY1c0w8/WGcGVqdOtda087m3y7drgRlY7W++sjz3IPtj5VbrzMC6sFftx97KLZU3G9kZWCO61zyeVm4JXmu4Z4yM6FH7OWLpJuvMwLqwZ83niIrjIPIzsEb0qAgHG2efb7PODKyRZ9R8Ll+2yTozsEZ0r/36VD7OrDEDa0SPmq+5K7ZYZwbWqN6130f4xpkFZmBVHmeB7iNWbrHODKwRPU6e+738/HylpqbK6XT6ejl10WAzsJxOpy666CLl5eVpzZo1vuaVVPHVQe9XCSvbv3+/UlJSgjavpPKZW4Fedzgccjj8S/B+aFV5d2yo8arrPZG4YRgB48FyNAybZNQhbguce/B4kN1t+Md/vsdukJrqGm8K+4maqClYjnWNUxM1SdQULMe6xutc088NqIDLB9imPcA6aoo7gsUDbFNBcq9ck63yva3Km0rVlg8St0l+98a+eJB/wqwtXjXXqj/7SjQC1xQ4Xsd7oBDvjby7oaZjL8BqAuYYLN6QNTkcNY+nym+r7/1eTfFQaqq82+t8b9tI97A1xWs7R1RNM5L35YFOfcHOEeEcT8HiNf3uUL58ZMZToHgo1yf/cRae8RQsHtI4i9B4ChSv7X4h5HEWhpqqHq5VzxHetMI9niriFblUzrWp3+8Fyz9UDdLAKi4u1iWXXKLt27drxYoV6tGjh9/rbdq0UVpaWvUp5pLWr1+vvn37NkQaAAAAAAAAOAnV+68Qut1uTZ48WWvXrtWiRYs0ePDggMtNmDBB//jHP7Sn0rMfVq5cqe3bt2vSpEn1TQMAAAAAAAAnqXrPwLrjjjv00Ucf6ZJLLlFubq7eeustv9enTp0qSbr33nu1aNEiDR8+XLfeeqsKCws1d+5cnXHGGZoxY0Z90wAAAAAAAMBJqt4NrO+++06StGTJEi1ZsqTa694GVkZGhr744gvdfvvt+uMf/6jo6GhdfPHFevLJJ2t8/hWsZ9nmSGdQYWSvSGcAAAAAAAAaW70bWKtXrw552Z49e2rp0qX13SQAAAAAAAB+Qer9DCwAAAAAAACgMdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdX7Ie4AAABNzdofI51BhcGdIp0BAACA9TEDCwAAAAAAAJbGDCwAANAw/vvfSGdQoRPTmgAAAE4mzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTkinQDQ2JZtjnQGFUb2inQGAAAAAAA0PczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl8VcILSJh338jnUKFXp0inQEAAAAAAIAPM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGmOSCcAAABODmt/jHQGFQZ3inQGAAAAaEjMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTkinQCACss2RzqDCiN7RToDAAAAAADK0cDCSS9h338jnUKFXp0inQEAAAAAAE0OXyEEAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTVIA6uwsFAPPPCARo8erZSUFBmGofnz51dbbvr06TIMo9r/unXr1hBpAAAAAAAA4CTkaIiV5OTk6KGHHlK7du3Up08frV69OuiyMTExevXVV/1iSUlJDZEGAAAAAAAATkIN0sBq1aqV9u/fr5YtWyozM1MDBgwIvkGHQ1OnTm2IzQIAAAAAAOAXoEG+QhgTE6OWLVuGvLzb7VZ+fn5DbBoAAAAAAAAnubA/xP348eNKTExUUlKSUlJSdOONN6qwsDDcaQAAAAAAAKCJaJCvEIaqVatWuuuuu3TWWWfJ4/Hos88+0wsvvKANGzZo9erVcjgCp1NSUqKSkhLfz97ZWy6XSy6XS5Jks9lks9nk8Xjk8Xh8y3rjbrdbpmnWGrfb7TIMw7feynGpfPZYKHGHwyHTNP3ihmHIbrdXy9EwDEn6OQ/Tbz2GYZNpeuSv/OH3DREv579N7+cRrCbTUzluyLDZy9ftt/4gccNWUVOguMftn0/QeOj7qbzuwLWW5xLsc69rvPbP3eVy1XjsSYZMj6vKauw/p+4OKW7YyveTf7zu+0lquuMpULypnyOoiZqaQk2maTbq9aku53K3211jTVa55kpGtf0hVd9Pnp/fbjPL12Aa/msJGDfL/6XSU3nzkgyz/EdPlXWEGvceg8GOMdNs3OtTXe4jPJ7ax5P/ZiNzzfXW5HLVfI4ov6Wp+d4oXPcRLlft54iGut9rqJpqOu9VpBmee9iaaqp8mg82zqTwj6dgcdOs+frk/7uDwjaeAsVDueaWj7PwjqdgcZer5vsIKXLjqWpNUu33Eb5ywziegsUrH66B7o1MT2R/z61ck8tlrfu9+tzDVj1P1FVYG1hz5szx+3nKlCnq0qWL7rvvPi1evFhTpkwJ+r5Zs2ZVi2dlZal58+aSpLS0NHXs2FE7d+7U4cOHfcu0bdtWbdu21fbt2+V0On3xDh06KD09XZs3b1ZRUZEv3q1bNyUnJysrK8tvZ/fu3VvR0dHKzMz0y6F///4qLS3Vxo0bfTG73a4BAwbI6XRq27ZtvnhcXJz69OmjnJwc7dixwxcvf4h9lEo8ThW7K3KMtsWrmSNVRe6jKvVUzFKLtScp1p6sY64cucyK3OPsqYqxx6vQdUBus8wXb+5IV5QRp/yyfTJVceAlRLWSTQ45y/b41eR2d6ixJs/ubyviRpQSolqrxF2oIvcRX9xhxCk+Kl3F7ryANR13HQlYU2HZoYA1FZRlV6/JFqesoqO17idn2TElRWXII5cKyvb74oZsSorOkMss1jHXoWo1lXqOBaypPvspMzO3xmNPSlbZoSyZlU62US16y7BHq/Sg/7EXfWp/me5SleVU7CfDsCu65QCZpU6V5VYce4YjTtFpfeQpypHLWXHs2WKSFJXSXe7CbLkL91Z8BnFpkprueOrevbuys7O1d29FTU39HEFNDVjT3r3K3ON/3uufkaFSl0sb91ecI+w2mwZkZMhZVKRthyrOEXFRUerTurVyCgu140jFOSIpLk7d09OVnZenvZVyTIuPV8fUVO08ckSHK804bpuUpLb9+59U+6nE42jU61NdzuWbNxfVWJNVrrlJURkqKiqqdT8dP7WZolwetc4pVmGcQ7lJ0RU5lrh16tESOeOj5IyP8sXji1xKdZbqaFK0CuMqbvmSCsuUXFimw8kxKo6x++IpzlIlFLl0IDVWZY6KSfrpucWKK/Vob3qcTMPQkZ+PtWDHnpo17vXJkdxRbudOuYsqjj17fFs5EtrKlbddnpKK/ZrTsvbxVJoX+Wuut6bMzJrPe6UFkiOpg+zN0lV2ZLNMV0VNUSndZMSE7z4i83jt54hQ91M4aqrtvFdaEPp+auyaMo9X1BTsXK648I+nYDU529V8fYrUeApUUyjX3NKC8I+nYDVlHq/53kiKzHgKVJNU+32Ed5yFczwFq8k7zoLdG5UVRWY8Baop87i17vfqc19e30dJGWbl1lgD8D7Efd68eZo+fXqtyxcVFSk+Pl4zZsyo9tcJvQLNwMrIyNCRI0eUmJgoqen/C/f6FTst86/Bg0d1rrGmtUt/CJBjw89WCiU+YMTpftFA+2P9ih1Baw33DKyBF3So8dhb/n3k/6Xn55Vo1BlNdzz90mfBUFMtNf33v3JXufTZf54JWzXusJWP+cpxQ+XNLY9pyhNC3PZznh6PR5VHn80wZOvc+aTaT+tX7LTMDKxBF3assaavPvshyHrCPwNr8KhOte6nnc+9LckaM7Da33ylpODH2Mqt1pmBdWGv2sfTyi2VNxvZGVgjutd83lu5JXit4Z4xMqJH7eeIpZusMwPrwp41n/cqjoPIz8Aa0aMiHGycfb7NOjOwRp5R8/Vp2SbrzMAa0b32a275OLPGDKwRPWq+N1qxxTozsEb1rv0+wjfOLDADq/I4C3RvtHKLdWZgjehhrfu9+tyX5+fnKzU1VU6n09fLqYuwzsAKJC4uTqmpqcrNzQ26TExMjGJiYqrFHQ5Hta8dej+0qrw7NtR4sK8z1iVuGEbAeLAcy79KaASIB35UWUPFq27T+5XGYDUFWk/w3Bu3plD2h/9765Jjw9dUOa9gx55hCzIsjdDjhmEEidukgPsvcLwpj6e6xqnpF1STYchhVB/DkgLGjSDL2wxDtrrEbbaAD548mfaT9/rRWNenmuJVz83ez8/q11xvLrXtJ1vle1tJRoB/fgwWt0nV+2ZV1lmXeNVcq/7sO/wb8foUNG7zHzfeXV/TeAq4qyJwzTUMmxyOms97ld9WtdaKeHjuIyrv9uDjLLT9VHu8YWqq6bxXNc36Hnu1x4PnHuh0HuwcEc7xFCzuHfPBrkN12X+NXVMo11z/cRbZ+/KQxlmExlOgeG33CyGPszDUVPVwrXqO8KYV7vFUEa/IpXKuVrjf8zqRe9hg+Ycq7A9xr6qgoEA5OTlKS0uLdCoAAAAAAACwoLA1sIqLi1VQUFAt/vDDD8s0TY0ePTpcqQAAAAAAAKAJabCvED7//PPKy8tTdna2JGnJkiW+B4DdfPPNOnr0qM4880xdccUVPz+sWlq6dKk++eQTjR49WpdeemlDpQIAwElh2eZIZ1BhZK9IZwAAAIBfsgZrYD3xxBPavXu37+f3339f77//viRp6tSpSk5O1tixY7V8+XK9/vrrcrvd6tSpk2bPnq0777wz4HcqAQAAAAAAgAZrYO3atavWZd58882G2hwAAAAAAAB+IZj2BAAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3NEOgEATdh//xvpDCp06hTpDIAGl7DPQmOsF2MMAAAAkcMMLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFiaI9IJAKiQsO+/kU6hQq9OtS6y9scw5BGiwbWnCwAAAABoopiBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3NEOgEAAMJp7Y+RzqDC4E6RzgAAAABoGpiBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3M0xEoKCws1d+5cff3111q/fr2OHj2qefPmafr06dWW3bp1q37/+9/rX//6l6Kjo3XxxRfrqaeeUlpaWkOkAgAIs2WbI51BhZG9Ip0BAAAAgMbQIA2snJwcPfTQQ2rXrp369Omj1atXB1xu7969Ou+885SUlKTZs2ersLBQTzzxhDZt2qT169crOjq6IdIBgGposgAAAABA09UgDaxWrVpp//79atmypTIzMzVgwICAy82ePVvHjh3Tt99+q3bt2kmSBg4cqAsvvFDz58/XNddc0xDpAAAAAAAA4CTSIM/AiomJUcuWLWtd7r333tPYsWN9zStJuuCCC9SlSxctXLiwIVIBAAAAAADASSZsD3Hft2+fDh06pP79+1d7beDAgcrKygpXKgAAAAAAAGhCGuQrhKHYv3+/pPKvG1bVqlUr5ebmqqSkRDExMdVeLykpUUlJie/n/Px8SZLL5ZLL5ZIk2Ww22Ww2eTweeTwe37LeuNvtlmmatcbtdrsMw/Ctt3Jcktxud0hxh8Mh0zT94oZhyG63V8vRMAxJ+jkP0289hmGTaXrkz5BhGA0SL+e/Te/nEaymquspzzFY7o1bUyj7qfy9gWs9sdxPvCaXy1XjsVeRr/96AuXe2DVJqnU8VeTaMMdefWryHgvBxplp2ir2U+V8jJ/jHrf/+oPGy88Rpsf/2JNh/3lD7lrjLlfdzxGB4lY573k/TsNWXpP/Z2DIsNmrf+7B4kb99pO3hJpqCny8R+YcIamW/VTlMwvTeAoUr/xZBjv2TNNs1OtTXWpyu901jierXHMlo9q5QKp+jvD8/HabWb4G0/BfS8C4Wf4vlZ7Km5dkmOU/eqqsI9S491gIdo4wzcDnw0icIzye2s97/psN/VzeGDW5XDWfy8tvaRrv+lSXmlyu2q9PVrjmVq6ppmtuRZqNc32qS02VL13BxpkU+Wuul2nWfB9RvnzgWv3CYThHhHJvVD7OwjuegsVdrprv96TIjaeqNUm138NW/OoQ+fvyyodroPty0xOZ8RSoJper8fsR4fpdo+p5oq7C1sAqKiqSpIANqtjYWN8ygV6fM2eOZs2aVS2elZWl5s2bS5LS0tLUsWNH7dy5U4cPH/Yt07ZtW7Vt21bbt2+X0+n0xTt06KD09HRt3rzZl5skdevWTcnJycrKyvLb2b1791Z0dLQyMzP9cujfv79KS0u1ceNGX8xut2vAgAFyOp3atm2bLx4XF6c+ffooJydHO3bs8MWTkpIkRanE41SxuyLHaFu8mjlSVeQ+qlJPYcXnZU9SrD1Zx1w5cpkVucfZUxVjj1eh64DcZpkv3tyRrigjTvll+2Sq4sBLiGolmxxylu3xq8nt7lBjTZWXtxtRSohqrVLPMRW5j/jiDiNO8VHpjV5TKPvJWXZMSVEZ8silgrL9vrghm5KiM+Qyi3XMdSgsNWVm5tZ47EkKeT81dk2Sah1PzrJjIe2ncNSUmZlbvo6kJHXv3l3Z2dnau3dvRa1HDDVzpOq460jA/VRYdijgsVdQll29JlucnKV7TrimrJLEOp8jAtVklfOe5/AxGbIpMTpDZZ6igPupxF0Y8NgrducFHE8nup8yjzevtSbJDPt4CnaOkFTjfnKW5fji4RxPgWqqfBwEO/ZKPI5GvT7VpabNm4tqHE9WueYmRWWoqKio1vuI46c2U5TLo9Y5xSqMcyg3qeIP38SWuHXq0RI546PkjI/yxeOLXEp1lupoUrQK4ypu+ZIKy5RcWKbDyTEqjrH74inOUiUUuXQgNVZljopJ+um5xYor9WhvepxMw9CRn4+FYOcINesv012qspyKmgzDruiWA2SWOlWWW3HeMxxxik7rI09RjlzOiv1ki0lSVEp3uQuz5S6sOO/Z49LkSO4ot3On3EUVx549vq0cCW3lytsuT0nFfs1pWft5rzSv4hwR1aK3DHu0Sg/61xR9anhqysys+VxeWiA5kjrI3ixdZUc2y3RV1BSV0k1GTLLKDmXJNBu/pszjtV+fQt1P4aiptmtuaUHo+6mxa8o8XlFTsN81FBf+8RSsJme7mu8jIjWeAtUUyr1RaUH4x1OwmjKP13y/J0VmPAWqSar9HtY7zsI5noLV5B1nwX53LyuKzHgKVFPm8cbvR4Trdw3vZKQTZZiVW2MNwPsQ93nz5mn69OnV4m+88Yauuuoqv/fcddddmjt3roqLi0OegZWRkaEjR44oMTFRknVmInjVteO5fsVOy/xr8OBRnWusae3SHwLkGJkZWANGnO4XDbQ/1q/YEbTWcM/AGnhBhxqPvXXLfrTMDKwho7vUOp7KP9vAtdYWb+iaBl7Q4edY4HG2fsWOiM2uqBofeEEHy/6rSGWhnve8x0G4x1OguPc4qKmmtUv/W22bkTpHDBnducb99PXyH0P6DALl3tA1DbygfbUcq4+znZaZgTXowo41jqevPvshyHrCf44YPKpTrfcRO597W5I1ZmC1v/lKScHPESu3WmcG1oW9aj/vrdxSebORnYE1onvN5/KVW4LXGu4ZIyN61H59WrrJOjOwLuxZ8zW34jiI/AysET0qwsHG2efbrDMDa+QZNd9HLNtknRlYI7rXfm9UPs6sMQNrRI+a7/dWbLHODKxRvWu/h/WNMwvMwKo8zgLdl6/cYp0ZWCN6nDwzsPLz85Wamiqn0+nr5dRF2GZgeb866P0qYWX79+9XSkpKwOaVVD5rK9BrDodDDod/Cd4PrSrvjg01XnW9JxI3DCNgPFiO5V8lNALEAz+qrKHiVbfp/UpjsJoCrSd47o1bUyj7w/+9dcmx4WuqnFewYy/U/VRTvKFqqm08Vc21vsdeTfHacq/tXODNIdzjKVDcm2tdzxF1jYfrvFf5swjneAoUr5prsPNYJMZTsNxr2k+Bz7eROUeEcqx6rx/hHE/+266Iez9Xq19zvbnUdh9hq3xvK8kI8M+PweI2qXrfrMo66xKvbZwZ3hKNIOMvYNwmBTve6xK3+Y8n766v6bwXcFcFyDFYvCFrcjhqPpdXflvVWivioeceLB5KTZV3e/BxFtp+qj3eMDXVdB6rmmZ9j73a48FzD3TZDXo9C+N4Chb3jvlg9wt12X+NXVMo90b+4yw84ylYPKRxFqHxFChe271qyOMsDDVVPVyrniO8aYV7PFXEK3KpnGtj9iPC8btGsPxDFbaHuLdp00ZpaWnVp5lLWr9+vfr27RuuVAAAAAAAANCEhK2BJUkTJkzQP/7xD+3ZU/H8h5UrV2r79u2aNGlSOFMBAAAAAABAE9FgXyF8/vnnlZeXp+zsbEnSkiVLfA8Au/nmm5WUlKR7771XixYt0vDhw3XrrbeqsLBQc+fO1RlnnKE</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -536,25 +546,30 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45638.66666666666</v>
+        <v>45639.5</v>
       </c>
       <c r="E3" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F3" t="n">
-        <v>41.3715397540904</v>
+        <v>32.81528883369784</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45638.66666666666</v>
+        <v>45639.5</v>
       </c>
       <c r="H3" t="n">
-        <v>25.70818089538373</v>
+        <v>18.40551019114638</v>
       </c>
       <c r="I3" t="n">
-        <v>11.0458534962149</v>
+        <v>4.163773324629497</v>
       </c>
       <c r="J3" t="n">
-        <v>41.3715397540904</v>
+        <v>32.81528883369784</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACKEElEQVR4nOzdeXhU5fn/8c+ZmewhwUCQHdlXWZRFUGRTBBWUTVCQRfqzrmi1atG2VK2g1brX1uVbUMEq4G5dWARLlcUoCggIylJ2DEtCINtknt8fcSYZMpNMSDJzBt+v6+LS3HPmzH3POc85Z+48c2IZY4wAAAAAAAAAm3JEOgEAAAAAAACgPDSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAKikiRMnyrIsjRs3LqTln3jiCVmWpQ4dOtRwZhXr37+/LMvS8uXLI/L6kydPlmVZmjNnTkRev7pE+n38JTnrrLNkWZZ27NgR6VQAAEAE0cACAKCSpk6dKkl65513dOTIkQqXnz17tt/zasqf/vQnWZalP/3pTzX6Oqe7aHofw9lIW758uSzLUv/+/Wv8tQAAAE5GAwsAgEq68MIL1apVK+Xn52vevHnlLvvll19q/fr1iomJ0bXXXhumDIN75ZVXtGnTJvXs2TPSqUQ13kcAAIDwooEFAEAlWZal6667TlLJ7KpgvI9ffvnlqlevXo3nVpGmTZuqXbt2SkxMjHQqUY33EQAAILxoYAEAcAomT54sp9Opr7/+WuvWrQu4TF5env71r39JKvv1wa+++krjx49X06ZNFRcXp7S0NF1yySX68MMPA66r9H2A3n33XQ0cOFBpaWm+r49ZlqX7779fknT//ffLsizfv8mTJ/vWU9FXzj799FONGTNGjRs3VlxcnNLT09WjRw/NmDFDhw4d8i1XWFiouXPnavz48WrXrp1SUlKUkJCgtm3batq0adq7d2+ob2WF5syZ46vj0KFDuvnmm33vW7NmzfSb3/wm6Fc533rrLf3qV79Sp06ddMYZZyg+Pl7NmzfXddddp++//77M8tX1Pi5dulQjR45UgwYNFBsbq3r16mnEiBFauXJlwOW9ryFJb775pi644AKlpKQoKSlJ559/fpn9wrvNP/vsM0nSgAED/HItfY+xr776SmPHjlXjxo0VGxurlJQUtWjRQqNGjdK7774bMJ+T9e/fXwMGDJAkffbZZ36vddZZZ/kt63a79Y9//EN9+vRRamqq4uPj1bp1a02bNk179uwJ6fWCefvtt33vTa1atdS/f/+gY8Zr4cKFGjJkiNLT0xUbG6tGjRppwoQJ2rhxY6Vff+vWrbruuuvUvHlzxcXFKTk5Wc2aNdNll10WtJm9ZcsW/frXv1bLli0VHx+v1NRUXXjhhZo7d2615b1jxw7ftjDG6IUXXtC5556rpKQkpaamavDgwUH3PQAAooYBAACnZNiwYUaSmTZtWsDH582bZySZhg0bGrfb7Ys/+eSTxuFwGEmma9euZvTo0eaCCy4wsbGxRpK5//77y6yrWbNmRpK55ZZbjCTTvXt3c/XVV5t+/fqZ//znP2bSpEmmS5cuRpLp0qWLmTRpku/fiy++6FtPv379jCSzbNmyMq9x6623Gkm+vMaNG2eGDh1qWrRoUeY5u3btMpJMamqqOe+888yYMWPMpZdeaho2bGgkmfT0dLN169YyrzFp0iQjycyePTvk93n27NlGkhk+fLhp2bKlqV27trnyyivNiBEjzBlnnGEkmbZt25qDBw+Wea7T6TSJiYmme/fuZuTIkWb48OG+epKSksznn39eJr+qvo933nmnkWQcDofp2bOnGTNmjOnVq5exLMs4nU7zz3/+s8xzvO/7H//4R2NZljn//PPN2LFjfblYlmXeeust3/KbNm0ykyZNMmeeeaaRZC655BK/XFesWGGMMWbJkiUmJibGV8/o0aPNiBEjTM+ePU1cXJy54oorQtoGs2bNMpdccomRZM4880y/17rzzjt9y+Xl5ZmLLrrISDLx8fFm6NChZuzYsaZJkyZGkqlbt6756quvQnpNL+++/5vf/MZv3+/Zs6fvfXv66afLPK+wsNBcddVVRpKJi4szffr0MWPGjPG9pwkJCeajjz4KOY/169eblJQU3/42cuRIM2bMGNO7d2+TnJxsunTpUuY58+fPN/Hx8UaSadeunRkxYoQZOHCgSUpKMpLMlClTqiXv7du3G0mmWbNmZtKkSSYmJsYMHDjQXHXVVaZNmza+da1atSrkegEAsBsaWAAAnKJ33nnHSDJ16tQx+fn5ZR73fpC/9957fbGPP/7YWJZl6tataz777DO/5detW2caN25sJJnly5f7Peb9EO90Os27774bMJ8ZM2YYSWbGjBlBcw7WeHn66ad9tXz66adlnrd69Wrzv//9z/dzdna2effdd8vUXVBQYKZPn24kmUsvvbTMeqrSwJJkzjvvPHPo0CHfY0eOHDF9+vQxksy4cePKPPf11183OTk5fjGPx2P+9re/GUmmY8eOxuPx+D1elffxhRdeMJJMq1atzLfffuv32GeffWZq1aplYmNjzZYtW/we89ZXu3btMk0Gbz5t2rQJOQ+vAQMGGElm7ty5ZR47evSoWblyZdAaT7Zs2TIjyfTr1y/oMvfcc4+RZFq2bGm2b9/uixcUFJipU6caSaZ58+YBx0sw3n3fsqwydbz++uvGsizjcrnM+vXr/R679957jSTTq1cvs23bNr/HFixYYJxOpznjjDPMkSNHQspjypQpRpL585//XOaxEydOBBzPcXFxJj4+3rz55pt+j+3YscOcffbZRpJ5+eWXq5y3t4HlbWJ9//33vsfcbre57rrrjCQzePDgkGoFAMCOaGABAHCKCgsLTf369Y0ks2DBAr/Hdu7c6ZtlVXomUq9evYwks3DhwoDrnD9/vpFkRo0a5Rf3foi/7rrrguZzqo2XwsJCk56ebiSV+aB9qho2bGgcDofJzs72i1e1gbV27doyj69bt85YlmUcDofZtWtXyOvt3bu3kWS+++47v/ipvo9FRUW+GWgZGRkBn/eXv/zFSPKbtWRMSQMr0EyivLw8k5qaaiT5NRGD5VFahw4djCRz+PDhoLWEqqIGVm5urklOTjaSzHvvvVfm8ePHj/tmjM2bNy/k1/Xu+1deeWXAx0eNGmUkmf/3//6fL3bo0CGTkJBg4uPjze7duwM+76abbjKSzDPPPBNSHpdeeqmRZL7++uuQlh87dqyRZB577LGAj69Zs8ZIMueee26V8y7dwAr03u/bt883C6ugoCCk/AEAsBvugQUAwClyuVyaNGmSJOmf//yn32OzZ8+Wx+NRv3791KpVK0lSZmam1qxZo4SEBA0bNizgOvv37y9J+uKLLwI+Pnr06GrKvsRXX32ln376SXXr1tWIESMq9dxvv/1Wjz/+uG699VZdd911mjx5siZPniy32y2Px6Mffvih2vLs0qWLunbtWiZ+9tlnq1u3bvJ4PPrPf/5T5vEffvhBzz77rG6//XZNnTrVl+OBAwckKeC9sE7F2rVrtXfvXrVs2VLnnntuwGUq2r6B9ou4uDi1aNFCkip9DynvX0kcP368/vvf/8rtdlfq+ZWRkZGhnJwcpaWlBawjMTFR48aNkyQtW7as0uv3jrVg8dL3I1u2bJlyc3N1/vnnq1GjRgGfV9G2OJn3vbzxxhv1ySefKC8vL+iyHo9HH330kSRp7NixAZfp3r27kpOTtXbtWt+6qpq3y+XSkCFDysTr16+vM844Q/n5+X73sgMAIJq4Ip0AAADR7LrrrtMjjzyiRYsWac+ePWrUqJGMMb6baJe+efv27dtljFFubq7i4uLKXe9PP/0UMH7yDbOrw86dOyVJbdu29d1IvCLHjx/Xtddeq7fffrvc5bKzs6ucn1fz5s3Lfezrr7/W7t27fbGioiLdcsstev7552WMqfEct23bJkn68ccfK3wfg23fpk2bBoynpKRIUrlNk0BmzZqldevW6aOPPtJHH32khIQEnXPOOerfv7/Gjx+v9u3bV2p95fE218rbTi1btvRbtjKCrdcbL73tvdti6dKlp7wtTnbXXXfpv//9r5YsWaIhQ4YoJiZGXbp00YUXXqhx48apR48evmUPHTrk26+aNGlS4boPHTqkRo0aVTnvBg0aKCYmJuDyKSkpOnLkSKX3IQAA7IIGFgAAVdCmTRv17dtXK1as0CuvvKLp06dr2bJl2rFjh1JTU/1mTHk8HklScnKyRo0adUqvl5CQUC15V9X06dP19ttvq127dnr44YfVo0cP1a1bV7GxsZKkPn36aOXKleU2jmpC6dd76qmn9I9//EP169fX448/rj59+ujMM89UfHy8JOmaa67Rv/71r2rL0bt969evr0suuaTcZevWrRsw7nBU7+T4+vXrKyMjQ5999pmWLFmizz//XKtXr9bnn3+umTNnatasWbrnnnuq9TUjpfR29G6LVq1a6fzzzy/3ee3atQtp/YmJiVq8eLG+/PJLffzxx/riiy/0xRdfKCMjQ48//rhuuukm/e1vf/N7fSn4zLHSvA3tquZd3fsPAAB2QgMLAIAqmjp1qlasWKHZs2dr+vTpvq8Tjhs3zq/h5J2JYVmW/vnPf9rmw6Z31s+WLVtkjAlpFtb8+fMlSW+88YY6d+5c5vGtW7dWb5IqnsEWzI4dOyRJjRs39sW8OT7//PMaPnx4medUd47e7VunTh3fDDw7sCxL/fv39331LC8vT3PmzNHNN9+se++9V6NHj/bNjKoK71feyttO3hlGwb4eV57t27erS5cuZeKBtr13W7Rt27bat0WPHj18s63cbrfeeecdTZw4Uc8995xGjx6tAQMGqG7dukpISFBubq4ee+yxoA3Lk9Vk3gAARDt7XDkDABDFxowZo5SUFG3dulUffPCB3nrrLUn+Xx+UpIYNG6pz5846duyYPv7442rPwzv7qbL3Oerevbvq1q2rn376Se+8805Izzl8+LAkqVmzZmUe++STT5SZmVmpHEKxbt06rVu3rkz8u+++09dffy2Hw6ELL7wwpBy/++47ffPNNwFf51TfR+8stI0bN+q7776r1HNP1ankGh8frxtuuEGdO3eWx+MJ+J6eymt57+l0+PBhvffee2Uez83N1euvvy5JGjBgQMj5er366qsB46+88oqkkntDSdKgQYMUGxur5cuX6+DBg5V+rVC5XC6NHj3aN+POu085nU5dfPHFkkoaqaEIV94AAEQjGlgAAFRRYmKirr76aknF98TKzc3V2Wef7XdPHK8///nPkqQpU6bo/fffL/O4MUarV6/WokWLKp2HdwZKZZsnLpdL9913nyTp+uuvD3gj9C+//NLvHkPeeyc988wzfst9//33uuGGGyr1+qEyxujGG2/UkSNHfLGsrCzdeOONMsZo1KhRfvcb8ub4t7/9ze8rXfv27dPEiRODNmJO9X2MiYnRjBkzZIzRiBEj9N///rfMMkVFRfr000+1atWqSq07mIpyfeyxx/S///2vTHzz5s2+GWiBGnzlvdbWrVtVWFhY5vH4+HjdfPPNkqQ777zTd281SSosLNRtt92m/fv3q3nz5qf0xwjefvttXwPMa+HChXrzzTflcrl06623+uJnnnmmbr31Vh0/flzDhg3T+vXry6wvPz9f7733njZv3hzS6z/33HMBb/i/f/9+ZWRkSPJ/L2fMmKHY2Fjdddddevnll/32Qa8NGzb4Gt41lTcAAKeNyPzxQwAATi9r1qzx/Rl7SebJJ58MuuxTTz1lXC6XkWRatWplLrvsMnPNNdeYiy++2NSrV89IMvfcc4/fc5o1a2Ykme3btwdd7/79+01SUpKRZM4//3wzefJkM3XqVPPPf/7Tt0y/fv2MJLNs2TK/53o8HnPDDTf48u/WrZsZN26cufTSS02LFi3KPOfNN980lmUZSebss88248aNMwMHDjQxMTFm4MCBpk+fPgFfZ9KkSUaSmT17dkVvqc/s2bONJDN8+HDTokULU7t2bTNixAgzcuRIk5aWZiSZ1q1bmwMHDvg9b9WqVSY2Ntb3Pl911VVmyJAhJiEhwXTs2NGMGDEiYC5VeR+NMeauu+7yvY8dO3Y0V1xxhRk3bpzp37+/qV27tpFk/v73v/s9x7t8MMFe74MPPjCSTGxsrLn88svNddddZ6ZOnWo+//xzY4wxqampRpJp166dGTFihLnmmmtM//79ffvfxIkTQ9gCJbp3724kmbZt25rx48ebqVOn+u2reXl5ZtCgQUaSSUhIMJdeeqkZO3asadq0qZFk6tSpYzIyMir1mt59//bbbzeSTI8ePcw111xjevXq5XvfHn/88TLPKywsNNdcc42RZBwOh+nWrZsZNWqUGTt2rDn//PN92/ijjz4KKY8uXboYSaZ58+Zm2LBhZvz48Wbw4MEmISHBSDIDBw40hYWFfs+ZP3++SUxMNJJM48aNzeDBg8348ePN0KFDTePGjY0kM3bs2CrnvX37diPJNGvWrML3sbxjCAAAdkYDCwCAanL22Wf7mgmZmZnlLrt+/Xpz/fXXm9atW5v4+HiTmJhoWrRoYS655BLz9NNPmz179vgtH+qHz//85z/moosuMmeccYZxOBxGkpk0aZLv8fIaL8YY89FHH5krrrjCnHnmmSYmJsakp6ebnj17mvvvv98cOnSozGsNGjTI1K1b1yQmJppOnTqZhx56yOTn5wd9nao0sCZNmmQOHjxofv3rX5vGjRub2NhY06RJEzNt2rQyuXmtW7fODB8+3DRo0MDEx8eb1q1bm7vvvttkZ2eXm0tV38fPP//cjB8/3jRr1szExcWZWrVqmTZt2pgrr7zSvPTSS+bw4cN+y59qA8sYY1588UVzzjnn+BolpWuaO3eumTJliunUqZNJS0szcXFxplmzZmbo0KHm7bffNh6PJ+hrBrJz505zzTXXmAYNGviaYCc3TQoLC81zzz1nzjvvPFOrVi0TGxtrWrZsaW699Vaze/fuSr2eMf77/vz5803v3r1NcnKySUpKMn379jXvv/9+uc//8MMPzciRI02jRo1MTEyMqV27tmnfvr0ZN26cee2118zx48dDyuODDz4wN954o+nWrZtJT083sbGxpnHjxqZ///7m5ZdfNgUFBQGft337dvOb3/zGdOrUySQlJZn4+HjTrFkz079/f/Pwww+bH374ocp508ACAPwSWMaE+c8DAQAAVMKcOXM0ZcoUTZo0iRtbAwAA/EJxDywAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANga98ACAAAAAACArTEDCwAAAAAAALZGAwsAAAAAAAC25op0AqfC4/Fo7969qlWrlizLinQ6AAAAAAAAKIcxRseOHVPDhg3lcFR+PlVUNrD27t2rJk2aRDoNAAAAAAAAVMKuXbvUuHHjSj8vKhtYtWrVklRcdEpKSoSzAQAAAAAAQHmys7PVpEkTX0+nsqKygeX92mBKSgoNLAAAAAAAgChxqreC4ibuAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALC1qPwrhAAAAAAAIPyMMSoqKpLb7Y50KrAJl8slp9N5yn9dMOTXqdG1AwAAAACAqGeM0dGjR/XTTz+pqKgo0unAZpxOp+rVq6fU1NQaa2TRwAIAAAAAAOXav3+/jh49qpSUFKWkpMjlctX4jBvYnzFGbrdb2dnZ2rdvn3Jzc9WgQYMaeS0aWAAAAAAAIKiioiJlZWUpPT1ddevWjXQ6sKFatWopLi5OmZmZqlevnpxOZ7W/BjdxBwAAAAAAQRUWFsoYo6SkpEinAhtLSkqSMUaFhYU1sn4aWAAAAAAAoEJ8ZRDlqen9gwYWAAAAAAAAbI0GFgAAAAAAAAKaPHmyzjrrrEinQQMLAAAAAAD8cs2ZM0eWZQX9t2rVqkinWKGNGzfqT3/6k3bs2BHpVGoMf4UQAAAAAAD84j3wwANq3rx5mXirVq0ikE3lbNy4Uffff7/69+9vi9lSNYEGFgAAAAAAOGWLNkQ6A2lwp6qvY+jQoerevXvVV4QawVcIAQAAAAAAyjFjxgw5HA4tXbrUL3799dcrNjZW3377rSRp+fLlsixLb7zxhu69917Vr19fSUlJGj58uHbt2lVmvatXr9aQIUOUmpqqxMRE9evXT59//nmZ5fbs2aOpU6eqYcOGiouLU/PmzXXjjTeqoKBAc+bM0ZgxYyRJAwYM8H31cfny5b7nf/TRR+rbt6+SkpJUq1YtXXbZZfruu+/KvM4777yjTp06KT4+Xp06ddLbb79dlbetWjEDCwAAAAAA/OJlZWUpMzPTL2ZZlurUqaPf//73ev/99zV16lStX79etWrV0ieffKIXX3xRDz74oLp06eL3vIceekiWZemee+7RwYMH9eSTT+qiiy7SN998o4SEBEnSp59+qqFDh+rcc8/1Nchmz56tgQMHasWKFerZs6ckae/everZs6eOHj2q66+/Xu3atdOePXu0cOFCnThxQhdeeKGmTZump59+Wvfee6/at28vSb7/vvrqq5o0aZIuueQSPfLIIzpx4oT+/ve/64ILLtDatWt9XzlctGiRRo0apQ4dOmjWrFk6dOiQpkyZosaNG9fk2x4yyxhjIp1EZWVnZys1NVVZWVlKSUmJdDoAAAAAAJy28vLytH37djVv3lzx8fFlHo/2rxDOmTNHU6ZMCfhYXFyc8vLyJEkbNmzQueeeq4kTJ+rRRx9Vp06d1KBBA61cuVIuV/H8oOXLl2vAgAFq1KiRNm3apFq1akmSFixYoKuuukpPPfWUpk2bJmOM2rZtqxYtWuijjz6SZVmSpNzcXHXs2FGtWrXSokWLJEmTJk3S3LlztXr16jJfcTTGyLIsLVy4UGPGjNGyZcvUv39/3+M5OTlq0qSJxowZoxdeeMEXP3DggNq2baurrrrKF+/WrZsOHDigTZs2KTU1VZK0ePFiDR48WM2aNavwBvEV7SdV7eUwAwsAAAAAAPzi/e1vf1ObNm38Yk6n0/f/nTp10v3336/p06dr3bp1yszM1KJFi3zNq9ImTpzoa15J0ujRo9WgQQN9+OGHmjZtmr755htt3bpVv//973Xo0CG/5w4aNEivvvqqPB6PpOKv9Q0bNizg/bm8ja9gFi9erKNHj+rqq6/2m13mdDrVq1cvLVu2TJK0b98+ffPNN/rd737na15J0sUXX6wOHTro+PHj5b5OONDAAgAAAAAAv3g9e/as8Cbud911l15//XWtWbNGM2fOVIcOHQIu17p1a7+fLctSq1atfLOYtm7dKql4dlUwWVlZKigoUHZ2tjp1OrUpZt7XGThwYMDHvTOhdu7cGTBvSWrbtq2+/vrrU3r96kQDCwAAAEC1s8NXiryq46+TAYAkbdu2zdcUWr9+/Smvxzu76tFHH1XXrl0DLpOcnKzDhw+f8muUfp1XX31V9evXL/N4oNljdhU9mQIAAAAAAESIx+PR5MmTlZKSottvv10zZ87U6NGjNXLkyDLLeptcXsYY/fDDD+rcubMkqWXLlpKKZ0BddNFFQV8zPT1dKSkp2rCh/N8KBPsqofd16tWrV+7rNGvWLGDekvT999+X+9rhQgMLAAAAiALMaAKAyHr88cf1xRdf6L333tNll12m5cuX68Ybb9SFF16ounXr+i37yiuvaPr06b77YC1cuFD79u3TPffcI0k699xz1bJlSz322GO65pprlJyc7Pf8n376Senp6XI4HLryyis1d+5cZWRkBL2Je1JSkiTp6NGjfo9fcsklSklJ0cyZMzVgwADFxMQEfJ0GDRqoa9euevnll/3ug7V48WJt3LjR1+CKJBpYAAAAAADgF++jjz7S5s2by8T79Omj/Px8/eEPf9DkyZM1bNgwScV/vbBr16666aabNH/+fL/npKWl6YILLtCUKVN04MABPfnkk2rVqpX+3//7f5Ikh8Ohl156SUOHDlXHjh01ZcoUNWrUSHv27NGyZcuUkpKi999/X5I0c+ZMLVq0SP369dP111+v9u3ba9++fVqwYIH++9//qnbt2urataucTqceeeQRZWVlKS4uTgMHDlS9evX097//Xddee63OOeccjRs3Tunp6frf//6nf//73zr//PP17LPPSpJmzZqlyy67TBdccIGuu+46HT58WM8884w6duyonJycmnzrQ0IDCwAAAAAA/OL98Y9/DBh/6aWX9Pzzz6tu3bp68sknffHWrVtr1qxZuu222zR//nxdddVVvsfuvfderVu3TrNmzdKxY8c0aNAgPffcc0pMTPQt079/f61cuVIPPvignn32WeXk5Kh+/frq1auXfv3rX/uWa9SokVavXq0//OEPmjdvnrKzs9WoUSMNHTrUt7769evrH//4h2bNmqWpU6eqqKhIy5YtU7169XTNNdeoYcOGevjhh/Xoo48qPz9fjRo1Ut++fTVlyhTf6wwZMkQLFizQ73//e02fPl0tW7bU7Nmz9e6772r58uXV9C6fOssYYyKdRGVlZ2crNTVVWVlZvjvmAwAAAKezaPsKYbTlCyC4vLw8bd++Xc2bN1d8fHyk07G15cuXa8CAAVqwYIFGjx4d6XTCqqL9pKq9HEd1JAkAAAAAAADUFBpYAAAAAAAAsDUaWAAAAAAAALA1buIOAAAAAABQDfr3768ovNV4VGAGFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAA+MWaM2eOLMtSfHy89uzZU+bx/v37q1OnThHIDKW5Ip0AAAAAAACIYh9/HOkMpCFDqryK/Px8Pfzww3rmmWeqISFUN2ZgAQAAAACAX7yuXbvqxRdf1N69eyOdCgKggQUAAAAAAH7x7r33XhUVFenhhx8udzm3260HH3xQLVu2VFxcnM466yzde++9ys/P9y1zxx13qE6dOjLG+GK33nqrLMvS008/7YsdOHBAlmXp73//e/UXdJrhK4QAAAAAftEWbYh0BiUGc5sdIGKaN2+uiRMn6sUXX9Tvfvc7NWzYMOByv/rVr/Tyyy9r9OjRuvPOO7V69WrNmjVLmzZt0ttvvy1J6tu3r5544gl99913vvtnrVixQg6HQytWrNC0adN8MUm68MILw1BhdGMGFgAAAAAAgKT77rtPbrdbjzzySMDHv/32W7388sv61a9+pQULFuimm27Syy+/rN/+9rd65513tGzZMknSBRdcIKmkQZWVlaX169dr1KhRvpj38bS0NHXo0KGGK4t+NLAAAAAAAAAktWjRQtdee61eeOEF7du3r8zjH374oaTirwiWduedd0qS/v3vf0uS0tPT1a5dO/3nP/+RJH3++edyOp266667dODAAW3dulVScQPrggsukGVZNVbT6YIGFgAAAAAAwM9+//vfy+12B7wX1s6dO+VwONSqVSu/eP369VW7dm3t3LnTF+vbt69vttWKFSvUvXt3de/eXWlpaVqxYoWys7P17bffqm/fvjVb0GmCBhYAAAAAAMDPWrRooQkTJgSdhSUppBlTF1xwgfbs2aNt27ZpxYoV6tu3ryzL0gUXXKAVK1boiy++kMfjoYEVIhpYAAAAAAAApXhnYZ18L6xmzZrJ4/H4vgLodeDAAR09elTNmjXzxbyNqcWLF+vLL7/0/XzhhRdqxYoVWrFihZKSknTuuefWcDWnBxpYAAAAAAAApbRs2VITJkzQ888/r/379/vil156qSTpySef9Fv+8ccflyRddtllvljz5s3VqFEjPfHEEyosLNT5558vqbix9eOPP2rhwoU677zz5HK5aria0wMNLAAAAAAAgJPcd999Kiws1Pfff++LdenSRZMmTdILL7ygsWPH6rnnntPkyZP1l7/8RVdeeaUGDBjgt46+ffvq+++/V6dOnXTGGWdIks455xwlJSVpy5YtfH2wEmhgAQAAAAAAnKRVq1aaMGFCmfhLL72k+++/X19++aVuv/12ffrpp5o+fbpef/31Mst6G1QXXHCBL+ZyudS7d2+/x1ExyxhjIp1EZWVnZys1NVVZWVlKSUmJdDoAAABAjVu0IdIZlBjcqeJloinfaMoViIS8vDxt375dzZs3V3x8fKTTgU1VtJ9UtZfDDCwAAAAAAADYWpUbWF9++aVuueUWdezYUUlJSWratKmuuuoqbdmyxW+5yZMny7KsMv/atWtX1RQAAAAAAABwGqvyre4feeQRff755xozZow6d+6s/fv369lnn9U555yjVatWqVOnkjmwcXFxeumll/yen5qaWtUUAAAAAAAAcBqrcgPrjjvu0GuvvabY2FhfbOzYsTr77LP18MMPa+7cuSUv5nIFvAEaAAAAEAnc+wgAgOhQ5a8Q9unTx695JUmtW7dWx44dtWnTpjLLFxUVKTs7u6ovCwAAAAAAgF+IGrmJuzFGBw4cUN26df3iJ06cUEpKilJTU5WWlqabb75ZOTk5NZECAAAAAAAAThNV/gphIPPmzdOePXv0wAMP+GINGjTQ3XffrXPOOUcej0cff/yxnnvuOX377bdavny5XK7gqeTn5ys/P9/3s3cGl9vtltvtliQ5HA45HA55PB55PB7fst54UVGRjDEVxp1OpyzL8q23dFwqnkEWStzlcskY4xe3LEtOp7NMjsHi1ERN1ERN1ERN1ERN1FSzNZmS1UhWce4y/rkHi1uO4pr845Ysh1PGeHTSygPHLYcsyyFjPHK7y6/JeEot7ymSZEqtp7gm4/HfTjVVk9td8XYKWmuZ3MNTU3n7XkmaFW+nmq6p9FCLtvFU2ulyjKCm4rjb7S45FpVab+n87RSvDLvlHs01ScX7R+leTel97+T9r7KqvYG1efNm3Xzzzerdu7cmTZrki8+aNctvuXHjxqlNmza67777tHDhQo0bNy7oOmfNmqX777+/THzt2rVKSkqSJKWnp6tly5bavn27fvrpJ98yjRs3VuPGjbVlyxZlZWX54i1atFC9evW0YcMG5ebm+uLt2rVT7dq1tXbtWr9B3LlzZ8XGxiojI8Mvh+7du6ugoEDr1q3zxZxOp3r06KGsrCxt3rzZF09ISFCXLl2UmZmpbdu2+eKpqalq37699u7dq927d/vi1ERN1ERN1ERN1ERN1FSzNRUcLakppm5nWc5YFRzwryn2zO4yRQUqzCypybKciq3fQ6YgS4WHS2qyXAmKTe8iT26m3FklNTniUhWT1l5FOXtVlFNSkzMhXa7aLVWUtV0ZGeXXVHBMcqW2kDOxngoPbZBxl9QUk9ZOVlxtFR5cK2NqvqaMExVvp6Ks7SrKLanJmdxYrlqN5T66RZ78ku0Ujpoq2vcKjoW+nWq6powTJTVF23g6HY8R1FRSU3x8vKTiplZeXp4v7nA4lJiYKLfb7TfxxOl0KiEhQYWFhSooKPDFXS6X4uPjlZ+f79fQiI2NVWxsrPLy8vxyjIuLU0xMjHJzc/2aePHx8XK5XDpx4oRfMyUhIUEOh0PHjx/3qykpKUkej8fvfbEsS0lJSdRUTTVJUmFhoTZsKLnBZOl9r6q3k7JMVVt7pezfv1/nn3++CgsLtWrVKjVs2LDc5XNzc5WcnKwpU6aU+euEpQWagdWkSRMdOnRIKSkpkuzTmfY6nbrt1ERN1ERN1ERN1ERNp2tNSzeWSjLCM7AGtS+/pqUbSy0f4RlYgzpUvJ0+WW+fGVgXdyx/3yvZDyI/A2tQh5JwtI2n0k6XYwQ1Fcfz8vL0v//9Ty1atPA1KkpjthI1ScW9m23btqlp06a+hmfpfS87O1t16tRRVlaWr5dTGdU2AysrK0tDhw7V0aNHtWLFigqbV1JxF7FOnTo6fPhwucvFxcUFHCQul6vMVw+9A/Zk3gEYajzYVxorE7csK2A8WI6VjVMTNQWLUxM1SdQULMfKxqmJmiRqCpZjZeN2rMkKdEdYK8glcoC4ZVlB4g4FWnl5cZer/JpKP81yBK7JcoSee7B4KDWV3ozBtkfQWoPmXrM1lbfvnZxmpbdfNdYUaEhFy3iqapya7FuTy+UqPjZIvv+ezG7xyrBb7tFeU6BeTaBYZVVLAysvL0/Dhg3Tli1btGTJEnXo0KHiJ0k6duyYMjMzlZ6eXh1pAAAAAAAA4DRU5b9CWFRUpLFjx2rlypVasGCBevfuXWaZvLw8HTt2rEz8wQcflDFGQ4YMqWoaAAAAAAAAtmNZlv70pz9FOo2oV+UZWHfeeafee+89DRs2TIcPH9bcuXP9Hp8wYYL279+vbt266eqrr1a7du0kSZ988ok+/PBDDRkyRFdccUVV0wAAAAAAAKiUUL+ut2zZMvXv379mk0G5qtzA+uabbyRJ77//vt5///0yj0+YMEG1a9fW5ZdfrsWLF+vll19WUVGRWrVqpZkzZ+q3v/1twO/yAgAAAACAKPDDD5HOQGrV6pSe9uqrr/r9/Morr2jx4sVl4u3btz/l1FA9qtzAWr58eYXL1K5du8zGBwAAAAAAiKQJEyb4/bxq1SotXry4TByRx9QnAAAAAACAII4fP64777xTTZo0UVxcnNq2bavHHntMxhi/5fLz8/Wb3/xG6enpqlWrloYPH67du3eXWd/OnTt10003qW3btkpISFCdOnU0ZswY7dixw7fMtm3bZFmWnnjiiTLP/+KLL2RZlv71r39Ve612RgMLAAAAAAAgAGOMhg8frieeeEJDhgzR448/rrZt2+quu+7SHXfc4bfsr371Kz355JMaPHiwHn74YcXExOiyyy4rs84vv/xSX3zxhcaNG6enn35aN9xwg5YuXar+/fvrxIkTkqQWLVro/PPP17x588o8f968eapVq9Yv7n7iVf4KIQAAAAAAwOnovffe06effqo///nPuu+++yRJN998s8aMGaOnnnpKt9xyi1q2bKlvv/1Wc+fO1U033aS//e1vvuXGjx+vdevW+a3zsssu0+jRo/1iw4YNU+/evfXmm2/q2muvlSRNnDhRv/71r7V582bfH8QrLCzU/PnzNXLkSCUmJtZ0+bbCDCwAAAAAAIAAPvzwQzmdTk2bNs0vfuedd8oYo48++si3nKQyy91+++1l1pmQkOD7/8LCQh06dEitWrVS7dq19fXXX/seu+qqqxQfH+83C+uTTz5RZmbmL/IeXTSwAAAAAAAAAti5c6caNmyoWrVq+cW9f5Vw586dvv86HA61bNnSb7m2bduWWWdubq7++Mc/+u6pVbduXaWnp+vo0aPKysryLVe7dm0NGzZMr732mi82b948NWrUSAMHDqy2GqMFDSwAAAAAAIAwufXWW/XQQw/pqquu0vz587Vo0SItXrxYderUkcfj8Vt24sSJ2rZtm7744gsdO3ZM7733nq6++mo5HL+8dg73wAIAAAAAAAigWbNmWrJkiY4dO+Y3C2vz5s2+x73/9Xg8+vHHH/1mXX3//fdl1rlw4UJNmjRJf/3rX32xvLw8HT16tMyyQ4YMUXp6uubNm6devXrpxIkTvntk/dLQwAIAAACAKLJoQ6QzKDG4U6QzAGrWpZdeqhdeeEHPPvuspk+f7os/8cQTsixLQ4cOlSQNHTpU9957r55++mnfTdwl6cknnyyzTqfTKWOMX+yZZ55RUVFRmWVdLpeuvvpqvfbaa9q0aZPOPvtsde7cuZqqiy40sAAAAAAAAAIYNmyYBgwYoPvuu087duxQly5dtGjRIr377ru6/fbbffe86tq1q66++mo999xzysrKUp8+fbR06VL98MMPZdZ5+eWX69VXX1Vqaqo6dOiglStXasmSJapTp07AHCZOnKinn35ay5Yt0yOPPFKj9doZDSwAAAAAAIAAHA6H3nvvPf3xj3/UG2+8odmzZ+uss87So48+qjvvvNNv2X/+85++r/u98847GjhwoP7973+rSZMmfss99dRTcjqdmjdvnvLy8nT++edryZIluuSSSwLmcO6556pjx47atGmTxo8fX2O12p1lTp63FgWys7OVmpqqrKwspaSkRDodAAAARKlo+ipWNOUqRVe+0ZSrFH35Ivrl5eVp+/btat68ueLj4yOdzi9St27dlJaWpqVLl0Y6laAq2k+q2sv55d22HgAAAAAAIEpkZGTom2++0cSJEyOdSkTxFUIAAAAAAACb2bBhg7766iv99a9/VYMGDTR27NhIpxRRzMACAAAAAACwmYULF2rKlCkqLCzUv/71r1/81zdpYAEAAAAAANjMn/70J3k8Hm3atEn9+vWLdDoRRwMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAFTIGBPpFGBjNb1/0MACAAAAAABBOZ1OSVJhYWGEM4GdefcP7/5S3WhgAQAAAACAoGJiYhQXF6esrCxmYSEgY4yysrIUFxenmJiYGnkNV42sFQAAAAAAnDbq1q2rPXv2aPfu3UpNTVVMTIwsy4p0WogwY4wKCwuVlZWlnJwcNWrUqMZeiwYWAAAAAAAoV0pKiiQpMzNTe/bsiXA2sJu4uDg1atTIt5/UBBpYAAAAAACgQikpKUpJSVFhYaGKiooinQ5swul01tjXBkujgQUAAAAAAEIWExMTloYFUBo3cQcAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK25Ip0AAAAAAOD0tGhDpDMoMbhTpDMAUBXMwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK25Ip0AAAAATh+LNkQ6gxKDO0U6AwAAUF2YgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW3NFOgEAAAAAAOxg0YZIZ1BicKdIZwDYCzOwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGtVbmB9+eWXuuWWW9SxY0clJSWpadOmuuqqq7Rly5Yyy27atElDhgxRcnKy0tLSdO211+qnn36qagoAAAAAAAA4jbmquoJHHnlEn3/+ucaMGaPOnTtr//79evbZZ3XOOedo1apV6tSpkyRp9+7duvDCC5WamqqZM2cqJydHjz32mNavX681a9YoNja2ysUAAAAAAADg9FPlBtYdd9yh1157za8BNXbsWJ199tl6+OGHNXfuXEnSzJkzdfz4cX311Vdq2rSpJKlnz566+OKLNWfOHF1//fVVTQUAAAAAAACnoSp/hbBPnz5lZk+1bt1aHTt21KZNm3yxN998U5dffrmveSVJF110kdq0aaP58+dXNQ0AAAAAAACcpmrkJu7GGB04cEB169aVJO3Zs0cHDx5U9+7dyyzbs2dPrV27tibSAAAAAAAAwGmgyl8hDGTevHnas2ePHnjgAUnSvn37JEkNGjQos2yDBg10+PBh5efnKy4uLuD68vPzlZ+f7/s5OztbkuR2u+V2uyVJDodDDodDHo9HHo/Ht6w3XlRUJGNMhXGn0ynLsnzrLR2XpKKiopDiLpdLxhi/uGVZcjqdZXIMFqcmaqImaqImaqImaoq2moxx/vw//nHLUVyTf9yS5XDKGI9kPBXHLYcsyxE87imSVJK7x1NxTf4vGzj3YPHqrsntLn87GU/wWmUV12Q8/tuppmpyuyve90LdTuGqqbzxVJJm9ex7Vamp9FALNs6k8I+nYHFjyj9GFC8fuFa/cBiOEaEc94rHWXjHU7C42835iZpOr5pOrquyqr2BtXnzZt18883q3bu3Jk2aJEnKzc2VpIANqvj4eN8ywRpYs2bN0v33318mvnbtWiUlJUmS0tPT1bJlS23fvt3vLxs2btxYjRs31pYtW5SVleWLt2jRQvXq1dOGDRt8+UlSu3btVLt2ba1du9ZvY3fu3FmxsbHKyMjwy6F79+4qKCjQunXrfDGn06kePXooKytLmzdv9sUTEhLUpUsXZWZmatu2bb54amqq2rdvr71792r37t2+ODVREzVREzVREzVRU7TVpMTuMkUFKswsqcmynIqt30OmIEuFh0tqslwJik3vIk9uptxZJTU54lIVk9ZeRTl7VZRTUpMzIV2u2i1VlLVdRbklNTmTG8tVq7HcR7fIk19SU2b9imsqOFpSU0zdzrKcsSo44F9T7JnhqSkjo/ztVHBMcqW2kDOxngoPbZBxl9QUk9ZOVlxtFR5cK2NqvqaMExXve6Fup3DUVNF4KjgW+naq6ZoyTpTUFOwYoYTwj6dgNWU1Lf8YEanxFKimUI57BcfCP56C1ZRxgvMTNZ1eNXknI50qy5RujVXR/v37df7556uwsFCrVq1Sw4YNJUkZGRnq0aOHXnnlFV177bV+z7n77rv16KOPKi8vr1IzsJo0aaJDhw4pJSVFEh1PaqImaqImaqImaqImO9S0dJN9ZmBd3KnimpZuLP2ykZ2BNah9+dtp6cbgtYZ7xsigDhXve5+st88MrIs7lj+eSvaDyM/AGtShJBxsnH262T4zsAafXf4xYtF6+8zAGtS+4uNe8TizxwysQR04P1HT6VVTdna26tSpo6ysLF8vpzKqbQZWVlaWhg4dqqNHj2rFihW+5pVU8tVB71cJS9u3b5/S0tKCNq+k4plbgR53uVxyufxL8L5pJ/Nu2FDjJ6/3VOKWZQWMB8uxsnFqoqZgcWqiJomaguVY2Tg1UZNETcFyDBS3LO//BK4pcNwhWWVzrHTc4Z+7t+zyagqwmoA5BotXZ00uV/nbqfTTTq61JB567sHiodRUerMH28dC3U4Vx6unpvLG08lpVnXfqzgePPdAQy3YMSKc4ylY3Dvmgx0jKrP9arqmUI57/uMsPOMpWDyUccb5iZqCxe1YU7D8Q1UtDay8vDwNGzZMW7Zs0ZIlS9ShQwe/xxs1aqT09PSyU8wlrVmzRl27dq2ONAAAAAAAAHAaqvJfISwqKtLYsWO1cuVKLViwQL179w643KhRo/TBBx9o165dvtjSpUu1ZcsWjRkzpqppAAAAAAAA4DRV5RlYd955p9577z0NGzZMhw8f1ty5c/0enzBhgiTp3nvv1YIFCzRgwADddtttysnJ0aOPPqqzzz5bU6ZMqWoaAAAAAAD8YizaEOkMSgzuFOkM8EtQ5QbWN998I0l6//339f7775d53NvAatKkiT777DPdcccd+t3vfqfY2Fhddtll+utf/1ru/a8AAAAAAADwy1blBtby5ctDXrZjx4765JNPqvqSAAAAAAAA+AWp8j2wAAAAAAAAgJpEAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC25op0AgAAAAAA4PS2aEOkMygxuFOkM8CpYAYWAAAAAAAAbI0GFgAAAAAAAGyNrxACAADYHF+7AAAAv3TMwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK25Ip0AAABA2P3wQ6QzKNGqVaQzAAAApSzaEOkMSgzuFOkM7IMZWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1V6QTAAAAQPlaLnol0imU6DQx0hkAAIBfIGZgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWXJFOANFn0YZIZ1BicKdIZwAAAAAAAGoaM7AAAAAAAABga8zAAgAA1eOHHyKdQYlWrSKdAQAAAKoRM7AAAAAAAABga8zAsgnuKwUAAAAAABAYM7AAAAAAAABga8zAAgAAvzgrf4x0BiV6c7suAACACtHAwmmPr2cCAAAAABDd+AohAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGytWhpYOTk5mjFjhoYMGaK0tDRZlqU5c+aUWW7y5MmyLKvMv3bt2lVHGgAAAAAAADgNuapjJZmZmXrggQfUtGlTdenSRcuXLw+6bFxcnF566SW/WGpqanWkAQAAAAAAgNNQtTSwGjRooH379ql+/frKyMhQjx49gr+gy6UJEyZUx8sCAAAAAADgF6BavkIYFxen+vXrh7x8UVGRsrOzq+OlAQAAAAAAcJoL+03cT5w4oZSUFKWmpiotLU0333yzcnJywp0GAAAAAAAAokS1fIUwVA0aNNDdd9+tc845Rx6PRx9//LGee+45ffvtt1q+fLlcrsDp5OfnKz8/3/ezd/aW2+2W2+2WJDkcDjkcDnk8Hnk8Ht+y3nhRUZGMMRXGnU6nLMvyrbd0XCqePRZK3OVyyRjjF7csS06ns0yOlmVJcsoYj2RK4rIcsixH8LinSJIJIV5ck/H41ySrOHcZ/9yNKb+m4vX7ViLLESD3YPFqrimU7WQ8wWu1HMU1+cdrria32377XqB4tI8naqImaopQTcbIYVkq8nhKH7HlsKyAcefPf8zF7Sl9rC2OS1KRMSHFXQ5HcU2l4lZRUbk1Fb+3/uvxHcv9o8Xn0GqIFzNl4idvD6nsdvL8/HSHKV6DsfzXEjBuin9T6Sn98pIsU/yj56R1hBr37oPB9jHvdUSkz7mS5PFUPJ78XzZw7uG6jnC7yz9GFF/TVM/1XlVrcrsrPkaE+xq2oprKO+6VpBmea9jyaip9mA82zqTwj6dgcWPKPz/5f3ZQ2MZToHgo51zvZ4dwjqdg8dKfHQKNMyly4+nkmqSKryN85Uboc26wcRbo2sh4Ivs5t3RNbrfNrveqcA178nGissLawJo1a5bfz+PGjVObNm103333aeHChRo3blzQ591///1l4mvXrlVSUpIkKT09XS1bttT27dv1008/+ZZp3LixGjdurC1btigrK8sXb9GiherVq6cNGzYoNzfXF2/Xrp1q166ttWvX+m3szp07KzY2VhkZGX45dO/eXQUFBVq3bp0v5nQ61aNHD2VlZWnz5s2+eEJCgrp06aLMzExt27bNFy++iX17FeXsVVHO7pL1JKTLVbulirK2qyi3pCZncmO5ajWW++gWefJLanKltpAzsZ4KD22QcZfUFJPWTlZcbRUeXCtTahDH1O0syxmrggP+NRV1KL+mggMlNVmuBMWmd5EnN1PurJKaHHGpikmr+ZpC2U4Fx6TYM7vLFBWoMLOkJstyKrZ+D5mCLBUeDk9NGSfst++1b99ee/fu1e7dJTVF+3iiJmqipgjV5HKpce3a2pKZqaxSubeoU0f1kpO1Yf9+5RYWltRUr55qJyRo7Z49Kip1YdS5QQPFulzK2LXLv6YmTVTgdmvdvn0lNTkc6tGkibLy8rT54MGSmnJzy60p35OlvKKS9z3WkaxEVx3lFh1RgadkZni8M1Xxzto67s6U25TUlOCsozhnsnLc+1VkSmpKctVTjJWg7MI9MiqpqVZMAznkUlahf02pMU2Um5tb4XY6cWaiYtweNczMU06CS4dTY0tyzC/SmUfylZUco6zkGF88OdetOlkFOpIaq5yEkku+1JxC1c4p1E+145QX5/TF07IKVCvXrf114lXoKpmkX+9wnhIKPNpdL0HGsnTo530t2L6nRHuccyUps37F46ngaMXXRuG6jsjIKP8YUXCs+q73qlpTxomKjxHhvoYtr6aKjnsFx0LfTjVdU8aJkpqCHcuVEP7xFKymrKbln58iNZ4C1RTKObfgWPjHU7CaMk6Ufx0hRWY8BapJqvg6wjvOIvU5t3RN3nEW7NqoMDeyn3NL15RxwmbXe1W4hq3qraQsY076NWYVeW/iPnv2bE2ePLnC5XNzc5WcnKwpU6aU+euEXoFmYDVp0kSHDh1SSkqKpOj/DffSTfaZgTX47PJrWrQ+8r/p8dY0sF3F22npxuC1hvu3wYM62G/f+8XPGKEmaqKm6qtp+3b7zMBq2bLcmr74eKvsMgOr9yWtKtxO2595TZI9ZmA1v/UaScH3saWb7HHOlaSLO1U8npZuLP2ykZ2BNah9+ceI4msae8zAGtSh4mPEJ+vtMwPr4o7lH/dK9oPIz8Aa1KEkHGycfbrZPjOwBp9d/vnJ/7ODwjaeAsUHta/4nOv97GCHGVilPzsEGmdLNtpnBtYlnSu+jvCNMxvMwCo9zgJdGy3daJ8ZWIM62Ox6rwrXsNnZ2apTp46ysrJ8vZzKCOsMrEASEhJUp04dHT58OOgycXFxiouLKxN3uVxlvnbofdNO5t2wocaDfZ2xMnHLsgLGg+VoWQ7JqkTcETj34PEgm9vyj//8+SBoTYHWU+ncq6mmULaH38tYgWsKHK/+mkqna6d9r7LxaBhP1ERNwXKsbJyaKhH/+QTiDLBseXFXsLhlhRy3LMs//vP7F/yca8mvq+OLB86luuKBXzPw9igdd5S+tlVxUynQmgPFHVLZvtlJ66xM/ORcT/7ZtxkifM6VJO+mL288BdxUAXIMFq/Omlyu8o8RpZ9W1eu98uKh1FR6s1f62raGrmHLi1d03Ds5zUhelwc6nAc7RoRzPAWLl/fZoXj5yIynQPFQzrn+4yw84ylYPKRxFqHxFChe0fVCyOMsDDWdvLuefIzwphWpz7mlayqdqy2u9352KtewwfIPVdhv4n6yY8eOKTMzU+np6ZFOBQAAAAAAADYUtgZWXl6ejh07Vib+4IMPyhijIUOGhCsVAAAAAAAARJFq+wrhs88+q6NHj2rv3r2SpPfff993A7Bbb71VR44cUbdu3XT11VerXbt2kqRPPvlEH374oYYMGaIrrriiulIBAAAAAADAaaTaGliPPfaYdu7c6fv5rbfe0ltvvSVJmjBhgmrXrq3LL79cixcv1ssvv6yioiK1atVKM2fO1G9/+9uA36kEAAAAAAAAqq2BtWPHjgqXefXVV6vr5QAAAAAAAPALwbQnAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANiaK9IJAACA08PKHyOdQYnerSKdAQAAAKoTM7AAAAAAAABga8zAAmxk0YZIZ1BicKdIZwAAAAAAQDFmYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWXJFOAAAABLZoQ6QzKDG4U6QzAAAAwC8ZM7AAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrrkgnACB6LdoQ6QxKDO4U6QwAAAAAADWFGVgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDX+CiFOe7X2/BDpFEp0ahXpDAD8YKNjQiuOCQAAAEAomIEFAAAAAAAAW6OBBQAAAAAAAFvjK4QAgF+UlT9GOoMSvfkGIQAAABASZmABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1qqlgZWTk6MZM2ZoyJAhSktLk2VZmjNnTsBlN23apCFDhig5OVlpaWm69tpr9dNPP1VHGgAAAAAAADgNuapjJZmZmXrggQfUtGlTdenSRcuXLw+43O7du3XhhRcqNTVVM2fOVE5Ojh577DGtX79ea9asUWxsbHWkAwAAAAAAgNNItTSwGjRooH379ql+/frKyMhQjx49Ai43c+ZMHT9+XF999ZWaNm0qSerZs6cuvvhizZkzR9dff311pAMAAAAAAIDTSLV8hTAuLk7169evcLk333xTl19+ua95JUkXXXSR2rRpo/nz51dHKgAAAAAAADjNhO0m7nv27NHBgwfVvXv3Mo/17NlTa9euDVcqAAAAAAAAiCLV8hXCUOzbt09S8dcNT9agQQMdPnxY+fn5iouLK/N4fn6+8vPzfT9nZ2dLktxut9xutyTJ4XDI4XDI4/HI4/H4lvXGi4qKZIypMO50OmVZlm+9peOSVFRUFFLc5XLJGOMXtyxLTqezTI6WZUlyyhiPZErishyyLEfwuKdIkgkhXlyT8fjXJKs4dxn/3I0pv6bi9ftWIssRIPdg8WquKZTtZIxHkuX9yf8tsBw/b//qiHvkzyp+30vF3W53ufueFPp2Cha3HMXbyT9e+e0kVTyefE+ppn2vKjV5d4Vg4yzajxHUVH01BRrDkTpGSCq/Jk9kxlOguNtd8XYyxpQ57vnWU8n4z2sMKR7ofS8qKip336vKsby6azp53Ehlx5Pn56c7TPEajOW/loBxU/ybSk/pl5dkmeIfPSetI9S4d1wFOxZ4ryNq6vxUmesIj6fiY4T/y0bmnOutKdA4K5178SVN5M+5kuR2V3wsD/c1bEU1lXd+KkkzPNew5dVU+tQVbJxJ4R9PweLGlH8d4f/ZQWEbT4HioVxHFI+zyJ5zS4+z8q6NpMiNp5Nrkiq+3ivz2SGCx4jSu2uga1jjiezn3NI1ud2nz3X5yceJygpbAys3N1eSAjao4uPjfcsEenzWrFm6//77y8TXrl2rpKQkSVJ6erpatmyp7du3+/1Vw8aNG6tx48basmWLsrKyfPEWLVqoXr162rBhgy83SWrXrp1q166ttWvX+m3szp07KzY2VhkZGX45dO/eXQUFBVq3bp0v5nQ61aNHD2VlZWnz5s2+eEJCgrp06aLMzExt27bNF09NTVWtPTHKKzqqvKKSHGMdyUp01dEJ9yEVeHJK3i9nquKdtZVTeFBuU5J7grOO4pzJOla4V0Wm0BdPctVTjCNBWQW7ZFSy49WKaSCHXMoq3OVXU1GHfuXW5Nn5VUncilGtmIbKL8pRbtEhX9xlJSg5pl6N17Q290iF2ymr8LhSY5rII7eOFe7zxS05lBrbRG6Tp+Pug2VqKvAcD1hTvicrYE25RUcC1nTcnemrKSPjcLn7Xq09mSFvp2A1pcQ2UaEnN2BNldlOOrtXheOp4NjP60ltIWdiPRUe2iDjLqkpJq2drLjaKjy4VqbUCSSmbmdZzlgVHPAfT7FndpcpKlBhZsm+Z1lOxdbvIVOQpcLDJePJciUoNr2LPLmZcmdtU8aJn9+X1FS1b99ee/fu1e7du33LR/sxgpqqrybJhDyeavoYIancmjz/y/TFK3ssr+5jRMbxkguOYNsp3+Mqc9yTSo7lOe79ZY/lVoKyC/dUqaZA22nDhtxy972qHMuru6bc3NwKx9OJMxMV4/aoYWaechJcOpxa8odv4vOLdOaRfGUlxygrOcYXT851q05WgY6kxionoeSSLzWnULVzCvVT7TjlxTl98bSsAtXKdWt/nXgVukom6dc7nKeEAo9210uQsSwd+vmYEOwYocRTP5Z7OeJSFZPWXkU5e1WUU3KMcCaky1W7pYqytqsot2TfcyY3lqtWY7mPbpEnv2S7Ztav+BhRcLRmz0+VqSkjo/zjXsExe5xzJSnjRMXH8lC3Uzhqquj85L2mqa59ryo1ea9ppODnXCWEfzwFqymrafnXEZEaT4FqCuU6ouBY+MdTsJoyTpR/bSRFZjwFqkmq+HrPO87COZ6C1eQdZ8GuYQtzIzOeAtWUceL0uS73TkY6VZYp3RqrBt6buM+ePVuTJ08uE3/llVd07bXX+j3n7rvv1qOPPqq8vLyQZ2A1adJEhw4dUkpKiqTon4mwZsl22/w2uPclrcutaeUnWwPkWP2zlUKJ9xh0ll800PZYs2Rb0FrDPQOr50Utyt33Vi36sUZmIpxKvM+QNhWOp6UbvSuJ/G+DB3Xw1sNsJWoqv6aVn/wgu8zA6jOkdbk1rV78o9/yNTVbKZR4z4ual8nx5O20Zsl228zA6nVxy3L3vS8+3hpkPeGfgdX7klYVjqftz7wmyR4zsJrfeo2k4MeCpZvsMwPr4k4VHyN85zIp7LMrTq5pUPvyj3tLNwavNdwzRgZ1qPhY/sl6+8zAurhj+eenkv0g8jOwvNc0UvBx9ulm+8zAGnx2+dcRi9bbZwbWoPYVX0cUjzN7zMAa1KH8a6MlG+0zA+uSzhVf75X57BDBGVilx1mga9ilG+0zA2tQh9Pnujw7O1t16tRRVlaWr5dTGWGbgeX96qD3q4Sl7du3T2lpaQGbV1LxrK1Aj7lcLrlc/iV437STeTdsqPGT13sqccuyAsaD5Vj8VUIrQDzwrcqqK37yaxbnEbymQOsJnnvN1hTK9vB/bmVyrP6aSucVbN8LdTuVF6+umioaTyenajmC1OQIcqixQo9blhUk7pAsh07eFYLlHs3HCGqqnpqC7e8/Pxry8tV1jCivpsDH28gcI0LZrt7zR02dn8qLn5y79321+znXm0tF48lR+tpWkhXg14/B4g6pbN/spHVWJn5yrif/bHlLPIVjeZXjJ52HvJu+vGNEwE1VjeenysRdrvKPe6WfFslzriS/827wcRbadqo4Xj01lXccK3NNU8V9r+J48NwDnXaDns/COJ6Cxb1jPtj1QmW2X03XFMp1hP84C894ChYPaZxFaDwFild0XRfyOAtDTSfvricfI7xphXs8lcRLcimda7RflwfLP1Rhu4l7o0aNlJ6eXnaauaQ1a9aoa9eu4UoFAAAAAAAAUSRsDSxJGjVqlD744APt2lVy/4elS5dqy5YtGjNmTDhTAQAAAAAAQJSotq8QPvvsszp69Kj27t0rSXr//fd9NwC79dZblZqaqnvvvVcLFizQgAEDdNtttyknJ0ePPvqozj77bE2ZMqW6UgEAAAAAAMBppNoaWI899ph27tzp+/mtt97SW2+9JUmaMGGCUlNT1aRJE3322We644479Lvf/U6xsbG67LLL9Ne//jXo/a8AAAAAAADwy1ZtDawdO3aEtFzHjh31ySefVNfLAgAAAAAA4DQX1ntgAQAAAAAAAJVFAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC25op0AgCA6LZoQ6QzKDG4U6QzAAAAAFATaGABOGW19vwQ6RRKdGpV7sM0WQAAAAAgevEVQgAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANiaK9IJAADKWrQh0hmUGNwp0hkAAAAA+KVjBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbM0V6QQAIBxq7fkh0imU6NQq0hlUK95bAAAAADWNGVgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNVekEwAAlFVrzw+RTqFEp1aRzgAAAADALxwzsAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrYW1gLV++XJZlBfy3atWqcKYCAAAAAACAKOGKxItOmzZNPXr08Iu1atUqEqkAAAAAAADA5iLSwOrbt69Gjx4diZcGAAAAAABAlInYPbCOHTsmt9sdqZcHAAAAAABAlIhIA2vKlClKSUlRfHy8BgwYoIyMjEikAQAAAAAAgCgQ1q8QxsbGatSoUbr00ktVt25dbdy4UY899pj69u2rL774Qt26dQv4vPz8fOXn5/t+zs7OliS53W7fLC6HwyGHwyGPxyOPx+Nb1hsvKiqSMabCuNPplGVZZWaHOZ1OSVJRUVFIcZfLJWOMX9yyLDmdzjI5WpYlST/nYfzWY1kOGeORv+Ib31dHvJj/a3rfj2A1nbye4hyD5V6zNYWynYqfG7jWU8v91Gtyu93l7nsl+fqvJ1DuNV2TpArHU0mu1bPvVaUm774QbJwZ44nIeAoUd7vdFR4jKjfOaramisaZ93nhHk+B4t5cyzuWB97fI3OMkFTB+cnjt3y4xlOgeOn3Mtg51xgT9vEULPeioqKg59xg+0GkjhEnHwukstcRnp+f7jDFazCW/1oCxk3xbyo9pV9ekmWKf/SctI5Q46XHmVT2esEY58//4x+3HMU1+cctWQ5n8ft18v4eKG45SrZToLinSKXfY4+n4us9/5cNnHuweHXX5HaXfw1bfEkTuFZZxTUZz0nfcKihmtzu4Odcb+6hbqdw1VTedXlJmtWz71WlptKnrmDjTAr/eAoWN6b8z0/Fyweu1S8chmNEKJ8Ji8dZeMdTsLjbXf7nXCly4+nkmqTg59wy4yyM4ylYvPTuGui63HgiM54C1eR213w/orxjeXX2WKr6LbywNrD69OmjPn36+H4ePny4Ro8erc6dO2v69On6+OOPAz5v1qxZuv/++8vE165dq6SkJElSenq6WrZsqe3bt+unn37yLdO4cWM1btxYW7ZsUVZWli/eokUL1atXTxs2bFBubq4v3q5dO9WuXVtr167129idO3dWbGxsmdli3bt3V0FBgdatW+eLOZ1O9ejRQ1lZWdq8ebMvnpCQoC5duigzM1Pbtm3zxVNTUyXFKN+TpbyikhxjHclKdNVRbtERFXhyfPF4Z6rinbV13J0ptynJPcFZR3HOZOW496vIFPriSa56irESlF24R0YlO16tmAZyyKWswl1+NRUVtSi3ptLLO60Y1YppqALPceUWHfLFXVaCkmPq1XhNoWynrMLjSo1pIo/cOla4zxe35FBqbBO5TZ6Ouw+GpaaMjMPl7nuSQt5ONV2TpArHU1bh8ZC2Uzhqysg4XLyO1FS1b99ee/fu1e7du33L5xZZERlPgWpauzarwmNE6fWEazwFq6mi415W4fGIjKdANXn3g/KO5ZIJ+3gKVpOkcs9PWYWZvng4x1OgmkrvB8HOufkeV9jHU7CaNmzIDXrObd++vW3OuakxTZSbm1vhdcSJMxMV4/aoYWaechJcOpwaW5JjfpHOPJKvrOQYZSXH+OLJuW7VySrQkdRY5SSUXPKl5hSqdk6hfqodp7w4py+ellWgWrlu7a8Tr0JXyST9eofzlFDg0e56CTKWpUM/7wvBro2U2F2mqECFmSU1WZZTsfV7yBRkqfBwyXHPciUoNr2LPLmZcmeVbCdHXKpi0tqrKGevinJKjuXOhHS5ardUUdZ2FeWW7HvO5MZy1Wos99Et8uSXbNfM+hVf7xUcLTlGxNTtLMsZq4ID/jXFnhmemjIyyr+GLTgmuVJbyJlYT4WHNsi4S2qKSWsnK662Cg+ulTE1X1PGieDnXO8xItTtFI6aKrouLzgW+naq6ZoyTpTUFOyzhhLCP56C1ZTVtPzPT5EaT4FqCuUzYcGx8I+nYDVlnCj/c64UmfEUqCYp+DnXe4zwjrNwjqdgNXnHWbDP7oW5kRlPgWrKOFHz/YjyjuXV2WPxTkY6VZYp3RqLkKuvvlpvvfWWTpw44esglhZoBlaTJk106NAhpaSkSIr+GVhrlmy3zW+De1/SutyaVn6yNUCOkZmB1WPQWX7RQNtjzZJtQWsN94yRnhe1KHffW7XoR9vMwOozpE2F46n4vQ1ca0Xx6q6p50Utfo4FHmdrlmyzzQysnhe1qPAYsWrRD5V4D2q2pp4XNfeLnjzOvPuBHWZgefeD8o7lKz/5ocxrRuoY0WdI63LPT6sX/xjSexAo9+quqfR+EOycu2bJdtvMwOp1cctyf8v4xcdbg6wn/MeI3pe0qvA6Yvszr0myxwys5rdeIyn4NdDSTfaZgXVxp4qv95ZuLP2ykZ2BNah9+dewSzcGrzXcM0YGdaj4t/afrLfPDKyLO5Z/XV6yH0R+BtagDiXhYOPs0832mYE1+OzyPz8tWm+fGViD2lf8mbB4nNljBtagDuV/zl2y0T4zsC7pXPHMHt84s8EMrNLjLNB1+dKN9pmBNajD6TMDKzs7W3Xq1FFWVpavl1MZEfkrhCdr0qSJCgoKdPz48YBFxMXFKS4urkzc5XLJ5fIvwfumnSxQY6y8+MnrPZW4ZVkB48FyLP4qoRUgHvhWZdUVP/k1vV9pDFZToPUEz71mawple/g/tzI5Vn9NpfMKtu+Fup3Ki1dXTRWNp5Nzreq+V168otwrOhZ4cwj3eAoU9+Za3jGicuOsZmuqaJyVfl44x1Og+Mm5BjuORWI8Bcu9vPNT4P0gMseIUM5n3vNHOMeT/2uXxL3vq93Pud5cKrqOcJS+tpVkBfj1Y7C4QyrbNztpnZWJVzTOLG+JVpDxFzDukILt75WJO/zHk3fTl3e9F3BTBcgxWLw6a3K5ysZL5176aSfXWhIPPfdg8VBqKr3Zg4+z0LZTxfHqqam849jJaVZ136s4Hjz3QKfdoOezMI6nYHHvmA92vVCZ7VfTNYXymdB/nIVnPAWLhzTOIjSeAsWD5VjpcRaGmk7eXU8+RnjTCvd4KomX5FI615rsR1Q2fio9lmD5hypif4WwtG3btik+Pl7JycmRTgUAAAAAAAA2E9YGVunvTXp9++23eu+99zR48OCAXT0AAAAAAAD8soX1K4Rjx45VQkKC+vTpo3r16mnjxo164YUXlJiYqIcffjicqQAAAAAAACBKhLWBdeWVV2revHl6/PHHlZ2drfT0dI0cOVIzZsxQq1atwpkKAAAAAAAAokRYG1jTpk3TtGnTwvmSAAAAAAAAiHLcdAoAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAws</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -567,28 +582,33 @@
         </is>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45638.66666666666</v>
+        <v>45639.5</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
-        <v>11.83727661616683</v>
+        <v>9.478904369302354</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45638.66666666666</v>
+        <v>45639.5</v>
       </c>
       <c r="H4" t="n">
-        <v>6.720334966500044</v>
+        <v>4.406639723296744</v>
       </c>
       <c r="I4" t="n">
-        <v>1.778232474044581</v>
+        <v>-0.200051486837198</v>
       </c>
       <c r="J4" t="n">
-        <v>11.83727661616683</v>
+        <v>9.478904369302354</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACZbklEQVR4nOzdeXhU9dn/8c+ZmWwkJJFAEEgUEhQCCC6ABWVRFAGVtu4rSPVxaZX607ZWq0WsirY+blh3K1ahFrU+xVaURahU3FIDiEJDJVAgbEnIhIRsM3N+f4SZzCQzmQmZzBzg/bour5Y7Z87c91m+58yd75wYpmmaAgAAAAAAACzKFu8EAAAAAAAAgLbQwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAgTvr27SvDMAL+S0pK0nHHHafLL79cq1atikke1113nQzD0Lx582Lyfp3Fuz23bNkS71SOeN7jFQAAIFZoYAEAEGdnnHGGpk+frunTp2vy5MnyeDxauHChxo0bp8cffzze6VnC4dRki2Ujbd68eTIMQ9ddd12nvxcAAEA8OeKdAAAAR7sbbrghoAFRV1enm266SX/84x/1i1/8QhdccIFOPPHE+CV4mFi+fLkaGxvVp0+feKcCAACAKGMGFgAAFpOcnKzf//73Sk1Nldvt1l/+8pd4p3RYyM/P18CBA5WQkBDvVAAAABBlNLAAALCgtLQ0DRgwQJJafRXtww8/1AUXXKDs7GwlJiaqd+/euvzyy1VYWBhyfRUVFbr99tt1/PHH+56zdeutt6qiouKQ8rv//vtlGIbuv/9+bd26VdOmTVOvXr2UnJysE088Uffff79qa2tbva6xsVFvvPGGrr76ag0cOFDp6elKSUnRgAEDNHPmTJWWlgYsv2XLFhmGoddee02SNGPGjIBnht1///2+ZcN9de/tt9/WpEmT1KNHDyUmJqpPnz665ppr9O2337Za1vu+ffv2lWmaevHFF3XaaacpNTVVGRkZmjhxoj799NOA13i/zrd161ZJUr9+/QJyXblypW/ZZcuW6cILL1TPnj2VkJCgY445RieccIKuueYaffzxx5HsAvXt21czZsyQJL322msB7zV+/PiAZQ8cOKBHHnlEp556qrp27aouXbpo8ODBuvfee7Vv376I3i+Ul156ybdtMjMzNWXKFH322Wchl3e5XHr55Zc1fvx4devWTUlJSerXr59uueUWbdu2rd3v/69//UuXX365cnJylJiYqPT0dOXl5eniiy/WX//615Cvufrqq3XccccpKSlJ3bp103nnnaf3338/anmvXLnSty8aGxv16KOPavDgwUpJSVFWVpYuuugibdiwod31AgBwtOIrhAAAWFRVVZUkKSkpyRe777779OCDD8owDI0ePVrHHXecNmzYoIULF+qdd97Riy++qB/96EcB69m9e7fGjBmjTZs26ZhjjtEFF1wgj8ej+fPn64MPPtDgwYMPOceSkhKddtppcjgcGjt2rGpra7VixQrNnj1by5Yt07Jly5ScnByQy7XXXquMjAwVFBRo6NChqqmp0Zo1azR37ly9+eabWr16tfr37y+pqZE3ffp0/fOf/9R3332nM844w/czSTr55JPD5uhyuXT11Vdr4cKFSkpK0mmnnaY+ffqouLhY8+fP11/+8hf95S9/0aRJk4K+fsaMGVqwYIHGjBmjCy64QGvWrNHSpUv18ccf6x//+IdOP/10SVL//v01ffp0vf3226qpqdHFF1+stLQ033qOPfZYSU3NJm/jaeTIkTrrrLNUW1ur7du3680331T37t01duzYsHVdcskl+uyzz/TJJ58oPz9fZ555pu9nAwcO9P3/iooKTZgwQWvWrFF6errOPvtsJSQk6B//+IceeughLViwQB999JH69u0b9j1buuOOO/Tkk0/qjDPO0Pe//319/fXXWrx4sZYuXaqFCxfqhz/8YcDy+/fv19SpU7Vy5UqlpaXptNNOU48ePfT111/r+eef11tvvaWlS5fqlFNOiej9ly9frsmTJ6uxsVHDhg3TqFGj5Ha7tWPHDv3973+X2+3W97///YDXPPXUU7rjjjvk8Xh08skn6/TTT9euXbu0cuVKLVmyRLNnz9avf/3rqOXd2NioKVOmaPXq1Ro7dqwKCgr0xRdf6N1339WKFStUVFR0SNseAICjjgkAAOLi+OOPNyWZr776aqufrV271rTZbKYk8w9/+INpmqa5ePFiU5KZnJxsLlmyJGD5l19+2ZRkJiQkmOvXrw/42SWXXGJKMseMGWNWVlb64uXl5ebpp59uSgqZRyizZs3yve773/++eeDAAd/Ptm3bZp544ommJPOXv/xlwOuqqqrMv/71r2Z9fX1AvKGhwbz77rtNSeaUKVNavd/06dPD5ujdniUlJQHxe+65x5Rknn766ebmzZsDfvbWW2+ZdrvdPOaYY8x9+/b54iUlJb76jj/+ePPf//6372cul8v80Y9+ZEoyJ06cGHEeXv369TMlmatWrWr1s927d5tfffVVyBpbevXVV01J5vTp00Muc/nll/vqLysr88X3799vTp482ZRkjh49OuL3NE3Tt21SUlLM5cuXB/zst7/9rSnJzMjIMHfv3h3ws6uuusqUZF5wwQWtfvbEE0+YkswTTjjBdLlcEeVx1llnmZLMN954o9XPKisrzU8//TQg9sEHH5iGYZjdu3c3//GPfwT8bN26dWZOTo4pyVy5cmWH816xYoVvO51yyinmzp07fT+rra01zzvvPFOSeeONN0ZUKwAARzsaWAAAxEmwBlZlZaX597//3czPzzclmb179zarq6tN0zTNCRMmmJLMO+64I+j6LrjgAlOS+T//8z++2H//+1/TZrOZhmGY33zzTavXFBUVdaiBlZKSEvDB3Ou9994zJZnp6elmbW1txOvt3bu3abPZzKqqqoD4oTawysvLzZSUFDM5Odncvn170Nf9+Mc/NiWZc+fO9cX8G1iLFi1q9ZqdO3eaksykpCSzoaEhbB7+unTpYmZkZISsoz3CNbC2bt3q2/9r165t9fPt27ebycnJpiTzk08+ifh9vdvm9ttvD/rz4cOHm5LMhx56yBf79ttvTcMwzN69e7fav15TpkwxJZnvvfdeRHkMGjTIlGRWVFREtLy3Yfv2228H/fnChQtNSebFF1/c4by9DSzDMMw1a9a0es1nn31mSjLz8vIiyh0AgKMdz8ACACDO/J/rlJmZqfPPP1/fffed8vPz9f777ys1NVUul0uffPKJJAX8xUJ/119/vSRpxYoVvtjHH38sj8ejU089VYMGDWr1mpNPPllDhw495NwnTpzo+2qcvwsuuEBZWVmqqqrSV1991erna9eu1eOPP67bbrtNP/rRj3Tdddfpuuuuk8vlksfj0X/+859DzsnfihUrVFtbqzPOOCPkXyf0Pi9q9erVrX7mcDiCfrXw2GOP1THHHKP6+nqVl5e3K6eRI0fK6XRq2rRp+te//iWPx9Ou17eHd/+fcsopQfdznz59dN5550kKPG4iNX369KDxadOmSVLAc7/ef/99maapyZMnq2vXrkFf19a+CGbkyJGSpKuvvlr//Oc/5XK5Qi5bVlamL774QikpKbrwwgsjfv+O5n3cccdp2LBhreIFBQWSpB07doTMGQAANOMZWAAAxJn/c50SExOVnZ2t733ve5o0aZIcjqZLdXl5uerq6iQ1PRw8mPz8fEmBH4i3b9/e5mu8P1u3bt0h5d7Wevv27avy8nJfDpJUU1Oja6+9Vu+++26b6/U+/6ujNm/eLKnpWUmGYbS57N69e1vFevXqFfKvGqanp2vfvn2+/RKpZ599VhdccIFef/11vf766+ratatGjBihs88+W9dee62OO+64dq2vLd5joa39FOy4iVSo9Xrj/vveuy9eeeUVvfLKK22uN9i+CGbOnDlat26dFi9erMWLFyslJUWnnnqqxo8fr6uvvtrXJJKantdmmqZqa2sDnisX7v07mneo/Zmeni5Jqq+vb3OdAACgCQ0sAADi7IYbbgg5q+pIYJqm7//ffffdevfddzVw4EA98sgjGjFihLp3767ExERJ0ujRo/Xpp58GvKYjvLOb+vfvrzPOOKPNZf0ffO5ls0V/snpBQYH+/e9/a8mSJfroo4+0evVqrVq1Sh999JEeeOABvfLKK7rmmmui/r7x4L8fvfvi5JNPDjojyZ/3wfjhHHvssSosLNQ//vEPLVu2TJ988ok+//xzffLJJ3r44Yc1Z84c3XXXXQHvn5aWposvvjjiGjqad2ccQwAAHI1oYAEAcBjIyspSUlKS6uvrtXnz5qBfB/POFPH/qpz3/2/ZsiXkutv6WTglJSVh15uTk+OLLVy4UJL05z//OWgNmzZtOuRcgsnNzZUkDRgwQPPmzYvqujvC4XBoypQpmjJliqSmGWePP/64Zs+erZtuukk//OEPlZqa2uH38e5/77ERTLDjJlIlJSVB/xJksH3v3RdnnHGGnnnmmXa/VyiGYWj8+PG+r/HV1dVp3rx5+slPfqJ77rlHl1xyifLz833vbxiG/vCHP0TcWOqsvAEAQPvwKyEAAA4DDodDZ555piSFbMT84Q9/kCSdddZZvtjYsWNlGIa++uorbdy4sdVr1q5de8hfH5SkJUuWaM+ePa3i77//vsrLy9W1a1eddtppvnhFRYUk6fjjj2/1mg8//FBlZWVB38c7Q6utZxwFM2HCBCUmJmrlypVB8+wMh5Jrenq67r//fmVmZurAgQMqLi6OynuNHTtWNptNa9as0dq1a1v9fOfOnfrggw8kBR43kXr99dfbjHubSpI0efJkSdKiRYva/bXL9khOTtbNN9+soUOHyuPx+I7v3r17a+jQodq/f7+v5kjEKm8AANA2GlgAABwm7rzzTknSc889p+XLlwf8bN68eVq0aJESEhL005/+1Bc/7rjj9MMf/lAej0e33HJLwLOl9u3bpx//+Mcd+rpebW2tbrnlFtXW1vpipaWlvlxvvvlmJScn+37mfSbR3LlzA9bz73//WzfffHPI9/HO5Pnmm2/alV/Pnj112223qaamRhdeeKG+/vrrVsvU19dr0aJFQRt8h6KtXA8cOKDHH3886LOSVq1apcrKStnt9oCZS5G817fffhv058cdd5wuvfRSmaapm266KeCB8zU1NbrxxhtVV1en0aNHa/To0RG9p7/nnnsu4EHtkvTEE0/oiy++UNeuXX1/WECSTjnlFF188cXatm2bLrrooqAz/2pqajR//nzt3r07ovd/7LHH9N///rdVfOPGjb7ZfP7N0gcffFBS0x9OeO+991q9zjRNff7551qyZEmn5g0AANqPrxACAHCYmDx5su699149+OCDOvfcc3XGGWfouOOO08aNG/XVV1/Jbrfr+eef1+DBgwNe9/vf/15r167VypUr1a9fP40fP16maWrFihXKysrS1KlTtWjRokPKadq0afrb3/6mvLw8jRkzRnV1dfroo49UU1OjUaNGafbs2QHLz5o1S5dcconuu+8+LVy4UIMHD9aePXu0atUqjRkzRr179w76l9x+8IMfaPbs2Xr66ae1fv165ebmymazaerUqZo6dWqbOT7yyCPauXOnFixY4HuOUV5enhwOh7Zv3641a9aopqZGixcvDvocrPa6+OKLtWLFCl1zzTWaOHGijjnmGEnSz3/+c/Xs2VN33nmnfv7zn+ukk07SCSecoISEBG3ZskWfffaZJOlXv/qVevToEdF7fe9731Pv3r1VVFSkU089VSeddJISEhI0YMAA/fznP5fUtP83btyozz//XPn5+TrrrLPkcDj0j3/8Q3v37lW/fv00f/78Q6r1pptu0tlnn60xY8aoT58+Wr9+vb7++mvZ7Xb94Q9/aPUXKl999VVVVlZq8eLFGjBggIYNG6Z+/frJNE1t2bJFa9euVUNDgzZs2KCePXuGff8HH3xQP//5zzVw4EAVFBQoJSVFpaWlvr9IOG3aNJ166qm+5S+88EI99dRTuvPOOzV16lT1799fAwYMUEZGhvbu3au1a9dqz549uuuuuzRx4sROyxsAABwCEwAAxMXxxx9vSjJfffXVdr1u8eLF5pQpU8ysrCzT4XCYxx57rHnppZean3/+ecjXlJWVmbfddpuZk5NjJiYmmjk5OebNN99s7t2715w+fXq785g1a5YpyZw1a5a5efNm88orrzR79uxpJiYmmv379zd//etfmzU1NUFf+/HHH5sTJkwwu3fvbnbp0sUcMmSI+dBDD5n19fXmuHHjTEnmihUrWr3u3XffNc844wyza9eupmEYvvf38m7PkpKSoO/7/vvvmxdddJHZp08fMyEhwczMzDQLCgrMK664wlywYEFAviUlJaYk8/jjjw+5DUK9n9vtNufMmWMOHjzYTE5ONiX5ampsbDSff/5588orrzQHDhxoZmRkmCkpKWZ+fr558cUXm8uXLw/5fqF8/fXX5tSpU80ePXqYNpvNlGSOGzcuYJmamhpzzpw55sknn2x26dLFTE5ONgsKCsx77rnHrKioaPd7emsyTdN87rnnzJNPPtlMSUkx09PTzUmTJpmffPJJyNe63W5zwYIF5pQpU8yePXuaCQkJZlZWljlkyBBzxowZ5rvvvms2NDRElMcbb7xhzpgxwxwyZIjZrVs3MykpyTz++OPNyZMnm++++67p8XiCvu7rr782b7zxRvOEE04wk5OTzS5duph5eXnmeeedZz799NPmjh07Opz3ihUrgu6LUNsRAAC0zTDNKP2ZHwAAcNS4//77NXv2bM2aNUv3339/vNMBAADAEY5nYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJ4BhYAAAAAAAAsjRlYAAAAAAAAsDQaWAAAAAAAALA0R7wT8PJ4PCotLVXXrl1lGEa80wEAAAAAAECUmKap/fv3q3fv3rLZ2j+fyjINrNLSUuXm5sY7DQAAAAAAAHSSbdu2KScnp92vs0wDq2vXrpKaCklPT49zNgAAAAAAAIiWqqoq5ebm+vo/7WWZBpb3a4Pp6ek0sAAAAAAAAI5Ah/rYKB7iDgAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLs8xfIQQAAAAAANZmmqbcbrdcLle8U4FFOBwO2e32Q/7rghG/T6euHQAAAAAAHPZM01RlZaX27t0rt9sd73RgMXa7XdnZ2crIyOi0RhYNLAAAAAAA0KZdu3apsrJS6enpSk9Pl8Ph6PQZN7A+0zTlcrlUVVWlnTt3qra2Vr169eqU96KBBQAAAAAAQnK73XI6nerRo4e6d+8e73RgQV27dlVSUpLKysqUnZ0tu90e9ffgIe4AAAAAACCkxsZGmaap1NTUeKcCC0tNTZVpmmpsbOyU9dPAAgAAAAAAYfGVQbSls48PGlgAAAAAAACwNBpYAAAAAAAACOq6665T3759450GDSwAAAAAAHD0mjdvngzDCPnfZ599Fu8Uw/r22291//33a8uWLfFOpdPwVwgBAAAAAMBR74EHHlC/fv1axfv37x+HbNrn22+/1ezZszV+/HhLzJbqDFFpYG3atEn33Xef/vnPf6qiokLHHXecrrrqKv3sZz9Tly5dovEWAAAAAADAgpasj3cG0sQhHV/H5MmTNXz48I6vCJ2iw18h3LZtm0aOHKnPPvtMt956q5588kmNGjVKs2bN0pVXXhmNHAEAAAAAAOJm1qxZstlsWr58eUD8xhtvVGJiotauXStJWrlypQzD0J///Gfdc889OvbYY5WamqqpU6dq27Ztrdb7+eefa9KkScrIyFCXLl00btw4ffLJJ62W27Fjh66//nr17t1bSUlJ6tevn2655RY1NDRo3rx5uvTSSyVJZ511lu+rjytXrvS9fvHixRozZoxSU1PVtWtXnX/++frmm29avc///d//aciQIUpOTtaQIUP07rvvdmSzRVWHZ2C9/vrrqqys1D//+U8NHjxYUtMO9Hg8+uMf/6h9+/bpmGOO6XCiAAAAAAAAncXpdKqsrCwgZhiGsrKydO+99+q9997T9ddfr6+//lpdu3bVhx9+qJdeekm/+c1vNGzYsIDXPfTQQzIMQ3fddZf27NmjJ598Uuecc47WrFmjlJQUSdJHH32kyZMn67TTTvM1yF599VWdffbZWrVqlUaOHClJKi0t1ciRI1VZWakbb7xRAwcO1I4dO/T222/rwIEDGjt2rGbOnKmnn35a99xzjwoKCiTJ97+vv/66pk+frvPOO0+PPvqoDhw4oOeee05nnnmmioqKfF85XLJkiS6++GINGjRIc+bMUXl5uWbMmKGcnJzO3OwR63ADq6qqSpLUs2fPgHivXr1ks9mUmJjY0bcAAAAAAADoVOecc06rWFJSkurq6pSQkKA//vGPOu2003THHXfod7/7na6//noNHz5cv/zlL1u9rqKiQhs2bFDXrl0lSaeeeqouu+wyvfTSS5o5c6ZM09TNN9+ss846S4sXL5ZhGJKkm266SYMHD9a9996rJUuWSJLuvvtu7dq1S59//nnAVxwfeOABmaapzMxMjRkzRk8//bTOPfdcjR8/3rdMdXW1Zs6cqRtuuEEvvviiLz59+nQNGDBADz/8sC9+1113qWfPnvrnP/+pjIwMSdK4ceM0ceJEHX/88R3cuh3X4QbW+PHj9eijj+r666/X7NmzlZWVpdWrV+u5557TzJkzlZqaGo08AQAAAAAAOs3vf/97nXjiiQExu93u+/9DhgzR7Nmzdffdd2vdunUqKyvTkiVL5HC0bq1MmzbN17ySpEsuuUS9evXS+++/r5kzZ2rNmjXatGmT7r33XpWXlwe8dsKECXr99dfl8XgkNX2t78ILLwz6fC5v4yuUpUuXqrKyUldeeWXA7DK73a7TTz9dK1askCTt3LlTa9as0S9/+Utf80qSzj33XA0aNEg1NTVtvk8sdLiBNWnSJP3mN7/Rww8/rEWLFvniv/rVr/Tggw+GfF19fb3q6+t9//bO5HK5XHK5XJIkm80mm80mj8fj23H+cbfbLdM0w8btdrsMw/Ct1z8uSW63O6K4w+GQaZoBccMwZLfbW+UYKk5N1ERN1ERN1ERN1ERN1ERN1ERN1HQ41eRyuWSapu/9/fNoZkjqzHjb/FMyDCNojqHiXiNGjAhoEnmX93/Nz372M7355pv64osv9NBDD6mgoMD3c//19+/fPyDujW3ZskWmaaq4uFhS00yoUCorK9XQ0KCqqioNGTKkzZr8941pmr64933OPvvsoO+Rnp4u0zS1devWVnl71z9gwAB99dVXreIt8/H+27+vIzUfey2P1faKyl8h7Nu3r8aOHauLL75YWVlZ+vvf/66HH35Yxx57rG699dagr5kzZ45mz57dKl5UVOSbtdWjRw/l5+erpKREe/fu9S2Tk5OjnJwcFRcXy+l0+uJ5eXnKzs7W+vXrVVtb64sPHDhQmZmZKioqCjgphw4dqsTERBUWFgbkMHz4cDU0NGjdunW+mN1u14gRI+R0OrVx40ZfPCUlRcOGDVNZWZk2b97si2dkZKigoEClX32l7X459khLU35WlkrKy7W3urq5powM5WRmqnjPHjn9cs/LylJ2WprWl5aqtrGxuabsbGWmpKho2za5/Qa9ob16KdHhUGGLh8MNz81VQ05OdGoqLdX27dubazoS9hM1URM1URM1URM1URM1URM1URM1hawpOTlZ9fX1SklJUWNjoxoaGnzLu1xJcjgS5HK5AnJxOByy2x1qbGwMaNZ54w0NDQFNkISEBNls9lbxxMREGYYRMAlGavp6n2maamhoUE1NU3PEMAylpqbK7Xarrq7Ot6zNZlOXLl3kcrkC1uM/w6q2ttY308jhcPhq9m+8bN26VZs2bZIkrVmzxrd8UlKSEhISfOuur69XTU2NkpOT5XA4dODAAbndbnk8HtXU1Pi204MPPqihQ4f61p+cnCyPx6OGhgYZhqEDBw74fhZJTXV1daqrq/PtJ+/yL730knr37q3ExEQ1NDT43t/haNo/Xt68/WvyNk+9cf+agjW11q8P/LOU3mOvqKhIHWGYbbUfI/Dmm2/qRz/6kYqLiwMe7DVjxgwtXLhQ//3vf5WVldXqdcFmYOXm5qq8vFzp6emSDs/OdKv4pk3y+Od4ME+PxyOP37pthiGbYcjt8QT0mkPF7Qf/qoDL47+WprgkuVvsVrthSP378xsEaqImaqImaqImaqImaqImaqImampXTXV1dfrvf/+rfv36KSUlpdXMm6XfSPGegXXuYL81tHMG1muvvaYZM2boiy++CDoDy8vj8Wjs2LHavHmzZsyYoTlz5ujtt9/WRRdd5Ft+xYoVOvvss/XLX/5SDz/8sC/u8XiUk5OjoUOHavHixfryyy91+umn6/nnn9eNN94Ysi6Px6Nu3brprLPOCvoXAb05vvPOO7r00kv10Ucfafz48b74W2+9pcsvv1wffPCBJk6cGHIb7Nq1S71799Zdd92lOXPmBKx/8ODBqqmpUUlJSZvbsq6uTlu2bFFubq6Sk5N9ce+xt2/fPmVlZcnpdPr6Pu3R4QbW2LFj5Xa7W/2Zx3fffVcXXXSRli5dGvRBaC1VVVUpIyPjkAuxrP/8J94ZNOvfP94ZAAAAAAAOM3V1dSopKVG/fv0CGhNeS9YHeVGMTRxy6K+dN2+eZsyYoS+//DLoc6a8HnvsMf385z/XokWLdP7552vMmDH6z3/+o2+++Ubdu3eXJK1cuVJnnXWW+vTpE/AQ97feekuXXXaZnnzySf30pz+Vx+PRiSeeKJvNpq+++kppaWkB77V371716NFDUtPXDN94441WD3GX5Pu64AcffKDJkyfr3Xff1Q9+8APfz72ThU455RQtXbpUCQkJId/nlFNO0e7du7Vhwwbfc7CWLl3qe4j7li1b2tyO4Y6TjvZ9OvwVwt27d+uYY45pFfdOQevodxwBAAAAAAA62+LFiwO+Suk1evRo1dfX67777tN1112nCy+8UFJT4+vkk0/Wj3/8Yy1cuDDgNd26ddOZZ56pGTNmaPfu3XryySfVv39//c///I+kppl1L7/8siZPnqzBgwdrxowZ6tOnj3bs2KEVK1YoPT1d7733niTp4Ycf1pIlSzRu3DjdeOONKigo0M6dO/XWW2/pn//8pzIzM3XyySfLbrfr0UcfldPpVFJSks4++2xlZ2frueee07XXXqtTTz1VV1xxhXr06KH//ve/+vvf/64zzjhDzzzzjKSmRz2df/75OvPMM/WjH/1IFRUVmjt3rgYPHqxqv0cgxUuHG1gnnniilixZouLi4oCn9f/pT3+SzWYL+C4nAAAAAACAFf36178OGn/55Zf1wgsvqHv37nryySd98RNOOEFz5szRT3/6Uy1cuFCXXXaZ72f33HOP1q1bpzlz5mj//v2aMGGCnn32WXXp0sW3zPjx4/Xpp5/qN7/5jZ555hlVV1fr2GOP1emnn66bbrrJt1yfPn30+eef67777tP8+fNVVVWlPn36aPLkyb71HXvssXr++ec1Z84cXX/99XK73VqxYoWys7N11VVXqXfv3nrkkUf0u9/9TvX19erTp4/GjBmjGTNm+N5n0qRJeuutt3Tvvffq7rvvVn5+vl599VX99a9/1cqVK6O0lQ9dh79C+PHHH+vss89WVlaWbr31VmVlZelvf/ubFi9erBtuuEEvvfRSROvhK4QxwFcIAQAAAADtFO6rYWjm/QrhW2+9pUsuuSTe6cSU5b9COHbsWK1evVr333+/nn32WZWXl6tfv3566KGH9Itf/KKjqwcAAAAAAMBRrsMNLEkaOXKk3n///WisCgAAAAAAAAhgi3cCAAAAAAAAQFuiMgMLAAAAAADgaDd+/Hh18FHjCIEZWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAA4Kg1b948GYah5ORk7dixo9XPx48fryFDhsQhM/hzxDsBAAAAAABwGPvgg3hnIE2a1OFV1NfX65FHHtHcuXOjkBCijRlYAAAAAADgqHfyySfrpZdeUmlpabxTQRA0sAAAAAAAwFHvnnvukdvt1iOPPNLmci6XS7/5zW+Un5+vpKQk9e3bV/fcc4/q6+t9y9xxxx3KysqSaZq+2G233SbDMPT000/7Yrt375ZhGHruueeiX9ARhgYWAAAAAAA46vXr10/Tpk0LOwvrhhtu0K9//WudeuqpeuKJJzRu3DjNmTNHV1xxhW+ZMWPGqKKiQt98840vtmrVKtlsNq1atSogJkljx47thIqOLDSwAAAAAAAAJP3qV7+Sy+XSo48+GvTna9eu1WuvvaYbbrhBb731ln784x/rtdde089+9jP93//9n1asWCFJOvPMMyU1N6icTqe+/vprXXzxxa0aWN26ddOgQYM6ubLDHw0sAAAAAAAASXl5ebr22mv14osvaufOna1+/v7770tq+oqgvzvvvFOS9Pe//12S1KNHDw0cOFAff/yxJOmTTz6R3W7Xz3/+c+3evVubNm2S1NTAOvPMM2UYRqfVdKSggQUAAAAAAHDQvffeK5fLFfRZWFu3bpXNZlP//v0D4scee6wyMzO1detWX2zMmDG+2VarVq3S8OHDNXz4cHXr1k2rVq1SVVWV1q5dqzFjxnRuQUcIGlgAAAAAAAAH5eXl6Zprrgk5C0tSRDOmzjzzTO3YsUObN2/WqlWrNGbMGBmGoTPPPFOrVq3S6tWr5fF4aGBFiAYWAAAAAACAH+8srJbPwjr++OPl8Xh8XwH02r17tyorK3X88cf7Yt7G1NKlS/Xll1/6/j127FitWrVKq1atUmpqqk477bROrubIQAMLAAAAAADAT35+vq655hq98MIL2rVrly8+ZcoUSdKTTz4ZsPzjjz8uSTr//PN9sX79+qlPnz564okn1NjYqDPOOENSU2Pru+++09tvv63vfe97cjgcnVzNkYEGFgAAAAAAQAu/+tWv1NjYqH//+9++2LBhwzR9+nS9+OKLuvzyy/Xss8/quuuu029/+1v94Ac/0FlnnRWwjjFjxujf//63hgwZomOOOUaSdOqppyo1NVXFxcV8fbAdaGABAAAAAAC00L9/f11zzTWt4i+//LJmz56tL7/8Urfffrs++ugj3X333XrzzTdbLettUJ155pm+mMPh0KhRowJ+jvAM0zTNeCchSVVVVcrIyJDT6VR6enq804me//wn3hk0a/FXEgAAAAAACKeurk4lJSXq16+fkpOT450OLCrccdLRvg8zsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAOolhGLr//vvjncZhjwYWAAAAAAA4KhmGEdF/K1eujHeqRz1HvBMAAAAAAACHsf/8J94ZSP37H9LLXn/99YB///GPf9TSpUtbxQsKCg45NUQHDSwAAAAAAHBUuuaaawL+/dlnn2np0qWt4og/vkIIAAAAAAAQQk1Nje68807l5uYqKSlJAwYM0GOPPSbTNAOWq6+v1//7f/9PPXr0UNeuXTV16lRt37691fq2bt2qH//4xxowYIBSUlKUlZWlSy+9VFu2bPEts3nzZhmGoSeeeKLV61evXi3DMPSnP/0p6rVaGQ0sAAAAAACAIEzT1NSpU/XEE09o0qRJevzxxzVgwAD9/Oc/1x133BGw7A033KAnn3xSEydO1COPPKKEhASdf/75rdb55ZdfavXq1briiiv09NNP6+abb9by5cs1fvx4HThwQJKUl5enM844Q/Pnz2/1+vnz56tr1676/ve/3zlFWxRfIQQAAAAAAAhi0aJF+uijj/Tggw/qV7/6lSTpJz/5iS699FI99dRTuvXWW5Wfn6+1a9fqjTfe0I9//GP9/ve/9y139dVXa926dQHrPP/883XJJZcExC688EKNGjVK77zzjq699lpJ0rRp03TTTTdp48aNGjhwoCSpsbFRCxcu1EUXXaQuXbp0dvmWwgwsAAAAAACAIN5//33Z7XbNnDkzIH7nnXfKNE0tXrzYt5ykVsvdfvvtrdaZkpLi+/+NjY0qLy9X//79lZmZqa+++sr3s8suu0zJyckBs7A+/PBDlZWVHZXP6KKBBQAAAAAAEMTWrVvVu3dvde3aNSDu/auEW7du9f2vzWZTfn5+wHIDBgxotc7a2lr9+te/9j1Tq3v37urRo4cqKyvldDp9y2VmZurCCy/UggULfLH58+erT58+Ovvss6NW4+EiKg2s6667ToZhhPxvx44d0XgbAAAAAACAw9ptt92mhx56SJdddpkWLlyoJUuWaOnSpcrKypLH4wlYdtq0adq8ebNWr16t/fv3a9GiRbryyitlsx1985Gi8gysm266Seecc05AzDRN3Xzzzerbt6/69OkTjbcBAAAAAACImeOPP17Lli3T/v37A2Zhbdy40fdz7/96PB599913AbOu/v3vf7da59tvv63p06frf//3f32xuro6VVZWtlp20qRJ6tGjh+bPn6/TTz9dBw4c8D0j62gTlZbdqFGjdM011wT8169fPx04cEBXX311NN4CAAAAAAAgpqZMmSK3261nnnkmIP7EE0/IMAxNnjxZknz/+/TTTwcs9+STT7Zap91ul2maAbG5c+fK7Xa3WtbhcOjKK6/UwoULNW/ePJ100kkaOnRoR0o6bHXaXyFcsGCBDMPQVVdd1VlvAQAAAAAA0GkuvPBCnXXWWfrVr36lLVu2aNiwYVqyZIn++te/6vbbb/c98+rkk0/WlVdeqWeffVZOp1OjR4/W8uXL9Z///KfVOi+44AK9/vrrysjI0KBBg/Tpp59q2bJlysrKCprDtGnT9PTTT2vFihV69NFHO7VeK+uUBpb3zzqOHj1affv27Yy3AAAAAAAA6FQ2m02LFi3Sr3/9a/35z3/Wq6++qr59++p3v/ud7rzzzoBl//CHP/i+7vd///d/Ovvss/X3v/9dubm5Acs99dRTstvtmj9/vurq6nTGGWdo2bJlOu+884LmcNppp2nw4MHasGHDUf0tN8NsOW8tCv72t7/pwgsv1LPPPqtbbrkl6DL19fWqr6/3/buqqkq5ubkqLy9Xenq6pKYDxWazyePxBDzIzBt3u90B0+5Cxe12uwzDkMvlCsjBbrdLUqtpeqHiDodDpmkGxA3DkN1ub5WjL75pkzz+OR7M0+PxyP/RbDbDkM0w5PZ4ZEYQtx98QL6rxQPe7IbRlHuL3Wo3DKl//+jUFGJ/HNb7iZqoiZqoiZqoiZqoiZqoiZqoiZqC5l5XV6f//ve/6tevn1JSUlp9/c37ms6Mt0dn5xKPmk499VR169ZNy5Yti2mO7YnX1dVpy5Ytys3NVXJysi/uPfb27dunrKwsOZ1OX9+nPTplBtaCBQuUkJCgyy67LOQyc+bM0ezZs1vFi4qKlJqaKknq0aOH8vPzVVJSor179/qWycnJUU5OjoqLiwP+xGReXp6ys7O1fv161dbW+uIDBw5UZmamioqKAk7KoUOHKjExUYWFhQE5DB8+XA0NDVq3bp0vZrfbNWLECDmdTt/D2iQpJSVFw4YNU1lZmTZv3uyLZ2RkqKCgQKVOp7b75dgjLU35WVkq2bdPe6urm2vKyFBOZqaKy8rk9Ms9LytL2WlpWr9rl2obG5trys5WZkqKinbskNtv0Bvaq5cSHQ4VbtsWWFNurhpqa6NTU2mptm/f3lzTkbCfqImaqImaqImaqImaqImaqImaqClkTcnJyaqvr1dKSooaGxvV0NDgW97hcPh+7t9QS0xMVGJiourq6gJyTEpKUkJCgmprawOaeMnJyXI4HDpw4EBAcyQlJUU2m001NTUBNaWmpsrj8QRsF8MwlJqaKrfbrbq6Ol/cZrOpS5cucrlcAZNp7Ha75WsqKirSmjVr9MorrwQsb7WavE2t9evXB9TkPfaKiorUEVGfgVVdXa2ePXvq7LPP1nvvvRdyOWZgMQPLUvuJmqiJmqiJmqiJmqiJmqiJmqiJmoLmzgyszomHs379ev3rX//S448/rrKyMn333XcBM5vimXs8ZmBFvYH1xhtv6Nprr9Wf/vQnXXHFFRG/rqqqShkZGYdciGUFeWBb3PTvH+8MAAAAAACHmbq6OpWUlKhfv36tGijoPPfff78eeOABDRgwQM8//7zGjRsX75TaFO446WjfxxaNJP3Nnz9faWlpmjp1arRXDQAAAAAAcFS4//775fF4tGHDBss3r2Ihqg2svXv3atmyZfrhD3+oLl26RHPVAAAAAAAAOEpFtYH15z//WS6X66j+s44AAAAAAACIrqg2sObPn6/s7Gydc8450VwtAAAAAACIsyg/QhtHmM4+PhzRXNmnn34azdUBAAAAAIA48/4VucbGRqWkpMQ5G1hVY2OjpObjJdqi/hB3AAAAAABw5EhISFBSUpKcTiezsBCUaZpyOp1KSkpSQkJCp7xHVGdgAQAAAACAI0/37t21Y8cObd++XRkZGUpISJBhGPFOC3FmmqYaGxvldDpVXV2tPn36dNp70cACAAAAAABtSk9PlySVlZVpx44dcc4GVpOUlKQ+ffr4jpPOQAMLAAAAAACElZ6ervT0dDU2Nsrtdsc7HViE3W7vtK8N+qOBBQAAAAAAIpaQkBCThgXgj4e4AwAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNIc8U4AAAAAQGtL1sc7g2YTh4Rf5nDLFwBweGEGFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACzNEe8EAAAAACDWlqyPdwbNJg6JdwYAYH3MwAIAAAAAAICl0cACAAAAAACApUWtgfXVV19p6tSp6tatm7p06aIhQ4bo6aefjtbqAQAAAAAAcJSKyjOwlixZogsvvFCnnHKK7rvvPqWlpem7777T9u3bo7F6AAAAoMOs9MwjieceAQDQHh1uYFVVVWnatGk6//zz9fbbb8tm41uJAAAAAAAAiJ4Od5sWLFig3bt366GHHpLNZlNNTY08Hk80cgMAAAAAAAA63sBatmyZ0tPTtWPHDg0YMEBpaWlKT0/XLbfcorq6umjkCAAAAAAAgKNYh79CuGnTJrlcLn3/+9/X9ddfrzlz5mjlypWaO3euKisr9ac//Sno6+rr61VfX+/7d1VVlSTJ5XLJ5XJJkmw2m2w2mzweT8CsLm/c7XbLNM2wcbvdLsMwfOv1j0uS2+2OKO5wOGSaZkDcMAzZ7fZWOfripimPf44H8/R4PPKfp2YzDNkMQ26PR2YEcbthNNXUYrab3TCacjfN1vEWuR9yTSH2x2G9n6iJmqiJmqiJmqjpiK/J9L9tMpriMgNrMmxNNQXGDRk2u0zToxYrCR43bDIMW+i4xy3JlDfVUDWZZlNNpiewplC5d2ZNHk8E+8njd//Zolb/HGNRk8sV/tgzzcj2UyxqcrkOv/Mpkjg1URM1UZN/vOXy7dXhBlZ1dbUOHDigm2++2fdXBy+66CI1NDTohRde0AMPPKATTjih1evmzJmj2bNnt4oXFRUpNTVVktSjRw/l5+erpKREe/fu9S2Tk5OjnJwcFRcXy+l0+uJ5eXnKzs7W+vXrVVtb64sPHDhQmZmZKioqCtiQQ4cOVWJiogoLCwNyGD58uBoaGrRu3TpfzG63a8SIEXI6ndq4caMvnpKSomHDhqmsrEybN2/2xTMyMlRQUKBSp1Pb/XLskZam/Kwslezbp73V1c01ZWQoJzNTxWVlcvrlnpeVpey0NK3ftUu1jY3NNWVnKzMlRUU7dsjtd+AN7dVLiQ6HCrdtC6wpN1cNtbXRqam0NOAB/UfEfqImaqImaqImarJKTdu3K8PtVkF9vUoTErQ9IaG5JpdL+Q0NKklM1F5H821cTmOjchobVZyUJOfBm0RJymtoULbLpfXJyar1e07pwLo6ZXo8KkpJkfvgL78kaWhtrRJNU4Vdung31hG1nxr2N++nxJ7DZbob1FjWXJNh2JV47AiZDU41VjTXZDhSlNhjmDy1ZXI5m2uyJWUooVuB3NWlclc312RP6SFHZr7czhK5a5trsqflyNE1R67KYnnqnSo80HZNZsJAGUmZatxTJNOv2ZHQfagMe6Iadgcee51ZU0lq+P3UsLt5Pzky8mTvkq3G8vUyXc01JXSLTU2FheGPPbcrsv0Ui5qK6g+/88nfkTJGUBM1UVPn1lRUVKSOMEz/NtohGDJkiL755hv94x//0NixY33xjz/+WOPGjdNrr72madOmtXpdsBlYubm5Ki8vV3p6uqT4dwej0vHctMk6M7D69z8iu7jURE3URE3URE1HVE0LFsiQZJfkOfifL8eD/4WKt5gXEjJul2RIavl7UG/ry5fhVVdFp6Y24rHcT8u/9fuBBWZgTRjUdk3LN1hnBta5Q8Lvp2XfWGcG1oSC8Mfe8g3WmYE1YdDhdz5FEqcmaqImavKP79u3T1lZWXI6nb6+T3t0eAZW79699c0336hnz54B8ezsbF+CwSQlJSkpKal1Qg6HHI7AtLwbrSXvRog03nK9hxI3DCNoPFSO3gZU0OWDvKc9yDraijtCxYO8p0Lk3u6a2hk/LPYTNVFTiBzbG6cmapKoKVSO7Y1TU3MDKtJ48MxDx0PdCPriLXI93PeTEWyjGcFrCh63KdhK2h232Q/mFBhvWZP3ds6whdhTQXIMFe9oTd5d09Z+CrZ9vbW2jnduTQ5H+GPMt33D7KfI44dek/dYOJzOp0jj1ERNEjWFyrG98SOxpvbo8EPcTzvtNEnSjh07AuKlpaWSmqaoAQAAAAAAAIeqww2syy67TJL0yiuvBMRffvllORwOjR8/vqNvAQAAAAAAgKNYh79CeMopp+hHP/qR/vCHP8jlcmncuHFauXKl3nrrLd19993q3bt3NPIEAAAAAADAUarDDSxJev7553Xcccfp1Vdf1bvvvqvjjz9eTzzxhG6//fZorB4AAAAAAABHsag0sBISEjRr1izNmjUrGqsDAAAAAAAAfDr8DCwAAAAAAACgM9HAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTninQAAAAAAoG1L1sc7g2YTh8Q7AwBHI2ZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0hzxTgAAAACHryXr451Bs4lD4p0BAADoLMzAAgAAAAAAgKUxAwsAAAAAEFXMzgQQbczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKV1uIG1cuVKGYYR9L/PPvssGjkCAAAAAADgKOaI1opmzpypESNGBMT69+8frdUDAAAAAADgKBW1BtaYMWN0ySWXRGt1AAAAAAAAgKQoPwNr//79crlc0VwlAAAAAAAAjnJRm4E1Y8YMVVdXy263a8yYMfrd736n4cOHR2v1AAAAAAB0iiXr451Bs4lD4p0BYE0dbmAlJibq4osv1pQpU9S9e3d9++23euyxxzRmzBitXr1ap5xyStDX1dfXq76+3vfvqqoqSZLL5fLN4rLZbLLZbPJ4PPJ4PL5lvXG32y3TNMPG7Xa7DMNoNTvMbrdLktxud0Rxh8Mh0zQD4oZhyG63t8rRFzdNefxzPJinx+ORx2/dNsOQzTDk9nhkRhC3H3xQvsvjv5amuCS5TbN1vEXuh1xTiP1xWO8naqImaqImaqImK9UkyS7Jc/A/X44H/wsVd0uB9xEh4vaD79Fy3rz94P/6MjxYc7iaZPrHDRk2u0zTI5me8HHDJsOwhY57WmQfMt5UVVv7KTCdg9WagTUZttjV5E011LFnmk3HnulpsadC5N6ZNXk8EZxPnsj2UyxqcrnCjxGmGb1jr6M1uVzhxwjTE9vzqa2aXK7w457pie351Fbc5Qo/ljct37rWeIwRlr4+HYnXXGqKWU0d/cZehxtYo0eP1ujRo33/njp1qi655BINHTpUd999tz744IOgr5szZ45mz57dKl5UVKTU1FRJUo8ePZSfn6+SkhLt3bvXt0xOTo5ycnJUXFwsp9Ppi+fl5Sk7O1vr169XbW2tLz5w4EBlZmaqqKgoYEMOHTpUiYmJKiwsDMhh+PDhamho0Lp163wxu92uESNGyOl0auPGjb54SkqKhg0bprKyMm3evNkXz8jIUEFBgUqdTm33y7FHWprys7JUsm+f9lZXN9eUkaGczEwVl5XJ6Zd7XlaWstPStH7XLtU2NjbXlJ2tzJQUFe3YIbffgTe0Vy8lOhwq3LYtsKbcXDXU1oavqaZGKQkJGta7t8qqq7W5vLy5ppQUFWRnq7SyMnhN5eXBa9qzJ3hNpaXBa9q2rammg8dByP3UrZsaXC6t27mzuSabTSNyc+WsrdXGPXua91Msajr5ZGsde6Wl2r59e3NN7T2fkpMj20/emto69jq6n3r3jk5NVhwjqImaqKnza/ryy+hen7w1Hcq41717+Jq6dFGG262C+nqVJiRoe0JCc00ul/IbGlSSmKi9jubbuJzGRuU0Nqo4KUlOu90Xz2toULbLpfXJyaq1NT85YmBdnTI9HhWlpMh98JdfkjS0tlaJpqnCLl2aAgf3V1v7yWxwqrGiuSbDkaLEHsPkqS2Ty9m8n2xJGUroViB3danc1c37yZ7SQ47MfLmdJXLXNh979rQcObrmyFVZLE9987HnyMiTvUu2GsvXy3Q177+EbgMltX3sNexv3k+JPYfLdDeosay5JsOwK/HY2NVUeODgfgpxPpkJA2UkZapxT5FMvw/LCd2HyrAnqmF34PnUmTWVpIYfIxp2R7afYlFTYWH4McLtit6x19GaiurDj3sNu2N7PrVVUyRjeWN1bM+ntmoqPBD++hTL8ylcTYf1NfdIvI+gpqjVVFRUpI4wTP82WhRdeeWV+stf/qIDBw74um3+gs3Ays3NVXl5udLT0yXFvzsYlY7npk3WmYHVv3/4mjZvbvqtr83WavZYqHin1ZSX1xQPtZ9KSoLW6rDZmmqKIPeo1nTCCdY69jrabS8pid6xFyTerv2Un2/J3yBYYj9REzVRU/iaiotjf80NEnfYbDLz88PXtGCBdWZgXXVVU7yN/fTh1/GfXdEUt+u8k9o+9pZ/q4DlJcV1BtaEQU3hUOfT8g3WmYF17pDwY8Syb6wzA2tCQfgxYvkG68zAmjAo/Li3dL11ZmBNKAg/li//1jozsCYMCn99WvK1dWZgTSg4jK+5R+J9BDVFraZ9+/YpKytLTqfT1/dpj6g9A6ul3NxcNTQ0qKamJmhiSUlJSkpKap2QwyGHIzAt70ZrKVhjrK14y/UeStwwjKDxUDl6b4aDLh/kPe1B1tFW3BEqHuQ9FSL3gJr81hcy91jV1CLXVrkfzCFYrYZhBI13ek1WOvbaGW+V+8HtEZVjL0Q84v10MLcO1xQmfljupzBxaqImaorTNTdEvN01Hfwv0njwvRE6HupG0BcPdy1WU00ygsVtktE6y3bHbcGzDxVv6xgLsvoQucemppaptjyfvIeQYQuxp4LkGCre0Zq8h2dbY0Sw7Rt6/3VuTQ5H+DHCt32jdOx1pCbvsdDWGGEE2e6dfT6FqimSsdz79lYYI/zTDZV7e/ZfZ9d02F9zj8T7CGqKOMdDiUcq+J1YFGzevFnJyclKS0vrrLcAAAAAAADAUaDDDSz/7016rV27VosWLdLEiRODdvUAAAAAAACASHX4K4SXX365UlJSNHr0aGVnZ+vbb7/Viy++qC5duuiRRx6JRo4AAAAAAAA4inW4gfWDH/xA8+fP1+OPP66qqir16NFDF110kWbNmqX+/ftHI0cAAAAAAHDQkvXxzqDZxCHxzgBHiw43sGbOnKmZM2dGIxcAAAAAAACgFR5QBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3PEOwEAAAAAAHDkWrI+3hk0mzgk3hngUDEDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJbmiHcCAAAAAAAAVrFkfbwzaDZxSLwzsA5mYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJ4BhYAAICFfFcW7wya5cc7AQAAgIOYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLc8Q7gSPdp9/FO4Nmo/rHOwMAAAAAAID2YwYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsrVMaWA899JAMw9CQIUM6Y/UAAAAAAAA4ikS9gbV9+3Y9/PDDSk1NjfaqAQAAAAAAcBRyRHuFP/vZz/S9731PbrdbZWVl0V49AAAAAAAAjjJRnYH18ccf6+2339aTTz4ZzdUCAAAAAADgKBa1Bpbb7dZtt92mG264QSeddFK0VgsAAAAAAICjXNS+Qvj8889r69atWrZsWUTL19fXq76+3vfvqqoqSZLL5ZLL5ZIk2Ww22Ww2eTweeTwe37LeuNvtlmmaYeN2u12GYfjW6x+XmppvkcQdDodM0wyIG4Yhu93eKkdvvCkPM2A9hmGTaXoUyJBhGFGJNzFbxVvmHrQmj0eGJLvNJo9pyuO3HUPFbVLzfvJbt80wZDMMuT2egGxCxe1GU00u73Y8uL9C7qeDObjNwFodNltTTRHkHtWaDuZolWMv1HkT8flkmpHtJ7+41Hp/hIq3az+53dGpyYJjBDVREzXFqCa/dXf4+uQXlw5h3AtTk+fgpdxmNl3NTcNvJWbTNcojNV/yJRlm0z89/sseYlx+7+kKcy327ieZ/nFDhs3edI8ScJ8SIm7Ymu+NgsU9bgXc14SM2yW1fewFpmM/WGxgTYYtdjV5Uw11Pplm0/lkegJrCpV7Z9bk8UQwRngi20+xqMnlCj9GmGb0jr2O1uRyhR/3TE9sz6e2anK5wo/lpie251NbcZcr/PWpafnWtcZjjIjkmmt6FLPzKVxNLlf4+4hYnk/haorkPqJp+1pjjPAeskfC/V7L5dsrKg2s8vJy/frXv9Z9992nHj16RPSaOXPmaPbs2a3iRUVFvgfA9+jRQ/n5+SopKdHevXt9y+Tk5CgnJ0fFxcVyOp2+eF5enrKzs7V+/XrV1tb64gMHDlRmZqaKiooCNuTQoUOVmJiowsLCgByGDx+uhoYGrVu3zhez2+0aMWKEnE6nNm7c6IunpKRo2LBhKisr0+bNm33xjIwMFRQUqN7jVJ27OcdEW5q6OLJU696nBk+1L55sz1CyPVM1rjK5zObcU+xZSrKnqdq1S26z0RdPdWQrwUhRVeMOmX635V0Teskmh5yN2wJqykjIVW1tbfiaamqUkpCgYb17q6ymRpvLy5vXkZKiguxslTqd2u633XukpSk/K0sl+/Zpb3VzTTkZGcrJzFRxWZmcfvsjLytL2WlpWr9rl2obm2samJ2tzJQUFe3YIbfHI1VUtL2funVTg8uldTt3Ntdks2lEbq6cdXXauGdP83aMRU2SpY690tJSbd++vbmm9p5PycmR7SdvTb16KdHhUOG2wGNveG5ux/eT2x2dmiw4RlBTJ9VUU9P2sVdbG/zYq64OPkZUVgYfI8rLg48Re/Y0jxGpqeFrWrWq4+dTtGoyjCPv2Iv29clb06HspwhqOtCzi5Lr3eq5r17OtAQ50xJ8y6fVupTlbNC+jERVpzTfxmVUNyqzulF7M5NUl2T3xbs5G9S11qVdWclqdDRPvM+uqFNKg0fbs1NkGs1drF5ltXK4TW3r2UWSVH5wf7W1n8wGpxormmsyHClK7DFMntoyuZzN+8mWlKGEbgVyV5fKXd28n+wpPeTIzJfbWSJ3bfOxZ0/LkaNrjlyVxfLUNx97jow82btkq7F8vUxX8/5L6DZQUtvHXsP+5v2U2HO4THeDGsuaazIMuxKPjV1NhQea4qHOJzNhoIykTDXuKZLp9wEnoftQGfZENewOPJ86s6aS1PBjecPuyPZTLGoqLAw/Rrhd0Tv2OlpTUX34ca9hd2zPp7ZqimQsb6yO7fnUVk2FB8Jfn2J5PoWrKZJrbsP+2J1P4WoqPBD+fi+W51O4miK5j2jYH7vzKVxNhQcO8/tyNY8RRUVF6gjDNFv8evAQ3HLLLVq2bJm++eYbJSYmSpLGjx+vsrIyrV+/Puhrgs3Ays3NVXl5udLT0yXFvzsYjd8Gr/5gk6wyA2vUef3D17R5s3VmYOXlNcVD7aeSkqa4VWZgnXCCpY69DnfbS0qsMwMrP9+Sv0GwxH6ipuC5b94cnWMvRLxdY0ReXviaiosDa+rM8ylcTXl5R96xV1xsnRlY+flhayqZu6ApHwvMwOp321VNNbWxnz78Ov6zK5ridp13UtvH3vJvFbB8U7Hxm4E1YVBTONT5tHyDNWZXSNK5Q8KP5cu+scbsCtP0aEJB+DFi+QZrzK6QpAmDwo97S9dbZwbWhILwY/nyb60zA2vCoPDXpyVfW2cG1oSC8Nfc5d/KMjOwJgwKf7/34TrrzMA6Z1D4+4im7WuNMcJ7rThs78v94vv27VNWVpacTqev79MeHZ6BtWnTJr344ot68sknVVpa6ovX1dWpsbFRW7ZsUXp6urp16xbwuqSkJCUlJbVOyOGQwxGYlnejteTdCJHGW673UOKGYQSNh8rRMAwF3GH64sEfPxatePD3DJ57QNyvBu+NfEsh4zZb0Ieq2YNsl7biDm+8Ra6tcj+YgyNILoZhBI13ek0WOvbaG2+V+8HtEXY/tYwH2Y6h4hHvp4O5dbimMPHDcj+FiR+1Nfm9T9zHCL+8QtYUy/MpXPxIPfaCvOchX59axtu7n8LUZPO/51VzUylgean176pavLYjce97tsw11H6SESxuk4Lcp7Q7bgt+jIWKt3WMBb1tCpp7bGpqmWrL88l7CBm2ELfsQXIMFe9oTd7Dv60xItj2Db3/OrcmhyP8GOHbvlE69jpSk/dYaGuMMIJ+1ujc8ylUTZGM5d63t8IY4Z9uqNzbs/86u6ZIrrn+L4v3GBF4Cxbic3EMz6fmHIPXFMl9RMD2jfMY4b99D8v78gjikerwQ9x37Nghj8ejmTNnql+/fr7/Pv/8cxUXF6tfv3564IEHOvo2AAAAAAAAOEp1eAbWkCFD9O6777aK33vvvdq/f7+eeuop5efnd/RtAAAAAAAAcJTqcAOre/fu+sEPftAq/uSTT0pS0J8BAAAAAAAAkerwVwgBAAAAAACAztThGVihrFy5srNWDQAAAAAAgKMIM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaY54JwBr+fS7eGfQbFT/eGcAAAAAAACsgBlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQe4g4AAI5o/IESAACAwx8zsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaR1uYH3zzTe69NJLlZeXpy5duqh79+4aO3as3nvvvWjkBwAAAAAAgKOco6Mr2Lp1q/bv36/p06erd+/eOnDggN555x1NnTpVL7zwgm688cZo5AkAAAAAAICjVIcbWFOmTNGUKVMCYrfeeqtOO+00Pf744zSwAAAAAAAA0CGd8gwsu92u3NxcVVZWdsbqAQAAAAAAcBTp8Awsr5qaGtXW1srpdGrRokVavHixLr/88mitHgAAAAAAAEepqDWw7rzzTr3wwguSJJvNposuukjPPPNMyOXr6+tVX1/v+3dVVZUkyeVyyeVy+dZjs9nk8Xjk8Xh8y3rjbrdbpmmGjdvtdhmG4Vuvf1yS3G53RHGHwyHTNAPihmHIbre3ytEbb8rDDFiPYdhkmh4FMmQYRlTiTcxW8Za5B6vJu76mHEPlHpuavPsr5H46uI/dZmAuDltTjv5xQ5LdZpPHNOWJIG6Tmo89v3XbDEM2w5Db4wnYAjbDkO1gjlY59kKdNxGfT6YZtFa70bSfXJ7A/Wc3mo69lvsjVLxd+8ntjk5NFhwjqKmTavJ4onPshYi3a4xwucLXFMvzKZKajrBjLx7X3GBx7zU0XE2egy+3mU1rMA2/lZhN+8rj/zaSDLPpnx7/ZQ8xLr/3DHct9u4nmf5xQ4bN3rS9ArZZiLhha76PCBb3uBWwLUPG7ZLaPvYC07EfLDawJsMWu5q8qYY6n0yz6XwyPYE1hcq9M2vyeCIYyz2R7adY1ORyhR8jTDN6x15Ha3K5wo97pie251NbNblc4cdy0xPb86mtuMsV/vrUtHzrWuMxRkRyzTU9itn5FK4mlyv8/V4sz6dwNUVyH9G0fa0xRngP2cP2vtwv3nL59opaA+v222/XJZdcotLSUi1cuFBut1sNDQ0hl58zZ45mz57dKl5UVKTU1FRJUo8ePZSfn6+SkhLt3bvXt0xOTo5ycnJUXFwsp9Ppi+fl5Sk7O1vr169XbW2tLz5w4EBlZmaqqKgoYEMOHTpUiYmJKiwsDMhh+PDhamho0Lp163wxu92uESNGyOl0auPGjb54SkqKhg0bprKyMm3evNkXz8jIUEFBgeo9TtW5m3NMtKWpiyNLte59avBU++LJ9gwl2zNV4yqTy2zOPcWepSR7mqpdu+Q2G33xVEe2EowUVTXukOn38alrQi/Z5JCzcVtATRkJuaqtrQ1bk7OxRnYjQV0TeqvBU6Nad7lveYeRorSE7JjVVFhY0fZ+6tZNDS6X1u3c2VyTzaYRubly1tVp4549ze+ZkKBhvXurrKZGm8uba8pISVFBdrZKnU5t9zuWeqSlKT8rSyX79mlvdXNNORkZysnMVHFZmZx+x1heVpaypbaPvYNNWkka2quXEh0OFW4L3E/Dc3ND11RbG7ym6urgNVVWBq+pvLyppoPnWcjzKTlZ2WlpWr9rl2obm/fTwOxsZaakqGjHDrn9Br1DqinS/eR2q6CgQKWlpdq+fXtzTf5jxJYtvrhvP+3Z03o/paVpfWlp8Jq2bet4TbW12lhT01xTmDGizZqsNO7961/NNXX02PPWdKj7ad++8DXV1ETn2IvGGFFREX4/xfJ8CldTJMdeTU3szqdw415qatjzKR7XXI9c2t/YXJMhmzIScyO6jzjQs4uS693qua9ezrQEOdMSfMun1bqU5WzQvoxEVac038ZlVDcqs7pRezOTVJdk98W7ORvUtdalXVnJanQ0Pzkiu6JOKQ0ebc9OkWk0d7F6ldXK4Ta1rWcXSVL5wfOqrTHCbHCqsaK5JsORosQew+SpLZPL2Tzu2ZIylNCtQO7qUrmrm/eTPaWHHJn5cjtL5K5tPvbsaTlydM2Rq7JYnvrmY9WRkSd7l2w1lq+X6WrefwndBkpqe9xr2N+8nxJ7DpfpblBjWXNNhmFX4rGxq6nwQFM81BhhJgyUkZSpxj1FMv0+4CR0HyrDnqiG3YFjeWfWVJIa/vrUsDuy/RSLmgoLw19z3a7oHXsdramoPvxnjYbdsT2f2qopkvuIxurYnk9t1VR4IPy9USzPp3A1RXK/17A/dudTuJoKD4S/h43l+RSupkjuyxv2x+58CldT4YFD70dY7bNGUVGROsIwzRa/xo2SiRMnqrKyUp9//rkMw2j182AzsHJzc1VeXq709HRJ8e8ORuO3was/2CSrzMAadV7/sDV9sWyzX47xnYE18pw8SW3sp5KSpni8Z1d44yec0Pax5zegxH12hSTlNW3fkOdTSYl1ZmDl54f/DcJ//tMcb2s/xaKmfv2acz/MfisScozYtKk5d8XgfGprP/XtGz73zZutMwMrLy/8fiouDqwpnmNEXl74Y2/z5tidT+Fyz8sLez6t/iBw+8bimhssbhg2fW9iftj7iJK5C5ryt8AMrH63XSWp7THiw6/jP7uiKW7XeSe1Pe4t/1YByzcVG78ZWBMGNYVDjRHLN1hjdoUknTsk/PVp2TfWmF1hmh5NKAh/zV2+wRqzKyRpwqDwnzWWrrfODKwJBeHvI5Z/G9vzqa34hEHh742WfG2dGVgTCsLf7y3/VjE7n8LVNGFQ+HvYD9dZZwbWOYPC35c3bV9rjBHea8WRMANr3759ysrKktPp9PV92iNqM7BauuSSS3TTTTepuLhYAwYMaPXzpKQkJSUltU7I4ZDDEZiWd6O15N0IkcZbrvdQ4oZhBI2HyrGpede6gWcYwZ+fH6148PcMnrt/3H99oXOPTU0tc22V+8EPPY4gDVLDMILGvR+4Io7bbEH/0oE9yL6Wwhx7QV4TLMdQ8ajX1GJ7tsr94GtD1eoIFe+Mmg7mFuo8CzlGhNpPnV1TO8aIdtcUr3EvWI6dfT6F2h+R5O732riPEX55hdxPsTyfwsUjOfb8fh73McJv+4a+Fsf+mhsqHskYYfO/51VzUylgeal136zFazsS975n2GuxDt4XGMHiNinINmt33Bb8vAkVb2uMCLoLg+Yem5paptpyjPAe5oYtxC17kBxDxTtak/fUamuMCLZ9Q++/zq3J4WidTMvcfds3SsdeR2ryHgttjRFGqPGtE8+nUDVFci32vr0Vxgj/dEPl3p7919k1RXK/5/+yeI8RgbdgIa7FMTyfmnMMXlMk998B2zfOY4T/9j0SP2u0R6g7sQ7zTi/zn34GAAAAAAAAtFeHG1h7/J5N4dXY2Kg//vGPSklJ0aBBgzr6FgAAAAAAADiKdfgrhDfddJOqqqo0duxY9enTR7t27dL8+fO1ceNG/e///q/S0tKikSfQyqffxTuDQKP6xzsDAAAAAACOTB1uYF1++eV65ZVX9Nxzz6m8vFxdu3bVaaedpkcffVRTp06NRo4AAAAAAAA4inW4gXXFFVfoiiuuiEYuAAAAAAAAQCud9hB3AAAAAAAAIBpoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0hzxTgAAABxePv0u3hk0G9U/3hkAAAAgFpiBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEtzxDsB4Gjx6XfxziDQqP7xzgAAAAAAgMgwAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJbGM7AAAIgzKz0jj+fjAQAAwIqYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS+twA+vLL7/UrbfeqsGDBys1NVXHHXecLrvsMhUXF0cjPwAAAAAAABzlHB1dwaOPPqpPPvlEl156qYYOHapdu3bpmWee0amnnqrPPvtMQ4YMiUaeAAAAAAAAOEp1uIF1xx13aMGCBUpMTPTFLr/8cp100kl65JFH9MYbb3T0LQAAAAAAAHAU63ADa/To0a1iJ5xwggYPHqwNGzZ0dPUAAAAAAAA4ynXKQ9xN09Tu3bvVvXv3zlg9AAAAAAAAjiIdnoEVzPz587Vjxw498MADIZepr69XfX29799VVVWSJJfLJZfLJUmy2Wyy2WzyeDzyeDy+Zb1xt9st0zTDxu12uwzD8K3XPy5Jbrc7orjD4ZBpmgFxwzBkt9tb5eiNN+VhBqzHMGwyTY8CGTIMIyrxJmareMvcg9XkXV9TjqFyj01N3v0Van807+P25Nh5NXlzDHXsBb4m9H6KVU0tz7NW55NpymYYcns8AWuxG03bwOUJ3AZ24+A2MM2I4g5bU47+cUOS3WaTxzTl8Y+73UHPs5BjhGEEzT1UPOo1+Y014caIiGuK97jnn7tC7KcQcdvBPD0ej/y38CHvp0hq8niic+xFoyaXK+x+as9YHiwezTEikmOvKd/oXZ86UpPL5Qp7PsXjmttWTeHuIzwHX24zm9ZgGn4rMZuOP4//20gyzKZ/evyXPcS4/N4z3LXYO0bI9I8bMmz2pu3V4toXNG7Ymq9PweIetwK2Zci4XVLbY0RgOvaDxQbWZNhiV5M31VBjhGkeHCM8gTWFyr0za/J4Irg+eSLbT7GoyeUKf801zegdex2tyeUK/1nD9MT2fGqrJpcr/H2E6Ynt+dRW3OUKf2/UtHzrWuMxRkRyv9d0KbbGGOFyhb+HjeX5FK6mSO7Lm7avNcYI7yF7KP0Iq33WaLl8e0W9gbVx40b95Cc/0ahRozR9+vSQy82ZM0ezZ89uFS8qKlJqaqokqUePHsrPz1dJSYn27t3rWyYnJ0c5OTkqLi6W0+n0xfPy8pSdna3169ertrbWFx84cKAyMzNVVFQUsCGHDh2qxMREFRYWBuQwfPhwNTQ0aN26db6Y3W7XiBEj5HQ6tXHjRl88JSVFw4YNU1lZmTZv3uyLZ2RkqKCgQPUep+rczTkm2tLUxZGlWvc+NXiqffFke4aS7ZmqcZXJZTbnnmLPUpI9TdWuXXKbjb54qiNbCUaKqhp3yPT7+NQ1oZdscsjZuC2gpoyEXNXW1oatydlYI7uRoK4JvdXgqVGtu9y3vMNIUVpCdsxqKiysaHM/Sd3kkUv7G3f6IoZsykjMlcusU41rT3OtMahJUpvHnrOxyhdvaz/Fqibv9g15PiUnKzstTet37VJtY/N+GpidrcyUFBXt2BHQ1Bjaq5cSHQ4VbgusaXhurhpcLq3b2VyT3WbTiNxcOevqtHFPc00pCQka1ru3ympqtLm8uaYMt1sFBQU</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update KPI calculations and forecast data export
- Enhanced 'calculated_kpis.py' to generate a comprehensive Excel export for total TBS forecast data
- Modified forecast prediction to use full future dataframe instead of just the last 14 days
- Added new Excel export functionality with table styling for total TBS forecast
- Uploaded the new 'total_tbs.xlsx' file to Dropbox for easier data access and analysis
</commit_message>
<xml_diff>
--- a/calculated_KPIs_alerts.xlsx
+++ b/calculated_KPIs_alerts.xlsx
@@ -1,40 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>critical</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>forecast</t>
+  </si>
+  <si>
+    <t>forecast_time</t>
+  </si>
+  <si>
+    <t>forecast_value</t>
+  </si>
+  <si>
+    <t>forecast_lower</t>
+  </si>
+  <si>
+    <t>forecast_upper</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>total_tbs</t>
+  </si>
+  <si>
+    <t>vert_tbs</t>
+  </si>
+  <si>
+    <t>pod_tbs</t>
+  </si>
+  <si>
+    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACPQklEQVR4nOzdeXxU5dn/8e9JhiwQEkwIsiv7KvtSEQREEVGwsgha1tKfu2jVanGpBSuouOvjVn1AkVYBaxU3NsFSFTEWEQSKjyyyQwhMEsg6c//+iDPJkJksJJlzBj/v18tXyzUnM9c159znPnPlnhPLGGMEAAAAAAAAOFSU3QkAAAAAAAAAZaGBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAEAYWZZV6f8GDRpkd9p+5557rizL0q5du+xOpUp87y1q1q5du2RZls4991y7UwEAABHOZXcCAAD8kkyePLlU7ODBg1q2bFnIx9u3b1+p11izZo0GDx6sgQMHas2aNaeVZyQbNGiQPvvsM61evdpRzb9gfE00Y0yNv9af//xnzZw5Uw8++KD+/Oc/1/jrAQAAVCcaWAAAhNH8+fNLxdasWeNvYAV7HNVv69atdqcAAACASqCBBQAAfnEqu6oNAAAA9uIeWAAAONzevXt16623qk2bNoqLi1NSUpIuuOACvfzyy/J4PAHbDho0SIMHD5YkffbZZwH30ip5H6IjR47o2Wef1fDhw9WiRQvFx8crMTFRvXr10qOPPqrc3Nxqy3/KlCmyLEvz58/Xxo0bNWrUKKWmpio+Pl5dunTRM888U6oOScrKytJf//pXjRo1Sm3atFGdOnVUp04dnXfeebrvvvt0/PjxgO3XrFkjy7L02WefSZIGDx4cUH/J1W1l3QOrsLBQr776qgYNGqTk5GTFxsaqRYsWuvHGG7Vnz55S2/ted9CgQSooKNCjjz6qTp06KT4+XikpKRo1alSpFV9//vOfA17/1PuelbzH2OLFi3XxxRcrJSVFtWrVUkpKijp27Kj/9//+n7777rvy3n7/88+cOVOSNHPmzIDXmjJlSsC2GRkZuvfee9WpUyfVrl1bdevWVc+ePfXYY48pJyenQq8XTGFhoR577DH/e1O/fn1dffXV2rZtW8ifycnJ0RNPPKFf/epXqlevnuLi4tSuXTvdfffdOnr0aKVzWLlypUaMGKGzzz5btWrV0llnnaU2bdpowoQJ+te//hX0Z1atWqVRo0apUaNGiomJUYMGDXTVVVfpyy+/rLa858+f798XJ06c0IwZM9S6dWvFxsaqYcOGmjx5svbt21fpegEAOJOwAgsAAAf7+uuvNWzYMGVkZKh58+b69a9/LbfbrTVr1uiLL77Qu+++q/fff18xMTGSpGHDhikuLk7Lli3T2WefrWHDhvmfq379+v7/v2zZMt12221q0qSJWrdurV/96lc6cuSIvvrqK/3xj3/Ue++9p9WrVys2Nrbaalm/fr1uvPFGNWzYUEOGDNGxY8e0Zs0a3X777fr3v/+tRYsWBTR1Nm7cqOuuu06pqalq166devbsqWPHjumbb77R7NmztWjRIq1bt04pKSmS5P+g/8knn+jQoUO69NJL1bBhQ//ztW7dutwcs7KyNHLkSK1Zs0YJCQnq2bOnUlNTtWnTJr300ktavHixVqxYoe7du5f62YKCAg0fPlxffPGFLrzwQnXo0EHr16/Xu+++q9WrV2vDhg3+JmK3bt00efJkvf7665JK3/ssISFBkjRr1iw9+OCDcrlc6tevn5o0aSK3262ffvpJr732mjp16qQuXbqUW9fkyZP17bffauPGjeratau6devmf6x///7+/79jxw5ddNFF2r17t1JTUzV8+HAVFBRo9erVuueee/T2229r5cqVOuuss8p9zVONGzdOS5cu1cCBA9WlSxetX79eixcv1scff6zly5fr/PPPD9h+//79GjZsmDZt2qTk5GT17t1bdevW1X/+8x/NnTtXixcv1po1a3TOOedU6PVff/11TZ06VZLUp08fDR48WDk5Odq7d6/eeust1a9fXxdeeGHAz9x111164oknFBUVpV69emnAgAH66aef9N5772np0qX661//6n/O6sjb7XarX79++umnnzRgwAB17txZX375pd544w199tln2rhxo5KSkirztgMAcOYwAADAVqtXrzaSzKnTcm5urjnnnHOMJHPDDTeY/Px8/2M//vijOffcc40kc++99wZ9voEDB4Z8zS1btpgvv/yyVDwjI8MMHTrUSDKPPfZYqcd9+ezcubPC9U2ePNlf30033WQKCgr8j23evNmkpqYaSeall14K+Lk9e/aYlStXGo/HExA/ceKEmTRpkv/5TjVw4EAjyaxevTpkTsHeb2OMufbaa40kc8UVV5hDhw4FPPbUU08ZSaZNmzamsLDQHy+5/7p3724OHDjgfywnJ8dceumlRpK57rrrKpyHMUX7Pz4+3iQkJJht27aVenzXrl1m69atIWs81YMPPmgkmQcffDDkNn379jWSzMiRI012drY/fvjwYdOjRw8jyVx77bUVfs2dO3f6a6xfv77ZuHGj/7HCwkJz6623GknmnHPOMbm5uf7HvF6vueCCC4wkM23aNJOZmel/rKCgwNx5551Gkhk8eHCFc2nRooWRZNauXVvqsUOHDpn//Oc/AbFXXnnFSDKtW7cOyNsYYz777DNTt25dExMTY7Zv317lvOfNm+d/ny699FLjdrv9j2VkZJhu3boZSWb27NkVrhcAgDMNDSwAAGwWqoG1YMECI8k0btw44MO9z5IlS4wkU7duXZOTk1Pq+cpqYJXlv//9r5FkevfuXeqxqjSwGjVqFJCnz3PPPedvDFXUiRMnjMvlMqmpqaUeO90G1pYtW4xlWaZx48YBjYeShg8fbiSZpUuX+mO+99uyLPPtt9+W+pl169YZSaZly5YVysPn8OHDRpLp0qVLyDoqo7wG1tq1a40kU7t2bXPw4MFSj6elpRlJJioqyuzZs6dCr1mygfX000+Xejw3N9c0adLESDILFy70xz/++GMjyXTr1i2g4enj8XhM586djSSzadOmCuVSu3Ztk5SUVKFtPR6Pady4sZFk0tLSgm7z2GOPGUnmzjvvrHLevgZWnTp1zP79+0v93FtvvWUkmYsuuqhC+QMAcCbiHlgAADjUmjVrJEnjx48P+lW+UaNG6ayzzlJWVpa++eabSj+/x+PRqlWr9NBDD+mmm27S1KlTNWXKFD388MOSpP/+979Vyv9UV199teLi4krFfV+f++GHH7R///5Sj3/xxRd69NFHdfPNN/tzvOmmmxQTE6MjR47o2LFj1ZLfRx99JGOMLrvsMtWtWzfoNoMGDfLndKrmzZura9eupeIdOnSQpErfwyg1NVXnnnuuvvvuO915553asmVLpX6+snzH27Bhw3T22WeXerxnz57q2rWrvF6v/z5jlXHq1yQlKTY2VuPGjQt4fUn68MMPJUmjR4+Wy1X6jhdRUVH+r/sF2xfB9OnTR263W5MmTdI333wjr9cbctsNGzZo//79atWqlXr27Bl0m2DHQlXz7tWrlxo1alQqfrrHEAAAZxLugQUAgEP5Pqy2aNEi6OOWZalFixY6duxYpT/Y/vDDD7rqqqv0/fffh9wmMzOzUs9ZnlB11K1bVykpKTp69Kj27t2rxo0bS5IOHz6s0aNH69///neZz5uZmXla92Q61Y4dOyRJr732ml577bUytz1y5EipWPPmzYNum5iYKEnKy8urdE5vvPGGxowZoyeffFJPPvmkkpOT1bdvX11yySWaOHFiwH3Nqqq8402SWrVqpY0bN1b6eKtXr57q1asX9DHf6+3du9cf8+2LBx54QA888ECZzx1sXwTzwgsv6IorrtCCBQu0YMEC1a1bV71799ZFF12kiRMnBuw/3+v/+OOPIW/2H+z1q5p3ecdQdf5xBQAAIg0NLAAAfoHGjBmj77//XldccYXuvvtudezYUYmJiapVq5by8/Or9ebtlWGM8f//3/3ud/r3v/+t888/XzNnzlTXrl111llnqVatWpKkxo0b68CBAwE/UxW+FTndunULupKqpL59+5aKRUVV/8L2AQMGaNeuXfrwww/12Wef6YsvvtCyZcv08ccf68EHH9S7776rIUOGVPvr2qHkfvTti/79+6tVq1Zl/lynTp0q9PwdOnTQf//7Xy1fvlyffvqpvvjiC61du1affvqpZs2apddee00TJkwIeP2GDRvq0ksvLfN5SzYRq5p3TRxDAACcKWhgAQDgUE2aNJFUvKojmJ07dwZsWxHbtm3Td999pwYNGujdd98t9VWnH3744TSyLZ8v11NlZWXp6NGjkqSmTZtKkk6cOKGPPvpIUVFR+uijj0qt3jlx4oQOHjxYrfk1a9ZMknTBBRfo+eefr9bnror4+HiNGTNGY8aMkVS0cuf+++/XK6+8ot/+9rfavXt3tbxORY4332OVOd4k6fjx4zp+/HjQVVi7du2SVLzvpeJ9ceWVV+quu+6q1GuVxeVyafjw4Ro+fLikotV7Tz75pGbOnKnrr79eV111lerUqeN//ZSUFM2fP7/Cz19TeQMAAIlf8wAA4FC+e+y8/fbbQb869O677+rYsWOqW7duwH16YmJiJEmFhYVBnzcjI0NS0QqmYPfpefPNN6uaelCLFy8O+jW6BQsWSJJat27tb4y43W55PB4lJiYGbXq8+eabIVdelVd/KJdddpkk6f333w/bV7V8q8kqk2tqaqoee+wxSdJPP/1U4XuAlfe++I63Tz75RIcOHSr1+IYNG/Ttt98G3MepMnz7uaT8/Hy9/fbbAa8vFe+LxYsXV9sKu2ASExP15z//WfXq1dPJkye1fft2SVLv3r1Vv359bdmypcyv2Z4qXHkDAPBLRAMLAACHGjt2rJo3b679+/frjjvuCGg87Ny5U3feeack6dZbbw24ObpvJcsPP/yggoKCUs/btm1bRUdHa9OmTQE3zpakpUuX6qmnnqqBaqT9+/frrrvuksfj8ce2bt2qWbNmSZJ+//vf++Nnn322zjrrLB0/frxU42PdunWaMWNGyNfx1V+ZxoMkde/eXaNHj9aePXs0atQo/8qgkk6cOKGFCxcGbfCcjrJy3b17t1599dWg9yJbunSpJOmss87y3x+pKq8lFX3trW/fvsrJydH111+vkydP+h9LT0/X9ddfL6nojwr4VhpVxkMPPaTNmzf7/+31enXPPfdo7969atasmUaPHu1/7Morr1Tv3r21fv16TZ06Nej9oo4dO6aXXnqpQs2/kydP6sknnwz6PGvXrtXx48cVHR3tf49q1aqlBx98UMYYXXXVVUHvw+bxePTpp59q3bp1NZY3AAAowb4/gAgAAIwxZvXq1UaSCTYtr1+/3iQnJxtJ5pxzzjHjxo0zw4cPN3FxcUaSufTSS01eXl6pn+vVq5eRZNq1a2d+85vfmGnTppl77rnH//htt91mJJmoqCgzcOBAc80115gePXoYSeb+++8Pmc8555xjJJmdO3dWuL7JkycbSeaGG24wcXFxpkWLFmb8+PHm0ksvNTExMUaSueqqq4zX6w34uaeeesqfR9++fc0111xjLrjgAmNZlpk4cWLIXD744AMjycTExJgrrrjC/Pa3vzXTpk0zn3/+uX+bUPVlZmaaIUOG+H++d+/e5uqrrzZjx441vXv39ue7detW/8/49t/AgQNDvgehXu+uu+4ykkz9+vXN1VdfbaZNm2amTZtm0tPTzYYNG4wkU6tWLX8eV199tenevbuRZCzLMq+++moF94IxBw8eNHXq1DGSzAUXXGCmTJlipk2bZv73f//Xv82PP/7of18bNGhgxowZY6688kqTmJhoJJkePXqYjIyMCr/mzp07jSTTvHlzc9VVV5latWqZSy65xIwfP960atXKSDJ16tQxa9euLfWz+/btM926dfNv069fPzN+/HgzatQo061bNxMdHW0kmZycnHLzOHbsmP9479q1qxkzZoy55pprzPnnn28syzKSzJ/+9KdSP/eHP/zBv+86depkrrzySjN+/HgzaNAgU69ePSPJvPjii1XOe968eUaSmTx5cpnv4znnnFNurQAAnKloYAEAYLOyGljGGPPTTz+Zm2++2bRs2dLExMSYunXrmvPPP9+8+OKLpqCgIOjP7N6921x77bWmUaNGxuVylfrw6/V6zWuvvWZ69uxpEhISTFJSkunfv7956623jDGhGy5VaWDNmzfP/Oc//zEjRowwKSkpJjY21nTq1Mk8+eSTIev45z//afr162fq1atnEhISTK9evcwLL7xgvF5vmbn89a9/NT169DC1a9f21zJv3jz/42W93x6Px/ztb38zw4cPN2effbapVauWSUlJMZ07dzZTp0417777rsnPz/dvX5UGVk5Ojrn77rtN69at/c0xX02ZmZnm6aefNldddZVp06aNSUhIMHXq1DFt27Y1kyZNMmlpaSFfL5R//etf5uKLLzZnnXWWiYqKCto0OXr0qJkxY4bp0KGDiYuLM7Vr1zbdu3c3jzzyiDl58mSlXq9k46WgoMA8/PDDpn379iY2NtYkJyeb0aNHm++//z7kz+fm5pqXXnrJDB482KSkpBiXy2UaNGhgunXrZm6++WazbNmyCuVRUFBgXnrpJXPNNdeY9u3bm6SkJBMfH29atWplRo8ebVatWhXyZz///HPzm9/8xpxzzjkmNjbW1K1b17Rt29b8+te/Nq+++mrQhl5l86aBBQBA+Sxj+II+AACoOVOmTNHrr7+uefPmacqUKXanAwAAgAjEPbAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBo3AMLAAAAAAAAjsYKLAAAAAAAADgaDSwAAAAAAAA4msvuBE6H1+vV/v37VbduXVmWZXc6AAAAAAAAKIMxRllZWWrcuLGioiq/nioiG1j79+9Xs2bN7E4DAAAAAAAAlbBnzx41bdq00j8XkQ2sunXrSioqOjEx0eZsAAAAAAAAUJbMzEw1a9bM39OprIhsYPm+NpiYmEgDCwAAAAAAIEKc7q2guIk7AAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAABwtIv8KIQAAAAAACD9jjDwejwoLC+1OBQ7hcrkUHR192n9dsMKvU6PPDgAAAAAAIp4xRsePH9eRI0fk8XjsTgcOEx0drQYNGigpKanGGlk0sAAAAAAAQJkOHjyo48ePKzExUYmJiXK5XDW+4gbOZ4xRYWGhMjMzdeDAAeXk5KhRo0Y18lo0sAAAAAAAQEgej0dut1upqamqX7++3enAgerWravY2Filp6erQYMGio6OrvbX4CbuAAAAAAAgpIKCAhljVKdOHbtTgYPVqVNHxhgVFBTUyPPTwAIAAAAAAOXiK4MoS00fHzSwAAAAAAAA4Gg0sAAAAAAAABDUlClTdO6559qdBg0sAAAAAADwyzV//nxZlhXyv3Xr1tmdYrm2bNmiP//5z9q1a5fdqdQY/gohAAAAAAD4xZs1a5ZatGhRKt66dWsbsqmcLVu2aObMmRo0aJAjVkvVBBpYAAAAAADgtC3fbHcG0tDOVX+Oyy67TL169ar6E6FG8BVCAAAAAACAMjz44IOKiorSqlWrAuLXXXedYmJitHHjRknSmjVrZFmW3n77bd17771q2LCh6tSpo5EjR2rPnj2lnverr77SsGHDlJSUpNq1a2vgwIH6/PPPS223b98+TZs2TY0bN1ZsbKxatGihG2+8Ufn5+Zo/f77Gjh0rSRo8eLD/q49r1qzx//zHH3+sAQMGqE6dOqpbt64uv/xyff/996Ve55///Kc6d+6suLg4de7cWe+++25V3rZqxQosAAAAAADwi+d2u5Wenh4QsyxLKSkpuv/++7V06VJNmzZNmzZtUt26dbVs2TL99a9/1UMPPaSuXbsG/NzDDz8sy7J0zz336PDhw3r66ad18cUX69tvv1V8fLwk6dNPP9Vll12mnj17+htk8+bN00UXXaS1a9eqT58+kqT9+/erT58+On78uK677jq1b99e+/bt05IlS3Ty5EldeOGFmj59up599lnde++96tChgyT5/3fBggWaPHmyLr30Uj366KM6efKkXnzxRfXv318bNmzwf+Vw+fLlGj16tDp27Kg5c+bo6NGjmjp1qpo2bVqTb3uFWcYYY3cSlZWZmamkpCS53W4lJibanQ4AAAAAAGes3Nxc7dy5Uy1atFBcXFypxyP9K4Tz58/X1KlTgz4WGxur3NxcSdLmzZvVs2dPTZo0SXPnzlXnzp3VqFEjffnll3K5itYHrVmzRoMHD1aTJk20detW1a1bV5K0ePFiXX311XrmmWc0ffp0GWPUrl07tWzZUh9//LEsy5Ik5eTkqFOnTmrdurWWL18uSZo8ebLefPNNffXVV6W+4miMkWVZWrJkicaOHavVq1dr0KBB/sezs7PVrFkzjR07Vq+88oo/fujQIbVr105XX321P969e3cdOnRIW7duVVJSkiRpxYoVGjp0qM4555xybxBf3nFS1V4OK7AAAAAAAMAv3v/8z/+obdu2AbHo6Gj//+/cubNmzpypGTNm6LvvvlN6erqWL1/ub16VNGnSJH/zSpLGjBmjRo0a6aOPPtL06dP17bff6ocfftD999+vo0ePBvzskCFDtGDBAnm9XklFX+sbMWJE0Ptz+RpfoaxYsULHjx/XNddcE7C6LDo6Wn379tXq1aslSQcOHNC3336rP/7xj/7mlSRdcskl6tixo06cOFHm64QDDSwAAAAAAPCL16dPn3Jv4v6HP/xBb731ltavX6/Zs2erY8eOQbdr06ZNwL8ty1Lr1q39q5h++OEHSUWrq0Jxu93Kz89XZmamOnc+vSVmvte56KKLgj7uWwm1e/fuoHlLUrt27fSf//zntF6/OtHAAgAAACKAE76i41ORr+pEWr4AUBE7duzwN4U2bdp02s/jW101d+5cdevWLeg2CQkJysjIOO3XKPk6CxYsUMOGDUs9Hmz1mFNFTqYAAAAAAAA28Xq9mjJlihITE3X77bdr9uzZGjNmjEaNGlVqW1+Ty8cYo//7v/9Tly5dJEmtWrWSVLQC6uKLLw75mqmpqUpMTNTmzWX/ViDUVwl9r9OgQYMyX+ecc84Jmrck/fe//y3ztcMlyu4EAAAAAAAAnO7JJ5/UF198oVdeeUUPPfSQ+vXrpxtvvLHUXy6UpDfeeENZWVn+fy9ZskQHDhzQZZddJknq2bOnWrVqpccff1zZ2dmlfv7IkSOSpKioKP3617/W0qVLlZaWVmo739/lq1OnjiTp+PHjAY9feumlSkxM1OzZs1VQUBDydRo1aqRu3brp9ddfl9vt9j++YsUKbdmypcz3JVxYgQUAAAAAAH7xPv74Y23btq1UvF+/fsrLy9MDDzygKVOmaMSIEZKK/npht27ddNNNN2nRokUBP5OcnKz+/ftr6tSpOnTokJ5++mm1bt1a/+///T9JRY2pV199VZdddpk6deqkqVOnqkmTJtq3b59Wr16txMRELV26VJI0e/ZsLV++XAMHDtR1112nDh066MCBA1q8eLH+/e9/q169eurWrZuio6P16KOPyu12KzY2VhdddJEaNGigF198URMnTlSPHj00fvx4paam6qefftKHH36oCy64QM8//7wkac6cObr88svVv39//fa3v1VGRoaee+45derUKWiTLdxoYAEAAAAAgF+8P/3pT0Hjr776ql5++WXVr19fTz/9tD/epk0bzZkzR7fddpsWLVqkq6++2v/Yvffeq++++05z5sxRVlaWhgwZohdeeEG1a9f2bzNo0CB9+eWXeuihh/T8888rOztbDRs2VN++fXX99df7t2vSpIm++uorPfDAA1q4cKEyMzPVpEkTXXbZZf7na9iwoV566SXNmTNH06ZNk8fj0erVq9WgQQNde+21aty4sR555BHNnTtXeXl5atKkiQYMGKCpU6f6X2fYsGFavHix7r//fs2YMUOtWrXSvHnz9N5772nNmjXV9C6fPsv41ptFkMzMTCUlJcntdvvvmA8AAACcySLtpuiRli+A0HJzc7Vz5061aNFCcXFxdqfjaGvWrNHgwYO1ePFijRkzxu50wqq846SqvRzugQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEfjJu4AAAAAAADVYNCgQYrAW41HBFZgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAACAX6z58+fLsizFxcVp3759pR4fNGiQOnfubENmKMlldwIAAAAAACCCffKJ3RlIw4ZV+Sny8vL0yCOP6LnnnquGhFDdWIEFAAAAAAB+8bp166a//vWv2r9/v92pIAgaWAAAAAAA4Bfv3nvvlcfj0SOPPFLmdoWFhXrooYfUqlUrxcbG6txzz9W9996rvLw8/zZ33HGHUlJSZIzxx2699VZZlqVnn33WHzt06JAsy9KLL75Y/QWdYWhgAQAAAACAX7wWLVpo0qRJ5a7C+t3vfqc//elP6tGjh5566ikNHDhQc+bM0fjx4/3bDBgwQBkZGfr+++/9sbVr1yoqKkpr164NiEnShRdeWAMVnVloYAEAAAAAAEi67777VFhYqEcffTTo4xs3btTrr7+u3/3ud1q8eLFuuukmvf7667rrrrv0z3/+U6tXr5Yk9e/fX1Jxg8rtdmvTpk0aPXp0qQZWcnKyOnbsWMOVRT4aWAAAAAAAAJJatmypiRMn6pVXXtGBAwdKPf7RRx9JKvqKYEl33nmnJOnDDz+UJKWmpqp9+/b617/+JUn6/PPPFR0drT/84Q86dOiQfvjhB0lFDaz+/fvLsqwaq+lMwV8hBAAAAPCLtnyz3RkUG9rZ7gwA3H///VqwYIEeeeQRPfPMMwGP7d69W1FRUWrdunVAvGHDhqpXr552797tjw0YMMDf8Fq7dq169eqlXr16KTk5WWvXrtXZZ5+tjRs36tprr635os4ArMACAAAAAAD4WcuWLTVhwoSQq7AkVWjFVP/+/bVv3z7t2LFDa9eu1YABA2RZlvr376+1a9fqiy++kNfr1YABA6q7hDMSDSwAAAAAAIAS7r///qD3wjrnnHPk9Xr9XwH0OXTokI4fP65zzjnHH/M1plasWKGvv/7a/+8LL7xQa9eu1dq1a1WnTh317Nmzhqs5M9DAAgAAAAAAKKFVq1aaMGGCXn75ZR08eNAfHz58uCTp6aefDtj+ySeflCRdfvnl/liLFi3UpEkTPfXUUyooKNAFF1wgqaix9eOPP2rJkiX61a9+JZeLuztVBO+SU7zxht0ZFJs0ye4MAAAAAACw1X333acFCxbov//9rzp16iRJ6tq1qyZPnqxXXnlFx48f18CBA7V+/Xq9/vrr+vWvf63BgwcHPMeAAQP01ltv6bzzztNZZ50lSerRo4fq1Kmj7du3c/+rSmAFFgAAAAAAwClat26tCRMmlIq/+uqrmjlzpr7++mvdfvvt+vTTTzVjxgy99dZbpbb1fW2wf//+/pjL5dL5558f8DjKZxljjN1JVFZmZqaSkpLkdruVmJhodzrVgxVYAAAAYRdJf30uknKVIivfSMoVsENubq527typFi1aKC4uzu504FDlHSdV7eWwAgsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjlblBtb333+vsWPHqmXLlqpdu7bq16+vCy+8UEuXLi217datWzVs2DAlJCQoOTlZEydO1JEjR6qaAgAAAAAAAM5grqo+we7du5WVlaXJkyercePGOnnypN555x2NHDlSL7/8sq677jpJ0t69e3XhhRcqKSlJs2fPVnZ2th5//HFt2rRJ69evV0xMTJWLAQAAAAAAwJmnyg2s4cOHa/jw4QGxW265RT179tSTTz7pb2DNnj1bJ06c0DfffKPmzZtLkvr06aNLLrlE8+fP928HAAAAAAAAlFQj98CKjo5Ws2bNdPz4cX/snXfe0RVXXOFvXknSxRdfrLZt22rRokU1kQYAAAAAAADOAFVegeVz4sQJ5eTkyO126/3339fHH3+scePGSZL27dunw4cPq1evXqV+rk+fPvroo4+qKw0AAAAAAACcYaqtgXXnnXfq5ZdfliRFRUVp1KhRev755yVJBw4ckCQ1atSo1M81atRIGRkZysvLU2xsbNDnzsvLU15env/fmZmZkqTCwkIVFhb6XzMqKkper1der9e/rS/u8XhkjCk3Hh0dLcuy/M9bMi5JHo+nQnGXyyVjTEDcsixFR0eXytGyLEVL8v78nz/Hn/8LFfdIMhWIR0uyJAVWVBTXz9sHxH9+P6pcU5B4xO8naqImaqImaqImajqjajIlL7Ksn6+OzClXRyHiVlRRTYFxS1ZUtIzx6pQnDx63omRZUTLGq8LCsmsy3hLbe0+54rOKajLeU674aqimwsLy91PIWkvlHp6ayjr2itMsfz/VdE0lh1qkjaeSzpRzBDUVxQsLC4vPRSWet2T+TopXhtNyj+SapKLjo2SvpuSxd+rxV1nV1sC6/fbbNWbMGO3fv1+LFi2Sx+NRfn6+JCknJ0eSgjao4uLi/NuEamDNmTNHM2fOLBXfsGGD6tSpI0lKTU1Vq1attHPnzoC/bNi0aVM1bdpU27dvl9vt9sdbtmypBg0aaPPmzf78JKl9+/aqV6+eNmzYEDCIu3TpopiYGKWlpQXk0KtXL+Xn5+u7777zx6Kjo9W7d2+53W5t27bNH4+Pj1fXrl2Vnp6uHTt2+ONJSUnqIGl/rVraW6uWP55aWKhW+fnaGROjI67iXdW0oEBNCwq0PTZW7uhof7xlfr4aFBZqc1yccqKKvx3aPjdX9bxebYiPl8eyimvKyVGMMUqrXTuwpp/3XZVr6tBB+/fv1969e4trivT9RE3URE3URE3URE1nVE35x4trqlW/i6zoGOUfCqwp5uxeMp58FaQX12RZ0Ypp2Fsm362CjOKaLFe8YlK7ypuTrkJ3cU1RsUmqldxBnuz98mQX1xQdnypXvVbyuHcqLa3smvKzJFdSS0XXbqCCo5tlCotrqpXcXlZsPRUc3iBjar6mtJPl7yePe6c8OcU1RSc0latuUxUe3y5vXvF+CkdN5R17+VkV3081XVPayeKaIm08nYnnCGoqrsn32d3j8Sg3N9cfj4qKUu3atVVYWBiw8CQ6Olrx8fEqKCjw9wakosZeXFyc8vLyAhoaMTExiomJUW5ubkCOsbGxqlWrlnJycgKaeHFxcXK5XDp58mRAMyU+Pl5RUVE6ceJEQE116tSR1+sNeF8sy1KdOnVqvKaoqCjNmDFD99577xlTU7D9JEkFBQXavHmzP17y2PMtRjpdlqlqay+EoUOH6vjx4/rqq6/0zTffqHfv3nrjjTc0ceLEgO3uvvtuzZ07V7m5uZVagdWsWTMdPXpUiYmJkpzTmfapdLd94ULnrMD6eR+dyb9BoCZqoiZqoiZqoiZqKiws1KotJZK0eQXWkA5l17RqS4ntbV6BNaRj+ftp2SbnrMC6pFPZx17xcWD/CqwhHYvDkTaeSjpTzhHUVBTPzc3VTz/9pJYtWwb93B7Jq5WiSiz+KMunn36qQYMGnVaOlmXpT3/6k/785z9XaPtIXYGVl5enHTt2qHnz5v6GZ8ljLzMzUykpKXK73f5eTmVU2wqsU40ZM0bXX3+9tm/f7v/qoO+rhCUdOHBAycnJIZtXUlEnL9jjLpdLLldgCb4BeyrfAKxo/NTnPZ24ZVlB46Fy9DWgKhoPnnnoeKidXSr+8yqtaqmpkvGI2E/URE0hcqxsnJqoSaKmUDlWNk5N1CSdXk1WsIssK8RVU5C4ZVkh4lEK9uRlxV2usmsq+WNWVPCarKiK5x4qXpGaSu7GUPsjZK0hc6/Zmso69k5Ns9L7rxprCjakImU8VTVOTc6tyeVyFZ0bJP//Bvi//1OQaNH24Yq3bh1ii7ItWLAg4N9vvPGGVqxYUSresWPHst+DMuK+x059/HSep6Iq+9zVGQ/WqwkWq6waa2D5lrC53W61a9dOqamppZYlStL69evVrVu3mkoDAAAAAAAgqAkTJgT8e926dVqxYkWpOOxXsbVyZTh8+HCpWEFBgd544w3Fx8erY8eiNbCjR4/WBx98oD179vi3W7VqlbZv366xY8dWNQ0AAAAAAIBqd+LECd15551q1qyZYmNj1a5dOz3++OOlvkaXl5en3//+90pNTVXdunU1cuTIgHua+ezevVs33XST2rVrp/j4eKWkpGjs2LHatWuXf5sdO3bIsiw99dRTpX7+iy++kGVZ+vvf/17ttTpZlVdgXX/99crMzNSFF16oJk2a6ODBg1q4cKG2bdumJ554QgkJCZKke++9V4sXL9bgwYN12223KTs7W3PnztV5552nqVOnVrkQAAAAAACA6mSM0ciRI7V69WpNmzZN3bp107Jly/SHP/xB+/btC2gw/e53v9Obb76pa6+9Vv369dOnn36qyy+/vNRzfv311/riiy80fvx4NW3aVLt27dKLL76oQYMGacuWLapdu7ZatmypCy64QAsXLtTvf//7gJ9fuHCh6tatqyuvvLLG63eSKjewxo0bp9dee00vvviijh49qrp166pnz5569NFHNXLkSP92zZo102effaY77rhDf/zjHxUTE6PLL79cTzzxRJn3vwIAAAAAALDD+++/r08//VR/+ctfdN9990mSbr75Zo0dO1bPPPOMbrnlFrVq1UobN27Um2++qZtuukn/8z//49/uN7/5TcBfc5Skyy+/XGPGjAmIjRgxQueff77eeecd/x+/mzRpkq6//npt27ZN7du3l1T0jbdFixZp1KhRql27dk2X7yhV/grh+PHjtWLFCh08eFAFBQXKyMjQihUrAppXPp06ddKyZct04sQJHTt2TG+++abOPvvsqqYAAAAAAABQ7T766CNFR0dr+vTpAfE777xTxhh9/PHH/u0kldru9ttvL/Wc8fHx/v9fUFCgo0ePqnXr1qpXr57+85//+B+7+uqrFRcXp4ULF/pjy5YtU3p6+i/yHl1VbmABAAAAAACciXbv3q3GjRurbt26AfEOHTr4H/f9b1RUlFq1ahWwXbt27Uo9Z05Ojv70pz/576lVv359paam6vjx43K73f7t6tWrpxEjRuhvf/ubP7Zw4UI1adJEF110UbXVGCloYAEAAAAAAITJrbfeqocfflhXX321Fi1apOXLl2vFihVKSUmR1+sN2HbSpEnasWOHvvjiC2VlZen999/XNddco6ioX147p8r3wAIAAAAAADgTnXPOOVq5cqWysrICVmFt27bN/7jvf71er3788ceAVVf//e9/Sz3nkiVLNHnyZD3xxBP+WG5uro4fP15q22HDhik1NVULFy5U3759dfLkSf89sn5pfnktOwAAAAAAgAoYPny4PB6Pnn/++YD4U089JcuydNlll0mS/3+fffbZgO2efvrpUs8ZHR0tY0xA7LnnnpPH4ym1rcvl0jXXXKNFixZp/vz5Ou+889SlS5eqlBSxWIEFAAAAAAAQxIgRIzR48GDdd9992rVrl7p27arly5frvffe0+233+6/51W3bt10zTXX6IUXXpDb7Va/fv20atUq/d///V+p57ziiiu0YMECJSUlqWPHjvryyy+1cuVKpaSkBM1h0qRJevbZZ7V69Wo9+uijNVqvk9HAAgAAAAAACCIqKkrvv/++/vSnP+ntt9/WvHnzdO6552ru3Lm68847A7b93//9X//X/f75z3/qoosu0ocffqhmzZoFbPfMM88oOjpaCxcuVG5uri644AKtXLlSl156adAcevbsqU6dOmnr1q36zW9+U2O1Op1lTl23FgEyMzOVlJQkt9utxMREu9OpHm+8YXcGxSZNsjsDAACAsFi+2e4Mig3tXPbjkZSrFFn5RlKugB1yc3O1c+dOtWjRQnFxcXan84vUvXt3JScna9WqVXanElJ5x0lVezncAwsAAAAAAMCh0tLS9O2332rSL3yxCV8hBAAAAAAAcJjNmzfrm2++0RNPPKFGjRpp3LhxdqdkKxpYAAAAABBB+Moj8MuwZMkSzZo1S+3atdPf//73X/zXN/kKIQAAAAAAgMP8+c9/ltfr1datWzVw4EC707EdDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAUC5jjN0pwMFq+viggQUAAAAAAEKKjo6WJBUUFNicCZzMd3z4jpfqRgMLAAAAAACEVKtWLcXGxsrtdrMKC0EZY+R2uxUbG6tatWrVyGu4auRZAQAAAADAGaN+/frat2+f9u7dq6SkJNWqVUuWZdmdFmxmjFFBQYHcbreys7PVpEmTGnstGlgAAAAAAKBMiYmJkqT09HTt27fP5mzgNLGxsWrSpIn/OKkJNLAAAAAAAEC5EhMTlZiYqIKCAnk8HrvTgUNER0fX2NcGS6KBBQAAAAAAKqxWrVphaVgAJXETdwAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADiay+4EAAAAcOZYvtnuDIoN7Wx3BgAAoLqwAgsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACOxk3cAQAAAAA1gj/sAKC6sAILAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACOVuUG1tdff61bbrlFnTp1Up06ddS8eXNdffXV2r59e8B2U6ZMkWVZpf5r3759VVMAAAAAAADAGcxV1Sd49NFH9fnnn2vs2LHq0qWLDh48qOeff149evTQunXr1LlzZ/+2sbGxevXVVwN+PikpqaopAAAAAAAA4AxW5QbWHXfcob/97W+KiYnxx8aNG6fzzjtPjzzyiN58883iF3O5NGHChKq+JAAAAAAAAH5BqvwVwn79+gU0rySpTZs26tSpk7Zu3Vpqe4/Ho8zMzKq+LAAAAAAAAH4hauQm7sYYHTp0SPXr1w+Inzx5UomJiUpKSlJycrJuvvlmZWdn10QKAAAAAAAAOENU+SuEwSxcuFD79u3TrFmz/LFGjRrp7rvvVo8ePeT1evXJJ5/ohRde0MaNG7VmzRq5XKFTycvLU15env/fvhVchYWFKiwslCRFRUUpKipKXq9XXq/Xv60v7vF4ZIwpNx4dHS3LsvzPWzIuFa0gq0jc5XLJGBMQtyxL0dHRpXK0LEvRkrw//+fP8ef/QsU9kkwF4tGSLEmBFRXF9fP2AfGf348q1xQkHvH7iZqoiZqoiZqoiZrKzN2Yn68wTGDciiqqKTBuyYqKljFeyXjLj1tRsqyo0HFv4FWQ11t+TYEvGzz3UPHqrqmwsOz9ZLyha5VVVJPxnnLFV0M1FRaWf+xVdD+Fq6ayxlNxmtVz7FWlppJDLdQ4k8I/nkLFjSn7HFG0ffBaA8JhOEdwLqcmarK3plPrqqxqb2Bt27ZNN998s84//3xNnjzZH58zZ07AduPHj1fbtm113333acmSJRo/fnzI55wzZ45mzpxZKr5hwwbVqVNHkpSamqpWrVpp586dOnLkiH+bpk2bqmnTptq+fbvcbrc/3rJlSzVo0ECbN29WTk6OP96+fXvVq1dPGzZsCNjZXbp0UUxMjNLS0gJy6NWrl/Lz8/Xdd9/5Y9HR0erdu7fcbre2bdvmj8fHx6tr165KT0/Xjh07/PGkpCR1kLS/Vi3trVXLH08tLFSr/HztjInRkRINvqYFBWpaUKDtsbFyR0f74y3z89WgsFCb4+KUE1W8uK59bq7qeb3aEB8vj2UV15SToxhjlFa7dmBNHk/11NShg/bv36+9e/cW1xTp+4maqImaqImaqImayqxJtXvJePJVkF5ck2VFK6Zhb5l8twoyimuyXPGKSe0qb066Ct3FNUXFJqlWcgd5svfLk11cU3R8qlz1Wsnj3ilPTnFN0QlN5arbVIXHt8ubV1xTesPya8o/XlxTrfpdZEXHKP9QYE0xZ4enprS0svdTfpbkSmqp6NoNVHB0s0xhcU21ktvLiq2ngsMbZEzN15R2svxjr6L7KRw1lTee8rMqvp9quqa0k8U1hTpHKD784ylUTe7mZZ8j7BpPwWriXE5N1GRvTVW9nZRlSrbGqujgwYO64IILVFBQoHXr1qlx48Zlbp+Tk6OEhARNnTq11F8nLCnYCqxmzZrp6NGjSkxMlHQGdDwXLnTOCqyJE6unJjrT1ERN1ERN1ERNv7iaVm11zgqsSzqXX9OqLSVf1t4VWEM6lL2fVm0JXWu4V2AN6Vj+sbdsk3NWYF3SqezxVHwc2L8Ca0jH4nCocfbpNueswBp6XtnniOWbnLMCa0gHzuXURE121pSZmamUlBS53W5/L6cyqm0Fltvt1mWXXabjx49r7dq15TavpKIOYEpKijIyMsrcLjY2VrGxsaXiLper1FcPfW/aqXw7tqLxUF9prEzcsqyg8VA5+hpQFY0Hzzx0PNTOLhX/eZVWtdRUyXhE7CdqoqYQOVY2Tk3UJFFTqBwrG6cm59TkX+xtBa8peDxKskrnWOl4VGDuvrLLqinI0wTNMVS8OmtyucreTyV/7NRai+MVzz1UvCI1ldztoY6xiu6n8uPVU1NZ4+nUNKt67JUfD517sKEW6hwRzvEUKu4b86HOEZXZfzVdE+dyagoVp6bw1FTWraMqoloaWLm5uRoxYoS2b9+ulStXqmPHjuX/kKSsrCylp6crNTW1OtIAAAAAAOC0Ld9sdwbFhna2OwPAWarcwPJ4PBo3bpy+/PJLvffeezr//PNLbZObm6uCggLVrVs3IP7QQw/JGKNhw4ZVNQ0AAAAAAACcoarcwLrzzjv1/vvva8SIEcrIyNCbb74Z8PiECRN08OBBde/eXddcc43at28vSVq2bJk++ugjDRs2TFdeeWVV0wAAAAAAAMAZqsoNrG+//VaStHTpUi1durTU4xMmTFC9evV0xRVXaMWKFXr99dfl8XjUunVrzZ49W3fddVfQ71MCAAAAAAAAUjU0sNasWVPuNvXq1dOCBQuq+lIAAAAAAAD4BWLpEwAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAczWV3AgAAAAAAoHKWb7Y7g2JDO9udAX4JWIEFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR3PZnQAAAADKtnyz3RkUG9rZ7gwAAMAvESuwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoLrsTQJEf0+3OoFgruxMAAAAAAAAogRVYAAAAAAAAcDRWYAEAAAAAgBq1fLPdGRQb2tnuDHA6WIEFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABH4x5YqDS+uwwAAAAAAMKJFVgAAAAAAABwNBpYAAAAAAAAcDQaWAAAAAAAAHA0GlgAAAAAAABwNBpYAAAAAAAAcDQaWAAAAAAAAHA0GlgAAAAAAABwNBpYAAAAAAAAcDSX3QkAAAAAAAA4xfLNdmdQbGhnuzNwDlZgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNGq3MD6+uuvdcstt6hTp06qU6eOmjdvrquvvlrbt28vte3WrVs1bNgwJSQkKDk5WRMnTtSRI0eqmgIAAAAAAADOYK6qPsGjjz6qzz//XGPHjlWXLl108OBBPf/88+rRo4fWrVunzp07S5L27t2rCy+8UElJSZo9e7ays7P1+OOPa9OmTVq/fr1iYmKqXAwQzPLNdmdQbGhnuzMAAAAAACDyVLmBdccdd+hvf/tbQANq3LhxOu+88/TII4/ozTfflCTNnj1bJ06c0DfffKPmzZtLkvr06aNLLrlE8+fP13XXXVfVVAAAAAAAAHAGqvJXCPv161dq9VSbNm3UqVMnbd261R975513dMUVV/ibV5J08cUXq23btlq0aFFV0wAAAAAAAMAZqkZu4m6M0aFDh1S/fn1J0r59+3T48GH16tWr1LZ9+vTRhg0baiINAAAAAAAAnAGq/BXCYBYuXKh9+/Zp1qxZkqQDBw5Ikho1alRq20aNGikjI0N5eXmKjY0N+nx5eXnKy8vz/zszM1OSVFhYqMLCQklSVFSUoqKi5PV65fV6/dv64h6PR8aYcuPR0dGyLMv/vCXjkuTxeCoUd7lcMsYExC3LUnR0dKkcLcuSJBlJxirxJKaow+iVpBJxyxT901ty29OM69TXlPzvR6iajLdk3JIVFS1jvJLxlh+3omRZUaHjXs/P70R58YrvJ+Mt2r7oH4E1WVFFNQXGa66mwkLnHXvB4pE+nqiJmqiJms60mszPFwN2zrnGW1STr7RQuRvjjDlXkrze8vdT4MsGzz1c1xGFhWUfe0XXNBXbTzVdU2Fh+eOpuo+9qtZU1jmiOM3wjqdguZc8fYQaZ1L4x1OouDFln/cCPzsobOMpWLwi53LfZ4dwjqdQ8ZKfHYKNM8m+8XRqTVL5c66/3DCOp1DxkodrsOsI43XGnCsVHQdnyrXRqeeJyqr2Bta2bdt088036/zzz9fkyZMlSTk5OZIUtEEVFxfn3yZUA2vOnDmaOXNmqfiGDRtUp04dSVJqaqpatWqlnTt3Bvxlw6ZNm6pp06bavn273G63P96yZUs1aNBAmzdv9ucnSe3bt1e9evW0YcOGgJ3dpUsXxcTEKC0tLSCHXr16KT8/X999950/Fh0drd69e8vtdmvbtm3+eHx8vLp27ar09HTt2LHDH09KSlKMJHdCLbkTavnjCTmFSnHn61hSjLLji3dVUnaB6mUX6Ei9WOXGRvvjye581c0p1MGUOBW4ihfXNcjIVXy+V3sbxMtYxd2qRuk5cnmM9pxdO6CmFh5PmTXlHyquyXLFKya1q7w56Sp0F9cUFZukWskd5MneL0/23uLniU+Vq14redw75ckp3k/RCU3lqttUhce3y5tXvJ9cSS0VXbuBCo5uliks3k+1ktvLiq3YfsrPkmLO7iXjyVdBenFNlhWtmIa9ZfLdKsgIT01pJ5137HXo0EH79+/X3r3FNUX6eKImaqImajrTasrPsn/OLTi8QcZ4lHay7JpU2xlzriSlNyx/P+UfL95Ptep3kRUdo/xDgTWF6zoiLa3sYy8/q+L7qaZrSjtZ/niq7mOvKjWVd47Iz6r4fqrpmnxjTAp9jlB8+MdTqJrczcs+79k1noLVVJFzeX5W+MdTqJrSTpY9P0n2jKdgNUnlz7m+cRbO8RSqJt84C3UdUZDjjDlXKjoOzpRrI99ipNNlmZKtsSo6ePCgLrjgAhUUFGjdunVq3LixJCktLU29e/fWG2+8oYkTJwb8zN133625c+cqNze3UiuwmjVrpqNHjyoxMVGS839zKpXd8dz1zELHrMBqffvEMmtavsn+3/T4OtMXtS9/P63aIlt/01My9yEdnXfsReJKBGqiJmqipl9aTau2SHbPub7fBg/pWHbuq7Y6Y86VpEs6l7+fit7b4lqD5R6u64ghHco+9oquaZyxAmtIx/LH07JNzlmBdUmnss8RxceB/SuwfGNMCj3OPt3mnBVYQ88r+7wX+NlBYRtPweJDOpR/Lvd9dnDCCqySnx2CjbOVW5yzAuvSLuXPuf5x5oAVWCXHWbDriFVbnDHnSkXHwZlybZSZmamUlBS53W5/L6cyqm0Fltvt1mWXXabjx49r7dq1/uaVVPzVQd9XCUs6cOCAkpOTQzavpKKVW8Eed7lccrkCS/C9aafy7diKxk993tOJW5YVNB4qR0vFTaWA7aWAY9ofD9F6rGz81Nf0faUxVE1WVLB4lGQFqamy8ajg+yNUvCL7I+BlrOA1BY9Xf00l03XSsVfZeCSMJ2qiplA5VjZOTdQk2V9TyenFrjnXN/+fmuqpufsXe9s850qSb1eWtZ+CPE3QHEPFq7Mml6vsYy/gOChnP5V+oHprKrnbQ17bVvOxV/qBytVU1jni1DTDNZ5KP+AqNcak0OeIcI6nUHHfmA91fqvM/qvpmipyLg8cZ+EZT6HiFRpnNo2nYPHy5tYKj7Mw1HTq4XrqOcKXlt1zrhR4HET6tVGo/CuqWhpYubm5GjFihLZv366VK1eqY8eOAY83adJEqamppZeYS1q/fr26detWHWkAAAAAAADgDFTlv0Lo8Xg0btw4ffnll1q8eLHOP//8oNuNHj1aH3zwgfbs2eOPrVq1Stu3b9fYsWOrmgYAAAAAAADOUFVegXXnnXfq/fff14gRI5SRkaE333wz4PEJEyZIku69914tXrxYgwcP1m233abs7GzNnTtX5513nqZOnVrVNAAAAAAAAHCGqnID69tvv5UkLV26VEuXLi31uK+B1axZM3322We644479Mc//lExMTG6/PLL9cQTT5R5/ysAAAAAAAD8slW5gbVmzZoKb9upUyctW7asqi8JAAAAAACAX5Aq3wMLAAAAAAAAqEnV8lcIAQAAIsnyzXZnUGxoZ7szAAAAcD5WYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0Vx2JwCg2PLNdmdQbGhnuzMAAAAAAKAIK7AAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaC67EwAAAGeG5ZvtzqDY0M52ZwAAAIDqxAosAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADhatTSwsrOz9eCDD2rYsGFKTk6WZVmaP39+qe2mTJkiy7JK/de+ffvqSAMAAAAAAABnIFd1PEl6erpmzZql5s2bq2vXrlqzZk3IbWNjY/Xqq68GxJKSkqojDQAAzijLN9udQbGhne3OAAAAAL9k1dLAatSokQ4cOKCGDRsqLS1NvXv3Dv2CLpcmTJhQHS8LAAAAAACAX4Bq+QphbGysGjZsWOHtPR6PMjMzq+OlAQAAAAAAcIYL+03cT548qcTERCUlJSk5OVk333yzsrOzw50GAAAAAAAAIkS1fIWwoho1aqS7775bPXr0kNfr1SeffKIXXnhBGzdu1Jo1a+RyBU8nLy9PeXl5/n/7Vm8VFhaqsLBQkhQVFaWoqCh5vV55vV7/tr64x+ORMabceHR0tCzL8j9vybhUtHqsInGXyyVjTEDcsixFR0eXytGyLEmSkWSsEk9iijqMXkkqEbdM0T+9Jbc9zbhOfU3J/36Eqsl4S8YtWVHRMsYrGW/5cStKlhUVOu71/PxOlBev+H4y3qLti/4RWJMVVVRTYLzmaiosLPvYkywZb2BNoXKv6ZqkyB1PweKRfo6gpl9oTd7S5z27zhGFheXXZMzpnctroiaPp+z9VNPzU2VqMqb8Y8/8fDFg55zrq8k3rEKNG2OcMedKktdb/jki8GXtmXN9NQUbZyVzL7qmCf94CpZ7YWH55z07xlNZNZV1Li9OM7zjKVjuJaeuUONMCv94ChU3puw5N/Czg8I2noLFK3Id4fvsYOecW3KclXUdITljzi36tFn+tZG/XBvnXF+85OEa7HrPeJ0x50pFx0HEXcOGmHNPPU9UVlgbWHPmzAn49/jx49W2bVvdd999WrJkicaPHx/y52bOnFkqvmHDBtWpU0eSlJqaqlatWmnnzp06cuSIf5umTZuqadOm2r59u9xutz/esmVLNWjQQJs3b1ZOTo4/3r59e9WrV08bNmwI2NldunRRTEyM0tLSAnLo1auX8vPz9d133/lj0dHR6t27t9xut7Zt2+aPx8fHq2vXrkpPT9eOHTv88aSkJMVIcifUkjuhlj+ekFOoFHe+jiXFKDu+eFclZReoXnaBjtSLVW5stD+e7M5X3ZxCHUyJU4GreHFdg4xcxed7tbdBvIxV3K1qlJ4jl8doz9m1A2pq4fGUWVP+oeKaLFe8YlK7ypuTrkJ3cU1RsUmqldxBnuz98mTvLX6e+FS56rWSx71Tnpzi/RSd0FSuuk1VeHy7vHnF+8mV1FLRtRuo4OhmmcLi/VQrub2s2Irtp/wsKebsXjKefBWkF9dkWdGKadhbJt+tgozw1JR2suxjT6qngsMbZEqcbGvV7yIrOkb5hwKPvZquSYrc8dShQwft379fe/cW1xTp5whq+mXWlH+49HnPrnNEWlr5NXnM6Z3La6Kmzabs/VTT81NlasrJKf/Yy8+yf8711ZR2sigeajyptjPmXElKb1j+OSL/uP1zrq+mtLSyzxH5WfaMp2A1pZ0s/7xnx3gKVVN55/L8rIrvp5quyTfGpNDzk+LDP55C1eRuXvaca9d4ClZTRa4j8rPsn3N9NaWdLPs6QnLGnGu54iWVf23kG2d2zrm+mnzjLNT1XkGOM+Zcqeg4iLRr2FBzblVvJWWZkq2xauC7ifu8efM0ZcqUcrfPyclRQkKCpk6dWuqvE/oEW4HVrFkzHT16VImJiZIi/7f2u55Z6JgVWK1vn1hmTcs32f+bHl9n+qL25e+nVVtk6296SuY+pGPZx96K7+3/TY8v90vPi9zxxMoeajpTalr5vXNWYA3pUH5Nq7Y6ZwXWxZ3K3k/LNjlnBdbQzuUfe6u2SHbPub6ahnQsCocaN6u2OmPOlaRLOpd/jih6b4trDZZ7uK4jgo2zkrkXXdM4YwXWkI7ln/dCjjMbzhGXdCr7XF58HNi/Ass3xqTQ4+zTbc5ZgTX0vLLn3MDPDgrbeAoWH9Kh/OsI32cHJ6zAKvnZIdg4W7nFGXOuZOnSLuVfG/nHmQNWYJUcZ8Gu91ZtccacKxUdB5F2DRtqzs3MzFRKSorcbre/l1MZYV2BFUx8fLxSUlKUkZERcpvY2FjFxsaWirtcrlJfO/S9aafy7diKxkN9nbEyccuygsZD5WipuKkUsL0UcEz74yFaj5WNn/qavq80hqrJigoWj1LR186qGI8Kvj9CxSuyPwJexgpeU/B49ddUMt1Qx16w97fogYrHq6umSB5PlY1TEzWFittZU5Bhads5wuUqvybfIt/Knstroibf2xpyzq3h+akyNVlW+cdeyZTsmnN9NZ2a6qm5+xd72zznSpJv15d1jgg2zuyYc0ONs5K5BxwHYRxPJXP0JVFyt1d6nNl0jijrXH5qmnaeI4JNUaHOEeEcT6HivjEfam6t3PmwZmuqyHVE4Diz97q8QuPMAXNueTlWepyFoaZTD9dTzxG+tOyec6XA4yBSrmFD5Rgq/4oKNmWHVVZWltLT05Wammp3KgAAAAAAAHCgsDWwcnNzlZWVVSr+0EMPyRijYcOGhSsVAAAAAAAARJBq+wrh888/r+PHj2v//v2SpKVLl/pvAHbrrbfq2LFj6t69u6655pqfb1YtLVu2TB999JGGDRumK6+8srpSARAmyzfbnUGxoZ3tzgAAAAAAUFOqrYH1+OOPa/fu3f5//+Mf/9A//vEPSdKECRNUr149XXHFFVqxYoVef/11eTwetW7dWrNnz9Zdd90V9DuVAAAAAAAAQLU1sHbt2lXuNgsWLKiulwMAAAAAAMAvBMueAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaC67EwAAIJyWb7Y7g2JDO9udAQAAABAZWIEFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEdz2Z0AAITD8s12Z1BsaGe7MwAAAACAyMIKLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaN3EHAFQJN8gHAAAAUNNYgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHc9mdAACgtOWb7c6g2NDOdmcAAAAA4JeOFVgAAAAAAABwNBpYAAAAAAAAcDQaWAAAAAAAAHA0GlgAAAAAAABwtGppYGVnZ+vBBx/UsGHDlJycLMuyNH/+/KDbbt26VcOGDVNCQoKSk5M1ceJEHTlypDrSAAAAAAAAwBmoWv4KYXp6umbNmqXmzZura9euWrNmTdDt9u7dqwsvvFBJSUmaPXu2srOz9fjjj2vTpk1av369YmJiqiMdAAAAAAAAnEGqpYHVqFEjHThwQA0bNlRaWpp69+4ddLvZs2frxIkT+uabb9S8eXNJUp8+fXTJJZdo/vz5uu6666ojHQAAAAAAAJxBquUrhLGxsWrYsGG5273zzju64oor/M0rSbr44ovVtm1bLVq0qDpSAQAAAAAAwBkmbDdx37dvnw4fPqxevXqVeqxPnz7asGFDuFIBAAAAAABABKmWrxBWxIEDByQVfd3wVI0aNVJGRoby8vIUGxtb6vG8vDzl5eX5/52ZmSlJKiwsVGFhoSQpKipKUVFR8nq98nq9/m19cY/HI2NMufHo6GhZluV/3pJxSfJ4PBWKu1wuGWMC4pZlKTo6ulSOlmVJkowkY5V4ElPUYfRKUom4ZYr+6S257WnGdeprSv73I1RNxlsybsmKipYxXsl4y49bUbKsqNBxr+fnd6K8eMX3k/EWbV/0j8CarKiimgLjNVdTYWHZx55kyXgDawqVe03XJJU/nvw/Us5+CkdNvkMh1DgzpnqPvarUVFhY/jnCeMM/nkLVVFhY9nnP99LhHk/B4r7joKxzuTEK+3gKVZNUzvzktWc8BYsXFpY+F4QcZ2EcT6Fq8nhCz7lFx4E94ylYTcaUfx1hfr4YsHPO9dVUcpxJpXM3xhlzriR5veVf7wW+rD1zrq+mYOOsZO5F1zT2z7lS0XEQas715e6EObdkTWVdlxenae+cK+NRyakr1DiT7J9zfYwp+7o88LODwjaegsUr8pnQ99nBzjm35Dgr63Ou5Iw5V7IkhZ5zS40zG+dcX7zk4Rrsutx4nTHnSkXHQU33I8o6l1dnj+XU80Rlha2BlZOTI0lBG1RxcXH+bYI9PmfOHM2cObNUfMOGDapTp44kKTU1Va1atdLOnTsD/qph06ZN1bRpU23fvl1ut9sfb9mypRo0aKDNmzf7c5Ok9u3bq169etqwYUPAzu7SpYtiYmKUlpYWkEOvXr2Un5+v7777zh+Ljo5W79695Xa7tW3bNn88Pj5eXbt2VXp6unbs2OGPJyUlKUaSO6GW3Am1/PGEnEKluPN1LClG2fHFuyopu0D1sgt0pF6scmOj/fFkd77q5hTqYEqcClzFi+saZOQqPt+rvQ3iZaziblWj9By5PEZ7zq4dUFMLj6fMmvIPFddkueIVk9pV3px0FbqLa4qKTVKt5A7yZO+XJ3tv8fPEp8pVr5U87p3y5BTvp+iEpnLVbarC49vlzSveT66kloqu3UAFRzfLFBbvp1rJ7WXFVmw/5WdJMWf3kvHkqyC9uCbLilZMw94y+W4VZISnprSTZR97Uj0VHN4gU+JkW6t+F1nRMco/FHjs1XRNUvnjKT+rYvspHDWlnSyKJyUlqUOHDtq/f7/27i2uyVNYvcdeVWrakFf+OSL/UPjHU6iayjvv5WfZM56C1eQ7Dso6l8uEfzyFqkkqe37KP2zPeApWU1pacU2h5lyPCf94ClXTZhN6zu3Qwb7xFKymnJzyryPys+yfc301+cZZqGsj1XbGnCtJ6Q3Lv97LP27/nOurKS2t7GvY/CxnzLlS0TVNqDnXd45wwpzrq6m863LfNY3dc27+oTT/GJNCf9ZQvP1zro+7edmfn5wy57rqVuwzYX6W/XOur6a0k2V/zpWcMedarnhJoedc3znCN87snHN9NfnGWajP7gU5zphzpaLjoKb7EWWdy6uzx+JbjHS6LFOyNVYNfDdxnzdvnqZMmVIq/sYbb2jixIkBP3P33Xdr7ty5ys3NrfAKrGbNmuno0aNKTEyUFPkrsHY9s9AxK7Ba3z6xzJqWb7L/Nz2+zvRF7cvfT6u2yNbf9JTMfUjHso+9Fd/b/5seX+6Xnlf+eFq1JXStvhzD9durIR1/joYYZ6u22v+bHp8hHcs/R6zYbO9vekrmPqRD2ec933HghBVYvuOgrHP58s2ybXVFsHFW1vy08nvnrMAa0qH838j5x5kDfht8caeyf8u4bJN9qytOjQ/tXP51RNE4c8Zvg0uOM6l07qu2OmPOlaRLOpd/veefy36uNVju4TpHBBtnJXMvuqaxf86Vio6D8n5rH3Kc2XCOuKRT2dflxceB/SuwfGNMCj3OPt1m/5zrM/S8sj8/BX52UNjGU7D4kA7lfyb0fXZwwgqskp8dgo2zlVucMedKli7tUv7KnlKfHWy8Li85zoJdl6/a4ow5Vyo6Ds6UFViZmZlKSUmR2+3293IqI2wrsHxfHfR9lbCkAwcOKDk5OWjzSipatRXsMZfLJZcrsATfm3Yq346taPzU5z2duGVZQeOhcrQkf1MpYHsp4Jj2x0O0HisbP/U1fV9pDFWTFRUsHiVZQWqqbDwq+P4IFa/I/gh4GSt4TcHj1V9TyXRDHXvB3t+iByoer66ayhtPp/5I6P1X8zWdeiicmrtv8WF1HXtVqcmXa1nnCCvYOaKGx1OomsobZyVfOpzjKVj81FSDn8dky3gKFS9rfgqyuW3nCJer/HOEf5yFcTwVv3ZgTb63NeSca9N4Cp57+dcRgePMnjnXV1N548y/2NvmOVeSfLu+rOu9YOPMrnNEsHFWMveA48DGOVcKPA4qPc5sOkeUdV1e6prGxnNEsGk31DnCzjm3+OdD51i0fWTMucX5lngem6/LKzTOHDDnlpdjpcdZGGo69XA99RzhS8vuOVcKPA5qsh9R2fjp9FhC5V9RwabsGtGkSROlpqaWXmYuaf369erWrVu4UgEAAAAAAEAECVsDS5JGjx6tDz74QHv27PHHVq1ape3bt2vs2LHhTAUAAAAAAAARotq+Qvj888/r+PHj2r9/vyRp6dKl/huA3XrrrUpKStK9996rxYsXa/DgwbrtttuUnZ2tuXPn6rzzztPUqVOrKxUAAAAAAACcQaqtgfX4449r9+7d/n//4x//0D/+8Q9J0oQJE5SUlKRmzZrps88+0x133KE//vGPiomJ0eWXX64nnngi5P2vAAAAAAAA8MtWbQ2sXbt2VWi7Tp06admyZdX1sgAAAAAAADjDhfUeWAAAAAAAAEBl0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKOFtYG1Zs0aWZYV9L9169aFMxUAAAAAAABECJcdLzp9+nT17t07INa6dWs7UgEAAAAAAIDD2dLAGjBggMaMGWPHSwMAAAAAACDC2HYPrKysLBUWFtr18gAAAAAAAIgQtjSwpk6dqsTERMXFxWnw4MFKS0uzIw0AAAAAAABEgLB+hTAmJkajR4/W8OHDVb9+fW3ZskWPP/64BgwYoC+++ELdu3cP+nN5eXnKy8vz/zszM1OSVFhY6F/FFRUVpaioKHm9Xnm9Xv+2vrjH45Exptx4dHS0LMsqtTosOjpakuTxeCoUd7lcMsYExC3LUnR0dKkcLcuSJBlJxirxJKaow+iVpBJxyxT901ty29OM69TXlPzvR6iajLdk3JIVFS1jvJLxlh+3omRZUaHjXs/P70R58YrvJ+Mt2r7oH4E1WVFFNQXGa66mwsKyjz3JkvGesjIxRO41XZNU/njy/0g5+ykcNfkOhVDjzJjqPfaqUlNhYfnnCOMN/3gKVVNhYdnnPd9Lh3s8BYv7joOyzuXGKOzjKVRNUjnzk9ee8RQsXlhY+lwQcpyFcTyFqsnjCT3nFh0H9oynYDUZU/51hPn5YsDOOddXU8lxJpXO3RhnzLmS5PWWf70X+LL2zLm+moKNs5K5F13T2D/nSkXHQag515e7E+bckjWVdV1enKa9c66MRyWnrlDjTLJ/zvUxpuzr8sDPDgrbeAoWr8hnQt9nBzvn3JLjrKzPuZIz5lzJkhR6zi01zmycc33xkodrsOty43XGnCsVHQc13Y8o61xenT2Wqn4LL6wNrH79+qlfv37+f48cOVJjxoxRly5dNGPGDH3yySdBf27OnDmaOXNmqfiGDRtUp04dSVJqaqpatWqlnTt36siRI/5tmjZtqqZNm2r79u1yu93+eMuWLdWgQQNt3rxZOTk5/nj79u1Vr149bdiwIWBnd+nSRTExMaVWi/Xq1Uv5+fn67rvv/LHo6Gj17t1bbrdb27Zt88fj4+PVtWtXpaena8eOHf54UlKSYiS5E2rJnVDLH0/IKVSKO1/HkmKUHV+8q5K</t>
+  </si>
+  <si>
+    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACGwElEQVR4nOzdd3xUVf7/8fdNhnQSDEUCAaSXUJWiKNKUooJLExSk7s+yKrq66qLrYgVdWfu6a/kKKLiKWHFFKYKLCmIUBQREpUiHUBIC6XN+f2RnkiEzKSSZewdfz8eDh+bMnbmfz9x77rnzmXPvWMYYIwAAAAAAAMChwuwOAAAAAAAAACgNBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAKmj8+PGyLEtjxowp1/JPPvmkLMtSu3btqjmysvXp00eWZWnlypW2rH/ixImyLEtz5syxZf1Vxe738bfknHPOkWVZ2rFjh92hAAAAG1HAAgCggqZMmSJJeu+993T06NEyl589e7bP86rL/fffL8uydP/991fres50ofQ+BrOQtnLlSlmWpT59+lT7ugAAAE5FAQsAgAq6+OKL1aJFC+Xk5Gj+/PmlLvv1119rw4YNqlGjhq699togRRjYq6++qs2bN6t79+52hxLSeB8BAACCiwIWAAAVZFmWJk+eLKlodlUgnsevuOIK1atXr9pjK0vjxo3Vpk0bxcTE2B1KSON9BAAACC4KWAAAnIaJEycqPDxc3377rdavX+93mezsbP373/+WVPLywW+++UZjx45V48aNFRkZqcTERA0cOFAfffSR39cqfh+g999/X/369VNiYqL38jHLsvTAAw9Ikh544AFZluX9N3HiRO/rlHXJ2aeffqpRo0YpOTlZkZGRqlu3rrp166bp06fr8OHD3uXy8vI0b948jR07Vm3atFF8fLyio6PVunVrTZ06VXv37i3vW1mmOXPmePM4fPiwbrrpJu/71qRJE/3xj38MeCnnO++8o9///vdq3769zjrrLEVFRalp06aaPHmyfvzxxxLLV9X7uHz5cg0fPlxJSUmKiIhQvXr1NGzYMK1evdrv8p51SNLbb7+tiy66SPHx8YqNjdWFF15YYr/wbPPPPvtMktS3b1+fWIvfY+ybb77R6NGjlZycrIiICMXHx6tZs2YaMWKE3n//fb/xnKpPnz7q27evJOmzzz7zWdc555zjs2x+fr7+9a9/qWfPnkpISFBUVJRatmypqVOnas+ePeVaXyDvvvuu972pWbOm+vTpE7DPeCxcuFCDBg1S3bp1FRERoYYNG2rcuHHatGlThdf/008/afLkyWratKkiIyMVFxenJk2a6PLLLw9YzN66dauuv/56NW/eXFFRUUpISNDFF1+sefPmVVncO3bs8G4LY4xefPFFnXfeeYqNjVVCQoIGDBgQcN8DACBkGAAAcFqGDBliJJmpU6f6fXz+/PlGkmnQoIHJz8/3tj/11FMmLCzMSDKdO3c2I0eONBdddJGJiIgwkswDDzxQ4rWaNGliJJmbb77ZSDJdu3Y1V199tendu7f573//ayZMmGA6depkJJlOnTqZCRMmeP+99NJL3tfp3bu3kWRWrFhRYh233HKLkeSNa8yYMWbw4MGmWbNmJZ6za9cuI8kkJCSY888/34waNcpcdtllpkGDBkaSqVu3rvnpp59KrGPChAlGkpk9e3a53+fZs2cbSWbo0KGmefPmplatWuZ3v/udGTZsmDnrrLOMJNO6dWtz8ODBEs8NDw83MTExpmvXrmb48OFm6NCh3nxiY2PNF198USK+yr6Pd9xxh5FkwsLCTPfu3c2oUaNMjx49jGVZJjw83LzyyislnuN53//6178ay7LMhRdeaEaPHu2NxbIs884773iX37x5s5kwYYI5++yzjSQzcOBAn1hXrVpljDFm2bJlpkaNGt58Ro4caYYNG2a6d+9uIiMjzZVXXlmubTBz5kwzcOBAI8mcffbZPuu64447vMtlZ2ebSy65xEgyUVFRZvDgwWb06NGmUaNGRpKpU6eO+eabb8q1Tg/Pvv/HP/7RZ9/v3r2793175plnSjwvLy/PXHXVVUaSiYyMND179jSjRo3yvqfR0dFm8eLF5Y5jw4YNJj4+3ru/DR8+3IwaNcpccMEFJi4uznTq1KnEcxYsWGCioqKMJNOmTRszbNgw069fPxMbG2skmUmTJlVJ3Nu3bzeSTJMmTcyECRNMjRo1TL9+/cxVV11lWrVq5X2tNWvWlDtfAACchgIWAACn6b333jOSTO3atU1OTk6Jxz0f5O+55x5v28cff2wsyzJ16tQxn332mc/y69evN8nJyUaSWblypc9jng/x4eHh5v333/cbz/Tp040kM3369IAxByq8PPPMM95cPv300xLP++qrr8yvv/7q/TsjI8O8//77JfLOzc0106ZNM5LMZZddVuJ1KlPAkmTOP/98c/jwYe9jR48eNT179jSSzJgxY0o894033jCZmZk+bW632/zjH/8wkkxKSopxu90+j1fmfXzxxReNJNOiRQvz/fff+zz22WefmZo1a5qIiAizdetWn8c8+dWqVatEkcETT6tWrcodh0ffvn2NJDNv3rwSjx07dsysXr06YI6nWrFihZFkevfuHXCZu+++20gyzZs3N9u3b/e25+bmmilTphhJpmnTpn77SyCefd+yrBJ5vPHGG8ayLONyucyGDRt8HrvnnnuMJNOjRw+zbds2n8feeustEx4ebs466yxz9OjRcsUxadIkI8k8/PDDJR47efKk3/4cGRlpoqKizNtvv+3z2I4dO0yHDh2MJDN37txKx+0pYHmKWD/++KP3sfz8fDN58mQjyQwYMKBcuQIA4EQUsAAAOE15eXmmfv36RpJ56623fB7buXOnd5ZV8ZlIPXr0MJLMwoUL/b7mggULjCQzYsQIn3bPh/jJkycHjOd0Cy95eXmmbt26RlKJD9qnq0GDBiYsLMxkZGT4tFe2gLVu3boSj69fv95YlmXCwsLMrl27yv26F1xwgZFkfvjhB5/2030fCwoKvDPQUlNT/T7vb3/7m5HkM2vJmKIClr+ZRNnZ2SYhIcFI8ikiBoqjuHbt2hlJ5siRIwFzKa+yClhZWVkmLi7OSDIffPBBicdPnDjhnTE2f/78cq/Xs+//7ne/8/v4iBEjjCTz//7f//O2HT582ERHR5uoqCize/duv8/7wx/+YCSZZ599tlxxXHbZZUaS+fbbb8u1/OjRo40kM2vWLL+Pr1271kgy5513XqXjLl7A8vfe79u3zzsLKzc3t1zxAwDgNNwDCwCA0+RyuTRhwgRJ0iuvvOLz2OzZs+V2u9W7d2+1aNFCkpSWlqa1a9cqOjpaQ4YM8fuaffr0kSR9+eWXfh8fOXJkFUVf5JtvvtGhQ4dUp04dDRs2rELP/f777/XEE0/olltu0eTJkzVx4kRNnDhR+fn5crvd+vnnn6sszk6dOqlz584l2jt06KAuXbrI7Xbrv//9b4nHf/75Zz333HO67bbbNGXKFG+MBw4ckCS/98I6HevWrdPevXvVvHlznXfeeX6XKWv7+tsvIiMj1axZM0mq8D2kPL+SOHbsWH3++efKz8+v0PMrIjU1VZmZmUpMTPSbR0xMjMaMGSNJWrFiRYVf39PXArUXvx/ZihUrlJWVpQsvvFANGzb0+7yytsWpPO/ljTfeqE8++UTZ2dkBl3W73Vq8eLEkafTo0X6X6dq1q+Li4rRu3Trva1U2bpfLpUGDBpVor1+/vs466yzl5OT43MsOAIBQ4rI7AAAAQtnkyZP12GOPacmSJdqzZ48aNmwoY4z3JtrFb96+fft2GWOUlZWlyMjIUl/30KFDfttPvWF2Vdi5c6ckqXXr1t4biZflxIkTuvbaa/Xuu++WulxGRkal4/No2rRpqY99++232r17t7etoKBAN998s1544QUZY6o9xm3btkmSfvnllzLfx0Dbt3Hjxn7b4+PjJanUook/M2fO1Pr167V48WItXrxY0dHROvfcc9WnTx+NHTtWbdu2rdDrlcZTXCttOzVv3txn2YoI9Lqe9uLb3rMtli9fftrb4lR33nmnPv/8cy1btkyDBg1SjRo11KlTJ1188cUaM2aMunXr5l328OHD3v2qUaNGZb724cOH1bBhw0rHnZSUpBo1avhdPj4+XkePHq3wPgQAgFNQwAIAoBJatWqlXr16adWqVXr11Vc1bdo0rVixQjt27FBCQoLPjCm32y1JiouL04gRI05rfdHR0VUSd2VNmzZN7777rtq0aaNHH31U3bp1U506dRQRESFJ6tmzp1avXl1q4ag6FF/f008/rX/961+qX7++nnjiCfXs2VNnn322oqKiJEnXXHON/v3vf1dZjJ7tW79+fQ0cOLDUZevUqeO3PSysaifH169fX6mpqfrss8+0bNkyffHFF/rqq6/0xRdfaMaMGZo5c6buvvvuKl2nXYpvR8+2aNGihS688MJSn9emTZtyvX5MTIyWLl2qr7/+Wh9//LG+/PJLffnll0pNTdUTTzyhP/zhD/rHP/7hs34p8Myx4jwF7crGXdX7DwAATkIBCwCASpoyZYpWrVql2bNna9q0ad7LCceMGeNTcPLMxLAsS6+88opjPmx6Zv1s3bpVxphyzcJasGCBJOnNN99Ux44dSzz+008/VW2QKpzBFsiOHTskScnJyd42T4wvvPCChg4dWuI5VR2jZ/vWrl3bOwPPCSzLUp8+fbyXnmVnZ2vOnDm66aabdM8992jkyJHemVGV4bnkrbTt5JlhFOjyuNJs375dnTp1KtHub9t7tkXr1q2rfFt069bNO9sqPz9f7733nsaPH6/nn39eI0eOVN++fVWnTh1FR0crKytLs2bNCliwPFV1xg0AQKhzxpkzAAAhbNSoUYqPj9dPP/2kDz/8UO+8844k38sHJalBgwbq2LGjjh8/ro8//rjK4/DMfqrofY66du2qOnXq6NChQ3rvvffK9ZwjR45Ikpo0aVLisU8++URpaWkViqE81q9fr/Xr15do/+GHH/Ttt98qLCxMF198cbli/OGHH/Tdd9/5Xc/pvo+eWWibNm3SDz/8UKHnnq7TiTUqKko33HCDOnbsKLfb7fc9PZ11ee7pdOTIEX3wwQclHs/KytIbb7whSerbt2+54/V47bXX/La/+uqrkoruDSVJ/fv3V0REhFauXKmDBw9WeF3l5XK5NHLkSO+MO88+FR4erksvvVRSUSG1PIIVNwAAoYgCFgAAlRQTE6Orr75aUuE9sbKystShQwefe+J4PPzww5KkSZMmadGiRSUeN8boq6++0pIlSyoch2cGSkWLJy6XS/fee68k6brrrvN7I/Svv/7a5x5DnnsnPfvssz7L/fjjj7rhhhsqtP7yMsboxhtv1NGjR71t6enpuvHGG2WM0YgRI3zuN+SJ8R//+IfPJV379u3T+PHjAxZiTvd9rFGjhqZPny5jjIYNG6bPP/+8xDIFBQX69NNPtWbNmgq9diBlxTpr1iz9+uuvJdq3bNninYHmr8BX2rp++ukn5eXllXg8KipKN910kyTpjjvu8N5bTZLy8vJ06623av/+/WratOlp/RjBu+++6y2AeSxcuFBvv/22XC6XbrnlFm/72WefrVtuuUUnTpzQkCFDtGHDhhKvl5OTow8++EBbtmwp1/qff/55vzf8379/v1JTUyX5vpfTp09XRESE7rzzTs2dO9dnH/TYuHGjt+BdXXEDAHDGsOfHDwEAOLOsXbvW+zP2ksxTTz0VcNmnn37auFwuI8m0aNHCXH755eaaa64xl156qalXr56RZO6++26f5zRp0sRIMtu3bw/4uvv37zexsbFGkrnwwgvNxIkTzZQpU8wrr7ziXaZ3795GklmxYoXPc91ut7nhhhu88Xfp0sWMGTPGXHbZZaZZs2YlnvP2228by7KMJNOhQwczZswY069fP1OjRg3Tr18/07NnT7/rmTBhgpFkZs+eXdZb6jV79mwjyQwdOtQ0a9bM1KpVywwbNswMHz7cJCYmGkmmZcuW5sCBAz7PW7NmjYmIiPC+z1dddZUZNGiQiY6ONikpKWbYsGF+Y6nM+2iMMXfeeaf3fUxJSTFXXnmlGTNmjOnTp4+pVauWkWT++c9/+jzHs3wggdb34YcfGkkmIiLCXHHFFWby5MlmypQp5osvvjDGGJOQkGAkmTZt2phhw4aZa665xvTp08e7/40fP74cW6BI165djSTTunVrM3bsWDNlyhSffTU7O9v079/fSDLR0dHmsssuM6NHjzaNGzc2kkzt2rVNampqhdbp2fdvu+02I8l069bNXHPNNaZHjx7e9+2JJ54o8by8vDxzzTXXGEkmLCzMdOnSxYwYMcKMHj3aXHjhhd5tvHjx4nLF0alTJyPJNG3a1AwZMsSMHTvWDBgwwERHRxtJpl+/fiYvL8/nOQsWLDAxMTFGkklOTjYDBgwwY8eONYMHDzbJyclGkhk9enSl496+fbuRZJo0aVLm+1jaMQQAACejgAUAQBXp0KGDt5iQlpZW6rIbNmww1113nWnZsqWJiooyMTExplmzZmbgwIHmmWeeMXv27PFZvrwfPv/73/+aSy65xJx11lkmLCzMSDITJkzwPl5a4cUYYxYvXmyuvPJKc/bZZ5saNWqYunXrmu7du5sHHnjAHD58uMS6+vfvb+rUqWNiYmJM+/btzSOPPGJycnICrqcyBawJEyaYgwcPmuuvv94kJyebiIgI06hRIzN16tQSsXmsX7/eDB061CQlJZmoqCjTsmVLc9ddd5mMjIxSY6ns+/jFF1+YsWPHmiZNmpjIyEhTs2ZN06pVK/O73/3OvPzyy+bIkSM+y59uAcsYY1566SVz7rnnegslxXOaN2+emTRpkmnfvr1JTEw0kZGRpkmTJmbw4MHm3XffNW63O+A6/dm5c6e55pprTFJSkrcIdmrRJC8vzzz//PPm/PPPNzVr1jQRERGmefPm5pZbbjG7d++u0PqM8d33FyxYYC644AITFxdnYmNjTa9evcyiRYtKff5HH31khg8fbho2bGhq1KhhatWqZdq2bWvGjBljXn/9dXPixIlyxfHhhx+aG2+80XTp0sXUrVvXREREmOTkZNOnTx8zd+5ck5ub6/d527dvN3/84x9N+/btTWxsrImKijJNmjQxffr0MY8++qj5+eefKx03BSwAwG+BZUyQfx4IAACgAubMmaNJkyZpwoQJ3NgaAADgN4p7YAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNG4BxYAAAAAAAAcjRlYAAAAAAAAcDQKWAAAAAAAAHA0l90BnA632629e/eqZs2asizL7nAAAAAAAABQCmOMjh8/rgYNGigsrOLzqUKygLV37141atTI7jAAAAAAAABQAbt27VJycnKFnxeSBayaNWtKKkw6Pj7e5mgAAAAAAABQmoyMDDVq1Mhb06mokCxgeS4bjI+Pp4AFAAAAAAAQIk73VlDcxB0AAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjhaSv0IIAAAAAACCzxijgoIC5efn2x0KHMLlcik8PPy0f12w3Oup1lcHAAAAAAAhzxijY8eO6dChQyooKLA7HDhMeHi46tWrp4SEhGorZFHAAgAAAAAApdq/f7+OHTum+Ph4xcfHy+VyVfuMGzifMUb5+fnKyMjQvn37lJWVpaSkpGpZFwUsAAAAAAAQUEFBgdLT01W3bl3VqVPH7nDgQDVr1lRkZKTS0tJUr149hYeHV/k6uIk7AAAAAAAIKC8vT8YYxcbG2h0KHCw2NlbGGOXl5VXL61PAAgAAAAAAZeKSQZSmuvcPClgAAAAAAABwNApYAAAAAAAA8GvixIk655xz7A6DAhYAAAAAAPjtmjNnjizLCvhvzZo1dodYpk2bNun+++/Xjh077A6l2vArhAAAAAAA4DfvwQcfVNOmTUu0t2jRwoZoKmbTpk164IEH1KdPH0fMlqoOFLAAAAAAAMBpW7LR7gikAe0r/xqDBw9W165dK/9CqBZcQggAAAAAAFCK6dOnKywsTMuXL/dpv+666xQREaHvv/9ekrRy5UpZlqU333xT99xzj+rXr6/Y2FgNHTpUu3btKvG6X331lQYNGqSEhATFxMSod+/e+uKLL0ost2fPHk2ZMkUNGjRQZGSkmjZtqhtvvFG5ubmaM2eORo0aJUnq27ev99LHlStXep+/ePFi9erVS7GxsapZs6Yuv/xy/fDDDyXW895776l9+/aKiopS+/bt9e6771bmbatSzMACAAAAAAC/eenp6UpLS/NpsyxLtWvX1l/+8hctWrRIU6ZM0YYNG1SzZk198skneumll/TQQw+pU6dOPs975JFHZFmW7r77bh08eFBPPfWULrnkEn333XeKjo6WJH366acaPHiwzjvvPG+BbPbs2erXr59WrVql7t27S5L27t2r7t2769ixY7ruuuvUpk0b7dmzRwsXLtTJkyd18cUXa+rUqXrmmWd0zz33qG3btpLk/e9rr72mCRMmaODAgXrsscd08uRJ/fOf/9RFF12kdevWeS85XLJkiUaMGKF27dpp5syZOnz4sCZNmqTk5OTqfNvLzTLGGLuDqKiMjAwlJCQoPT1d8fHxdocDAAAAAMAZKzs7W9u3b1fTpk0VFRVV4vFQv4Rwzpw5mjRpkt/HIiMjlZ2dLUnauHGjzjvvPI0fP16PP/642rdvr6SkJK1evVouV+H8oJUrV6pv375q2LChNm/erJo1a0qS3nrrLV111VV6+umnNXXqVBlj1Lp1azVr1kyLFy+WZVmSpKysLKWkpKhFixZasmSJJGnChAmaN2+evvrqqxKXOBpjZFmWFi5cqFGjRmnFihXq06eP9/HMzEw1atRIo0aN0osvvuhtP3DggFq3bq2rrrrK296lSxcdOHBAmzdvVkJCgiRp6dKlGjBggJo0aVLmDeLL2k8qW8thBhYAAAAAAPjN+8c//qFWrVr5tIWHh3v/v3379nrggQc0bdo0rV+/XmlpaVqyZIm3eFXc+PHjvcUrSRo5cqSSkpL00UcfaerUqfruu+/0008/6S9/+YsOHz7s89z+/fvrtddek9vtllR4Wd+QIUP83p/LU/gKZOnSpTp27Jiuvvpqn9ll4eHh6tGjh1asWCFJ2rdvn7777jv9+c9/9havJOnSSy9Vu3btdOLEiVLXEwwUsAAAAAAAwG9e9+7dy7yJ+5133qk33nhDa9eu1YwZM9SuXTu/y7Vs2dLnb8uy1KJFC+8spp9++klS4eyqQNLT05Wbm6uMjAy1b396U8w86+nXr5/fxz0zoXbu3Ok3bklq3bq1vv3229Naf1WigAUAAACEACdcouNRnkt1Qi1eACiPbdu2eYtCGzZsOO3X8cyuevzxx9W5c2e/y8TFxenIkSOnvY7i63nttddUv379Eo/7mz3mVKETKQAAAAAAgE3cbrcmTpyo+Ph43XbbbZoxY4ZGjhyp4cOHl1jWU+TyMMbo559/VseOHSVJzZs3l1Q4A+qSSy4JuM66desqPj5eGzeW/q1AoEsJPeupV69eqetp0qSJ37gl6ccffyx13cESZncAAAAAAAAATvfEE0/oyy+/1IsvvqiHHnpIPXv21I033ljilwsl6dVXX9Xx48e9fy9cuFD79u3T4MGDJUnnnXeemjdvrlmzZikzM7PE8w8dOiRJCgsL0+9+9zstWrRIqampJZbz/C5fbGysJOnYsWM+jw8cOFDx8fGaMWOG8vLyAq4nKSlJnTt31ty5c5Wenu59fOnSpdq0aVOp70uwMAMLAAAAAAD85i1evFhbtmwp0d6zZ0/l5OTovvvu08SJEzVkyBBJhb9e2LlzZ/3hD3/QggULfJ6TmJioiy66SJMmTdKBAwf01FNPqUWLFvp//+//SSosTL388ssaPHiwUlJSNGnSJDVs2FB79uzRihUrFB8fr0WLFkmSZsyYoSVLlqh379667rrr1LZtW+3bt09vvfWWPv/8c9WqVUudO3dWeHi4HnvsMaWnpysyMlL9+vVTvXr19M9//lPXXnutzj33XI0ZM0Z169bVr7/+qv/85z+68MIL9dxzz0mSZs6cqcsvv1wXXXSRJk+erCNHjujZZ59VSkqK3yJbsFHAAgAAAAAAv3l//etf/ba//PLLeuGFF1SnTh099dRT3vaWLVtq5syZuvXWW7VgwQJdddVV3sfuuecerV+/XjNnztTx48fVv39/Pf/884qJifEu06dPH61evVoPPfSQnnvuOWVmZqp+/frq0aOHrr/+eu9yDRs21FdffaX77rtP8+fPV0ZGhho2bKjBgwd7X69+/fr617/+pZkzZ2rKlCkqKCjQihUrVK9ePV1zzTVq0KCBHn30UT3++OPKyclRw4YN1atXL02aNMm7nkGDBumtt97SX/7yF02bNk3NmzfX7Nmz9f7772vlypVV9C6fPst45puFkIyMDCUkJCg9Pd17x3wAAADgTBZqN0UPtXgBBJadna3t27eradOmioqKsjscR1u5cqX69u2rt956SyNHjrQ7nKAqaz+pbC2He2ABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRuIk7AAAAAABAFejTp49C8FbjIYEZWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwtEoXsL7++mvdfPPNSklJUWxsrBo3bqyrrrpKW7du9Vlu4sSJsiyrxL82bdpUNgQAAAAAAACcwVyVfYHHHntMX3zxhUaNGqWOHTtq//79eu6553TuuedqzZo1at++vXfZyMhIvfzyyz7PT0hIqGwIAAAAAAAAp2XOnDmaNGmSIiMj9csvv6hhw4Y+j/fp00dpaWnauHGjTRFCqoIC1u23367XX39dERER3rbRo0erQ4cOevTRRzVv3ryilblcGjduXGVXCQAAAAAAnOLjj+2OQBo0qNIvkZOTo0cffVTPPvtsFQSEqlbpSwh79uzpU7ySpJYtWyolJUWbN28usXxBQYEyMjIqu1oAAAAAAIAq07lzZ7300kvau3ev3aHAj2q5ibsxRgcOHFCdOnV82k+ePKn4+HglJCQoMTFRN910kzIzM6sjBAAAAAAAgHK75557VFBQoEcffbTU5fLz8/XQQw+pefPmioyM1DnnnKN77rlHOTk53mVuv/121a5dW8YYb9stt9wiy7L0zDPPeNsOHDggy7L0z3/+s+oTOsNU+hJCf+bPn689e/bowQcf9LYlJSXprrvu0rnnniu3262PP/5Yzz//vL7//nutXLlSLlfgUHJycnx2BM8Mrvz8fOXn50uSwsLCFBYWJrfbLbfb7V3W015QUOCz4wRqDw8Pl2VZ3tct3i4VziArT7vL5ZIxxqfdsiyFh4eXiDFQOzmREzmREzmREzmREzmRkyd245ZkhcmywmTcBZKKcpJVmJNx++YkqzB2mYJytVthhTn5tluywsJljPt/QUj5+WXnVHz5/714gNiDkxP7HjmR0+nnlJ+fX3QsKva63vjl03vtafcTV3lYluXN6ZxzztG1116rl156SX/+85+VlJTks6wxRpZl6fe//73mzp2rkSNH6vbbb9fatWs1c+ZMbd68We+8844k6aKLLtKTTz6pH374QSkpKZKkVatWKSwsTKtWrdLUqVNljNF///tfSVKvXr28r+/vPT7dnILZLhW+R8VrNcX3vVP3v4qq8gLWli1bdNNNN+mCCy7QhAkTvO0zZ870WW7MmDFq1aqV7r33Xi1cuFBjxowJ+JozZ87UAw88UKJ93bp1io2NlSTVrVtXzZs31/bt23Xo0CHvMsnJyUpOTtbWrVuVnp7ubW/WrJnq1aunjRs3Kisry9vepk0b1apVS+vWrfPpxB07dlRERIRSU1N9Yujatatyc3O1fv16b1t4eLi6deum9PR0bdmyxdseHR2tTp06KS0tTdu2bfO2JyQkqG3bttq7d692797tbScnciInciInciInciIncvLklHtcciU0U3hMPeUd3iiTX5RTjcQ2siJrKe/gOpliBZwadTrKCo9Q7gHfnCLO7ipTkKu8tKKcLCtcEfW7yeSmK+9IUU6WK1oRdTvJnZWm/PTCnFJPlp1TQfp2FWQV5RQelyxXzWTlH9sqd07RdgpGTux75EROlc8pKipKUmFRKzs729seFhammP+1Fy9QhIWFKaJGjRLt4eHhquFyKT8/3ycWl8slV3i48vLyfIp1nvbc3FyfokmNGjUUHhbmbc8/ccL7HoeFhenE//72iI2Nldvt9nlfLMvytktSVlaW/vjHP+q1117TY489plmzZiknJ0cFBQVyu93Kzs7W1q1bNXfuXE2YMEHPPfecJGnKlCmqV6+eZs2apcWLF+viiy9Wly5dJBUWrZo3b64jR45ow4YNuvLKK7Vq1Srv+lasWKGzzjpLTZo0UUFBgVwul06ePOmT6+nk5Hc7xcQoPz/fZ4JQeHi4oqOjlZeXp9zcXJ/3PSoqSjk5OT7bLyIiQhEREcrOzvbZfpGRkZKkvLw8n5vdF9/3Kns7KctUtrRXzP79+3XhhRcqLy9Pa9asUYMGDUpdPisrS3FxcZo0aVKJXycszt8MrEaNGunw4cOKj4+X5JzKtMeZVG0nJ3IiJ3IiJ3IiJ3IiJ/tzWr5JjpmB1b9d2Tl9ssE5M7AuTWHfIydyqkxO2dnZ+vXXX9WsWTNvoaI465NP7J+BNXCgnyXKZlmWZs+ercmTJ2vt2rXq2rWrJk+erDfeeEO//PKLkpKS1LdvX6WlpWnDhg169NFHdc899+iHH35Q27Ztva9z4MABJSUl6fbbb9esWbMkSe3atVPnzp31+uuv66OPPtKwYcP0+eefq0ePHtq6datatGih8847T40aNdJ7773njSdUZ2Dl5ORo27Ztaty4sbfgWXzfy8jIUO3atZWenu6t5VRElc3ASk9P1+DBg3Xs2DGtWrWqzOKVVFhFrF27to4cOVLqcpGRkX47icvlKnHpoafDnsrTAcvbHuiSxoq0W5bltz1QjBVtJydyCtROTuQkkVOgGCvaTk7kJJFToBgr2k5OlcvJKvawFeY/JysswOm9Vf52y7ICtId5gyiecqDYiy/vG2Og2Ks3p9K205KNJR7537/ytvuPPXB7oI9hLg1o76eV/kRONufkcrkKjw2S97+n8t8axPYAcZVH8dwsy9J9992nefPm6bHHHtPTTz/ts9zOnTsVFhamli1b+rwX9evXV61atfTrr79623v16qWPPvpIlmXp888/V9euXdWtWzclJiZq1apVOvvss/X999/rmmuu8XmtQO/x6eRkR7u/Wo2/toqqkpu4Z2dna8iQIdq6das+/PBDtWvXrlzPO378uNLS0lS3bt2qCAMAAAAAAKBSmjVrpnHjxunFF1/Uvn37/C5TniLTRRddpD179mjbtm1atWqVevXqJcuydNFFF2nVqlX68ssv5Xa71atXr6pO4YxU6QJWQUGBRo8erdWrV+utt97SBRdcUGKZ7OxsHT9+vET7Qw89JGOMBg0aVNkwAAAAAAAAqsRf/vIX5efn67HHHvNpb9Kkidxut3766Sef9gMHDujYsWNq0qSJt81TmFq6dKm+/vpr798XX3yxVq1apVWrVik2NlbnnXdeNWdzZqj0JYR33HGHPvjgAw0ZMkRHjhzRvHnzfB4fN26c9u/fry5duujqq69WmzZtJEmffPKJPvroIw0aNEhXXnllZcMAAAAAAACoEs2bN9e4ceP0wgsvqEmTJt7L3y677DLdc889euqpp/TCCy94l3/iiSckSZdffrm3rWnTpmrYsKGefPJJ5eXl6cILL5RUWNj605/+pIULF+r888+v9KV1vxWVfpe+++47SdKiRYu0aNGiEo+PGzdOtWrV0hVXXKGlS5dq7ty5KigoUIsWLTRjxgz96U9/8nstLwAAAAAAgF3uvfdevfbaa/rxxx+VkpIiSerUqZMmTJigF198UceOHVPv3r21du1azZ07V7/73e/Ut29fn9fo1auX3njjDXXo0EFnnXWWJOncc89VbGystm7dqmuuuSboeYWqShewVq5cWeYytWrV0muvvVbZVQEAAAAAAARFixYtNG7cOM2dO9en/eWXX1azZs00Z84cvfvuu6pfv76mTZum6dOnl3gNTwHroosu8ra5XC5dcMEFWrZsGfe/qgDLVPb3GW2QkZGhhISE0/7pRQAAACDUlPylPPv4+6W8U4VSvKEUK2CH7Oxsbd++XU2bNlVUVJTd4cChytpPKlvL4UJLAAAA/GZRuAAAIDRw8ykAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAACAamJZlu6//367wwh5FLAAAAAAAMBvkmVZ5fq3cuVKu0P9zXPZHQAAAAAAAAhhP/9sdwRSixan9bTXXnvN5+9XX31VS5cuLdHetm3b0w4NVYMCFgAAAAAA+E0aN26cz99r1qzR0qVLS7TDflxCCAAAAAAAEMCJEyd0xx13qFGjRoqMjFTr1q01a9YsGWN8lsvJydEf//hH1a1bVzVr1tTQoUO1e/fuEq+3c+dO/eEPf1Dr1q0VHR2t2rVra9SoUdqxY4d3mW3btsmyLD355JMlnv/ll1/Ksiz9+9//rvJcnYwCFgAAAAAAgB/GGA0dOlRPPvmkBg0apCeeeEKtW7fWnXfeqdtvv91n2d///vd66qmnNGDAAD366KOqUaOGLr/88hKv+fXXX+vLL7/UmDFj9Mwzz+iGG27Q8uXL1adPH508eVKS1KxZM1144YWaP39+iefPnz9fNWvW1JVXXlk9STsUlxACAAAAAAD48cEHH+jTTz/Vww8/rHvvvVeSdNNNN2nUqFF6+umndfPNN6t58+b6/vvvNW/ePP3hD3/QP/7xD+9yY8eO1fr1631e8/LLL9fIkSN92oYMGaILLrhAb7/9tq699lpJ0vjx43X99ddry5YtatOmjSQpLy9PCxYs0PDhwxUTE1Pd6TsKM7AAAAAAAAD8+OijjxQeHq6pU6f6tN9xxx0yxmjx4sXe5SSVWO62224r8ZrR0dHe/8/Ly9Phw4fVokUL1apVS99++633sauuukpRUVE+s7A++eQTpaWl/Sbv0UUBCwAAAAAAwI+dO3eqQYMGqlmzpk+751cJd+7c6f1vWFiYmjdv7rNc69atS7xmVlaW/vrXv3rvqVWnTh3VrVtXx44dU3p6une5WrVqaciQIXr99de9bfPnz1fDhg3Vr1+/KssxVFDAAgAAAAAACJJbbrlFjzzyiK666iotWLBAS5Ys0dKlS1W7dm253W6fZcePH69t27bpyy+/1PHjx/XBBx/o6quvVljYb6+cwz2wAAAAAAAA/GjSpImWLVum48eP+8zC2rJli/dxz3/dbrd++eUXn1lXP/74Y4nXXLhwoSZMmKC///3v3rbs7GwdO3asxLKDBg1S3bp1NX/+fPXo0UMnT5703iPrt+a3V7IDAAAAAAAoh8suu0wFBQV67rnnfNqffPJJWZalwYMHS5L3v88884zPck899VSJ1wwPD5cxxqft2WefVUFBQYllXS6Xrr76ai1YsEBz5sxRhw4d1LFjx8qkFLKYgQUAAAAAAODHkCFD1LdvX917773asWOHOnXqpCVLluj999/Xbbfd5r3nVefOnXX11Vfr+eefV3p6unr27Knly5fr559/LvGaV1xxhV577TUlJCSoXbt2Wr16tZYtW6batWv7jWH8+PF65plntGLFCj322GPVmq+TUcACAAAAAADwIywsTB988IH++te/6s0339Ts2bN1zjnn6PHHH9cdd9zhs+wrr7zivdzvvffeU79+/fSf//xHjRo18lnu6aefVnh4uObPn6/s7GxdeOGFWrZsmQYOHOg3hvPOO08pKSnavHmzxo4dW225Op1lTp23FgIyMjKUkJCg9PR0xcfH2x0OAAAAQtSSjXZHUGRA+9IfD6VYpdCKN5RiBeyQnZ2t7du3q2nTpoqKirI7nN+kLl26KDExUcuXL7c7lIDK2k8qW8vhHlgAAAAAAAAOlZqaqu+++07jx4+3OxRbcQkhAAAAAACAw2zcuFHffPON/v73vyspKUmjR4+2OyRbMQMLAAAAAADAYRYuXKhJkyYpLy9P//73v3/zl28yAwsAAAAAQgj37AJ+G+6//37df//9dofhGMzAAgAAAAAAgKNRwAIAAAAAAICjUcACAAAAAABlMsbYHQIcrLr3DwpYAAAAAAAgoPDwcElSXl6ezZHAyTz7h2d/qWoUsAAAAAAAQEA1atRQZGSk0tPTmYUFv4wxSk9PV2RkpGrUqFEt6+BXCAEAAAAAQKnq1KmjPXv2aPfu3UpISFCNGjVkWZbdYcFmxhjl5eUpPT1dmZmZatiwYbWtiwIWAAAAAAAoVXx8vCQpLS1Ne/bssTkaOE1kZKQaNmzo3U+qAwUsAAAAAABQpvj4eMXHxysvL08FBQV2hwOHCA8Pr7bLBoujgAUAAAAAAMqtRo0aQSlYAMVxE3cAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4msvuAAAAAHDmWLLR7giKDGhvdwQAAKCqMAMLAAAAAAAAjkYBCwAAAAAAAI7GJYQAAAAAgGrBZcUAqgozsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GiVLmB9/fXXuvnmm5WSkqLY2Fg1btxYV111lbZu3Vpi2c2bN2vQoEGKi4tTYmKirr32Wh06dKiyIQAAAAAAAOAM5qrsCzz22GP64osvNGrUKHXs2FH79+/Xc889p3PPPVdr1qxR+/btJUm7d+/WxRdfrISEBM2YMUOZmZmaNWuWNmzYoLVr1yoiIqLSyQAAAAAAAODMU+kC1u23367XX3/dpwA1evRodejQQY8++qjmzZsnSZoxY4ZOnDihb775Ro0bN5Ykde/eXZdeeqnmzJmj6667rrKhAAAAAAAA4AxU6UsIe/bsWWL2VMuWLZWSkqLNmzd7295++21dccUV3uKVJF1yySVq1aqVFixYUNkwAAAAAAAAcIaqlpu4G2N04MAB1alTR5K0Z88eHTx4UF27di2xbPfu3bVu3brqCAMAAAAAAABngEpfQujP/PnztWfPHj344IOSpH379kmSkpKSSiyblJSkI0eOKCcnR5GRkX5fLycnRzk5Od6/MzIyJEn5+fnKz8+XJIWFhSksLExut1tut9u7rKe9oKBAxpgy28PDw2VZlvd1i7dLUkFBQbnaXS6XjDE+7ZZlKTw8vESMgdrJiZzIiZzIiZzIiZxCLSdjwv/3P77tVlhhTr7tlqywcBnjloy77HYrTJYVFrjdXSCpKHa3u+ycfFfrP/ZA7VWdU35+6dvJuAPnKqswJ+P23U7VlVN+ftn7Xnm3U7ByKq0/FYVZNfteZXIq3tUC9TMp+P0pULsxpR8jCpf3n6tPcxCOERzLyYmc7M3p1LwqqsoLWFu2bNFNN92kCy64QBMmTJAkZWVlSZLfAlVUVJR3mUAFrJkzZ+qBBx4o0b5u3TrFxsZKkurWravmzZtr+/btPr9smJycrOTkZG3dulXp6ene9mbNmqlevXrauHGjNz5JatOmjWrVqqV169b5bOyOHTsqIiJCqampPjF07dpVubm5Wr9+vbctPDxc3bp1U3p6urZs2eJtj46OVqdOnZSWlqZt27Z52xMSEtS2bVvt3btXu3fv9raTEzmREzmREzmREzmFWk6K6SpTkKu8tKKcLCtcEfW7yeSmK+9IUU6WK1oRdTvJnZWm/PSinMIiE1Qjsa0KMveqILMop/DounLVaq6C9O0qyCrKKTwuWa6ayco/tlXunKKc0uqXnVPusaKcatTpKCs8QrkHfHOKODs4OaWmlr6dco9LroRmCo+pp7zDG2Xyi3KqkdhGVmQt5R1cJ2OqP6fUk2Xve+XdTsHIqaz+lHu8/NupunNKPVmUU6BjhKKD358C5ZTeuPRjhF39yV9OHMvJiZzszckzGel0WaZ4aayS9u/frwsvvFB5eXlas2aNGjRoIElKTU1Vt27d9Oqrr+raa6/1ec5dd92lxx9/XNnZ2RWagdWoUSMdPnxY8fHxkqh4khM5kRM5kRM5kRM5OSGn5ZudMwPr0vZl57R8U/HV2jsDq3/b0rfT8k2Bcw32DKz+7cre9z7Z4JwZWJemlN6fivYD+2dg9W9X1Byon326xTkzsAZ0KP0YsWSDc2Zg9W/LsZycyMnOnDIyMlS7dm2lp6d7azkVUWUzsNLT0zV48GAdO3ZMq1at8havpKJLBz2XEha3b98+JSYmBixeSYUzt/w97nK55HL5puB5007l2bDlbT/1dU+n3bIsv+2BYqxoOzmRU6B2ciIniZwCxVjRdnIiJ4mcAsXor92yPP/jPyf/7WGSVTLGCreH+cbuSbu0nPy8jN8YA7VXZU4uV+nbqfjTTs21qL38sQdqL09OxTd7oH2svNup7Paqyam0/nRqmJXd98puDxy7v64W6BgRzP4UqN3T5wMdIyqy/ao7J47l5BSonZyCk1Og+MurSgpY2dnZGjJkiLZu3aply5apXbt2Po83bNhQdevWLTnFXNLatWvVuXPnqggDAAAAAAAAZ6BK/wphQUGBRo8erdWrV+utt97SBRdc4He5ESNG6MMPP9SuXbu8bcuXL9fWrVs1atSoyoYBAAAAAACAM1SlZ2Ddcccd+uCDDzRkyBAdOXJE8+bN83l83LhxkqR77rlHb731lvr27atbb71VmZmZevzxx9WhQwdNmjSpsmEAAAAAAADgDFXpAtZ3330nSVq0aJEWLVpU4nFPAatRo0b67LPPdPvtt+vPf/6zIiIidPnll+vvf/97qfe/AgAAAAAAwG9bpQtYK1euLPeyKSkp+uSTTyq7SgAAAAAAAPyGVNmvEAIAAAAAEMqWbLQ7giID2tsdAeAslb6JOwAAAAAAAFCdKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNFcdgeA/3n1VbsjKDJ+vN0RAAAAAAAAeDEDCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACO5rI7AAAAAAAAUDFLNtodQZEB7e2OAL8FzMACAAAAAACAo1HAAgAAAAAAgKNRwAIAAAAAAICjcQ8sAAAAh+M+JwAA4LeOGVgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNG7ijgrjRrIAAAAAACCYmIEFAAAAAAAAR2MGlkP8kmZ3BEWa2x0AAAAAAABAMczAAgAAAAAAgKNRwAIAAAAAAICjUcACAAAAAACAo1HAAgAAAAAAgKNRwAIAAAAAAICjUcACAAAAAACAo7nsDgCobks22h1BkQHt7Y4AAAAAAIDQwwwsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GvfAAgAAAAAA1Yp7E6OymIEFAAAAAAAAR6OABQAAAAAAAEejgAUAAAAAAABHo4AFAAAAAAAAR6OABQAAAAAAAEejgAUAAAAAAABHo4AFAAAAAAAAR6OABQAAAAAAAEejgAUAAAAAAABHo4AFAAAAAAAAR3PZHQAAAAAAAIBTLNlodwRFBrS3OwLnYAYWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHM1ldwAAAADBtmSj3REUGdDe7ggAAACcjxlYAAAAAAAAcDQKWAAAAAAAAHC0KilgZWZmavr06Ro0aJASExNlWZbmzJlTYrmJEyfKsqwS/9q0aVMVYQAAAAAAAOAMVCX3wEpLS9ODDz6oxo0bq1OnTlq5cmXAZSMjI/Xyyy/7tCUkJFRFGAAAAAAAADgDVUkBKykpSfv27VP9+vWVmpqqbt26BV6hy6Vx48ZVxWqBMw43FQYAAAAAoKQquYQwMjJS9evXL/fyBQUFysjIqIpVAwAAAAAA4AwX9Ju4nzx5UvHx8UpISFBiYqJuuukmZWZmBjsMAAAAAAAAhIgquYSwvJKSknTXXXfp3HPPldvt1scff6znn39e33//vVauXCmXy384OTk5ysnJ8f7tmb2Vn5+v/Px8SVJYWJjCwsLkdrvldru9y3raCwoKZIwpsz08PFyWZXlft3i7VDh7rDztLpdLxhifdsuyFB4eXiJGy7IkSUaSsYq9iCmsMLolqVi7ZQr/dBdf9jTbdeo6Je/7ESgn4y7ebskKC5cxbsm4y263wmRZYYHb3QX/eyfKai//djLuwuUL//DNyQorzMm3vfpyys8vfd+TLBm3b06BYq/unKTQ7U/+2kP9GEFO5EROVZtTdY9PFTmWG1N2TuZ/JwN2jrmenDybK9D2MMYZY64kud1l73u+q7VnzPXklJ9fen8qPKepun2vMjnl55d9jLCjP5WWU2nHiKIwg9uf/MVe/JAYqJ9Jwe9PgdqNKf1Y7vvZQUHrT/7ayzM+eT47BLM/BWov/tnBXz+T7OtPp+YklX0e4U3XxjHX0158d/V3HmHczhhzpcL94Ew53zv1OFFRQS1gzZw50+fvMWPGqFWrVrr33nu1cOFCjRkzJuDzHnjggRLt69atU2xsrCSpbt26at68ubZv365Dhw55l0lOTlZycrK2bt2q9PR0b3uzZs1Ur149bdy4UVlZWd72Nm3aqFatWlq3bp3Pxu7YsaMiIiKUmprqE0PXrl2Vm5ur9evXe9vCw8PVrVs3paena8uWLd726OhoderUSWlpadq2bZu3PSEhQRGS0uNqKD2uhrc9LitftdNzdTQhQpnRRZsqITNPtTLzdKhWpLIjw73tiem5qpmVr/21o5TnKppcV+9ItqJz3dpdL1rGKqpWJaVlyVVgtOvsGJ+cmhYUlJpT7oGinCxXtCLqdpI7K0356UU5hUUmqEZiWxVk7lVB5u6i14muK1et5ipI366CrKLtFB6XLFfNZOUf2yp3TtF2ciU0U3hMPeUd3iiTX7SdaiS2kRVZvu2Ue1yKOLurTEGu8tKKcrKscEXU7yaTm668I8HJKfVk6fueVEt5B9fJFDvY1qjTUVZ4hHIP+O571Z2TFLr9qW3bttq7d6927y7KKdSPEeRETuRUtTlV9/hUkWN5VlbZOeUet3/M9eSUerL07aQYZ4y5kpRWv+x9L/eY/WOuJ6fU1NL7U+7xqt33KpNT6smyjxF29KdAOZV1jMg9Xv7tVN05efqYFPi4p+jg96dAOaU3Lv1Ybld/8pdTecan3OPB70+Bcko9WfqYK9nTn/zlJJV9HuHpZ3aOuZ6cPP0s0HlEXpYzxlypcD84U873KnsrKcsUL41VAc9N3GfPnq2JEyeWuXxWVpbi4uI0adKkEr9O6OFvBlajRo10+PBhxcfHSwr9b4N3PD3fMTOwWtx2bak5Ldlg/zc9nsp0vzZlb6flm2TrNz3FY+/frvR9b+kP9n/T44l9YIfQ7U9n6owRciIncqq6nD7Z4JwZWAPal53T8k2S3WOuJ6f+7QqbA22P5ZudMeZK0qXty973Ct/bolz9xR6s84j+bUvvT4XnNM6YgdW/XdnHiID9zIYZI5emlH6MKNoP7J+B5eljUuB+9ukW58zAGtCh9GO572cHBa0/+Wvv37bs8cnz2cEJM7CKf3bw18+WbXLODKyBHcs+j/D2MwfMwCrez/ydRyzf5IwxVyrcD86U872MjAzVrl1b6enp3lpORQR1BpY/0dHRql27to4cORJwmcjISEVGRpZod7lcJS479Lxpp/Js2PK2B7qcsSLtlmX5bQ8Uo6WiopLP8pLPPu1tD1B6rGj7qev0XNIYKCcrzF97mAovO6tke5j/7RGovTzbw2c1lv+c/LdXfU7Fww207/l7fwsfKH97VeUUyv2pou3kRE6B2snpzMypusenihzLLavsnIqHZNeY68np1FBPjd072dvmMVeSPJu+tH3Pz8vYMuZaVphcrtL7k89+UAX7XqD28uRUfLNXuJ9VY38K1F7WMeLUMO08Rvg79AU6RgSzPwVq9/T5QMfsih0Pqzen8oxPvv3M3vPycvUzm/qTv/ayzhfK3c+CkNOpu+upxwhPWHaPuZLvfhDq53uB4i8vf0N2UB0/flxpaWmqW7eu3aEAAAAAAADAgYJWwMrOztbx48dLtD/00EMyxmjQoEHBCgUAAAAAAAAhpMouIXzuued07Ngx7d27V5K0aNEi7w3AbrnlFh09elRdunTR1Vdf/b+bVUuffPKJPvroIw0aNEhXXnllVYUCAAAAAACAM0iVFbBmzZqlnTt3ev9+55139M4770iSxo0bp1q1aumKK67Q0qVLNXfuXBUUFKhFixaaMWOG/vSnP/m9phIAAAAAAACosgLWjh07ylzmtddeq6rVAQAAAAAA4DeCaU8AAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNJfdAQAAgDPDko12R1BkQHu7IwAAAEBVYgYWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAczWV3AAAAwL8lG+2OoMiA9nZHAAAAgN8yZmABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0biJO4DTxg2mAQAAAADBwAwsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOJrL7gAAAAimJRvtjqDIgPZ2RwAAAACEBmZgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0aqkgJWZmanp06dr0KBBSkxMlGVZmjNnjt9lN2/erEGDBikuLk6JiYm69tprdejQoaoIAwAAAAAAAGcgV1W8SFpamh588EE1btxYnTp10sqVK/0ut3v3bl188cVKSEjQjBkzlJmZqVmzZmnDhg1au3atIiIiqiIcAAAAAAAAnEGqpICVlJSkffv2qX79+kpNTVW3bt38LjdjxgydOHFC33zzjRo3bixJ6t69uy699FLNmTNH1113XVWEAwAAAAAAgDNIlVxCGBkZqfr165e53Ntvv60rrrjCW7ySpEsuuUStWrXSggULqiIUAAAAAAAAnGGCdhP3PXv26ODBg+ratWuJx7p3765169YFKxQAAAAAAACEkCq5hLA89u3bJ6nwcsNTJSUl6ciRI8rJyVFkZGSJx3NycpSTk+P9OyMjQ5KUn5+v/Px8SVJYWJjCwsLkdrvldru9y3raCwoKZIwpsz08PFyWZXlft3i7JBUUFJSr3eVyyRjj025ZlsLDw0vEaFmWJMlIMlaxFzGFFUa3JBVrt0zhn+7iy55mu05dp+R9PwLlZNzF2y1ZYeEyxi0Zd9ntVpgsKyxwu7vgf+9EWe3l307GXbh84R++OVlhhTn5tldfTvn5pe97kiXj9s0pUOzVnZNUdn/yPqWM7RSMnDy7QqB+FurHCHKqupyMUdD7U6BjhFRGTm57+pO/9vz8sreTMad3LK+OnAoKSt/3qnt8qkhOxpTdn8z/TgbsHHM9OXm6VaBjgTHOGHMlye0u+xjhu1p7xlxPTv76WfHYC89p7B9zpcL9oKxjuR39qbScShufisIMbn/yF3vxoStQP5OC358CtRtT+nmE72cHBa0/+Wsvz3mE57ODnWNu8X5W2rmR5Iwxt/DTZtnneyU+O9h4jCi+u/o7hzVuZ4y5UuF+cKacl596nKiooBWwsrKyJMlvgSoqKsq7jL/HZ86cqQceeKBE+7p16xQbGytJqlu3rpo3b67t27f7/KphcnKykpOTtXXrVqWnp3vbmzVrpnr16mnjxo3e2CSpTZs2qlWrltatW+ezsTt27KiIiAilpqb6xNC1a1fl5uZq/fr13rbw8HB169ZN6enp2rJli7c9OjpanTp1UlpamrZt2+ZtT0hIUISk9LgaSo+r4W2Py8pX7fRcHU2IUGZ00aZKyMxTrcw8HaoVqezIcG97Ynquambla3/tKOW5iibX1TuSrehct3bXi5axiqpVSWlZchUY7To7xienpgUFpeaUe6AoJ8sVrYi6neTOSlN+elFOYZEJqpHYVgWZe1WQubvodaLrylWruQrSt6sgq2g7hccly1UzWfnHtsqdU7SdXAnNFB5TT3mHN8rkF22nGoltZEWWbzvlHpcizu4qU5CrvLSinCwrXBH1u8nkpivvSHBySj1Z+r4n1VLewXUyxQ62Nep0lBUeodwDvvtedeckld2fco+XbzsFI6fUk4XtCQkJatu2rfbu3avdu4tyOpJfuJ3yj/nfTnlH/O97uYdK5hQWWUu5+08/p/q1Kn6M8JdTqB/37MpJJvj9KdAxQio9p9yD9vQnfzmlppa9nQrM6R3LqyOnjab0fa+6x6eK5JSVVXZ/yj1u/5jryclzvA10jFCMM8ZcSUqrX/YxIveY/WOuJ6fU1NKPe7nHnTHmSoXnNGUdy+3oT4FyKmt88pzTBLs/+cvJ08ekwGOuooPfnwLllN649PMIp4y5rprlO4/IPW7/mOvJKfVk6edGkjPGXMsVLans8z1PP7NzzPXk5Olngc5h87KcMeZKhfvBmXJe7pmMdLosU7w0VgU8N3GfPXu2Jk6cWKL91Vdf1bXXXuvznLvuukuPP/64srOzyz0Dq1GjRjp8+LDi4+Mlhf5MhB1Pz3fMDKwWt11bak5LNtj/TY+nMt2vTdnbafkm2fpNT/HY+7crfd9b+oP93/R4Yh/Yoez+tHxT4Fw9MQbr26v+7f7XGqCfLd9s/zc9Hv3bOfdbkeLOlG96To19yUY5ZgbWwA6l57TsB+fMwOrftuzt5O1nDvg2+JKU0ve9TzY4ZwbWgPZl96fC460zvg32HG8DHQuWb3bGmCtJl7Yv+xjhHcv+l6u/2IN1jPDXz4rHXnhOY/+YKxXuB2UdywP2MxuOEZemlD4+Fe0H9s/A8vQxKXA/+3SLc2ZgDehQ+nmE72cHBa0/+Wvv37bs8wjPZwcnzMAq/tnBXz9btskZY65kaWDHss/3Snx2sPG8vHg/83cOu3yTM8ZcqXA/OFPOyzMyMlS7dm2lp6d7azkVEbQZWJ5LBz2XEha3b98+JSYm+i1eSYWztvw95nK55HL5puB5007l2bDlbT/1dU+n3bIsv+2BYrQkb1HJZ3nJZ5/2tgcoPVa0/dR1ei5pDJSTFeavPUyy/ORU0fYw/9sjUHt5tofPaiz/Oflvr/qciocbaN/z9/4WPlD+9qrKqaz+dOpTAm+/6s/p1F3h1Ng9kw+rat+rTE6eWCt6jKhoeygc9+zIybJkS38K1F5aTn4Wt+0Y4XKVvZ28/SyI/alo3b45ed7WgGNuNY9PFcnJssruT8VDsmvM9eR0aqinxu6d7G3zmCtJnk1f2jHCXz+z6xjhr58Vj91nP7BxzJV894MK9zObjhGljU8lzmlsPEb4G3YDHSOC2Z8CtXv6fKDzhYodD+0bc4viLfY6Np+Xl6ufOWDMLSvGCvezIOR06u566jHCE5bdY67kux+E+nl5oPjLy9+QXS0aNmyounXrlpxmLmnt2rXq3LlzsEIBAAAAAABACAlaAUuSRowYoQ8//FC7du3yti1fvlxbt27VqFGjghkKAAAAAAAAQkSVXUL43HPP6dixY9q7d68kadGiRd4bgN1yyy1KSEjQPffco7feekt9+/bVrbfeqszMTD3++OPq0KGDJk2aVFWhAAAAAAAA4AxSZQWsWbNmaefOnd6/33nnHb3zzjuSpHHjxikhIUGNGjXSZ599pttvv11//vOfFRERocsvv1x///vfA97/CgDgbEs22h1BkQHt7Y4AAAAAQHWosgLWjh07yrVcSkqKPvnkk6paLQAAAAAAAM5wQb0HFgAAAAAAAFBRFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoLrsDAACUtGSj3REUGdDe7ggAAAAA/NYxAwsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACOFtQC1sqVK2VZlt9/a9asCWYoAAAAAAAACBEuO1Y6depUdevWzaetRYsWdoQCAAAAAAAAh7OlgNWrVy+NHDnSjlUDAAAAAAAgxNh2D6zjx48rPz/frtUDAAAAAAAgRNhSwJo0aZLi4+MVFRWlvn37KjU11Y4wAAAAAAAAEAKCeglhRESERowYocsuu0x16tTRpk2bNGvWLPXq1UtffvmlunTp4vd5OTk5ysnJ8f6dkZEhScrPz/fO4goLC1NYWJjcbrfcbrd3WU97QUGBjDFltoeHh8uyrBKzw8LDwyVJBQUF5Wp3uVwyxvi0W5al8PDwEjFaliVJMpKMVexFTGGF0S1JxdotU/inu/iyp9muU9cped+PQDkZd/F2S1ZYuIxxS8ZddrsVJssKC9zuLvjfO1FWe/m3k3EXLl/4h29OVlhhTr7t1ZdTfn7p+55kybhPmZkYIPbqzkkquz95n1LGdgpGTp5dIVA/M6Zq973K5JSfX/YxwriD358C5ZSfX/pxz7PqYPcnf+2e/aC0Y7kxCnp/CpSTVMb45LanP/lrz88veSwI2M+C2J8C5VRQEHjMLdwP7OlP/nIypuzzCPO/kwE7x1xPTsX7mVQydmOcMeZKkttd9vme72rtGXM9OfnrZ8VjLzynsX/MlQr3g0Bjrid2J4y5xXMq7by8KEx7x1yZAhUfugL1M8n+MdfDmNLPy30/Oyho/clfe3k+E3o+O9g55hbvZ6V9zpWcMeZKlqTAY26JfmbjmOtpL767+jsvN25njLlS4X5Q3fWI0o7lVVljqexVeEEtYPXs2VM9e/b0/j106FCNHDlSHTt21LRp0/Txxx/7fd7MmTP1wAMPlGhft26dYmNjJUl169ZV8+bNtX37dh06dMi7THJyspKTk7V161alp6d725s1a6Z69epp48aNysrK8ra3adNGtWrV0rp163w2dseOHRUREVFitljXrl2Vm5ur9evXe9vCw8PVrVs3paena8uWLd726OhoderUSWlpadq2bZu3PSEhQRGS0uNqKD2uhrc9LitftdNzdTQhQpnRRZsqITNPtTLzdKhWpLIjw73tiem5qpmVr/21o5TnKppcV+9ItqJz3dpdL1rGKqpWJaVlyVVgtOvsGJ+cmhYUlJpT7oGinCxXtCLqdpI7K0356UU5hUUmqEZiWxVk7lVB5u6i14muK1et5ipI366CrKLtFB6XLFfNZOUf2yp3TtF2ciU0U3hMPeUd3iiTX7SdaiS2kRVZvu2Ue1yKOLurTEGu8tKKcrKscEXU7yaTm668I8HJKfVk6fueVEt5B9fJFDvY1qjTUVZ4hHIP+O571Z2TVHZ/yj1evu0UjJxSTxa2JyQkqG3bttq7d6927y7KqSC/ave9yuS0LqfsY0TugeD3p0A5lXXcyz1uT3/yl5NnPyjtWC4T/P4UKCep9PEp96A9/clfTqmpRTkFGnMLTPD7U6CcNprAY27btvb1J385ZWWVfR6Re9z+MdeTk6efBTo3UowzxlxJSqtf9vle7jH7x1xPTqmppZ/D5h53xpgrFZ7TBBpzPccIJ4y5npzKOi/3nNPYPebmHkj19jEp8GcNRds/5nqkNy7985NTxlxXzfJ9Jsw9bv+Y68kp9WTpn3MlZ4y5litaUuAx13OM8PQzO8dcT06efhbos3teljPGXKlwP6juekRpx/KqrLF4JiOdLssUL43Z5Oqrr9Y777yjkydPeiuIxfmbgdWoUSMdPnxY8fHxkkJ/BtaOp+c7ZgZWi9uuLTWnJRvs/6bHU5nu16bs7bR8k2z9pqd47P3blb7vLf3B/m96PLEP7FB2f1q+KXCunhiD9e1V/3b/aw3Qz5Zvtv+bHo/+7co+RizdaO83PcVj79+29OOeZz9wwgwsz35Q2rF8yUbZNrvCXz8rbXxa9oNzZmD1b1v2N3LefuaAb4MvSSn9W8ZPNtg3u+LU9gHtyz6PKOxnzvg2uHg/k0rGvnyzM8ZcSbq0fdnne96x7H+5+os9WMcIf/2seOyF5zT2j7lS4X5Q1rf2AfuZDceIS1NKPy8v2g/sn4Hl6WNS4H726Rb7x1yPAR1K//zk+9lBQetP/tr7ty37M6Hns4MTZmAV/+zgr58t2+SMMVeyNLBj2TN7Snx2sPG8vHg/83devnyTM8ZcqXA/OFNmYGVkZKh27dpKT0/31nIqwpZfITxVo0aNlJubqxMnTvhNIjIyUpGRkSXaXS6XXC7fFDxv2qn8FcZKaz/1dU+n3bIsv+2BYrQkb1HJZ3nJZ5/2tgcoPVa0/dR1ei5pDJSTFeavPUyy/ORU0fYw/9sjUHt5tofPaiz/Oflvr/qciocbaN/z9/4WPlD+9qrKqaz+dOpTAm+/6s/p1F3h1Ng9kw+rat+rTE6eWEs7Rlj+jhHV3J8C5VRWPyu+6mD2J3/tp4bq/zgmW/pToPbSxic/i9t2jHC5yj5GePtZEPtT0bp9c/K8rQHHXJv6k//Yyz6P8O1n9oy5npzK6mfeyd42j7mS5Nn0pZ3v+etndh0j/PWz4rH77Ac2jrmS735Q4X5m0zGitPPyEuc0Nh4j/A27gY4Rdo65Rc8PHGPh8qEx5hbFW+x1bD4vL1c/c8CYW1aMFe5nQcjp1N311GOEJyy7x1zJdz+oznpERdtPp8YSKP7y8jdkB922bdsUFRWluLg4u0MBAAAAAACAwwS1gFX8ukmP77//Xh988IEGDBjgt6oHAAAAAACA37agXkI4evRoRUdHq2fPnqpXr542bdqkF198UTExMXr00UeDGQoAAAAAAABCRFALWL/73e80f/58PfHEE8rIyFDdunU1fPhwTZ8+XS1atAhmKAAAAAAAAAgRQS1gTZ06VVOnTg3mKgEAAAAAABDiuOkUAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcLegFrJycHN19991q0KCBoqOj1aNHDy1dujTYYQAAAAAAACBEBL2ANXHiRD3xxBMaO3asnn76aYWHh+uyyy7T559/HuxQAAAAAAAAEAJcwVzZ2rVr9cYbb+jxxx/Xn/70J0nS+PHj1b59e91111368ssvgxkOAAAAAAAAQkBQZ2AtXLhQ4eHhuu6667xtUVFRmjJlilavXq1du3YFMxwAAAAAAACEgKAWsNatW6dWrVopPj7ep7179+6SpO+++y6Y4QAAAAAAACAEBPUSwn379ikpKalEu6dt7969fp+Xk5OjnJwc79/p6emSpCNHjig/P1+SFBYWprCwMLndbrndbu+ynva</t>
+  </si>
+  <si>
+    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACA5UlEQVR4nOzdd3xTdfv/8fdp0sVokbIpe1tkD0W2imxvGaK3bPwiLvSnt3rjYijguhXF24mCA1TABQrKEBSRIVoQBKy3DIECUkbL6Epyfn/UhIYmHdAmJ/h6Ph48lCsnOdeVMz7JxeecGKZpmgIAAAAAAAAsKizYCQAAAAAAAAD5oYEFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAgIXUrl1bhmF4/YmMjFTNmjU1ZMgQrVmzJiB5jBw5UoZhaM6cOQFZX0lxv5979uwJdioXPff+CgAAUBJoYAEAYEFXXnmlRowYoREjRqhXr15yuVyaP3++unTpoueeey7Y6VlCKDXZAtlImzNnjgzD0MiRI0t8XQAAAIFiD3YCAAAgr1tuucWrAZGRkaFbb71V77zzjh544AH17dtXDRs2DF6CIWLlypXKzs5W9erVg50KAAAALgAzsAAACAFRUVH673//q9KlS8vpdOrjjz8OdkohoV69emrcuLHCw8ODnQoAAAAuAA0sAABCRJkyZdSoUSNJynMp2ldffaW+ffuqUqVKioiIULVq1TRkyBBt2rTJ7+sdO3ZM99xzj2rVquW5z9add96pY8eOnVd+kyZNkmEYmjRpkvbu3avhw4eratWqioqKUsOGDTVp0iSlp6fneV52drbee+893XzzzWrcuLFiYmIUHR2tRo0aafz48UpOTvZafs+ePTIMQ2+//bYkadSoUV73DJs0aZJn2YIu3Vu4cKF69uypihUrKiIiQtWrV9fQoUO1ffv2PMu611u7dm2ZpqnXX39drVu3VunSpRUbG6sePXpo3bp1Xs9xX863d+9eSVKdOnW8cl29erVn2RUrVqhfv36qXLmywsPDdckll6hBgwYaOnSovv3228JsAtWuXVujRo2SJL399tte6+ratavXsmfOnNGTTz6pVq1aqWzZsipVqpQSEhL0yCOP6Pjx44Vanz9vvPGG570pV66cevfurfXr1/td3uFwaNasWeratavKly+vyMhI1alTR7fddpv27dtX5PX/+OOPGjJkiOLj4xUREaGYmBjVrVtXAwcO1Geffeb3OTfffLNq1qypyMhIlS9fXtdee62WLFlSbHmvXr3asy2ys7P11FNPKSEhQdHR0YqLi9OAAQO0Y8eOItcLAMDfAZcQAgAQQtLS0iRJkZGRntijjz6qJ554QoZhqEOHDqpZs6Z27Nih+fPn66OPPtLrr7+u0aNHe73O4cOH1alTJ/3222+65JJL1LdvX7lcLs2dO1dffvmlEhISzjvH3bt3q3Xr1rLb7ercubPS09O1atUqTZ48WStWrNCKFSsUFRXllcuwYcMUGxurJk2aqFmzZjp9+rQ2b96smTNn6oMPPtD333+v+vXrS8pp5I0YMULfffedfv/9d1155ZWexySpRYsWBebocDh08803a/78+YqMjFTr1q1VvXp1JSUlae7cufr444/18ccfq2fPnj6fP2rUKM2bN0+dOnVS3759tXnzZi1fvlzffvutvvnmG7Vv316SVL9+fY0YMUILFy7U6dOnNXDgQJUpU8bzOlWqVJGU02xyN57atWunbt26KT09Xfv379cHH3ygChUqqHPnzgXWNWjQIK1fv15r165VvXr11LFjR89jjRs39vz/sWPHdNVVV2nz5s2KiYlR9+7dFR4erm+++UZTp07VvHnz9PXXX6t27doFrvNc9957r2bMmKErr7xS1113nbZu3aqlS5dq+fLlmj9/vq6//nqv5U+ePKn+/ftr9erVKlOmjFq3bq2KFStq69atevXVV7VgwQItX75cLVu2LNT6V65cqV69eik7O1vNmzfXFVdcIafTqQMHDuiLL76Q0+nUdddd5/WcF154Qffee69cLpdatGih9u3b69ChQ1q9erWWLVumyZMn67HHHiu2vLOzs9W7d299//336ty5s5o0aaKNGzfqk08+0apVq5SYmHhe7z0AABc1EwAAWEatWrVMSebs2bPzPLZlyxYzLCzMlGS+9dZbpmma5tKlS01JZlRUlLls2TKv5WfNmmVKMsPDw81t27Z5PTZo0CBTktmpUyfzxIkTnvjRo0fN9u3bm5L85uHPxIkTPc+77rrrzDNnznge27dvn9mwYUNTkvnvf//b63lpaWnmZ599ZmZmZnrFs7KyzAkTJpiSzN69e+dZ34gRIwrM0f1+7t692yv+0EMPmZLM9u3bm7t27fJ6bMGCBabNZjMvueQS8/jx45747t27PfXVqlXL/PXXXz2PORwOc/To0aYks0ePHoXOw61OnTqmJHPNmjV5Hjt8+LD5008/+a3xXLNnzzYlmSNGjPC7zJAhQzz1p6SkeOInT540e/XqZUoyO3ToUOh1mqbpeW+io6PNlStXej329NNPm5LM2NhY8/Dhw16P/fOf/zQlmX379s3z2PPPP29KMhs0aGA6HI5C5dGtWzdTkvnee+/leezEiRPmunXrvGJffvmlaRiGWaFCBfObb77xeuznn3824+PjTUnm6tWrLzjvVatWed6nli1bmgcPHvQ8lp6ebl577bWmJHPs2LGFqhUAgL8TGlgAAFiIrwbWiRMnzC+++MKsV6+eKcmsVq2aeerUKdM0TfOqq64yJZn33nuvz9fr27evKcn8v//7P0/sjz/+MMPCwkzDMMxffvklz3MSExMvqIEVHR3t9cXcbfHixaYkMyYmxkxPTy/061arVs0MCwsz09LSvOLn28A6evSoGR0dbUZFRZn79+/3+bzbb7/dlGTOnDnTE8vdwFq0aFGe5xw8eNCUZEZGRppZWVkF5pFbqVKlzNjYWL91FEVBDay9e/d6tv+WLVvyPL5//34zKirKlGSuXbu20Ot1vzf33HOPz8fbtGljSjKnTp3qiW3fvt00DMOsVq1anu3r1rt3b1OSuXjx4kLlcemll5qSzGPHjhVqeXfDduHChT4fnz9/vinJHDhw4AXn7W5gGYZhbt68Oc9z1q9fb0oy69atW6jcAQD4O+EeWAAAWFDu+zqVK1dOffr00e+//6569eppyZIlKl26tBwOh9auXStJXr9YmNuYMWMkSatWrfLEvv32W7lcLrVq1UqXXnppnue0aNFCzZo1O+/ce/To4bk0Lre+ffsqLi5OaWlp+umnn/I8vmXLFj333HO66667NHr0aI0cOVIjR46Uw+GQy+XS//73v/POKbdVq1YpPT1dV155pd9fJ3TfL+r777/P85jdbvd5aWGVKlV0ySWXKDMzU0ePHi1STu3atVNqaqqGDx+uH3/8US6Xq0jPLwr39m/ZsqXP7Vy9enVde+21krz3m8IaMWKEz/jw4cMlyeu+X0uWLJFpmurVq5fKli3r83n5bQtf2rVrJ0m6+eab9d1338nhcPhdNiUlRRs3blR0dLT69etX6PVfaN41a9ZU8+bN88SbNGkiSTpw4IDfnAEA+LviHlgAAFhQ7vs6RUREqFKlSrr88svVs2dP2e05w/fRo0eVkZEhKefm4L7Uq1dPkvcX4v379+f7HPdjP//883nlnt/r1q5dW0ePHvXkIEmnT5/WsGHD9Mknn+T7uu77f12oXbt2Scq5V5JhGPkue+TIkTyxqlWr+v1Vw5iYGB0/ftyzXQrr5ZdfVt++ffXuu+/q3XffVdmyZdW2bVt1795dw4YNU82aNYv0evlx7wv5bSdf+01h+Xtddzz3tndvizfffFNvvvlmvq/ra1v4Mn36dP38889aunSpli5dqujoaLVq1Updu3bVzTff7GkSSTn3azNNU+np6V73lSto/Reat7/tGRMTI0nKzMzM9zUBAPg7ooEFAIAF3XLLLX5nVV0MTNP0/P+ECRP0ySefqHHjxnryySfVtm1bVahQQREREZKkDh06aN26dV7PuRDu2U3169fXlVdeme+yuW987hYWVvwT2Js0aaJff/1Vy5Yt09dff63vv/9ea9as0ddff60pU6bozTff1NChQ4t9vcGQezu6t0WLFi18zkjKzX1j/IJUqVJFmzZt0jfffKMVK1Zo7dq12rBhg9auXatp06Zp+vTpevDBB73WX6ZMGQ0cOLDQNVxo3iWxDwEAcLGjgQUAQIiKi4tTZGSkMjMztWvXLp+Xg7lniuS+VM79/3v27PH72vk9VpDdu3cX+Lrx8fGe2Pz58yVJH374oc8afvvtt/POxZcaNWpIkho1aqQ5c+YU62tfCLvdrt69e6t3796ScmacPffcc5o8ebJuvfVWXX/99SpduvQFr8e9/d37hi++9pvC2r17t89fgvS17d3b4sorr9RLL71U5HX5YxiGunbt6rmMLyMjQ3PmzNEdd9yhhx56SIMGDVK9evU86zcMQ2+99VahG0sllTcAAPCPf/4BACBE2e12dezYUZL8NmLeeustSVK3bt08sc6dO8swDP3000/auXNnnuds2bLlvC8flKRly5bpzz//zBNfsmSJjh49qrJly6p169ae+LFjxyRJtWrVyvOcr776SikpKT7X456hld89jny56qqrFBERodWrV/vMsyScT64xMTGaNGmSypUrpzNnzigpKalY1tW5c2eFhYVp8+bN2rJlS57HDx48qC+//FKS935TWO+++26+cXdTSZJ69eolSVq0aFGRL7ssiqioKI0bN07NmjWTy+Xy7N/VqlVTs2bNdPLkSU/NhRGovAEAwFk0sAAACGH33XefJOmVV17RypUrvR6bM2eOFi1apPDwcN19992eeM2aNXX99dfL5XLptttu87q31PHjx3X77bdf0OV66enpuu2225Senu6JJScne3IdN26coqKiPI+570k0c+ZMr9f59ddfNW7cOL/rcc/k+eWXX4qUX+XKlXXXXXfp9OnT6tevn7Zu3ZpnmczMTC1atMhng+985JfrmTNn9Nxzz/m8V9KaNWt04sQJ2Ww2r5lLhVnX9u3bfT5es2ZNDR48WKZp6tZbb/W64fzp06c1duxYZWRkqEOHDurQoUOh1pnbK6+84nWjdkl6/vnntXHjRpUtW9bzwwKS1LJlSw0cOFD79u3TgAEDfM78O336tObOnavDhw8Xav3PPvus/vjjjzzxnTt3embz5W6WPvHEE5Jyfjhh8eLFeZ5nmqY2bNigZcuWlWjeAAAgf1xCCABACOvVq5ceeeQRPfHEE7rmmmt05ZVXqmbNmtq5c6d++ukn2Ww2vfrqq0pISPB63n//+19t2bJFq1evVp06ddS1a1eZpqlVq1YpLi5O/fv316JFi84rp+HDh+vzzz9X3bp11alTJ2VkZOjrr7/W6dOndcUVV2jy5Mley0+cOFGDBg3So48+qvnz5yshIUF//vmn1qxZo06dOqlatWo+f8ntH//4hyZPnqwXX3xR27ZtU40aNRQWFqb+/furf//++eb45JNP6uDBg5o3b57nPkZ169aV3W7X/v37tXnzZp0+fVpLly71eR+soho4cKBWrVqloUOHqkePHrrkkkskSffff78qV66s++67T/fff78uu+wyNWjQQOHh4dqzZ4/Wr18vSXr44YdVsWLFQq3r8ssvV7Vq1ZSYmKhWrVrpsssuU3h4uBo1aqT7779fUs7237lzpzZs2KB69eqpW7dustvt+uabb3TkyBHVqVNHc+fOPa9ab731VnXv3l2dOnVS9erVtW3bNm3dulU2m01vvfVWnl+onD17tk6cOKGlS5eqUaNGat68uerUqSPTNLVnzx5t2bJFWVlZ2rFjhypXrlzg+p944gndf//9aty4sZo0aaLo6GglJyd7fpFw+PDhatWqlWf5fv366YUXXtB9992n/v37q379+mrUqJFiY2N15MgRbdmyRX/++acefPBB9ejRo8TyBgAABTABAIBl1KpVy5Rkzp49u0jPW7p0qdm7d28zLi7OtNvtZpUqVczBgwebGzZs8PuclJQU86677jLj4+PNiIgIMz4+3hw3bpx55MgRc8SIEUXOY+LEiaYkc+LEieauXbvMm266yaxcubIZERFh1q9f33zsscfM06dP+3zut99+a1511VVmhQoVzFKlSplNmzY1p06damZmZppdunQxJZmrVq3K87xPPvnEvPLKK82yZcuahmF41u/mfj93797tc71LliwxBwwYYFavXt0MDw83y5UrZzZp0sS88cYbzXnz5nnlu3v3blOSWatWLb/vgb/1OZ1Oc/r06WZCQoIZFRVlSvLUlJ2dbb766qvmTTfdZDZu3NiMjY01o6OjzXr16pkDBw40V65c6Xd9/mzdutXs37+/WbFiRTMsLMyUZHbp0sVrmdOnT5vTp083W7RoYZYqVcqMiooymzRpYj700EPmsWPHirxOd02maZqvvPKK2aJFCzM6OtqMiYkxe/bsaa5du9bvc51Opzlv3jyzd+/eZuXKlc3w8HAzLi7ObNq0qTlq1Cjzk08+MbOysgqVx3vvvWeOGjXKbNq0qVm+fHkzMjLSrFWrltmrVy/zk08+MV0ul8/nbd261Rw7dqzZoEEDMyoqyixVqpRZt25d89prrzVffPFF88CBAxec96pVq3xuC3/vIwAAOMswzWL6SR8AAPC3NmnSJE2ePFkTJ07UpEmTgp0OAAAALiLcAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJbGPbAAAAAAAABgaczAAgAAAAAAgKXRwAIAAAAAAICl2YOdwPlwuVxKTk5W2bJlZRhGsNMBAAAAAABAPkzT1MmTJ1WtWjWFhRV9PlVINrCSk5NVo0aNYKcBAAAAAACAIti3b5/i4+OL/LyQbGCVLVtWUk7RMTExQc4GAAAAAAAA+UlLS1ONGjU8PZ2iCskGlvuywZiYGBpYAAAAAAAAIeJ8bwXFTdwBAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGkh+SuEAAAAAAAg8EzTlNPplMPhCHYqsAi73S6bzXbevy5Y6PWU6KsDAAAAAICQZ5qmTpw4oSNHjsjpdAY7HViMzWZTpUqVFBsbW2KNLBpYAAAAAAAgX4cOHdKJEycUExOjmJgY2e32Ep9xA+szTVMOh0NpaWk6ePCg0tPTVbVq1RJZFw0sAAAAAADgl9PpVGpqqipWrKgKFSoEOx1YUNmyZRUZGamUlBRVqlRJNput2NfBTdwBAAAAAIBf2dnZMk1TpUuXDnYqsLDSpUvLNE1lZ2eXyOvTwAIAAAAAAAXikkHkp6T3DxpYAAAAAAAAsDQaWAAAAAAAAPBp5MiRql27drDToIEFAAAAAAD+vubMmSPDMPz+Wb9+fbBTLND27ds1adIk7dmzJ9iplBh+hRAAAAAAAPztTZkyRXXq1MkTr1+/fhCyKZrt27dr8uTJ6tq1qyVmS5WEYmlgnTp1Ss8884w2bNigjRs36vjx45o9e7ZGjhzpWcblcumdd97Rxx9/rMTERB07dkx16tTRjTfeqH/961+KiooqjlQAAAAAAEAALdsW7AykHk0v/DV69eqlNm3aXPgLoUQUyyWEKSkpmjJlinbs2KHmzZv7XObMmTMaNWqUjhw5onHjxmnGjBlq166dJk6cqF69esk0zeJIBQAAAAAAoFhNnDhRYWFhWrlypVd87NixioiI0JYtWyRJq1evlmEY+vDDD/XQQw+pSpUqKl26tPr37699+/bled0NGzaoZ8+eio2NValSpdSlSxetXbs2z3IHDhzQmDFjVK1aNUVGRqpOnTq67bbblJWVpTlz5mjw4MGSpG7dunkufVy9erXn+UuXLlWnTp1UunRplS1bVn369NEvv/ySZz2ffvqpmjZtqqioKDVt2lSffPLJhbxtxapYZmBVrVpVBw8eVJUqVbRp0ya1bds2zzIRERFau3atOnTo4In93//9n2rXrq2JEydq5cqVuvrqq4sjHQAAAAAAgCJJTU1VSkqKV8wwDMXFxemRRx7R4sWLNWbMGG3dulVly5bVV199pTfeeEOPP/54nsk8U6dOlWEYevDBB/Xnn39qxowZuvrqq7V582ZFR0dLkr7++mv16tVLrVu39jTIZs+ere7du2vNmjVq166dJCk5OVnt2rXTiRMnNHbsWDVu3FgHDhzQwoULdebMGXXu3Fnjx4/Xiy++qIceekhNmjSRJM9/3333XY0YMULXXnutnnrqKZ05c0avvPKKOnbsqMTERM8lh8uWLdPAgQN16aWXavr06Tp69KhGjRql+Pj4knzbC61YGliRkZGqUqVKvstERER4Na/crr/+ek2cOFE7duyggQUAAAAAAILCV08iMjJSGRkZCg8P1zvvvKPWrVvr3nvv1TPPPKMxY8aoTZs2+ve//53neceOHdOOHTtUtmxZSVKrVq10ww036I033tD48eNlmqbGjRunbt26aenSpTIMQ5J06623KiEhQY888oiWLVsmSZowYYIOHTqkDRs2eF3iOGXKFJmmqXLlyqlTp0568cUXdc0116hr166eZU6dOqXx48frlltu0euvv+6JjxgxQo0aNdK0adM88QcffFCVK1fWd999p9jYWElSly5d1KNHD9WqVesC390LF/SbuB86dEiSVKFChSBnAgAAAAAA/q7++9//qmHDhl4xm83m+f+mTZtq8uTJmjBhgn7++WelpKRo2bJlstvztlaGDx/uaV5J0qBBg1S1alUtWbJE48eP1+bNm/Xbb7/pkUce0dGjR72ee9VVV+ndd9+Vy+WSlHNZX79+/Xzen8vd+PJn+fLlOnHihG666Sav2WU2m03t27fXqlWrJEkHDx7U5s2b9e9//9vTvJKka665RpdeeqlOnz6d73oCIegNrKeffloxMTHq1auX32UyMzOVmZnp+XtaWpokyeFwyOFwSJLCwsIUFhYml8vl2ci5406n0+s+W/7iNptNhmF4Xjd3XJKcTmeh4na7XaZpesUNw5DNZsuTo784NVETNVETNVETNVETNVETNVETNVFTsGtyOBye1/N9/2pDUnDj53tbbcMwPDW1bdvW0yTKHc9d8/33368PPvhAGzdu1NSpU9WkSROZpulZ3r1s/fr1veLu2J49e2Sapn777TdJOTOh/Dlx4oSysrKUlpamhISEfO8dfm6u7v8mJSVJkrp37+7zeTExMZKkPXv2eOWd+z1o1KiRfvrppzxxf3nk7tXk3vfO3f+KKqgNrGnTpmnFihV6+eWXVa5cOb/LTZ8+XZMnT84TT0xMVOnSpSVJFStWVL169bR7924dOXLEs0x8fLzi4+OVlJSk1NRUT7xu3bqqVKmStm3bpvT0dE+8cePGKleunBITE70O4mbNmikiIkKbNm3yyqFNmzbKysrSzz//7InZbDa1bdtWqamp2rlzpyceHR2t5s2bKyUlRbt27fLEY2Nj1eSHH5QcHq794eGeeEWHQ/WysrQ7IkJHcnV047OzFZ+draTISKXm6gbXzcpSJYdD26KilB529v78jTMyVM7lUmJ0tJy5urPN0tMVYZraVKqUd03/+Efx1NSkiZKTk7V///6zNYX6dqImaqImaqImaqImaqImaqImavob1hQVFSUpp6mVkZHhiYeFhUkqJafT6dWgCAsLU3h4RJ64zWaT3R4uh8PhlYvdbpfNZld2drZXs84dz8rK8mqahIeHKyzM5omfPu3wvMdhYWF5ZgyVLl1aLpfL630xDMMTl6T09HSdPn1aYWFhKlWqlBwOh9dkGpvNpv3793uaT5s3b9bp06dlt9sVFRWlzMxMz3uTmZmp7OxsRUREKCMjQ06nU06nUy6XSw6Hw7POJ554Qs2aNZOUc+slm82mjIwMT/PrzJkznvXnV5M7T/f63dvJ/fdZs2apVq1acjgcys7O9rxGRESEJHm2UWZmZp6a3A3M06dPKyIiwqsmt8jISElSdna2tm07+7OUufc992Sk82WYxfzzf+6buM+ePVsjR470u9yHH36om266SaNHj9asWbPyfU1fM7Bq1Kiho0ePerqFVulMuxW52z53rlySXLleI+yvP/7iTnn3oP3FbcrpS5/b63S3vpznxocNK56aLPwvCNRETdRETdRETdRETdRETdRETdRUuJoyMjL0xx9/qG7dup5GRW7Lfwn+DKxrEnw8XAiGYWj27NkaPXq0Nm7c6HMGlpvL5VLnzp21a9cujRo1StOnT9fChQs1YMAAz/KrV69W9+7d9e9//1vTpk3zmpkVHx+vZs2aaenSpdq0aZPatWunV199VWPHjvXKJ/d6XS6Xypcvr27duuX7i4AfffSRBg8erK+//lrdunXzvMaCBQs0ZMgQffnll7r22mt9zpwyDEPJycmqXr26HnzwQU2fPt0rl6ZNm+r06dPavXu33/dGyund7Nq1SzVr1vQ0PHPve2lpaYqLi1Nqaqqnl1MUQZmBtXz5cg0fPlx9+vTRq6++WuDykZGRPg8Su92e51pT9wF7LvcBWNi4r2tYixo3DMNn3F+O7gZUYeO+M/cf97ex88T/mqVVLDUVMR4S24maqMlPjkWNUxM1SdTkL8eixqmJmiRq8pdjUePURE0SNfnLsajxi6Umu90u46/vie7/5hXcuN+0CiF3bbnrO7fW559/Xt9//70WLVqkPn366JtvvtHtt9+uLl26qEKFCl7Pf/fdd/XQQw+pbNmyMgxDCxcu1MGDB/Xggw/KMAy1bt1a9erV03/+8x/dfPPNKlOmjNd6jxw5oooVK8pms+kf//iH3nvvPf3444957oPlnqnlfr57Rp47j549eyomJkbTp09X9+7dFZ7rqi9JnvVUq1ZNLVq00DvvvKMJEyZ47oO1YsUKbd++XbVq1cr3vckd99Wr8RUrqoA3sDZs2KDrr79ebdq00fz58y+4AAAAAAAAgAu1dOlSr0s+3Tp06KDMzEw9+uijGjlypPr16ydJmjNnjlq0aKHbb79d8+fP93pO+fLl1bFjR40aNUqHDx/WjBkzVL9+ff3f//2fpJym5KxZs9SrVy8lJCRo1KhRql69ug4cOKBVq1YpJiZGixcvlpRz+6Vly5apS5cuGjt2rJo0aaKDBw9qwYIF+u6771SuXDm1aNFCNptNTz31lFJTUxUZGanu3burUqVKeuWVVzRs2DC1atVKN954oypWrKg//vhDX3zxha688kq99NJLknJu39SnTx917NhRo0eP1rFjxzRz5kwlJCTo1KlTJfnWF0pAu0c7duxQnz59VLt2bX3++eeKjo4O5OoBAAAAAAB8euyxx3zGZ82apddee00VKlTQjBkzPPEGDRpo+vTpuvvuuzV//nzdcMMNnsceeugh/fzzz5o+fbpOnjypq666Si+//LJK5boHddeuXbVu3To9/vjjeumll3Tq1ClVqVJF7du316233upZrnr16tqwYYMeffRRzZ07V2lpaapevbp69erleb0qVaro1Vdf1fTp0zVmzBg5nU6tWrVKlSpV0j//+U9Vq1ZNTz75pJ555hllZmaqevXq6tSpk0aNGuVZT8+ePbVgwQI98sgjmjBhgurVq6fZs2frs88+0+rVq4vpXT5/xXYPrJdeekknTpxQcnKyXnnlFQ0YMEAtW7aUJN11110KCwtTQkKCDhw4oGnTpql69epez69Xr56uuOKKQq0rLS1NsbGx533dpCW9806wMzhr+PBgZwAAAAAAsIiMjAzt3r1bderU8dzbCL6tXr1a3bp104IFCzRo0KBgpxNQBe0nF9rLKbYZWM8++6z27t3r+fvHH3+sjz/+WJI0dOhQSdK+ffskSf/+97/zPH/EiBGFbmABAAAAAADg76PYGlh79uwpcJli/sFDAAAAAAAA/A34+nE7AAAAAAAAwDL4CUAAAAAAAIBi0LVrV64+KyHMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAH9bc+bMkWEYioqK0oEDB/I83rVrVzVt2jQImSE3e7ATAAAAAAAAIezLL4OdgdSz5wW/RGZmpp588knNnDmzGBJCcWMGFgAAAAAA+Ntr0aKF3njjDSUnJwc7FfhAAwsAAAAAAPztPfTQQ3I6nXryySfzXc7hcOjxxx9XvXr1FBkZqdq1a+uhhx5SZmamZ5l7771XcXFxMk3TE7vrrrtkGIZefPFFT+zw4cMyDEOvvPJK8Rd0kaGBBQAAAAAA/vbq1Kmj4cOHFzgL65ZbbtFjjz2mVq1a6fnnn1eXLl00ffp03XjjjZ5lOnXqpGPHjumXX37xxNasWaOwsDCtWbPGKyZJnTt3LoGKLi40sAAAAAAAACQ9/PDDcjgceuqpp3w+vmXLFr399tu65ZZbtGDBAt1+++16++239a9//UuffvqpVq1aJUnq2LGjpLMNqtTUVG3dulUDBw7M08AqX768Lr300hKuLPTRwAIAAAAAAJBUt25dDRs2TK+//roOHjyY5/ElS5ZIyrlEMLf77rtPkvTFF19IkipWrKjGjRvr22+/lSStXbtWNptN999/vw4fPqzffvtNUk4Dq2PHjjIMo8RquljQwAIAAAAAAPjLI488IofD4fNeWHv37lVYWJjq16/vFa9SpYrKlSunvXv3emKdOnXyzLZas2aN2rRpozZt2qh8+fJas2aN0tLStGXLFnXq1KlkC7pI0MACAAAAAAD4S926dTV06FC/s7AkFWrGVMeOHXXgwAHt2rVLa9asUadOnWQYhjp27Kg1a9bo+++/l8vlooFVSDSwAAAAAAAAcnHPwjr3Xli1atWSy+XyXALodvjwYZ04cUK1atXyxNyNqeXLl+uHH37w/L1z585as2aN1qxZo9KlS6t169YlXM3FgQYWAAAAAABALvXq1dPQoUP12muv6dChQ5547969JUkzZszwWv65556TJPXp08cTq1OnjqpXr67nn39e2dnZuvLKKyXlNLZ+//13LVy4UJdffrnsdnsJV3NxoIEFAAAAAABwjocffljZ2dn69ddfPbHmzZtrxIgRev311zVkyBC9/PLLGjlypJ5++mn94x//ULdu3bxeo1OnTvr111/VtGlTXXLJJZKkVq1aqXTp0kpKSuLywSKggQUAAAAAAHCO+vXra+jQoXnis2bN0uTJk/XDDz/onnvu0ddff60JEybogw8+yLOsu0HVsWNHT8xut+uKK67wehwFM0zTNIOdRFGlpaUpNjZWqampiomJCXY6xeOdd4KdwVnDhwc7AwAAAACARWRkZGj37t2qU6eOoqKigp0OLKqg/eRCeznMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAKCGGYWjSpEnBTiPk0cACAAAAAAB/S4ZhFOrP6tWrg53q35492AkAAAAAAIAQ9r//BTsDqX7983rau+++6/X3d955R8uXL88Tb9KkyXmnhuJBAwsAAAAAAPwtDR061Ovv69ev1/Lly/PEEXxcQggAAAAAAODH6dOndd9996lGjRqKjIxUo0aN9Oyzz8o0Ta/lMjMz9f/+3/9TxYoVVbZsWfXv31/79+/P83p79+7V7bffrkaNGik6OlpxcXEaPHiw9uzZ41lm165dMgxDzz//fJ7nf//99zIMQ++//36x12plNLAAAAAAAAB8ME1T/fv31/PPP6+ePXvqueeeU6NGjXT//ffr3nvv9Vr2lltu0YwZM9SjRw89+eSTCg8PV58+ffK85g8//KDvv/9eN954o1588UWNGzdOK1euVNeuXXXmzBlJUt26dXXllVdq7ty5eZ4/d+5clS1bVtddd13JFG1RXEIIAAAAAADgw6JFi/T111/riSee0MMPPyxJuuOOOzR48GC98MILuvPOO1WvXj1t2bJF7733nm6//Xb997//9Sx388036+eff/Z6zT59+mjQoEFesX79+umKK67QRx99pGHDhkmShg8frltvvVU7d+5U48aNJUnZ2dmaP3++BgwYoFKlSpV0+ZbCDCwAAAAAAAAflixZIpvNpvHjx3vF77vvPpmmqaVLl3qWk5RnuXvuuSfPa0ZHR3v+Pzs7W0ePHlX9+vVVrlw5/fTTT57HbrjhBkVFRXnNwvrqq6+UkpLyt7xHFw0sAAAAAAAAH/bu3atq1aqpbNmyXnH3rxLu3bvX89+wsDDVq1fPa7lGjRrlec309HQ99thjnntqVahQQRUrVtSJEyeUmprqWa5cuXLq16+f5s2b54nNnTtX1atXV/fu3YutxlBBAwsAAAAAACBA7rrrLk2dOlU33HCD5s+fr2XLlmn58uWKi4uTy+XyWnb48OHatWuXvv/+e508eVKLFi3STTfdpLCwv187h3tgAQAAAAAA+FCrVi2tWLFCJ0+e9JqFtXPnTs/j7v+6XC79/vvvXrOufv311zyvuXDhQo0YMUL/+c9/PLGMjAydOHEiz7I9e/ZUxYoVNXfuXLVv315nzpzx3CPr7+bv17IDAAAAAAAohN69e8vpdOqll17yij///PMyDEO9evWSJM9/X3zxRa/lZsyYkec1bTabTNP0is2cOVNOpzPPsna7XTfddJPmz5+vOXPm6LLLLlOzZs0upKSQxQwsAAAAAAAAH/r166du3brp4Ycf1p49e9S8eXMtW7ZMn332me655x7PPa9atGihm266SS+//LJSU1PVoUMHrVy5Uv/73//yvGbfvn317rvvKjY2VpdeeqnWrVunFStWKC4uzmcOw4cP14svvqhVq1bpqaeeKtF6rYwGFgAAAAAAgA9hYWFatGiRHnvsMX344YeaPXu2ateurWeeeUb33Xef17JvvfWW53K/Tz/9VN27d9cXX3yhGjVqeC33wgsvyGazae7cucrIyNCVV16pFStW6Nprr/WZQ+vWrZWQkKAdO3bo5ptvLrFarc4wz523FgLS0tIUGxur1NRUxcTEBDud4vHOO8HO4Kzhw4OdAQAAAADAIjIyMrR7927VqVNHUVFRwU7nb6lly5YqX768Vq5cGexU/CpoP7nQXg73wAIAAAAAALCoTZs2afPmzRr+N59swiWEAAAAAAAAFrNt2zb9+OOP+s9//qOqVatqyJAhwU4pqJiBBQAAAAAAYDELFy7UqFGjlJ2drffff/9vf/kmDSwAAAAAAACLmTRpklwul3bs2KEuXboEO52go4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAApkmmawU4CFlfT+QQMLAAAAAAD4ZbPZJEnZ2dlBzgRW5t4/3PtLcaOBBQAAAAAA/AoPD1dkZKRSU1OZhQWfTNNUamqqIiMjFR4eXiLrsJfIqwIAAAAAgItGhQoVdODAAe3fv1+xsbEKDw+XYRjBTgtBZpqmsrOzlZqaqlOnTql69eolti4aWAAAAAAAIF8xMTGSpJSUFB04cCDI2cBqIiMjVb16dc9+UhJoYAEAAAAAgALFxMQoJiZG2dnZcjqdwU4HFmGz2UrsssHcaGABAAAAAIBCCw8PD0jDAsitWG7ifurUKU2cOFE9e/ZU+fLlZRiG5syZ43PZHTt2qGfPnipTpozKly+vYcOG6ciRI8WRBgAAAAAAAC5CxTIDKyUlRVOmTFHNmjXVvHlzrV692udy+/fvV+fOnRUbG6tp06bp1KlTevbZZ7V161Zt3LhRERERxZEOAAAAAAAALiLF0sCqWrWqDh48qCpVqmjTpk1q27atz+WmTZum06dP68cff1TNmjUlSe3atdM111yjOXPmaOzYscWRDgAAAAAAAC4ixXIJYWRkpKpUqVLgch999JH69u3raV5J0tVXX62GDRtq/vz5xZEKAAAAAAAALjLF0sAqjAMHDujPP/9UmzZt8jzWrl07JSYmBioVAAAAAAAAhJCA/QrhwYMHJeVcbniuqlWr6tixY8rMzFRkZGSexzMzM5WZmen5e1pamiTJ4XDI4XBIksLCwhQWFiaXyyWXy+VZ1h13Op0yTbPAuM1mk2EYntfNHZeU56dC/cXtdrtM0/SKG4Yhm82WJ0fDMGST5PrrjyfHv/74izslmYWI2yQZkrwryonrr+W94n+9Hxdck494yG8naqImaqImaqImaqImaqImaqImaqImaipyTefWVVQBa2Clp6dLks8GVVRUlGcZX49Pnz5dkydPzhNPTExU6dKlJUkVK1ZUvXr1tHv3bq9fNYyPj1d8fLySkpKUmprqidetW1eVKlXStm3bPLlJUuPGjVWuXDklJiZ6bexmzZopIiJCmzZt8sqhTZs2ysrK0s8//+yJ2Ww2tW3bVqmpqdq5c6cnHh0drebNmyslJUW7du3yxGNjY9VEUnJ4uPbn+inSig6H6mVlaXdEhI7Yz26q+OxsxWdnKykyUqk2mydeNytLlRwObYuKUnrY2cl1jTMyVM7lUmJ0tJyGcbam9HRFmKY2lSrlXZPTWTw1NWmi5ORk7d+//2xNob6dqImaqImaqImaqImaqImaqImaqImaqKnINbknI50vw8zdGisG7pu4z549WyNHjswTf+eddzRs2DCv5zzwwAN65plnlJGRUegZWDVq1NDRo0cVExMj6SLoeM6da50ZWH9tn1Dp4nrlfpF0pqmJmqiJmqiJmqiJmqiJmqiJmqiJmi6mmtLS0hQXF6fU1FRPL6coAjYDy33poPtSwtwOHjyo8uXL+2xeSTmztnw9ZrfbZbd7l+B+087l3rCFjZ/7uucTNwzDZ9xfju4GVGHjvjP3H/e3sfPE/5qlVSw1FTEeEtuJmqjJT45FjVMTNUnU5C/HosapiZokavKXY1Hj1ERNEjX5y7GocWqiJoma3Dn6y7+wAnYT9+rVq6tixYp5prxJ0saNG9WiRYtApQIAAAAAAIAQErAGliQNHDhQn3/+ufbt2+eJrVy5UklJSRo8eHAgUwEAAAAAAECIKLZLCF966SWdOHFCycnJkqTFixd7bgB21113KTY2Vg899JAWLFigbt266e6779apU6f0zDPP6LLLLtOoUaOKKxUAAAAAAABcRIrtJu61a9fW3r17fT62e/du1a5dW5L0yy+/6N5779V3332niIgI9enTR//5z39UuXLlQq8rLS1NsbGx533jL0t6551gZ3DW8OHBzgAAAAAAAFxELrSXU2wzsPbs2VOo5RISEvTVV18V12oBAAAAAABwkQvoPbAAAAAAAACAoqKBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEsLeAPrt99+04033qj4+HiVKlVKjRs31pQpU3TmzJlApwIAAAAAAIAQYA/kyvbt26d27dopNjZWd955p8qXL69169Zp4sSJ+vHHH/XZZ58FMh0AAAAAAACEgIA2sN59912dOHFC3333nRISEiRJY8eOlcvl0jvvvKPjx4/rkksuCWRKAAAAAAAAsLiAXkKYlpYmSapcubJXvGrVqgoLC1NEREQg0wEAAAAAAEAICGgDq2vXrpKkMWPGaPPmzdq3b58+/PBDvfLKKxo/frxKly4dyHQAAAAAAAAQAgJ6CWHPnj31+OOPa9q0aVq0aJEn/vDDD+uJJ57w+7zMzExlZmZ6/u6eyeVwOORwOCRJYWFhCgsLk8vlksvl8izrjjudTpmmWWDcZrPJMAzP6+aOS5LT6SxU3G63yzRNr7hhGLLZbHlyNAxDNkmuv/54cvzrj7+4U5JZiLhNkiHJu6KcuP5a3iv+1/txwTX5iIf8dqImaqImaqImaqImaqImaqImaqImaqKmItd0bl1FFdAGliTVrl1bnTt31sCBAxUXF6cvvvhC06ZNU5UqVXTnnXf6fM706dM1efLkPPHExETPrK2KFSuqXr162r17t44cOeJZJj4+XvHx8UpKSlJqaqonXrduXVWqVEnbtm1Tenq6J964cWOVK1dOiYmJXhu7WbNmioiI0KZNm7xyaNOmjbKysvTzzz97YjabTW3btlVqaqp27tzpiUdHR6t58+ZKSUnRrl27PPHY2Fg1kZQcHq794eGeeEWHQ/WysrQ7IkJH7Gc3VXx2tuKzs5UUGalUm80Tr5uVpUoOh7ZFRSk97OzkusYZGSrncikxOlpOwzhbU3q6IkxTm0qV8q7J6Syempo0UXJysvbv33+2plDfTtRETdRETdRETdRETdRETdRETdRETdRU5Jrck5HOl2Hmbo2VsA8++ECjR49WUlKS4uPjPfFRo0Zp/vz5+uOPPxQXF5fneb5mYNWoUUNHjx5VTEyMpIug4zl3rnVmYA0bVjw10ZmmJmqiJmqiJmqiJmqiJmqiJmqiJmqiJodDaWlpiouLU2pqqqeXUxQBbWB17txZTqdTa9eu9Yp/8sknGjBggJYvX66rr766wNdJS0tTbGzseRdtSe+8E+wMzho+PNgZAAAAAACAi8iF9nICehP3w4cP5+kMSlJ2drYkXfD1kAAAAAAAALj4BLSB1bBhQyUmJiopKckr/v777yssLEzNmjULZDoAAAAAAAAIAQG9ifv999+vpUuXqlOnTrrzzjsVFxenzz//XEuXLtUtt9yiatWqBTIdAAAAAAAAhICANrA6d+6s77//XpMmTdLLL7+so0ePqk6dOpo6daoeeOCBQKYCAAAAAACAEBHQBpYktWvXTkuWLAn0agEAAAAAABCiAnoPLAAAAAAAAKCoaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNLswU4AAAAAQMGWbQt2Bmf1aBrsDAAAfzc0sAAAAAAUOxpuAIDixCWEAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDR7sBMAAAAAgmXZtmBncFaPpsHO4O+L/QAArC8oM7B++ukn9e/fX+XLl1epUqXUtGlTvfjii8FIBQAAAAAAABYX8BlYy5YtU79+/dSyZUs9+uijKlOmjH7//Xft378/0KkAAAAAAAAgBAS0gZWWlqbhw4erT58+WrhwocLCuAUXAAAAAAAA8hfQDtK8efN0+PBhTZ06VWFhYTp9+rRcLlcgUwAAAAAAAECICWgDa8WKFYqJidGBAwfUqFEjlSlTRjExMbrtttuUkZERyFQAAAAAAAAQIgJ6CeFvv/0mh8Oh6667TmPGjNH06dO1evVqzZw5UydOnND777/v83mZmZnKzMz0/D0tLU2S5HA45HA4JElhYWEKCwuTy+XymtXljjudTpmmWWDcZrPJMAzP6+aOS5LT6SxU3G63yzRNr7hhGLLZbHlyNAxDNkmuv/54cvzrj7+4U5JZiLhNkiHJu6KcuP5a3iv+1/txwTX5iIf8dqImaqImaqImaqKmi6omM/eHLOOvT0fmOZ+O/MSNsJyavOOGjDCbTNOlc17cd9wIk2GEyTRdcjjyr8l05Vredc4nPiOnJtN1zie+EqrJ4Sh4O/mtNU/ugakpv33vbJoFb6eSrin3oRZqx1NuF8s5gpqoiZqKr6Zz6yqqgDawTp06pTNnzmjcuHGeXx0cMGCAsrKy9Nprr2nKlClq0KBBnudNnz5dkydPzhNPTExU6dKlJUkVK1ZUvXr1tHv3bh05csSzTHx8vOLj45WUlKTU1FRPvG7duqpUqZK2bdum9PR0T7xx48YqV66cEhMTvTZ2s2bNFBERoU2bNnnl0KZNG2VlZennn3/2xGw2m9q2bavU1FTt3LnTE4+Ojlbz5s2VkpKiXbt2eeKxsbFqIik5PFz7w8M98YoOh+plZWl3RISO2M9uqvjsbMVnZyspMlKpNpsnXjcrS5UcDm2LilJ6rvuLNc7IUDmXS4nR0XIaxtma0tMVYZraVKqUd01OZ/HU1KSJkpOTvW7QH/LbiZqoiZqoiZqoiZouqpqyTpytKbxCMxm2CGUd9q4ponIbmc4sZaecrckwbIqo0lZmVqqyj52tybBHK6Jic7nSU+RIPVtTWGSswss3kfNUspynztZki64oe7l6cqbu1qZN+deUdVKyx9aVrVQlZR/dJtNxtqbw8o1lRJZT9p+JMs2Sr2nTmYK3kzN1t5zpZ2uylYmXvWy8HCeS5Mo8u50CUVNB+17WycJvp5KuadOZszWF2vF0MZ4jqImaqKn4anJPRjpfhpm7NVbCmjZtql9++UXffPONOnfu7Il/++236tKli95++20NHz48z/N8zcCqUaOGjh49qpiYGEkXQcdz7lzrzMAaNqx4aqIzTU3URE3URE3URE0Wr2nl9lxJBnkG1lVN8q9p5fZcywd5BtZVlxa8nb7aap0ZWNck5L/vnd0Pgj8D66pLz4ZD7XjK7WI5R1ATNVFT8dWUlpamuLg4paameno5RRHQGVjVqlXTL7/8osqVK3vFK1WqJEk6fvy4z+dFRkYqMjIyT9xut8tu9y7B/aady71hCxs/93XPJ24Yhs+4vxzdDajCxn1n7j/ub2Pnif81S6tYaipiPCS2EzVRk58cixqnJmqSqMlfjkWNUxM1SedXk+HrQ5bh51OTj7hhGH7iYfL14vnF7fb8a8r9NCPMd01GWOFz9xcvTE25N6O/7eG3Vr+5l2xN+e1756ZZ5O1XjDX5OqRC5Xi60Dg1UZNETf5yLGrcijX5y7+wAnoT99atW0uSDhw44BVPTk6WlDNFDQAAAAAAAMgtoA2sG264QZL05ptvesVnzZolu92url27BjIdAAAAAAAAhICAXkLYsmVLjR49Wm+99ZYcDoe6dOmi1atXa8GCBZowYYKqVasWyHQAAAAAAAAQAgLawJKkV199VTVr1tTs2bP1ySefqFatWnr++ed1zz33BDoVAAAAAAAAhICAN7DCw8M1ceJETZw4MdCrBgAAAAAAQAgK6D2wAAAAAAAAgKKigQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEsL+E3cAQAAAADnb9m2YGdwVo+mwc4AwN8FM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBp9mAnAAAAgIvHsm3BzuCsHk2DnQEAACguzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXxK4QAAAAAgBLBL5MCKC7MwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXZg50AAAAAAABWsGxbsDM4q0fTYGcAWAszsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBp3MQdAAAAAIAQww3n8XfDDCwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBq/QggAAAAAAEoUv5qIC8UMLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYmj3YCQAAACB/y7YFO4OzejQNdgYAAODviAYWAAAAAADAX/iHI2viEkIAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBq/QmgRv6cEO4Oz6gU7AQAAAAAAgFyYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEsLegNr6tSpMgxDTZs2DXYqAAAAAAAAsKCgNrD279+vadOmqXTp0sFMAwAAAAAAABZmD+bK//Wvf+nyyy+X0+lUSkpKMFMBAAAAAACARQVtBta3336rhQsXasaMGcFKAQAAAAAAACEgKA0sp9Opu+66S7fccosuu+yyYKQAAAAAAACAEBGUSwhfffVV7d27VytWrCjU8pmZmcrMzPT8PS0tTZLkcDjkcDgkSWFhYQoLC5PL5ZLL5fIs6447nU6Zpllg3GazyTAMz+vmjks5zbfCxO12u0zT9IobhiGbzZYnR8MwJEmmJNPI9SJmTofRJUm54oaZ81dX7mXPM65z1yl53o8LrclXPNS3EzVREzVREzVRUzBqMv/6MGCE2WSaLnfAXZXvuBEmwwjzH3c5lfPpo6B4Tk2mK6cmd2n+cjdN21//4x03wnJq8o6XbE0uV8HbyXu1vnP3Fy/umhyO/Pc90+W/1nO3U0nX5HAUfDwV9753oTXld444m2Zgjydfuec+ffg7zqTAH0/+4qaZ/3kvZ3nftXqFA3COKMy5POc4C+zx5C/ucOQ/PknBO57OrUkqeMz1lBvA48lfPPfu6utzhOmyxpgr5ewHF8tno3PPE0UV8AbW0aNH9dhjj+nRRx9VxYoVC/Wc6dOna/LkyXniiYmJnhvAV6xYUfXq1dPu3bt15MgRzzLx8fGKj49XUlKSUlNTPfG6deuqUqVK2rZtm9LT0z3xxo0bq1y5ckpMTPTa2M2aNVNERIQ2bdrklUObNm2UlZWln3/+2ROz2Wxq27atUlNTtXPnTk88OjpazZs3V0pKinbt2uWJx8bGKkJSaplwpZYJ98TLpDsUl5ql47EROhV9dlPFnspWuVPZOlIuUhmRNk+8fGqWyqY7dCguStn2s5PrKh3LUHSWS/srRcs0znarqqaky+40ta9yKa+a6jidxVJTkyZNlJycrP3793viob6dqImaqImaqImaglFT1knJsEcromJzudJT5Eg9W1NYZKzCyzeR81SynKfO1mSLrih7uXpypu6WM/1sTbYy8bKXjZfjRJJcmWdrssfWla1UJWUf3SbTcbam8PKNZUSWU/afiTJNpzadyb8mlWoj05ml7JSzNRmGTRFV2srMSlX2sbPbqaRrSqlS8HbKOnF2O4VXaCbDFqGsw941RVQOTE2bNuW/72WdLPx2KumaNp0p+Hgq7n3vQmoq6ByRdbLw26mka3IfY5L/c4SiA388+asptWb+571gHU++airMuTzrZOCPJ381bTqT//gkBed48lWTVPCY6z7OAnk8+avJfZz5+xyRnW6NMVfK2Q8uls9G7slI58swc7fGAuC2227TihUr9MsvvygiIkKS1LVrV6WkpGjbtm0+n+NrBlaNGjV09OhRxcTESLL+v5xK+Xc897ww1zIzsOrfM6xYagrFf+GmJmqiJmqiJmqyYk0rt0tWmYF11aX5575yh3VmYF3TtODtlPPenq3VV+6BmjFyVZP8972V2/3XGugZI1ddWvDx9NVW68zAuiYh/3PE2f0g+DOw3MeY5P84+3qndWZg9bgs//Pesq3WmYF1VZOCz+U5x5k1ZmBddWn+49OK7daZgXVts4LHXM9xZoEZWLmPM1+fI1Zut8aYK+XsBxfLZ6O0tDTFxcUpNTXV08spioDOwPrtt9/0+uuva8aMGUpOTvbEMzIylJ2drT179igmJkbly5f3el5kZKQiIyPzvJ7dbpfd7l2C+007l3vDFjZ+7uueT9wwDJ9xfzkaOttU8lpe8tqnPXE/rceixs9dp/uSxuKoqajxUNhO1ERN/nIsapyaqEmiJn85FjV+sddkhOWOh3kHzjce5jt3/3H7X7nmn7tnsrfhuybf8ZKpyb0p89tOPl7GZ47+4sVZk92e/77ntR8UsJ3yPlC8NeXe7H4/2xbzvpf3gaLVlN854tw0A3U85X3AnucYk/yfIwJ5PPmLu495f+e3omy/kq6pMOdy7+MsMMeTv3ihjrMgHU++4gWNrYU+zgJQ07m767nnCHdawR5zJe/9INQ/G/nLv7ACehP3AwcOyOVyafz48apTp47nz4YNG5SUlKQ6depoypQpgUwJAAAAAAAAFhfQGVhNmzbVJ598kif+yCOP6OTJk3rhhRdUr169QKYEAAAAAAAAiwtoA6tChQr6xz/+kSc+Y8YMSfL5GAAAAAAAAP7eAnoJIQAAAAAAAFBUAZ2B5c/q1auDnQIAAAAAAAAsihlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNEvcAwuhZdm2YGdwVo+mwc4AAAAAAACUNGZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0rgHFgAA+Nvhfo4AAAChhRlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDR7sBMAStqybcHO4KweTYOdAQAAAAAAoYcZWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNH6FEAAAFAt+9RUAAAAlhRlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNHuwEwBw1rJtwc7grB5Ng50BAAAAAAA5mIEFAAAAAAAAS2MGFgAAFsWsTAAAACAHM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaQFtYP3www+68847lZCQoNKlS6tmzZq64YYblJSUFMg0AAAAAAAAEELsgVzZU089pbVr12rw4MFq1qyZDh06pJdeekmtWrXS+vXr1bRp00CmAwAAAAAAgBAQ0AbWvffeq3nz5ikiIsITGzJkiC677DI9+eSTeu+99wKZDgAAAAAAAEJAQBtYHTp0yBNr0KCBEhIStGPHjkCmAgAAAAAAgBAR9Ju4m6apw4cPq0KFCsFOBQAAAAAAABYU0BlYvsydO1cHDhzQlClT/C6TmZmpzMxMz9/T0tIkSQ6HQw6HQ5IUFhamsLAwuVwuuVwuz7LuuNPplGmaBcZtNpsMw/C8bu64JDmdzkLF7Xa7TNP0ihuGIZvNlidHwzAkSaYk08j1ImZOh9ElSbnihpnzV1fuZc8zrnPXKXneD381ma7ccUNGmE2m6ZJMV8FxI0yGEeY/7nL+9U4UFC/8djJdOcvn/MW7JiMspybveMnV5HDkv+9JhkyXd03+ci/pmqTQPZ58xUP9HEFNf9OaXHnPe8E6RzgcBddkmud3Li+JmpzO/LdTSY9PRanJNAve98y/PgwEc8x11+Q+rPwdN6ZpjTFXklyugs8R3qsNzpjrrsnXcZY795zPNIE/nnzl7nAUfN4LxvGUX035ncvPphnY48lX7rmHLn/HmRT448lf3DTzH3O9vzsoYMeTr3hhPke4vzsEc8zNfZzl9zlCssaYm/Nts+DPRp5ygzjmuuO5d1dfn/dMlzXGXClnPwi5z7B+xtxzzxNFFdQG1s6dO3XHHXfoiiuu0IgRI/wuN336dE2ePDlPPDExUaVLl5YkVaxYUfXq1dPu3bt15MgRzzLx8fGKj49XUlKSUlNTPfG6deuqUqVK2rZtm9LT0z3xxo0bq1y5ckpMTPTa2M2aNVNERIQ2bdrklUObNm2UlZWln3/+2ROz2Wxq27atUlNTtXPnTk88OjpazZs3V0pKinbt2uWJx8bGKkJSaplwpZYJ98TLpDsUl5ql47EROhV9dlPFnspWuVPZOlIuUhmRNk+8fGqWyqY7dCguStn2s5PrKh3LUHSWS/srRcs0znarqqaky+40ta9yKa+a6jid+daUdfhsTYY9WhEVm8uVniJH6tmawiJjFV6+iZynkuU8tf/s60RXlL1cPTlTd8uZfnY72crEy142Xo4TSXJlnt1O9ti6spWqpOyj22Q6zm6n8PKNZUQWbjtlnZQiKreR6cxSdsrZmgzDpogqbWVmpSr7WGBq2nQm/31PKqfsPxNl5jrZhldoJsMWoazD3vteSdckhe7x1KRJEyUnJ2v//rM1hfo5gpr+njVl/Zn3vBesc8SmTQXX5DTP71xeEjVtM/PfTiU9PhWlpvT0gve9rJPBH3PdNW06kxP3dzyplDXGXElKqVLwOSLrRPDHXHdNmzblf47IOhmc48lXTZvOFHzeC8bx5K+mgs7lWScLv51Kuib3MSb5H58UHfjjyV9NqTXzH3ODdTz5qqkwnyOyTgZ/zHXXtOlM/p8jJGuMuYY9WlLBn43cx1kwx1x3Te7jzN/nvex0a4y5Us5+EGqfYf2Nue7JSOfLMHO3xgLo0KFDuvLKK5Wdna3169erWrVqfpf1NQOrRo0aOnr0qGJiYiSF/r/a73lhrmVmYNW/Z1i+NS3bGvx/6XF3prs3Lng7rdyuoP5LT+7cr7o0/31v+S/B/5ced+7XXha6xxMze6gpv5qWbVPQZlf4Os7yq2nFL9aZgXVVk4K308od1pmBdXVC/vveV1utMwOrR9OCj6eV26Vgj7numq66NCfs71ywcoc1xlxJuqZpweeInPf2bK2+cg/UOcLXcZY795zPNNaYgXXVpQWfy/0eZ0E4R1yTkP/4dHY/CP4MLPcxJvk/zr7eaZ0ZWD0uy/9zhPd3BwXsePIVv6pJwZ8j3N8drDADK/d3B1/H2Yrt1hhzJUPXNiv4857nOLPADKzcx5mvz7Art1tjzJVy9oOL5XN5Wlqa4uLilJqa6unlFEVQZmClpqaqV69eOnHihNasWZNv80qSIiMjFRkZmSdut9tlt3uX4H7TzuXesIWNn/u65xM3DMNn3F+Ohs42lbyWl7z2aU/cT+uxqPFz1+m+pNFfTUaYr3iYZPioqajxMN/bw1+8MNvDazWG75p8x4u/ptzp+tv3fL2/OQ8UPl5cNRV0PC3blucR3zn6PdUUJW74iedMn+7R9Jyon9xD+RxBTcVTk2EoKMeTv3h+NflYPGjnCLu94O3knuRb1HN5SdTkflv9jrklPD4VpSbDKPh4yp1SsMZcd03npnpu7p7J3kEecyXJvenzO0f4Os6CdY7wdZzlzt1rPwjg8ZQ7R3cSuTd7kY+zIJ0j8hufzk0zmOcIX8Ouv3NEII8nf3H3Me/v80LRzofBG3PP5pvrdYL8ubxQx5kFxtyCcizycRaAms7dXc89R7jTCvaYK3nvB6H+udxf/oUV8AZWRkaG+vXrp6SkJK1YsUKXXnppwU8CAAAAAADA31ZAG1hOp1NDhgzRunXr9Nlnn+mKK64I5OoBAAAAAAAQggLawLrvvvu0aNEi9evXT8eOHdN7773n9fjQoUMDmQ4AAAAAAABCQEAbWJs3b5YkLV68WIsXL87zOA0sAAAAAAAAnCugDazVq1cHcnUAAAAAAAC4CPj63RUAAAAAAADAMmhgAQAAAAAAwNJoYAEAAAAAAMDSAnoPLADAxWfZtmBncFaPpsHOAAAAAEBJYAYWAAAAAAAALI0ZWAD+FpglBAAAAAChixlYAAAAAAAAsDRmYAGABTFjDAAAAADOYgYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACwt4A2szMxMPfjgg6pWrZqio6PVvn17LV++PNBpAAAAAAAAIEQEvIE1cuRIPffcc7r55pv1wgsvyGazqXfv3vruu+8CnQoAAAAAAABCgD2QK9u4caM++OADPfPMM/rXv/4lSRo+fLiaNm2qBx54QN9//30g0wEAAAAAAEAICOgMrIULF8pms2ns2LGeWFRUlMaMGaN169Zp3759gUwHAAAAAAAAISCgDazExEQ1bNhQMTExXvF27dpJkjZv3hzIdAAAAAAAABACAnoJ4cGDB1W1atU8cXcsOTnZ5/MyMzOVmZnp+Xtqaqok6dixY3I4HJKksLAwhYWFyeVyyeVyeZZ1x51Op0zTLDBus9lkGIbndXPHJcnpdBYqbrfbZZqmV9wwDNlstjw5GoahkxnpMiXJyPUiZs5f/cZzx84zrnNfW2ffX381nUrLHTdkhNlkmi7JdBUcN8JkGGH+4y5nrsTyi+dsp2PHCt5Op9Jyls+p2bsmIyynJu94ydV07Fj++97pU4ZMl3dN/nIv6ZrS0go+nk6l+a/VnaNhBKamY8f+ivo5zk6dLN5970JqOnas4HPEqbTAH0/+ajp2LP/znns/CPTx5Cvu3g/yO5efOqmAH0/+akpLy398OpUWnOPJV/zYsbznAr/HWQCPJ381HT/uf8zN2Q+Cczz5qik1teDPETnHWXDHXHdNuY8zKW/up05aY8yVpBMnCv685xnL/qrVV+6BOkf4Os5y557zmSb4Y66Usx/4G3Pdufs9zoJwjkhNzf9z+dn9ILhjrkyn5xiT/B9np08Ff8x1S03N//uT93cHBex48hU/frzg74Tu7w7BHHNzH2f5fc89fcoaY65kKC3N/5ib5zgL4pjrjuc+znx9Lj+VZo0xV8rZD0q6H5Hfubw4eyxpaTk7Qe7HiyKgDaz09HRFRkbmiUdFRXke92X69OmaPHlynnidOnWKN0HkeGhcsDMAAAAAAAAXoZMnTyo2NrbIzwtoAys6OtprJpVbRkaG53FfJkyYoHvvvdfzd5fLpWPHjikuLk6Gce60or+ntLQ01ahRQ/v27ctziaYVhVK+oZSrFFr5hlKuUmjlG0q5SqGVbyjlKoVWvqGUqxRa+YZSrlJo5RtKuUqhlW8o5SqFVr6hlKsUWvmGUq5SaOUbSrlKoZdvIJimqZMnT6patWrn9fyANrCqVq2qAwcO5IkfPHhQkvwWERkZmWfmVrly5Yo9v4tBTExMSB0coZRvKOUqhVa+oZSrFFr5hlKuUmjlG0q5SqGVbyjlKoVWvqGUqxRa+YZSrlJo5RtKuUqhlW8o5SqFVr6hlKsUWvmGUq5S6OVb0s5n5pVbQG/i3qJFCyUlJXmue3TbsGGD53EAAAAAAAAgt4A2sAYNGiSn06nXX3/dE8vMzNTs2bPVvn171ahRI5DpAAAAAAAAIAQE9BLC9u3ba/DgwZowYYL+/PNP1a9fX2+//bb27NmjN998M5CpXHQiIyM1ceJEnzfJt6JQyjeUcpVCK99QylUKrXxDKVcptPINpVyl0Mo3lHKVQivfUMpVCq18QylXKbTyDaVcpdDKN5RylUIr31DKVQqtfEMpVyn08g0Fhnm+v194njIyMvToo4/qvffe0/Hjx9WsWTM9/vjjuvbaawOZBgAAAAAAAEJEwBtYAAAAAAAAQFEE9B5YAAAAAAAAQFHRwAIAAAAAAICl0cACAAAAAACApdHACnGZmZl68MEHVa1aNUVHR6t9+/Zavnx5sNPy6dSpU5o4caJ69uyp8uXLyzAMzZkzJ9hp+fTDDz/ozjvvVEJCgkqXLq2aNWvqhhtuUFJSUrBT8+mXX37R4MGDVbduXZUqVUoVKlRQ586dtXjx4mCnVihTp06VYRhq2rRpsFPJY/Xq1TIMw+ef9evXBzs9n3766Sf1799f5cuXV6lSpdS0aVO9+OKLwU4rj5EjR/p9bw3D0IEDB4KdopfffvtNN954o+Lj41WqVCk1btxYU6ZM0ZkzZ4Kdmk8//vijevbsqZiYGJUtW1Y9evTQ5s2bg51WkcaCHTt2qGfPnipTpozKly+vYcOG6ciRI5bLdePGjbr99tvVunVrhYeHyzCMgOWYW2HydblcmjNnjvr3768aNWqodOnSatq0qZ544gllZGRYKldJeuONN9SlSxdVrlxZkZGRqlOnjkaNGqU9e/YELNei5Jtbdna2Lr30UhmGoWeffTYwiarwufo7Bzdu3DhguRYlXyln/33llVfUokULRUdHKy4uTt27d9eWLVsslWt+Y9s111wTkFyLkq8kzZ8/X5dffrnKlSunuLg4denSRV988YUlc33ppZfUpEkTRUZGqnr16rr33nt1+vTpgOValO8</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,94 +108,36 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -424,194 +425,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>metric</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>critical</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>forecast</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>forecast_time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>forecast_value</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>forecast_lower</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>forecast_upper</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>total_tbs</t>
-        </is>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>45639.5</v>
-      </c>
-      <c r="E2" t="n">
-        <v>23</v>
-      </c>
-      <c r="F2" t="n">
-        <v>38.64986855885751</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>45639.5</v>
-      </c>
-      <c r="H2" t="n">
-        <v>22.62707112525826</v>
-      </c>
-      <c r="I2" t="n">
-        <v>7.137494636139678</v>
-      </c>
-      <c r="J2" t="n">
-        <v>38.64986855885751</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACWB0lEQVR4nOzdeXxU9fX/8fedmWyQzYREtqDsq4CyFVwAUUBErCyCFgVKf+5b1WpdWkUrqLhV/WrdvuCCXwXUKnVhEyxVEGMji0CxsgiELYRMEsg2M/f3R5xJJplJJiSZucHX8/Hoo+bMnXvPmXs/994cPnNjmKZpCgAAAAAAALAoW6QTAAAAAAAAAGpCAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwCAMDIMo87/GzZsWKTT9jn99NNlGIZ27doV6VTqxfvZonHt2rVLhmHo9NNPj3QqAACgiXNEOgEAAH5Jpk2bVi124MABLV26NOjr3bp1q9M2Vq9ereHDh2vo0KFavXr1CeXZlA0bNkxffPGFVq1aZanmXyDeJpppmo2+rQcffFCzZs3SAw88oAcffLDRtwcAANCQaGABABBG8+fPrxZbvXq1r4EV6HU0vK1bt0Y6BQAAANQBDSwAAPCLU9dZbQAAAIgsnoEFAIDF7d27VzfffLM6d+6s2NhYJSUl6eyzz9ZLL70kt9vtt+ywYcM0fPhwSdIXX3zh9yytys8hOnz4sJ599lmNGTNG7du3V1xcnBITE9W/f3899thjKi4ubrD8p0+fLsMwNH/+fG3YsEHjx49XWlqa4uLi1Lt3b/31r3+tVockFRQU6JVXXtH48ePVuXNnNW/eXM2bN9cZZ5yh++67T3l5eX7Lr169WoZh6IsvvpAkDR8+3K/+yrPbanoGlsvl0quvvqphw4YpJSVFMTExat++va6//nrt2bOn2vLe7Q4bNkxlZWV67LHH1LNnT8XFxSk1NVXjx4+vNuPrwQcf9Nt+1eeeVX7G2KJFi3TBBRcoNTVVUVFRSk1NVY8ePfT//t//08aNG2v7+H3rnzVrliRp1qxZftuaPn2637K5ubm699571bNnTzVr1kwJCQnq16+fHn/8cRUVFYW0vUBcLpcef/xx32fTokULXX755dq2bVvQ9xQVFenJJ5/Ur371KyUnJys2NlZdu3bVXXfdpSNHjtQ5hxUrVuiSSy7RqaeeqqioKJ1yyinq3Lmzpk6dqn/+858B37Ny5UqNHz9erVq1UnR0tNLT03XZZZdp7dq1DZb3/Pnzffvi2LFjuueee9SpUyfFxMSoZcuWmjZtmvbt21fnegEAOJkwAwsAAAv75ptvNHr0aOXm5qpdu3b69a9/LafTqdWrV+urr77SBx98oI8++kjR0dGSpNGjRys2NlZLly7VqaeeqtGjR/vW1aJFC99/L126VLfeeqvatGmjTp066Ve/+pUOHz6sr7/+Wn/84x/14YcfatWqVYqJiWmwWtavX6/rr79eLVu21IgRI3T06FGtXr1at912m/71r39p4cKFfk2dDRs26JprrlFaWpq6du2qfv366ejRo/r22281e/ZsLVy4UOvWrVNqaqok+X7R/+yzz3Tw4EGNGjVKLVu29K2vU6dOteZYUFCgcePGafXq1YqPj1e/fv2UlpamTZs26W9/+5sWLVqk5cuX68wzz6z23rKyMo0ZM0ZfffWVzjvvPHXv3l3r16/XBx98oFWrVikrK8vXROzbt6+mTZum119/XVL1Z5/Fx8dLkh566CE98MADcjgcGjJkiNq0aSOn06mffvpJr732mnr27KnevXvXWte0adP03XffacOGDerTp4/69u3re+2cc87x/feOHTt0/vnna/fu3UpLS9OYMWNUVlamVatW6e6779a7776rFStW6JRTTql1m1VNnjxZS5Ys0dChQ9W7d2+tX79eixYt0qeffqply5Zp8ODBfstnZ2dr9OjR2rRpk1JSUjRgwAAlJCTo3//+t+bOnatFixZp9erVOu2000La/uuvv64ZM2ZIkgYOHKjhw4erqKhIe/fu1TvvvKMWLVrovPPO83vPnXfeqSeffFI2m039+/fXueeeq59++kkffvihlixZoldeecW3zobI2+l0asiQIfrpp5907rnnqlevXlq7dq3eeOMNffHFF9qwYYOSkpLq8rEDAHDyMAEAQEStWrXKlGRWvSwXFxebp512minJvO6668zS0lLfaz/++KN5+umnm5LMe++9N+D6hg4dGnSbW7ZsMdeuXVstnpuba44cOdKUZD7++OPVXvfms3PnzpDrmzZtmq++G264wSwrK/O9tnnzZjMtLc2UZP7tb3/ze9+ePXvMFStWmG632y9+7Ngx8+qrr/atr6qhQ4eaksxVq1YFzSnQ522apnnllVeaksyxY8eaBw8e9Hvt6aefNiWZnTt3Nl0uly9eef+deeaZ5v79+32vFRUVmaNGjTIlmddcc03IeZhm+f6Pi4sz4+PjzW3btlV7fdeuXebWrVuD1ljVAw88YEoyH3jggaDLDBo0yJRkjhs3ziwsLPTFDx06ZJ511lmmJPPKK68MeZs7d+701diiRQtzw4YNvtdcLpd58803m5LM0047zSwuLva95vF4zLPPPtuUZM6cOdPMz8/3vVZWVmbecccdpiRz+PDhIefSvn17U5K5Zs2aaq8dPHjQ/Pe//+0Xe/nll01JZqdOnfzyNk3T/OKLL8yEhAQzOjra3L59e73znjdvnu9zGjVqlOl0On2v5ebmmn379jUlmbNnzw65XgAATjY0sAAAiLBgDaw333zTlGS2bt3a75d7r8WLF5uSzISEBLOoqKja+mpqYNXkP//5jynJHDBgQLXX6tPAatWqlV+eXs8995yvMRSqY8eOmQ6Hw0xLS6v22ok2sLZs2WIahmG2bt3ar/FQ2ZgxY0xJ5pIlS3wx7+dtGIb53XffVXvPunXrTElmhw4dQsrD69ChQ6Yks3fv3kHrqIvaGlhr1qwxJZnNmjUzDxw4UO31zMxMU5Jps9nMPXv2hLTNyg2sZ555ptrrxcXFZps2bUxJ5oIFC3zxTz/91JRk9u3b16/h6eV2u81evXqZksxNmzaFlEuzZs3MpKSkkJZ1u91m69atTUlmZmZmwGUef/xxU5J5xx131DtvbwOrefPmZnZ2drX3vfPOO6Yk8/zzzw8pfwAATkY8AwsAAItavXq1JGnKlCkBv8o3fvx4nXLKKSooKNC3335b5/W73W6tXLlSDz/8sG644QbNmDFD06dP1yOPPCJJ+s9//lOv/Ku6/PLLFRsbWy3u/frcDz/8oOzs7Gqvf/XVV3rsscd04403+nK84YYbFB0drcOHD+vo0aMNkt8nn3wi0zR10UUXKSEhIeAyw4YN8+VUVbt27dSnT59q8e7du0tSnZ9hlJaWptNPP10bN27UHXfcoS1bttTp/XXlPd5Gjx6tU089tdrr/fr1U58+feTxeHzPGauLql+TlKSYmBhNnjzZb/uS9PHHH0uSJkyYIIej+hMvbDab7+t+gfZFIAMHDpTT6dTVV1+tb7/9Vh6PJ+iyWVlZys7OVseOHdWvX7+AywQ6Fuqbd//+/dWqVatq8RM9hgAAOJnwDCwAACzK+8tq+/btA75uGIbat2+vo0eP1vkX2x9++EGXXXaZvv/++6DL5Ofn12mdtQlWR0JCglJTU3XkyBHt3btXrVu3liQdOnRIEyZM0L/+9a8a15ufn39Cz2SqaseOHZKk1157Ta+99lqNyx4+fLharF27dgGXTUxMlCSVlJTUOac33nhDEydO1FNPPaWnnnpKKSkpGjRokC688EJdddVVfs81q6/ajjdJ6tixozZs2FDn4y05OVnJyckBX/Nub+/evb6Yd1/86U9/0p/+9Kca1x1oXwTywgsvaOzYsXrzzTf15ptvKiEhQQMGDND555+vq666ym//ebf/448/Bn3Yf6Dt1zfv2o6hhvzjCgAANDU0sAAA+AWaOHGivv/+e40dO1Z33XWXevToocTEREVFRam0tLRBH95eF6Zp+v77d7/7nf71r39p8ODBmjVrlvr06aNTTjlFUVFRkqTWrVtr//79fu+pD++MnL59+wacSVXZoEGDqsVstoaf2H7uuedq165d+vjjj/XFF1/oq6++0tKlS/Xpp5/qgQce0AcffKARI0Y0+HYjofJ+9O6Lc845Rx07dqzxfT179gxp/d27d9d//vMfLVu2TJ9//rm++uorrVmzRp9//rkeeughvfbaa5o6darf9lu2bKlRo0bVuN7KTcT65t0YxxAAACcLGlgAAFhUmzZtJFXM6ghk586dfsuGYtu2bdq4caPS09P1wQcfVPuq0w8//HAC2dbOm2tVBQUFOnLkiCSpbdu2kqRjx47pk08+kc1m0yeffFJt9s6xY8d04MCBBs0vIyNDknT22Wfr+eefb9B110dcXJwmTpyoiRMnSiqfuXP//ffr5Zdf1m9/+1vt3r27QbYTyvHmfa0ux5sk5eXlKS8vL+AsrF27dkmq2PdSxb649NJLdeedd9ZpWzVxOBwaM2aMxowZI6l89t5TTz2lWbNm6dprr9Vll12m5s2b+7afmpqq+fPnh7z+xsobAABI/DMPAAAW5X3Gzrvvvhvwq0MffPCBjh49qoSEBL/n9ERHR0uSXC5XwPXm5uZKKp/BFOg5PW+99VZ9Uw9o0aJFAb9G9+abb0qSOnXq5GuMOJ1Oud1uJSYmBmx6vPXWW0FnXtVWfzAXXXSRJOmjjz4K21e1vLPJ6pJrWlqaHn/8cUnSTz/9FPIzwGr7XLzH22effaaDBw9Wez0rK0vfffed33Oc6sK7nysrLS3Vu+++67d9qWJfLFq0qMFm2AWSmJioBx98UMnJyTp+/Li2b98uSRowYIBatGihLVu21Pg126rClTcAAL9ENLAAALCoSZMmqV27dsrOztbtt9/u13jYuXOn7rjjDknSzTff7PdwdO9Mlh9++EFlZWXV1tulSxfZ7XZt2rTJ78HZkrRkyRI9/fTTjVCNlJ2drTvvvFNut9sX27p1qx566CFJ0u9//3tf/NRTT9Upp5yivLy8ao2PdevW6Z577gm6HW/9dWk8SNKZZ56pCRMmaM+ePRo/frxvZlBlx44d04IFCwI2eE5ETbnu3r1br776asBnkS1ZskSSdMopp/iej1SfbUnlX3sbNGiQioqKdO211+r48eO+13JycnTttddKKv+jAt6ZRnXx8MMPa/Pmzb6fPR6P7r77bu3du1cZGRmaMGGC77VLL71UAwYM0Pr16zVjxoyAz4s6evSo/va3v4XU/Dt+/LieeuqpgOtZs2aN8vLyZLfbfZ9RVFSUHnjgAZmmqcsuuyzgc9jcbrc+//xzrVu3rtHyBgAAlUTuDyACAADTNM1Vq1aZksxAl+X169ebKSkppiTztNNOMydPnmyOGTPGjI2NNSWZo0aNMktKSqq9r3///qYks2vXruZvfvMbc+bMmebdd9/te/3WW281JZk2m80cOnSoecUVV5hnnXWWKcm8//77g+Zz2mmnmZLMnTt3hlzftGnTTEnmddddZ8bGxprt27c3p0yZYo4aNcqMjo42JZmXXXaZ6fF4/N739NNP+/IYNGiQecUVV5hnn322aRiGedVVVwXN5R//+IcpyYyOjjbHjh1r/va3vzVnzpxpfvnll75lgtWXn59vjhgxwvf+AQMGmJdffrk5adIkc8CAAb58t27d6nuPd/8NHTo06GcQbHt33nmnKcls0aKFefnll5szZ840Z86caebk5JhZWVmmJDMqKsqXx+WXX26eeeaZpiTTMAzz1VdfDXEvmOaBAwfM5s2bm5LMs88+25w+fbo5c+ZM83//9399y/z444++zzU9Pd2cOHGieemll5qJiYmmJPOss84yc3NzQ97mzp07TUlmu3btzMsuu8yMiooyL7zwQnPKlClmx44dTUlm8+bNzTVr1lR77759+8y+ffv6lhkyZIg5ZcoUc/z48Wbfvn1Nu91uSjKLiopqzePo0aO+471Pnz7mxIkTzSuuuMIcPHiwaRiGKcn885//XO19f/jDH3z7rmfPnuall15qTpkyxRw2bJiZnJxsSjJffPHFeuc9b948U5I5bdq0Gj/H0047rdZaAQA4WdHAAgAgwmpqYJmmaf7000/mjTfeaHbo0MGMjo42ExISzMGDB5svvviiWVZWFvA9u3fvNq+88kqzVatWpsPhqPbLr8fjMV977TWzX79+Znx8vJmUlGSec8455jvvvGOaZvCGS30aWPPmzTP//e9/m5dccomZmppqxsTEmD179jSfeuqpoHX8/e9/N4cMGWImJyeb8fHxZv/+/c0XXnjB9Hg8NebyyiuvmGeddZbZrFkzXy3z5s3zvV7T5+12u823337bHDNmjHnqqaeaUVFRZmpqqtmrVy9zxowZ5gcffGCWlpb6lq9PA6uoqMi86667zE6dOvmaY96a8vPzzWeeeca87LLLzM6dO5vx8fFm8+bNzS5duphXX321mZmZGXR7wfzzn/80L7jgAvOUU04xbTZbwKbJkSNHzHvuucfs3r27GRsbazZr1sw888wzzUcffdQ8fvx4nbZXufFSVlZmPvLII2a3bt3MmJgYMyUlxZwwYYL5/fffB31/cXGx+be//c0cPny4mZqaajocDjM9Pd3s27eveeONN5pLly4NKY+ysjLzb3/7m3nFFVeY3bp1M5OSksy4uDizY8eO5oQJE8yVK1cGfe+XX35p/uY3vzFPO+00MyYmxkxISDC7dOli/vrXvzZfffXVgA29uuZNAwsAgNoZpskX9AEAQOOZPn26Xn/9dc2bN0/Tp0+PdDoAAABogngGFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI1nYAEAAAAAAMDSmIEFAAAAAAAAS6OBBQAAAAAAAEtz1HcF33//vR588EF9++23OnDggJo1a6YePXroD3/4gy655BLfct4/oV1V165dtW3btjpt0+PxKDs7WwkJCTIMo74lAAAAAAAAoBGZpqmCggK1bt1aNlvd51PVu4G1e/duFRQUaNq0aWrdurWOHz+u9957T+PGjdNLL72ka665xrdsTEyMXn31Vb/3JyUl1Xmb2dnZysjIqG/qAAAAAAAACKM9e/aobdu2dX5fozzE3e12q1+/fiouLvbNrpo+fboWL16swsLCeq/f6XQqOTlZe/bsUWJiYr3XBwAAAAAAgMaTn5+vjIwM5eXlndBkpnrPwArEbrcrIyND33zzTbXX3G63jh07Vq/Gk/drg4mJiTSwAAAAAAAAmogTfRRUgz3E/dixY8rJydGPP/6op59+Wp9++qlGjBjht8zx48eVmJiopKQkpaSk6MYbb2yQGVkAAAAAAAA4eTXYDKw77rhDL730kiTJZrNp/Pjxev75532vt2rVSnfddZfOOusseTweffbZZ3rhhRe0YcMGrV69Wg5H8FRKSkpUUlLi+zk/P1+S5HK55HK5fNu02WzyeDzyeDy+Zb1xt9utyt+WDBa32+0yDMO33spxqXwGWShxh8Mh0zT94oZhyG63V8sxWJyaqImaqImaqImaqImaqImaqImaqImaqOlkqKlqXXXVYA2s2267TRMnTlR2drYWLlwot9ut0tJS3+tz5szxW37KlCnq0qWL7rvvPi1evFhTpkwJuu45c+Zo1qxZ1eJZWVlq3ry5JCktLU0dO3bUzp07dfjwYd8ybdu2Vdu2bbV9+3Y5nU5fvEOHDkpPT9fmzZtVVFTki3fr1k3JycnKysry29m9e/dWdHS0MjMz/XLo37+/SktLtXHjRl/MbrdrwIABcjqdfn9hMS4uTn369FFOTo527NjhiyclJal79+7Kzs7W3r17fXFqoiZqoiZqoiZqoiZqoiZqoiZqoiZqoqaToSbvZKQT1SgPcZekkSNHKi8vT19//XXQ7zcWFRUpPj5eM2bMqPbXCSsLNAMrIyNDR44c8T0Di44nNVETNVETNVETNVETNVETNVETNVETNVGTNWvKz89XamqqnE7nCT3PvNEaWC+//LKuvfZabdu2TV27dg26XHp6us455xy9//77Ia87Pz9fSUlJJ1w0AAAAAAAAwqe+vZxG+SuEknxTxipPKauqoKBAOTk5SktLa6w0AAAAAABAA/HO7Knv84xw8nA4HL6ZVo26nfqu4NChQ0pPT/eLlZWV6Y033lBcXJx69Oih4uJilZWVKSEhwW+5hx9+WKZpavTo0fVNAwAAAAAANBLTNJWXl6fDhw9X+8oaYLfblZ6erqSkpEZrZNW7gXXttdcqPz9f5513ntq0aaMDBw5owYIF2rZtm5588knFx8dr165dOvPMM3XFFVeoW7dukqSlS5fqk08+0ejRo3XppZfWuxAAAAAAANA4Dhw4oLy8PCUmJioxMVEOh6PRZ9zA+kzT9D3fav/+/SoqKlKrVq0aZVv1bmBNnjxZr732ml588UUdOXJECQkJ6tevnx577DGNGzdOkpScnKyxY8dq+fLlev311+V2u9WpUyfNnj1bd955p2w2W70LAQAAAAAADc/tdsvpdCotLU0tWrSIdDqwoISEBMXExCgnJ0fp6em+B8w3pEZ7iHtj4iHuAAAAAACER3FxsXbu3KnTTz9dcXFxkU4HFlVUVKRdu3apffv2io2NrfZ6fXs5TH0CAAAAAAC14iuDqEljHx80sAAAAAAAAGBpNLAAAAAAAAAQ0PTp03X66adHOg0aWAAAAAAA4Jdr/vz5Mgwj6P/WrVsX6RRrtWXLFj344IPatWtXpFNpNPX+K4QAAAAAAABN3UMPPaT27dtXi3fq1CkC2dTNli1bNGvWLA0bNswSs6UaAw0sAAAAAABwwpZtjnQG0she9V/HRRddpP79+9d/RWgUfIUQAAAAAACgBg888IBsNptWrlzpF7/mmmsUHR2tDRs2SJJWr14twzD07rvv6t5771XLli3VvHlzjRs3Tnv27Km23q+//lqjR49WUlKSmjVrpqFDh+rLL7+stty+ffs0c+ZMtW7dWjExMWrfvr2uv/56lZaWav78+Zo0aZIkafjw4b6vPq5evdr3/k8//VTnnnuumjdvroSEBF188cX6/vvvq23n73//u3r16qXY2Fj16tVLH3zwQX0+tgbFDCwAAAAAAPCL53Q6lZOT4xczDEOpqam6//77tWTJEs2cOVObNm1SQkKCli5dqldeeUUPP/yw+vTp4/e+Rx55RIZh6O6779ahQ4f0zDPP6IILLtB3332nuLg4SdLnn3+uiy66SP369fM1yObNm6fzzz9fa9as0cCBAyVJ2dnZGjhwoPLy8nTNNdeoW7du2rdvnxYvXqzjx4/rvPPO0y233KJnn31W9957r7p37y5Jvv9/8803NW3aNI0aNUqPPfaYjh8/rhdffFHnnHOOsrKyfF85XLZsmSZMmKAePXpozpw5OnLkiGbMmKG2bds25sceMsM0TTPSSdRVfn6+kpKS5HQ6lZiYGOl0AAAAAAA4aRUXF2vnzp1q3769YmNjq73e1L9COH/+fM2YMSPgazExMSouLpYkbd68Wf369dPVV1+tuXPnqlevXmrVqpXWrl0rh6N8ftDq1as1fPhwtWnTRlu3blVCQoIkadGiRbr88sv117/+VbfccotM01TXrl3VoUMHffrppzIMQ5JUVFSknj17qlOnTlq2bJkkadq0aXrrrbf09ddfV/uKo2maMgxDixcv1qRJk7Rq1SoNGzbM93phYaEyMjI0adIkvfzyy774wYMH1bVrV11++eW++JlnnqmDBw9q69atSkpKkiQtX75cI0eO1GmnnVbrA+JrO07q28thBhYAAAAAAPjF+5//+R916dLFL2a3233/3atXL82aNUv33HOPNm7cqJycHC1btszXvKrs6quv9jWvJGnixIlq1aqVPvnkE91yyy367rvv9MMPP+j+++/XkSNH/N47YsQIvfnmm/J4PJLKv9Z3ySWXBHw+l7fxFczy5cuVl5enK664wm92md1u16BBg7Rq1SpJ0v79+/Xdd9/pj3/8o695JUkXXnihevTooWPHjtW4nXCggQUAAAAAAH7xBg4cWOtD3P/whz/onXfe0fr16zV79mz16NEj4HKdO3f2+9kwDHXq1Mk3i+mHH36QVD67Khin06nS0lLl5+erV68Tm2Lm3c75558f8HXvTKjdu3cHzFuSunbtqn//+98ntP2GRAMLAAAAQIOzwleKvBrir5MBgCTt2LHD1xTatGnTCa/HO7tq7ty56tu3b8Bl4uPjlZube8LbqLydN998Uy1btqz2eqDZY1bVdDIFAAAAfsFoCAFAZHk8Hk2fPl2JiYm67bbbNHv2bE2cOFHjx4+vtqy3yeVlmqb++9//qnfv3pKkjh07SiqfAXXBBRcE3WZaWpoSExO1eXPNF4FgXyX0bic9Pb3G7Zx22mkB85ak//znPzVuO1xskU4AAAAAAADA6p566il99dVXevnll/Xwww9ryJAhuv7666v95UJJeuONN1RQUOD7efHixdq/f78uuugiSVK/fv3UsWNHPfHEEyosLKz2/sOHD0uSbDabfv3rX2vJkiXKzMystpz37/I1b95ckpSXl+f3+qhRo5SYmKjZs2errKws6HZatWqlvn376vXXX5fT6fS9vnz5cm3ZsqXGzyVcmIEFAAAAAAB+8T799FNt27atWnzIkCEqKSnRn/70J02fPl2XXHKJpPK/Xti3b1/dcMMNWrhwod97UlJSdM4552jGjBk6ePCgnnnmGXXq1En/7//9P0nljalXX31VF110kXr27KkZM2aoTZs22rdvn1atWqXExEQtWbJEkjR79mwtW7ZMQ4cO1TXXXKPu3btr//79WrRokf71r38pOTlZffv2ld1u12OPPSan06mYmBidf/75Sk9P14svvqirrrpKZ511lqZMmaK0tDT99NNP+vjjj3X22Wfr+eeflyTNmTNHF198sc455xz99re/VW5urp577jn17NkzYJMt3GhgAQAAAACAX7w///nPAeOvvvqqXnrpJbVo0ULPPPOML965c2fNmTNHt956qxYuXKjLL7/c99q9996rjRs3as6cOSooKNCIESP0wgsvqFmzZr5lhg0bprVr1+rhhx/W888/r8LCQrVs2VKDBg3Stdde61uuTZs2+vrrr/WnP/1JCxYsUH5+vtq0aaOLLrrIt76WLVvqb3/7m+bMmaOZM2fK7XZr1apVSk9P15VXXqnWrVvr0Ucf1dy5c1VSUqI2bdro3HPP1YwZM3zbGT16tBYtWqT7779f99xzjzp27Kh58+bpww8/1OrVqxvoUz5xhumdb9aE5OfnKykpSU6n0/fEfAAAAOBk1tSegdXU8gUQXHFxsXbu3Kn27dsrNjY20ulY2urVqzV8+HAtWrRIEydOjHQ6YVXbcVLfXg7PwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXxEHcAAAAAAIAGMGzYMDXBR403CczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAv1jz58+XYRiKjY3Vvn37qr0+bNgw9erVKwKZoTJHpBMAAAAAAABN2GefRToDafToeq+ipKREjz76qJ577rkGSAgNjRlYAAAAAADgF69v37565ZVXlJ2dHelUEAANLAAAAAAA8It37733yu1269FHH61xOZfLpYcfflgdO3ZUTEyMTj/9dN17770qKSnxLXP77bcrNTVVpmn6YjfffLMMw9Czzz7rix08eFCGYejFF19s+IJOMnyFEAAAAMAv2rLNkc6gwkgeswNETPv27XX11VfrlVde0R//+Ee1bt064HK/+93v9Prrr2vixIm644479PXXX2vOnDnaunWrPvjgA0nSueeeq6efflrff/+97/lZa9askc1m05o1a3TLLbf4YpJ03nnnhaHCpo0ZWAAAAAAAAJLuu+8+uVwuPfbYYwFf37Bhg15//XX97ne/06JFi3TDDTfo9ddf15133qm///3vWrVqlSTpnHPOkVTRoHI6ndq0aZMmTJjgi3lfT0lJUY8ePRq5sqaPBhYAAAAAAICkDh066KqrrtLLL7+s/fv3V3v9k08+kVT+FcHK7rjjDknSxx9/LElKS0tTt27d9M9//lOS9OWXX8put+sPf/iDDh48qB9++EFSeQPrnHPOkWEYjVbTyYIGFgAAAAAAwM/uv/9+uVyugM/C2r17t2w2mzp16uQXb9mypZKTk7V7925f7Nxzz/XNtlqzZo369++v/v37KyUlRWvWrFF+fr42bNigc889t3ELOknQwAIAAAAAAPhZhw4dNHXq1KCzsCSFNGPqnHPO0b59+7Rjxw6tWbNG5557rgzD0DnnnKM1a9boq6++ksfjoYEVIhpYAAAAAAAAlXhnYVV9FtZpp50mj8fj+wqg18GDB5WXl6fTTjvNF/M2ppYvX65vvvnG9/N5552nNWvWaM2aNWrevLn69evXyNWcHGhgAQAAAAAAVNKxY0dNnTpVL730kg4cOOCLjxkzRpL0zDPP+C3/1FNPSZIuvvhiX6x9+/Zq06aNnn76aZWVlenss8+WVN7Y+vHHH7V48WL96le/ksPhaORqTg40sAAAAAAAAKq47777VFZWpv/85z++WJ8+fTRt2jS9/PLLmjx5sl544QVNnz5djz/+uH79619r+PDhfus499xz9Z///Ee9evXSKaecIkk666yz1Lx5c23fvp2vD9YBDSwAAAAAAIAqOnXqpKlTp1aLv/rqq5o1a5a++eYb3Xbbbfr88891zz336J133qm2rLdBdc455/hiDodDgwcP9nsdtTNM0zQjnURd5efnKykpSU6nU4mJiZFOBwAAAGh0yzZHOoMKI3vVvkxTyrcp5QpEQnFxsXbu3Kn27dsrNjY20unAomo7Turby2EGFgAAAAAAACyNBhYAAAAAAAAsjUfdAwAA4BeLr44BANA0MAMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAKCRGIahBx98MNJpNHn1bmB9//33mjRpkjp06KBmzZqpRYsWOu+887RkyZJqy27dulWjR49WfHy8UlJSdNVVV+nw4cP1TQEAAAAAAKDODMMI6X+rV6+OdKq/eI76rmD37t0qKCjQtGnT1Lp1ax0/flzvvfeexo0bp5deeknXXHONJGnv3r0677zzlJSUpNmzZ6uwsFBPPPGENm3apPXr1ys6OrrexQAAAAAAgDD7738jnYHUqdMJve3NN9/0+/mNN97Q8uXLq8W7d+9+wqmhYdS7gTVmzBiNGTPGL3bTTTepX79+euqpp3wNrNmzZ+vYsWP69ttv1a5dO0nSwIEDdeGFF2r+/Pm+5QAAAAAAAMJh6tSpfj+vW7dOy5cvrxZH5DXKM7DsdrsyMjKUl5fni7333nsaO3asr3klSRdccIG6dOmihQsXNkYaAAAAAAAA9XLs2DHdcccdysjIUExMjLp27aonnnhCpmn6LVdSUqLf//73SktLU0JCgsaNG6e9e/dWW9/u3bt1ww03qGvXroqLi1NqaqomTZqkXbt2+ZbZsWOHDMPQ008/Xe39X331lQzD0P/93/81eK1WVu8ZWF7Hjh1TUVGRnE6nPvroI3366aeaPHmyJGnfvn06dOiQ+vfvX+19AwcO1CeffNJQaQAAAAAAADQI0zQ1btw4rVq1SjNnzlTfvn21dOlS/eEPf9C+ffv8Gky/+93v9NZbb+nKK6/UkCFD9Pnnn+viiy+uts5vvvlGX331laZMmaK2bdtq165devHFFzVs2DBt2bJFzZo1U4cOHXT22WdrwYIF+v3vf+/3/gULFighIUGXXnppo9dvJQ3WwLrjjjv00ksvSZJsNpvGjx+v559/XpK0f/9+SVKrVq2qva9Vq1bKzc1VSUmJYmJiAq67pKREJSUlvp/z8/MlSS6XSy6Xy7dNm80mj8cjj8fjW9Ybd7vdft3RYHG73S7DMHzrrRyXJLfbHVLc4XDINE2/uGEYstvt1XIMFqcmaqImaqImaqImaqKmxq3JrFiNZJTnLtM/92Bxw1Zek3/ckGGzyzQ9qrLywHHDJsOwyTQ9crlqrsn0VFre45ZU6V/+jfKaTI//fmqsmlyu2vdT0Fqr5R6emmo69irSrH0/NXZNlYdaUxtPlZ0s5whqKo+7XK6Kc1GVWUeSZASLG0b44gFeD0XVdVf97w8//FCff/65Hn74Yd13330yDEM33HCDLr/8cv31r3/VjTfeqI4dO2rjxo166623dP311+t//ud/JEk33HCDpk6dqo0bN8o0Td+6x4wZo4kTJ/pta+zYsRoyZIjee+8939cXr7rqKl133XXaunWrunXrJkkqKyvTwoULNX78eMXFxUX+c6/CNE2/Xk3lY6/q8VdXDdbAuu222zRx4kRlZ2dr4cKFcrvdKi0tlSQVFRVJUsAGVWxsrG+ZYA2sOXPmaNasWdXiWVlZat68uSQpLS1NHTt21M6dO/3+smHbtm3Vtm1bbd++XU6n0xfv0KGD0tPTtXnzZl9+ktStWzclJycrKyvLbxD37t1b0dHRyszM9Muhf//+Ki0t1caNG30xu92uAQMGyOl0atu2bb54XFyc+vTpo5ycHO3YscMXT0pKUvfu3ZWdne03vZCaqImaqImaqImaqImaGrem0ryKmqJa9JZhj1bpQf+aok/tL9NdqrKcipoMw67olgNkljpVlltRk+GIU3RaH3mKcuRyVtRki0lSVEp3uQuz5S6sqMkelyZHcke5nTuVmVlzTaUFkiOpg+zN0lV2ZLNMV0VNUSndZMQkq+xQlkyz8WvKPF77fnI7d8pdVFGTPb6tHAlt5crbLk9JxX4KR021HXulBaHvp8auKfN4RU1NbTydjOcIaqqoyfu7u9vtVnFxsS9us9nUTJLL7VbZzz0ASbLZ7YqNiZHL5VJZWVnFZ+NwKCY6WqVlZXJXamhERUUpKipKJaWl8lTKMSo6WlEOh4pLSmRWauJFx8TIYberuLhYpmnKc+yY7zO22Ww69vPPXs2bN5fH4/H7XAzDUPPmzf1qqtxkcblc+uijj2S32zVz5kwVFxcrLi5OZWVluv7667V48WJ9+OGHuvHGG33fLPvd737n23Z0dLRuu+02vf322yorK/PFvb2PoqIilZSUKD8/X61atVJycrL+/e9/a/z48TJNUxdffLFiY2P11ltv6S9/+YuOHTumTz/9VDk5OZowYYIkhVSTbz81ayaXy+U3Qchut/tqKq20/xwOh2JjY1VSUuL3mURHRys6OlrFxcV+x5K3prKyMm3evNkXr3zseScjnSjDDNY2q6eRI0cqLy9PX3/9tb799lsNGDBAb7zxhq666iq/5e666y7NnTtXxcXFdZqBlZGRoSNHjigxMVGSdTrTXidTt52aqImaqImaqImaqOlkrWnllkpJRngG1ojuNde0ckul5SM8A2tEj9r309JN1pmBdWHPmo+9iuMg8jOwRvSoCDe18VTZyXKOoKbyeHFxsX766Sd16NAh4O/txo8/Rn4m0An+FcKq677pppv0wgsv+GZMXXTRRdqyZYt2797tt7zT6dQpp5yiO+64Q3PnztX111+vV155RcXFxXI4KuYKFRQUKCkpSX/+85/14IMPSipvXD366KOaN2+e9u3b57f9GTNm6LXXXvP9PHnyZH377bf6789/6fHKK6/UmjVrtHv3btlsgR9rHqkZWCUlJdqxY4fatWvna3hWPvby8/OVmpoqp9Pp6+XURYPNwKpq4sSJuvbaa7V9+3bfVwe9XyWsbP/+/UpJSQnavJLKO3mBXnc4HH4HhlQxYKvyDsBQ41XXeyJxwzACxoPlWNc4NVFTsDg1UZNETcFyrGucmqhJoqZgOdY1bsWajED3/kaQW+QAccMwgsRtCrTymuIOR801VX6bYQtck2ELPfdg8VBqqrwbg+2PoLUGzb1xa6rp2KuaZp33XwPWFGhINZXxVN84NVm3JofDUX5ukHz/X1XE40FeD0XldYf635U/j2CvVd2GN37LLbdo3rx5uu222zR48GAlJSXJMAxNmTJFHo/H7/1XX321Fi1apLVr1+qMM87QRx99pBtuuCHoPg6Ub7jjgXo1gWJ11WgNLO8UNqfTqa5duyotLa3atERJWr9+vfr27dtYaQAAAAAAAJyQ0047TStWrFBBQYESEhJ8ce9XQ0877TTf/3s8Hv3444/q2rWrb7n//Oc/1da5ePFiTZs2TU8++aQvVlxcrLy8vGrLjh49WmlpaVqwYIEGDRqk48ePV/tm2y9F4PlmdXDo0KFqsbKyMr3xxhuKi4tTjx7lc2AnTJigf/zjH9qzZ49vuZUrV2r79u2aNGlSfdMAAAAAAABoUGPGjJHb7fb9kTqvp59+WoZh6KKLLpIk3/8/++yzfss988wz1dZpt9urfQXvueeeq/ZVTql85tIVV1yhhQsXav78+TrjjDPUu3fv+pTUZNV7Bta1116r/Px8nXfeeWrTpo0OHDigBQsWaNu2bXryyScVHx8vSbr33nu1aNEiDR8+XLfeeqsKCws1d+5cnXHGGZoxY0a9CwEAAACAX4Jlm2tfJlxG9op0BkDjuuSSSzR8+HDdd9992rVrl/r06aNly5bpww8/1G233aaOHTtKkvr27asrrrhCL7zwgpxOp4YMGaKVK1f6nl1V2dixY/Xmm28qKSlJPXr00Nq1a7VixQqlpqYGzOHqq6/Ws88+q1WrVumxxx5r1HqtrN4NrMmTJ+u1117Tiy++qCNHjighIUH9+vXTY489pnHjxvmWy8jI0BdffKHbb79df/zjHxUdHa2LL75YTz75ZI3PvwIAAAAAAIgEm82mjz76SH/+85/17rvvat68eTr99NM1d+5c3XHHHX7L/u///q/v635///vfdf755+vjjz9WRkaG33J//etfZbfbtWDBAhUXF+vss8/WihUrNGrUqIA59OvXTz179tTWrVv1m9/8ptFqtbpG+yuEjSk/P19JSUkn/OR6AAAAQGpaM1maUq5S08q3KeUqNb180fQVFxdr586dat++ve+vyyG8zjzzTKWkpGjlypWRTiWo2o6T+vZy6v0MLAAAAAAAADSOzMxMfffdd7r66qsjnUpENdpfIQQAAAAAAMCJ2bx5s7799ls9+eSTatWqlSZPnhzplCKKGVgAAAAAAAAWs3jxYs2YMUNlZWX6v//7v1/81zdpYAEAAAAAAFjMgw8+KI/Ho61bt2ro0KGRTifiaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAgFqZphnpFGBhjX180MACAAAAAABB2e12SVJZWVmEM4GVeY8P7/HS0GhgAQAAAACAoKKiohQTEyOn08ksLARkmqacTqdiYmIUFRXVKNtwNMpaAQAAAADASaNFixbat2+f9u7dq6SkJEVFRckwjEinhQgzTVNlZWVyOp0qLCxUmzZtGm1bNLAAAAAAAECNEhMTJUk5OTnat29fhLOB1cTExKhNmza+46Qx0MACAAAAAAC1SkxMVGJiosrKyuR2uyOdDizCbrc32tcGK6OBBQAAAAAAQhYVFRWWhgVQGQ9xBwAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKU5Ip0AAAAAAODktGxzpDOoMLJXpDMAUB/MwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKU5Ip0AAAAATh7LNkc6gwoje0U6AwAA0FCYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLc0Q6AQAAAAAArGDZ5khnUGFkr0hnAFgLM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGn1bmB98803uummm9SzZ081b95c7dq10+WXX67t27f7LTd9+nQZhlHtf926datvCgAAAAAAADiJOeq7gscee0xffvmlJk2apN69e+vAgQN6/vnnddZZZ2ndunXq1avib3/GxMTo1Vdf9Xt/UlJSfVMAAAAAAADASazeDazbb79db7/9tqKjo32xyZMn64wzztCjjz6qt956q2JjDoemTp1a300CAAAAAADgF6TeXyEcMmSIX/NKkjp37qyePXtq69at1ZZ3u93Kz8+v72YBAAAAAADwC9EoD3E3TVMHDx5UixYt/OLHjx9XYmKikpKSlJKSohtvvFGFhYWNkQIAAAAAAABOEvX+CmEgCxYs0L59+/TQQw/5Yq1atdJdd92ls846Sx6PR5999pleeOEFbdiwQatXr5bDETyVkpISlZSU+H72zuByuVxyuVySJJvNJpvNJo/HI4/H41vWG3e73TJNs9a43W6XYRi+9VaOS+UzyEKJOxwOmabpFzcMQ3a7vVqOweLURE3URE3URE3URE1NrSbTtP/8H/5xw1Zek3/ckGGzyzQ9kumpPW7YZBi24HGPW1JF7h5P7TX5bzZw7sHiDV2Ty1XzfjI9wWuVUV6T6fHfT41Vk8tV+7EX6n4KV001jaeKNBvm2KtPTZWHWrBxJoV/PAWLm2bN54jy5QPX6hcOwzkilPNe+TgL73gKFne5uD5R08lVU9W66qrBG1jbtm3TjTfeqMGDB2vatGm++Jw5c/yWmzJlirp06aL77rtPixcv1pQpU4Kuc86cOZo1a1a1eFZWlpo3by5JSktLU8eOHbVz504dPnzYt0zbtm3Vtm1bbd++XU6n0xfv0KGD0tPTtXnzZhUVFfni3bp1U3JysrKysvx2du/evRUdHa3MzEy/HPr376/S0lJt3LjRF7Pb7RowYICcTqe2bdvmi8fFxalPnz7KycnRjh07fPGkpCR1795d2dnZ2rt3ry9OTdRETdRETdRETdTU1GpSs/4y3aUqy6moyTDsim45QGapU2W5FTUZjjhFp/WRpyhHLmdFTbaYJEWldJe7MFvuwoqa7HFpciR3lNu5U+6iiprs8W3lSGgrV952eUoqasppWXtNpXkVNUW16C3DHq3Sg/41RZ8anpoyM2veT6UFkiOpg+zN0lV2ZLNMV0VNUSndZMQkq+xQlkyz8WvKPF77sRfqfgpHTbWNp9KC0PdTY9eUebyipmDnCMWFfzwFq8nZruZzRKTGU6CaQjnvlRaEfzwFqynzONcnajq5aqrv46QMs3JrrJ4OHDigs88+W2VlZVq3bp1at25d4/JFRUWKj4/XjBkzqv11wsoCzcDKyMjQkSNHlJiYKImOJzVREzVREzVREzVRkxVqWrnVOjOwLuxVe00rt1TebGRnYI3oXvN+WrkleK3hnjEyokftx97STdaZgXVhz5rHU8VxEPkZWCN6VISDjbPPt1lnBtbIM2o+RyzbZJ0ZWCO6137eKx9n1piBNaIH1ydqOrlqys/PV2pqqpxOp6+XUxcNNgPL6XTqoosuUl5entasWVNr80oq7wCmpqYqNze3xuViYmIUExNTLe5wOKp99dD7oVXl3bGhxoN9pbEuccMwAsaD5VjXODVRU7A4NVGTRE3BcqxrnJqoSaKmYDkGihuG9z8C1xQ4bpOM6jnWOW7zz91bdk01BVhNwByDxRuyJoej5v1U+W1Va62Ih557sHgoNVXe7cGOsVD3U+3xhqmppvFUNc36Hnu1x4PnHmioBTtHhHM8BYt7x3ywc0Rd9l9j1xTKec9/nIVnPAWLhzLOuD5RU7C4FWuq6dFRoWiQBlZxcbEuueQSbd++XStWrFCPHj1qf5OkgoIC5eTkKC0trSHSAAAAAAAAwEmo3g0st9utyZMna+3atfrwww81ePDgassUFxerrKxMCQkJfvGHH35Ypmlq9OjR9U0DAAAAAAAAJ6l6N7DuuOMOffTRR7rkkkuUm5urt956y+/1qVOn6sCBAzrzzDN1xRVXqFu3bpKkpUuX6pNPPtHo0aN16aWX1jcNAAAAAAAAnKTq3cD67rvvJElLlizRkiVLqr0+depUJScna+zYsVq+fLlef/11ud1uderUSbNnz9add94Z8PuUAAAAAAAAgNQADazVq1fXukxycrLefPPN+m4KAAAAAAAAv0AN9lcIAQAAAABAeCzbHOkMKozsFekM8EvAd/cAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGmOSCcAAAAAAABObss2RzqDCiN7RToDnAhmYAEAAAAAAMDSmIEFAAB+ef7730hnUKFTp9qXeeONxs8jVFdfHekMAADALxAzsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpPMQdAADA4n7MiXQGFTpGOgEAAPCLxAwsAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoPcQcAAAAAAPjZss2RzqDCyF6RzsA6mIEFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6t3A+ubb77RTTfdpJ49e6p58+Zq166dLr/8cm3fvr3aslu3btXo0aMVHx+vlJQUXXXVVTp8+HB9UwAAAAAAAMBJzFHfFTz22GP68ssvNWnSJPXu3VsHDhzQ888/r7POOkvr1q1Tr169JEl79+7Veeedp6SkJM2ePVuFhYV64okntGnTJq1fv17R0dH1LgYAAAAAAAAnn3o3sG6//Xa9/fbbfg2oyZMn64wzztCjjz6qt956S5I0e/ZsHTt2TN9++63atWsnSRo4cKAuvPBCzZ8/X9dcc019UwEAAAAAAMBJqN5fIRwyZEi12VOdO3dWz549tXXrVl/svffe09ixY33NK0m64IIL1KVLFy1cuLC+aQAAAAAAAOAk1SgPcTdNUwcPHlSLFi0kSfv27dOhQ4fUv3//assOHDhQWVlZjZEGAAAAAAAATgL1/gphIAsWLNC+ffv00EMPSZL2798vSWrVqlW1ZVu1aqXc3FyVlJQoJiYm4PpKSkpUUlLi+zk/P1+S5HK55HK5JEk2m002m00ej0cej8e3rDfudrtlmmatcbvdLsMwfOutHJckt9sdUtzhcMg0Tb+4YRiy2+3VcgwWpyZqoiZqoiZqoqZGqsk05amc4895ejweeSqt22YYshmG3B6PzBDidsMor8lTeS3lcUlym2b1eJXcA9XkMX7erimZkkzDb/HAcbO8Lo8kVYobZvmPnirrCDXu3V/B9odp2n/+D/+4YSuvyT9uyLDZZZoeyfTUHjdsMgxb8LjHXV74zzye2o89/80Gzj1YvKFrcrlqHk+mJ3itMsprMj3+46mxanK5aj9HhLqfwlVTTeeIijQb5tirT02VT4nBxpkU/vEULG6aNZ/Ly5cPXKtfOAzniFCuT+XjLLzjKVjc5ar5mitFbjxVrUmq/T7CV24Yx1OweOXDNdB9hOmJzHgKVJPLdfLc71U9T9RVgzewtm3bphtvvFGDBw/WtGnTJElFRUWSFLBBFRsb61smWANrzpw5mjVrVrV4VlaWmjdvLklKS0tTx44dtXPnTr+/bNi2bVu1bdtW27dvl9Pp9MU7dOig9PR0bd682ZefJHXr1k3JycnKysry29m9e/dWdHS0MjMz/XLo37+/SktLtXHjRl/MbrdrwIABcjqd2rZtmy8eFxenPn36KCcnRzt27PDFk5KS1L17d2VnZ2vv3r2+ODVREzVREzVREzU1Uk1Op/ZWyjEtPl4dU1O18+hRHS4srKgpKUltk5O1PSdHzkq5d0hNVXp8vDYfOKCisrKKmtLTlRwXp6x9++SudLPXu1UrRTscytyzx7+mjAyVFhXVWtPxU5spyuVR65xiFcY5lJtU8fiG2BK3Tj1aImd8lJzxUb54fJFLqc5SHU2KVmFcxS1fUmGZkgvLdDg5RsUxdl88xVmqhCKXDqTGqsxRMUk/PbdYcaUe7U2Pk2kYOvLzfgm2n9Ssv0x3qcpyKmoyDLuiWw6QWepUWW7FfjIccYpO6yNPUY5czor9ZItJUlRKd7kLs+UurDj27HFpciR3lNu5U+6iimPPHt9WjoS2cuVtl6ekYr/mtKz92CvNqzj2olr0lmGPVulB/5qiTw1PTZmZNY+n0gLJkdRB9mbpKjuyWaaroqaolG4yYpJVdihLptn4NWUer/0cEep+CkdNtZ0jSgtC30+NXVPm8Yqagp33FBf+8RSsJme7ms/lkRpPgWoK5fpUWhD+8RSspszjNV9zpciMp0A1SbXfR3jHWTjHU7CavOMs2H1EWVFkxlOgmjKPnzz3e97JSCfKMM0q/xRYDwcOHNDZZ5+tsrIyrVu3Tq1bt5YkZWZmasCAAXrjjTd01VVX+b3nrrvu0ty5c1VcXFynGVgZGRk6cuSIEhMTJTX9fw1euTWy/9JT2cgzmlYXt7KTpTNNTdRETdRETY1c0w8/WGcGVqdOtda087m3y7drgRlY7W++sjz3IPtj5VbrzMC6sFftx97KLZU3G9kZWCO61zyeVm4JXmu4Z4yM6FH7OWLpJuvMwLqwZ83niIrjIPIzsEb0qAgHG2efb7PODKyRZ9R8Ll+2yTozsEZ0r/36VD7OrDEDa0SPmq+5K7ZYZwbWqN6130f4xpkFZmBVHmeB7iNWbrHODKwRPU6e+738/HylpqbK6XT6ejl10WAzsJxOpy666CLl5eVpzZo1vuaVVPHVQe9XCSvbv3+/UlJSgjavpPKZW4Fedzgccjj8S/B+aFV5d2yo8arrPZG4YRgB48FyNAybZNQhbguce/B4kN1t+Md/vsdukJrqGm8K+4maqClYjnWNUxM1SdQULMe6xutc088NqIDLB9imPcA6aoo7gsUDbFNBcq9ck63yva3Km0rVlg8St0l+98a+eJB/wqwtXjXXqj/7SjQC1xQ4Xsd7oBDvjby7oaZjL8BqAuYYLN6QNTkcNY+nym+r7/1eTfFQaqq82+t8b9tI97A1xWs7R1RNM5L35YFOfcHOEeEcT8HiNf3uUL58ZMZToHgo1yf/cRae8RQsHtI4i9B4ChSv7X4h5HEWhpqqHq5VzxHetMI9niriFblUzrWp3+8Fyz9UDdLAKi4u1iWXXKLt27drxYoV6tGjh9/rbdq0UVpaWvUp5pLWr1+vvn37NkQaAAAAAAAAOAnV+68Qut1uTZ48WWvXrtWiRYs0ePDggMtNmDBB//jHP7Sn0rMfVq5cqe3bt2vSpEn1TQMAAAAAAAAnqXrPwLrjjjv00Ucf6ZJLLlFubq7eeustv9enTp0qSbr33nu1aNEiDR8+XLfeeqsKCws1d+5cnXHGGZoxY0Z90wAAAAAAAMBJqt4NrO+++06StGTJEi1ZsqTa694GVkZGhr744gvdfvvt+uMf/6jo6GhdfPHFevLJJ2t8/hWsZ9nmSGdQYWSvSGcAAAAAAAAaW70bWKtXrw552Z49e2rp0qX13SQAAAAAAAB+Qer9DCwAAAAAAACgMdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdX7Ie4AAABNzdofI51BhcGdIp0BAACA9TEDCwAAAAAAAJbGDCwAANAw/vvfSGdQoRPTmgAAAE4mzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTkinQDQ2JZtjnQGFUb2inQGAAAAAAA0PczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl8VcILSJh338jnUKFXp0inQEAAAAAAIAPM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGmOSCcAAABODmt/jHQGFQZ3inQGAAAAaEjMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTkinQCACss2RzqDCiN7RToDAAAAAADK0cDCSS9h338jnUKFXp0inQEAAAAAAE0OXyEEAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTVIA6uwsFAPPPCARo8erZSUFBmGofnz51dbbvr06TIMo9r/unXr1hBpAAAAAAAA4CTkaIiV5OTk6KGHHlK7du3Up08frV69OuiyMTExevXVV/1iSUlJDZEGAAAAAAAATkIN0sBq1aqV9u/fr5YtWyozM1MDBgwIvkGHQ1OnTm2IzQIAAAAAAOAXoEG+QhgTE6OWLVuGvLzb7VZ+fn5DbBoAAAAAAAAnubA/xP348eNKTExUUlKSUlJSdOONN6qwsDDcaQAAAAAAAKCJaJCvEIaqVatWuuuuu3TWWWfJ4/Hos88+0wsvvKANGzZo9erVcjgCp1NSUqKSkhLfz97ZWy6XSy6XS5Jks9lks9nk8Xjk8Xh8y3rjbrdbpmnWGrfb7TIMw7feynGpfPZYKHGHwyHTNP3ihmHIbrdXy9EwDEn6OQ/Tbz2GYZNpeuSv/OH3DREv579N7+cRrCbTUzluyLDZy9ftt/4gccNWUVOguMftn0/QeOj7qbzuwLWW5xLsc69rvPbP3eVy1XjsSYZMj6vKauw/p+4OKW7YyveTf7zu+0lquuMpULypnyOoiZqaQk2maTbq9aku53K3211jTVa55kpGtf0hVd9Pnp/fbjPL12Aa/msJGDfL/6XSU3nzkgyz/EdPlXWEGvceg8GOMdNs3OtTXe4jPJ7ax5P/ZiNzzfXW5HLVfI4ov6Wp+d4oXPcRLlft54iGut9rqJpqOu9VpBmee9iaaqp8mg82zqTwj6dgcdOs+frk/7uDwjaeAsVDueaWj7PwjqdgcZer5vsIKXLjqWpNUu33Eb5ywziegsUrH66B7o1MT2R/z61ck8tlrfu9+tzDVj1P1FVYG1hz5szx+3nKlCnq0qWL7rvvPi1evFhTpkwJ+r5Zs2ZVi2dlZal58+aSpLS0NHXs2FE7d+7U4cOHfcu0bdtWbdu21fbt2+V0On3xDh06KD09XZs3b1ZRUZEv3q1bNyUnJysrK8tvZ/fu3VvR0dHKzMz0y6F///4qLS3Vxo0bfTG73a4BAwbI6XRq27ZtvnhcXJz69OmjnJwc7dixwxcvf4h9lEo8ThW7K3KMtsWrmSNVRe6jKvVUzFKLtScp1p6sY64cucyK3OPsqYqxx6vQdUBus8wXb+5IV5QRp/yyfTJVceAlRLWSTQ45y/b41eR2d6ixJs/ubyviRpQSolqrxF2oIvcRX9xhxCk+Kl3F7ryANR13HQlYU2HZoYA1FZRlV6/JFqesoqO17idn2TElRWXII5cKyvb74oZsSorOkMss1jHXoWo1lXqOBaypPvspMzO3xmNPSlbZoSyZlU62US16y7BHq/Sg/7EXfWp/me5SleVU7CfDsCu65QCZpU6V5VYce4YjTtFpfeQpypHLWXHs2WKSFJXSXe7CbLkL91Z8BnFpkprueOrevbuys7O1d29FTU39HEFNDVjT3r3K3ON/3uufkaFSl0sb91ecI+w2mwZkZMhZVKRthyrOEXFRUerTurVyCgu140jFOSIpLk7d09OVnZenvZVyTIuPV8fUVO08ckSHK804bpuUpLb9+59U+6nE42jU61NdzuWbNxfVWJNVrrlJURkqKiqqdT8dP7WZolwetc4pVmGcQ7lJ0RU5lrh16tESOeOj5IyP8sXji1xKdZbqaFK0CuMqbvmSCsuUXFimw8kxKo6x++IpzlIlFLl0IDVWZY6KSfrpucWKK/Vob3qcTMPQkZ+PtWDHnpo17vXJkdxRbudOuYsqjj17fFs5EtrKlbddnpKK/ZrTsvbxVJoX+Wuut6bMzJrPe6UFkiOpg+zN0lV2ZLNMV0VNUSndZMSE7z4i83jt54hQ91M4aqrtvFdaEPp+auyaMo9X1BTsXK648I+nYDU529V8fYrUeApUUyjX3NKC8I+nYDVlHq/53kiKzHgKVJNU+32Ed5yFczwFq8k7zoLdG5UVRWY8Baop87i17vfqc19e30dJGWbl1lgD8D7Efd68eZo+fXqtyxcVFSk+Pl4zZsyo9tcJvQLNwMrIyNCRI0eUmJgoqen/C/f6FTst86/Bg0d1rrGmtUt/CJBjw89WCiU+YMTpftFA+2P9ih1Baw33DKyBF3So8dhb/n3k/6Xn55Vo1BlNdzz90mfBUFMtNf33v3JXufTZf54JWzXusJWP+cpxQ+XNLY9pyhNC3PZznh6PR5VHn80wZOvc+aTaT+tX7LTMDKxBF3assaavPvshyHrCPwNr8KhOte6nnc+9LckaM7Da33ylpODH2Mqt1pmBdWGv2sfTyi2VNxvZGVgjutd83lu5JXit4Z4xMqJH7eeIpZusMwPrwp41n/cqjoPIz8Aa0aMiHGycfb7NOjOwRp5R8/Vp2SbrzMAa0b32a275OLPGDKwRPWq+N1qxxTozsEb1rv0+wjfOLDADq/I4C3RvtHKLdWZgjehhrfu9+tyX5+fnKzU1VU6n09fLqYuwzsAKJC4uTqmpqcrNzQ26TExMjGJiYqrFHQ5Hta8dej+0qrw7NtR4sK8z1iVuGEbAeLAcy79KaASIB35UWUPFq27T+5XGYDUFWk/w3Bu3plD2h/9765Jjw9dUOa9gx55hCzIsjdDjhmEEidukgPsvcLwpj6e6xqnpF1STYchhVB/DkgLGjSDL2wxDtrrEbbaAD548mfaT9/rRWNenmuJVz83ez8/q11xvLrXtJ1vle1tJRoB/fgwWt0nV+2ZV1lmXeNVcq/7sO/wb8foUNG7zHzfeXV/TeAq4qyJwzTUMmxyOms97ld9WtdaKeHjuIyrv9uDjLLT9VHu8YWqq6bxXNc36Hnu1x4PnHuh0HuwcEc7xFCzuHfPBrkN12X+NXVMo11z/cRbZ+/KQxlmExlOgeG33CyGPszDUVPVwrXqO8KYV7vFUEa/IpXKuVrjf8zqRe9hg+Ycq7A9xr6qgoEA5OTlKS0uLdCoAAAAAAACwoLA1sIqLi1VQUFAt/vDDD8s0TY0ePTpcqQAAAAAAAKAJabCvED7//PPKy8tTdna2JGnJkiW+B4DdfPPNOnr0qM4880xdccUVPz+sWlq6dKk++eQTjR49WpdeemlDpQIAwElh2eZIZ1BhZK9IZwAAAIBfsgZrYD3xxBPavXu37+f3339f77//viRp6tSpSk5O1tixY7V8+XK9/vrrcrvd6tSpk2bPnq0777wz4HcqAQAAAAAAgAZrYO3atavWZd58882G2hwAAAAAAAB+IZj2BAAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3NEOgEATdh//xvpDCp06hTpDIAGl7DPQmOsF2MMAAAAkcMMLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFiaI9IJAKiQsO+/kU6hQq9OtS6y9scw5BGiwbWnCwAAAABoopiBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3NEOgEAAMJp7Y+RzqDC4E6RzgAAAABoGpiBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3M0xEoKCws1d+5cff3111q/fr2OHj2qefPmafr06dWW3bp1q37/+9/rX//6l6Kjo3XxxRfrqaeeUlpaWkOkAgAIs2WbI51BhZG9Ip0BAAAAgMbQIA2snJwcPfTQQ2rXrp369Omj1atXB1xu7969Ou+885SUlKTZs2ersLBQTzzxhDZt2qT169crOjq6IdIBgGposgAAAABA09UgDaxWrVpp//79atmypTIzMzVgwICAy82ePVvHjh3Tt99+q3bt2kmSBg4cqAsvvFDz58/XNddc0xDpAAAAAAAA4CTSIM/AiomJUcuWLWtd7r333tPYsWN9zStJuuCCC9SlSxctXLiwIVIBAAAAAADASSZsD3Hft2+fDh06pP79+1d7beDAgcrKygpXKgAAAAAAAGhCGuQrhKHYv3+/pPKvG1bVqlUr5ebmqqSkRDExMdVeLykpUUlJie/n/Px8SZLL5ZLL5ZIk2Ww22Ww2eTweeTwe37LeuNvtlmmatcbtdrsMw/Ctt3Jcktxud0hxh8Mh0zT94oZhyG63V8vRMAxJ+jkP0289hmGTaXrkz5BhGA0SL+e/Te/nEaymquspzzFY7o1bUyj7qfy9gWs9sdxPvCaXy1XjsVeRr/96AuXe2DVJqnU8VeTaMMdefWryHgvBxplp2ir2U+V8jJ/jHrf/+oPGy88Rpsf/2JNh/3lD7lrjLlfdzxGB4lY573k/TsNWXpP/Z2DIsNmrf+7B4kb99pO3hJpqCny8R+YcIamW/VTlMwvTeAoUr/xZBjv2TNNs1OtTXWpyu901jierXHMlo9q5QKp+jvD8/HabWb4G0/BfS8C4Wf4vlZ7Km5dkmOU/eqqsI9S491gIdo4wzcDnw0icIzye2s97/psN/VzeGDW5XDWfy8tvaRrv+lSXmlyu2q9PVrjmVq6ppmtuRZqNc32qS02VL13BxpkU+Wuul2nWfB9RvnzgWv3CYThHhHJvVD7OwjuegsVdrprv96TIjaeqNUm138NW/OoQ+fvyyodroPty0xOZ8RSoJper8fsR4fpdo+p5oq7C1sAqKiqSpIANqtjYWN8ygV6fM2eOZs2aVS2elZWl5s2bS5LS0tLUsWNH7dy5U4cPH/Yt07ZtW7Vt21bbt2+X0+n0xTt06KD09HRt3rzZl5skdevWTcnJycrKyvLb2b1791Z0dLQyMzP9cujfv79KS0u1ceNGX8xut2vAgAFyOp3atm2bLx4XF6c+ffooJydHO3bs8MWTkpIkRanE41SxuyLHaFu8mjlSVeQ+qlJPYcXnZU9SrD1Zx1w5cpkVucfZUxVjj1eh64DcZpkv3tyRrigjTvll+2Sq4sBLiGolmxxylu3xq8nt7lBjTZWXtxtRSohqrVLPMRW5j/jiDiNO8VHpjV5TKPvJWXZMSVEZ8silgrL9vrghm5KiM+Qyi3XMdSgsNWVm5tZ47EkKeT81dk2Sah1PzrJjIe2ncNSUmZlbvo6kJHXv3l3Z2dnau3dvRa1HDDVzpOq460jA/VRYdijgsVdQll29JlucnKV7TrimrJLEOp8jAtVklfOe5/AxGbIpMTpDZZ6igPupxF0Y8NgrducFHE8nup8yjzevtSbJDPt4CnaOkFTjfnKW5fji4RxPgWqqfBwEO/ZKPI5GvT7VpabNm4tqHE9WueYmRWWoqKio1vuI46c2U5TLo9Y5xSqMcyg3qeIP38SWuHXq0RI546PkjI/yxeOLXEp1lupoUrQK4ypu+ZIKy5RcWKbDyTEqjrH74inOUiUUuXQgNVZljopJ+um5xYor9WhvepxMw9CRn4+FYOcINesv012qspyKmgzDruiWA2SWOlWWW3HeMxxxik7rI09RjlzOiv1ki0lSVEp3uQuz5S6sOO/Z49LkSO4ot3On3EUVx549vq0cCW3lytsuT0nFfs1pWft5rzSv4hwR1aK3DHu0Sg/61xR9anhqysys+VxeWiA5kjrI3ixdZUc2y3RV1BSV0k1GTLLKDmXJNBu/pszjtV+fQt1P4aiptmtuaUHo+6mxa8o8XlFTsN81FBf+8RSsJme7mu8jIjWeAtUUyr1RaUH4x1OwmjKP13y/J0VmPAWqSar9HtY7zsI5noLV5B1nwX53LyuKzHgKVFPm8cbvR4Trdw3vZKQTZZiVW2MNwPsQ93nz5mn69OnV4m+88Yauuuoqv/fcddddmjt3roqLi0OegZWRkaEjR44oMTFRknVmInjVteO5fsVOy/xr8OBRnWusae3SHwLkGJkZWANGnO4XDbQ/1q/YEbTWcM/AGnhBhxqPvXXLfrTMDKwho7vUOp7KP9vAtdYWb+iaBl7Q4edY4HG2fsWOiM2uqBofeEEHy/6rSGWhnve8x0G4x1OguPc4qKmmtUv/W22bkTpHDBnducb99PXyH0P6DALl3tA1DbygfbUcq4+znZaZgTXowo41jqevPvshyHrCf44YPKpTrfcRO597W5I1ZmC1v/lKScHPESu3WmcG1oW9aj/vrdxSebORnYE1onvN5/KVW4LXGu4ZIyN61H59WrrJOjOwLuxZ8zW34jiI/AysET0qwsHG2efbrDMDa+QZNd9HLNtknRlYI7rXfm9UPs6sMQNrRI+a7/dWbLHODKxRvWu/h/WNMwvMwKo8zgLdl6/cYp0ZWCN6nDwzsPLz85Wamiqn0+nr5dRF2GZgeb866P0qYWX79+9XSkpKwOaVVD5rK9BrDodDDod/Cd4PrSrvjg01XnW9JxI3DCNgPFiO5V8lNALEAz+qrKHiVbfp/UpjsJoCrSd47o1bUyj7w/+9dcmx4WuqnFewYy/U/VRTvKFqqm08Vc21vsdeTfHacq/tXODNIdzjKVDcm2tdzxF1jYfrvFf5swjneAoUr5prsPNYJMZTsNxr2k+Bz7eROUeEcqx6rx/hHE/+266Iez9Xq19zvbnUdh9hq3xvK8kI8M+PweI2qXrfrMo66xKvbZwZ3hKNIOMvYNwmBTve6xK3+Y8n766v6bwXcFcFyDFYvCFrcjhqPpdXflvVWivioeceLB5KTZV3e/BxFtp+qj3eMDXVdB6rmmZ9j73a48FzD3TZDXo9C+N4Chb3jvlg9wt12X+NXVMo90b+4yw84ylYPKRxFqHxFChe271qyOMsDDVVPVyrniO8aYV7PFXEK3KpnGtj9iPC8btGsPxDFbaHuLdp00ZpaWnVp5lLWr9+vfr27RuuVAAAAAAAANCEhK2BJUkTJkzQP/7xD+3ZU/H8h5UrV2r79u2aNGlSOFMBAAAAAABAE9FgXyF8/vnnlZeXp+zsbEnSkiVLfA8Au/nmm5WUlKR7771XixYt0vDhw3XrrbeqsLBQc+fO1RlnnKE</t>
-        </is>
+      <c r="D2" s="2">
+        <v>45687</v>
+      </c>
+      <c r="E2">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>37.64114853713622</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45687</v>
+      </c>
+      <c r="H2">
+        <v>22.07845885499383</v>
+      </c>
+      <c r="I2">
+        <v>5.412539116244487</v>
+      </c>
+      <c r="J2">
+        <v>37.64114853713622</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>vert_tbs</t>
-        </is>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>45639.5</v>
-      </c>
-      <c r="E3" t="n">
-        <v>17</v>
-      </c>
-      <c r="F3" t="n">
-        <v>32.81528883369784</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>45639.5</v>
-      </c>
-      <c r="H3" t="n">
-        <v>18.40551019114638</v>
-      </c>
-      <c r="I3" t="n">
-        <v>4.163773324629497</v>
-      </c>
-      <c r="J3" t="n">
-        <v>32.81528883369784</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACKEElEQVR4nOzdeXhU5fn/8c+ZmewhwUCQHdlXWZRFUGRTBBWUTVCQRfqzrmi1atG2VK2g1brX1uVbUMEq4G5dWARLlcUoCggIylJ2DEtCINtknt8fcSYZMpNMSDJzBt+v6+LS3HPmzH3POc85Z+48c2IZY4wAAAAAAAAAm3JEOgEAAAAAAACgPDSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAKikiRMnyrIsjRs3LqTln3jiCVmWpQ4dOtRwZhXr37+/LMvS8uXLI/L6kydPlmVZmjNnTkRev7pE+n38JTnrrLNkWZZ27NgR6VQAAEAE0cACAKCSpk6dKkl65513dOTIkQqXnz17tt/zasqf/vQnWZalP/3pTzX6Oqe7aHofw9lIW758uSzLUv/+/Wv8tQAAAE5GAwsAgEq68MIL1apVK+Xn52vevHnlLvvll19q/fr1iomJ0bXXXhumDIN75ZVXtGnTJvXs2TPSqUQ13kcAAIDwooEFAEAlWZal6667TlLJ7KpgvI9ffvnlqlevXo3nVpGmTZuqXbt2SkxMjHQqUY33EQAAILxoYAEAcAomT54sp9Opr7/+WuvWrQu4TF5env71r39JKvv1wa+++krjx49X06ZNFRcXp7S0NF1yySX68MMPA66r9H2A3n33XQ0cOFBpaWm+r49ZlqX7779fknT//ffLsizfv8mTJ/vWU9FXzj799FONGTNGjRs3VlxcnNLT09WjRw/NmDFDhw4d8i1XWFiouXPnavz48WrXrp1SUlKUkJCgtm3batq0adq7d2+ob2WF5syZ46vj0KFDuvnmm33vW7NmzfSb3/wm6Fc533rrLf3qV79Sp06ddMYZZyg+Pl7NmzfXddddp++//77M8tX1Pi5dulQjR45UgwYNFBsbq3r16mnEiBFauXJlwOW9ryFJb775pi644AKlpKQoKSlJ559/fpn9wrvNP/vsM0nSgAED/HItfY+xr776SmPHjlXjxo0VGxurlJQUtWjRQqNGjdK7774bMJ+T9e/fXwMGDJAkffbZZ36vddZZZ/kt63a79Y9//EN9+vRRamqq4uPj1bp1a02bNk179uwJ6fWCefvtt33vTa1atdS/f/+gY8Zr4cKFGjJkiNLT0xUbG6tGjRppwoQJ2rhxY6Vff+vWrbruuuvUvHlzxcXFKTk5Wc2aNdNll10WtJm9ZcsW/frXv1bLli0VHx+v1NRUXXjhhZo7d2615b1jxw7ftjDG6IUXXtC5556rpKQkpaamavDgwUH3PQAAooYBAACnZNiwYUaSmTZtWsDH582bZySZhg0bGrfb7Ys/+eSTxuFwGEmma9euZvTo0eaCCy4wsbGxRpK5//77y6yrWbNmRpK55ZZbjCTTvXt3c/XVV5t+/fqZ//znP2bSpEmmS5cuRpLp0qWLmTRpku/fiy++6FtPv379jCSzbNmyMq9x6623Gkm+vMaNG2eGDh1qWrRoUeY5u3btMpJMamqqOe+888yYMWPMpZdeaho2bGgkmfT0dLN169YyrzFp0iQjycyePTvk93n27NlGkhk+fLhp2bKlqV27trnyyivNiBEjzBlnnGEkmbZt25qDBw+Wea7T6TSJiYmme/fuZuTIkWb48OG+epKSksznn39eJr+qvo933nmnkWQcDofp2bOnGTNmjOnVq5exLMs4nU7zz3/+s8xzvO/7H//4R2NZljn//PPN2LFjfblYlmXeeust3/KbNm0ykyZNMmeeeaaRZC655BK/XFesWGGMMWbJkiUmJibGV8/o0aPNiBEjTM+ePU1cXJy54oorQtoGs2bNMpdccomRZM4880y/17rzzjt9y+Xl5ZmLLrrISDLx8fFm6NChZuzYsaZJkyZGkqlbt6756quvQnpNL+++/5vf/MZv3+/Zs6fvfXv66afLPK+wsNBcddVVRpKJi4szffr0MWPGjPG9pwkJCeajjz4KOY/169eblJQU3/42cuRIM2bMGNO7d2+TnJxsunTpUuY58+fPN/Hx8UaSadeunRkxYoQZOHCgSUpKMpLMlClTqiXv7du3G0mmWbNmZtKkSSYmJsYMHDjQXHXVVaZNmza+da1atSrkegEAsBsaWAAAnKJ33nnHSDJ16tQx+fn5ZR73fpC/9957fbGPP/7YWJZl6tataz777DO/5detW2caN25sJJnly5f7Peb9EO90Os27774bMJ8ZM2YYSWbGjBlBcw7WeHn66ad9tXz66adlnrd69Wrzv//9z/dzdna2effdd8vUXVBQYKZPn24kmUsvvbTMeqrSwJJkzjvvPHPo0CHfY0eOHDF9+vQxksy4cePKPPf11183OTk5fjGPx2P+9re/GUmmY8eOxuPx+D1elffxhRdeMJJMq1atzLfffuv32GeffWZq1aplYmNjzZYtW/we89ZXu3btMk0Gbz5t2rQJOQ+vAQMGGElm7ty5ZR47evSoWblyZdAaT7Zs2TIjyfTr1y/oMvfcc4+RZFq2bGm2b9/uixcUFJipU6caSaZ58+YBx0sw3n3fsqwydbz++uvGsizjcrnM+vXr/R679957jSTTq1cvs23bNr/HFixYYJxOpznjjDPMkSNHQspjypQpRpL585//XOaxEydOBBzPcXFxJj4+3rz55pt+j+3YscOcffbZRpJ5+eWXq5y3t4HlbWJ9//33vsfcbre57rrrjCQzePDgkGoFAMCOaGABAHCKCgsLTf369Y0ks2DBAr/Hdu7c6ZtlVXomUq9evYwks3DhwoDrnD9/vpFkRo0a5Rf3foi/7rrrguZzqo2XwsJCk56ebiSV+aB9qho2bGgcDofJzs72i1e1gbV27doyj69bt85YlmUcDofZtWtXyOvt3bu3kWS+++47v/ipvo9FRUW+GWgZGRkBn/eXv/zFSPKbtWRMSQMr0EyivLw8k5qaaiT5NRGD5VFahw4djCRz+PDhoLWEqqIGVm5urklOTjaSzHvvvVfm8ePHj/tmjM2bNy/k1/Xu+1deeWXAx0eNGmUkmf/3//6fL3bo0CGTkJBg4uPjze7duwM+76abbjKSzDPPPBNSHpdeeqmRZL7++uuQlh87dqyRZB577LGAj69Zs8ZIMueee26V8y7dwAr03u/bt883C6ugoCCk/AEAsBvugQUAwClyuVyaNGmSJOmf//yn32OzZ8+Wx+NRv3791KpVK0lSZmam1qxZo4SEBA0bNizgOvv37y9J+uKLLwI+Pnr06GrKvsRXX32ln376SXXr1tWIESMq9dxvv/1Wjz/+uG699VZdd911mjx5siZPniy32y2Px6Mffvih2vLs0qWLunbtWiZ+9tlnq1u3bvJ4PPrPf/5T5vEffvhBzz77rG6//XZNnTrVl+OBAwckKeC9sE7F2rVrtXfvXrVs2VLnnntuwGUq2r6B9ou4uDi1aNFCkip9DynvX0kcP368/vvf/8rtdlfq+ZWRkZGhnJwcpaWlBawjMTFR48aNkyQtW7as0uv3jrVg8dL3I1u2bJlyc3N1/vnnq1GjRgGfV9G2OJn3vbzxxhv1ySefKC8vL+iyHo9HH330kSRp7NixAZfp3r27kpOTtXbtWt+6qpq3y+XSkCFDysTr16+vM844Q/n5+X73sgMAIJq4Ip0AAADR7LrrrtMjjzyiRYsWac+ePWrUqJGMMb6baJe+efv27dtljFFubq7i4uLKXe9PP/0UMH7yDbOrw86dOyVJbdu29d1IvCLHjx/Xtddeq7fffrvc5bKzs6ucn1fz5s3Lfezrr7/W7t27fbGioiLdcsstev7552WMqfEct23bJkn68ccfK3wfg23fpk2bBoynpKRIUrlNk0BmzZqldevW6aOPPtJHH32khIQEnXPOOerfv7/Gjx+v9u3bV2p95fE218rbTi1btvRbtjKCrdcbL73tvdti6dKlp7wtTnbXXXfpv//9r5YsWaIhQ4YoJiZGXbp00YUXXqhx48apR48evmUPHTrk26+aNGlS4boPHTqkRo0aVTnvBg0aKCYmJuDyKSkpOnLkSKX3IQAA7IIGFgAAVdCmTRv17dtXK1as0CuvvKLp06dr2bJl2rFjh1JTU/1mTHk8HklScnKyRo0adUqvl5CQUC15V9X06dP19ttvq127dnr44YfVo0cP1a1bV7GxsZKkPn36aOXKleU2jmpC6dd76qmn9I9//EP169fX448/rj59+ujMM89UfHy8JOmaa67Rv/71r2rL0bt969evr0suuaTcZevWrRsw7nBU7+T4+vXrKyMjQ5999pmWLFmizz//XKtXr9bnn3+umTNnatasWbrnnnuq9TUjpfR29G6LVq1a6fzzzy/3ee3atQtp/YmJiVq8eLG+/PJLffzxx/riiy/0xRdfKCMjQ48//rhuuukm/e1vf/N7fSn4zLHSvA3tquZd3fsPAAB2QgMLAIAqmjp1qlasWKHZs2dr+vTpvq8Tjhs3zq/h5J2JYVmW/vnPf9rmw6Z31s+WLVtkjAlpFtb8+fMlSW+88YY6d+5c5vGtW7dWb5IqnsEWzI4dOyRJjRs39sW8OT7//PMaPnx4medUd47e7VunTh3fDDw7sCxL/fv39331LC8vT3PmzNHNN9+se++9V6NHj/bNjKoK71feyttO3hlGwb4eV57t27erS5cuZeKBtr13W7Rt27bat0WPHj18s63cbrfeeecdTZw4Uc8995xGjx6tAQMGqG7dukpISFBubq4ee+yxoA3Lk9Vk3gAARDt7XDkDABDFxowZo5SUFG3dulUffPCB3nrrLUn+Xx+UpIYNG6pz5846duyYPv7442rPwzv7qbL3Oerevbvq1q2rn376Se+8805Izzl8+LAkqVmzZmUe++STT5SZmVmpHEKxbt06rVu3rkz8u+++09dffy2Hw6ELL7wwpBy/++47ffPNNwFf51TfR+8stI0bN+q7776r1HNP1ankGh8frxtuuEGdO3eWx+MJ+J6eymt57+l0+PBhvffee2Uez83N1euvvy5JGjBgQMj5er366qsB46+88oqkkntDSdKgQYMUGxur5cuX6+DBg5V+rVC5XC6NHj3aN+POu085nU5dfPHFkkoaqaEIV94AAEQjGlgAAFRRYmKirr76aknF98TKzc3V2Wef7XdPHK8///nPkqQpU6bo/fffL/O4MUarV6/WokWLKp2HdwZKZZsnLpdL9913nyTp+uuvD3gj9C+//NLvHkPeeyc988wzfst9//33uuGGGyr1+qEyxujGG2/UkSNHfLGsrCzdeOONMsZo1KhRfvcb8ub4t7/9ze8rXfv27dPEiRODNmJO9X2MiYnRjBkzZIzRiBEj9N///rfMMkVFRfr000+1atWqSq07mIpyfeyxx/S///2vTHzz5s2+GWiBGnzlvdbWrVtVWFhY5vH4+HjdfPPNkqQ777zTd281SSosLNRtt92m/fv3q3nz5qf0xwjefvttXwPMa+HChXrzzTflcrl06623+uJnnnmmbr31Vh0/flzDhg3T+vXry6wvPz9f7733njZv3hzS6z/33HMBb/i/f/9+ZWRkSPJ/L2fMmKHY2Fjdddddevnll/32Qa8NGzb4Gt41lTcAAKeNyPzxQwAATi9r1qzx/Rl7SebJJ58MuuxTTz1lXC6XkWRatWplLrvsMnPNNdeYiy++2NSrV89IMvfcc4/fc5o1a2Ykme3btwdd7/79+01SUpKRZM4//3wzefJkM3XqVPPPf/7Tt0y/fv2MJLNs2TK/53o8HnPDDTf48u/WrZsZN26cufTSS02LFi3KPOfNN980lmUZSebss88248aNMwMHDjQxMTFm4MCBpk+fPgFfZ9KkSUaSmT17dkVvqc/s2bONJDN8+HDTokULU7t2bTNixAgzcuRIk5aWZiSZ1q1bmwMHDvg9b9WqVSY2Ntb3Pl911VVmyJAhJiEhwXTs2NGMGDEiYC5VeR+NMeauu+7yvY8dO3Y0V1xxhRk3bpzp37+/qV27tpFk/v73v/s9x7t8MMFe74MPPjCSTGxsrLn88svNddddZ6ZOnWo+//xzY4wxqampRpJp166dGTFihLnmmmtM//79ffvfxIkTQ9gCJbp3724kmbZt25rx48ebqVOn+u2reXl5ZtCgQUaSSUhIMJdeeqkZO3asadq0qZFk6tSpYzIyMir1mt59//bbbzeSTI8ePcw111xjevXq5XvfHn/88TLPKywsNNdcc42RZBwOh+nWrZsZNWqUGTt2rDn//PN92/ijjz4KKY8uXboYSaZ58+Zm2LBhZvz48Wbw4MEmISHBSDIDBw40hYWFfs+ZP3++SUxMNJJM48aNzeDBg8348ePN0KFDTePGjY0kM3bs2CrnvX37diPJNGvWrML3sbxjCAAAdkYDCwCAanL22Wf7mgmZmZnlLrt+/Xpz/fXXm9atW5v4+HiTmJhoWrRoYS655BLz9NNPmz179vgtH+qHz//85z/moosuMmeccYZxOBxGkpk0aZLv8fIaL8YY89FHH5krrrjCnHnmmSYmJsakp6ebnj17mvvvv98cOnSozGsNGjTI1K1b1yQmJppOnTqZhx56yOTn5wd9nao0sCZNmmQOHjxofv3rX5vGjRub2NhY06RJEzNt2rQyuXmtW7fODB8+3DRo0MDEx8eb1q1bm7vvvttkZ2eXm0tV38fPP//cjB8/3jRr1szExcWZWrVqmTZt2pgrr7zSvPTSS+bw4cN+y59qA8sYY1588UVzzjnn+BolpWuaO3eumTJliunUqZNJS0szcXFxplmzZmbo0KHm7bffNh6PJ+hrBrJz505zzTXXmAYNGviaYCc3TQoLC81zzz1nzjvvPFOrVi0TGxtrWrZsaW699Vaze/fuSr2eMf77/vz5803v3r1NcnKySUpKMn379jXvv/9+uc//8MMPzciRI02jRo1MTEyMqV27tmnfvr0ZN26cee2118zx48dDyuODDz4wN954o+nWrZtJT083sbGxpnHjxqZ///7m5ZdfNgUFBQGft337dvOb3/zGdOrUySQlJZn4+HjTrFkz079/f/Pwww+bH374ocp508ACAPwSWMaE+c8DAQAAVMKcOXM0ZcoUTZo0iRtbAwAA/EJxDywAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANga98ACAAAAAACArTEDCwAAAAAAALZGAwsAAAAAAAC25op0AqfC4/Fo7969qlWrlizLinQ6AAAAAAAAKIcxRseOHVPDhg3lcFR+PlVUNrD27t2rJk2aRDoNAAAAAAAAVMKuXbvUuHHjSj8vKhtYtWrVklRcdEpKSoSzAQAAAAAAQHmys7PVpEkTX0+nsqKygeX92mBKSgoNLAAAAAAAgChxqreC4ibuAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALC1qPwrhAAAAAAAIPyMMSoqKpLb7Y50KrAJl8slp9N5yn9dMOTXqdG1AwAAAACAqGeM0dGjR/XTTz+pqKgo0unAZpxOp+rVq6fU1NQaa2TRwAIAAAAAAOXav3+/jh49qpSUFKWkpMjlctX4jBvYnzFGbrdb2dnZ2rdvn3Jzc9WgQYMaeS0aWAAAAAAAIKiioiJlZWUpPT1ddevWjXQ6sKFatWopLi5OmZmZqlevnpxOZ7W/BjdxBwAAAAAAQRUWFsoYo6SkpEinAhtLSkqSMUaFhYU1sn4aWAAAAAAAoEJ8ZRDlqen9gwYWAAAAAAAAbI0GFgAAAAAAAAKaPHmyzjrrrEinQQMLAAAAAAD8cs2ZM0eWZQX9t2rVqkinWKGNGzfqT3/6k3bs2BHpVGoMf4UQAAAAAAD84j3wwANq3rx5mXirVq0ikE3lbNy4Uffff7/69+9vi9lSNYEGFgAAAAAAOGWLNkQ6A2lwp6qvY+jQoerevXvVV4QawVcIAQAAAAAAyjFjxgw5HA4tXbrUL3799dcrNjZW3377rSRp+fLlsixLb7zxhu69917Vr19fSUlJGj58uHbt2lVmvatXr9aQIUOUmpqqxMRE9evXT59//nmZ5fbs2aOpU6eqYcOGiouLU/PmzXXjjTeqoKBAc+bM0ZgxYyRJAwYM8H31cfny5b7nf/TRR+rbt6+SkpJUq1YtXXbZZfruu+/KvM4777yjTp06KT4+Xp06ddLbb79dlbetWjEDCwAAAAAA/OJlZWUpMzPTL2ZZlurUqaPf//73ev/99zV16lStX79etWrV0ieffKIXX3xRDz74oLp06eL3vIceekiWZemee+7RwYMH9eSTT+qiiy7SN998o4SEBEnSp59+qqFDh+rcc8/1Nchmz56tgQMHasWKFerZs6ckae/everZs6eOHj2q66+/Xu3atdOePXu0cOFCnThxQhdeeKGmTZump59+Wvfee6/at28vSb7/vvrqq5o0aZIuueQSPfLIIzpx4oT+/ve/64ILLtDatWt9XzlctGiRRo0apQ4dOmjWrFk6dOiQpkyZosaNG9fk2x4yyxhjIp1EZWVnZys1NVVZWVlKSUmJdDoAAAAAAJy28vLytH37djVv3lzx8fFlHo/2rxDOmTNHU6ZMCfhYXFyc8vLyJEkbNmzQueeeq4kTJ+rRRx9Vp06d1KBBA61cuVIuV/H8oOXLl2vAgAFq1KiRNm3apFq1akmSFixYoKuuukpPPfWUpk2bJmOM2rZtqxYtWuijjz6SZVmSpNzcXHXs2FGtWrXSokWLJEmTJk3S3LlztXr16jJfcTTGyLIsLVy4UGPGjNGyZcvUv39/3+M5OTlq0qSJxowZoxdeeMEXP3DggNq2baurrrrKF+/WrZsOHDigTZs2KTU1VZK0ePFiDR48WM2aNavwBvEV7SdV7eUwAwsAAAAAAPzi/e1vf1ObNm38Yk6n0/f/nTp10v3336/p06dr3bp1yszM1KJFi3zNq9ImTpzoa15J0ujRo9WgQQN9+OGHmjZtmr755htt3bpVv//973Xo0CG/5w4aNEivvvqqPB6PpOKv9Q0bNizg/bm8ja9gFi9erKNHj+rqq6/2m13mdDrVq1cvLVu2TJK0b98+ffPNN/rd737na15J0sUXX6wOHTro+PHj5b5OONDAAgAAAAAAv3g9e/as8Cbud911l15//XWtWbNGM2fOVIcOHQIu17p1a7+fLctSq1atfLOYtm7dKql4dlUwWVlZKigoUHZ2tjp1OrUpZt7XGThwYMDHvTOhdu7cGTBvSWrbtq2+/vrrU3r96kQDCwAAAEC1s8NXiryq46+TAYAkbdu2zdcUWr9+/Smvxzu76tFHH1XXrl0DLpOcnKzDhw+f8muUfp1XX31V9evXL/N4oNljdhU9mQIAAAAAAESIx+PR5MmTlZKSottvv10zZ87U6NGjNXLkyDLLeptcXsYY/fDDD+rcubMkqWXLlpKKZ0BddNFFQV8zPT1dKSkp2rCh/N8KBPsqofd16tWrV+7rNGvWLGDekvT999+X+9rhQgMLAAAAiALMaAKAyHr88cf1xRdf6L333tNll12m5cuX68Ybb9SFF16ounXr+i37yiuvaPr06b77YC1cuFD79u3TPffcI0k699xz1bJlSz322GO65pprlJyc7Pf8n376Senp6XI4HLryyis1d+5cZWRkBL2Je1JSkiTp6NGjfo9fcsklSklJ0cyZMzVgwADFxMQEfJ0GDRqoa9euevnll/3ug7V48WJt3LjR1+CKJBpYAAAAAADgF++jjz7S5s2by8T79Omj/Px8/eEPf9DkyZM1bNgwScV/vbBr16666aabNH/+fL/npKWl6YILLtCUKVN04MABPfnkk2rVqpX+3//7f5Ikh8Ohl156SUOHDlXHjh01ZcoUNWrUSHv27NGyZcuUkpKi999/X5I0c+ZMLVq0SP369dP111+v9u3ba9++fVqwYIH++9//qnbt2urataucTqceeeQRZWVlKS4uTgMHDlS9evX097//Xddee63OOeccjRs3Tunp6frf//6nf//73zr//PP17LPPSpJmzZqlyy67TBdccIGuu+46HT58WM8884w6duyonJycmnzrQ0IDCwAAAAAA/OL98Y9/DBh/6aWX9Pzzz6tu3bp68sknffHWrVtr1qxZuu222zR//nxdddVVvsfuvfderVu3TrNmzdKxY8c0aNAgPffcc0pMTPQt079/f61cuVIPPvignn32WeXk5Kh+/frq1auXfv3rX/uWa9SokVavXq0//OEPmjdvnrKzs9WoUSMNHTrUt7769evrH//4h2bNmqWpU6eqqKhIy5YtU7169XTNNdeoYcOGevjhh/Xoo48qPz9fjRo1Ut++fTVlyhTf6wwZMkQLFizQ73//e02fPl0tW7bU7Nmz9e6772r58uXV9C6fOssYYyKdRGVlZ2crNTVVWVlZvjvmAwAAAKezaPsKYbTlCyC4vLw8bd++Xc2bN1d8fHyk07G15cuXa8CAAVqwYIFGjx4d6XTCqqL9pKq9HEd1JAkAAAAAAADUFBpYAAAAAAAAsDUaWAAAAAAAALA1buIOAAAAAABQDfr3768ovNV4VGAGFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAA+MWaM2eOLMtSfHy89uzZU+bx/v37q1OnThHIDKW5Ip0AAAAAAACIYh9/HOkMpCFDqryK/Px8Pfzww3rmmWeqISFUN2ZgAQAAAACAX7yuXbvqxRdf1N69eyOdCgKggQUAAAAAAH7x7r33XhUVFenhhx8udzm3260HH3xQLVu2VFxcnM466yzde++9ys/P9y1zxx13qE6dOjLG+GK33nqrLMvS008/7YsdOHBAlmXp73//e/UXdJrhK4QAAAAAftEWbYh0BiUGc5sdIGKaN2+uiRMn6sUXX9Tvfvc7NWzYMOByv/rVr/Tyyy9r9OjRuvPOO7V69WrNmjVLmzZt0ttvvy1J6tu3r5544gl99913vvtnrVixQg6HQytWrNC0adN8MUm68MILw1BhdGMGFgAAAAAAgKT77rtPbrdbjzzySMDHv/32W7388sv61a9+pQULFuimm27Syy+/rN/+9rd65513tGzZMknSBRdcIKmkQZWVlaX169dr1KhRvpj38bS0NHXo0KGGK4t+NLAAAAAAAAAktWjRQtdee61eeOEF7du3r8zjH374oaTirwiWduedd0qS/v3vf0uS0tPT1a5dO/3nP/+RJH3++edyOp266667dODAAW3dulVScQPrggsukGVZNVbT6YIGFgAAAAAAwM9+//vfy+12B7wX1s6dO+VwONSqVSu/eP369VW7dm3t3LnTF+vbt69vttWKFSvUvXt3de/eXWlpaVqxYoWys7P17bffqm/fvjVb0GmCBhYAAAAAAMDPWrRooQkTJgSdhSUppBlTF1xwgfbs2aNt27ZpxYoV6tu3ryzL0gUXXKAVK1boiy++kMfjoYEVIhpYAAAAAAAApXhnYZ18L6xmzZrJ4/H4vgLodeDAAR09elTNmjXzxbyNqcWLF+vLL7/0/XzhhRdqxYoVWrFihZKSknTuuefWcDWnBxpYAAAAAAAApbRs2VITJkzQ888/r/379/vil156qSTpySef9Fv+8ccflyRddtllvljz5s3VqFEjPfHEEyosLNT5558vqbix9eOPP2rhwoU677zz5HK5aria0wMNLAAAAAAAgJPcd999Kiws1Pfff++LdenSRZMmTdILL7ygsWPH6rnnntPkyZP1l7/8RVdeeaUGDBjgt46+ffvq+++/V6dOnXTGGWdIks455xwlJSVpy5YtfH2wEmhgAQAAAAAAnKRVq1aaMGFCmfhLL72k+++/X19++aVuv/12ffrpp5o+fbpef/31Mst6G1QXXHCBL+ZyudS7d2+/x1ExyxhjIp1EZWVnZys1NVVZWVlKSUmJdDoAAABAjVu0IdIZlBjcqeJloinfaMoViIS8vDxt375dzZs3V3x8fKTTgU1VtJ9UtZfDDCwAAAAAAADYWpUbWF9++aVuueUWdezYUUlJSWratKmuuuoqbdmyxW+5yZMny7KsMv/atWtX1RQAAAAAAABwGqvyre4feeQRff755xozZow6d+6s/fv369lnn9U555yjVatWqVOnkjmwcXFxeumll/yen5qaWtUUAAAAAAAAcBqrcgPrjjvu0GuvvabY2FhfbOzYsTr77LP18MMPa+7cuSUv5nIFvAEaAAAAEAnc+wgAgOhQ5a8Q9unTx695JUmtW7dWx44dtWnTpjLLFxUVKTs7u6ovCwAAAAAAgF+IGrmJuzFGBw4cUN26df3iJ06cUEpKilJTU5WWlqabb75ZOTk5NZECAAAAAAAAThNV/gphIPPmzdOePXv0wAMP+GINGjTQ3XffrXPOOUcej0cff/yxnnvuOX377bdavny5XK7gqeTn5ys/P9/3s3cGl9vtltvtliQ5HA45HA55PB55PB7fst54UVGRjDEVxp1OpyzL8q23dFwqnkEWStzlcskY4xe3LEtOp7NMjsHi1ERN1ERN1ERN1ERN1FSzNZmS1UhWce4y/rkHi1uO4pr845Ysh1PGeHTSygPHLYcsyyFjPHK7y6/JeEot7ymSZEqtp7gm4/HfTjVVk9td8XYKWmuZ3MNTU3n7XkmaFW+nmq6p9FCLtvFU2ulyjKCm4rjb7S45FpVab+n87RSvDLvlHs01ScX7R+leTel97+T9r7KqvYG1efNm3Xzzzerdu7cmTZrki8+aNctvuXHjxqlNmza67777tHDhQo0bNy7oOmfNmqX777+/THzt2rVKSkqSJKWnp6tly5bavn27fvrpJ98yjRs3VuPGjbVlyxZlZWX54i1atFC9evW0YcMG5ebm+uLt2rVT7dq1tXbtWr9B3LlzZ8XGxiojI8Mvh+7du6ugoEDr1q3zxZxOp3r06KGsrCxt3rzZF09ISFCXLl2UmZmpbdu2+eKpqalq37699u7dq927d/vi1ERN1ERN1ERN1ERN1FSzNRUcLakppm5nWc5YFRzwryn2zO4yRQUqzCypybKciq3fQ6YgS4WHS2qyXAmKTe8iT26m3FklNTniUhWT1l5FOXtVlFNSkzMhXa7aLVWUtV0ZGeXXVHBMcqW2kDOxngoPbZBxl9QUk9ZOVlxtFR5cK2NqvqaMExVvp6Ks7SrKLanJmdxYrlqN5T66RZ78ku0Ujpoq2vcKjoW+nWq6powTJTVF23g6HY8R1FRSU3x8vKTiplZeXp4v7nA4lJiYKLfb7TfxxOl0KiEhQYWFhSooKPDFXS6X4uPjlZ+f79fQiI2NVWxsrPLy8vxyjIuLU0xMjHJzc/2aePHx8XK5XDpx4oRfMyUhIUEOh0PHjx/3qykpKUkej8fvfbEsS0lJSdRUTTVJUmFhoTZsKLnBZOl9r6q3k7JMVVt7pezfv1/nn3++CgsLtWrVKjVs2LDc5XNzc5WcnKwpU6aU+euEpQWagdWkSRMdOnRIKSkpkuzTmfY6nbrt1ERN1ERN1ERN1ERNp2tNSzeWSjLCM7AGtS+/pqUbSy0f4RlYgzpUvJ0+WW+fGVgXdyx/3yvZDyI/A2tQh5JwtI2n0k6XYwQ1Fcfz8vL0v//9Ty1atPA1KkpjthI1ScW9m23btqlp06a+hmfpfS87O1t16tRRVlaWr5dTGdU2AysrK0tDhw7V0aNHtWLFigqbV1JxF7FOnTo6fPhwucvFxcUFHCQul6vMVw+9A/Zk3gEYajzYVxorE7csK2A8WI6VjVMTNQWLUxM1SdQULMfKxqmJmiRqCpZjZeN2rMkKdEdYK8glcoC4ZVlB4g4FWnl5cZer/JpKP81yBK7JcoSee7B4KDWV3ozBtkfQWoPmXrM1lbfvnZxmpbdfNdYUaEhFy3iqapya7FuTy+UqPjZIvv+ezG7xyrBb7tFeU6BeTaBYZVVLAysvL0/Dhg3Tli1btGTJEnXo0KHiJ0k6duyYMjMzlZ6eXh1pAAAAAAAA4DRU5b9CWFRUpLFjx2rlypVasGCBevfuXWaZvLw8HTt2rEz8wQcflDFGQ4YMqWoaAAAAAAAAtmNZlv70pz9FOo2oV+UZWHfeeafee+89DRs2TIcPH9bcuXP9Hp8wYYL279+vbt266eqrr1a7du0kSZ988ok+/PBDDRkyRFdccUVV0wAAAAAAAKiUUL+ut2zZMvXv379mk0G5qtzA+uabbyRJ77//vt5///0yj0+YMEG1a9fW5ZdfrsWLF+vll19WUVGRWrVqpZkzZ+q3v/1twO/yAgAAAACAKPDDD5HOQGrV6pSe9uqrr/r9/Morr2jx4sVl4u3btz/l1FA9qtzAWr58eYXL1K5du8zGBwAAAAAAiKQJEyb4/bxq1SotXry4TByRx9QnAAAAAACAII4fP64777xTTZo0UVxcnNq2bavHHntMxhi/5fLz8/Wb3/xG6enpqlWrloYPH67du3eXWd/OnTt10003qW3btkpISFCdOnU0ZswY7dixw7fMtm3bZFmWnnjiiTLP/+KLL2RZlv71r39Ve612RgMLAAAAAAAgAGOMhg8frieeeEJDhgzR448/rrZt2+quu+7SHXfc4bfsr371Kz355JMaPHiwHn74YcXExOiyyy4rs84vv/xSX3zxhcaNG6enn35aN9xwg5YuXar+/fvrxIkTkqQWLVro/PPP17x588o8f968eapVq9Yv7n7iVf4KIQAAAAAAwOnovffe06effqo///nPuu+++yRJN998s8aMGaOnnnpKt9xyi1q2bKlvv/1Wc+fO1U033aS//e1vvuXGjx+vdevW+a3zsssu0+jRo/1iw4YNU+/evfXmm2/q2muvlSRNnDhRv/71r7V582bfH8QrLCzU/PnzNXLkSCUmJtZ0+bbCDCwAAAAAAIAAPvzwQzmdTk2bNs0vfuedd8oYo48++si3nKQyy91+++1l1pmQkOD7/8LCQh06dEitWrVS7dq19fXXX/seu+qqqxQfH+83C+uTTz5RZmbmL/IeXTSwAAAAAAAAAti5c6caNmyoWrVq+cW9f5Vw586dvv86HA61bNnSb7m2bduWWWdubq7++Mc/+u6pVbduXaWnp+vo0aPKysryLVe7dm0NGzZMr732mi82b948NWrUSAMHDqy2GqMFDSwAAAAAAIAwufXWW/XQQw/pqquu0vz587Vo0SItXrxYderUkcfj8Vt24sSJ2rZtm7744gsdO3ZM7733nq6++mo5HL+8dg73wAIAAAAAAAigWbNmWrJkiY4dO+Y3C2vz5s2+x73/9Xg8+vHHH/1mXX3//fdl1rlw4UJNmjRJf/3rX32xvLw8HT16tMyyQ4YMUXp6uubNm6devXrpxIkTvntk/dLQwAIAAACAKLJoQ6QzKDG4U6QzAGrWpZdeqhdeeEHPPvuspk+f7os/8cQTsixLQ4cOlSQNHTpU9957r55++mnfTdwl6cknnyyzTqfTKWOMX+yZZ55RUVFRmWVdLpeuvvpqvfbaa9q0aZPOPvtsde7cuZqqiy40sAAAAAAAAAIYNmyYBgwYoPvuu087duxQly5dtGjRIr377ru6/fbbffe86tq1q66++mo999xzysrKUp8+fbR06VL98MMPZdZ5+eWX69VXX1Vqaqo6dOiglStXasmSJapTp07AHCZOnKinn35ay5Yt0yOPPFKj9doZDSwAAAAAAIAAHA6H3nvvPf3xj3/UG2+8odmzZ+uss87So48+qjvvvNNv2X/+85++r/u98847GjhwoP7973+rSZMmfss99dRTcjqdmjdvnvLy8nT++edryZIluuSSSwLmcO6556pjx47atGmTxo8fX2O12p1lTp63FgWys7OVmpqqrKwspaSkRDodAAAARKlo+ipWNOUqRVe+0ZSrFH35Ivrl5eVp+/btat68ueLj4yOdzi9St27dlJaWpqVLl0Y6laAq2k+q2sv55d22HgAAAAAAIEpkZGTom2++0cSJEyOdSkTxFUIAAAAAAACb2bBhg7766iv99a9/VYMGDTR27NhIpxRRzMACAAAAAACwmYULF2rKlCkqLCzUv/71r1/81zdpYAEAAAAAANjMn/70J3k8Hm3atEn9+vWLdDoRRwMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAFTIGBPpFGBjNb1/0MACAAAAAABBOZ1OSVJhYWGEM4GdefcP7/5S3WhgAQAAAACAoGJiYhQXF6esrCxmYSEgY4yysrIUFxenmJiYGnkNV42sFQAAAAAAnDbq1q2rPXv2aPfu3UpNTVVMTIwsy4p0WogwY4wKCwuVlZWlnJwcNWrUqMZeiwYWAAAAAAAoV0pKiiQpMzNTe/bsiXA2sJu4uDg1atTIt5/UBBpYAAAAAACgQikpKUpJSVFhYaGKiooinQ5swul01tjXBkujgQUAAAAAAEIWExMTloYFUBo3cQcAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK25Ip0AAAAAAOD0tGhDpDMoMbhTpDMAUBXMwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK25Ip0AAAAATh+LNkQ6gxKDO0U6AwAAUF2YgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW3NFOgEAAAAAAOxg0YZIZ1BicKdIZwDYCzOwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGtVbmB9+eWXuuWWW9SxY0clJSWpadOmuuqqq7Rly5Yyy27atElDhgxRcnKy0tLSdO211+qnn36qagoAAAAAAAA4jbmquoJHHnlEn3/+ucaMGaPOnTtr//79evbZZ3XOOedo1apV6tSpkyRp9+7duvDCC5WamqqZM2cqJydHjz32mNavX681a9YoNja2ysUAAAAAAADg9FPlBtYdd9yh1157za8BNXbsWJ199tl6+OGHNXfuXEnSzJkzdfz4cX311Vdq2rSpJKlnz566+OKLNWfOHF1//fVVTQUAAAAAAACnoSp/hbBPnz5lZk+1bt1aHTt21KZNm3yxN998U5dffrmveSVJF110kdq0aaP58+dXNQ0AAAAAAACcpmrkJu7GGB04cEB169aVJO3Zs0cHDx5U9+7dyyzbs2dPrV27tibSAAAAAAAAwGmgyl8hDGTevHnas2ePHnjgAUnSvn37JEkNGjQos2yDBg10+PBh5efnKy4uLuD68vPzlZ+f7/s5OztbkuR2u+V2uyVJDodDDodDHo9HHo/Ht6w3XlRUJGNMhXGn0ynLsnzrLR2XpKKiopDiLpdLxhi/uGVZcjqdZXIMFqcmaqImaqImaqImaoq2moxx/vw//nHLUVyTf9yS5XDKGI9kPBXHLYcsyxE87imSVJK7x1NxTf4vGzj3YPHqrsntLn87GU/wWmUV12Q8/tuppmpyuyve90LdTuGqqbzxVJJm9ex7Vamp9FALNs6k8I+nYHFjyj9GFC8fuFa/cBiOEaEc94rHWXjHU7C42835iZpOr5pOrquyqr2BtXnzZt18883q3bu3Jk2aJEnKzc2VpIANqvj4eN8ywRpYs2bN0v33318mvnbtWiUlJUmS0tPT1bJlS23fvt3vLxs2btxYjRs31pYtW5SVleWLt2jRQvXq1dOGDRt8+UlSu3btVLt2ba1du9ZvY3fu3FmxsbHKyMjwy6F79+4qKCjQunXrfDGn06kePXooKytLmzdv9sUTEhLUpUsXZWZmatu2bb54amqq2rdvr71792r37t2+ODVREzVREzVREzVRU7TVpMTuMkUFKswsqcmynIqt30OmIEuFh0tqslwJik3vIk9uptxZJTU54lIVk9ZeRTl7VZRTUpMzIV2u2i1VlLVdRbklNTmTG8tVq7HcR7fIk19SU2b9imsqOFpSU0zdzrKcsSo44F9T7JnhqSkjo/ztVHBMcqW2kDOxngoPbZBxl9QUk9ZOVlxtFR5cK2NqvqaMExXve6Fup3DUVNF4KjgW+naq6ZoyTpTUFOwYoYTwj6dgNWU1Lf8YEanxFKimUI57BcfCP56C1ZRxgvMTNZ1eNXknI50qy5RujVXR/v37df7556uwsFCrVq1Sw4YNJUkZGRnq0aOHXnnlFV177bV+z7n77rv16KOPKi8vr1IzsJo0aaJDhw4pJSVFEh1PaqImaqImaqImaqImO9S0dJN9ZmBd3KnimpZuLP2ykZ2BNah9+dtp6cbgtYZ7xsigDhXve5+st88MrIs7lj+eSvaDyM/AGtShJBxsnH262T4zsAafXf4xYtF6+8zAGtS+4uNe8TizxwysQR04P1HT6VVTdna26tSpo6ysLF8vpzKqbQZWVlaWhg4dqqNHj2rFihW+5pVU8tVB71cJS9u3b5/S0tKCNq+k4plbgR53uVxyufxL8L5pJ/Nu2FDjJ6/3VOKWZQWMB8uxsnFqoqZgcWqiJomaguVY2Tg1UZNETcFyDBS3LO//BK4pcNwhWWVzrHTc4Z+7t+zyagqwmoA5BotXZ00uV/nbqfTTTq61JB567sHiodRUerMH28dC3U4Vx6unpvLG08lpVnXfqzgePPdAQy3YMSKc4ylY3Dvmgx0jKrP9arqmUI57/uMsPOMpWDyUccb5iZqCxe1YU7D8Q1UtDay8vDwNGzZMW7Zs0ZIlS9ShQwe/xxs1aqT09PSyU8wlrVmzRl27dq2ONAAAAAAAAHAaqvJfISwqKtLYsWO1cuVKLViwQL179w643KhRo/TBBx9o165dvtjSpUu1ZcsWjRkzpqppAAAAAAAA4DRV5RlYd955p9577z0NGzZMhw8f1ty5c/0enzBhgiTp3nvv1YIFCzRgwADddtttysnJ0aOPPqqzzz5bU6ZMqWoaAAAAAAD8YizaEOkMSgzuFOkM8EtQ5QbWN998I0l6//339f7775d53NvAatKkiT777DPdcccd+t3vfqfY2Fhddtll+utf/1ru/a8AAAAAAADwy1blBtby5ctDXrZjx4765JNPqvqSAAAAAAAA+AWp8j2wAAAAAAAAgJpEAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC25op0AgAAAAAA4PS2aEOkMygxuFOkM8CpYAYWAAAAAAAAbI0GFgAAAAAAAGyNrxACAADYHF+7AAAAv3TMwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK25Ip0AAABA2P3wQ6QzKNGqVaQzAAAApSzaEOkMSgzuFOkM7IMZWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1V6QTAAAAQPlaLnol0imU6DQx0hkAAIBfIGZgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWXJFOANFn0YZIZ1BicKdIZwAAAAAAAGoaM7AAAAAAAABga8zAAgAA1eOHHyKdQYlWrSKdAQAAAKoRM7AAAAAAAABga8zAsgnuKwUAAAAAABAYM7AAAAAAAABga8zAAgAAvzgrf4x0BiV6c7suAACACtHAwmmPr2cCAAAAABDd+AohAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGytWhpYOTk5mjFjhoYMGaK0tDRZlqU5c+aUWW7y5MmyLKvMv3bt2lVHGgAAAAAAADgNuapjJZmZmXrggQfUtGlTdenSRcuXLw+6bFxcnF566SW/WGpqanWkAQAAAAAAgNNQtTSwGjRooH379ql+/frKyMhQjx49gr+gy6UJEyZUx8sCAAAAAADgF6BavkIYFxen+vXrh7x8UVGRsrOzq+OlAQAAAAAAcJoL+03cT5w4oZSUFKWmpiotLU0333yzcnJywp0GAAAAAAAAokS1fIUwVA0aNNDdd9+tc845Rx6PRx9//LGee+45ffvtt1q+fLlcrsDp5OfnKz8/3/ezd/aW2+2W2+2WJDkcDjkcDnk8Hnk8Ht+y3nhRUZGMMRXGnU6nLMvyrbd0XCqePRZK3OVyyRjjF7csS06ns0yOlmVJcsoYj2RK4rIcsixH8LinSJIJIV5ck/H41ySrOHcZ/9yNKb+m4vX7ViLLESD3YPFqrimU7WQ8wWu1HMU1+cdrria32377XqB4tI8naqImaopQTcbIYVkq8nhKH7HlsKyAcefPf8zF7Sl9rC2OS1KRMSHFXQ5HcU2l4lZRUbk1Fb+3/uvxHcv9o8Xn0GqIFzNl4idvD6nsdvL8/HSHKV6DsfzXEjBuin9T6Sn98pIsU/yj56R1hBr37oPB9jHvdUSkz7mS5PFUPJ78XzZw7uG6jnC7yz9GFF/TVM/1XlVrcrsrPkaE+xq2oprKO+6VpBmea9jyaip9mA82zqTwj6dgcWPKPz/5f3ZQ2MZToHgo51zvZ4dwjqdg8dKfHQKNMyly4+nkmqSKryN85Uboc26wcRbo2sh4Ivs5t3RNbrfNrveqcA178nGissLawJo1a5bfz+PGjVObNm103333aeHChRo3blzQ591///1l4mvXrlVSUpIkKT09XS1bttT27dv1008/+ZZp3LixGjdurC1btigrK8sXb9GiherVq6cNGzYoNzfXF2/Xrp1q166ttWvX+m3szp07KzY2VhkZGX45dO/eXQUFBVq3bp0v5nQ61aNHD2VlZWnz5s2+eEJCgrp06aLMzExt27bNFy++iX17FeXsVVHO7pL1JKTLVbulirK2qyi3pCZncmO5ajWW++gWefJLanKltpAzsZ4KD22QcZfUFJPWTlZcbRUeXCtTahDH1O0syxmrggP+NRV1KL+mggMlNVmuBMWmd5EnN1PurJKaHHGpikmr+ZpC2U4Fx6TYM7vLFBWoMLOkJstyKrZ+D5mCLBUeDk9NGSfst++1b99ee/fu1e7dJTVF+3iiJmqipgjV5HKpce3a2pKZqaxSubeoU0f1kpO1Yf9+5RYWltRUr55qJyRo7Z49Kip1YdS5QQPFulzK2LXLv6YmTVTgdmvdvn0lNTkc6tGkibLy8rT54MGSmnJzy60p35OlvKKS9z3WkaxEVx3lFh1RgadkZni8M1Xxzto67s6U25TUlOCsozhnsnLc+1VkSmpKctVTjJWg7MI9MiqpqVZMAznkUlahf02pMU2Um5tb4XY6cWaiYtweNczMU06CS4dTY0tyzC/SmUfylZUco6zkGF88OdetOlkFOpIaq5yEkku+1JxC1c4p1E+145QX5/TF07IKVCvXrf114lXoKpmkX+9wnhIKPNpdL0HGsnTo530t2L6nRHuccyUps37F46ngaMXXRuG6jsjIKP8YUXCs+q73qlpTxomKjxHhvoYtr6aKjnsFx0LfTjVdU8aJkpqCHcuVEP7xFKymrKbln58iNZ4C1RTKObfgWPjHU7CaMk6Ufx0hRWY8BapJqvg6wjvOIvU5t3RN3nEW7NqoMDeyn3NL15RxwmbXe1W4hq3qraQsY076NWYVeW/iPnv2bE2ePLnC5XNzc5WcnKwpU6aU+euEXoFmYDVp0kSHDh1SSkqKpOj/DffSTfaZgTX47PJrWrQ+8r/p8dY0sF3F22npxuC1hvu3wYM62G/f+8XPGKEmaqKm6qtp+3b7zMBq2bLcmr74eKvsMgOr9yWtKtxO2595TZI9ZmA1v/UaScH3saWb7HHOlaSLO1U8npZuLP2ykZ2BNah9+ceI4msae8zAGtSh4mPEJ+vtMwPr4o7lH/dK9oPIz8Aa1KEkHGycfbrZPjOwBp9d/vnJ/7ODwjaeAsUHta/4nOv97GCHGVilPzsEGmdLNtpnBtYlnSu+jvCNMxvMwCo9zgJdGy3daJ8ZWIM62Ox6rwrXsNnZ2apTp46ysrJ8vZzKCOsMrEASEhJUp04dHT58OOgycXFxiouLKxN3uVxlvnbofdNO5t2wocaDfZ2xMnHLsgLGg+VoWQ7JqkTcETj34PEgm9vyj//8+SBoTYHWU+ncq6mmULaH38tYgWsKHK/+mkqna6d9r7LxaBhP1ERNwXKsbJyaKhH/+QTiDLBseXFXsLhlhRy3LMs//vP7F/yca8mvq+OLB86luuKBXzPw9igdd5S+tlVxUynQmgPFHVLZvtlJ66xM/ORcT/7ZtxkifM6VJO+mL288BdxUAXIMFq/Omlyu8o8RpZ9W1eu98uKh1FR6s1f62raGrmHLi1d03Ds5zUhelwc6nAc7RoRzPAWLl/fZoXj5yIynQPFQzrn+4yw84ylYPKRxFqHxFChe0fVCyOMsDDWdvLuefIzwphWpz7mlayqdqy2u9352KtewwfIPVdhv4n6yY8eOKTMzU+np6ZFOBQAAAAAAADYUtgZWXl6ejh07Vib+4IMPyhijIUOGhCsVAAAAAAAARJFq+wrhs88+q6NHj2rv3r2SpPfff993A7Bbb71VR44cUbdu3XT11VerXbt2kqRPPvlEH374oYYMGaIrrriiulIBAAAAAADAaaTaGliPPfaYdu7c6fv5rbfe0ltvvSVJmjBhgmrXrq3LL79cixcv1ssvv6yioiK1atVKM2fO1G9/+9uA36kEAAAAAAAAqq2BtWPHjgqXefXVV6vr5QAAAAAAAPALwbQnAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANiaK9IJAACA08PKHyOdQYnerSKdAQAAAKoTM7AAAAAAAABga8zAAmxk0YZIZ1BicKdIZwAAAAAAQDFmYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWXJFOAAAABLZoQ6QzKDG4U6QzAAAAwC8ZM7AAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrrkgnACB6LdoQ6QxKDO4U6QwAAAAAADWFGVgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDX+CiFOe7X2/BDpFEp0ahXpDAD8YKNjQiuOCQAAAEAomIEFAAAAAAAAW6OBBQAAAAAAAFvjK4QAgF+UlT9GOoMSvfkGIQAAABASZmABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1qqlgZWTk6MZM2ZoyJAhSktLk2VZmjNnTsBlN23apCFDhig5OVlpaWm69tpr9dNPP1VHGgAAAAAAADgNuapjJZmZmXrggQfUtGlTdenSRcuXLw+43O7du3XhhRcqNTVVM2fOVE5Ojh577DGtX79ea9asUWxsbHWkAwAAAAAAgNNItTSwGjRooH379ql+/frKyMhQjx49Ai43c+ZMHT9+XF999ZWaNm0qSerZs6cuvvhizZkzR9dff311pAMAAAAAAIDTSLV8hTAuLk7169evcLk333xTl19+ua95JUkXXXSR2rRpo/nz51dHKgAAAAAAADjNhO0m7nv27NHBgwfVvXv3Mo/17NlTa9euDVcqAAAAAAAAiCLV8hXCUOzbt09S8dcNT9agQQMdPnxY+fn5iouLK/N4fn6+8vPzfT9nZ2dLktxut9xutyTJ4XDI4XDI4/HI4/H4lvXGi4qKZIypMO50OmVZlm+9peOSVFRUFFLc5XLJGOMXtyxLTqezTI6WZUlyyhiPZErishyyLEfwuKdIkgkhXlyT8fjXJKs4dxn/3I0pv6bi9ftWIssRIPdg8WquKZTtZIxHkuX9yf8tsBw/b//qiHvkzyp+30vF3W53ufueFPp2Cha3HMXbyT9e+e0kVTyefE+ppn2vKjV5d4Vg4yzajxHUVH01BRrDkTpGSCq/Jk9kxlOguNtd8XYyxpQ57vnWU8n4z2sMKR7ofS8qKip336vKsby6azp53Ehlx5Pn56c7TPEajOW/loBxU/ybSk/pl5dkmeIfPSetI9S4d1wFOxZ4ryNq6vxUmesIj6fiY4T/y0bmnOutKdA4K5178SVN5M+5kuR2V3wsD/c1bEU1lXd+KkkzPNew5dVU+tQVbJxJ4R9PweLGlH8d4f/ZQWEbT4HioVxHFI+zyJ5zS4+z8q6NpMiNp5Nrkiq+3ivz2SGCx4jSu2uga1jjiezn3NI1ud2nz3X5yceJygpbAys3N1eSAjao4uPjfcsEenzWrFm6//77y8TXrl2rpKQkSVJ6erpatmyp7du3+/1Vw8aNG6tx48basmWLsrKyfPEWLVqoXr162rBhgy83SWrXrp1q166ttWvX+m3szp07KzY2VhkZGX45dO/eXQUFBVq3bp0v5nQ61aNHD2VlZWnz5s2+eEJCgrp06aLMzExt27bNF09NTVWtPTHKKzqqvKKSHGMdyUp01dEJ9yEVeHJK3i9nquKdtZVTeFBuU5J7grOO4pzJOla4V0Wm0BdPctVTjCNBWQW7ZFSy49WKaSCHXMoq3OVXU1GHfuXW5Nn5VUncilGtmIbKL8pRbtEhX9xlJSg5pl6N17Q290iF2ymr8LhSY5rII7eOFe7zxS05lBrbRG6Tp+Pug2VqKvAcD1hTvicrYE25RUcC1nTcnemrKSPjcLn7Xq09mSFvp2A1pcQ2UaEnN2BNldlOOrtXheOp4NjP60ltIWdiPRUe2iDjLqkpJq2drLjaKjy4VqbUCSSmbmdZzlgVHPAfT7FndpcpKlBhZsm+Z1lOxdbvIVOQpcLDJePJciUoNr2LPLmZcmdtU8aJn9+X1FS1b99ee/fu1e7du33LR/sxgpqqrybJhDyeavoYIancmjz/y/TFK3ssr+5jRMbxkguOYNsp3+Mqc9yTSo7lOe79ZY/lVoKyC/dUqaZA22nDhtxy972qHMuru6bc3NwKx9OJMxMV4/aoYWaechJcOpxa8odv4vOLdOaRfGUlxygrOcYXT851q05WgY6kxionoeSSLzWnULVzCvVT7TjlxTl98bSsAtXKdWt/nXgVukom6dc7nKeEAo9210uQsSwd+vmYEOwYocRTP5Z7OeJSFZPWXkU5e1WUU3KMcCaky1W7pYqytqsot2TfcyY3lqtWY7mPbpEnv2S7Ztav+BhRcLRmz0+VqSkjo/zjXsExe5xzJSnjRMXH8lC3Uzhqquj85L2mqa59ryo1ea9ppODnXCWEfzwFqymrafnXEZEaT4FqCuU6ouBY+MdTsJoyTpR/bSRFZjwFqkmq+HrPO87COZ6C1eQdZ8GuYQtzIzOeAtWUceL0uS73TkY6VZYp3RqrBt6buM+ePVuTJ08uE3/llVd07bXX+j3n7rvv1qOPPqq8vLyQZ2A1adJEhw4dUkpKiqTon4mwZsl22/w2uPclrcutaeUnWwPkWP2zlUKJ9xh0ll800PZYs2Rb0FrDPQOr50Utyt33Vi36sUZmIpxKvM+QNhWOp6UbvSuJ/G+DB3Xw1sNsJWoqv6aVn/wgu8zA6jOkdbk1rV78o9/yNTVbKZR4z4ual8nx5O20Zsl228zA6nVxy3L3vS8+3hpkPeGfgdX7klYVjqftz7wmyR4zsJrfeo2k4MeCpZvsMwPr4k4VHyN85zIp7LMrTq5pUPvyj3tLNwavNdwzRgZ1qPhY/sl6+8zAurhj+eenkv0g8jOwvNc0UvBx9ulm+8zAGnx2+dcRi9bbZwbWoPYVX0cUjzN7zMAa1KH8a6MlG+0zA+uSzhVf75X57BDBGVilx1mga9ilG+0zA2tQh9Pnujw7O1t16tRRVlaWr5dTGWGbgeX96qD3q4Sl7du3T2lpaQGbV1LxrK1Aj7lcLrlc/iV437STeTdsqPGT13sqccuyAsaD5Vj8VUIrQDzwrcqqK37yaxbnEbymQOsJnnvN1hTK9vB/bmVyrP6aSucVbN8LdTuVF6+umioaTyenajmC1OQIcqixQo9blhUk7pAsh07eFYLlHs3HCGqqnpqC7e8/Pxry8tV1jCivpsDH28gcI0LZrt7zR02dn8qLn5y79321+znXm0tF48lR+tpWkhXg14/B4g6pbN/spHVWJn5yrif/bHlLPIVjeZXjJ52HvJu+vGNEwE1VjeenysRdrvKPe6WfFslzriS/827wcRbadqo4Xj01lXccK3NNU8V9r+J48NwDnXaDns/COJ6Cxb1jPtj1QmW2X03XFMp1hP84C894ChYPaZxFaDwFild0XRfyOAtDTSfvricfI7xphXs8lcRLcimda7RflwfLP1Rhu4l7o0aNlJ6eXnaauaQ1a9aoa9eu4UoFAAAAAAAAUSRsDSxJGjVqlD744APt2lVy/4elS5dqy5YtGjNmTDhTAQAAAAAAQJSotq8QPvvsszp69Kj27t0rSXr//fd9NwC79dZblZqaqnvvvVcLFizQgAEDdNtttyknJ0ePPvqozj77bE2ZMqW6UgEAAAAAAMBppNoaWI899ph27tzp+/mtt97SW2+9JUmaMGGCUlNT1aRJE3322We644479Lvf/U6xsbG67LLL9Ne//jXo/a8AAAAAAADwy1ZtDawdO3aEtFzHjh31ySefVNfLAgAAAAAA4DQX1ntgAQAAAAAAAJVFAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC25op0AgCA6LZoQ6QzKDG4U6QzAAAAAFATaGABOGW19vwQ6RRKdGpV7sM0WQAAAAAgevEVQgAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANiaK9IJAADKWrQh0hmUGNwp0hkAAAAA+KVjBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbM0V6QQAIBxq7fkh0imU6NQq0hlUK95bAAAAADWNGVgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNVekEwAAlFVrzw+RTqFEp1aRzgAAAADALxwzsAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrYW1gLV++XJZlBfy3atWqcKYCAAAAAACAKOGKxItOmzZNPXr08Iu1atUqEqkAAAAAAADA5iLSwOrbt69Gjx4diZcGAAAAAABAlInYPbCOHTsmt9sdqZcHAAAAAABAlIhIA2vKlClKSUlRfHy8BgwYoIyMjEikAQAAAAAAgCgQ1q8QxsbGatSoUbr00ktVt25dbdy4UY899pj69u2rL774Qt26dQv4vPz8fOXn5/t+zs7OliS53W7fLC6HwyGHwyGPxyOPx+Nb1hsvKiqSMabCuNPplGVZZWaHOZ1OSVJRUVFIcZfLJWOMX9yyLDmdzjI5WpYlST/nYfzWY1kOGeORv+Ib31dHvJj/a3rfj2A1nbye4hyD5V6zNYWynYqfG7jWU8v91Gtyu93l7nsl+fqvJ1DuNV2TpArHU0mu1bPvVaUm774QbJwZ44nIeAoUd7vdFR4jKjfOaramisaZ93nhHk+B4t5cyzuWB97fI3OMkFTB+cnjt3y4xlOgeOn3Mtg51xgT9vEULPeioqKg59xg+0GkjhEnHwukstcRnp+f7jDFazCW/1oCxk3xbyo9pV9ekmWKf/SctI5Q46XHmVT2esEY58//4x+3HMU1+cctWQ5n8ft18v4eKG45SrZToLinSKXfY4+n4us9/5cNnHuweHXX5HaXfw1bfEkTuFZZxTUZz0nfcKihmtzu4Odcb+6hbqdw1VTedXlJmtWz71WlptKnrmDjTAr/eAoWN6b8z0/Fyweu1S8chmNEKJ8Ji8dZeMdTsLjbXf7nXCly4+nkmqTg59wy4yyM4ylYvPTuGui63HgiM54C1eR213w/orxjeXX2WKr6LbywNrD69OmjPn36+H4ePny4Ro8erc6dO2v69On6+OOPAz5v1qxZuv/++8vE165dq6SkJElSenq6WrZsqe3bt+unn37yLdO4cWM1btxYW7ZsUVZWli/eokUL1atXTxs2bFBubq4v3q5dO9WuXVtr167129idO3dWbGxsmdli3bt3V0FBgdatW+eLOZ1O9ejRQ1lZWdq8ebMvnpCQoC5duigzM1Pbtm3zxVNTUyXFKN+TpbyikhxjHclKdNVRbtERFXhyfPF4Z6rinbV13J0ptynJPcFZR3HOZOW496vIFPriSa56irESlF24R0YlO16tmAZyyKWswl1+NRUVtSi3ptLLO60Y1YppqALPceUWHfLFXVaCkmPq1XhNoWynrMLjSo1pIo/cOla4zxe35FBqbBO5TZ6Ouw+GpaaMjMPl7nuSQt5ONV2TpArHU1bh8ZC2Uzhqysg4XLyO1FS1b99ee/fu1e7du33L5xZZERlPgWpauzarwmNE6fWEazwFq6mi415W4fGIjKdANXn3g/KO5ZIJ+3gKVpOkcs9PWYWZvng4x1OgmkrvB8HOufkeV9jHU7CaNmzIDXrObd++vW3OuakxTZSbm1vhdcSJMxMV4/aoYWaechJcOpwaW5JjfpHOPJKvrOQYZSXH+OLJuW7VySrQkdRY5SSUXPKl5hSqdk6hfqodp7w4py+ellWgWrlu7a8Tr0JXyST9eofzlFDg0e56CTKWpUM/7wvBro2U2F2mqECFmSU1WZZTsfV7yBRkqfBwyXHPciUoNr2LPLmZcmeVbCdHXKpi0tqrKGevinJKjuXOhHS5ardUUdZ2FeWW7HvO5MZy1Wos99Et8uSXbNfM+hVf7xUcLTlGxNTtLMsZq4ID/jXFnhmemjIyyr+GLTgmuVJbyJlYT4WHNsi4S2qKSWsnK662Cg+ulTE1X1PGieDnXO8xItTtFI6aKrouLzgW+naq6ZoyTpTUFOyzhhLCP56C1ZTVtPzPT5EaT4FqCuUzYcGx8I+nYDVlnCj/c64UmfEUqCYp+DnXe4zwjrNwjqdgNXnHWbDP7oW5kRlPgWrKOFHz/YjyjuXV2WPxTkY6VZYp3RqLkKuvvlpvvfWWTpw44esglhZoBlaTJk106NAhpaSkSIr+GVhrlmy3zW+De1/SutyaVn6yNUCOkZmB1WPQWX7RQNtjzZJtQWsN94yRnhe1KHffW7XoR9vMwOozpE2F46n4vQ1ca0Xx6q6p50Utfo4FHmdrlmyzzQysnhe1qPAYsWrRD5V4D2q2pp4XNfeLnjzOvPuBHWZgefeD8o7lKz/5ocxrRuoY0WdI63LPT6sX/xjSexAo9+quqfR+EOycu2bJdtvMwOp1cctyf8v4xcdbg6wn/MeI3pe0qvA6Yvszr0myxwys5rdeIyn4NdDSTfaZgXVxp4qv95ZuLP2ykZ2BNah9+dewSzcGrzXcM0YGdaj4t/afrLfPDKyLO5Z/XV6yH0R+BtagDiXhYOPs0832mYE1+OzyPz8tWm+fGViD2lf8mbB4nNljBtagDuV/zl2y0T4zsC7pXPHMHt84s8EMrNLjLNB1+dKN9pmBNajD6TMDKzs7W3Xq1FFWVpavl1MZEfkrhCdr0qSJCgoKdPz48YBFxMXFKS4urkzc5XLJ5fIvwfumnSxQY6y8+MnrPZW4ZVkB48FyLP4qoRUgHvhWZdUVP/k1vV9pDFZToPUEz71mawple/g/tzI5Vn9NpfMKtu+Fup3Ki1dXTRWNp5Nzreq+V168otwrOhZ4cwj3eAoU9+Za3jGicuOsZmuqaJyVfl44x1Og+Mm5BjuORWI8Bcu9vPNT4P0gMseIUM5n3vNHOMeT/2uXxL3vq93Pud5cKrqOcJS+tpVkBfj1Y7C4QyrbNztpnZWJVzTOLG+JVpDxFzDukILt75WJO/zHk3fTl3e9F3BTBcgxWLw6a3K5ysZL5176aSfXWhIPPfdg8VBqKr3Zg4+z0LZTxfHqqam849jJaVZ136s4Hjz3QKfdoOezMI6nYHHvmA92vVCZ7VfTNYXymdB/nIVnPAWLhzTOIjSeAsWD5VjpcRaGmk7eXU8+RnjTCvd4KomX5FI615rsR1Q2fio9lmD5hypif4WwtG3btik+Pl7JycmRTgUAAAAAAAA2E9YGVunvTXp9++23eu+99zR48OCAXT0AAAAAAAD8soX1K4Rjx45VQkKC+vTpo3r16mnjxo164YUXlJiYqIcffjicqQAAAAAAACBKhLWBdeWVV2revHl6/PHHlZ2drfT0dI0cOVIzZsxQq1atwpkKAAAAAAAAokRYG1jTpk3TtGnTwvmSAAAAAAAAiHLcdAoAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAws</t>
-        </is>
+      <c r="D3" s="2">
+        <v>45687</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>32.66228956634455</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45687</v>
+      </c>
+      <c r="H3">
+        <v>17.51022447277154</v>
+      </c>
+      <c r="I3">
+        <v>2.338072152989103</v>
+      </c>
+      <c r="J3">
+        <v>32.66228956634455</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>pod_tbs</t>
-        </is>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>45639.5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9.478904369302354</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>45639.5</v>
-      </c>
-      <c r="H4" t="n">
-        <v>4.406639723296744</v>
-      </c>
-      <c r="I4" t="n">
-        <v>-0.200051486837198</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9.478904369302354</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACZbklEQVR4nOzdeXhU9dn/8c+ZmWwkJJFAEEgUEhQCCC6ABWVRFAGVtu4rSPVxaZX607ZWq0WsirY+blh3K1ahFrU+xVaURahU3FIDiEJDJVAgbEnIhIRsM3N+f4SZzCQzmQmZzBzg/bour5Y7Z87c91m+58yd75wYpmmaAgAAAAAAACzKFu8EAAAAAAAAgLbQwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAgTvr27SvDMAL+S0pK0nHHHafLL79cq1atikke1113nQzD0Lx582Lyfp3Fuz23bNkS71SOeN7jFQAAIFZoYAEAEGdnnHGGpk+frunTp2vy5MnyeDxauHChxo0bp8cffzze6VnC4dRki2Ujbd68eTIMQ9ddd12nvxcAAEA8OeKdAAAAR7sbbrghoAFRV1enm266SX/84x/1i1/8QhdccIFOPPHE+CV4mFi+fLkaGxvVp0+feKcCAACAKGMGFgAAFpOcnKzf//73Sk1Nldvt1l/+8pd4p3RYyM/P18CBA5WQkBDvVAAAABBlNLAAALCgtLQ0DRgwQJJafRXtww8/1AUXXKDs7GwlJiaqd+/euvzyy1VYWBhyfRUVFbr99tt1/PHH+56zdeutt6qiouKQ8rv//vtlGIbuv/9+bd26VdOmTVOvXr2UnJysE088Uffff79qa2tbva6xsVFvvPGGrr76ag0cOFDp6elKSUnRgAEDNHPmTJWWlgYsv2XLFhmGoddee02SNGPGjIBnht1///2+ZcN9de/tt9/WpEmT1KNHDyUmJqpPnz665ppr9O2337Za1vu+ffv2lWmaevHFF3XaaacpNTVVGRkZmjhxoj799NOA13i/zrd161ZJUr9+/QJyXblypW/ZZcuW6cILL1TPnj2VkJCgY445RieccIKuueYaffzxx5HsAvXt21czZsyQJL322msB7zV+/PiAZQ8cOKBHHnlEp556qrp27aouXbpo8ODBuvfee7Vv376I3i+Ul156ybdtMjMzNWXKFH322Wchl3e5XHr55Zc1fvx4devWTUlJSerXr59uueUWbdu2rd3v/69//UuXX365cnJylJiYqPT0dOXl5eniiy/WX//615Cvufrqq3XccccpKSlJ3bp103nnnaf3338/anmvXLnSty8aGxv16KOPavDgwUpJSVFWVpYuuugibdiwod31AgBwtOIrhAAAWFRVVZUkKSkpyRe777779OCDD8owDI0ePVrHHXecNmzYoIULF+qdd97Riy++qB/96EcB69m9e7fGjBmjTZs26ZhjjtEFF1wgj8ej+fPn64MPPtDgwYMPOceSkhKddtppcjgcGjt2rGpra7VixQrNnj1by5Yt07Jly5ScnByQy7XXXquMjAwVFBRo6NChqqmp0Zo1azR37ly9+eabWr16tfr37y+pqZE3ffp0/fOf/9R3332nM844w/czSTr55JPD5uhyuXT11Vdr4cKFSkpK0mmnnaY+ffqouLhY8+fP11/+8hf95S9/0aRJk4K+fsaMGVqwYIHGjBmjCy64QGvWrNHSpUv18ccf6x//+IdOP/10SVL//v01ffp0vf3226qpqdHFF1+stLQ033qOPfZYSU3NJm/jaeTIkTrrrLNUW1ur7du3680331T37t01duzYsHVdcskl+uyzz/TJJ58oPz9fZ555pu9nAwcO9P3/iooKTZgwQWvWrFF6errOPvtsJSQk6B//+IceeughLViwQB999JH69u0b9j1buuOOO/Tkk0/qjDPO0Pe//319/fXXWrx4sZYuXaqFCxfqhz/8YcDy+/fv19SpU7Vy5UqlpaXptNNOU48ePfT111/r+eef11tvvaWlS5fqlFNOiej9ly9frsmTJ6uxsVHDhg3TqFGj5Ha7tWPHDv3973+X2+3W97///YDXPPXUU7rjjjvk8Xh08skn6/TTT9euXbu0cuVKLVmyRLNnz9avf/3rqOXd2NioKVOmaPXq1Ro7dqwKCgr0xRdf6N1339WKFStUVFR0SNseAICjjgkAAOLi+OOPNyWZr776aqufrV271rTZbKYk8w9/+INpmqa5ePFiU5KZnJxsLlmyJGD5l19+2ZRkJiQkmOvXrw/42SWXXGJKMseMGWNWVlb64uXl5ebpp59uSgqZRyizZs3yve773/++eeDAAd/Ptm3bZp544ommJPOXv/xlwOuqqqrMv/71r2Z9fX1AvKGhwbz77rtNSeaUKVNavd/06dPD5ujdniUlJQHxe+65x5Rknn766ebmzZsDfvbWW2+ZdrvdPOaYY8x9+/b54iUlJb76jj/+ePPf//6372cul8v80Y9+ZEoyJ06cGHEeXv369TMlmatWrWr1s927d5tfffVVyBpbevXVV01J5vTp00Muc/nll/vqLysr88X3799vTp482ZRkjh49OuL3NE3Tt21SUlLM5cuXB/zst7/9rSnJzMjIMHfv3h3ws6uuusqUZF5wwQWtfvbEE0+YkswTTjjBdLlcEeVx1llnmZLMN954o9XPKisrzU8//TQg9sEHH5iGYZjdu3c3//GPfwT8bN26dWZOTo4pyVy5cmWH816xYoVvO51yyinmzp07fT+rra01zzvvPFOSeeONN0ZUKwAARzsaWAAAxEmwBlZlZaX597//3czPzzclmb179zarq6tN0zTNCRMmmJLMO+64I+j6LrjgAlOS+T//8z++2H//+1/TZrOZhmGY33zzTavXFBUVdaiBlZKSEvDB3Ou9994zJZnp6elmbW1txOvt3bu3abPZzKqqqoD4oTawysvLzZSUFDM5Odncvn170Nf9+Mc/NiWZc+fO9cX8G1iLFi1q9ZqdO3eaksykpCSzoaEhbB7+unTpYmZkZISsoz3CNbC2bt3q2/9r165t9fPt27ebycnJpiTzk08+ifh9vdvm9ttvD/rz4cOHm5LMhx56yBf79ttvTcMwzN69e7fav15TpkwxJZnvvfdeRHkMGjTIlGRWVFREtLy3Yfv2228H/fnChQtNSebFF1/c4by9DSzDMMw1a9a0es1nn31mSjLz8vIiyh0AgKMdz8ACACDO/J/rlJmZqfPPP1/fffed8vPz9f777ys1NVUul0uffPKJJAX8xUJ/119/vSRpxYoVvtjHH38sj8ejU089VYMGDWr1mpNPPllDhw495NwnTpzo+2qcvwsuuEBZWVmqqqrSV1991erna9eu1eOPP67bbrtNP/rRj3Tdddfpuuuuk8vlksfj0X/+859DzsnfihUrVFtbqzPOOCPkXyf0Pi9q9erVrX7mcDiCfrXw2GOP1THHHKP6+nqVl5e3K6eRI0fK6XRq2rRp+te//iWPx9Ou17eHd/+fcsopQfdznz59dN5550kKPG4iNX369KDxadOmSVLAc7/ef/99maapyZMnq2vXrkFf19a+CGbkyJGSpKuvvlr//Oc/5XK5Qi5bVlamL774QikpKbrwwgsjfv+O5n3cccdp2LBhreIFBQWSpB07doTMGQAANOMZWAAAxJn/c50SExOVnZ2t733ve5o0aZIcjqZLdXl5uerq6iQ1PRw8mPz8fEmBH4i3b9/e5mu8P1u3bt0h5d7Wevv27avy8nJfDpJUU1Oja6+9Vu+++26b6/U+/6ujNm/eLKnpWUmGYbS57N69e1vFevXqFfKvGqanp2vfvn2+/RKpZ599VhdccIFef/11vf766+ratatGjBihs88+W9dee62OO+64dq2vLd5joa39FOy4iVSo9Xrj/vveuy9eeeUVvfLKK22uN9i+CGbOnDlat26dFi9erMWLFyslJUWnnnqqxo8fr6uvvtrXJJKantdmmqZqa2sDnisX7v07mneo/Zmeni5Jqq+vb3OdAACgCQ0sAADi7IYbbgg5q+pIYJqm7//ffffdevfddzVw4EA98sgjGjFihLp3767ExERJ0ujRo/Xpp58GvKYjvLOb+vfvrzPOOKPNZf0ffO5ls0V/snpBQYH+/e9/a8mSJfroo4+0evVqrVq1Sh999JEeeOABvfLKK7rmmmui/r7x4L8fvfvi5JNPDjojyZ/3wfjhHHvssSosLNQ//vEPLVu2TJ988ok+//xzffLJJ3r44Yc1Z84c3XXXXQHvn5aWposvvjjiGjqad2ccQwAAHI1oYAEAcBjIyspSUlKS6uvrtXnz5qBfB/POFPH/qpz3/2/ZsiXkutv6WTglJSVh15uTk+OLLVy4UJL05z//OWgNmzZtOuRcgsnNzZUkDRgwQPPmzYvqujvC4XBoypQpmjJliqSmGWePP/64Zs+erZtuukk//OEPlZqa2uH38e5/77ERTLDjJlIlJSVB/xJksH3v3RdnnHGGnnnmmXa/VyiGYWj8+PG+r/HV1dVp3rx5+slPfqJ77rlHl1xyifLz833vbxiG/vCHP0TcWOqsvAEAQPvwKyEAAA4DDodDZ555piSFbMT84Q9/kCSdddZZvtjYsWNlGIa++uorbdy4sdVr1q5de8hfH5SkJUuWaM+ePa3i77//vsrLy9W1a1eddtppvnhFRYUk6fjjj2/1mg8//FBlZWVB38c7Q6utZxwFM2HCBCUmJmrlypVB8+wMh5Jrenq67r//fmVmZurAgQMqLi6OynuNHTtWNptNa9as0dq1a1v9fOfOnfrggw8kBR43kXr99dfbjHubSpI0efJkSdKiRYva/bXL9khOTtbNN9+soUOHyuPx+I7v3r17a+jQodq/f7+v5kjEKm8AANA2GlgAABwm7rzzTknSc889p+XLlwf8bN68eVq0aJESEhL005/+1Bc/7rjj9MMf/lAej0e33HJLwLOl9u3bpx//+Mcd+rpebW2tbrnlFtXW1vpipaWlvlxvvvlmJScn+37mfSbR3LlzA9bz73//WzfffHPI9/HO5Pnmm2/alV/Pnj112223qaamRhdeeKG+/vrrVsvU19dr0aJFQRt8h6KtXA8cOKDHH3886LOSVq1apcrKStnt9oCZS5G817fffhv058cdd5wuvfRSmaapm266KeCB8zU1NbrxxhtVV1en0aNHa/To0RG9p7/nnnsu4EHtkvTEE0/oiy++UNeuXX1/WECSTjnlFF188cXatm2bLrrooqAz/2pqajR//nzt3r07ovd/7LHH9N///rdVfOPGjb7ZfP7N0gcffFBS0x9OeO+991q9zjRNff7551qyZEmn5g0AANqPrxACAHCYmDx5su699149+OCDOvfcc3XGGWfouOOO08aNG/XVV1/Jbrfr+eef1+DBgwNe9/vf/15r167VypUr1a9fP40fP16maWrFihXKysrS1KlTtWjRokPKadq0afrb3/6mvLw8jRkzRnV1dfroo49UU1OjUaNGafbs2QHLz5o1S5dcconuu+8+LVy4UIMHD9aePXu0atUqjRkzRr179w76l9x+8IMfaPbs2Xr66ae1fv165ebmymazaerUqZo6dWqbOT7yyCPauXOnFixY4HuOUV5enhwOh7Zv3641a9aopqZGixcvDvocrPa6+OKLtWLFCl1zzTWaOHGijjnmGEnSz3/+c/Xs2VN33nmnfv7zn+ukk07SCSecoISEBG3ZskWfffaZJOlXv/qVevToEdF7fe9731Pv3r1VVFSkU089VSeddJISEhI0YMAA/fznP5fUtP83btyozz//XPn5+TrrrLPkcDj0j3/8Q3v37lW/fv00f/78Q6r1pptu0tlnn60xY8aoT58+Wr9+vb7++mvZ7Xb94Q9/aPUXKl999VVVVlZq8eLFGjBggIYNG6Z+/frJNE1t2bJFa9euVUNDgzZs2KCePXuGff8HH3xQP//5zzVw4EAVFBQoJSVFpaWlvr9IOG3aNJ166qm+5S+88EI99dRTuvPOOzV16lT1799fAwYMUEZGhvbu3au1a9dqz549uuuuuzRx4sROyxsAABwCEwAAxMXxxx9vSjJfffXVdr1u8eLF5pQpU8ysrCzT4XCYxx57rHnppZean3/+ecjXlJWVmbfddpuZk5NjJiYmmjk5OebNN99s7t2715w+fXq785g1a5YpyZw1a5a5efNm88orrzR79uxpJiYmmv379zd//etfmzU1NUFf+/HHH5sTJkwwu3fvbnbp0sUcMmSI+dBDD5n19fXmuHHjTEnmihUrWr3u3XffNc844wyza9eupmEYvvf38m7PkpKSoO/7/vvvmxdddJHZp08fMyEhwczMzDQLCgrMK664wlywYEFAviUlJaYk8/jjjw+5DUK9n9vtNufMmWMOHjzYTE5ONiX5ampsbDSff/5588orrzQHDhxoZmRkmCkpKWZ+fr558cUXm8uXLw/5fqF8/fXX5tSpU80ePXqYNpvNlGSOGzcuYJmamhpzzpw55sknn2x26dLFTE5ONgsKCsx77rnHrKioaPd7emsyTdN87rnnzJNPPtlMSUkx09PTzUmTJpmffPJJyNe63W5zwYIF5pQpU8yePXuaCQkJZlZWljlkyBBzxowZ5rvvvms2NDRElMcbb7xhzpgxwxwyZIjZrVs3MykpyTz++OPNyZMnm++++67p8XiCvu7rr782b7zxRvOEE04wk5OTzS5duph5eXnmeeedZz799NPmjh07Opz3ihUrgu6LUNsRAAC0zTDNKP2ZHwAAcNS4//77NXv2bM2aNUv3339/vNMBAADAEY5nYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJ4BhYAAAAAAAAsjRlYAAAAAAAAsDQaWAAAAAAAALA0R7wT8PJ4PCotLVXXrl1lGEa80wEAAAAAAECUmKap/fv3q3fv3rLZ2j+fyjINrNLSUuXm5sY7DQAAAAAAAHSSbdu2KScnp92vs0wDq2vXrpKaCklPT49zNgAAAAAAAIiWqqoq5ebm+vo/7WWZBpb3a4Pp6ek0sAAAAAAAAI5Ah/rYKB7iDgAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLs8xfIQQAAAAAANZmmqbcbrdcLle8U4FFOBwO2e32Q/7rghG/T6euHQAAAAAAHPZM01RlZaX27t0rt9sd73RgMXa7XdnZ2crIyOi0RhYNLAAAAAAA0KZdu3apsrJS6enpSk9Pl8Ph6PQZN7A+0zTlcrlUVVWlnTt3qra2Vr169eqU96KBBQAAAAAAQnK73XI6nerRo4e6d+8e73RgQV27dlVSUpLKysqUnZ0tu90e9ffgIe4AAAAAACCkxsZGmaap1NTUeKcCC0tNTZVpmmpsbOyU9dPAAgAAAAAAYfGVQbSls48PGlgAAAAAAACwNBpYAAAAAAAACOq6665T3759450GDSwAAAAAAHD0mjdvngzDCPnfZ599Fu8Uw/r22291//33a8uWLfFOpdPwVwgBAAAAAMBR74EHHlC/fv1axfv37x+HbNrn22+/1ezZszV+/HhLzJbqDFFpYG3atEn33Xef/vnPf6qiokLHHXecrrrqKv3sZz9Tly5dovEWAAAAAADAgpasj3cG0sQhHV/H5MmTNXz48I6vCJ2iw18h3LZtm0aOHKnPPvtMt956q5588kmNGjVKs2bN0pVXXhmNHAEAAAAAAOJm1qxZstlsWr58eUD8xhtvVGJiotauXStJWrlypQzD0J///Gfdc889OvbYY5WamqqpU6dq27Ztrdb7+eefa9KkScrIyFCXLl00btw4ffLJJ62W27Fjh66//nr17t1bSUlJ6tevn2655RY1NDRo3rx5uvTSSyVJZ511lu+rjytXrvS9fvHixRozZoxSU1PVtWtXnX/++frmm29avc///d//aciQIUpOTtaQIUP07rvvdmSzRVWHZ2C9/vrrqqys1D//+U8NHjxYUtMO9Hg8+uMf/6h9+/bpmGOO6XCiAAAAAAAAncXpdKqsrCwgZhiGsrKydO+99+q9997T9ddfr6+//lpdu3bVhx9+qJdeekm/+c1vNGzYsIDXPfTQQzIMQ3fddZf27NmjJ598Uuecc47WrFmjlJQUSdJHH32kyZMn67TTTvM1yF599VWdffbZWrVqlUaOHClJKi0t1ciRI1VZWakbb7xRAwcO1I4dO/T222/rwIEDGjt2rGbOnKmnn35a99xzjwoKCiTJ97+vv/66pk+frvPOO0+PPvqoDhw4oOeee05nnnmmioqKfF85XLJkiS6++GINGjRIc+bMUXl5uWbMmKGcnJzO3OwR63ADq6qqSpLUs2fPgHivXr1ks9mUmJjY0bcAAAAAAADoVOecc06rWFJSkurq6pSQkKA//vGPOu2003THHXfod7/7na6//noNHz5cv/zlL1u9rqKiQhs2bFDXrl0lSaeeeqouu+wyvfTSS5o5c6ZM09TNN9+ss846S4sXL5ZhGJKkm266SYMHD9a9996rJUuWSJLuvvtu7dq1S59//nnAVxwfeOABmaapzMxMjRkzRk8//bTOPfdcjR8/3rdMdXW1Zs6cqRtuuEEvvviiLz59+nQNGDBADz/8sC9+1113qWfPnvrnP/+pjIwMSdK4ceM0ceJEHX/88R3cuh3X4QbW+PHj9eijj+r666/X7NmzlZWVpdWrV+u5557TzJkzlZqaGo08AQAAAAAAOs3vf/97nXjiiQExu93u+/9DhgzR7Nmzdffdd2vdunUqKyvTkiVL5HC0bq1MmzbN17ySpEsuuUS9evXS+++/r5kzZ2rNmjXatGmT7r33XpWXlwe8dsKECXr99dfl8XgkNX2t78ILLwz6fC5v4yuUpUuXqrKyUldeeWXA7DK73a7TTz9dK1askCTt3LlTa9as0S9/+Utf80qSzj33XA0aNEg1NTVtvk8sdLiBNWnSJP3mN7/Rww8/rEWLFvniv/rVr/Tggw+GfF19fb3q6+t9//bO5HK5XHK5XJIkm80mm80mj8fj23H+cbfbLdM0w8btdrsMw/Ct1z8uSW63O6K4w+GQaZoBccMwZLfbW+UYKk5N1ERN1ERN1ERN1ERN1ERN1ERN1HQ41eRyuWSapu/9/fNoZkjqzHjb/FMyDCNojqHiXiNGjAhoEnmX93/Nz372M7355pv64osv9NBDD6mgoMD3c//19+/fPyDujW3ZskWmaaq4uFhS00yoUCorK9XQ0KCqqioNGTKkzZr8941pmr64933OPvvsoO+Rnp4u0zS1devWVnl71z9gwAB99dVXreIt8/H+27+vIzUfey2P1faKyl8h7Nu3r8aOHauLL75YWVlZ+vvf/66HH35Yxx57rG699dagr5kzZ45mz57dKl5UVOSbtdWjRw/l5+erpKREe/fu9S2Tk5OjnJwcFRcXy+l0+uJ5eXnKzs7W+vXrVVtb64sPHDhQmZmZKioqCjgphw4dqsTERBUWFgbkMHz4cDU0NGjdunW+mN1u14gRI+R0OrVx40ZfPCUlRcOGDVNZWZk2b97si2dkZKigoEClX32l7X459khLU35WlkrKy7W3urq5powM5WRmqnjPHjn9cs/LylJ2WprWl5aqtrGxuabsbGWmpKho2za5/Qa9ob16KdHhUGGLh8MNz81VQ05OdGoqLdX27dubazoS9hM1URM1URM1URM1URM1URM1URM1hawpOTlZ9fX1SklJUWNjoxoaGnzLu1xJcjgS5HK5AnJxOByy2x1qbGwMaNZ54w0NDQFNkISEBNls9lbxxMREGYYRMAlGavp6n2maamhoUE1NU3PEMAylpqbK7Xarrq7Ot6zNZlOXLl3kcrkC1uM/w6q2ttY308jhcPhq9m+8bN26VZs2bZIkrVmzxrd8UlKSEhISfOuur69XTU2NkpOT5XA4dODAAbndbnk8HtXU1Pi204MPPqihQ4f61p+cnCyPx6OGhgYZhqEDBw74fhZJTXV1daqrq/PtJ+/yL730knr37q3ExEQ1NDT43t/haNo/Xt68/WvyNk+9cf+agjW11q8P/LOU3mOvqKhIHWGYbbUfI/Dmm2/qRz/6kYqLiwMe7DVjxgwtXLhQ//3vf5WVldXqdcFmYOXm5qq8vFzp6emSDs/OdKv4pk3y+Od4ME+PxyOP37pthiGbYcjt8QT0mkPF7Qf/qoDL47+WprgkuVvsVrthSP378xsEaqImaqImaqImaqImaqImaqImampXTXV1dfrvf/+rfv36KSUlpdXMm6XfSPGegXXuYL81tHMG1muvvaYZM2boiy++CDoDy8vj8Wjs2LHavHmzZsyYoTlz5ujtt9/WRRdd5Ft+xYoVOvvss/XLX/5SDz/8sC/u8XiUk5OjoUOHavHixfryyy91+umn6/nnn9eNN94Ysi6Px6Nu3brprLPOCvoXAb05vvPOO7r00kv10Ucfafz48b74W2+9pcsvv1wffPCBJk6cGHIb7Nq1S71799Zdd92lOXPmBKx/8ODBqqmpUUlJSZvbsq6uTlu2bFFubq6Sk5N9ce+xt2/fPmVlZcnpdPr6Pu3R4QbW2LFj5Xa7W/2Zx3fffVcXXXSRli5dGvRBaC1VVVUpIyPjkAuxrP/8J94ZNOvfP94ZAAAAAAAOM3V1dSopKVG/fv0CGhNeS9YHeVGMTRxy6K+dN2+eZsyYoS+//DLoc6a8HnvsMf385z/XokWLdP7552vMmDH6z3/+o2+++Ubdu3eXJK1cuVJnnXWW+vTpE/AQ97feekuXXXaZnnzySf30pz+Vx+PRiSeeKJvNpq+++kppaWkB77V371716NFDUtPXDN94441WD3GX5Pu64AcffKDJkyfr3Xff1Q9+8APfz72ThU455RQtXbpUCQkJId/nlFNO0e7du7Vhwwbfc7CWLl3qe4j7li1b2tyO4Y6TjvZ9OvwVwt27d+uYY45pFfdOQevodxwBAAAAAAA62+LFiwO+Suk1evRo1dfX67777tN1112nCy+8UFJT4+vkk0/Wj3/8Yy1cuDDgNd26ddOZZ56pGTNmaPfu3XryySfVv39//c///I+kppl1L7/8siZPnqzBgwdrxowZ6tOnj3bs2KEVK1YoPT1d7733niTp4Ycf1pIlSzRu3DjdeOONKigo0M6dO/XWW2/pn//8pzIzM3XyySfLbrfr0UcfldPpVFJSks4++2xlZ2frueee07XXXqtTTz1VV1xxhXr06KH//ve/+vvf/64zzjhDzzzzjKSmRz2df/75OvPMM/WjH/1IFRUVmjt3rgYPHqxqv0cgxUuHG1gnnniilixZouLi4oCn9f/pT3+SzWYL+C4nAAAAAACAFf36178OGn/55Zf1wgsvqHv37nryySd98RNOOEFz5szRT3/6Uy1cuFCXXXaZ72f33HOP1q1bpzlz5mj//v2aMGGCnn32WXXp0sW3zPjx4/Xpp5/qN7/5jZ555hlVV1fr2GOP1emnn66bbrrJt1yfPn30+eef67777tP8+fNVVVWlPn36aPLkyb71HXvssXr++ec1Z84cXX/99XK73VqxYoWys7N11VVXqXfv3nrkkUf0u9/9TvX19erTp4/GjBmjGTNm+N5n0qRJeuutt3Tvvffq7rvvVn5+vl599VX99a9/1cqVK6O0lQ9dh79C+PHHH+vss89WVlaWbr31VmVlZelvf/ubFi9erBtuuEEvvfRSROvhK4QxwFcIAQAAAADtFO6rYWjm/QrhW2+9pUsuuSTe6cSU5b9COHbsWK1evVr333+/nn32WZWXl6tfv3566KGH9Itf/KKjqwcAAAAAAMBRrsMNLEkaOXKk3n///WisCgAAAAAAAAhgi3cCAAAAAAAAQFuiMgMLAAAAAADgaDd+/Hh18FHjCIEZWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAA4Kg1b948GYah5ORk7dixo9XPx48fryFDhsQhM/hzxDsBAAAAAABwGPvgg3hnIE2a1OFV1NfX65FHHtHcuXOjkBCijRlYAAAAAADgqHfyySfrpZdeUmlpabxTQRA0sAAAAAAAwFHvnnvukdvt1iOPPNLmci6XS7/5zW+Un5+vpKQk9e3bV/fcc4/q6+t9y9xxxx3KysqSaZq+2G233SbDMPT000/7Yrt375ZhGHruueeiX9ARhgYWAAAAAAA46vXr10/Tpk0LOwvrhhtu0K9//WudeuqpeuKJJzRu3DjNmTNHV1xxhW+ZMWPGqKKiQt98840vtmrVKtlsNq1atSogJkljx47thIqOLDSwAAAAAAAAJP3qV7+Sy+XSo48+GvTna9eu1WuvvaYbbrhBb731ln784x/rtdde089+9jP93//9n1asWCFJOvPMMyU1N6icTqe+/vprXXzxxa0aWN26ddOgQYM6ubLDHw0sAAAAAAAASXl5ebr22mv14osvaufOna1+/v7770tq+oqgvzvvvFOS9Pe//12S1KNHDw0cOFAff/yxJOmTTz6R3W7Xz3/+c+3evVubNm2S1NTAOvPMM2UYRqfVdKSggQUAAAAAAHDQvffeK5fLFfRZWFu3bpXNZlP//v0D4scee6wyMzO1detWX2zMmDG+2VarVq3S8OHDNXz4cHXr1k2rVq1SVVWV1q5dqzFjxnRuQUcIGlgAAAAAAAAH5eXl6Zprrgk5C0tSRDOmzjzzTO3YsUObN2/WqlWrNGbMGBmGoTPPPFOrVq3S6tWr5fF4aGBFiAYWAAAAAACAH+8srJbPwjr++OPl8Xh8XwH02r17tyorK3X88cf7Yt7G1NKlS/Xll1/6/j127FitWrVKq1atUmpqqk477bROrubIQAMLAAAAAADAT35+vq655hq98MIL2rVrly8+ZcoUSdKTTz4ZsPzjjz8uSTr//PN9sX79+qlPnz564okn1NjYqDPOOENSU2Pru+++09tvv63vfe97cjgcnVzNkYEGFgAAAAAAQAu/+tWv1NjYqH//+9++2LBhwzR9+nS9+OKLuvzyy/Xss8/quuuu029/+1v94Ac/0FlnnRWwjjFjxujf//63hgwZomOOOUaSdOqppyo1NVXFxcV8fbAdaGABAAAAAAC00L9/f11zzTWt4i+//LJmz56tL7/8Urfffrs++ugj3X333XrzzTdbLettUJ155pm+mMPh0KhRowJ+jvAM0zTNeCchSVVVVcrIyJDT6VR6enq804me//wn3hk0a/FXEgAAAAAACKeurk4lJSXq16+fkpOT450OLCrccdLRvg8zsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAOolhGLr//vvjncZhjwYWAAAAAAA4KhmGEdF/K1eujHeqRz1HvBMAAAAAAACHsf/8J94ZSP37H9LLXn/99YB///GPf9TSpUtbxQsKCg45NUQHDSwAAAAAAHBUuuaaawL+/dlnn2np0qWt4og/vkIIAAAAAAAQQk1Nje68807l5uYqKSlJAwYM0GOPPSbTNAOWq6+v1//7f/9PPXr0UNeuXTV16lRt37691fq2bt2qH//4xxowYIBSUlKUlZWlSy+9VFu2bPEts3nzZhmGoSeeeKLV61evXi3DMPSnP/0p6rVaGQ0sAAAAAACAIEzT1NSpU/XEE09o0qRJevzxxzVgwAD9/Oc/1x133BGw7A033KAnn3xSEydO1COPPKKEhASdf/75rdb55ZdfavXq1briiiv09NNP6+abb9by5cs1fvx4HThwQJKUl5enM844Q/Pnz2/1+vnz56tr1676/ve/3zlFWxRfIQQAAAAAAAhi0aJF+uijj/Tggw/qV7/6lSTpJz/5iS699FI99dRTuvXWW5Wfn6+1a9fqjTfe0I9//GP9/ve/9y139dVXa926dQHrPP/883XJJZcExC688EKNGjVK77zzjq699lpJ0rRp03TTTTdp48aNGjhwoCSpsbFRCxcu1EUXXaQuXbp0dvmWwgwsAAAAAACAIN5//33Z7XbNnDkzIH7nnXfKNE0tXrzYt5ykVsvdfvvtrdaZkpLi+/+NjY0qLy9X//79lZmZqa+++sr3s8suu0zJyckBs7A+/PBDlZWVHZXP6KKBBQAAAAAAEMTWrVvVu3dvde3aNSDu/auEW7du9f2vzWZTfn5+wHIDBgxotc7a2lr9+te/9j1Tq3v37urRo4cqKyvldDp9y2VmZurCCy/UggULfLH58+erT58+Ovvss6NW4+EiKg2s6667ToZhhPxvx44d0XgbAAAAAACAw9ptt92mhx56SJdddpkWLlyoJUuWaOnSpcrKypLH4wlYdtq0adq8ebNWr16t/fv3a9GiRbryyitlsx1985Gi8gysm266Seecc05AzDRN3Xzzzerbt6/69OkTjbcBAAAAAACImeOPP17Lli3T/v37A2Zhbdy40fdz7/96PB599913AbOu/v3vf7da59tvv63p06frf//3f32xuro6VVZWtlp20qRJ6tGjh+bPn6/TTz9dBw4c8D0j62gTlZbdqFGjdM011wT8169fPx04cEBXX311NN4CAAAAAAAgpqZMmSK3261nnnkmIP7EE0/IMAxNnjxZknz/+/TTTwcs9+STT7Zap91ul2maAbG5c+fK7Xa3WtbhcOjKK6/UwoULNW/ePJ100kkaOnRoR0o6bHXaXyFcsGCBDMPQVVdd1VlvAQAAAAAA0GkuvPBCnXXWWfrVr36lLVu2aNiwYVqyZIn++te/6vbbb/c98+rkk0/WlVdeqWeffVZOp1OjR4/W8uXL9Z///KfVOi+44AK9/vrrysjI0KBBg/Tpp59q2bJlysrKCprDtGnT9PTTT2vFihV69NFHO7VeK+uUBpb3zzqOHj1affv27Yy3AAAAAAAA6FQ2m02LFi3Sr3/9a/35z3/Wq6++qr59++p3v/ud7rzzzoBl//CHP/i+7vd///d/Ovvss/X3v/9dubm5Acs99dRTstvtmj9/vurq6nTGGWdo2bJlOu+884LmcNppp2nw4MHasGHDUf0tN8NsOW8tCv72t7/pwgsv1LPPPqtbbrkl6DL19fWqr6/3/buqqkq5ubkqLy9Xenq6pKYDxWazyePxBDzIzBt3u90B0+5Cxe12uwzDkMvlCsjBbrdLUqtpeqHiDodDpmkGxA3DkN1ub5WjL75pkzz+OR7M0+PxyP/RbDbDkM0w5PZ4ZEYQtx98QL6rxQPe7IbRlHuL3Wo3DKl//+jUFGJ/HNb7iZqoiZqoiZqoiZqoiZqoiZqoiZqC5l5XV6f//ve/6tevn1JSUlp9/c37ms6Mt0dn5xKPmk499VR169ZNy5Yti2mO7YnX1dVpy5Ytys3NVXJysi/uPfb27dunrKwsOZ1OX9+nPTplBtaCBQuUkJCgyy67LOQyc+bM0ezZs1vFi4qKlJqaKknq0aOH8vPzVVJSor179/qWycnJUU5OjoqLiwP+xGReXp6ys7O1fv161dbW+uIDBw5UZmamioqKAk7KoUOHKjExUYWFhQE5DB8+XA0NDVq3bp0vZrfbNWLECDmdTt/D2iQpJSVFw4YNU1lZmTZv3uyLZ2RkqKCgQKVOp7b75dgjLU35WVkq2bdPe6urm2vKyFBOZqaKy8rk9Ms9LytL2WlpWr9rl2obG5trys5WZkqKinbskNtv0Bvaq5cSHQ4VbtsWWFNurhpqa6NTU2mptm/f3lzTkbCfqImaqImaqImaqImaqImaqImaqClkTcnJyaqvr1dKSooaGxvV0NDgW97hcPh+7t9QS0xMVGJiourq6gJyTEpKUkJCgmprawOaeMnJyXI4HDpw4EBAcyQlJUU2m001NTUBNaWmpsrj8QRsF8MwlJqaKrfbrbq6Ol/cZrOpS5cucrlcAZNp7Ha75WsqKirSmjVr9MorrwQsb7WavE2t9evXB9TkPfaKiorUEVGfgVVdXa2ePXvq7LPP1nvvvRdyOWZgMQPLUvuJmqiJmqiJmqiJmqiJmqiJmqiJmoLmzgyszomHs379ev3rX//S448/rrKyMn333XcBM5vimXs8ZmBFvYH1xhtv6Nprr9Wf/vQnXXHFFRG/rqqqShkZGYdciGUFeWBb3PTvH+8MAAAAAACHmbq6OpWUlKhfv36tGijoPPfff78eeOABDRgwQM8//7zGjRsX75TaFO446WjfxxaNJP3Nnz9faWlpmjp1arRXDQAAAAAAcFS4//775fF4tGHDBss3r2Ihqg2svXv3atmyZfrhD3+oLl26RHPVAAAAAAAAOEpFtYH15z//WS6X66j+s44AAAAAAACIrqg2sObPn6/s7Gydc8450VwtAAAAAACIsyg/QhtHmM4+PhzRXNmnn34azdUBAAAAAIA48/4VucbGRqWkpMQ5G1hVY2OjpObjJdqi/hB3AAAAAABw5EhISFBSUpKcTiezsBCUaZpyOp1KSkpSQkJCp7xHVGdgAQAAAACAI0/37t21Y8cObd++XRkZGUpISJBhGPFOC3FmmqYaGxvldDpVXV2tPn36dNp70cACAAAAAABtSk9PlySVlZVpx44dcc4GVpOUlKQ+ffr4jpPOQAMLAAAAAACElZ6ervT0dDU2Nsrtdsc7HViE3W7vtK8N+qOBBQAAAAAAIpaQkBCThgXgj4e4AwAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNIc8U4AAAAAQGtL1sc7g2YTh4Rf5nDLFwBweGEGFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACzNEe8EAAAAACDWlqyPdwbNJg6JdwYAYH3MwAIAAAAAAICl0cACAAAAAACApUWtgfXVV19p6tSp6tatm7p06aIhQ4bo6aefjtbqAQAAAAAAcJSKyjOwlixZogsvvFCnnHKK7rvvPqWlpem7777T9u3bo7F6AAAAoMOs9MwjieceAQDQHh1uYFVVVWnatGk6//zz9fbbb8tm41uJAAAAAAAAiJ4Od5sWLFig3bt366GHHpLNZlNNTY08Hk80cgMAAAAAAAA63sBatmyZ0tPTtWPHDg0YMEBpaWlKT0/XLbfcorq6umjkCAAAAAAAgKNYh79CuGnTJrlcLn3/+9/X9ddfrzlz5mjlypWaO3euKisr9ac//Sno6+rr61VfX+/7d1VVlSTJ5XLJ5XJJkmw2m2w2mzweT8CsLm/c7XbLNM2wcbvdLsMwfOv1j0uS2+2OKO5wOGSaZkDcMAzZ7fZWOfripimPf44H8/R4PPKfp2YzDNkMQ26PR2YEcbthNNXUYrab3TCacjfN1vEWuR9yTSH2x2G9n6iJmqiJmqiJmqjpiK/J9L9tMpriMgNrMmxNNQXGDRk2u0zToxYrCR43bDIMW+i4xy3JlDfVUDWZZlNNpiewplC5d2ZNHk8E+8njd//Zolb/HGNRk8sV/tgzzcj2UyxqcrkOv/Mpkjg1URM1UZN/vOXy7dXhBlZ1dbUOHDigm2++2fdXBy+66CI1NDTohRde0AMPPKATTjih1evmzJmj2bNnt4oXFRUpNTVVktSjRw/l5+erpKREe/fu9S2Tk5OjnJwcFRcXy+l0+uJ5eXnKzs7W+vXrVVtb64sPHDhQmZmZKioqCtiQQ4cOVWJiogoLCwNyGD58uBoaGrRu3TpfzG63a8SIEXI6ndq4caMvnpKSomHDhqmsrEybN2/2xTMyMlRQUKBSp1Pb/XLskZam/Kwslezbp73V1c01ZWQoJzNTxWVlcvrlnpeVpey0NK3ftUu1jY3NNWVnKzMlRUU7dsjtd+AN7dVLiQ6HCrdtC6wpN1cNtbXRqam0NOAB/UfEfqImaqImaqImarJKTdu3K8PtVkF9vUoTErQ9IaG5JpdL+Q0NKklM1F5H821cTmOjchobVZyUJOfBm0RJymtoULbLpfXJyar1e07pwLo6ZXo8KkpJkfvgL78kaWhtrRJNU4Vdung31hG1nxr2N++nxJ7DZbob1FjWXJNh2JV47AiZDU41VjTXZDhSlNhjmDy1ZXI5m2uyJWUooVuB3NWlclc312RP6SFHZr7czhK5a5trsqflyNE1R67KYnnqnSo80HZNZsJAGUmZatxTJNOv2ZHQfagMe6Iadgcee51ZU0lq+P3UsLt5Pzky8mTvkq3G8vUyXc01JXSLTU2FheGPPbcrsv0Ui5qK6g+/88nfkTJGUBM1UVPn1lRUVKSOMEz/NtohGDJkiL755hv94x//0NixY33xjz/+WOPGjdNrr72madOmtXpdsBlYubm5Ki8vV3p6uqT4dwej0vHctMk6M7D69z8iu7jURE3URE3URE1HVE0LFsiQZJfkOfifL8eD/4WKt5gXEjJul2RIavl7UG/ry5fhVVdFp6Y24rHcT8u/9fuBBWZgTRjUdk3LN1hnBta5Q8Lvp2XfWGcG1oSC8Mfe8g3WmYE1YdDhdz5FEqcmaqImavKP79u3T1lZWXI6nb6+T3t0eAZW79699c0336hnz54B8ezsbF+CwSQlJSkpKal1Qg6HHI7AtLwbrSXvRog03nK9hxI3DCNoPFSO3gZU0OWDvKc9yDraijtCxYO8p0Lk3u6a2hk/LPYTNVFTiBzbG6cmapKoKVSO7Y1TU3MDKtJ48MxDx0PdCPriLXI93PeTEWyjGcFrCh63KdhK2h232Q/mFBhvWZP3ds6whdhTQXIMFe9oTd5d09Z+CrZ9vbW2jnduTQ5H+GPMt33D7KfI44dek/dYOJzOp0jj1ERNEjWFyrG98SOxpvbo8EPcTzvtNEnSjh07AuKlpaWSmqaoAQAAAAAAAIeqww2syy67TJL0yiuvBMRffvllORwOjR8/vqNvAQAAAAAAgKNYh79CeMopp+hHP/qR/vCHP8jlcmncuHFauXKl3nrrLd19993q3bt3NPIEAAAAAADAUarDDSxJev7553Xcccfp1Vdf1bvvvqvjjz9eTzzxhG6//fZorB4AAAAAAABHsag0sBISEjRr1izNmjUrGqsDAAAAAAAAfDr8DCwAAAAAAACgM9HAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTninQAAAAAAoG1L1sc7g2YTh8Q7AwBHI2ZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0hzxTgAAAACHryXr451Bs4lD4p0BAADoLMzAAgAAAAAAgKUxAwsAAAAAEFXMzgQQbczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKV1uIG1cuVKGYYR9L/PPvssGjkCAAAAAADgKOaI1opmzpypESNGBMT69+8frdUDAAAAAADgKBW1BtaYMWN0ySWXRGt1AAAAAAAAgKQoPwNr//79crlc0VwlAAAAAAAAjnJRm4E1Y8YMVVdXy263a8yYMfrd736n4cOHR2v1AAAAAAB0iiXr451Bs4lD4p0BYE0dbmAlJibq4osv1pQpU9S9e3d9++23euyxxzRmzBitXr1ap5xyStDX1dfXq76+3vfvqqoqSZLL5fLN4rLZbLLZbPJ4PPJ4PL5lvXG32y3TNMPG7Xa7DMNoNTvMbrdLktxud0Rxh8Mh0zQD4oZhyG63t8rRFzdNefxzPJinx+ORx2/dNsOQzTDk9nhkRhC3H3xQvsvjv5amuCS5TbN1vEXuh1xTiP1xWO8naqImaqImaqImK9UkyS7Jc/A/X44H/wsVd0uB9xEh4vaD79Fy3rz94P/6MjxYc7iaZPrHDRk2u0zTI5me8HHDJsOwhY57WmQfMt5UVVv7KTCdg9WagTUZttjV5E011LFnmk3HnulpsadC5N6ZNXk8EZxPnsj2UyxqcrnCjxGmGb1jr6M1uVzhxwjTE9vzqa2aXK7w457pie351Fbc5Qo/ljct37rWeIwRlr4+HYnXXGqKWU0d/cZehxtYo0eP1ujRo33/njp1qi655BINHTpUd999tz744IOgr5szZ45mz57dKl5UVKTU1FRJUo8ePZSfn6+SkhLt3bvXt0xOTo5ycnJUXFwsp9Ppi+fl5Sk7O1vr169XbW2tLz5w4EBlZmaqqKgoYEMOHTpUiYmJKiwsDMhh+PDhamho0Lp163wxu92uESNGyOl0auPGjb54SkqKhg0bprKyMm3evNkXz8jIUEFBgUqdTm33y7FHWprys7JUsm+f9lZXN9eUkaGczEwVl5XJ6Zd7XlaWstPStH7XLtU2NjbXlJ2tzJQUFe3YIbffgTe0Vy8lOhwq3LYtsKbcXDXU1oavqaZGKQkJGta7t8qqq7W5vLy5ppQUFWRnq7SyMnhN5eXBa9qzJ3hNpaXBa9q2rammg8dByP3UrZsaXC6t27mzuSabTSNyc+WsrdXGPXua91Msajr5ZGsde6Wl2r59e3NN7T2fkpMj20/emto69jq6n3r3jk5NVhwjqImaqKnza/ryy+hen7w1Hcq41717+Jq6dFGG262C+nqVJiRoe0JCc00ul/IbGlSSmKi9jubbuJzGRuU0Nqo4KUlOu90Xz2toULbLpfXJyaq1NT85YmBdnTI9HhWlpMh98JdfkjS0tlaJpqnCLl2aAgf3V1v7yWxwqrGiuSbDkaLEHsPkqS2Ty9m8n2xJGUroViB3danc1c37yZ7SQ47MfLmdJXLXNh979rQcObrmyFVZLE9987HnyMiTvUu2GsvXy3Q177+EbgMltX3sNexv3k+JPYfLdDeosay5JsOwK/HY2NVUeODgfgpxPpkJA2UkZapxT5FMvw/LCd2HyrAnqmF34PnUmTWVpIYfIxp2R7afYlFTYWH4McLtit6x19GaiurDj3sNu2N7PrVVUyRjeWN1bM+ntmoqPBD++hTL8ylcTYf1NfdIvI+gpqjVVFRUpI4wTP82WhRdeeWV+stf/qIDBw74um3+gs3Ays3NVXl5udLT0yXFvzsYlY7npk3WmYHVv3/4mjZvbvqtr83WavZYqHin1ZSX1xQPtZ9KSoLW6rDZmmqKIPeo1nTCCdY69jrabS8pid6xFyTerv2Un2/J3yBYYj9REzVRU/iaiotjf80NEnfYbDLz88PXtGCBdWZgXXVVU7yN/fTh1/GfXdEUt+u8k9o+9pZ/q4DlJcV1BtaEQU3hUOfT8g3WmYF17pDwY8Syb6wzA2tCQfgxYvkG68zAmjAo/Li3dL11ZmBNKAg/li//1jozsCYMCn99WvK1dWZgTSg4jK+5R+J9BDVFraZ9+/YpKytLTqfT1/dpj6g9A6ul3NxcNTQ0qKamJmhiSUlJSkpKap2QwyGHIzAt70ZrKVhjrK14y/UeStwwjKDxUDl6b4aDLh/kPe1B1tFW3BEqHuQ9FSL3gJr81hcy91jV1CLXVrkfzCFYrYZhBI13ek1WOvbaGW+V+8HtEZVjL0Q84v10MLcO1xQmfljupzBxaqImaorTNTdEvN01Hfwv0njwvRE6HupG0BcPdy1WU00ygsVtktE6y3bHbcGzDxVv6xgLsvoQucemppaptjyfvIeQYQuxp4LkGCre0Zq8h2dbY0Sw7Rt6/3VuTQ5H+DHCt32jdOx1pCbvsdDWGGEE2e6dfT6FqimSsdz79lYYI/zTDZV7e/ZfZ9d02F9zj8T7CGqKOMdDiUcq+J1YFGzevFnJyclKS0vrrLcAAAAAAADAUaDDDSz/7016rV27VosWLdLEiRODdvUAAAAAAACASHX4K4SXX365UlJSNHr0aGVnZ+vbb7/Viy++qC5duuiRRx6JRo4AAAAAAAA4inW4gfWDH/xA8+fP1+OPP66qqir16NFDF110kWbNmqX+/ftHI0cAAAAAAHDQkvXxzqDZxCHxzgBHiw43sGbOnKmZM2dGIxcAAAAAAACgFR5QBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS3PEOwEAAAAAAHDkWrI+3hk0mzgk3hngUDEDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJbmiHcCAAAAAAAAVrFkfbwzaDZxSLwzsA5mYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJ4BhYAAICFfFcW7wya5cc7AQAAgIOYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLc8Q7gSPdp9/FO4Nmo/rHOwMAAAAAAID2YwYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsrVMaWA899JAMw9CQIUM6Y/UAAAAAAAA4ikS9gbV9+3Y9/PDDSk1NjfaqAQAAAAAAcBRyRHuFP/vZz/S9731PbrdbZWVl0V49AAAAAAAAjjJRnYH18ccf6+2339aTTz4ZzdUCAAAAAADgKBa1Bpbb7dZtt92mG264QSeddFK0VgsAAAAAAICjXNS+Qvj8889r69atWrZsWUTL19fXq76+3vfvqqoqSZLL5ZLL5ZIk2Ww22Ww2eTweeTwe37LeuNvtlmmaYeN2u12GYfjW6x+XmppvkcQdDodM0wyIG4Yhu93eKkdvvCkPM2A9hmGTaXoUyJBhGFGJNzFbxVvmHrQmj0eGJLvNJo9pyuO3HUPFbVLzfvJbt80wZDMMuT2egGxCxe1GU00u73Y8uL9C7qeDObjNwFodNltTTRHkHtWaDuZolWMv1HkT8flkmpHtJ7+41Hp/hIq3az+53dGpyYJjBDVREzXFqCa/dXf4+uQXlw5h3AtTk+fgpdxmNl3NTcNvJWbTNcojNV/yJRlm0z89/sseYlx+7+kKcy327ieZ/nFDhs3edI8ScJ8SIm7Ymu+NgsU9bgXc14SM2yW1fewFpmM/WGxgTYYtdjV5Uw11Pplm0/lkegJrCpV7Z9bk8UQwRngi20+xqMnlCj9GmGb0jr2O1uRyhR/3TE9sz6e2anK5wo/lpie251NbcZcr/PWpafnWtcZjjIjkmmt6FLPzKVxNLlf4+4hYnk/haorkPqJp+1pjjPAeskfC/V7L5dsrKg2s8vJy/frXv9Z9992nHj16RPSaOXPmaPbs2a3iRUVFvgfA9+jRQ/n5+SopKdHevXt9y+Tk5CgnJ0fFxcVyOp2+eF5enrKzs7V+/XrV1tb64gMHDlRmZqaKiooCNuTQoUOVmJiowsLCgByGDx+uhoYGrVu3zhez2+0aMWKEnE6nNm7c6IunpKRo2LBhKisr0+bNm33xjIwMFRQUqN7jVJ27OcdEW5q6OLJU696nBk+1L55sz1CyPVM1rjK5zObcU+xZSrKnqdq1S26z0RdPdWQrwUhRVeMOmX635V0Teskmh5yN2wJqykjIVW1tbfiaamqUkpCgYb17q6ymRpvLy5vXkZKiguxslTqd2u633XukpSk/K0sl+/Zpb3VzTTkZGcrJzFRxWZmcfvsjLytL2WlpWr9rl2obm2samJ2tzJQUFe3YIbfHI1VUtL2funVTg8uldTt3Ntdks2lEbq6cdXXauGdP83aMRU2SpY690tJSbd++vbmm9p5PycmR7SdvTb16KdHhUOG2wGNveG5ux/eT2x2dmiw4RlBTJ9VUU9P2sVdbG/zYq64OPkZUVgYfI8rLg48Re/Y0jxGpqeFrWrWq4+dTtGoyjCPv2Iv29clb06HspwhqOtCzi5Lr3eq5r17OtAQ50xJ8y6fVupTlbNC+jERVpzTfxmVUNyqzulF7M5NUl2T3xbs5G9S11qVdWclqdDRPvM+uqFNKg0fbs1NkGs1drF5ltXK4TW3r2UWSVH5wf7W1n8wGpxormmsyHClK7DFMntoyuZzN+8mWlKGEbgVyV5fKXd28n+wpPeTIzJfbWSJ3bfOxZ0/LkaNrjlyVxfLUNx97jow82btkq7F8vUxX8/5L6DZQUtvHXsP+5v2U2HO4THeDGsuaazIMuxKPjV1NhQea4qHOJzNhoIykTDXuKZLp9wEnoftQGfZENewOPJ86s6aS1PBjecPuyPZTLGoqLAw/Rrhd0Tv2OlpTUX34ca9hd2zPp7ZqimQsb6yO7fnUVk2FB8Jfn2J5PoWrKZJrbsP+2J1P4WoqPBD+fi+W51O4miK5j2jYH7vzKVxNhQcO8/tyNY8RRUVF6gjDNFv8evAQ3HLLLVq2bJm++eYbJSYmSpLGjx+vsrIyrV+/Puhrgs3Ays3NVXl5udLT0yXFvzsYjd8Gr/5gk6wyA2vUef3D17R5s3VmYOXlNcVD7aeSkqa4VWZgnXCCpY69DnfbS0qsMwMrP9+Sv0GwxH6ipuC5b94cnWMvRLxdY0ReXviaiosDa+rM8ylcTXl5R96xV1xsnRlY+flhayqZu6ApHwvMwOp321VNNbWxnz78Ov6zK5ridp13UtvH3vJvFbB8U7Hxm4E1YVBTONT5tHyDNWZXSNK5Q8KP5cu+scbsCtP0aEJB+DFi+QZrzK6QpAmDwo97S9dbZwbWhILwY/nyb60zA2vCoPDXpyVfW2cG1oSC8Nfc5d/KMjOwJgwKf7/34TrrzMA6Z1D4+4im7WuNMcJ7rThs78v94vv27VNWVpacTqev79MeHZ6BtWnTJr344ot68sknVVpa6ovX1dWpsbFRW7ZsUXp6urp16xbwuqSkJCUlJbVOyOGQwxGYlnejteTdCJHGW673UOKGYQSNh8rRMAwF3GH64sEfPxatePD3DJ57QNyvBu+NfEsh4zZb0Ieq2YNsl7biDm+8Ra6tcj+YgyNILoZhBI13ek0WOvbaG2+V+8HtEXY/tYwH2Y6h4hHvp4O5dbimMPHDcj+FiR+1Nfm9T9zHCL+8QtYUy/MpXPxIPfaCvOchX59axtu7n8LUZPO/51VzUylgean176pavLYjce97tsw11H6SESxuk4Lcp7Q7bgt+jIWKt3WMBb1tCpp7bGpqmWrL88l7CBm2ELfsQXIMFe9oTd7Dv60xItj2Db3/OrcmhyP8GOHbvlE69jpSk/dYaGuMMIJ+1ujc8ylUTZGM5d63t8IY4Z9uqNzbs/86u6ZIrrn+L4v3GBF4Cxbic3EMz6fmHIPXFMl9RMD2jfMY4b99D8v78gjikerwQ9x37Nghj8ejmTNnql+/fr7/Pv/8cxUXF6tfv3564IEHOvo2AAAAAAAAOEp1eAbWkCFD9O6777aK33vvvdq/f7+eeuop5efnd/RtAAAAAAAAcJTqcAOre/fu+sEPftAq/uSTT0pS0J8BAAAAAAAAkerwVwgBAAAAAACAztThGVihrFy5srNWDQAAAAAAgKMIM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaY54JwBr+fS7eGfQbFT/eGcAAAAAAACsgBlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQe4g4AAI5o/IESAACAwx8zsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaR1uYH3zzTe69NJLlZeXpy5duqh79+4aO3as3nvvvWjkBwAAAAAAgKOco6Mr2Lp1q/bv36/p06erd+/eOnDggN555x1NnTpVL7zwgm688cZo5AkAAAAAAICjVIcbWFOmTNGUKVMCYrfeeqtOO+00Pf744zSwAAAAAAAA0CGd8gwsu92u3NxcVVZWdsbqAQAAAAAAcBTp8Awsr5qaGtXW1srpdGrRokVavHixLr/88mitHgAAAAAAAEepqDWw7rzzTr3wwguSJJvNposuukjPPPNMyOXr6+tVX1/v+3dVVZUkyeVyyeVy+dZjs9nk8Xjk8Xh8y3rjbrdbpmmGjdvtdhmG4Vuvf1yS3G53RHGHwyHTNAPihmHIbre3ytEbb8rDDFiPYdhkmh4FMmQYRlTiTcxW8Za5B6vJu76mHEPlHpuavPsr5H46uI/dZmAuDltTjv5xQ5LdZpPHNOWJIG6Tmo89v3XbDEM2w5Db4wnYAjbDkO1gjlY59kKdNxGfT6YZtFa70bSfXJ7A/Wc3mo69lvsjVLxd+8ntjk5NFhwjqKmTavJ4onPshYi3a4xwucLXFMvzKZKajrBjLx7X3GBx7zU0XE2egy+3mU1rMA2/lZhN+8rj/zaSDLPpnx7/ZQ8xLr/3DHct9u4nmf5xQ4bN3rS9ArZZiLhha76PCBb3uBWwLUPG7ZLaPvYC07EfLDawJsMWu5q8qYY6n0yz6XwyPYE1hcq9M2vyeCIYyz2R7adY1ORyhR8jTDN6x15Ha3K5wo97pie251NbNblc4cdy0xPb86mtuMsV/vrUtHzrWuMxRkRyzTU9itn5FK4mlyv8/V4sz6dwNUVyH9G0fa0xRngP2cP2vtwv3nL59opaA+v222/XJZdcotLSUi1cuFBut1sNDQ0hl58zZ45mz57dKl5UVKTU1FRJUo8ePZSfn6+SkhLt3bvXt0xOTo5ycnJUXFwsp9Ppi+fl5Sk7O1vr169XbW2tLz5w4EBlZmaqqKgoYEMOHTpUiYmJKiwsDMhh+PDhamho0Lp163wxu92uESNGyOl0auPGjb54SkqKhg0bprKyMm3evNkXz8jIUEFBgeo9TtW5m3NMtKWpiyNLte59avBU++LJ9gwl2zNV4yqTy2zOPcWepSR7mqpdu+Q2G33xVEe2EowUVTXukOn38alrQi/Z5JCzcVtATRkJuaqtrQ1bk7OxRnYjQV0TeqvBU6Nad7lveYeRorSE7JjVVFhY0fZ+6tZNDS6X1u3c2VyTzaYRubly1tVp4549ze+ZkKBhvXurrKZGm8uba8pISVFBdrZKnU5t9zuWeqSlKT8rSyX79mlvdXNNORkZysnMVHFZmZx+x1heVpaypbaPvYNNWkka2quXEh0OFW4L3E/Dc3ND11RbG7ym6urgNVVWBq+pvLyppoPnWcjzKTlZ2WlpWr9rl2obm/fTwOxsZaakqGjHDrn9Br1DqinS/eR2q6CgQKWlpdq+fXtzTf5jxJYtvrhvP+3Z03o/paVpfWlp8Jq2bet4TbW12lhT01xTmDGizZqsNO7961/NNXX02PPWdKj7ad++8DXV1ETn2IvGGFFREX4/xfJ8CldTJMdeTU3szqdw415qatjzKR7XXI9c2t/YXJMhmzIScyO6jzjQs4uS693qua9ezrQEOdMSfMun1bqU5WzQvoxEVac038ZlVDcqs7pRezOTVJdk98W7ORvUtdalXVnJanQ0Pzkiu6JOKQ0ebc9OkWk0d7F6ldXK4Ta1rWcXSVL5wfOqrTHCbHCqsaK5JsORosQew+SpLZPL2Tzu2ZIylNCtQO7qUrmrm/eTPaWHHJn5cjtL5K5tPvbsaTlydM2Rq7JYnvrmY9WRkSd7l2w1lq+X6WrefwndBkpqe9xr2N+8nxJ7DpfpblBjWXNNhmFX4rGxq6nwQFM81BhhJgyUkZSpxj1FMv0+4CR0HyrDnqiG3YFjeWfWVJIa/vrUsDuy/RSLmgoLw19z3a7oHXsdramoPvxnjYbdsT2f2qopkvuIxurYnk9t1VR4IPy9USzPp3A1RXK/17A/dudTuJoKD4S/h43l+RSupkjuyxv2x+58CldT4YFD70dY7bNGUVGROsIwzRa/xo2SiRMnqrKyUp9//rkMw2j182AzsHJzc1VeXq709HRJ8e8ORuO3was/2CSrzMAadV7/sDV9sWyzX47xnYE18pw8SW3sp5KSpni8Z1d44yec0Pax5zegxH12hSTlNW3fkOdTSYl1ZmDl54f/DcJ//tMcb2s/xaKmfv2acz/MfisScozYtKk5d8XgfGprP/XtGz73zZutMwMrLy/8fiouDqwpnmNEXl74Y2/z5tidT+Fyz8sLez6t/iBw+8bimhssbhg2fW9iftj7iJK5C5ryt8AMrH63XSWp7THiw6/jP7uiKW7XeSe1Pe4t/1YByzcVG78ZWBMGNYVDjRHLN1hjdoUknTsk/PVp2TfWmF1hmh5NKAh/zV2+wRqzKyRpwqDwnzWWrrfODKwJBeHvI5Z/G9vzqa34hEHh742WfG2dGVgTCsLf7y3/VjE7n8LVNGFQ+HvYD9dZZwbWOYPC35c3bV9rjBHea8WRMANr3759ysrKktPp9PV92iNqM7BauuSSS3TTTTepuLhYAwYMaPXzpKQkJSUltU7I4ZDDEZiWd6O15N0IkcZbrvdQ4oZhBI2HyrGpede6gWcYwZ+fH6148PcMnrt/3H99oXOPTU0tc22V+8EPPY4gDVLDMILGvR+4Io7bbEH/0oE9yL6Wwhx7QV4TLMdQ8ajX1GJ7tsr94GtD1eoIFe+Mmg7mFuo8CzlGhNpPnV1TO8aIdtcUr3EvWI6dfT6F2h+R5O732riPEX55hdxPsTyfwsUjOfb8fh73McJv+4a+Fsf+mhsqHskYYfO/51VzUylgeal136zFazsS975n2GuxDt4XGMHiNinINmt33Bb8vAkVb2uMCLoLg+Yem5paptpyjPAe5oYtxC17kBxDxTtak/fUamuMCLZ9Q++/zq3J4WidTMvcfds3SsdeR2ryHgttjRFGqPGtE8+nUDVFci32vr0Vxgj/dEPl3p7919k1RXK/5/+yeI8RgbdgIa7FMTyfmnMMXlMk998B2zfOY4T/9j0SP2u0R6g7sQ7zTi/zn34GAAAAAAAAtFeHG1h7/J5N4dXY2Kg//vGPSklJ0aBBgzr6FgAAAAAAADiKdfgrhDfddJOqqqo0duxY9enTR7t27dL8+fO1ceNG/e///q/S0tKikSfQyqffxTuDQKP6xzsDAAAAAACOTB1uYF1++eV65ZVX9Nxzz6m8vFxdu3bVaaedpkcffVRTp06NRo4AAAAAAAA4inW4gXXFFVfoiiuuiEYuAAAAAAAAQCud9hB3AAAAAAAAIBpoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0hzxTgAAABxePv0u3hk0G9U/3hkAAAAgFpiBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEtzxDsB4Gjx6XfxziDQqP7xzgAAAAAAgMgwAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJbGM7AAAIgzKz0jj+fjAQAAwIqYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS+twA+vLL7/UrbfeqsGDBys1NVXHHXecLrvsMhUXF0cjPwAAAAAAABzlHB1dwaOPPqpPPvlEl156qYYOHapdu3bpmWee0amnnqrPPvtMQ4YMiUaeAAAAAAAAOEp1uIF1xx13aMGCBUpMTPTFLr/8cp100kl65JFH9MYbb3T0LQAAAAAAAHAU63ADa/To0a1iJ5xwggYPHqwNGzZ0dPUAAAAAAAA4ynXKQ9xN09Tu3bvVvXv3zlg9AAAAAAAAjiIdnoEVzPz587Vjxw498MADIZepr69XfX29799VVVWSJJfLJZfLJUmy2Wyy2WzyeDzyeDy+Zb1xt9st0zTDxu12uwzD8K3XPy5Jbrc7orjD4ZBpmgFxwzBkt9tb5eiNN+VhBqzHMGwyTY8CGTIMIyrxJmareMvcg9XkXV9TjqFyj01N3v0Van807+P25Nh5NXlzDHXsBb4m9H6KVU0tz7NW55NpymYYcns8AWuxG03bwOUJ3AZ24+A2MM2I4g5bU47+cUOS3WaTxzTl8Y+73UHPs5BjhGEEzT1UPOo1+Y014caIiGuK97jnn7tC7KcQcdvBPD0ej/y38CHvp0hq8niic+xFoyaXK+x+as9YHiwezTEikmOvKd/oXZ86UpPL5Qp7PsXjmttWTeHuIzwHX24zm9ZgGn4rMZuOP4//20gyzKZ/evyXPcS4/N4z3LXYO0bI9I8bMmz2pu3V4toXNG7Ymq9PweIetwK2Zci4XVLbY0RgOvaDxQbWZNhiV5M31VBjhGkeHCM8gTWFyr0za/J4Irg+eSLbT7GoyeUKf801zegdex2tyeUK/1nD9MT2fGqrJpcr/H2E6Ynt+dRW3OUKf2/UtHzrWuMxRkRyv9d0KbbGGOFyhb+HjeX5FK6mSO7Lm7avNcYI7yF7KP0Iq33WaLl8e0W9gbVx40b95Cc/0ahRozR9+vSQy82ZM0ezZ89uFS8qKlJqaqokqUePHsrPz1dJSYn27t3rWyYnJ0c5OTkqLi6W0+n0xfPy8pSdna3169ertrbWFx84cKAyMzNVVFQUsCGHDh2qxMREFRYWBuQwfPhwNTQ0aN26db6Y3W7XiBEj5HQ6tXHjRl88JSVFw4YNU1lZmTZv3uyLZ2RkqKCgQPUep+rczTkm2tLUxZGlWvc+NXiqffFke4aS7ZmqcZXJZTbnnmLPUpI9TdWuXXKbjb54qiNbCUaKqhp3yPT7+NQ1oZdscsjZuC2gpoyEXNXW1oatydlYI7uRoK4JvdXgqVGtu9y3vMNIUVpCdsxqKiysaHM/Sd3kkUv7G3f6IoZsykjMlcusU41rT3OtMahJUpvHnrOxyhdvaz/Fqibv9g15PiUnKzstTet37VJtY/N+GpidrcyUFBXt2BHQ1Bjaq5cSHQ4VbgusaXhurhpcLq3b2VyT3WbTiNxcOevqtHFPc00pCQka1ru3ympqtLm8uaYMt1sFBQU</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45687</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>9.16309809196412</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45687</v>
+      </c>
+      <c r="H4">
+        <v>4.348516376332625</v>
+      </c>
+      <c r="I4">
+        <v>-0.6612457159234781</v>
+      </c>
+      <c r="J4">
+        <v>9.16309809196412</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update requirements.txt to include specific versions of torch and neuralprophet
</commit_message>
<xml_diff>
--- a/calculated_KPIs_alerts.xlsx
+++ b/calculated_KPIs_alerts.xlsx
@@ -58,13 +58,13 @@
     <t>pod_tbs</t>
   </si>
   <si>
-    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACPQklEQVR4nOzdeXxU5dn/8e9JhiwQEkwIsiv7KvtSEQREEVGwsgha1tKfu2jVanGpBSuouOvjVn1AkVYBaxU3NsFSFTEWEQSKjyyyQwhMEsg6c//+iDPJkJksJJlzBj/v18tXyzUnM9c159znPnPlnhPLGGMEAAAAAAAAOFSU3QkAAAAAAAAAZaGBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAEAYWZZV6f8GDRpkd9p+5557rizL0q5du+xOpUp87y1q1q5du2RZls4991y7UwEAABHOZXcCAAD8kkyePLlU7ODBg1q2bFnIx9u3b1+p11izZo0GDx6sgQMHas2aNaeVZyQbNGiQPvvsM61evdpRzb9gfE00Y0yNv9af//xnzZw5Uw8++KD+/Oc/1/jrAQAAVCcaWAAAhNH8+fNLxdasWeNvYAV7HNVv69atdqcAAACASqCBBQAAfnEqu6oNAAAA9uIeWAAAONzevXt16623qk2bNoqLi1NSUpIuuOACvfzyy/J4PAHbDho0SIMHD5YkffbZZwH30ip5H6IjR47o2Wef1fDhw9WiRQvFx8crMTFRvXr10qOPPqrc3Nxqy3/KlCmyLEvz58/Xxo0bNWrUKKWmpio+Pl5dunTRM888U6oOScrKytJf//pXjRo1Sm3atFGdOnVUp04dnXfeebrvvvt0/PjxgO3XrFkjy7L02WefSZIGDx4cUH/J1W1l3QOrsLBQr776qgYNGqTk5GTFxsaqRYsWuvHGG7Vnz55S2/ted9CgQSooKNCjjz6qTp06KT4+XikpKRo1alSpFV9//vOfA17/1PuelbzH2OLFi3XxxRcrJSVFtWrVUkpKijp27Kj/9//+n7777rvy3n7/88+cOVOSNHPmzIDXmjJlSsC2GRkZuvfee9WpUyfVrl1bdevWVc+ePfXYY48pJyenQq8XTGFhoR577DH/e1O/fn1dffXV2rZtW8ifycnJ0RNPPKFf/epXqlevnuLi4tSuXTvdfffdOnr0aKVzWLlypUaMGKGzzz5btWrV0llnnaU2bdpowoQJ+te//hX0Z1atWqVRo0apUaNGiomJUYMGDXTVVVfpyy+/rLa858+f798XJ06c0IwZM9S6dWvFxsaqYcOGmjx5svbt21fpegEAOJOwAgsAAAf7+uuvNWzYMGVkZKh58+b69a9/LbfbrTVr1uiLL77Qu+++q/fff18xMTGSpGHDhikuLk7Lli3T2WefrWHDhvmfq379+v7/v2zZMt12221q0qSJWrdurV/96lc6cuSIvvrqK/3xj3/Ue++9p9WrVys2Nrbaalm/fr1uvPFGNWzYUEOGDNGxY8e0Zs0a3X777fr3v/+tRYsWBTR1Nm7cqOuuu06pqalq166devbsqWPHjumbb77R7NmztWjRIq1bt04pKSmS5P+g/8knn+jQoUO69NJL1bBhQ//ztW7dutwcs7KyNHLkSK1Zs0YJCQnq2bOnUlNTtWnTJr300ktavHixVqxYoe7du5f62YKCAg0fPlxffPGFLrzwQnXo0EHr16/Xu+++q9WrV2vDhg3+JmK3bt00efJkvf7665JK3/ssISFBkjRr1iw9+OCDcrlc6tevn5o0aSK3262ffvpJr732mjp16qQuXbqUW9fkyZP17bffauPGjeratau6devmf6x///7+/79jxw5ddNFF2r17t1JTUzV8+HAVFBRo9erVuueee/T2229r5cqVOuuss8p9zVONGzdOS5cu1cCBA9WlSxetX79eixcv1scff6zly5fr/PPPD9h+//79GjZsmDZt2qTk5GT17t1bdevW1X/+8x/NnTtXixcv1po1a3TOOedU6PVff/11TZ06VZLUp08fDR48WDk5Odq7d6/eeust1a9fXxdeeGHAz9x111164oknFBUVpV69emnAgAH66aef9N5772np0qX661//6n/O6sjb7XarX79++umnnzRgwAB17txZX375pd544w199tln2rhxo5KSkirztgMAcOYwAADAVqtXrzaSzKnTcm5urjnnnHOMJHPDDTeY/Px8/2M//vijOffcc40kc++99wZ9voEDB4Z8zS1btpgvv/yyVDwjI8MMHTrUSDKPPfZYqcd9+ezcubPC9U2ePNlf30033WQKCgr8j23evNmkpqYaSeall14K+Lk9e/aYlStXGo/HExA/ceKEmTRpkv/5TjVw4EAjyaxevTpkTsHeb2OMufbaa40kc8UVV5hDhw4FPPbUU08ZSaZNmzamsLDQHy+5/7p3724OHDjgfywnJ8dceumlRpK57rrrKpyHMUX7Pz4+3iQkJJht27aVenzXrl1m69atIWs81YMPPmgkmQcffDDkNn379jWSzMiRI012drY/fvjwYdOjRw8jyVx77bUVfs2dO3f6a6xfv77ZuHGj/7HCwkJz6623GknmnHPOMbm5uf7HvF6vueCCC4wkM23aNJOZmel/rKCgwNx5551Gkhk8eHCFc2nRooWRZNauXVvqsUOHDpn//Oc/AbFXXnnFSDKtW7cOyNsYYz777DNTt25dExMTY7Zv317lvOfNm+d/ny699FLjdrv9j2VkZJhu3boZSWb27NkVrhcAgDMNDSwAAGwWqoG1YMECI8k0btw44MO9z5IlS4wkU7duXZOTk1Pq+cpqYJXlv//9r5FkevfuXeqxqjSwGjVqFJCnz3PPPedvDFXUiRMnjMvlMqmpqaUeO90G1pYtW4xlWaZx48YBjYeShg8fbiSZpUuX+mO+99uyLPPtt9+W+pl169YZSaZly5YVysPn8OHDRpLp0qVLyDoqo7wG1tq1a40kU7t2bXPw4MFSj6elpRlJJioqyuzZs6dCr1mygfX000+Xejw3N9c0adLESDILFy70xz/++GMjyXTr1i2g4enj8XhM586djSSzadOmCuVSu3Ztk5SUVKFtPR6Pady4sZFk0tLSgm7z2GOPGUnmzjvvrHLevgZWnTp1zP79+0v93FtvvWUkmYsuuqhC+QMAcCbiHlgAADjUmjVrJEnjx48P+lW+UaNG6ayzzlJWVpa++eabSj+/x+PRqlWr9NBDD+mmm27S1KlTNWXKFD388MOSpP/+979Vyv9UV199teLi4krFfV+f++GHH7R///5Sj3/xxRd69NFHdfPNN/tzvOmmmxQTE6MjR47o2LFj1ZLfRx99JGOMLrvsMtWtWzfoNoMGDfLndKrmzZura9eupeIdOnSQpErfwyg1NVXnnnuuvvvuO915553asmVLpX6+snzH27Bhw3T22WeXerxnz57q2rWrvF6v/z5jlXHq1yQlKTY2VuPGjQt4fUn68MMPJUmjR4+Wy1X6jhdRUVH+r/sF2xfB9OnTR263W5MmTdI333wjr9cbctsNGzZo//79atWqlXr27Bl0m2DHQlXz7tWrlxo1alQqfrrHEAAAZxLugQUAgEP5Pqy2aNEi6OOWZalFixY6duxYpT/Y/vDDD7rqqqv0/fffh9wmMzOzUs9ZnlB11K1bVykpKTp69Kj27t2rxo0bS5IOHz6s0aNH69///neZz5uZmXla92Q61Y4dOyRJr732ml577bUytz1y5EipWPPmzYNum5iYKEnKy8urdE5vvPGGxowZoyeffFJPPvmkkpOT1bdvX11yySWaOHFiwH3Nqqq8402SWrVqpY0bN1b6eKtXr57q1asX9DHf6+3du9cf8+2LBx54QA888ECZzx1sXwTzwgsv6IorrtCCBQu0YMEC1a1bV71799ZFF12kiRMnBuw/3+v/+OOPIW/2H+z1q5p3ecdQdf5xBQAAIg0NLAAAfoHGjBmj77//XldccYXuvvtudezYUYmJiapVq5by8/Or9ebtlWGM8f//3/3ud/r3v/+t888/XzNnzlTXrl111llnqVatWpKkxo0b68CBAwE/UxW+FTndunULupKqpL59+5aKRUVV/8L2AQMGaNeuXfrwww/12Wef6YsvvtCyZcv08ccf68EHH9S7776rIUOGVPvr2qHkfvTti/79+6tVq1Zl/lynTp0q9PwdOnTQf//7Xy1fvlyffvqpvvjiC61du1affvqpZs2apddee00TJkwIeP2GDRvq0ksvLfN5SzYRq5p3TRxDAACcKWhgAQDgUE2aNJFUvKojmJ07dwZsWxHbtm3Td999pwYNGujdd98t9VWnH3744TSyLZ8v11NlZWXp6NGjkqSmTZtKkk6cOKGPPvpIUVFR+uijj0qt3jlx4oQOHjxYrfk1a9ZMknTBBRfo+eefr9bnror4+HiNGTNGY8aMkVS0cuf+++/XK6+8ot/+9rfavXt3tbxORY4332OVOd4k6fjx4zp+/HjQVVi7du2SVLzvpeJ9ceWVV+quu+6q1GuVxeVyafjw4Ro+fLikotV7Tz75pGbOnKnrr79eV111lerUqeN//ZSUFM2fP7/Cz19TeQMAAIlf8wAA4FC+e+y8/fbbQb869O677+rYsWOqW7duwH16YmJiJEmFhYVBnzcjI0NS0QqmYPfpefPNN6uaelCLFy8O+jW6BQsWSJJat27tb4y43W55PB4lJiYGbXq8+eabIVdelVd/KJdddpkk6f333w/bV7V8q8kqk2tqaqoee+wxSdJPP/1U4XuAlfe++I63Tz75RIcOHSr1+IYNG/Ttt98G3MepMnz7uaT8/Hy9/fbbAa8vFe+LxYsXV9sKu2ASExP15z//WfXq1dPJkye1fft2SVLv3r1Vv359bdmypcyv2Z4qXHkDAPBLRAMLAACHGjt2rJo3b679+/frjjvuCGg87Ny5U3feeack6dZbbw24ObpvJcsPP/yggoKCUs/btm1bRUdHa9OmTQE3zpakpUuX6qmnnqqBaqT9+/frrrvuksfj8ce2bt2qWbNmSZJ+//vf++Nnn322zjrrLB0/frxU42PdunWaMWNGyNfx1V+ZxoMkde/eXaNHj9aePXs0atQo/8qgkk6cOKGFCxcGbfCcjrJy3b17t1599dWg9yJbunSpJOmss87y3x+pKq8lFX3trW/fvsrJydH111+vkydP+h9LT0/X9ddfL6nojwr4VhpVxkMPPaTNmzf7/+31enXPPfdo7969atasmUaPHu1/7Morr1Tv3r21fv16TZ06Nej9oo4dO6aXXnqpQs2/kydP6sknnwz6PGvXrtXx48cVHR3tf49q1aqlBx98UMYYXXXVVUHvw+bxePTpp59q3bp1NZY3AAAowb4/gAgAAIwxZvXq1UaSCTYtr1+/3iQnJxtJ5pxzzjHjxo0zw4cPN3FxcUaSufTSS01eXl6pn+vVq5eRZNq1a2d+85vfmGnTppl77rnH//htt91mJJmoqCgzcOBAc80115gePXoYSeb+++8Pmc8555xjJJmdO3dWuL7JkycbSeaGG24wcXFxpkWLFmb8+PHm0ksvNTExMUaSueqqq4zX6w34uaeeesqfR9++fc0111xjLrjgAmNZlpk4cWLIXD744AMjycTExJgrrrjC/Pa3vzXTpk0zn3/+uX+bUPVlZmaaIUOG+H++d+/e5uqrrzZjx441vXv39ue7detW/8/49t/AgQNDvgehXu+uu+4ykkz9+vXN1VdfbaZNm2amTZtm0tPTzYYNG4wkU6tWLX8eV199tenevbuRZCzLMq+++moF94IxBw8eNHXq1DGSzAUXXGCmTJlipk2bZv73f//Xv82PP/7of18bNGhgxowZY6688kqTmJhoJJkePXqYjIyMCr/mzp07jSTTvHlzc9VVV5latWqZSy65xIwfP960atXKSDJ16tQxa9euLfWz+/btM926dfNv069fPzN+/HgzatQo061bNxMdHW0kmZycnHLzOHbsmP9479q1qxkzZoy55pprzPnnn28syzKSzJ/+9KdSP/eHP/zBv+86depkrrzySjN+/HgzaNAgU69ePSPJvPjii1XOe968eUaSmTx5cpnv4znnnFNurQAAnKloYAEAYLOyGljGGPPTTz+Zm2++2bRs2dLExMSYunXrmvPPP9+8+OKLpqCgIOjP7N6921x77bWmUaNGxuVylfrw6/V6zWuvvWZ69uxpEhISTFJSkunfv7956623jDGhGy5VaWDNmzfP/Oc//zEjRowwKSkpJjY21nTq1Mk8+eSTIev45z//afr162fq1atnEhISTK9evcwLL7xgvF5vmbn89a9/NT169DC1a9f21zJv3jz/42W93x6Px/ztb38zw4cPN2effbapVauWSUlJMZ07dzZTp0417777rsnPz/dvX5UGVk5Ojrn77rtN69at/c0xX02ZmZnm6aefNldddZVp06aNSUhIMHXq1DFt27Y1kyZNMmlpaSFfL5R//etf5uKLLzZnnXWWiYqKCto0OXr0qJkxY4bp0KGDiYuLM7Vr1zbdu3c3jzzyiDl58mSlXq9k46WgoMA8/PDDpn379iY2NtYkJyeb0aNHm++//z7kz+fm5pqXXnrJDB482KSkpBiXy2UaNGhgunXrZm6++WazbNmyCuVRUFBgXnrpJXPNNdeY9u3bm6SkJBMfH29atWplRo8ebVatWhXyZz///HPzm9/8xpxzzjkmNjbW1K1b17Rt29b8+te/Nq+++mrQhl5l86aBBQBA+Sxj+II+AACoOVOmTNHrr7+uefPmacqUKXanAwAAgAjEPbAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBo3AMLAAAAAAAAjsYKLAAAAAAAADgaDSwAAAAAAAA4msvuBE6H1+vV/v37VbduXVmWZXc6AAAAAAAAKIMxRllZWWrcuLGioiq/nioiG1j79+9Xs2bN7E4DAAAAAAAAlbBnzx41bdq00j8XkQ2sunXrSioqOjEx0eZsAAAAAAAAUJbMzEw1a9bM39OprIhsYPm+NpiYmEgDCwAAAAAAIEKc7q2guIk7AAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAABwtIv8KIQAAAAAACD9jjDwejwoLC+1OBQ7hcrkUHR192n9dsMKvU6PPDgAAAAAAIp4xRsePH9eRI0fk8XjsTgcOEx0drQYNGigpKanGGlk0sAAAAAAAQJkOHjyo48ePKzExUYmJiXK5XDW+4gbOZ4xRYWGhMjMzdeDAAeXk5KhRo0Y18lo0sAAAAAAAQEgej0dut1upqamqX7++3enAgerWravY2Filp6erQYMGio6OrvbX4CbuAAAAAAAgpIKCAhljVKdOHbtTgYPVqVNHxhgVFBTUyPPTwAIAAAAAAOXiK4MoS00fHzSwAAAAAAAA4Gg0sAAAAAAAABDUlClTdO6559qdBg0sAAAAAADwyzV//nxZlhXyv3Xr1tmdYrm2bNmiP//5z9q1a5fdqdQY/gohAAAAAAD4xZs1a5ZatGhRKt66dWsbsqmcLVu2aObMmRo0aJAjVkvVBBpYAAAAAADgtC3fbHcG0tDOVX+Oyy67TL169ar6E6FG8BVCAAAAAACAMjz44IOKiorSqlWrAuLXXXedYmJitHHjRknSmjVrZFmW3n77bd17771q2LCh6tSpo5EjR2rPnj2lnverr77SsGHDlJSUpNq1a2vgwIH6/PPPS223b98+TZs2TY0bN1ZsbKxatGihG2+8Ufn5+Zo/f77Gjh0rSRo8eLD/q49r1qzx//zHH3+sAQMGqE6dOqpbt64uv/xyff/996Ve55///Kc6d+6suLg4de7cWe+++25V3rZqxQosAAAAAADwi+d2u5Wenh4QsyxLKSkpuv/++7V06VJNmzZNmzZtUt26dbVs2TL99a9/1UMPPaSuXbsG/NzDDz8sy7J0zz336PDhw3r66ad18cUX69tvv1V8fLwk6dNPP9Vll12mnj17+htk8+bN00UXXaS1a9eqT58+kqT9+/erT58+On78uK677jq1b99e+/bt05IlS3Ty5EldeOGFmj59up599lnde++96tChgyT5/3fBggWaPHmyLr30Uj366KM6efKkXnzxRfXv318bNmzwf+Vw+fLlGj16tDp27Kg5c+bo6NGjmjp1qpo2bVqTb3uFWcYYY3cSlZWZmamkpCS53W4lJibanQ4AAAAAAGes3Nxc7dy5Uy1atFBcXFypxyP9K4Tz58/X1KlTgz4WGxur3NxcSdLmzZvVs2dPTZo0SXPnzlXnzp3VqFEjffnll3K5itYHrVmzRoMHD1aTJk20detW1a1bV5K0ePFiXX311XrmmWc0ffp0GWPUrl07tWzZUh9//LEsy5Ik5eTkqFOnTmrdurWWL18uSZo8ebLefPNNffXVV6W+4miMkWVZWrJkicaOHavVq1dr0KBB/sezs7PVrFkzjR07Vq+88oo/fujQIbVr105XX321P969e3cdOnRIW7duVVJSkiRpxYoVGjp0qM4555xybxBf3nFS1V4OK7AAAAAAAMAv3v/8z/+obdu2AbHo6Gj//+/cubNmzpypGTNm6LvvvlN6erqWL1/ub16VNGnSJH/zSpLGjBmjRo0a6aOPPtL06dP17bff6ocfftD999+vo0ePBvzskCFDtGDBAnm9XklFX+sbMWJE0Ptz+RpfoaxYsULHjx/XNddcE7C6LDo6Wn379tXq1aslSQcOHNC3336rP/7xj/7mlSRdcskl6tixo06cOFHm64QDDSwAAAAAAPCL16dPn3Jv4v6HP/xBb731ltavX6/Zs2erY8eOQbdr06ZNwL8ty1Lr1q39q5h++OEHSUWrq0Jxu93Kz89XZmamOnc+vSVmvte56KKLgj7uWwm1e/fuoHlLUrt27fSf//zntF6/OtHAAgAAACKAE76i41ORr+pEWr4AUBE7duzwN4U2bdp02s/jW101d+5cdevWLeg2CQkJysjIOO3XKPk6CxYsUMOGDUs9Hmz1mFNFTqYAAAAAAAA28Xq9mjJlihITE3X77bdr9uzZGjNmjEaNGlVqW1+Ty8cYo//7v/9Tly5dJEmtWrWSVLQC6uKLLw75mqmpqUpMTNTmzWX/ViDUVwl9r9OgQYMyX+ecc84Jmrck/fe//y3ztcMlyu4EAAAAAAAAnO7JJ5/UF198oVdeeUUPPfSQ+vXrpxtvvLHUXy6UpDfeeENZWVn+fy9ZskQHDhzQZZddJknq2bOnWrVqpccff1zZ2dmlfv7IkSOSpKioKP3617/W0qVLlZaWVmo739/lq1OnjiTp+PHjAY9feumlSkxM1OzZs1VQUBDydRo1aqRu3brp9ddfl9vt9j++YsUKbdmypcz3JVxYgQUAAAAAAH7xPv74Y23btq1UvF+/fsrLy9MDDzygKVOmaMSIEZKK/npht27ddNNNN2nRokUBP5OcnKz+/ftr6tSpOnTokJ5++mm1bt1a/+///T9JRY2pV199VZdddpk6deqkqVOnqkmTJtq3b59Wr16txMRELV26VJI0e/ZsLV++XAMHDtR1112nDh066MCBA1q8eLH+/e9/q169eurWrZuio6P16KOPyu12KzY2VhdddJEaNGigF198URMnTlSPHj00fvx4paam6qefftKHH36oCy64QM8//7wkac6cObr88svVv39//fa3v1VGRoaee+45derUKWiTLdxoYAEAAAAAgF+8P/3pT0Hjr776ql5++WXVr19fTz/9tD/epk0bzZkzR7fddpsWLVqkq6++2v/Yvffeq++++05z5sxRVlaWhgwZohdeeEG1a9f2bzNo0CB9+eWXeuihh/T8888rOztbDRs2VN++fXX99df7t2vSpIm++uorPfDAA1q4cKEyMzPVpEkTXXbZZf7na9iwoV566SXNmTNH06ZNk8fj0erVq9WgQQNde+21aty4sR555BHNnTtXeXl5atKkiQYMGKCpU6f6X2fYsGFavHix7r//fs2YMUOtWrXSvHnz9N5772nNmjXV9C6fPsv41ptFkMzMTCUlJcntdvvvmA8AAACcySLtpuiRli+A0HJzc7Vz5061aNFCcXFxdqfjaGvWrNHgwYO1ePFijRkzxu50wqq846SqvRzugQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEfjJu4AAAAAAADVYNCgQYrAW41HBFZgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAACAX6z58+fLsizFxcVp3759pR4fNGiQOnfubENmKMlldwIAAAAAACCCffKJ3RlIw4ZV+Sny8vL0yCOP6LnnnquGhFDdWIEFAAAAAAB+8bp166a//vWv2r9/v92pIAgaWAAAAAAA4Bfv3nvvlcfj0SOPPFLmdoWFhXrooYfUqlUrxcbG6txzz9W9996rvLw8/zZ33HGHUlJSZIzxx2699VZZlqVnn33WHzt06JAsy9KLL75Y/QWdYWhgAQAAAACAX7wWLVpo0qRJ5a7C+t3vfqc//elP6tGjh5566ikNHDhQc+bM0fjx4/3bDBgwQBkZGfr+++/9sbVr1yoqKkpr164NiEnShRdeWAMVnVloYAEAAAAAAEi67777VFhYqEcffTTo4xs3btTrr7+u3/3ud1q8eLFuuukmvf7667rrrrv0z3/+U6tXr5Yk9e/fX1Jxg8rtdmvTpk0aPXp0qQZWcnKyOnbsWMOVRT4aWAAAAAAAAJJatmypiRMn6pVXXtGBAwdKPf7RRx9JKvqKYEl33nmnJOnDDz+UJKWmpqp9+/b617/+JUn6/PPPFR0drT/84Q86dOiQfvjhB0lFDaz+/fvLsqwaq+lMwV8hBAAAAPCLtnyz3RkUG9rZ7gwA3H///VqwYIEeeeQRPfPMMwGP7d69W1FRUWrdunVAvGHDhqpXr552797tjw0YMMDf8Fq7dq169eqlXr16KTk5WWvXrtXZZ5+tjRs36tprr635os4ArMACAAAAAAD4WcuWLTVhwoSQq7AkVWjFVP/+/bVv3z7t2LFDa9eu1YABA2RZlvr376+1a9fqiy++kNfr1YABA6q7hDMSDSwAAAAAAIAS7r///qD3wjrnnHPk9Xr9XwH0OXTokI4fP65zzjnHH/M1plasWKGvv/7a/+8LL7xQa9eu1dq1a1WnTh317Nmzhqs5M9DAAgAAAAAAKKFVq1aaMGGCXn75ZR08eNAfHz58uCTp6aefDtj+ySeflCRdfvnl/liLFi3UpEkTPfXUUyooKNAFF1wgqaix9eOPP2rJkiX61a9+JZeLuztVBO+SU7zxht0ZFJs0ye4MAAAAAACw1X333acFCxbov//9rzp16iRJ6tq1qyZPnqxXXnlFx48f18CBA7V+/Xq9/vrr+vWvf63BgwcHPMeAAQP01ltv6bzzztNZZ50lSerRo4fq1Kmj7du3c/+rSmAFFgAAAAAAwClat26tCRMmlIq/+uqrmjlzpr7++mvdfvvt+vTTTzVjxgy99dZbpbb1fW2wf//+/pjL5dL5558f8DjKZxljjN1JVFZmZqaSkpLkdruVmJhodzrVgxVYAAAAYRdJf30uknKVIivfSMoVsENubq527typFi1aKC4uzu504FDlHSdV7eWwAgsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjlblBtb333+vsWPHqmXLlqpdu7bq16+vCy+8UEuXLi217datWzVs2DAlJCQoOTlZEydO1JEjR6qaAgAAAAAAAM5grqo+we7du5WVlaXJkyercePGOnnypN555x2NHDlSL7/8sq677jpJ0t69e3XhhRcqKSlJs2fPVnZ2th5//HFt2rRJ69evV0xMTJWLAQAAAAAAwJmnyg2s4cOHa/jw4QGxW265RT179tSTTz7pb2DNnj1bJ06c0DfffKPmzZtLkvr06aNLLrlE8+fP928HAAAAAAAAlFQj98CKjo5Ws2bNdPz4cX/snXfe0RVXXOFvXknSxRdfrLZt22rRokU1kQYAAAAAAADOAFVegeVz4sQJ5eTkyO126/3339fHH3+scePGSZL27dunw4cPq1evXqV+rk+fPvroo4+qKw0AAAAAAACcYaqtgXXnnXfq5ZdfliRFRUVp1KhRev755yVJBw4ckCQ1atSo1M81atRIGRkZysvLU2xsbNDnzsvLU15env/fmZmZkqTCwkIVFhb6XzMqKkper1der9e/rS/u8XhkjCk3Hh0dLcuy/M9bMi5JHo+nQnGXyyVjTEDcsixFR0eXytGyLEVL8v78nz/Hn/8LFfdIMhWIR0uyJAVWVBTXz9sHxH9+P6pcU5B4xO8naqImaqImaqImajqjajIlL7Ksn6+OzClXRyHiVlRRTYFxS1ZUtIzx6pQnDx63omRZUTLGq8LCsmsy3hLbe0+54rOKajLeU674aqimwsLy91PIWkvlHp6ayjr2itMsfz/VdE0lh1qkjaeSzpRzBDUVxQsLC4vPRSWet2T+TopXhtNyj+SapKLjo2SvpuSxd+rxV1nV1sC6/fbbNWbMGO3fv1+LFi2Sx+NRfn6+JCknJ0eSgjao4uLi/NuEamDNmTNHM2fOLBXfsGGD6tSpI0lKTU1Vq1attHPnzoC/bNi0aVM1bdpU27dvl9vt9sdbtmypBg0aaPPmzf78JKl9+/aqV6+eNmzYEDCIu3TpopiYGKWlpQXk0KtXL+Xn5+u7777zx6Kjo9W7d2+53W5t27bNH4+Pj1fXrl2Vnp6uHTt2+ONJSUnqIGl/rVraW6uWP55aWKhW+fnaGROjI67iXdW0oEBNCwq0PTZW7uhof7xlfr4aFBZqc1yccqKKvx3aPjdX9bxebYiPl8eyimvKyVGMMUqrXTuwpp/3XZVr6tBB+/fv1969e4trivT9RE3URE3URE3URE1nVE35x4trqlW/i6zoGOUfCqwp5uxeMp58FaQX12RZ0Ypp2Fsm362CjOKaLFe8YlK7ypuTrkJ3cU1RsUmqldxBnuz98mQX1xQdnypXvVbyuHcqLa3smvKzJFdSS0XXbqCCo5tlCotrqpXcXlZsPRUc3iBjar6mtJPl7yePe6c8OcU1RSc0latuUxUe3y5vXvF+CkdN5R17+VkV3081XVPayeKaIm08nYnnCGoqrsn32d3j8Sg3N9cfj4qKUu3atVVYWBiw8CQ6Olrx8fEqKCjw9wakosZeXFyc8vLyAhoaMTExiomJUW5ubkCOsbGxqlWrlnJycgKaeHFxcXK5XDp58mRAMyU+Pl5RUVE6ceJEQE116tSR1+sNeF8sy1KdOnVqvKaoqCjNmDFD99577xlTU7D9JEkFBQXavHmzP17y2PMtRjpdlqlqay+EoUOH6vjx4/rqq6/0zTffqHfv3nrjjTc0ceLEgO3uvvtuzZ07V7m5uZVagdWsWTMdPXpUiYmJkpzTmfapdLd94ULnrMD6eR+dyb9BoCZqoiZqoiZqoiZqKiws1KotJZK0eQXWkA5l17RqS4ntbV6BNaRj+ftp2SbnrMC6pFPZx17xcWD/CqwhHYvDkTaeSjpTzhHUVBTPzc3VTz/9pJYtWwb93B7Jq5WiSiz+KMunn36qQYMGnVaOlmXpT3/6k/785z9XaPtIXYGVl5enHTt2qHnz5v6GZ8ljLzMzUykpKXK73f5eTmVU2wqsU40ZM0bXX3+9tm/f7v/qoO+rhCUdOHBAycnJIZtXUlEnL9jjLpdLLldgCb4BeyrfAKxo/NTnPZ24ZVlB46Fy9DWgKhoPnnnoeKidXSr+8yqtaqmpkvGI2E/URE0hcqxsnJqoSaKmUDlWNk5N1CSdXk1WsIssK8RVU5C4ZVkh4lEK9uRlxV2usmsq+WNWVPCarKiK5x4qXpGaSu7GUPsjZK0hc6/Zmso69k5Ns9L7rxprCjakImU8VTVOTc6tyeVyFZ0bJP//Bvi//1OQaNH24Yq3bh1ii7ItWLAg4N9vvPGGVqxYUSresWPHst+DMuK+x059/HSep6Iq+9zVGQ/WqwkWq6waa2D5lrC53W61a9dOqamppZYlStL69evVrVu3mkoDAAAAAAAgqAkTJgT8e926dVqxYkWpOOxXsbVyZTh8+HCpWEFBgd544w3Fx8erY8eiNbCjR4/WBx98oD179vi3W7VqlbZv366xY8dWNQ0AAAAAAIBqd+LECd15551q1qyZYmNj1a5dOz3++OOlvkaXl5en3//+90pNTVXdunU1cuTIgHua+ezevVs33XST2rVrp/j4eKWkpGjs2LHatWuXf5sdO3bIsiw99dRTpX7+iy++kGVZ+vvf/17ttTpZlVdgXX/99crMzNSFF16oJk2a6ODBg1q4cKG2bdumJ554QgkJCZKke++9V4sXL9bgwYN12223KTs7W3PnztV5552nqVOnVrkQAAAAAACA6mSM0ciRI7V69WpNmzZN3bp107Jly/SHP/xB+/btC2gw/e53v9Obb76pa6+9Vv369dOnn36qyy+/vNRzfv311/riiy80fvx4NW3aVLt27dKLL76oQYMGacuWLapdu7ZatmypCy64QAsXLtTvf//7gJ9fuHCh6tatqyuvvLLG63eSKjewxo0bp9dee00vvviijh49qrp166pnz5569NFHNXLkSP92zZo102effaY77rhDf/zjHxUTE6PLL79cTzzxRJn3vwIAAAAAALDD+++/r08//VR/+ctfdN9990mSbr75Zo0dO1bPPPOMbrnlFrVq1UobN27Um2++qZtuukn/8z//49/uN7/5TcBfc5Skyy+/XGPGjAmIjRgxQueff77eeecd/x+/mzRpkq6//npt27ZN7du3l1T0jbdFixZp1KhRql27dk2X7yhV/grh+PHjtWLFCh08eFAFBQXKyMjQihUrAppXPp06ddKyZct04sQJHTt2TG+++abOPvvsqqYAAAAAAABQ7T766CNFR0dr+vTpAfE777xTxhh9/PHH/u0kldru9ttvL/Wc8fHx/v9fUFCgo0ePqnXr1qpXr57+85//+B+7+uqrFRcXp4ULF/pjy5YtU3p6+i/yHl1VbmABAAAAAACciXbv3q3GjRurbt26AfEOHTr4H/f9b1RUlFq1ahWwXbt27Uo9Z05Ojv70pz/576lVv359paam6vjx43K73f7t6tWrpxEjRuhvf/ubP7Zw4UI1adJEF110UbXVGCloYAEAAAAAAITJrbfeqocfflhXX321Fi1apOXLl2vFihVKSUmR1+sN2HbSpEnasWOHvvjiC2VlZen999/XNddco6ioX147p8r3wAIAAAAAADgTnXPOOVq5cqWysrICVmFt27bN/7jvf71er3788ceAVVf//e9/Sz3nkiVLNHnyZD3xxBP+WG5uro4fP15q22HDhik1NVULFy5U3759dfLkSf89sn5pfnktOwAAAAAAgAoYPny4PB6Pnn/++YD4U089JcuydNlll0mS/3+fffbZgO2efvrpUs8ZHR0tY0xA7LnnnpPH4ym1rcvl0jXXXKNFixZp/vz5Ou+889SlS5eqlBSxWIEFAAAAAAAQxIgRIzR48GDdd9992rVrl7p27arly5frvffe0+233+6/51W3bt10zTXX6IUXXpDb7Va/fv20atUq/d///V+p57ziiiu0YMECJSUlqWPHjvryyy+1cuVKpaSkBM1h0qRJevbZZ7V69Wo9+uijNVqvk9HAAgAAAAAACCIqKkrvv/++/vSnP+ntt9/WvHnzdO6552ru3Lm68847A7b93//9X//X/f75z3/qoosu0ocffqhmzZoFbPfMM88oOjpaCxcuVG5uri644AKtXLlSl156adAcevbsqU6dOmnr1q36zW9+U2O1Op1lTl23FgEyMzOVlJQkt9utxMREu9OpHm+8YXcGxSZNsjsDAACAsFi+2e4Mig3tXPbjkZSrFFn5RlKugB1yc3O1c+dOtWjRQnFxcXan84vUvXt3JScna9WqVXanElJ5x0lVezncAwsAAAAAAMCh0tLS9O2332rSL3yxCV8hBAAAAAAAcJjNmzfrm2++0RNPPKFGjRpp3LhxdqdkKxpYAAAAABBB+Moj8MuwZMkSzZo1S+3atdPf//73X/zXN/kKIQAAAAAAgMP8+c9/ltfr1datWzVw4EC707EdDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAUC5jjN0pwMFq+viggQUAAAAAAEKKjo6WJBUUFNicCZzMd3z4jpfqRgMLAAAAAACEVKtWLcXGxsrtdrMKC0EZY+R2uxUbG6tatWrVyGu4auRZAQAAAADAGaN+/frat2+f9u7dq6SkJNWqVUuWZdmdFmxmjFFBQYHcbreys7PVpEmTGnstGlgAAAAAAKBMiYmJkqT09HTt27fP5mzgNLGxsWrSpIn/OKkJNLAAAAAAAEC5EhMTlZiYqIKCAnk8HrvTgUNER0fX2NcGS6KBBQAAAAAAKqxWrVphaVgAJXETdwAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADiay+4EAAAAcOZYvtnuDIoN7Wx3BgAAoLqwAgsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACOxk3cAQAAAAA1gj/sAKC6sAILAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACORgMLAAAAAAAAjkYDCwAAAAAAAI5GAwsAAAAAAACOVuUG1tdff61bbrlFnTp1Up06ddS8eXNdffXV2r59e8B2U6ZMkWVZpf5r3759VVMAAAAAAADAGcxV1Sd49NFH9fnnn2vs2LHq0qWLDh48qOeff149evTQunXr1LlzZ/+2sbGxevXVVwN+PikpqaopAAAAAAAA4AxW5QbWHXfcob/97W+KiYnxx8aNG6fzzjtPjzzyiN58883iF3O5NGHChKq+JAAAAAAAAH5BqvwVwn79+gU0rySpTZs26tSpk7Zu3Vpqe4/Ho8zMzKq+LAAAAAAAAH4hauQm7sYYHTp0SPXr1w+Inzx5UomJiUpKSlJycrJuvvlmZWdn10QKAAAAAAAAOENU+SuEwSxcuFD79u3TrFmz/LFGjRrp7rvvVo8ePeT1evXJJ5/ohRde0MaNG7VmzRq5XKFTycvLU15env/fvhVchYWFKiwslCRFRUUpKipKXq9XXq/Xv60v7vF4ZIwpNx4dHS3LsvzPWzIuFa0gq0jc5XLJGBMQtyxL0dHRpXK0LEvRkrw//+fP8ef/QsU9kkwF4tGSLEmBFRXF9fP2AfGf348q1xQkHvH7iZqoiZqoiZqoiZrKzN2Yn68wTGDciiqqKTBuyYqKljFeyXjLj1tRsqyo0HFv4FWQ11t+TYEvGzz3UPHqrqmwsOz9ZLyha5VVVJPxnnLFV0M1FRaWf+xVdD+Fq6ayxlNxmtVz7FWlppJDLdQ4k8I/nkLFjSn7HFG0ffBaA8JhOEdwLqcmarK3plPrqqxqb2Bt27ZNN998s84//3xNnjzZH58zZ07AduPHj1fbtm113333acmSJRo/fnzI55wzZ45mzpxZKr5hwwbVqVNHkpSamqpWrVpp586dOnLkiH+bpk2bqmnTptq+fbvcbrc/3rJlSzVo0ECbN29WTk6OP96+fXvVq1dPGzZsCNjZXbp0UUxMjNLS0gJy6NWrl/Lz8/Xdd9/5Y9HR0erdu7fcbre2bdvmj8fHx6tr165KT0/Xjh07/PGkpCR1kLS/Vi3trVXLH08tLFSr/HztjInRkRINvqYFBWpaUKDtsbFyR0f74y3z89WgsFCb4+KUE1W8uK59bq7qeb3aEB8vj2UV15SToxhjlFa7dmBNHk/11NShg/bv36+9e/cW1xTp+4maqImaqImaqImayqxJtXvJePJVkF5ck2VFK6Zhb5l8twoyimuyXPGKSe0qb066Ct3FNUXFJqlWcgd5svfLk11cU3R8qlz1Wsnj3ilPTnFN0QlN5arbVIXHt8ubV1xTesPya8o/XlxTrfpdZEXHKP9QYE0xZ4enprS0svdTfpbkSmqp6NoNVHB0s0xhcU21ktvLiq2ngsMbZEzN15R2svxjr6L7KRw1lTee8rMqvp9quqa0k8U1hTpHKD784ylUTe7mZZ8j7BpPwWriXE5N1GRvTVW9nZRlSrbGqujgwYO64IILVFBQoHXr1qlx48Zlbp+Tk6OEhARNnTq11F8nLCnYCqxmzZrp6NGjSkxMlHQGdDwXLnTOCqyJE6unJjrT1ERN1ERN1ERNv7iaVm11zgqsSzqXX9OqLSVf1t4VWEM6lL2fVm0JXWu4V2AN6Vj+sbdsk3NWYF3SqezxVHwc2L8Ca0jH4nCocfbpNueswBp6XtnniOWbnLMCa0gHzuXURE121pSZmamUlBS53W5/L6cyqm0Fltvt1mWXXabjx49r7dq15TavpKIOYEpKijIyMsrcLjY2VrGxsaXiLper1FcPfW/aqXw7tqLxUF9prEzcsqyg8VA5+hpQFY0Hzzx0PNTOLhX/eZVWtdRUyXhE7CdqoqYQOVY2Tk3UJFFTqBwrG6cm59TkX+xtBa8peDxKskrnWOl4VGDuvrLLqinI0wTNMVS8OmtyucreTyV/7NRai+MVzz1UvCI1ldztoY6xiu6n8uPVU1NZ4+nUNKt67JUfD517sKEW6hwRzvEUKu4b86HOEZXZfzVdE+dyagoVp6bw1FTWraMqoloaWLm5uRoxYoS2b9+ulStXqmPHjuX/kKSsrCylp6crNTW1OtIAAAAAAOC0Ld9sdwbFhna2OwPAWarcwPJ4PBo3bpy+/PJLvffeezr//PNLbZObm6uCggLVrVs3IP7QQw/JGKNhw4ZVNQ0AAAAAAACcoarcwLrzzjv1/vvva8SIEcrIyNCbb74Z8PiECRN08OBBde/eXddcc43at28vSVq2bJk++ugjDRs2TFdeeWVV0wAAAAAAAMAZqsoNrG+//VaStHTpUi1durTU4xMmTFC9evV0xRVXaMWKFXr99dfl8XjUunVrzZ49W3fddVfQ71MCAAAAAAAAUjU0sNasWVPuNvXq1dOCBQuq+lIAAAAAAAD4BWLpEwAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAcjQYWAAAAAAAAHI0GFgAAAAAAAByNBhYAAAAAAAAczWV3AgAAAAAAoHKWb7Y7g2JDO9udAX4JWIEFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR3PZnQAAAADKtnyz3RkUG9rZ7gwAAMAvESuwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoLrsTQJEf0+3OoFgruxMAAAAAAAAogRVYAAAAAAAAcDRWYAEAAAAAgBq1fLPdGRQb2tnuDHA6WIEFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABH4x5YqDS+uwwAAAAAAMKJFVgAAAAAAABwNBpYAAAAAAAAcDQaWAAAAAAAAHA0GlgAAAAAAABwNBpYAAAAAAAAcDQaWAAAAAAAAHA0GlgAAAAAAABwNBpYAAAAAAAAcDSX3QkAAAAAAAA4xfLNdmdQbGhnuzNwDlZgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNGq3MD6+uuvdcstt6hTp06qU6eOmjdvrquvvlrbt28vte3WrVs1bNgwJSQkKDk5WRMnTtSRI0eqmgIAAAAAAADOYK6qPsGjjz6qzz//XGPHjlWXLl108OBBPf/88+rRo4fWrVunzp07S5L27t2rCy+8UElJSZo9e7ays7P1+OOPa9OmTVq/fr1iYmKqXAwQzPLNdmdQbGhnuzMAAAAAACDyVLmBdccdd+hvf/tbQANq3LhxOu+88/TII4/ozTfflCTNnj1bJ06c0DfffKPmzZtLkvr06aNLLrlE8+fP13XXXVfVVAAAAAAAAHAGqvJXCPv161dq9VSbNm3UqVMnbd261R975513dMUVV/ibV5J08cUXq23btlq0aFFV0wAAAAAAAMAZqkZu4m6M0aFDh1S/fn1J0r59+3T48GH16tWr1LZ9+vTRhg0baiINAAAAAAAAnAGq/BXCYBYuXKh9+/Zp1qxZkqQDBw5Ikho1alRq20aNGikjI0N5eXmKjY0N+nx5eXnKy8vz/zszM1OSVFhYqMLCQklSVFSUoqKi5PV65fV6/dv64h6PR8aYcuPR0dGyLMv/vCXjkuTxeCoUd7lcMsYExC3LUnR0dKkcLcuSJBlJxirxJKaow+iVpBJxyxT901ty29OM69TXlPzvR6iajLdk3JIVFS1jvJLxlh+3omRZUaHjXs/P70R58YrvJ+Mt2r7oH4E1WVFFNQXGa66mwkLnHXvB4pE+nqiJmqiJms60mszPFwN2zrnGW1STr7RQuRvjjDlXkrze8vdT4MsGzz1c1xGFhWUfe0XXNBXbTzVdU2Fh+eOpuo+9qtZU1jmiOM3wjqdguZc8fYQaZ1L4x1OouDFln/cCPzsobOMpWLwi53LfZ4dwjqdQ8ZKfHYKNM8m+8XRqTVL5c66/3DCOp1DxkodrsOsI43XGnCsVHQdnyrXRqeeJyqr2Bta2bdt088036/zzz9fkyZMlSTk5OZIUtEEVFxfn3yZUA2vOnDmaOXNmqfiGDRtUp04dSVJqaqpatWqlnTt3Bvxlw6ZNm6pp06bavn273G63P96yZUs1aNBAmzdv9ucnSe3bt1e9evW0YcOGgJ3dpUsXxcTEKC0tLSCHXr16KT8/X999950/Fh0drd69e8vtdmvbtm3+eHx8vLp27ar09HTt2LHDH09KSlKMJHdCLbkTavnjCTmFSnHn61hSjLLji3dVUnaB6mUX6Ei9WOXGRvvjye581c0p1MGUOBW4ihfXNcjIVXy+V3sbxMtYxd2qRuk5cnmM9pxdO6CmFh5PmTXlHyquyXLFKya1q7w56Sp0F9cUFZukWskd5MneL0/23uLniU+Vq14redw75ckp3k/RCU3lqttUhce3y5tXvJ9cSS0VXbuBCo5uliks3k+1ktvLiq3YfsrPkmLO7iXjyVdBenFNlhWtmIa9ZfLdKsgIT01pJ5137HXo0EH79+/X3r3FNUX6eKImaqImajrTasrPsn/OLTi8QcZ4lHay7JpU2xlzriSlNyx/P+UfL95Ptep3kRUdo/xDgTWF6zoiLa3sYy8/q+L7qaZrSjtZ/niq7mOvKjWVd47Iz6r4fqrpmnxjTAp9jlB8+MdTqJrczcs+79k1noLVVJFzeX5W+MdTqJrSTpY9P0n2jKdgNUnlz7m+cRbO8RSqJt84C3UdUZDjjDlXKjoOzpRrI99ipNNlmZKtsSo6ePCgLrjgAhUUFGjdunVq3LixJCktLU29e/fWG2+8oYkTJwb8zN133625c+cqNze3UiuwmjVrpqNHjyoxMVGS839zKpXd8dz1zELHrMBqffvEMmtavsn+3/T4OtMXtS9/P63aIlt/01My9yEdnXfsReJKBGqiJmqipl9aTau2SHbPub7fBg/pWHbuq7Y6Y86VpEs6l7+fit7b4lqD5R6u64ghHco+9oquaZyxAmtIx/LH07JNzlmBdUmnss8RxceB/SuwfGNMCj3OPt3mnBVYQ88r+7wX+NlBYRtPweJDOpR/Lvd9dnDCCqySnx2CjbOVW5yzAuvSLuXPuf5x5oAVWCXHWbDriFVbnDHnSkXHwZlybZSZmamUlBS53W5/L6cyqm0Fltvt1mWXXabjx49r7dq1/uaVVPzVQd9XCUs6cOCAkpOTQzavpKKVW8Eed7lccrkCS/C9aafy7diKxk993tOJW5YVNB4qR0vFTaWA7aWAY9ofD9F6rGz81Nf0faUxVE1WVLB4lGQFqamy8ajg+yNUvCL7I+BlrOA1BY9Xf00l03XSsVfZeCSMJ2qiplA5VjZOTdQk2V9TyenFrjnXN/+fmuqpufsXe9s850qSb1eWtZ+CPE3QHEPFq7Mml6vsYy/gOChnP5V+oHprKrnbQ17bVvOxV/qBytVU1jni1DTDNZ5KP+AqNcak0OeIcI6nUHHfmA91fqvM/qvpmipyLg8cZ+EZT6HiFRpnNo2nYPHy5tYKj7Mw1HTq4XrqOcKXlt1zrhR4HET6tVGo/CuqWhpYubm5GjFihLZv366VK1eqY8eOAY83adJEqamppZeYS1q/fr26detWHWkAAAAAAADgDFTlv0Lo8Xg0btw4ffnll1q8eLHOP//8oNuNHj1aH3zwgfbs2eOPrVq1Stu3b9fYsWOrmgYAAAAAAADOUFVegXXnnXfq/fff14gRI5SRkaE333wz4PEJEyZIku69914tXrxYgwcP1m233abs7GzNnTtX5513nqZOnVrVNAAAAAAAAHCGqnID69tvv5UkLV26VEuXLi31uK+B1axZM3322We644479Mc//lExMTG6/PLL9cQTT5R5/ysAAAAAAAD8slW5gbVmzZoKb9upUyctW7asqi8JAAAAAACAX5Aq3wMLAAAAAAAAqEnV8lcIAQAAIsnyzXZnUGxoZ7szAAAAcD5WYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0WhgAQAAAAAAwNFoYAEAAAAAAMDRaGABAAAAAADA0Vx2JwCg2PLNdmdQbGhnuzMAAAAAAKAIK7AAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaC67EwAAAGeG5ZvtzqDY0M52ZwAAAIDqxAosAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADhatTSwsrOz9eCDD2rYsGFKTk6WZVmaP39+qe2mTJkiy7JK/de+ffvqSAMAAAAAAABnIFd1PEl6erpmzZql5s2bq2vXrlqzZk3IbWNjY/Xqq68GxJKSkqojDQAAzijLN9udQbGhne3OAAAAAL9k1dLAatSokQ4cOKCGDRsqLS1NvXv3Dv2CLpcmTJhQHS8LAAAAAACAX4Bq+QphbGysGjZsWOHtPR6PMjMzq+OlAQAAAAAAcIYL+03cT548qcTERCUlJSk5OVk333yzsrOzw50GAAAAAAAAIkS1fIWwoho1aqS7775bPXr0kNfr1SeffKIXXnhBGzdu1Jo1a+RyBU8nLy9PeXl5/n/7Vm8VFhaqsLBQkhQVFaWoqCh5vV55vV7/tr64x+ORMabceHR0tCzL8j9vybhUtHqsInGXyyVjTEDcsixFR0eXytGyLEmSkWSsEk9iijqMXkkqEbdM0T+9Jbc9zbhOfU3J/36Eqsl4S8YtWVHRMsYrGW/5cStKlhUVOu71/PxOlBev+H4y3qLti/4RWJMVVVRTYLzmaiosLPvYkywZb2BNoXKv6ZqkyB1PweKRfo6gpl9oTd7S5z27zhGFheXXZMzpnctroiaPp+z9VNPzU2VqMqb8Y8/8fDFg55zrq8k3rEKNG2OcMedKktdb/jki8GXtmXN9NQUbZyVzL7qmCf94CpZ7YWH55z07xlNZNZV1Li9OM7zjKVjuJaeuUONMCv94ChU3puw5N/Czg8I2noLFK3Id4fvsYOecW3KclXUdITljzi36tFn+tZG/XBvnXF+85OEa7HrPeJ0x50pFx0HEXcOGmHNPPU9UVlgbWHPmzAn49/jx49W2bVvdd999WrJkicaPHx/y52bOnFkqvmHDBtWpU0eSlJqaqlatWmnnzp06cuSIf5umTZuqadOm2r59u9xutz/esmVLNWjQQJs3b1ZOTo4/3r59e9WrV08bNmwI2NldunRRTEyM0tLSAnLo1auX8vPz9d133/lj0dHR6t27t9xut7Zt2+aPx8fHq2vXrkpPT9eOHTv88aSkJMVIcifUkjuhlj+ekFOoFHe+jiXFKDu+eFclZReoXnaBjtSLVW5stD+e7M5X3ZxCHUyJU4GreHFdg4xcxed7tbdBvIxV3K1qlJ4jl8doz9m1A2pq4fGUWVP+oeKaLFe8YlK7ypuTrkJ3cU1RsUmqldxBnuz98mTvLX6e+FS56rWSx71Tnpzi/RSd0FSuuk1VeHy7vHnF+8mV1FLRtRuo4OhmmcLi/VQrub2s2Irtp/wsKebsXjKefBWkF9dkWdGKadhbJt+tgozw1JR2suxjT6qngsMbZEqcbGvV7yIrOkb5hwKPvZquSYrc8dShQwft379fe/cW1xTp5whq+mXWlH+49HnPrnNEWlr5NXnM6Z3La6Kmzabs/VTT81NlasrJKf/Yy8+yf8711ZR2sigeajyptjPmXElKb1j+OSL/uP1zrq+mtLSyzxH5WfaMp2A1pZ0s/7xnx3gKVVN55/L8rIrvp5quyTfGpNDzk+LDP55C1eRuXvaca9d4ClZTRa4j8rPsn3N9NaWdLPs6QnLGnGu54iWVf23kG2d2zrm+mnzjLNT1XkGOM+Zcqeg4iLRr2FBzblVvJWWZkq2xauC7ifu8efM0ZcqUcrfPyclRQkKCpk6dWuqvE/oEW4HVrFkzHT16VImJiZIi/7f2u55Z6JgVWK1vn1hmTcs32f+bHl9n+qL25e+nVVtk6296SuY+pGPZx96K7+3/TY8v90vPi9zxxMoeajpTalr5vXNWYA3pUH5Nq7Y6ZwXWxZ3K3k/LNjlnBdbQzuUfe6u2SHbPub6ahnQsCocaN6u2OmPOlaRLOpd/jih6b4trDZZ7uK4jgo2zkrkXXdM4YwXWkI7ln/dCjjMbzhGXdCr7XF58HNi/Ass3xqTQ4+zTbc5ZgTX0vLLn3MDPDgrbeAoWH9Kh/OsI32cHJ6zAKvnZIdg4W7nFGXOuZOnSLuVfG/nHmQNWYJUcZ8Gu91ZtccacKxUdB5F2DRtqzs3MzFRKSorcbre/l1MZYV2BFUx8fLxSUlKUkZERcpvY2FjFxsaWirtcrlJfO/S9aafy7diKxkN9nbEyccuygsZD5WipuKkUsL0UcEz74yFaj5WNn/qavq80hqrJigoWj1LR186qGI8Kvj9CxSuyPwJexgpeU/B49ddUMt1Qx16w97fogYrHq6umSB5PlY1TEzWFittZU5Bhads5wuUqvybfIt/Knstroibf2xpyzq3h+akyNVlW+cdeyZTsmnN9NZ2a6qm5+xd72zznSpJv15d1jgg2zuyYc0ONs5K5BxwHYRxPJXP0JVFyt1d6nNl0jijrXH5qmnaeI4JNUaHOEeEcT6HivjEfam6t3PmwZmuqyHVE4Diz97q8QuPMAXNueTlWepyFoaZTD9dTzxG+tOyec6XA4yBSrmFD5Rgq/4oKNmWHVVZWltLT05Wammp3KgAAAAAAAHCgsDWwcnNzlZWVVSr+0EMPyRijYcOGhSsVAAAAAAAARJBq+wrh888/r+PHj2v//v2SpKVLl/pvAHbrrbfq2LFj6t69u6655pqfb1YtLVu2TB999JGGDRumK6+8srpSARAmyzfbnUGxoZ3tzgAAAAAAUFOqrYH1+OOPa/fu3f5//+Mf/9A//vEPSdKECRNUr149XXHFFVqxYoVef/11eTwetW7dWrNnz9Zdd90V9DuVAAAAAAAAQLU1sHbt2lXuNgsWLKiulwMAAAAAAMAvBMueAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaC67EwAAIJyWb7Y7g2JDO9udAQAAABAZWIEFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEdz2Z0AAITD8s12Z1BsaGe7MwAAAACAyMIKLAAAAAAAADgaDSwAAAAAAAA4Gg0sAAAAAAAAOBoNLAAAAAAAADgaN3EHAFQJN8gHAAAAUNNYgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHo4EFAAAAAAAAR6OBBQAAAAAAAEejgQUAAAAAAABHc9mdAACgtOWb7c6g2NDOdmcAAAAA4JeOFVgAAAAAAABwNBpYAAAAAAAAcDQaWAAAAAAAAHA0GlgAAAAAAABwtGppYGVnZ+vBBx/UsGHDlJycLMuyNH/+/KDbbt26VcOGDVNCQoKSk5M1ceJEHTlypDrSAAAAAAAAwBmoWv4KYXp6umbNmqXmzZura9euWrNmTdDt9u7dqwsvvFBJSUmaPXu2srOz9fjjj2vTpk1av369YmJiqiMdAAAAAAAAnEGqpYHVqFEjHThwQA0bNlRaWpp69+4ddLvZs2frxIkT+uabb9S8eXNJUp8+fXTJJZdo/vz5uu6666ojHQAAAAAAAJxBquUrhLGxsWrYsGG5273zzju64oor/M0rSbr44ovVtm1bLVq0qDpSAQAAAAAAwBkmbDdx37dvnw4fPqxevXqVeqxPnz7asGFDuFIBAAAAAABABKmWrxBWxIEDByQVfd3wVI0aNVJGRoby8vIUGxtb6vG8vDzl5eX5/52ZmSlJKiwsVGFhoSQpKipKUVFR8nq98nq9/m19cY/HI2NMufHo6GhZluV/3pJxSfJ4PBWKu1wuGWMC4pZlKTo6ulSOlmVJkowkY5V4ElPUYfRKUom4ZYr+6S257WnGdeprSv73I1RNxlsybsmKipYxXsl4y49bUbKsqNBxr+fnd6K8eMX3k/EWbV/0j8CarKiimgLjNVdTYWHZx55kyXgDawqVe03XJJU/nvw/Us5+CkdNvkMh1DgzpnqPvarUVFhY/jnCeMM/nkLVVFhY9nnP99LhHk/B4r7joKxzuTEK+3gKVZNUzvzktWc8BYsXFpY+F4QcZ2EcT6Fq8nhCz7lFx4E94ylYTcaUfx1hfr4YsHPO9dVUcpxJpXM3xhlzriR5veVf7wW+rD1zrq+mYOOsZO5F1zT2z7lS0XEQas715e6EObdkTWVdlxenae+cK+NRyakr1DiT7J9zfYwp+7o88LODwjaegsUr8pnQ99nBzjm35Dgr63Ou5Iw5V7IkhZ5zS40zG+dcX7zk4Rrsutx4nTHnSkXHQU33I8o6l1dnj+XU80Rlha2BlZOTI0lBG1RxcXH+bYI9PmfOHM2cObNUfMOGDapTp44kKTU1Va1atdLOnTsD/qph06ZN1bRpU23fvl1ut9sfb9mypRo0aKDNmzf7c5Ok9u3bq169etqwYUPAzu7SpYtiYmKUlpYWkEOvXr2Un5+v7777zh+Ljo5W79695Xa7tW3bNn88Pj5eXbt2VXp6unbs2OGPJyUlKUaSO6GW3Am1/PGEnEKluPN1LClG2fHFuyopu0D1sgt0pF6scmOj/fFkd77q5hTqYEqcClzFi+saZOQqPt+rvQ3iZaziblWj9By5PEZ7zq4dUFMLj6fMmvIPFddkueIVk9pV3px0FbqLa4qKTVKt5A7yZO+XJ3tv8fPEp8pVr5U87p3y5BTvp+iEpnLVbarC49vlzSveT66kloqu3UAFRzfLFBbvp1rJ7WXFVmw/5WdJMWf3kvHkqyC9uCbLilZMw94y+W4VZISnprSTZR97Uj0VHN4gU+JkW6t+F1nRMco/FHjs1XRNUvnjKT+rYvspHDWlnSyKJyUlqUOHDtq/f7/27i2uyVNYvcdeVWrakFf+OSL/UPjHU6iayjvv5WfZM56C1eQ7Dso6l8uEfzyFqkkqe37KP2zPeApWU1pacU2h5lyPCf94ClXTZhN6zu3Qwb7xFKymnJzyryPys+yfc301+cZZqGsj1XbGnCtJ6Q3Lv97LP27/nOurKS2t7GvY/CxnzLlS0TVNqDnXd45wwpzrq6m863LfNY3dc27+oTT/GJNCf9ZQvP1zro+7edmfn5wy57rqVuwzYX6W/XOur6a0k2V/zpWcMedarnhJoedc3znCN87snHN9NfnGWajP7gU5zphzpaLjoKb7EWWdy6uzx+JbjHS6LFOyNVYNfDdxnzdvnqZMmVIq/sYbb2jixIkBP3P33Xdr7ty5ys3NrfAKrGbNmuno0aNKTEyUFPkrsHY9s9AxK7Ba3z6xzJqWb7L/Nz2+zvRF7cvfT6u2yNbf9JTMfUjHso+9Fd/b/5seX+6Xnlf+eFq1JXStvhzD9durIR1/joYYZ6u22v+bHp8hHcs/R6zYbO9vekrmPqRD2ec933HghBVYvuOgrHP58s2ybXVFsHFW1vy08nvnrMAa0qH838j5x5kDfht8caeyf8u4bJN9qytOjQ/tXP51RNE4c8Zvg0uOM6l07qu2OmPOlaRLOpd/veefy36uNVju4TpHBBtnJXMvuqaxf86Vio6D8n5rH3Kc2XCOuKRT2dflxceB/SuwfGNMCj3OPt1m/5zrM/S8sj8/BX52UNjGU7D4kA7lfyb0fXZwwgqskp8dgo2zlVucMedKli7tUv7KnlKfHWy8Li85zoJdl6/a4ow5Vyo6Ds6UFViZmZlKSUmR2+3293IqI2wrsHxfHfR9lbCkAwcOKDk5OWjzSipatRXsMZfLJZcrsATfm3Yq346taPzU5z2duGVZQeOhcrQkf1MpYHsp4Jj2x0O0HisbP/U1fV9pDFWTFRUsHiVZQWqqbDwq+P4IFa/I/gh4GSt4TcHj1V9TyXRDHXvB3t+iByoer66ayhtPp/5I6P1X8zWdeiicmrtv8WF1HXtVqcmXa1nnCCvYOaKGx1OomsobZyVfOpzjKVj81FSDn8dky3gKFS9rfgqyuW3nCJer/HOEf5yFcTwVv3ZgTb63NeSca9N4Cp57+dcRgePMnjnXV1N548y/2NvmOVeSfLu+rOu9YOPMrnNEsHFWMveA48DGOVcKPA4qPc5sOkeUdV1e6prGxnNEsGk31DnCzjm3+OdD51i0fWTMucX5lngem6/LKzTOHDDnlpdjpcdZGGo69XA99RzhS8vuOVcKPA5qsh9R2fjp9FhC5V9RwabsGtGkSROlpqaWXmYuaf369erWrVu4UgEAAAAAAEAECVsDS5JGjx6tDz74QHv27PHHVq1ape3bt2vs2LHhTAUAAAAAAAARotq+Qvj888/r+PHj2r9/vyRp6dKl/huA3XrrrUpKStK9996rxYsXa/DgwbrtttuUnZ2tuXPn6rzzztPUqVOrKxUAAAAAAACcQaqtgfX4449r9+7d/n//4x//0D/+8Q9J0oQJE5SUlKRmzZrps88+0x133KE//vGPiomJ0eWXX64nnngi5P2vAAAAAAAA8MtWbQ2sXbt2VWi7Tp06admyZdX1sgAAAAAAADjDhfUeWAAAAAAAAEBl0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKPRwAIAAAAAAICj0cACAAAAAACAo9HAAgAAAAAAgKOFtYG1Zs0aWZYV9L9169aFMxUAAAAAAABECJcdLzp9+nT17t07INa6dWs7UgEAAAAAAIDD2dLAGjBggMaMGWPHSwMAAAAAACDC2HYPrKysLBUWFtr18gAAAAAAAIgQtjSwpk6dqsTERMXFxWnw4MFKS0uzIw0AAAAAAABEgLB+hTAmJkajR4/W8OHDVb9+fW3ZskWPP/64BgwYoC+++ELdu3cP+nN5eXnKy8vz/zszM1OSVFhY6F/FFRUVpaioKHm9Xnm9Xv+2vrjH45Exptx4dHS0LMsqtTosOjpakuTxeCoUd7lcMsYExC3LUnR0dKkcLcuSJBlJxirxJKaow+iVpBJxyxT901ty29OM69TXlPzvR6iajLdk3JIVFS1jvJLxlh+3omRZUaHjXs/P70R58YrvJ+Mt2r7oH4E1WVFFNQXGa66mwsKyjz3JkvGesjIxRO41XZNU/njy/0g5+ykcNfkOhVDjzJjqPfaqUlNhYfnnCOMN/3gKVVNhYdnnPd9Lh3s8BYv7joOyzuXGKOzjKVRNUjnzk9ee8RQsXlhY+lwQcpyFcTyFqsnjCT3nFh0H9oynYDUZU/51hPn5YsDOOddXU8lxJpXO3RhnzLmS5PWWf70X+LL2zLm+moKNs5K5F13T2D/nSkXHQag515e7E+bckjWVdV1enKa9c66MRyWnrlDjTLJ/zvUxpuzr8sDPDgrbeAoWr8hnQt9nBzvn3JLjrKzPuZIz5lzJkhR6zi01zmycc33xkodrsOty43XGnCsVHQc13Y8o61xenT2Wqn4LL6wNrH79+qlfv37+f48cOVJjxoxRly5dNGPGDH3yySdBf27OnDmaOXNmqfiGDRtUp04dSVJqaqpatWqlnTt36siRI/5tmjZtqqZNm2r79u1yu93+eMuWLdWgQQNt3rxZOTk5/nj79u1Vr149bdiwIWBnd+nSRTExMaVWi/Xq1Uv5+fn67rvv/LHo6Gj17t1bbrdb27Zt88fj4+PVtWtXpaena8eOHf54UlKSYiS5E2rJnVDLH0/IKVSKO1/HkmKUHV+8q5K</t>
-  </si>
-  <si>
-    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACGwElEQVR4nOzdd3xUVf7/8fdNhnQSDEUCAaSXUJWiKNKUooJLExSk7s+yKrq66qLrYgVdWfu6a/kKKLiKWHFFKYKLCmIUBQREpUiHUBIC6XN+f2RnkiEzKSSZewdfz8eDh+bMnbmfz9x77rnzmXPvWMYYIwAAAAAAAMChwuwOAAAAAAAAACgNBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAKmj8+PGyLEtjxowp1/JPPvmkLMtSu3btqjmysvXp00eWZWnlypW2rH/ixImyLEtz5syxZf1Vxe738bfknHPOkWVZ2rFjh92hAAAAG1HAAgCggqZMmSJJeu+993T06NEyl589e7bP86rL/fffL8uydP/991fres50ofQ+BrOQtnLlSlmWpT59+lT7ugAAAE5FAQsAgAq6+OKL1aJFC+Xk5Gj+/PmlLvv1119rw4YNqlGjhq699togRRjYq6++qs2bN6t79+52hxLSeB8BAACCiwIWAAAVZFmWJk+eLKlodlUgnsevuOIK1atXr9pjK0vjxo3Vpk0bxcTE2B1KSON9BAAACC4KWAAAnIaJEycqPDxc3377rdavX+93mezsbP373/+WVPLywW+++UZjx45V48aNFRkZqcTERA0cOFAfffSR39cqfh+g999/X/369VNiYqL38jHLsvTAAw9Ikh544AFZluX9N3HiRO/rlHXJ2aeffqpRo0YpOTlZkZGRqlu3rrp166bp06fr8OHD3uXy8vI0b948jR07Vm3atFF8fLyio6PVunVrTZ06VXv37i3vW1mmOXPmePM4fPiwbrrpJu/71qRJE/3xj38MeCnnO++8o9///vdq3769zjrrLEVFRalp06aaPHmyfvzxxxLLV9X7uHz5cg0fPlxJSUmKiIhQvXr1NGzYMK1evdrv8p51SNLbb7+tiy66SPHx8YqNjdWFF15YYr/wbPPPPvtMktS3b1+fWIvfY+ybb77R6NGjlZycrIiICMXHx6tZs2YaMWKE3n//fb/xnKpPnz7q27evJOmzzz7zWdc555zjs2x+fr7+9a9/qWfPnkpISFBUVJRatmypqVOnas+ePeVaXyDvvvuu972pWbOm+vTpE7DPeCxcuFCDBg1S3bp1FRERoYYNG2rcuHHatGlThdf/008/afLkyWratKkiIyMVFxenJk2a6PLLLw9YzN66dauuv/56NW/eXFFRUUpISNDFF1+sefPmVVncO3bs8G4LY4xefPFFnXfeeYqNjVVCQoIGDBgQcN8DACBkGAAAcFqGDBliJJmpU6f6fXz+/PlGkmnQoIHJz8/3tj/11FMmLCzMSDKdO3c2I0eONBdddJGJiIgwkswDDzxQ4rWaNGliJJmbb77ZSDJdu3Y1V199tendu7f573//ayZMmGA6depkJJlOnTqZCRMmeP+99NJL3tfp3bu3kWRWrFhRYh233HKLkeSNa8yYMWbw4MGmWbNmJZ6za9cuI8kkJCSY888/34waNcpcdtllpkGDBkaSqVu3rvnpp59KrGPChAlGkpk9e3a53+fZs2cbSWbo0KGmefPmplatWuZ3v/udGTZsmDnrrLOMJNO6dWtz8ODBEs8NDw83MTExpmvXrmb48OFm6NCh3nxiY2PNF198USK+yr6Pd9xxh5FkwsLCTPfu3c2oUaNMjx49jGVZJjw83LzyyislnuN53//6178ay7LMhRdeaEaPHu2NxbIs884773iX37x5s5kwYYI5++yzjSQzcOBAn1hXrVpljDFm2bJlpkaNGt58Ro4caYYNG2a6d+9uIiMjzZVXXlmubTBz5kwzcOBAI8mcffbZPuu64447vMtlZ2ebSy65xEgyUVFRZvDgwWb06NGmUaNGRpKpU6eO+eabb8q1Tg/Pvv/HP/7RZ9/v3r2793175plnSjwvLy/PXHXVVUaSiYyMND179jSjRo3yvqfR0dFm8eLF5Y5jw4YNJj4+3ru/DR8+3IwaNcpccMEFJi4uznTq1KnEcxYsWGCioqKMJNOmTRszbNgw069fPxMbG2skmUmTJlVJ3Nu3bzeSTJMmTcyECRNMjRo1TL9+/cxVV11lWrVq5X2tNWvWlDtfAACchgIWAACn6b333jOSTO3atU1OTk6Jxz0f5O+55x5v28cff2wsyzJ16tQxn332mc/y69evN8nJyUaSWblypc9jng/x4eHh5v333/cbz/Tp040kM3369IAxByq8PPPMM95cPv300xLP++qrr8yvv/7q/TsjI8O8//77JfLOzc0106ZNM5LMZZddVuJ1KlPAkmTOP/98c/jwYe9jR48eNT179jSSzJgxY0o894033jCZmZk+bW632/zjH/8wkkxKSopxu90+j1fmfXzxxReNJNOiRQvz/fff+zz22WefmZo1a5qIiAizdetWn8c8+dWqVatEkcETT6tWrcodh0ffvn2NJDNv3rwSjx07dsysXr06YI6nWrFihZFkevfuHXCZu+++20gyzZs3N9u3b/e25+bmmilTphhJpmnTpn77SyCefd+yrBJ5vPHGG8ayLONyucyGDRt8HrvnnnuMJNOjRw+zbds2n8feeustEx4ebs466yxz9OjRcsUxadIkI8k8/PDDJR47efKk3/4cGRlpoqKizNtvv+3z2I4dO0yHDh2MJDN37txKx+0pYHmKWD/++KP3sfz8fDN58mQjyQwYMKBcuQIA4EQUsAAAOE15eXmmfv36RpJ56623fB7buXOnd5ZV8ZlIPXr0MJLMwoUL/b7mggULjCQzYsQIn3bPh/jJkycHjOd0Cy95eXmmbt26RlKJD9qnq0GDBiYsLMxkZGT4tFe2gLVu3boSj69fv95YlmXCwsLMrl27yv26F1xwgZFkfvjhB5/2030fCwoKvDPQUlNT/T7vb3/7m5HkM2vJmKIClr+ZRNnZ2SYhIcFI8ikiBoqjuHbt2hlJ5siRIwFzKa+yClhZWVkmLi7OSDIffPBBicdPnDjhnTE2f/78cq/Xs+//7ne/8/v4iBEjjCTz//7f//O2HT582ERHR5uoqCize/duv8/7wx/+YCSZZ599tlxxXHbZZUaS+fbbb8u1/OjRo40kM2vWLL+Pr1271kgy5513XqXjLl7A8vfe79u3zzsLKzc3t1zxAwDgNNwDCwCA0+RyuTRhwgRJ0iuvvOLz2OzZs+V2u9W7d2+1aNFCkpSWlqa1a9cqOjpaQ4YM8fuaffr0kSR9+eWXfh8fOXJkFUVf5JtvvtGhQ4dUp04dDRs2rELP/f777/XEE0/olltu0eTJkzVx4kRNnDhR+fn5crvd+vnnn6sszk6dOqlz584l2jt06KAuXbrI7Xbrv//9b4nHf/75Zz333HO67bbbNGXKFG+MBw4ckCS/98I6HevWrdPevXvVvHlznXfeeX6XKWv7+tsvIiMj1axZM0mq8D2kPL+SOHbsWH3++efKz8+v0PMrIjU1VZmZmUpMTPSbR0xMjMaMGSNJWrFiRYVf39PXArUXvx/ZihUrlJWVpQsvvFANGzb0+7yytsWpPO/ljTfeqE8++UTZ2dkBl3W73Vq8eLEkafTo0X6X6dq1q+Li4rRu3Trva1U2bpfLpUGDBpVor1+/vs466yzl5OT43MsOAIBQ4rI7AAAAQtnkyZP12GOPacmSJdqzZ48aNmwoY4z3JtrFb96+fft2GWOUlZWlyMjIUl/30KFDfttPvWF2Vdi5c6ckqXXr1t4biZflxIkTuvbaa/Xuu++WulxGRkal4/No2rRpqY99++232r17t7etoKBAN998s1544QUZY6o9xm3btkmSfvnllzLfx0Dbt3Hjxn7b4+PjJanUook/M2fO1Pr167V48WItXrxY0dHROvfcc9WnTx+NHTtWbdu2rdDrlcZTXCttOzVv3txn2YoI9Lqe9uLb3rMtli9fftrb4lR33nmnPv/8cy1btkyDBg1SjRo11KlTJ1188cUaM2aMunXr5l328OHD3v2qUaNGZb724cOH1bBhw0rHnZSUpBo1avhdPj4+XkePHq3wPgQAgFNQwAIAoBJatWqlXr16adWqVXr11Vc1bdo0rVixQjt27FBCQoLPjCm32y1JiouL04gRI05rfdHR0VUSd2VNmzZN7777rtq0aaNHH31U3bp1U506dRQRESFJ6tmzp1avXl1q4ag6FF/f008/rX/961+qX7++nnjiCfXs2VNnn322oqKiJEnXXHON/v3vf1dZjJ7tW79+fQ0cOLDUZevUqeO3PSysaifH169fX6mpqfrss8+0bNkyffHFF/rqq6/0xRdfaMaMGZo5c6buvvvuKl2nXYpvR8+2aNGihS688MJSn9emTZtyvX5MTIyWLl2qr7/+Wh9//LG+/PJLffnll0pNTdUTTzyhP/zhD/rHP/7hs34p8Myx4jwF7crGXdX7DwAATkIBCwCASpoyZYpWrVql2bNna9q0ad7LCceMGeNTcPLMxLAsS6+88opjPmx6Zv1s3bpVxphyzcJasGCBJOnNN99Ux44dSzz+008/VW2QKpzBFsiOHTskScnJyd42T4wvvPCChg4dWuI5VR2jZ/vWrl3bOwPPCSzLUp8+fbyXnmVnZ2vOnDm66aabdM8992jkyJHemVGV4bnkrbTt5JlhFOjyuNJs375dnTp1KtHub9t7tkXr1q2rfFt069bNO9sqPz9f7733nsaPH6/nn39eI0eOVN++fVWnTh1FR0crKytLs2bNCliwPFV1xg0AQKhzxpkzAAAhbNSoUYqPj9dPP/2kDz/8UO+8844k38sHJalBgwbq2LGjjh8/ro8//rjK4/DMfqrofY66du2qOnXq6NChQ3rvvffK9ZwjR45Ikpo0aVLisU8++URpaWkViqE81q9fr/Xr15do/+GHH/Ttt98qLCxMF198cbli/OGHH/Tdd9/5Xc/pvo+eWWibNm3SDz/8UKHnnq7TiTUqKko33HCDOnbsKLfb7fc9PZ11ee7pdOTIEX3wwQclHs/KytIbb7whSerbt2+54/V47bXX/La/+uqrkoruDSVJ/fv3V0REhFauXKmDBw9WeF3l5XK5NHLkSO+MO88+FR4erksvvVRSUSG1PIIVNwAAoYgCFgAAlRQTE6Orr75aUuE9sbKystShQwefe+J4PPzww5KkSZMmadGiRSUeN8boq6++0pIlSyoch2cGSkWLJy6XS/fee68k6brrrvN7I/Svv/7a5x5DnnsnPfvssz7L/fjjj7rhhhsqtP7yMsboxhtv1NGjR71t6enpuvHGG2WM0YgRI3zuN+SJ8R//+IfPJV379u3T+PHjAxZiTvd9rFGjhqZPny5jjIYNG6bPP/+8xDIFBQX69NNPtWbNmgq9diBlxTpr1iz9+uuvJdq3bNninYHmr8BX2rp++ukn5eXllXg8KipKN910kyTpjjvu8N5bTZLy8vJ06623av/+/WratOlp/RjBu+++6y2AeSxcuFBvv/22XC6XbrnlFm/72WefrVtuuUUnTpzQkCFDtGHDhhKvl5OTow8++EBbtmwp1/qff/55vzf8379/v1JTUyX5vpfTp09XRESE7rzzTs2dO9dnH/TYuHGjt+BdXXEDAHDGsOfHDwEAOLOsXbvW+zP2ksxTTz0VcNmnn37auFwuI8m0aNHCXH755eaaa64xl156qalXr56RZO6++26f5zRp0sRIMtu3bw/4uvv37zexsbFGkrnwwgvNxIkTzZQpU8wrr7ziXaZ3795GklmxYoXPc91ut7nhhhu88Xfp0sWMGTPGXHbZZaZZs2YlnvP2228by7KMJNOhQwczZswY069fP1OjRg3Tr18/07NnT7/rmTBhgpFkZs+eXdZb6jV79mwjyQwdOtQ0a9bM1KpVywwbNswMHz7cJCYmGkmmZcuW5sCBAz7PW7NmjYmIiPC+z1dddZUZNGiQiY6ONikpKWbYsGF+Y6nM+2iMMXfeeaf3fUxJSTFXXnmlGTNmjOnTp4+pVauWkWT++c9/+jzHs3wggdb34YcfGkkmIiLCXHHFFWby5MlmypQp5osvvjDGGJOQkGAkmTZt2phhw4aZa665xvTp08e7/40fP74cW6BI165djSTTunVrM3bsWDNlyhSffTU7O9v079/fSDLR0dHmsssuM6NHjzaNGzc2kkzt2rVNampqhdbp2fdvu+02I8l069bNXHPNNaZHjx7e9+2JJ54o8by8vDxzzTXXGEkmLCzMdOnSxYwYMcKMHj3aXHjhhd5tvHjx4nLF0alTJyPJNG3a1AwZMsSMHTvWDBgwwERHRxtJpl+/fiYvL8/nOQsWLDAxMTFGkklOTjYDBgwwY8eONYMHDzbJyclGkhk9enSl496+fbuRZJo0aVLm+1jaMQQAACejgAUAQBXp0KGDt5iQlpZW6rIbNmww1113nWnZsqWJiooyMTExplmzZmbgwIHmmWeeMXv27PFZvrwfPv/73/+aSy65xJx11lkmLCzMSDITJkzwPl5a4cUYYxYvXmyuvPJKc/bZZ5saNWqYunXrmu7du5sHHnjAHD58uMS6+vfvb+rUqWNiYmJM+/btzSOPPGJycnICrqcyBawJEyaYgwcPmuuvv94kJyebiIgI06hRIzN16tQSsXmsX7/eDB061CQlJZmoqCjTsmVLc9ddd5mMjIxSY6ns+/jFF1+YsWPHmiZNmpjIyEhTs2ZN06pVK/O73/3OvPzyy+bIkSM+y59uAcsYY1566SVz7rnnegslxXOaN2+emTRpkmnfvr1JTEw0kZGRpkmTJmbw4MHm3XffNW63O+A6/dm5c6e55pprTFJSkrcIdmrRJC8vzzz//PPm/PPPNzVr1jQRERGmefPm5pZbbjG7d++u0PqM8d33FyxYYC644AITFxdnYmNjTa9evcyiRYtKff5HH31khg8fbho2bGhq1KhhatWqZdq2bWvGjBljXn/9dXPixIlyxfHhhx+aG2+80XTp0sXUrVvXREREmOTkZNOnTx8zd+5ck5ub6/d527dvN3/84x9N+/btTWxsrImKijJNmjQxffr0MY8++qj5+eefKx03BSwAwG+BZUyQfx4IAACgAubMmaNJkyZpwoQJ3NgaAADgN4p7YAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNG4BxYAAAAAAAAcjRlYAAAAAAAAcDQKWAAAAAAAAHA0l90BnA632629e/eqZs2asizL7nAAAAAAAABQCmOMjh8/rgYNGigsrOLzqUKygLV37141atTI7jAAAAAAAABQAbt27VJycnKFnxeSBayaNWtKKkw6Pj7e5mgAAAAAAABQmoyMDDVq1Mhb06mokCxgeS4bjI+Pp4AFAAAAAAAQIk73VlDcxB0AAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjhaSv0IIAAAAAACCzxijgoIC5efn2x0KHMLlcik8PPy0f12w3Oup1lcHAAAAAAAhzxijY8eO6dChQyooKLA7HDhMeHi46tWrp4SEhGorZFHAAgAAAAAApdq/f7+OHTum+Ph4xcfHy+VyVfuMGzifMUb5+fnKyMjQvn37lJWVpaSkpGpZFwUsAAAAAAAQUEFBgdLT01W3bl3VqVPH7nDgQDVr1lRkZKTS0tJUr149hYeHV/k6uIk7AAAAAAAIKC8vT8YYxcbG2h0KHCw2NlbGGOXl5VXL61PAAgAAAAAAZeKSQZSmuvcPClgAAAAAAABwNApYAAAAAAAA8GvixIk655xz7A6DAhYAAAAAAPjtmjNnjizLCvhvzZo1dodYpk2bNun+++/Xjh077A6l2vArhAAAAAAA4DfvwQcfVNOmTUu0t2jRwoZoKmbTpk164IEH1KdPH0fMlqoOFLAAAAAAAMBpW7LR7gikAe0r/xqDBw9W165dK/9CqBZcQggAAAAAAFCK6dOnKywsTMuXL/dpv+666xQREaHvv/9ekrRy5UpZlqU333xT99xzj+rXr6/Y2FgNHTpUu3btKvG6X331lQYNGqSEhATFxMSod+/e+uKLL0ost2fPHk2ZMkUNGjRQZGSkmjZtqhtvvFG5ubmaM2eORo0aJUnq27ev99LHlStXep+/ePFi9erVS7GxsapZs6Yuv/xy/fDDDyXW895776l9+/aKiopS+/bt9e6771bmbatSzMACAAAAAAC/eenp6UpLS/NpsyxLtWvX1l/+8hctWrRIU6ZM0YYNG1SzZk198skneumll/TQQw+pU6dOPs975JFHZFmW7r77bh08eFBPPfWULrnkEn333XeKjo6WJH366acaPHiwzjvvPG+BbPbs2erXr59WrVql7t27S5L27t2r7t2769ixY7ruuuvUpk0b7dmzRwsXLtTJkyd18cUXa+rUqXrmmWd0zz33qG3btpLk/e9rr72mCRMmaODAgXrsscd08uRJ/fOf/9RFF12kdevWeS85XLJkiUaMGKF27dpp5syZOnz4sCZNmqTk5OTqfNvLzTLGGLuDqKiMjAwlJCQoPT1d8fHxdocDAAAAAMAZKzs7W9u3b1fTpk0VFRVV4vFQv4Rwzpw5mjRpkt/HIiMjlZ2dLUnauHGjzjvvPI0fP16PP/642rdvr6SkJK1evVouV+H8oJUrV6pv375q2LChNm/erJo1a0qS3nrrLV111VV6+umnNXXqVBlj1Lp1azVr1kyLFy+WZVmSpKysLKWkpKhFixZasmSJJGnChAmaN2+evvrqqxKXOBpjZFmWFi5cqFGjRmnFihXq06eP9/HMzEw1atRIo0aN0osvvuhtP3DggFq3bq2rrrrK296lSxcdOHBAmzdvVkJCgiRp6dKlGjBggJo0aVLmDeLL2k8qW8thBhYAAAAAAPjN+8c//qFWrVr5tIWHh3v/v3379nrggQc0bdo0rV+/XmlpaVqyZIm3eFXc+PHjvcUrSRo5cqSSkpL00UcfaerUqfruu+/0008/6S9/+YsOHz7s89z+/fvrtddek9vtllR4Wd+QIUP83p/LU/gKZOnSpTp27Jiuvvpqn9ll4eHh6tGjh1asWCFJ2rdvn7777jv9+c9/9havJOnSSy9Vu3btdOLEiVLXEwwUsAAAAAAAwG9e9+7dy7yJ+5133qk33nhDa9eu1YwZM9SuXTu/y7Vs2dLnb8uy1KJFC+8spp9++klS4eyqQNLT05Wbm6uMjAy1b396U8w86+nXr5/fxz0zoXbu3Ok3bklq3bq1vv3229Naf1WigAUAAACEACdcouNRnkt1Qi1eACiPbdu2eYtCGzZsOO3X8cyuevzxx9W5c2e/y8TFxenIkSOnvY7i63nttddUv379Eo/7mz3mVKETKQAAAAAAgE3cbrcmTpyo+Ph43XbbbZoxY4ZGjhyp4cOHl1jWU+TyMMbo559/VseOHSVJzZs3l1Q4A+qSSy4JuM66desqPj5eGzeW/q1AoEsJPeupV69eqetp0qSJ37gl6ccffyx13cESZncAAAAAAAAATvfEE0/oyy+/1IsvvqiHHnpIPXv21I033ljilwsl6dVXX9Xx48e9fy9cuFD79u3T4MGDJUnnnXeemjdvrlmzZikzM7PE8w8dOiRJCgsL0+9+9zstWrRIqampJZbz/C5fbGysJOnYsWM+jw8cOFDx8fGaMWOG8vLyAq4nKSlJnTt31ty5c5Wenu59fOnSpdq0aVOp70uwMAMLAAAAAAD85i1evFhbtmwp0d6zZ0/l5OTovvvu08SJEzVkyBBJhb9e2LlzZ/3hD3/QggULfJ6TmJioiy66SJMmTdKBAwf01FNPqUWLFvp//+//SSosTL388ssaPHiwUlJSNGnSJDVs2FB79uzRihUrFB8fr0WLFkmSZsyYoSVLlqh379667rrr1LZtW+3bt09vvfWWPv/8c9WqVUudO3dWeHi4HnvsMaWnpysyMlL9+vVTvXr19M9//lPXXnutzj33XI0ZM0Z169bVr7/+qv/85z+68MIL9dxzz0mSZs6cqcsvv1wXXXSRJk+erCNHjujZZ59VSkqK3yJbsFHAAgAAAAAAv3l//etf/ba//PLLeuGFF1SnTh099dRT3vaWLVtq5syZuvXWW7VgwQJdddVV3sfuuecerV+/XjNnztTx48fVv39/Pf/884qJifEu06dPH61evVoPPfSQnnvuOWVmZqp+/frq0aOHrr/+eu9yDRs21FdffaX77rtP8+fPV0ZGhho2bKjBgwd7X69+/fr617/+pZkzZ2rKlCkqKCjQihUrVK9ePV1zzTVq0KCBHn30UT3++OPKyclRw4YN1atXL02aNMm7nkGDBumtt97SX/7yF02bNk3NmzfX7Nmz9f7772vlypVV9C6fPst45puFkIyMDCUkJCg9Pd17x3wAAADgTBZqN0UPtXgBBJadna3t27eradOmioqKsjscR1u5cqX69u2rt956SyNHjrQ7nKAqaz+pbC2He2ABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRuIk7AAAAAABAFejTp49C8FbjIYEZWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwtEoXsL7++mvdfPPNSklJUWxsrBo3bqyrrrpKW7du9Vlu4sSJsiyrxL82bdpUNgQAAAAAAACcwVyVfYHHHntMX3zxhUaNGqWOHTtq//79eu6553TuuedqzZo1at++vXfZyMhIvfzyyz7PT0hIqGwIAAAAAAAAp2XOnDmaNGmSIiMj9csvv6hhw4Y+j/fp00dpaWnauHGjTRFCqoIC1u23367XX39dERER3rbRo0erQ4cOevTRRzVv3ryilblcGjduXGVXCQAAAAAAnOLjj+2OQBo0qNIvkZOTo0cffVTPPvtsFQSEqlbpSwh79uzpU7ySpJYtWyolJUWbN28usXxBQYEyMjIqu1oAAAAAAIAq07lzZ7300kvau3ev3aHAj2q5ibsxRgcOHFCdOnV82k+ePKn4+HglJCQoMTFRN910kzIzM6sjBAAAAAAAgHK75557VFBQoEcffbTU5fLz8/XQQw+pefPmioyM1DnnnKN77rlHOTk53mVuv/121a5dW8YYb9stt9wiy7L0zDPPeNsOHDggy7L0z3/+s+oTOsNU+hJCf+bPn689e/bowQcf9LYlJSXprrvu0rnnniu3262PP/5Yzz//vL7//nutXLlSLlfgUHJycnx2BM8Mrvz8fOXn50uSwsLCFBYWJrfbLbfb7V3W015QUOCz4wRqDw8Pl2VZ3tct3i4VziArT7vL5ZIxxqfdsiyFh4eXiDFQOzmREzmREzmREzmREzmRkyd245ZkhcmywmTcBZKKcpJVmJNx++YkqzB2mYJytVthhTn5tluywsJljPt/QUj5+WXnVHz5/714gNiDkxP7HjmR0+nnlJ+fX3QsKva63vjl03vtafcTV3lYluXN6ZxzztG1116rl156SX/+85+VlJTks6wxRpZl6fe//73mzp2rkSNH6vbbb9fatWs1c+ZMbd68We+8844k6aKLLtKTTz6pH374QSkpKZKkVatWKSwsTKtWrdLUqVNljNF///tfSVKvXr28r+/vPT7dnILZLhW+R8VrNcX3vVP3v4qq8gLWli1bdNNNN+mCCy7QhAkTvO0zZ870WW7MmDFq1aqV7r33Xi1cuFBjxowJ+JozZ87UAw88UKJ93bp1io2NlSTVrVtXzZs31/bt23Xo0CHvMsnJyUpOTtbWrVuVnp7ubW/WrJnq1aunjRs3Kisry9vepk0b1apVS+vWrfPpxB07dlRERIRSU1N9Yujatatyc3O1fv16b1t4eLi6deum9PR0bdmyxdseHR2tTp06KS0tTdu2bfO2JyQkqG3bttq7d692797tbScnciInciInciInciIncvLklHtcciU0U3hMPeUd3iiTX5RTjcQ2siJrKe/gOpliBZwadTrKCo9Q7gHfnCLO7ipTkKu8tKKcLCtcEfW7yeSmK+9IUU6WK1oRdTvJnZWm/PTCnFJPlp1TQfp2FWQV5RQelyxXzWTlH9sqd07RdgpGTux75EROlc8pKipKUmFRKzs729seFhammP+1Fy9QhIWFKaJGjRLt4eHhquFyKT8/3ycWl8slV3i48vLyfIp1nvbc3FyfokmNGjUUHhbmbc8/ccL7HoeFhenE//72iI2Nldvt9nlfLMvytktSVlaW/vjHP+q1117TY489plmzZiknJ0cFBQVyu93Kzs7W1q1bNXfuXE2YMEHPPfecJGnKlCmqV6+eZs2apcWLF+viiy9Wly5dJBUWrZo3b64jR45ow4YNuvLKK7Vq1Srv+lasWKGzzjpLTZo0UUFBgVwul06ePOmT6+nk5Hc7xcQoPz/fZ4JQeHi4oqOjlZeXp9zcXJ/3PSoqSjk5OT7bLyIiQhEREcrOzvbZfpGRkZKkvLw8n5vdF9/3Kns7KctUtrRXzP79+3XhhRcqLy9Pa9asUYMGDUpdPisrS3FxcZo0aVKJXycszt8MrEaNGunw4cOKj4+X5JzKtMeZVG0nJ3IiJ3IiJ3IiJ3IiJ/tzWr5JjpmB1b9d2Tl9ssE5M7AuTWHfIydyqkxO2dnZ+vXXX9WsWTNvoaI465NP7J+BNXCgnyXKZlmWZs+ercmTJ2vt2rXq2rWrJk+erDfeeEO//PKLkpKS1LdvX6WlpWnDhg169NFHdc899+iHH35Q27Ztva9z4MABJSUl6fbbb9esWbMkSe3atVPnzp31+uuv66OPPtKwYcP0+eefq0ePHtq6datatGih8847T40aNdJ7773njSdUZ2Dl5ORo27Ztaty4sbfgWXzfy8jIUO3atZWenu6t5VRElc3ASk9P1+DBg3Xs2DGtWrWqzOKVVFhFrF27to4cOVLqcpGRkX47icvlKnHpoafDnsrTAcvbHuiSxoq0W5bltz1QjBVtJydyCtROTuQkkVOgGCvaTk7kJJFToBgr2k5OlcvJKvawFeY/JysswOm9Vf52y7ICtId5gyiecqDYiy/vG2Og2Ks3p9K205KNJR7537/ytvuPPXB7oI9hLg1o76eV/kRONufkcrkKjw2S97+n8t8axPYAcZVH8dwsy9J9992nefPm6bHHHtPTTz/ts9zOnTsVFhamli1b+rwX9evXV61atfTrr79623v16qWPPvpIlmXp888/V9euXdWtWzclJiZq1apVOvvss/X999/rmmuu8XmtQO/x6eRkR7u/Wo2/toqqkpu4Z2dna8iQIdq6das+/PBDtWvXrlzPO378uNLS0lS3bt2qCAMAAAAAAKBSmjVrpnHjxunFF1/Uvn37/C5TniLTRRddpD179mjbtm1atWqVevXqJcuydNFFF2nVqlX68ssv5Xa71atXr6pO4YxU6QJWQUGBRo8erdWrV+utt97SBRdcUGKZ7OxsHT9+vET7Qw89JGOMBg0aVNkwAAAAAAAAqsRf/vIX5efn67HHHvNpb9Kkidxut3766Sef9gMHDujYsWNq0qSJt81TmFq6dKm+/vpr798XX3yxVq1apVWrVik2NlbnnXdeNWdzZqj0JYR33HGHPvjgAw0ZMkRHjhzRvHnzfB4fN26c9u/fry5duujqq69WmzZtJEmffPKJPvroIw0aNEhXXnllZcMAAAAAAACoEs2bN9e4ceP0wgsvqEmTJt7L3y677DLdc889euqpp/TCCy94l3/iiSckSZdffrm3rWnTpmrYsKGefPJJ5eXl6cILL5RUWNj605/+pIULF+r888+v9KV1vxWVfpe+++47SdKiRYu0aNGiEo+PGzdOtWrV0hVXXKGlS5dq7ty5KigoUIsWLTRjxgz96U9/8nstLwAAAAAAgF3uvfdevfbaa/rxxx+VkpIiSerUqZMmTJigF198UceOHVPv3r21du1azZ07V7/73e/Ut29fn9fo1auX3njjDXXo0EFnnXWWJOncc89VbGystm7dqmuuuSboeYWqShewVq5cWeYytWrV0muvvVbZVQEAAAAAAARFixYtNG7cOM2dO9en/eWXX1azZs00Z84cvfvuu6pfv76mTZum6dOnl3gNTwHroosu8ra5XC5dcMEFWrZsGfe/qgDLVPb3GW2QkZGhhISE0/7pRQAAACDUlPylPPv4+6W8U4VSvKEUK2CH7Oxsbd++XU2bNlVUVJTd4cChytpPKlvL4UJLAAAA/GZRuAAAIDRw8ykAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAACAamJZlu6//367wwh5FLAAAAAAAMBvkmVZ5fq3cuVKu0P9zXPZHQAAAAAAAAhhP/9sdwRSixan9bTXXnvN5+9XX31VS5cuLdHetm3b0w4NVYMCFgAAAAAA+E0aN26cz99r1qzR0qVLS7TDflxCCAAAAAAAEMCJEyd0xx13qFGjRoqMjFTr1q01a9YsGWN8lsvJydEf//hH1a1bVzVr1tTQoUO1e/fuEq+3c+dO/eEPf1Dr1q0VHR2t2rVra9SoUdqxY4d3mW3btsmyLD355JMlnv/ll1/Ksiz9+9//rvJcnYwCFgAAAAAAgB/GGA0dOlRPPvmkBg0apCeeeEKtW7fWnXfeqdtvv91n2d///vd66qmnNGDAAD366KOqUaOGLr/88hKv+fXXX+vLL7/UmDFj9Mwzz+iGG27Q8uXL1adPH508eVKS1KxZM1144YWaP39+iefPnz9fNWvW1JVXXlk9STsUlxACAAAAAAD48cEHH+jTTz/Vww8/rHvvvVeSdNNNN2nUqFF6+umndfPNN6t58+b6/vvvNW/ePP3hD3/QP/7xD+9yY8eO1fr1631e8/LLL9fIkSN92oYMGaILLrhAb7/9tq699lpJ0vjx43X99ddry5YtatOmjSQpLy9PCxYs0PDhwxUTE1Pd6TsKM7AAAAAAAAD8+OijjxQeHq6pU6f6tN9xxx0yxmjx4sXe5SSVWO62224r8ZrR0dHe/8/Ly9Phw4fVokUL1apVS99++633sauuukpRUVE+s7A++eQTpaWl/Sbv0UUBCwAAAAAAwI+dO3eqQYMGqlmzpk+751cJd+7c6f1vWFiYmjdv7rNc69atS7xmVlaW/vrXv3rvqVWnTh3VrVtXx44dU3p6une5WrVqaciQIXr99de9bfPnz1fDhg3Vr1+/KssxVFDAAgAAAAAACJJbbrlFjzzyiK666iotWLBAS5Ys0dKlS1W7dm253W6fZcePH69t27bpyy+/1PHjx/XBBx/o6quvVljYb6+cwz2wAAAAAAAA/GjSpImWLVum48eP+8zC2rJli/dxz3/dbrd++eUXn1lXP/74Y4nXXLhwoSZMmKC///3v3rbs7GwdO3asxLKDBg1S3bp1NX/+fPXo0UMnT5703iPrt+a3V7IDAAAAAAAoh8suu0wFBQV67rnnfNqffPJJWZalwYMHS5L3v88884zPck899VSJ1wwPD5cxxqft2WefVUFBQYllXS6Xrr76ai1YsEBz5sxRhw4d1LFjx8qkFLKYgQUAAAAAAODHkCFD1LdvX917773asWOHOnXqpCVLluj999/Xbbfd5r3nVefOnXX11Vfr+eefV3p6unr27Knly5fr559/LvGaV1xxhV577TUlJCSoXbt2Wr16tZYtW6batWv7jWH8+PF65plntGLFCj322GPVmq+TUcACAAAAAADwIywsTB988IH++te/6s0339Ts2bN1zjnn6PHHH9cdd9zhs+wrr7zivdzvvffeU79+/fSf//xHjRo18lnu6aefVnh4uObPn6/s7GxdeOGFWrZsmQYOHOg3hvPOO08pKSnavHmzxo4dW225Op1lTp23FgIyMjKUkJCg9PR0xcfH2x0OAAAAQtSSjXZHUGRA+9IfD6VYpdCKN5RiBeyQnZ2t7du3q2nTpoqKirI7nN+kLl26KDExUcuXL7c7lIDK2k8qW8vhHlgAAAAAAAAOlZqaqu+++07jx4+3OxRbcQkhAAAAAACAw2zcuFHffPON/v73vyspKUmjR4+2OyRbMQMLAAAAAADAYRYuXKhJkyYpLy9P//73v3/zl28yAwsAAAAAQgj37AJ+G+6//37df//9dofhGMzAAgAAAAAAgKNRwAIAAAAAAICjUcACAAAAAABlMsbYHQIcrLr3DwpYAAAAAAAgoPDwcElSXl6ezZHAyTz7h2d/qWoUsAAAAAAAQEA1atRQZGSk0tPTmYUFv4wxSk9PV2RkpGrUqFEt6+BXCAEAAAAAQKnq1KmjPXv2aPfu3UpISFCNGjVkWZbdYcFmxhjl5eUpPT1dmZmZatiwYbWtiwIWAAAAAAAoVXx8vCQpLS1Ne/bssTkaOE1kZKQaNmzo3U+qAwUsAAAAAABQpvj4eMXHxysvL08FBQV2hwOHCA8Pr7bLBoujgAUAAAAAAMqtRo0aQSlYAMVxE3cAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4msvuAAAAAHDmWLLR7giKDGhvdwQAAKCqMAMLAAAAAAAAjkYBCwAAAAAAAI7GJYQAAAAAgGrBZcUAqgozsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GiVLmB9/fXXuvnmm5WSkqLY2Fg1btxYV111lbZu3Vpi2c2bN2vQoEGKi4tTYmKirr32Wh06dKiyIQAAAAAAAOAM5qrsCzz22GP64osvNGrUKHXs2FH79+/Xc889p3PPPVdr1qxR+/btJUm7d+/WxRdfrISEBM2YMUOZmZmaNWuWNmzYoLVr1yoiIqLSyQAAAAAAAODMU+kC1u23367XX3/dpwA1evRodejQQY8++qjmzZsnSZoxY4ZOnDihb775Ro0bN5Ykde/eXZdeeqnmzJmj6667rrKhAAAAAAAA4AxU6UsIe/bsWWL2VMuWLZWSkqLNmzd7295++21dccUV3uKVJF1yySVq1aqVFixYUNkwAAAAAAAAcIaqlpu4G2N04MAB1alTR5K0Z88eHTx4UF27di2xbPfu3bVu3brqCAMAAAAAAABngEpfQujP/PnztWfPHj344IOSpH379kmSkpKSSiyblJSkI0eOKCcnR5GRkX5fLycnRzk5Od6/MzIyJEn5+fnKz8+XJIWFhSksLExut1tut9u7rKe9oKBAxpgy28PDw2VZlvd1i7dLUkFBQbnaXS6XjDE+7ZZlKTw8vESMgdrJiZzIiZzIiZzIiZxCLSdjwv/3P77tVlhhTr7tlqywcBnjloy77HYrTJYVFrjdXSCpKHa3u+ycfFfrP/ZA7VWdU35+6dvJuAPnKqswJ+P23U7VlVN+ftn7Xnm3U7ByKq0/FYVZNfteZXIq3tUC9TMp+P0pULsxpR8jCpf3n6tPcxCOERzLyYmc7M3p1LwqqsoLWFu2bNFNN92kCy64QBMmTJAkZWVlSZLfAlVUVJR3mUAFrJkzZ+qBBx4o0b5u3TrFxsZKkurWravmzZtr+/btPr9smJycrOTkZG3dulXp6ene9mbNmqlevXrauHGjNz5JatOmjWrVqqV169b5bOyOHTsqIiJCqampPjF07dpVubm5Wr9+vbctPDxc3bp1U3p6urZs2eJtj46OVqdOnZSWlqZt27Z52xMSEtS2bVvt3btXu3fv9raTEzmREzmREzmREzmFWk6K6SpTkKu8tKKcLCtcEfW7yeSmK+9IUU6WK1oRdTvJnZWm/PSinMIiE1Qjsa0KMveqILMop/DounLVaq6C9O0qyCrKKTwuWa6ayco/tlXunKKc0uqXnVPusaKcatTpKCs8QrkHfHOKODs4OaWmlr6dco9LroRmCo+pp7zDG2Xyi3KqkdhGVmQt5R1cJ2OqP6fUk2Xve+XdTsHIqaz+lHu8/NupunNKPVmUU6BjhKKD358C5ZTeuPRjhF39yV9OHMvJiZzszckzGel0WaZ4aayS9u/frwsvvFB5eXlas2aNGjRoIElKTU1Vt27d9Oqrr+raa6/1ec5dd92lxx9/XNnZ2RWagdWoUSMdPnxY8fHxkqh4khM5kRM5kRM5kRM5OSGn5ZudMwPr0vZl57R8U/HV2jsDq3/b0rfT8k2Bcw32DKz+7cre9z7Z4JwZWJemlN6fivYD+2dg9W9X1Byon326xTkzsAZ0KP0YsWSDc2Zg9W/LsZycyMnOnDIyMlS7dm2lp6d7azkVUWUzsNLT0zV48GAdO3ZMq1at8havpKJLBz2XEha3b98+JSYmBixeSYUzt/w97nK55HL5puB5007l2bDlbT/1dU+n3bIsv+2BYqxoOzmRU6B2ciIniZwCxVjRdnIiJ4mcAsXor92yPP/jPyf/7WGSVTLGCreH+cbuSbu0nPy8jN8YA7VXZU4uV+nbqfjTTs21qL38sQdqL09OxTd7oH2svNup7Paqyam0/nRqmJXd98puDxy7v64W6BgRzP4UqN3T5wMdIyqy/ao7J47l5BSonZyCk1Og+MurSgpY2dnZGjJkiLZu3aply5apXbt2Po83bNhQdevWLTnFXNLatWvVuXPnqggDAAAAAAAAZ6BK/wphQUGBRo8erdWrV+utt97SBRdc4He5ESNG6MMPP9SuXbu8bcuXL9fWrVs1atSoyoYBAAAAAACAM1SlZ2Ddcccd+uCDDzRkyBAdOXJE8+bN83l83LhxkqR77rlHb731lvr27atbb71VmZmZevzxx9WhQwdNmjSpsmEAAAAAAADgDFXpAtZ3330nSVq0aJEWLVpU4nFPAatRo0b67LPPdPvtt+vPf/6zIiIidPnll+vvf/97qfe/AgAAAAAAwG9bpQtYK1euLPeyKSkp+uSTTyq7SgAAAAAAAPyGVNmvEAIAAAAAEMqWbLQ7giID2tsdAeAslb6JOwAAAAAAAFCdKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNFcdgeA/3n1VbsjKDJ+vN0RAAAAAAAAeDEDCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACO5rI7AAAAAAAAUDFLNtodQZEB7e2OAL8FzMACAAAAAACAo1HAAgAAAAAAgKNRwAIAAAAAAICjcQ8sAAAAh+M+JwAA4LeOGVgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNG7ijgrjRrIAAAAAACCYmIEFAAAAAAAAR2MGlkP8kmZ3BEWa2x0AAAAAAABAMczAAgAAAAAAgKNRwAIAAAAAAICjUcACAAAAAACAo1HAAgAAAAAAgKNRwAIAAAAAAICjUcACAAAAAACAo7nsDgCobks22h1BkQHt7Y4AAAAAAIDQwwwsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GvfAAgAAAAAA1Yp7E6OymIEFAAAAAAAAR6OABQAAAAAAAEejgAUAAAAAAABHo4AFAAAAAAAAR6OABQAAAAAAAEejgAUAAAAAAABHo4AFAAAAAAAAR6OABQAAAAAAAEejgAUAAAAAAABHo4AFAAAAAAAAR3PZHQAAAAAAAIBTLNlodwRFBrS3OwLnYAYWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHM1ldwAAAADBtmSj3REUGdDe7ggAAACcjxlYAAAAAAAAcDQKWAAAAAAAAHC0KilgZWZmavr06Ro0aJASExNlWZbmzJlTYrmJEyfKsqwS/9q0aVMVYQAAAAAAAOAMVCX3wEpLS9ODDz6oxo0bq1OnTlq5cmXAZSMjI/Xyyy/7tCUkJFRFGAAAAAAAADgDVUkBKykpSfv27VP9+vWVmpqqbt26BV6hy6Vx48ZVxWqBMw43FQYAAAAAoKQquYQwMjJS9evXL/fyBQUFysjIqIpVAwAAAAAA4AwX9Ju4nzx5UvHx8UpISFBiYqJuuukmZWZmBjsMAAAAAAAAhIgquYSwvJKSknTXXXfp3HPPldvt1scff6znn39e33//vVauXCmXy384OTk5ysnJ8f7tmb2Vn5+v/Px8SVJYWJjCwsLkdrvldru9y3raCwoKZIwpsz08PFyWZXlft3i7VDh7rDztLpdLxhifdsuyFB4eXiJGy7IkSUaSsYq9iCmsMLolqVi7ZQr/dBdf9jTbdeo6Je/7ESgn4y7ebskKC5cxbsm4y263wmRZYYHb3QX/eyfKai//djLuwuUL//DNyQorzMm3vfpyys8vfd+TLBm3b06BYq/unKTQ7U/+2kP9GEFO5EROVZtTdY9PFTmWG1N2TuZ/JwN2jrmenDybK9D2MMYZY64kud1l73u+q7VnzPXklJ9fen8qPKepun2vMjnl55d9jLCjP5WWU2nHiKIwg9uf/MVe/JAYqJ9Jwe9PgdqNKf1Y7vvZQUHrT/7ayzM+eT47BLM/BWov/tnBXz+T7OtPp+YklX0e4U3XxjHX0158d/V3HmHczhhzpcL94Ew53zv1OFFRQS1gzZw50+fvMWPGqFWrVrr33nu1cOFCjRkzJuDzHnjggRLt69atU2xsrCSpbt26at68ubZv365Dhw55l0lOTlZycrK2bt2q9PR0b3uzZs1Ur149bdy4UVlZWd72Nm3aqFatWlq3bp3Pxu7YsaMiIiKUmprqE0PXrl2Vm5ur9evXe9vCw8PVrVs3paena8uWLd726OhoderUSWlpadq2bZu3PSEhQRGS0uNqKD2uhrc9LitftdNzdTQhQpnRRZsqITNPtTLzdKhWpLIjw73tiem5qpmVr/21o5TnKppcV+9ItqJz3dpdL1rGKqpWJaVlyVVgtOvsGJ+cmhYUlJpT7oGinCxXtCLqdpI7K0356UU5hUUmqEZiWxVk7lVB5u6i14muK1et5ipI366CrKLtFB6XLFfNZOUf2yp3TtF2ciU0U3hMPeUd3iiTX7SdaiS2kRVZvu2Ue1yKOLurTEGu8tKKcrKscEXU7yaTm668I8HJKfVk6fueVEt5B9fJFDvY1qjTUVZ4hHIP+O571Z2TFLr9qW3bttq7d6927y7KKdSPEeRETuRUtTlV9/hUkWN5VlbZOeUet3/M9eSUerL07aQYZ4y5kpRWv+x9L/eY/WOuJ6fU1NL7U+7xqt33KpNT6smyjxF29KdAOZV1jMg9Xv7tVN05efqYFPi4p+jg96dAOaU3Lv1Ybld/8pdTecan3OPB70+Bcko9WfqYK9nTn/zlJJV9HuHpZ3aOuZ6cPP0s0HlEXpYzxlypcD84U873KnsrKcsUL41VAc9N3GfPnq2JEyeWuXxWVpbi4uI0adKkEr9O6OFvBlajRo10+PBhxcfHSwr9b4N3PD3fMTOwWtx2bak5Ldlg/zc9nsp0vzZlb6flm2TrNz3FY+/frvR9b+kP9n/T44l9YIfQ7U9n6owRciIncqq6nD7Z4JwZWAPal53T8k2S3WOuJ6f+7QqbA22P5ZudMeZK0qXty973Ct/bolz9xR6s84j+bUvvT4XnNM6YgdW/XdnHiID9zIYZI5emlH6MKNoP7J+B5eljUuB+9ukW58zAGtCh9GO572cHBa0/+Wvv37bs8cnz2cEJM7CKf3bw18+WbXLODKyBHcs+j/D2MwfMwCrez/ydRyzf5IwxVyrcD86U872MjAzVrl1b6enp3lpORQR1BpY/0dHRql27to4cORJwmcjISEVGRpZod7lcJS479Lxpp/Js2PK2B7qcsSLtlmX5bQ8Uo6WiopLP8pLPPu1tD1B6rGj7qev0XNIYKCcrzF97mAovO6tke5j/7RGovTzbw2c1lv+c/LdXfU7Fww207/l7fwsfKH97VeUUyv2pou3kRE6B2snpzMypusenihzLLavsnIqHZNeY68np1FBPjd072dvmMVeSPJu+tH3Pz8vYMuZaVphcrtL7k89+UAX7XqD28uRUfLNXuJ9VY38K1F7WMeLUMO08Rvg79AU6RgSzPwVq9/T5QMfsih0Pqzen8oxPvv3M3vPycvUzm/qTv/ayzhfK3c+CkNOpu+upxwhPWHaPuZLvfhDq53uB4i8vf0N2UB0/flxpaWmqW7eu3aEAAAAAAADAgYJWwMrOztbx48dLtD/00EMyxmjQoEHBCgUAAAAAAAAhpMouIXzuued07Ngx7d27V5K0aNEi7w3AbrnlFh09elRdunTR1Vdf/b+bVUuffPKJPvroIw0aNEhXXnllVYUCAAAAAACAM0iVFbBmzZqlnTt3ev9+55139M4770iSxo0bp1q1aumKK67Q0qVLNXfuXBUUFKhFixaaMWOG/vSnP/m9phIAAAAAAACosgLWjh07ylzmtddeq6rVAQAAAAAA4DeCaU8AAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNApYAAAAAAAAcDQKWAAAAAAAAHA0ClgAAAAAAABwNJfdAQAAgDPDko12R1BkQHu7IwAAAEBVYgYWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAczWV3AAAAwL8lG+2OoMiA9nZHAAAAgN8yZmABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0biJO4DTxg2mAQAAAADBwAwsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOJrL7gAAAAimJRvtjqDIgPZ2RwAAAACEBmZgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0ShgAQAAAAAAwNEoYAEAAAAAAMDRKGABAAAAAADA0aqkgJWZmanp06dr0KBBSkxMlGVZmjNnjt9lN2/erEGDBikuLk6JiYm69tprdejQoaoIAwAAAAAAAGcgV1W8SFpamh588EE1btxYnTp10sqVK/0ut3v3bl188cVKSEjQjBkzlJmZqVmzZmnDhg1au3atIiIiqiIcAAAAAAAAnEGqpICVlJSkffv2qX79+kpNTVW3bt38LjdjxgydOHFC33zzjRo3bixJ6t69uy699FLNmTNH1113XVWEAwAAAAAAgDNIlVxCGBkZqfr165e53Ntvv60rrrjCW7ySpEsuuUStWrXSggULqiIUAAAAAAAAnGGCdhP3PXv26ODBg+ratWuJx7p3765169YFKxQAAAAAAACEkCq5hLA89u3bJ6nwcsNTJSUl6ciRI8rJyVFkZGSJx3NycpSTk+P9OyMjQ5KUn5+v/Px8SVJYWJjCwsLkdrvldru9y3raCwoKZIwpsz08PFyWZXlft3i7JBUUFJSr3eVyyRjj025ZlsLDw0vEaFmWJMlIMlaxFzGFFUa3JBVrt0zhn+7iy55mu05dp+R9PwLlZNzF2y1ZYeEyxi0Zd9ntVpgsKyxwu7vgf+9EWe3l307GXbh84R++OVlhhTn5tldfTvn5pe97kiXj9s0pUOzVnZNUdn/yPqWM7RSMnDy7QqB+FurHCHKqupyMUdD7U6BjhFRGTm57+pO/9vz8sreTMad3LK+OnAoKSt/3qnt8qkhOxpTdn8z/TgbsHHM9OXm6VaBjgTHOGHMlye0u+xjhu1p7xlxPTv76WfHYC89p7B9zpcL9oKxjuR39qbScShufisIMbn/yF3vxoStQP5OC358CtRtT+nmE72cHBa0/+Wsvz3mE57ODnWNu8X5W2rmR5Iwxt/DTZtnneyU+O9h4jCi+u/o7hzVuZ4y5UuF+cKacl596nKiooBWwsrKyJMlvgSoqKsq7jL/HZ86cqQceeKBE+7p16xQbGytJqlu3rpo3b67t27f7/KphcnKykpOTtXXrVqWnp3vbmzVrpnr16mnjxo3e2CSpTZs2qlWrltatW+ezsTt27KiIiAilpqb6xNC1a1fl5uZq/fr13rbw8HB169ZN6enp2rJli7c9OjpanTp1UlpamrZt2+ZtT0hIUISk9LgaSo+r4W2Py8pX7fRcHU2IUGZ00aZKyMxTrcw8HaoVqezIcG97Ynquambla3/tKOW5iibX1TuSrehct3bXi5axiqpVSWlZchUY7To7xienpgUFpeaUe6AoJ8sVrYi6neTOSlN+elFOYZEJqpHYVgWZe1WQubvodaLrylWruQrSt6sgq2g7hccly1UzWfnHtsqdU7SdXAnNFB5TT3mHN8rkF22nGoltZEWWbzvlHpcizu4qU5CrvLSinCwrXBH1u8nkpivvSHBySj1Z+r4n1VLewXUyxQ62Nep0lBUeodwDvvtedeckld2fco+XbzsFI6fUk4XtCQkJatu2rfbu3avdu4tyOpJfuJ3yj/nfTnlH/O97uYdK5hQWWUu5+08/p/q1Kn6M8JdTqB/37MpJJvj9KdAxQio9p9yD9vQnfzmlppa9nQrM6R3LqyOnjab0fa+6x6eK5JSVVXZ/yj1u/5jryclzvA10jFCMM8ZcSUqrX/YxIveY/WOuJ6fU1NKPe7nHnTHmSoXnNGUdy+3oT4FyKmt88pzTBLs/+cvJ08ekwGOuooPfnwLllN649PMIp4y5rprlO4/IPW7/mOvJKfVk6edGkjPGXMsVLans8z1PP7NzzPXk5Olngc5h87KcMeZKhfvBmXJe7pmMdLosU7w0VgU8N3GfPXu2Jk6cWKL91Vdf1bXXXuvznLvuukuPP/64srOzyz0Dq1GjRjp8+LDi4+Mlhf5MhB1Pz3fMDKwWt11bak5LNtj/TY+nMt2vTdnbafkm2fpNT/HY+7crfd9b+oP93/R4Yh/Yoez+tHxT4Fw9MQbr26v+7f7XGqCfLd9s/zc9Hv3bOfdbkeLOlG96To19yUY5ZgbWwA6l57TsB+fMwOrftuzt5O1nDvg2+JKU0ve9TzY4ZwbWgPZl96fC460zvg32HG8DHQuWb3bGmCtJl7Yv+xjhHcv+l6u/2IN1jPDXz4rHXnhOY/+YKxXuB2UdywP2MxuOEZemlD4+Fe0H9s/A8vQxKXA/+3SLc2ZgDehQ+nmE72cHBa0/+Wvv37bs8wjPZwcnzMAq/tnBXz9btskZY65kaWDHss/3Snx2sPG8vHg/83cOu3yTM8ZcqXA/OFPOyzMyMlS7dm2lp6d7azkVEbQZWJ5LBz2XEha3b98+JSYm+i1eSYWztvw95nK55HL5puB5007l2bDlbT/1dU+n3bIsv+2BYrQkb1HJZ3nJZ5/2tgcoPVa0/dR1ei5pDJSTFeavPUyy/ORU0fYw/9sjUHt5tofPaiz/Oflvr/qciocbaN/z9/4WPlD+9qrKqaz+dOpTAm+/6s/p1F3h1Ng9kw+rat+rTE6eWCt6jKhoeygc9+zIybJkS38K1F5aTn4Wt+0Y4XKVvZ28/SyI/alo3b45ed7WgGNuNY9PFcnJssruT8VDsmvM9eR0aqinxu6d7G3zmCtJnk1f2jHCXz+z6xjhr58Vj91nP7BxzJV894MK9zObjhGljU8lzmlsPEb4G3YDHSOC2Z8CtXv6fKDzhYodD+0bc4viLfY6Np+Xl6ufOWDMLSvGCvezIOR06u566jHCE5bdY67kux+E+nl5oPjLy9+QXS0aNmyounXrlpxmLmnt2rXq3LlzsEIBAAAAAABACAlaAUuSRowYoQ8//FC7du3yti1fvlxbt27VqFGjghkKAAAAAAAAQkSVXUL43HPP6dixY9q7d68kadGiRd4bgN1yyy1KSEjQPffco7feekt9+/bVrbfeqszMTD3++OPq0KGDJk2aVFWhAAAAAAAA4AxSZQWsWbNmaefOnd6/33nnHb3zzjuSpHHjxikhIUGNGjXSZ599pttvv11//vOfFRERocsvv1x///vfA97/CgDgbEs22h1BkQHt7Y4AAAAAQHWosgLWjh07yrVcSkqKPvnkk6paLQAAAAAAAM5wQb0HFgAAAAAAAFBRFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoFLAAAAAAAADgaBSwAAAAAAAA4GgUsAAAAAAAAOBoLrsDAACUtGSj3REUGdDe7ggAAAAA/NYxAwsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACORgELAAAAAAAAjkYBCwAAAAAAAI5GAQsAAAAAAACOFtQC1sqVK2VZlt9/a9asCWYoAAAAAAAACBEuO1Y6depUdevWzaetRYsWdoQCAAAAAAAAh7OlgNWrVy+NHDnSjlUDAAAAAAAgxNh2D6zjx48rPz/frtUDAAAAAAAgRNhSwJo0aZLi4+MVFRWlvn37KjU11Y4wAAAAAAAAEAKCeglhRESERowYocsuu0x16tTRpk2bNGvWLPXq1UtffvmlunTp4vd5OTk5ysnJ8f6dkZEhScrPz/fO4goLC1NYWJjcbrfcbrd3WU97QUGBjDFltoeHh8uyrBKzw8LDwyVJBQUF5Wp3uVwyxvi0W5al8PDwEjFaliVJMpKMVexFTGGF0S1JxdotU/inu/iyp9muU9cped+PQDkZd/F2S1ZYuIxxS8ZddrsVJssKC9zuLvjfO1FWe/m3k3EXLl/4h29OVlhhTr7t1ZdTfn7p+55kybhPmZkYIPbqzkkquz95n1LGdgpGTp5dIVA/M6Zq973K5JSfX/YxwriD358C5ZSfX/pxz7PqYPcnf+2e/aC0Y7kxCnp/CpSTVMb45LanP/lrz88veSwI2M+C2J8C5VRQEHjMLdwP7OlP/nIypuzzCPO/kwE7x1xPTsX7mVQydmOcMeZKkttd9vme72rtGXM9OfnrZ8VjLzynsX/MlQr3g0Bjrid2J4y5xXMq7by8KEx7x1yZAhUfugL1M8n+MdfDmNLPy30/Oyho/clfe3k+E3o+O9g55hbvZ6V9zpWcMeZKlqTAY26JfmbjmOtpL767+jsvN25njLlS4X5Q3fWI0o7lVVljqexVeEEtYPXs2VM9e/b0/j106FCNHDlSHTt21LRp0/Txxx/7fd7MmTP1wAMPlGhft26dYmNjJUl169ZV8+bNtX37dh06dMi7THJyspKTk7V161alp6d725s1a6Z69epp48aNysrK8ra3adNGtWrV0rp163w2dseOHRUREVFitljXrl2Vm5ur9evXe9vCw8PVrVs3paena8uWLd726OhoderUSWlpadq2bZu3PSEhQRGS0uNqKD2uhrc9LitftdNzdTQhQpnRRZsqITNPtTLzdKhWpLIjw73tiem5qpmVr/21o5TnKppcV+9ItqJz3dpdL1rGKqpWJaVlyVVgtOvsGJ+cmhYUlJpT7oGinCxXtCLqdpI7K0356UU5hUUmqEZiWxVk7lVB5u6i14muK1et5ipI366CrKLtFB6XLFfNZOUf2yp3TtF2ciU0U3hMPeUd3iiTX7SdaiS2kRVZvu2Ue1yKOLurTEGu8tKKcrKscEXU7yaTm668I8HJKfVk6fueVEt5B9fJFDvY1qjTUVZ4hHIP+O571Z2TVHZ/yj1evu0UjJxSTxa2JyQkqG3bttq7d6927y7KqSC/ave9yuS0LqfsY0TugeD3p0A5lXXcyz1uT3/yl5NnPyjtWC4T/P4UKCep9PEp96A9/clfTqmpRTkFGnMLTPD7U6CcNprAY27btvb1J385ZWWVfR6Re9z+MdeTk6efBTo3UowzxlxJSqtf9vle7jH7x1xPTqmppZ/D5h53xpgrFZ7TBBpzPccIJ4y5npzKOi/3nNPYPebmHkj19jEp8GcNRds/5nqkNy7985NTxlxXzfJ9Jsw9bv+Y68kp9WTpn3MlZ4y5litaUuAx13OM8PQzO8dcT06efhbos3teljPGXKlwP6juekRpx/KqrLF4JiOdLssUL43Z5Oqrr9Y777yjkydPeiuIxfmbgdWoUSMdPnxY8fHxkkJ/BtaOp+c7ZgZWi9uuLTWnJRvs/6bHU5nu16bs7bR8k2z9pqd47P3blb7vLf3B/m96PLEP7FB2f1q+KXCunhiD9e1V/3b/aw3Qz5Zvtv+bHo/+7co+RizdaO83PcVj79+29OOeZz9wwgwsz35Q2rF8yUbZNrvCXz8rbXxa9oNzZmD1b1v2N3LefuaAb4MvSSn9W8ZPNtg3u+LU9gHtyz6PKOxnzvg2uHg/k0rGvnyzM8ZcSbq0fdnne96x7H+5+os9WMcIf/2seOyF5zT2j7lS4X5Q1rf2AfuZDceIS1NKPy8v2g/sn4Hl6WNS4H726Rb7x1yPAR1K//zk+9lBQetP/tr7ty37M6Hns4MTZmAV/+zgr58t2+SMMVeyNLBj2TN7Snx2sPG8vHg/83devnyTM8ZcqXA/OFNmYGVkZKh27dpKT0/31nIqwpZfITxVo0aNlJubqxMnTvhNIjIyUpGRkSXaXS6XXC7fFDxv2qn8FcZKaz/1dU+n3bIsv+2BYrQkb1HJZ3nJZ5/2tgcoPVa0/dR1ei5pDJSTFeavPUyy/ORU0fYw/9sjUHt5tofPaiz/Oflvr/qciocbaN/z9/4WPlD+9qrKqaz+dOpTAm+/6s/p1F3h1Ng9kw+rat+rTE6eWEs7Rlj+jhHV3J8C5VRWPyu+6mD2J3/tp4bq/zgmW/pToPbSxic/i9t2jHC5yj5GePtZEPtT0bp9c/K8rQHHXJv6k//Yyz6P8O1n9oy5npzK6mfeyd42j7mS5Nn0pZ3v+etndh0j/PWz4rH77Ac2jrmS735Q4X5m0zGitPPyEuc0Nh4j/A27gY4Rdo65Rc8PHGPh8qEx5hbFW+x1bD4vL1c/c8CYW1aMFe5nQcjp1N311GOEJyy7x1zJdz+oznpERdtPp8YSKP7y8jdkB922bdsUFRWluLg4u0MBAAAAAACAwwS1gFX8ukmP77//Xh988IEGDBjgt6oHAAAAAACA37agXkI4evRoRUdHq2fPnqpXr542bdqkF198UTExMXr00UeDGQoAAAAAAABCRFALWL/73e80f/58PfHEE8rIyFDdunU1fPhwTZ8+XS1atAhmKAAAAAAAAAgRQS1gTZ06VVOnTg3mKgEAAAAAABDiuOkUAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcjQIWAAAAAAAAHI0CFgAAAAAAAByNAhYAAAAAAAAcLegFrJycHN19991q0KCBoqOj1aNHDy1dujTYYQAAAAAAACBEBL2ANXHiRD3xxBMaO3asnn76aYWHh+uyyy7T559/HuxQAAAAAAAAEAJcwVzZ2rVr9cYbb+jxxx/Xn/70J0nS+PHj1b59e91111368ssvgxkOAAAAAAAAQkBQZ2AtXLhQ4eHhuu6667xtUVFRmjJlilavXq1du3YFMxwAAAAAAACEgKAWsNatW6dWrVopPj7ep7179+6SpO+++y6Y4QAAAAAAACAEBPUSwn379ikpKalEu6dt7969fp+Xk5OjnJwc79/p6emSpCNHjig/P1+SFBYWprCwMLndbrndbu+ynva</t>
-  </si>
-  <si>
-    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACA5UlEQVR4nOzdd3xTdfv/8fdp0sVokbIpe1tkD0W2imxvGaK3bPwiLvSnt3rjYijguhXF24mCA1TABQrKEBSRIVoQBKy3DIECUkbL6Epyfn/UhIYmHdAmJ/h6Ph48lCsnOdeVMz7JxeecGKZpmgIAAAAAAAAsKizYCQAAAAAAAAD5oYEFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAgIXUrl1bhmF4/YmMjFTNmjU1ZMgQrVmzJiB5jBw5UoZhaM6cOQFZX0lxv5979uwJdioXPff+CgAAUBJoYAEAYEFXXnmlRowYoREjRqhXr15yuVyaP3++unTpoueeey7Y6VlCKDXZAtlImzNnjgzD0MiRI0t8XQAAAIFiD3YCAAAgr1tuucWrAZGRkaFbb71V77zzjh544AH17dtXDRs2DF6CIWLlypXKzs5W9erVg50KAAAALgAzsAAACAFRUVH673//q9KlS8vpdOrjjz8OdkohoV69emrcuLHCw8ODnQoAAAAuAA0sAABCRJkyZdSoUSNJynMp2ldffaW+ffuqUqVKioiIULVq1TRkyBBt2rTJ7+sdO3ZM99xzj2rVquW5z9add96pY8eOnVd+kyZNkmEYmjRpkvbu3avhw4eratWqioqKUsOGDTVp0iSlp6fneV52drbee+893XzzzWrcuLFiYmIUHR2tRo0aafz48UpOTvZafs+ePTIMQ2+//bYkadSoUV73DJs0aZJn2YIu3Vu4cKF69uypihUrKiIiQtWrV9fQoUO1ffv2PMu611u7dm2ZpqnXX39drVu3VunSpRUbG6sePXpo3bp1Xs9xX863d+9eSVKdOnW8cl29erVn2RUrVqhfv36qXLmywsPDdckll6hBgwYaOnSovv3228JsAtWuXVujRo2SJL399tte6+ratavXsmfOnNGTTz6pVq1aqWzZsipVqpQSEhL0yCOP6Pjx44Vanz9vvPGG570pV66cevfurfXr1/td3uFwaNasWeratavKly+vyMhI1alTR7fddpv27dtX5PX/+OOPGjJkiOLj4xUREaGYmBjVrVtXAwcO1Geffeb3OTfffLNq1qypyMhIlS9fXtdee62WLFlSbHmvXr3asy2ys7P11FNPKSEhQdHR0YqLi9OAAQO0Y8eOItcLAMDfAZcQAgAQQtLS0iRJkZGRntijjz6qJ554QoZhqEOHDqpZs6Z27Nih+fPn66OPPtLrr7+u0aNHe73O4cOH1alTJ/3222+65JJL1LdvX7lcLs2dO1dffvmlEhISzjvH3bt3q3Xr1rLb7ercubPS09O1atUqTZ48WStWrNCKFSsUFRXllcuwYcMUGxurJk2aqFmzZjp9+rQ2b96smTNn6oMPPtD333+v+vXrS8pp5I0YMULfffedfv/9d1155ZWexySpRYsWBebocDh08803a/78+YqMjFTr1q1VvXp1JSUlae7cufr444/18ccfq2fPnj6fP2rUKM2bN0+dOnVS3759tXnzZi1fvlzffvutvvnmG7Vv316SVL9+fY0YMUILFy7U6dOnNXDgQJUpU8bzOlWqVJGU02xyN57atWunbt26KT09Xfv379cHH3ygChUqqHPnzgXWNWjQIK1fv15r165VvXr11LFjR89jjRs39vz/sWPHdNVVV2nz5s2KiYlR9+7dFR4erm+++UZTp07VvHnz9PXXX6t27doFrvNc9957r2bMmKErr7xS1113nbZu3aqlS5dq+fLlmj9/vq6//nqv5U+ePKn+/ftr9erVKlOmjFq3bq2KFStq69atevXVV7VgwQItX75cLVu2LNT6V65cqV69eik7O1vNmzfXFVdcIafTqQMHDuiLL76Q0+nUdddd5/WcF154Qffee69cLpdatGih9u3b69ChQ1q9erWWLVumyZMn67HHHiu2vLOzs9W7d299//336ty5s5o0aaKNGzfqk08+0apVq5SYmHhe7z0AABc1EwAAWEatWrVMSebs2bPzPLZlyxYzLCzMlGS+9dZbpmma5tKlS01JZlRUlLls2TKv5WfNmmVKMsPDw81t27Z5PTZo0CBTktmpUyfzxIkTnvjRo0fN9u3bm5L85uHPxIkTPc+77rrrzDNnznge27dvn9mwYUNTkvnvf//b63lpaWnmZ599ZmZmZnrFs7KyzAkTJpiSzN69e+dZ34gRIwrM0f1+7t692yv+0EMPmZLM9u3bm7t27fJ6bMGCBabNZjMvueQS8/jx45747t27PfXVqlXL/PXXXz2PORwOc/To0aYks0ePHoXOw61OnTqmJHPNmjV5Hjt8+LD5008/+a3xXLNnzzYlmSNGjPC7zJAhQzz1p6SkeOInT540e/XqZUoyO3ToUOh1mqbpeW+io6PNlStXej329NNPm5LM2NhY8/Dhw16P/fOf/zQlmX379s3z2PPPP29KMhs0aGA6HI5C5dGtWzdTkvnee+/leezEiRPmunXrvGJffvmlaRiGWaFCBfObb77xeuznn3824+PjTUnm6tWrLzjvVatWed6nli1bmgcPHvQ8lp6ebl577bWmJHPs2LGFqhUAgL8TGlgAAFiIrwbWiRMnzC+++MKsV6+eKcmsVq2aeerUKdM0TfOqq64yJZn33nuvz9fr27evKcn8v//7P0/sjz/+MMPCwkzDMMxffvklz3MSExMvqIEVHR3t9cXcbfHixaYkMyYmxkxPTy/061arVs0MCwsz09LSvOLn28A6evSoGR0dbUZFRZn79+/3+bzbb7/dlGTOnDnTE8vdwFq0aFGe5xw8eNCUZEZGRppZWVkF5pFbqVKlzNjYWL91FEVBDay9e/d6tv+WLVvyPL5//34zKirKlGSuXbu20Ot1vzf33HOPz8fbtGljSjKnTp3qiW3fvt00DMOsVq1anu3r1rt3b1OSuXjx4kLlcemll5qSzGPHjhVqeXfDduHChT4fnz9/vinJHDhw4AXn7W5gGYZhbt68Oc9z1q9fb0oy69atW6jcAQD4O+EeWAAAWFDu+zqVK1dOffr00e+//6569eppyZIlKl26tBwOh9auXStJXr9YmNuYMWMkSatWrfLEvv32W7lcLrVq1UqXXnppnue0aNFCzZo1O+/ce/To4bk0Lre+ffsqLi5OaWlp+umnn/I8vmXLFj333HO66667NHr0aI0cOVIjR46Uw+GQy+XS//73v/POKbdVq1YpPT1dV155pd9fJ3TfL+r777/P85jdbvd5aWGVKlV0ySWXKDMzU0ePHi1STu3atVNqaqqGDx+uH3/8US6Xq0jPLwr39m/ZsqXP7Vy9enVde+21krz3m8IaMWKEz/jw4cMlyeu+X0uWLJFpmurVq5fKli3r83n5bQtf2rVrJ0m6+eab9d1338nhcPhdNiUlRRs3blR0dLT69etX6PVfaN41a9ZU8+bN88SbNGkiSTpw4IDfnAEA+LviHlgAAFhQ7vs6RUREqFKlSrr88svVs2dP2e05w/fRo0eVkZEhKefm4L7Uq1dPkvcX4v379+f7HPdjP//883nlnt/r1q5dW0ePHvXkIEmnT5/WsGHD9Mknn+T7uu77f12oXbt2Scq5V5JhGPkue+TIkTyxqlWr+v1Vw5iYGB0/ftyzXQrr5ZdfVt++ffXuu+/q3XffVdmyZdW2bVt1795dw4YNU82aNYv0evlx7wv5bSdf+01h+Xtddzz3tndvizfffFNvvvlmvq/ra1v4Mn36dP38889aunSpli5dqujoaLVq1Updu3bVzTff7GkSSTn3azNNU+np6V73lSto/Reat7/tGRMTI0nKzMzM9zUBAPg7ooEFAIAF3XLLLX5nVV0MTNP0/P+ECRP0ySefqHHjxnryySfVtm1bVahQQREREZKkDh06aN26dV7PuRDu2U3169fXlVdeme+yuW987hYWVvwT2Js0aaJff/1Vy5Yt09dff63vv/9ea9as0ddff60pU6bozTff1NChQ4t9vcGQezu6t0WLFi18zkjKzX1j/IJUqVJFmzZt0jfffKMVK1Zo7dq12rBhg9auXatp06Zp+vTpevDBB73WX6ZMGQ0cOLDQNVxo3iWxDwEAcLGjgQUAQIiKi4tTZGSkMjMztWvXLp+Xg7lniuS+VM79/3v27PH72vk9VpDdu3cX+Lrx8fGe2Pz58yVJH374oc8afvvtt/POxZcaNWpIkho1aqQ5c+YU62tfCLvdrt69e6t3796ScmacPffcc5o8ebJuvfVWXX/99SpduvQFr8e9/d37hi++9pvC2r17t89fgvS17d3b4sorr9RLL71U5HX5YxiGunbt6rmMLyMjQ3PmzNEdd9yhhx56SIMGDVK9evU86zcMQ2+99VahG0sllTcAAPCPf/4BACBE2e12dezYUZL8NmLeeustSVK3bt08sc6dO8swDP3000/auXNnnuds2bLlvC8flKRly5bpzz//zBNfsmSJjh49qrJly6p169ae+LFjxyRJtWrVyvOcr776SikpKT7X456hld89jny56qqrFBERodWrV/vMsyScT64xMTGaNGmSypUrpzNnzigpKalY1tW5c2eFhYVp8+bN2rJlS57HDx48qC+//FKS935TWO+++26+cXdTSZJ69eolSVq0aFGRL7ssiqioKI0bN07NmjWTy+Xy7N/VqlVTs2bNdPLkSU/NhRGovAEAwFk0sAAACGH33XefJOmVV17RypUrvR6bM2eOFi1apPDwcN19992eeM2aNXX99dfL5XLptttu87q31PHjx3X77bdf0OV66enpuu2225Senu6JJScne3IdN26coqKiPI+570k0c+ZMr9f59ddfNW7cOL/rcc/k+eWXX4qUX+XKlXXXXXfp9OnT6tevn7Zu3ZpnmczMTC1atMhng+985JfrmTNn9Nxzz/m8V9KaNWt04sQJ2Ww2r5lLhVnX9u3bfT5es2ZNDR48WKZp6tZbb/W64fzp06c1duxYZWRkqEOHDurQoUOh1pnbK6+84nWjdkl6/vnntXHjRpUtW9bzwwKS1LJlSw0cOFD79u3TgAEDfM78O336tObOnavDhw8Xav3PPvus/vjjjzzxnTt3embz5W6WPvHEE5Jyfjhh8eLFeZ5nmqY2bNigZcuWlWjeAAAgf1xCCABACOvVq5ceeeQRPfHEE7rmmmt05ZVXqmbNmtq5c6d++ukn2Ww2vfrqq0pISPB63n//+19t2bJFq1evVp06ddS1a1eZpqlVq1YpLi5O/fv316JFi84rp+HDh+vzzz9X3bp11alTJ2VkZOjrr7/W6dOndcUVV2jy5Mley0+cOFGDBg3So48+qvnz5yshIUF//vmn1qxZo06dOqlatWo+f8ntH//4hyZPnqwXX3xR27ZtU40aNRQWFqb+/furf//++eb45JNP6uDBg5o3b57nPkZ169aV3W7X/v37tXnzZp0+fVpLly71eR+soho4cKBWrVqloUOHqkePHrrkkkskSffff78qV66s++67T/fff78uu+wyNWjQQOHh4dqzZ4/Wr18vSXr44YdVsWLFQq3r8ssvV7Vq1ZSYmKhWrVrpsssuU3h4uBo1aqT7779fUs7237lzpzZs2KB69eqpW7dustvt+uabb3TkyBHVqVNHc+fOPa9ab731VnXv3l2dOnVS9erVtW3bNm3dulU2m01vvfVWnl+onD17tk6cOKGlS5eqUaNGat68uerUqSPTNLVnzx5t2bJFWVlZ2rFjhypXrlzg+p944gndf//9aty4sZo0aaLo6GglJyd7fpFw+PDhatWqlWf5fv366YUXXtB9992n/v37q379+mrUqJFiY2N15MgRbdmyRX/++acefPBB9ejRo8TyBgAABTABAIBl1KpVy5Rkzp49u0jPW7p0qdm7d28zLi7OtNvtZpUqVczBgwebGzZs8PuclJQU86677jLj4+PNiIgIMz4+3hw3bpx55MgRc8SIEUXOY+LEiaYkc+LEieauXbvMm266yaxcubIZERFh1q9f33zsscfM06dP+3zut99+a1511VVmhQoVzFKlSplNmzY1p06damZmZppdunQxJZmrVq3K87xPPvnEvPLKK82yZcuahmF41u/mfj93797tc71LliwxBwwYYFavXt0MDw83y5UrZzZp0sS88cYbzXnz5nnlu3v3blOSWatWLb/vgb/1OZ1Oc/r06WZCQoIZFRVlSvLUlJ2dbb766qvmTTfdZDZu3NiMjY01o6OjzXr16pkDBw40V65c6Xd9/mzdutXs37+/WbFiRTMsLMyUZHbp0sVrmdOnT5vTp083W7RoYZYqVcqMiooymzRpYj700EPmsWPHirxOd02maZqvvPKK2aJFCzM6OtqMiYkxe/bsaa5du9bvc51Opzlv3jyzd+/eZuXKlc3w8HAzLi7ObNq0qTlq1Cjzk08+MbOysgqVx3vvvWeOGjXKbNq0qVm+fHkzMjLSrFWrltmrVy/zk08+MV0ul8/nbd261Rw7dqzZoEEDMyoqyixVqpRZt25d89prrzVffPFF88CBAxec96pVq3xuC3/vIwAAOMswzWL6SR8AAPC3NmnSJE2ePFkTJ07UpEmTgp0OAAAALiLcAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJbGPbAAAAAAAABgaczAAgAAAAAAgKXRwAIAAAAAAICl2YOdwPlwuVxKTk5W2bJlZRhGsNMBAAAAAABAPkzT1MmTJ1WtWjWFhRV9PlVINrCSk5NVo0aNYKcBAAAAAACAIti3b5/i4+OL/LyQbGCVLVtWUk7RMTExQc4GAAAAAAAA+UlLS1ONGjU8PZ2iCskGlvuywZiYGBpYAAAAAAAAIeJ8bwXFTdwBAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGkh+SuEAAAAAAAg8EzTlNPplMPhCHYqsAi73S6bzXbevy5Y6PWU6KsDAAAAAICQZ5qmTpw4oSNHjsjpdAY7HViMzWZTpUqVFBsbW2KNLBpYAAAAAAAgX4cOHdKJEycUExOjmJgY2e32Ep9xA+szTVMOh0NpaWk6ePCg0tPTVbVq1RJZFw0sAAAAAADgl9PpVGpqqipWrKgKFSoEOx1YUNmyZRUZGamUlBRVqlRJNput2NfBTdwBAAAAAIBf2dnZMk1TpUuXDnYqsLDSpUvLNE1lZ2eXyOvTwAIAAAAAAAXikkHkp6T3DxpYAAAAAAAAsDQaWAAAAAAAAPBp5MiRql27drDToIEFAAAAAAD+vubMmSPDMPz+Wb9+fbBTLND27ds1adIk7dmzJ9iplBh+hRAAAAAAAPztTZkyRXXq1MkTr1+/fhCyKZrt27dr8uTJ6tq1qyVmS5WEYmlgnTp1Ss8884w2bNigjRs36vjx45o9e7ZGjhzpWcblcumdd97Rxx9/rMTERB07dkx16tTRjTfeqH/961+KiooqjlQAAAAAAEAALdsW7AykHk0v/DV69eqlNm3aXPgLoUQUyyWEKSkpmjJlinbs2KHmzZv7XObMmTMaNWqUjhw5onHjxmnGjBlq166dJk6cqF69esk0zeJIBQAAAAAAoFhNnDhRYWFhWrlypVd87NixioiI0JYtWyRJq1evlmEY+vDDD/XQQw+pSpUqKl26tPr37699+/bled0NGzaoZ8+eio2NValSpdSlSxetXbs2z3IHDhzQmDFjVK1aNUVGRqpOnTq67bbblJWVpTlz5mjw4MGSpG7dunkufVy9erXn+UuXLlWnTp1UunRplS1bVn369NEvv/ySZz2ffvqpmjZtqqioKDVt2lSffPLJhbxtxapYZmBVrVpVBw8eVJUqVbRp0ya1bds2zzIRERFau3atOnTo4In93//9n2rXrq2JEydq5cqVuvrqq4sjHQAAAAAAgCJJTU1VSkqKV8wwDMXFxemRRx7R4sWLNWbMGG3dulVly5bVV199pTfeeEOPP/54nsk8U6dOlWEYevDBB/Xnn39qxowZuvrqq7V582ZFR0dLkr7++mv16tVLrVu39jTIZs+ere7du2vNmjVq166dJCk5OVnt2rXTiRMnNHbsWDVu3FgHDhzQwoULdebMGXXu3Fnjx4/Xiy++qIceekhNmjSRJM9/3333XY0YMULXXnutnnrqKZ05c0avvPKKOnbsqMTERM8lh8uWLdPAgQN16aWXavr06Tp69KhGjRql+Pj4knzbC61YGliRkZGqUqVKvstERER4Na/crr/+ek2cOFE7duyggQUAAAAAAILCV08iMjJSGRkZCg8P1zvvvKPWrVvr3nvv1TPPPKMxY8aoTZs2+ve//53neceOHdOOHTtUtmxZSVKrVq10ww036I033tD48eNlmqbGjRunbt26aenSpTIMQ5J06623KiEhQY888oiWLVsmSZowYYIOHTqkDRs2eF3iOGXKFJmmqXLlyqlTp0568cUXdc0116hr166eZU6dOqXx48frlltu0euvv+6JjxgxQo0aNdK0adM88QcffFCVK1fWd999p9jYWElSly5d1KNHD9WqVesC390LF/SbuB86dEiSVKFChSBnAgAAAAAA/q7++9//qmHDhl4xm83m+f+mTZtq8uTJmjBhgn7++WelpKRo2bJlstvztlaGDx/uaV5J0qBBg1S1alUtWbJE48eP1+bNm/Xbb7/pkUce0dGjR72ee9VVV+ndd9+Vy+WSlHNZX79+/Xzen8vd+PJn+fLlOnHihG666Sav2WU2m03t27fXqlWrJEkHDx7U5s2b9e9//9vTvJKka665RpdeeqlOnz6d73oCIegNrKeffloxMTHq1auX32UyMzOVmZnp+XtaWpokyeFwyOFwSJLCwsIUFhYml8vl2ci5406n0+s+W/7iNptNhmF4Xjd3XJKcTmeh4na7XaZpesUNw5DNZsuTo784NVETNVETNVETNVETNVETNVETNVFTsGtyOBye1/N9/2pDUnDj53tbbcMwPDW1bdvW0yTKHc9d8/33368PPvhAGzdu1NSpU9WkSROZpulZ3r1s/fr1veLu2J49e2Sapn777TdJOTOh/Dlx4oSysrKUlpamhISEfO8dfm6u7v8mJSVJkrp37+7zeTExMZKkPXv2eOWd+z1o1KiRfvrppzxxf3nk7tXk3vfO3f+KKqgNrGnTpmnFihV6+eWXVa5cOb/LTZ8+XZMnT84TT0xMVOnSpSVJFStWVL169bR7924dOXLEs0x8fLzi4+OVlJSk1NRUT7xu3bqqVKmStm3bpvT0dE+8cePGKleunBITE70O4mbNmikiIkKbNm3yyqFNmzbKysrSzz//7InZbDa1bdtWqamp2rlzpyceHR2t5s2bKyUlRbt27fLEY2Nj1eSHH5QcHq794eGeeEWHQ/WysrQ7IkJHcnV047OzFZ+draTISKXm6gbXzcpSJYdD26KilB529v78jTMyVM7lUmJ0tJy5urPN0tMVYZraVKqUd03/+Efx1NSkiZKTk7V///6zNYX6dqImaqImaqImaqImaqImaqImavob1hQVFSUpp6mVkZHhiYeFhUkqJafT6dWgCAsLU3h4RJ64zWaT3R4uh8PhlYvdbpfNZld2drZXs84dz8rK8mqahIeHKyzM5omfPu3wvMdhYWF5ZgyVLl1aLpfL630xDMMTl6T09HSdPn1aYWFhKlWqlBwOh9dkGpvNpv3793uaT5s3b9bp06dlt9sVFRWlzMxMz3uTmZmp7OxsRUREKCMjQ06nU06nUy6XSw6Hw7POJ554Qs2aNZOUc+slm82mjIwMT/PrzJkznvXnV5M7T/f63dvJ/fdZs2apVq1acjgcys7O9rxGRESEJHm2UWZmZp6a3A3M06dPKyIiwqsmt8jISElSdna2tm07+7OUufc992Sk82WYxfzzf+6buM+ePVsjR470u9yHH36om266SaNHj9asWbPyfU1fM7Bq1Kiho0ePerqFVulMuxW52z53rlySXLleI+yvP/7iTnn3oP3FbcrpS5/b63S3vpznxocNK56aLPwvCNRETdRETdRETdRETdRETdRETdRUuJoyMjL0xx9/qG7dup5GRW7Lfwn+DKxrEnw8XAiGYWj27NkaPXq0Nm7c6HMGlpvL5VLnzp21a9cujRo1StOnT9fChQs1YMAAz/KrV69W9+7d9e9//1vTpk3zmpkVHx+vZs2aaenSpdq0aZPatWunV199VWPHjvXKJ/d6XS6Xypcvr27duuX7i4AfffSRBg8erK+//lrdunXzvMaCBQs0ZMgQffnll7r22mt9zpwyDEPJycmqXr26HnzwQU2fPt0rl6ZNm+r06dPavXu33/dGyund7Nq1SzVr1vQ0PHPve2lpaYqLi1Nqaqqnl1MUQZmBtXz5cg0fPlx9+vTRq6++WuDykZGRPg8Su92e51pT9wF7LvcBWNi4r2tYixo3DMNn3F+O7gZUYeO+M/cf97ex88T/mqVVLDUVMR4S24maqMlPjkWNUxM1SdTkL8eixqmJmiRq8pdjUePURE0SNfnLsajxi6Umu90u46/vie7/5hXcuN+0CiF3bbnrO7fW559/Xt9//70WLVqkPn366JtvvtHtt9+uLl26qEKFCl7Pf/fdd/XQQw+pbNmyMgxDCxcu1MGDB/Xggw/KMAy1bt1a9erV03/+8x/dfPPNKlOmjNd6jxw5oooVK8pms+kf//iH3nvvPf3444957oPlnqnlfr57Rp47j549eyomJkbTp09X9+7dFZ7rqi9JnvVUq1ZNLVq00DvvvKMJEyZ47oO1YsUKbd++XbVq1cr3vckd99Wr8RUrqoA3sDZs2KDrr79ebdq00fz58y+4AAAAAAAAgAu1dOlSr0s+3Tp06KDMzEw9+uijGjlypPr16ydJmjNnjlq0aKHbb79d8+fP93pO+fLl1bFjR40aNUqHDx/WjBkzVL9+ff3f//2fpJym5KxZs9SrVy8lJCRo1KhRql69ug4cOKBVq1YpJiZGixcvlpRz+6Vly5apS5cuGjt2rJo0aaKDBw9qwYIF+u6771SuXDm1aNFCNptNTz31lFJTUxUZGanu3burUqVKeuWVVzRs2DC1atVKN954oypWrKg//vhDX3zxha688kq99NJLknJu39SnTx917NhRo0eP1rFjxzRz5kwlJCTo1KlTJfnWF0pAu0c7duxQnz59VLt2bX3++eeKjo4O5OoBAAAAAAB8euyxx3zGZ82apddee00VKlTQjBkzPPEGDRpo+vTpuvvuuzV//nzdcMMNnsceeugh/fzzz5o+fbpOnjypq666Si+//LJK5boHddeuXbVu3To9/vjjeumll3Tq1ClVqVJF7du316233upZrnr16tqwYYMeffRRzZ07V2lpaapevbp69erleb0qVaro1Vdf1fTp0zVmzBg5nU6tWrVKlSpV0j//+U9Vq1ZNTz75pJ555hllZmaqevXq6tSpk0aNGuVZT8+ePbVgwQI98sgjmjBhgurVq6fZs2frs88+0+rVq4vpXT5/xXYPrJdeekknTpxQcnKyXnnlFQ0YMEAtW7aUJN11110KCwtTQkKCDhw4oGnTpql69epez69Xr56uuOKKQq0rLS1NsbGx533dpCW9806wMzhr+PBgZwAAAAAAsIiMjAzt3r1bderU8dzbCL6tXr1a3bp104IFCzRo0KBgpxNQBe0nF9rLKbYZWM8++6z27t3r+fvHH3+sjz/+WJI0dOhQSdK+ffskSf/+97/zPH/EiBGFbmABAAAAAADg76PYGlh79uwpcJli/sFDAAAAAAAA/A34+nE7AAAAAAAAwDL4CUAAAAAAAIBi0LVrV64+KyHMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAH9bc+bMkWEYioqK0oEDB/I83rVrVzVt2jQImSE3e7ATAAAAAAAAIezLL4OdgdSz5wW/RGZmpp588knNnDmzGBJCcWMGFgAAAAAA+Ntr0aKF3njjDSUnJwc7FfhAAwsAAAAAAPztPfTQQ3I6nXryySfzXc7hcOjxxx9XvXr1FBkZqdq1a+uhhx5SZmamZ5l7771XcXFxMk3TE7vrrrtkGIZefPFFT+zw4cMyDEOvvPJK8Rd0kaGBBQAAAAAA/vbq1Kmj4cOHFzgL65ZbbtFjjz2mVq1a6fnnn1eXLl00ffp03XjjjZ5lOnXqpGPHjumXX37xxNasWaOwsDCtWbPGKyZJnTt3LoGKLi40sAAAAAAAACQ9/PDDcjgceuqpp3w+vmXLFr399tu65ZZbtGDBAt1+++16++239a9//UuffvqpVq1aJUnq2LGjpLMNqtTUVG3dulUDBw7M08AqX768Lr300hKuLPTRwAIAAAAAAJBUt25dDRs2TK+//roOHjyY5/ElS5ZIyrlEMLf77rtPkvTFF19IkipWrKjGjRvr22+/lSStXbtWNptN999/vw4fPqzffvtNUk4Dq2PHjjIMo8RquljQwAIAAAAAAPjLI488IofD4fNeWHv37lVYWJjq16/vFa9SpYrKlSunvXv3emKdOnXyzLZas2aN2rRpozZt2qh8+fJas2aN0tLStGXLFnXq1KlkC7pI0MACAAAAAAD4S926dTV06FC/s7AkFWrGVMeOHXXgwAHt2rVLa9asUadOnWQYhjp27Kg1a9bo+++/l8vlooFVSDSwAAAAAAAAcnHPwjr3Xli1atWSy+XyXALodvjwYZ04cUK1atXyxNyNqeXLl+uHH37w/L1z585as2aN1qxZo9KlS6t169YlXM3FgQYWAAAAAABALvXq1dPQoUP12muv6dChQ5547969JUkzZszwWv65556TJPXp08cTq1OnjqpXr67nn39e2dnZuvLKKyXlNLZ+//13LVy4UJdffrnsdnsJV3NxoIEFAAAAAABwjocffljZ2dn69ddfPbHmzZtrxIgRev311zVkyBC9/PLLGjlypJ5++mn94x//ULdu3bxeo1OnTvr111/VtGlTXXLJJZKkVq1aqXTp0kpKSuLywSKggQUAAAAAAHCO+vXra+jQoXnis2bN0uTJk/XDDz/onnvu0ddff60JEybogw8+yLOsu0HVsWNHT8xut+uKK67wehwFM0zTNIOdRFGlpaUpNjZWqampiomJCXY6xeOdd4KdwVnDhwc7AwAAAACARWRkZGj37t2qU6eOoqKigp0OLKqg/eRCeznMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAKCGGYWjSpEnBTiPk0cACAAAAAAB/S4ZhFOrP6tWrg53q35492AkAAAAAAIAQ9r//BTsDqX7983rau+++6/X3d955R8uXL88Tb9KkyXmnhuJBAwsAAAAAAPwtDR061Ovv69ev1/Lly/PEEXxcQggAAAAAAODH6dOndd9996lGjRqKjIxUo0aN9Oyzz8o0Ta/lMjMz9f/+3/9TxYoVVbZsWfXv31/79+/P83p79+7V7bffrkaNGik6OlpxcXEaPHiw9uzZ41lm165dMgxDzz//fJ7nf//99zIMQ++//36x12plNLAAAAAAAAB8ME1T/fv31/PPP6+ePXvqueeeU6NGjXT//ffr3nvv9Vr2lltu0YwZM9SjRw89+eSTCg8PV58+ffK85g8//KDvv/9eN954o1588UWNGzdOK1euVNeuXXXmzBlJUt26dXXllVdq7ty5eZ4/d+5clS1bVtddd13JFG1RXEIIAAAAAADgw6JFi/T111/riSee0MMPPyxJuuOOOzR48GC98MILuvPOO1WvXj1t2bJF7733nm6//Xb997//9Sx388036+eff/Z6zT59+mjQoEFesX79+umKK67QRx99pGHDhkmShg8frltvvVU7d+5U48aNJUnZ2dmaP3++BgwYoFKlSpV0+ZbCDCwAAAAAAAAflixZIpvNpvHjx3vF77vvPpmmqaVLl3qWk5RnuXvuuSfPa0ZHR3v+Pzs7W0ePHlX9+vVVrlw5/fTTT57HbrjhBkVFRXnNwvrqq6+UkpLyt7xHFw0sAAAAAAAAH/bu3atq1aqpbNmyXnH3rxLu3bvX89+wsDDVq1fPa7lGjRrlec309HQ99thjnntqVahQQRUrVtSJEyeUmprqWa5cuXLq16+f5s2b54nNnTtX1atXV/fu3YutxlBBAwsAAAAAACBA7rrrLk2dOlU33HCD5s+fr2XLlmn58uWKi4uTy+XyWnb48OHatWuXvv/+e508eVKLFi3STTfdpLCwv187h3tgAQAAAAAA+FCrVi2tWLFCJ0+e9JqFtXPnTs/j7v+6XC79/vvvXrOufv311zyvuXDhQo0YMUL/+c9/PLGMjAydOHEiz7I9e/ZUxYoVNXfuXLVv315nzpzx3CPr7+bv17IDAAAAAAAohN69e8vpdOqll17yij///PMyDEO9evWSJM9/X3zxRa/lZsyYkec1bTabTNP0is2cOVNOpzPPsna7XTfddJPmz5+vOXPm6LLLLlOzZs0upKSQxQwsAAAAAAAAH/r166du3brp4Ycf1p49e9S8eXMtW7ZMn332me655x7PPa9atGihm266SS+//LJSU1PVoUMHrVy5Uv/73//yvGbfvn317rvvKjY2VpdeeqnWrVunFStWKC4uzmcOw4cP14svvqhVq1bpqaeeKtF6rYwGFgAAAAAAgA9hYWFatGiRHnvsMX344YeaPXu2ateurWeeeUb33Xef17JvvfWW53K/Tz/9VN27d9cXX3yhGjVqeC33wgsvyGazae7cucrIyNCVV16pFStW6Nprr/WZQ+vWrZWQkKAdO3bo5ptvLrFarc4wz523FgLS0tIUGxur1NRUxcTEBDud4vHOO8HO4Kzhw4OdAQAAAADAIjIyMrR7927VqVNHUVFRwU7nb6lly5YqX768Vq5cGexU/CpoP7nQXg73wAIAAAAAALCoTZs2afPmzRr+N59swiWEAAAAAAAAFrNt2zb9+OOP+s9//qOqVatqyJAhwU4pqJiBBQAAAAAAYDELFy7UqFGjlJ2drffff/9vf/kmDSwAAAAAAACLmTRpklwul3bs2KEuXboEO52go4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAApkmmawU4CFlfT+QQMLAAAAAAD4ZbPZJEnZ2dlBzgRW5t4/3PtLcaOBBQAAAAAA/AoPD1dkZKRSU1OZhQWfTNNUamqqIiMjFR4eXiLrsJfIqwIAAAAAgItGhQoVdODAAe3fv1+xsbEKDw+XYRjBTgtBZpqmsrOzlZqaqlOnTql69eolti4aWAAAAAAAIF8xMTGSpJSUFB04cCDI2cBqIiMjVb16dc9+UhJoYAEAAAAAgALFxMQoJiZG2dnZcjqdwU4HFmGz2UrsssHcaGABAAAAAIBCCw8PD0jDAsitWG7ifurUKU2cOFE9e/ZU+fLlZRiG5syZ43PZHTt2qGfPnipTpozKly+vYcOG6ciRI8WRBgAAAAAAAC5CxTIDKyUlRVOmTFHNmjXVvHlzrV692udy+/fvV+fOnRUbG6tp06bp1KlTevbZZ7V161Zt3LhRERERxZEOAAAAAAAALiLF0sCqWrWqDh48qCpVqmjTpk1q27atz+WmTZum06dP68cff1TNmjUlSe3atdM111yjOXPmaOzYscWRDgAAAAAAAC4ixXIJYWRkpKpUqVLgch999JH69u3raV5J0tVXX62GDRtq/vz5xZEKAAAAAAAALjLF0sAqjAMHDujPP/9UmzZt8jzWrl07JSYmBioVAAAAAAAAhJCA/QrhwYMHJeVcbniuqlWr6tixY8rMzFRkZGSexzMzM5WZmen5e1pamiTJ4XDI4XBIksLCwhQWFiaXyyWXy+VZ1h13Op0yTbPAuM1mk2EYntfNHZeU56dC/cXtdrtM0/SKG4Yhm82WJ0fDMGST5PrrjyfHv/74izslmYWI2yQZkrwryonrr+W94n+9Hxdck494yG8naqImaqImaqImaqImaqImaqImaqImaipyTefWVVQBa2Clp6dLks8GVVRUlGcZX49Pnz5dkydPzhNPTExU6dKlJUkVK1ZUvXr1tHv3bq9fNYyPj1d8fLySkpKUmprqidetW1eVKlXStm3bPLlJUuPGjVWuXDklJiZ6bexmzZopIiJCmzZt8sqhTZs2ysrK0s8//+yJ2Ww2tW3bVqmpqdq5c6cnHh0drebNmyslJUW7du3yxGNjY9VEUnJ4uPbn+inSig6H6mVlaXdEhI7Yz26q+OxsxWdnKykyUqk2mydeNytLlRwObYuKUnrY2cl1jTMyVM7lUmJ0tJyGcbam9HRFmKY2lSrlXZPTWTw1NWmi5ORk7d+//2xNob6dqImaqImaqImaqImaqImaqImaqImaqKnINbknI50vw8zdGisG7pu4z549WyNHjswTf+eddzRs2DCv5zzwwAN65plnlJGRUegZWDVq1NDRo0cVExMj6SLoeM6da50ZWH9tn1Dp4nrlfpF0pqmJmqiJmqiJmqiJmqiJmqiJmqiJmi6mmtLS0hQXF6fU1FRPL6coAjYDy33poPtSwtwOHjyo8uXL+2xeSTmztnw9ZrfbZbd7l+B+087l3rCFjZ/7uucTNwzDZ9xfju4GVGHjvjP3H/e3sfPE/5qlVSw1FTEeEtuJmqjJT45FjVMTNUnU5C/HosapiZokavKXY1Hj1ERNEjX5y7GocWqiJoma3Dn6y7+wAnYT9+rVq6tixYp5prxJ0saNG9WiRYtApQIAAAAAAIAQErAGliQNHDhQn3/+ufbt2+eJrVy5UklJSRo8eHAgUwEAAAAAAECIKLZLCF966SWdOHFCycnJkqTFixd7bgB21113KTY2Vg899JAWLFigbt266e6779apU6f0zDPP6LLLLtOoUaOKKxUAAAAAAABcRIrtJu61a9fW3r17fT62e/du1a5dW5L0yy+/6N5779V3332niIgI9enTR//5z39UuXLlQq8rLS1NsbGx533jL0t6551gZ3DW8OHBzgAAAAAAAFxELrSXU2wzsPbs2VOo5RISEvTVV18V12oBAAAAAABwkQvoPbAAAAAAAACAoqKBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEsLeAPrt99+04033qj4+HiVKlVKjRs31pQpU3TmzJlApwIAAAAAAIAQYA/kyvbt26d27dopNjZWd955p8qXL69169Zp4sSJ+vHHH/XZZ58FMh0AAAAAAACEgIA2sN59912dOHFC3333nRISEiRJY8eOlcvl0jvvvKPjx4/rkksuCWRKAAAAAAAAsLiAXkKYlpYmSapcubJXvGrVqgoLC1NEREQg0wEAAAAAAEAICGgDq2vXrpKkMWPGaPPmzdq3b58+/PBDvfLKKxo/frxKly4dyHQAAAAAAAAQAgJ6CWHPnj31+OOPa9q0aVq0aJEn/vDDD+uJJ57w+7zMzExlZmZ6/u6eyeVwOORwOCRJYWFhCgsLk8vlksvl8izrjjudTpmmWWDcZrPJMAzP6+aOS5LT6SxU3G63yzRNr7hhGLLZbHlyNAxDNkmuv/54cvzrj7+4U5JZiLhNkiHJu6KcuP5a3iv+1/txwTX5iIf8dqImaqImaqImaqImaqImaqImaqImaqKmItd0bl1FFdAGliTVrl1bnTt31sCBAxUXF6cvvvhC06ZNU5UqVXTnnXf6fM706dM1efLkPPHExETPrK2KFSuqXr162r17t44cOeJZJj4+XvHx8UpKSlJqaqonXrduXVWqVEnbtm1Tenq6J964cWOVK1dOiYmJXhu7WbNmioiI0KZNm7xyaNOmjbKysvTzzz97YjabTW3btlVqaqp27tzpiUdHR6t58+ZKSUnRrl27PPHY2Fg1kZQcHq794eGeeEWHQ/WysrQ7IkJH7Gc3VXx2tuKzs5UUGalUm80Tr5uVpUoOh7ZFRSk97OzkusYZGSrncikxOlpOwzhbU3q6IkxTm0qV8q7J6Syempo0UXJysvbv33+2plDfTtRETdRETdRETdRETdRETdRETdRETdRU5Jrck5HOl2Hmbo2VsA8++ECjR49WUlKS4uPjPfFRo0Zp/vz5+uOPPxQXF5fneb5mYNWoUUNHjx5VTEyMpIug4zl3rnVmYA0bVjw10ZmmJmqiJmqiJmqiJmqiJmqiJmqiJmqiJodDaWlpiouLU2pqqqeXUxQBbWB17txZTqdTa9eu9Yp/8sknGjBggJYvX66rr766wNdJS0tTbGzseRdtSe+8E+wMzho+PNgZAAAAAACAi8iF9nICehP3w4cP5+kMSlJ2drYkXfD1kAAAAAAAALj4BLSB1bBhQyUmJiopKckr/v777yssLEzNmjULZDoAAAAAAAAIAQG9ifv999+vpUuXqlOnTrrzzjsVFxenzz//XEuXLtUtt9yiatWqBTIdAAAAAAAAhICANrA6d+6s77//XpMmTdLLL7+so0ePqk6dOpo6daoeeOCBQKYCAAAAAACAEBHQBpYktWvXTkuWLAn0agEAAAAAABCiAnoPLAAAAAAAAKCoaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNLswU4AAAAAQMGWbQt2Bmf1aBrsDAAAfzc0sAAAAAAUOxpuAIDixCWEAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDR7sBMAAAAAgmXZtmBncFaPpsHO4O+L/QAArC8oM7B++ukn9e/fX+XLl1epUqXUtGlTvfjii8FIBQAAAAAAABYX8BlYy5YtU79+/dSyZUs9+uijKlOmjH7//Xft378/0KkAAAAAAAAgBAS0gZWWlqbhw4erT58+WrhwocLCuAUXAAAAAAAA8hfQDtK8efN0+PBhTZ06VWFhYTp9+rRcLlcgUwAAAAAAAECICWgDa8WKFYqJidGBAwfUqFEjlSlTRjExMbrtttuUkZERyFQAAAAAAAAQIgJ6CeFvv/0mh8Oh6667TmPGjNH06dO1evVqzZw5UydOnND777/v83mZmZnKzMz0/D0tLU2S5HA45HA4JElhYWEKCwuTy+XymtXljjudTpmmWWDcZrPJMAzP6+aOS5LT6SxU3G63yzRNr7hhGLLZbHlyNAxDNkmuv/54cvzrj7+4U5JZiLhNkiHJu6KcuP5a3iv+1/txwTX5iIf8dqImaqImaqImaqKmi6omM/eHLOOvT0fmOZ+O/MSNsJyavOOGjDCbTNOlc17cd9wIk2GEyTRdcjjyr8l05Vredc4nPiOnJtN1zie+EqrJ4Sh4O/mtNU/ugakpv33vbJoFb6eSrin3oRZqx1NuF8s5gpqoiZqKr6Zz6yqqgDawTp06pTNnzmjcuHGeXx0cMGCAsrKy9Nprr2nKlClq0KBBnudNnz5dkydPzhNPTExU6dKlJUkVK1ZUvXr1tHv3bh05csSzTHx8vOLj45WUlKTU1FRPvG7duqpUqZK2bdum9PR0T7xx48YqV66cEhMTvTZ2s2bNFBERoU2bNnnl0KZNG2VlZennn3/2xGw2m9q2bavU1FTt3LnTE4+Ojlbz5s2VkpKiXbt2eeKxsbFqIik5PFz7w8M98YoOh+plZWl3RISO2M9uqvjsbMVnZyspMlKpNpsnXjcrS5UcDm2LilJ6rvuLNc7IUDmXS4nR0XIaxtma0tMVYZraVKqUd01OZ/HU1KSJkpOTvW7QH/LbiZqoiZqoiZqoiZouqpqyTpytKbxCMxm2CGUd9q4ponIbmc4sZaecrckwbIqo0lZmVqqyj52tybBHK6Jic7nSU+RIPVtTWGSswss3kfNUspynztZki64oe7l6cqbu1qZN+deUdVKyx9aVrVQlZR/dJtNxtqbw8o1lRJZT9p+JMs2Sr2nTmYK3kzN1t5zpZ2uylYmXvWy8HCeS5Mo8u50CUVNB+17WycJvp5KuadOZszWF2vF0MZ4jqImaqKn4anJPRjpfhpm7NVbCmjZtql9++UXffPONOnfu7Il/++236tKli95++20NHz48z/N8zcCqUaOGjh49qpiYGEkXQcdz7lzrzMAaNqx4aqIzTU3URE3URE3URE0Wr2nl9lxJBnkG1lVN8q9p5fZcywd5BtZVlxa8nb7aap0ZWNck5L/vnd0Pgj8D66pLz4ZD7XjK7WI5R1ATNVFT8dWUlpamuLg4paameno5RRHQGVjVqlXTL7/8osqVK3vFK1WqJEk6fvy4z+dFRkYqMjIyT9xut8tu9y7B/aady71hCxs/93XPJ24Yhs+4vxzdDajCxn1n7j/ub2Pnif81S6tYaipiPCS2EzVRk58cixqnJmqSqMlfjkWNUxM1SedXk+HrQ5bh51OTj7hhGH7iYfL14vnF7fb8a8r9NCPMd01GWOFz9xcvTE25N6O/7eG3Vr+5l2xN+e1756ZZ5O1XjDX5OqRC5Xi60Dg1UZNETf5yLGrcijX5y7+wAnoT99atW0uSDhw44BVPTk6WlDNFDQAAAAAAAMgtoA2sG264QZL05ptvesVnzZolu92url27BjIdAAAAAAAAhICAXkLYsmVLjR49Wm+99ZYcDoe6dOmi1atXa8GCBZowYYKqVasWyHQAAAAAAAAQAgLawJKkV199VTVr1tTs2bP1ySefqFatWnr++ed1zz33BDoVAAAAAAAAhICAN7DCw8M1ceJETZw4MdCrBgAAAAAAQAgK6D2wAAAAAAAAgKKigQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEsL+E3cAQAAAADnb9m2YGdwVo+mwc4AwN8FM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBp9mAnAAAAgIvHsm3BzuCsHk2DnQEAACguzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXxK4QAAAAAgBLBL5MCKC7MwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXZg50AAAAAAABWsGxbsDM4q0fTYGcAWAszsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBp3MQdAAAAAIAQww3n8XfDDCwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBq/QggAAAAAAEoUv5qIC8UMLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYmj3YCQAAACB/y7YFO4OzejQNdgYAAODviAYWAAAAAADAX/iHI2viEkIAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBq/QmgRv6cEO4Oz6gU7AQAAAAAAgFyYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEsLegNr6tSpMgxDTZs2DXYqAAAAAAAAsKCgNrD279+vadOmqXTp0sFMAwAAAAAAABZmD+bK//Wvf+nyyy+X0+lUSkpKMFMBAAAAAACARQVtBta3336rhQsXasaMGcFKAQAAAAAAACEgKA0sp9Opu+66S7fccosuu+yyYKQAAAAAAACAEBGUSwhfffVV7d27VytWrCjU8pmZmcrMzPT8PS0tTZLkcDjkcDgkSWFhYQoLC5PL5ZLL5fIs6447nU6Zpllg3GazyTAMz+vmjks5zbfCxO12u0zT9IobhiGbzZYnR8MwJEmmJNPI9SJmTofRJUm54oaZ81dX7mXPM65z1yl53o8LrclXPNS3EzVREzVREzVRUzBqMv/6MGCE2WSaLnfAXZXvuBEmwwjzH3c5lfPpo6B4Tk2mK6cmd2n+cjdN21//4x03wnJq8o6XbE0uV8HbyXu1vnP3Fy/umhyO/Pc90+W/1nO3U0nX5HAUfDwV9753oTXld444m2Zgjydfuec+ffg7zqTAH0/+4qaZ/3kvZ3nftXqFA3COKMy5POc4C+zx5C/ucOQ/PknBO57OrUkqeMz1lBvA48lfPPfu6utzhOmyxpgr5ewHF8tno3PPE0UV8AbW0aNH9dhjj+nRRx9VxYoVC/Wc6dOna/LkyXniiYmJnhvAV6xYUfXq1dPu3bt15MgRzzLx8fGKj49XUlKSUlNTPfG6deuqUqVK2rZtm9LT0z3xxo0bq1y5ckpMTPTa2M2aNVNERIQ2bdrklUObNm2UlZWln3/+2ROz2Wxq27atUlNTtXPnTk88OjpazZs3V0pKinbt2uWJx8bGKkJSaplwpZYJ98TLpDsUl5ql47EROhV9dlPFnspWuVPZOlIuUhmRNk+8fGqWyqY7dCguStn2s5PrKh3LUHSWS/srRcs0znarqqaky+40ta9yKa+a6jidxVJTkyZNlJycrP3793viob6dqImaqImaqImaglFT1knJsEcromJzudJT5Eg9W1NYZKzCyzeR81SynKfO1mSLrih7uXpypu6WM/1sTbYy8bKXjZfjRJJcmWdrssfWla1UJWUf3SbTcbam8PKNZUSWU/afiTJNpzadyb8mlWoj05ml7JSzNRmGTRFV2srMSlX2sbPbqaRrSqlS8HbKOnF2O4VXaCbDFqGsw941RVQOTE2bNuW/72WdLPx2KumaNp0p+Hgq7n3vQmoq6ByRdbLw26mka3IfY5L/c4SiA388+asptWb+571gHU++airMuTzrZOCPJ381bTqT//gkBed48lWTVPCY6z7OAnk8+avJfZz5+xyRnW6NMVfK2Q8uls9G7slI58swc7fGAuC2227TihUr9MsvvygiIkKS1LVrV6WkpGjbtm0+n+NrBlaNGjV09OhRxcTESLL+v5xK+Xc897ww1zIzsOrfM6xYagrFf+GmJmqiJmqiJmqyYk0rt0tWmYF11aX5575yh3VmYF3TtODtlPPenq3VV+6BmjFyVZP8972V2/3XGugZI1ddWvDx9NVW68zAuiYh/3PE2f0g+DOw3MeY5P84+3qndWZg9bgs//Pesq3WmYF1VZOCz+U5x5k1ZmBddWn+49OK7daZgXVts4LHXM9xZoEZWLmPM1+fI1Zut8aYK+XsBxfLZ6O0tDTFxcUpNTXV08spioDOwPrtt9/0+uuva8aMGUpOTvbEMzIylJ2drT179igmJkbly5f3el5kZKQiIyPzvJ7dbpfd7l2C+007l3vDFjZ+7uueT9wwDJ9xfzkaOttU8lpe8tqnPXE/rceixs9dp/uSxuKoqajxUNhO1ERN/nIsapyaqEmiJn85FjV+sddkhOWOh3kHzjce5jt3/3H7X7nmn7tnsrfhuybf8ZKpyb0p89tOPl7GZ47+4sVZk92e/77ntR8UsJ3yPlC8NeXe7H4/2xbzvpf3gaLVlN854tw0A3U85X3AnucYk/yfIwJ5PPmLu495f+e3omy/kq6pMOdy7+MsMMeTv3ihjrMgHU++4gWNrYU+zgJQ07m767nnCHdawR5zJe/9INQ/G/nLv7ACehP3AwcOyOVyafz48apTp47nz4YNG5SUlKQ6depoypQpgUwJAAAAAAAAFhfQGVhNmzbVJ598kif+yCOP6OTJk3rhhRdUr169QKYEAAAAAAAAiwtoA6tChQr6xz/+kSc+Y8YMSfL5GAAAAAAAAP7eAnoJIQAAAAAAAFBUAZ2B5c/q1auDnQIAAAAAAAAsihlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNEvcAwuhZdm2YGdwVo+mwc4AAAAAAACUNGZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0rgHFgAA+Nvhfo4AAAChhRlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDR7sBMAStqybcHO4KweTYOdAQAAAAAAoYcZWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNH6FEAAAFAt+9RUAAAAlhRlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNHuwEwBw1rJtwc7grB5Ng50BAAAAAAA5mIEFAAAAAAAAS2MGFgAAFsWsTAAAACAHM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaQFtYP3www+68847lZCQoNKlS6tmzZq64YYblJSUFMg0AAAAAAAAEELsgVzZU089pbVr12rw4MFq1qyZDh06pJdeekmtWrXS+vXr1bRp00CmAwAAAAAAgBAQ0AbWvffeq3nz5ikiIsITGzJkiC677DI9+eSTeu+99wKZDgAAAAAAAEJAQBtYHTp0yBNr0KCBEhIStGPHjkCmAgAAAAAAgBAR9Ju4m6apw4cPq0KFCsFOBQAAAAAAABYU0BlYvsydO1cHDhzQlClT/C6TmZmpzMxMz9/T0tIkSQ6HQw6HQ5IUFhamsLAwuVwuuVwuz7LuuNPplGmaBcZtNpsMw/C8bu64JDmdzkLF7Xa7TNP0ihuGIZvNlidHwzAkSaYk08j1ImZOh9ElSbnihpnzV1fuZc8zrnPXKXneD381ma7ccUNGmE2m6ZJMV8FxI0yGEeY/7nL+9U4UFC/8djJdOcvn/MW7JiMspybveMnV5HDkv+9JhkyXd03+ci/pmqTQPZ58xUP9HEFNf9OaXHnPe8E6RzgcBddkmud3Li+JmpzO/LdTSY9PRanJNAve98y/PgwEc8x11+Q+rPwdN6ZpjTFXklyugs8R3qsNzpjrrsnXcZY795zPNIE/nnzl7nAUfN4LxvGUX035ncvPphnY48lX7rmHLn/HmRT448lf3DTzH3O9vzsoYMeTr3hhPke4vzsEc8zNfZzl9zlCssaYm/Nts+DPRp5ygzjmuuO5d1dfn/dMlzXGXClnPwi5z7B+xtxzzxNFFdQG1s6dO3XHHXfoiiuu0IgRI/wuN336dE2ePDlPPDExUaVLl5YkVaxYUfXq1dPu3bt15MgRzzLx8fGKj49XUlKSUlNTPfG6deuqUqVK2rZtm9LT0z3xxo0bq1y5ckpMTPTa2M2aNVNERIQ2bdrklUObNm2UlZWln3/+2ROz2Wxq27atUlNTtXPnTk88OjpazZs3V0pKinbt2uWJx8bGKkJSaplwpZYJ98TLpDsUl5ql47EROhV9dlPFnspWuVPZOlIuUhmRNk+8fGqWyqY7dCguStn2s5PrKh3LUHSWS/srRcs0znarqqaky+40ta9yKa+a6jid+daUdfhsTYY9WhEVm8uVniJH6tmawiJjFV6+iZynkuU8tf/s60RXlL1cPTlTd8uZfnY72crEy142Xo4TSXJlnt1O9ti6spWqpOyj22Q6zm6n8PKNZUQWbjtlnZQiKreR6cxSdsrZmgzDpogqbWVmpSr7WGBq2nQm/31PKqfsPxNl5jrZhldoJsMWoazD3vteSdckhe7x1KRJEyUnJ2v//rM1hfo5gpr+njVl/Zn3vBesc8SmTQXX5DTP71xeEjVtM/PfTiU9PhWlpvT0gve9rJPBH3PdNW06kxP3dzyplDXGXElKqVLwOSLrRPDHXHdNmzblf47IOhmc48lXTZvOFHzeC8bx5K+mgs7lWScLv51Kuib3MSb5H58UHfjjyV9NqTXzH3ODdTz5qqkwnyOyTgZ/zHXXtOlM/p8jJGuMuYY9WlLBn43cx1kwx1x3Te7jzN/nvex0a4y5Us5+EGqfYf2Nue7JSOfLMHO3xgLo0KFDuvLKK5Wdna3169erWrVqfpf1NQOrRo0aOnr0qGJiYiSF/r/a73lhrmVmYNW/Z1i+NS3bGvx/6XF3prs3Lng7rdyuoP5LT+7cr7o0/31v+S/B/5ced+7XXha6xxMze6gpv5qWbVPQZlf4Os7yq2nFL9aZgXVVk4K308od1pmBdXVC/vveV1utMwOrR9OCj6eV26Vgj7numq66NCfs71ywcoc1xlxJuqZpweeInPf2bK2+cg/UOcLXcZY795zPNNaYgXXVpQWfy/0eZ0E4R1yTkP/4dHY/CP4MLPcxJvk/zr7eaZ0ZWD0uy/9zhPd3BwXsePIVv6pJwZ8j3N8drDADK/d3B1/H2Yrt1hhzJUPXNiv4857nOLPADKzcx5mvz7Art1tjzJVy9oOL5XN5Wlqa4uLilJqa6unlFEVQZmClpqaqV69eOnHihNasWZNv80qSIiMjFRkZmSdut9tlt3uX4H7TzuXesIWNn/u65xM3DMNn3F+Ohs42lbyWl7z2aU/cT+uxqPFz1+m+pNFfTUaYr3iYZPioqajxMN/bw1+8MNvDazWG75p8x4u/ptzp+tv3fL2/OQ8UPl5cNRV0PC3blucR3zn6PdUUJW74iedMn+7R9Jyon9xD+RxBTcVTk2EoKMeTv3h+NflYPGjnCLu94O3knuRb1HN5SdTkflv9jrklPD4VpSbDKPh4yp1SsMZcd03npnpu7p7J3kEecyXJvenzO0f4Os6CdY7wdZzlzt1rPwjg8ZQ7R3cSuTd7kY+zIJ0j8hufzk0zmOcIX8Ouv3NEII8nf3H3Me/v80LRzofBG3PP5pvrdYL8ubxQx5kFxtyCcizycRaAms7dXc89R7jTCvaYK3nvB6H+udxf/oUV8AZWRkaG+vXrp6SkJK1YsUKXXnppwU8CAAAAAADA31ZAG1hOp1NDhgzRunXr9Nlnn+mKK64I5OoBAAAAAAAQggLawLrvvvu0aNEi9evXT8eOHdN7773n9fjQoUMDmQ4AAAAAAABCQEAbWJs3b5YkLV68WIsXL87zOA0sAAAAAAAAnCugDazVq1cHcnUAAAAAAAC4CPj63RUAAAAAAADAMmhgAQAAAAAAwNJoYAEAAAAAAMDSAnoPLADAxWfZtmBncFaPpsHOAAAAAEBJYAYWAAAAAAAALI0ZWAD+FpglBAAAAAChixlYAAAAAAAAsDRmYAGABTFjDAAAAADOYgYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACwt4A2szMxMPfjgg6pWrZqio6PVvn17LV++PNBpAAAAAAAAIEQEvIE1cuRIPffcc7r55pv1wgsvyGazqXfv3vruu+8CnQoAAAAAAABCgD2QK9u4caM++OADPfPMM/rXv/4lSRo+fLiaNm2qBx54QN9//30g0wEAAAAAAEAICOgMrIULF8pms2ns2LGeWFRUlMaMGaN169Zp3759gUwHAAAAAAAAISCgDazExEQ1bNhQMTExXvF27dpJkjZv3hzIdAAAAAAAABACAnoJ4cGDB1W1atU8cXcsOTnZ5/MyMzOVmZnp+Xtqaqok6dixY3I4HJKksLAwhYWFyeVyyeVyeZZ1x51Op0zTLDBus9lkGIbndXPHJcnpdBYqbrfbZZqmV9wwDNlstjw5GoahkxnpMiXJyPUiZs5f/cZzx84zrnNfW2ffX381nUrLHTdkhNlkmi7JdBUcN8JkGGH+4y5nrsTyi+dsp2PHCt5Op9Jyls+p2bsmIyynJu94ydV07Fj++97pU4ZMl3dN/nIv6ZrS0go+nk6l+a/VnaNhBKamY8f+ivo5zk6dLN5970JqOnas4HPEqbTAH0/+ajp2LP/znns/CPTx5Cvu3g/yO5efOqmAH0/+akpLy398OpUWnOPJV/zYsbznAr/HWQCPJ381HT/uf8zN2Q+Cczz5qik1teDPETnHWXDHXHdNuY8zKW/up05aY8yVpBMnCv685xnL/qrVV+6BOkf4Os5y557zmSb4Y66Usx/4G3Pdufs9zoJwjkhNzf9z+dn9ILhjrkyn5xiT/B9np08Ff8x1S03N//uT93cHBex48hU/frzg74Tu7w7BHHNzH2f5fc89fcoaY65kKC3N/5ib5zgL4pjrjuc+znx9Lj+VZo0xV8rZD0q6H5Hfubw4eyxpaTk7Qe7HiyKgDaz09HRFRkbmiUdFRXke92X69OmaPHlynnidOnWKN0HkeGhcsDMAAAAAAAAXoZMnTyo2NrbIzwtoAys6OtprJpVbRkaG53FfJkyYoHvvvdfzd5fLpWPHjikuLk6Gce60or+ntLQ01ahRQ/v27ctziaYVhVK+oZSrFFr5hlKuUmjlG0q5SqGVbyjlKoVWvqGUqxRa+YZSrlJo5RtKuUqhlW8o5SqFVr6hlKsUWvmGUq5SaOUbSrlKoZdvIJimqZMnT6patWrn9fyANrCqVq2qAwcO5IkfPHhQkvwWERkZmWfmVrly5Yo9v4tBTExMSB0coZRvKOUqhVa+oZSrFFr5hlKuUmjlG0q5SqGVbyjlKoVWvqGUqxRa+YZSrlJo5RtKuUqhlW8o5SqFVr6hlKsUWvmGUq5S6OVb0s5n5pVbQG/i3qJFCyUlJXmue3TbsGGD53EAAAAAAAAgt4A2sAYNGiSn06nXX3/dE8vMzNTs2bPVvn171ahRI5DpAAAAAAAAIAQE9BLC9u3ba/DgwZowYYL+/PNP1a9fX2+//bb27NmjN998M5CpXHQiIyM1ceJEnzfJt6JQyjeUcpVCK99QylUKrXxDKVcptPINpVyl0Mo3lHKVQivfUMpVCq18QylXKbTyDaVcpdDKN5RylUIr31DKVQqtfEMpVyn08g0Fhnm+v194njIyMvToo4/qvffe0/Hjx9WsWTM9/vjjuvbaawOZBgAAAAAAAEJEwBtYAAAAAAAAQFEE9B5YAAAAAAAAQFHRwAIAAAAAAICl0cACAAAAAACApdHACnGZmZl68MEHVa1aNUVHR6t9+/Zavnx5sNPy6dSpU5o4caJ69uyp8uXLyzAMzZkzJ9hp+fTDDz/ozjvvVEJCgkqXLq2aNWvqhhtuUFJSUrBT8+mXX37R4MGDVbduXZUqVUoVKlRQ586dtXjx4mCnVihTp06VYRhq2rRpsFPJY/Xq1TIMw+ef9evXBzs9n3766Sf1799f5cuXV6lSpdS0aVO9+OKLwU4rj5EjR/p9bw3D0IEDB4KdopfffvtNN954o+Lj41WqVCk1btxYU6ZM0ZkzZ4Kdmk8//vijevbsqZiYGJUtW1Y9evTQ5s2bg51WkcaCHTt2qGfPnipTpozKly+vYcOG6ciRI5bLdePGjbr99tvVunVrhYeHyzCMgOWYW2HydblcmjNnjvr3768aNWqodOnSatq0qZ544gllZGRYKldJeuONN9SlSxdVrlxZkZGRqlOnjkaNGqU9e/YELNei5Jtbdna2Lr30UhmGoWeffTYwiarwufo7Bzdu3DhguRYlXyln/33llVfUokULRUdHKy4uTt27d9eWLVsslWt+Y9s111wTkFyLkq8kzZ8/X5dffrnKlSunuLg4denSRV988YUlc33ppZfUpEkTRUZGqnr16rr33nt1+vTpgOValO8</t>
+    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACmsElEQVR4nOzdeXhU9dn/8c+ZmeyrgUQCBGVTNgHZFBQURUAUbRERrQrUVlutS9Xaqm0RfQruS7XaWvuI68+KVSuPC5tgsagYiygCYgVRFsEQmCxkm5nv7484WzIzScgyJ+H9ui4vyT1nzrnvOevc+Z4TyxhjBAAAAAAAANiUI94JAAAAAAAAALHQwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgCgDVmW1eT/Tj311HinHXD00UfLsix99dVX8U6lWfyfLVrXV199JcuydPTRR8c7FQAA0M654p0AAACHk1mzZtWLffvtt1qyZEnU1/v169ekZaxatUrjx4/XKaecolWrVh1Snu3ZqaeeqnfeeUcrV660VfMvEn8TzRjT6su67bbbNG/ePM2dO1e33XZbqy8PAACgJdHAAgCgDS1cuLBebNWqVYEGVqTX0fI2bdoU7xQAAADQBDSwAADAYaepo9oAAAAQXzwDCwAAm9uxY4euvvpq9e3bV8nJycrKytJJJ52kv/zlL/J6vWHTnnrqqRo/frwk6Z133gl7llboc4i+++47/fGPf9SUKVPUs2dPpaSkKDMzUyNGjNBdd92lysrKFst/9uzZsixLCxcu1Pr16zVt2jTl5uYqJSVFgwcP1kMPPVSvDkkqLS3VX//6V02bNk19+/ZVWlqa0tLSdNxxx+nWW2/VgQMHwqZftWqVLMvSO++8I0kaP358WP2ho9tiPQPL4/HoiSee0KmnnqqcnBwlJSWpZ8+e+vnPf65vvvmm3vT+5Z566qmqqanRXXfdpYEDByolJUWdOnXStGnT6o34uu2228KWX/e5Z6HPGFu0aJEmTJigTp06KSEhQZ06ddKAAQP005/+VJ988klDH39g/vPmzZMkzZs3L2xZs2fPDpu2uLhYt9xyiwYOHKjU1FRlZGRo+PDhuvvuu1VRUdGo5UXi8Xh09913Bz6bzp07a8aMGdq8eXPU91RUVOi+++7TiSeeqOzsbCUnJ+vYY4/VTTfdpH379jU5h+XLl2vq1Kk68sgjlZCQoCOOOEJ9+/bVxRdfrH/9618R37NixQpNmzZN+fn5SkxMVF5enn74wx/qvffea7G8Fy5cGFgX5eXluvnmm9WnTx8lJSWpS5cumjVrlnbu3NnkegEA6EgYgQUAgI19+OGHmjx5soqLi9WjRw/94Ac/kNvt1qpVq7RmzRq98soreu2115SYmChJmjx5spKTk7VkyRIdeeSRmjx5cmBenTt3Dvx7yZIluvbaa9WtWzf16dNHJ554or777jt98MEH+s1vfqN//vOfWrlypZKSklqslrVr1+rnP/+5unTpotNPP1379+/XqlWrdN111+ndd9/Viy++GNbUWb9+vS6//HLl5ubq2GOP1fDhw7V//3599NFHmj9/vl588UW9//776tSpkyQFvui/9dZb2rNnjyZNmqQuXboE5tenT58GcywtLdU555yjVatWKT09XcOHD1dubq4+/fRT/fnPf9aiRYu0bNkyHX/88fXeW1NToylTpmjNmjUaN26c+vfvr7Vr1+qVV17RypUrtW7dukATcejQoZo1a5aeeuopSfWffZaeni5Juv322zV37ly5XC6NGTNG3bp1k9vt1tdff62//e1vGjhwoAYPHtxgXbNmzdLHH3+s9evXa8iQIRo6dGjgtZNPPjnw761bt+q0007T9u3blZubqylTpqimpkYrV67Ur3/9a/3973/X8uXLdcQRRzS4zLouuOACLV68WKeccooGDx6stWvXatGiRXrzzTe1dOlSjR49Omz6Xbt2afLkyfr000+Vk5OjkSNHKiMjQ//5z390zz33aNGiRVq1apWOOuqoRi3/qaee0pw5cyRJo0aN0vjx41VRUaEdO3bohRdeUOfOnTVu3Liw99x4442677775HA4NGLECI0dO1Zff/21/vnPf2rx4sX661//GphnS+Ttdrs1ZswYff311xo7dqwGDRqk9957T08//bTeeecdrV+/XllZWU352AEA6DgMAACIq5UrVxpJpu5pubKy0hx11FFGkvnZz35mqqurA699+eWX5uijjzaSzC233BJxfqecckrUZW7cuNG899579eLFxcVm4sSJRpK5++67673uz2fbtm2Nrm/WrFmB+q688kpTU1MTeG3Dhg0mNzfXSDJ//vOfw973zTffmOXLlxuv1xsWLy8vN5deemlgfnWdcsopRpJZuXJl1Jwifd7GGHPRRRcZSebss882e/bsCXvtgQceMJJM3759jcfjCcRD19/xxx9vdu/eHXitoqLCTJo0yUgyl19+eaPzMKZ2/aekpJj09HSzefPmeq9/9dVXZtOmTVFrrGvu3LlGkpk7d27UaU444QQjyZxzzjmmrKwsEN+7d68ZNmyYkWQuuuiiRi9z27ZtgRo7d+5s1q9fH3jN4/GYq6++2kgyRx11lKmsrAy85vP5zEknnWQkmcsuu8yUlJQEXqupqTE33HCDkWTGjx/f6Fx69uxpJJnVq1fXe23Pnj3mP//5T1js8ccfN5JMnz59wvI2xph33nnHZGRkmMTERLNly5Zm5/3kk08GPqdJkyYZt9sdeK24uNgMHTrUSDLz589vdL0AAHQ0NLAAAIizaA2sZ555xkgyXbt2Dfty7/fSSy8ZSSYjI8NUVFTUm1+sBlYsn3/+uZFkRo4cWe+15jSw8vPzw/L0e/jhhwONocYqLy83LpfL5Obm1nvtUBtYGzduNJZlma5du4Y1HkJNmTLFSDKLFy8OxPyft2VZ5uOPP673nvfff99IMr169WpUHn579+41kszgwYOj1tEUDTWwVq9ebSSZ1NRU8+2339Z7vbCw0EgyDofDfPPNN41aZmgD68EHH6z3emVlpenWrZuRZJ577rlA/M033zSSzNChQ8Mann5er9cMGjTISDKffvppo3JJTU01WVlZjZrW6/Warl27GkmmsLAw4jR33323kWRuuOGGZuftb2ClpaWZXbt21XvfCy+8YCSZ0047rVH5AwDQEfEMLAAAbGrVqlWSpJkzZ0a8lW/atGk64ogjVFpaqo8++qjJ8/d6vVqxYoXuuOMOXXnllZozZ45mz56tP/zhD5Kkzz//vFn51zVjxgwlJyfXi/tvn/viiy+0a9eueq+vWbNGd911l6666qpAjldeeaUSExP13Xffaf/+/S2S3xtvvCFjjM4880xlZGREnObUU08N5FRXjx49NGTIkHrx/v37S1KTn2GUm5uro48+Wp988oluuOEGbdy4sUnvbyr/9jZ58mQdeeSR9V4fPny4hgwZIp/PF3jOWFPUvU1SkpKSknTBBReELV+SXn/9dUnSeeedJ5er/hMvHA5H4Ha/SOsiklGjRsntduvSSy/VRx99JJ/PF3XadevWadeuXerdu7eGDx8ecZpI20Jz8x4xYoTy8/PrxQ91GwIAoCPhGVgAANiU/8tqz549I75uWZZ69uyp/fv3N/mL7RdffKEf/vCH+uyzz6JOU1JS0qR5NiRaHRkZGerUqZP27dunHTt2qGvXrpKkvXv36rzzztO7774bc74lJSWH9EymurZu3SpJ+tvf/qa//e1vMaf97rvv6sV69OgRcdrMzExJUlVVVZNzevrppzV9+nTdf//9uv/++5WTk6MTTjhBZ5xxhi655JKw55o1V0PbmyT17t1b69evb/L2lp2drezs7Iiv+Ze3Y8eOQMy/Ln73u9/pd7/7Xcx5R1oXkTz66KM6++yz9cwzz+iZZ55RRkaGRo4cqdNOO02XXHJJ2PrzL//LL7+M+rD/SMtvbt4NbUMt+ccVAABob2hgAQBwGJo+fbo+++wznX322brppps0YMAAZWZmKiEhQdXV1S368PamMMYE/v2Tn/xE7777rkaPHq158+ZpyJAhOuKII5SQkCBJ6tq1q3bv3h32nubwj8gZOnRoxJFUoU444YR6MYej5Qe2jx07Vl999ZVef/11vfPOO1qzZo2WLFmiN998U3PnztUrr7yi008/vcWXGw+h69G/Lk4++WT17t075vsGDhzYqPn3799fn3/+uZYuXaq3335ba9as0erVq/X222/r9ttv19/+9jddfPHFYcvv0qWLJk2aFHO+oU3E5ubdGtsQAAAdBQ0sAABsqlu3bpKCozoi2bZtW9i0jbF582Z98sknysvL0yuvvFLvVqcvvvjiELJtmD/XukpLS7Vv3z5JUvfu3SVJ5eXleuONN+RwOPTGG2/UG71TXl6ub7/9tkXzKygokCSddNJJeuSRR1p03s2RkpKi6dOna/r06ZJqR+789re/1eOPP64f//jH2r59e4sspzHbm/+1pmxvknTgwAEdOHAg4iisr776SlJw3UvBdXHuuefqxhtvbNKyYnG5XJoyZYqmTJkiqXb03v3336958+bpiiuu0A9/+EOlpaUFlt+pUyctXLiw0fNvrbwBAIDEr3kAALAp/zN2/v73v0e8deiVV17R/v37lZGREfacnsTEREmSx+OJON/i4mJJtSOYIj2n59lnn21u6hEtWrQo4m10zzzzjCSpT58+gcaI2+2W1+tVZmZmxKbHs88+G3XkVUP1R3PmmWdKkl577bU2u1XLP5qsKbnm5ubq7rvvliR9/fXXjX4GWEOfi397e+utt7Rnz556r69bt04ff/xx2HOcmsK/nkNVV1fr73//e9jypeC6WLRoUYuNsIskMzNTt912m7Kzs3Xw4EFt2bJFkjRy5Eh17txZGzdujHmbbV1tlTcAAIcjGlgAANjU+eefrx49emjXrl26/vrrwxoP27Zt0w033CBJuvrqq8Meju4fyfLFF1+opqam3nyPOeYYOZ1Offrpp2EPzpakxYsX64EHHmiFaqRdu3bpxhtvlNfrDcQ2bdqk22+/XZL0y1/+MhA/8sgjdcQRR+jAgQP1Gh/vv/++br755qjL8dfflMaDJB1//PE677zz9M0332jatGmBkUGhysvL9dxzz0Vs8ByKWLlu375dTzzxRMRnkS1evFiSdMQRRwSej9ScZUm1t72dcMIJqqio0BVXXKGDBw8GXisqKtIVV1whqfaPCvhHGjXFHXfcoQ0bNgR+9vl8+vWvf60dO3aooKBA5513XuC1c889VyNHjtTatWs1Z86ciM+L2r9/v/785z83qvl38OBB3X///RHns3r1ah04cEBOpzPwGSUkJGju3LkyxuiHP/xhxOeweb1evf3223r//fdbLW8AABAifn8AEQAAGGPMypUrjSQT6bS8du1ak5OTYySZo446ylxwwQVmypQpJjk52UgykyZNMlVVVfXeN2LECCPJHHvsseZHP/qRueyyy8yvf/3rwOvXXnutkWQcDoc55ZRTzIUXXmiGDRtmJJnf/va3UfM56qijjCSzbdu2Rtc3a9YsI8n87Gc/M8nJyaZnz55m5syZZtKkSSYxMdFIMj/84Q+Nz+cLe98DDzwQyOOEE04wF154oTnppJOMZVnmkksuiZrL//3f/xlJJjEx0Zx99tnmxz/+sbnsssvMv//978A00eorKSkxp59+euD9I0eONDNmzDDnn3++GTlyZCDfTZs2Bd7jX3+nnHJK1M8g2vJuvPFGI8l07tzZzJgxw1x22WXmsssuM0VFRWbdunVGkklISAjkMWPGDHP88ccbScayLPPEE080ci0Y8+2335q0tDQjyZx00klm9uzZ5rLLLjP/+7//G5jmyy+/DHyueXl5Zvr06ebcc881mZmZRpIZNmyYKS4ubvQyt23bZiSZHj16mB/+8IcmISHBnHHGGWbmzJmmd+/eRpJJS0szq1evrvfenTt3mqFDhwamGTNmjJk5c6aZNm2aGTp0qHE6nUaSqaioaDCP/fv3B7b3IUOGmOnTp5sLL7zQjB492liWZSSZ3//+9/Xe96tf/Sqw7gYOHGjOPfdcM3PmTHPqqaea7OxsI8k89thjzc77ySefNJLMrFmzYn6ORx11VIO1AgDQUdHAAgAgzmI1sIwx5uuvvzZXXXWV6dWrl0lMTDQZGRlm9OjR5rHHHjM1NTUR37N9+3Zz0UUXmfz8fONyuep9+fX5fOZvf/ubGT58uElPTzdZWVnm5JNPNi+88IIxJnrDpTkNrCeffNL85z//MVOnTjWdOnUySUlJZuDAgeb++++PWserr75qxowZY7Kzs016eroZMWKEefTRR43P54uZy1//+lczbNgwk5qaGqjlySefDLwe6/P2er3m+eefN1OmTDFHHnmkSUhIMJ06dTKDBg0yc+bMMa+88oqprq4OTN+cBlZFRYW56aabTJ8+fQLNMX9NJSUl5sEHHzQ//OEPTd++fU16erpJS0szxxxzjLn00ktNYWFh1OVF869//ctMmDDBHHHEEcbhcERsmuzbt8/cfPPNpn///iY5Odmkpqaa448/3tx5553m4MGDTVpeaOOlpqbG/OEPfzD9+vUzSUlJJicnx5x33nnms88+i/r+yspK8+c//9mMHz/edOrUybhcLpOXl2eGDh1qrrrqKrNkyZJG5VFTU2P+/Oc/mwsvvND069fPZGVlmZSUFNO7d29z3nnnmRUrVkR977///W/zox/9yBx11FEmKSnJZGRkmGOOOcb84Ac/ME888UTEhl5T86aBBQBAwyxjuEEfAAC0ntmzZ+upp57Sk08+qdmzZ8c7HQAAALRDPAMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2xjOwAAAAAAAAYGuMwAIAAAAAAICt0cACAAAAAACArbnincCh8Pl82rVrlzIyMmRZVrzTAQAAAAAAQAzGGJWWlqpr165yOJo+nqpdNrB27dqlgoKCeKcBAAAAAACAJvjmm2/UvXv3Jr+vXTawMjIyJNUWnZmZGedsAAAAAAAAEEtJSYkKCgoCPZ2mapcNLP9tg5mZmTSwAAAAAAAA2olDfRQUD3EHAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK21y79CCAAAAAAAmsfr9aqmpibeaaCdc7lccjqdh/zXBRu9nFadOwAAAAAAsBVjjL799lsdOHAg3qmgg3A6ncrLy1NWVlarNbJoYAEAAAAAcBjxN6/y8vKUmpra6iNn0HEZY+TxeFRSUqLdu3eroqJC+fn5rbIsGlgAAAAAABwmvF5voHnVqVOneKeDDiIjI0NJSUkqKipSXl6enE5niy+Dh7gDAAAAAHCY8D/zKjU1Nc6ZoKNJS0uTMabVnqtGAwsAAAAAgMMMtw2ipbX2NkUDCwAAAAAAALZGAwsAAAAAAOAwMHv2bB199NHxTuOQ0MACAAAAAAAdwsKFC2VZVtT/3n///Xin2KCNGzfqtttu01dffRXvVGyFv0IIAAAAAAA6lNtvv109e/asF+/Tp08csmmajRs3at68eTr11FPb7Wip1kADCwAAAAAAaOmGeGdQa+Kg5s/jzDPP1IgRI5o/I9gGtxACAAAAAIDDxty5c+VwOLRixYqw+OWXX67ExEStX79ekrRq1SpZlqW///3vuuWWW9SlSxelpaXpnHPO0TfffFNvvh988IEmT56srKwspaam6pRTTtG///3vetPt3LlTl112mbp27aqkpCT17NlTP//5z1VdXa2FCxfq/PPPlySNHz8+cOvjqlWrAu9/8803NXbsWKWlpSkjI0NnnXWWPvvss3rLefXVVzVo0CAlJydr0KBBeuWVV5rzscUdI7AAAAAAAECH4na7VVRUFBazLEudOnXSb3/7Wy1evFiXXXaZPv30U2VkZGjJkiX661//qjvuuENDhgwJe98f/vAHWZalX//619q7d68efPBBTZgwQR9//LFSUlIkSW+//bbOPPNMDR8+PNAge/LJJ3Xaaadp9erVGjVqlCRp165dGjVqlA4cOKDLL79c/fr1086dO/XSSy/p4MGDGjdunK655hr98Y9/1C233KL+/ftLUuD/zzzzjGbNmqVJkybprrvu0sGDB/XYY4/p5JNP1rp16wK3HC5dulTnnXeeBgwYoAULFmjfvn2aM2eOunfv3pofe6uyjDEm3kk0VUlJibKysuR2u5WZmRnvdAAAAAAAaBcqKyu1bds29ezZU8nJyWGvdYRbCBcuXKg5c+ZEfC0pKUmVlZWSpA0bNmj48OG69NJLdc8992jQoEHKz8/Xe++9J5erdqzPqlWrNH78eHXr1k2bNm1SRkaGJGnRokWaMWOGHnroIV1zzTUyxujYY49Vr1699Oabb8qyLElSRUWFBg4cqD59+mjp0qWSpFmzZunZZ5/VBx98UO8WR2OMLMvSSy+9pPPPP18rV67UqaeeGni9rKxMBQUFOv/88/X4448H4nv27NGxxx6rGTNmBOLHH3+89uzZo02bNikrK0uStGzZMk2cOFFHHXVUqzwgPta2JTW/l8MILAAAAAAA0KH86U9/0jHHHBMWczqdgX8PGjRI8+bN080336xPPvlERUVFWrp0aaB5FerSSy8NNK8kafr06crPz9cbb7yha665Rh9//LG++OIL/fa3v9W+ffvC3nv66afrmWeekc/nk1R7W9/UqVMjPp/L3/iKZtmyZTpw4IAuvPDCsNFlTqdTJ5xwglauXClJ2r17tz7++GP95je/CTSvJOmMM87QgAEDVF5eHnM5dkUDCwAAAAAAdCijRo1q8CHuv/rVr/TCCy9o7dq1mj9/vgYMGBBxur59+4b9bFmW+vTpExjF9MUXX0iqHV0VjdvtVnV1tUpKSjRo0KENMfMv57TTTov4un9U0/bt2yPmLUnHHnus/vOf/xzS8uONBhYAAADQDtjl1h6pcbf3tLd8ARx+tm7dGmgKffrpp4c8H//oqnvuuUdDhw6NOE16erqKi4sPeRmhy3nmmWfUpUuXeq9HGj3WkXTs6gAAAAAAAOrw+XyaPXu2MjMzdd1112n+/PmaPn26pk2bVm9af5PLzxij//73vxo8eLAkqXfv3pJqR0BNmDAh6jJzc3OVmZmpDRtid/ij3UroX05eXl7M5Rx11FER85akzz//POay7cwR7wQAAAAAAADa0v333681a9bo8ccf1x133KExY8bo5z//eb2/XChJTz/9tEpLSwM/v/TSS9q9e7fOPPNMSdLw4cPVu3dv3XvvvSorK6v3/u+++06S5HA49IMf/ECLFy9WYWFhven8f2MvLS1NknTgwIGw1ydNmqTMzEzNnz9fNTU1UZeTn5+voUOH6qmnnpLb7Q68vmzZMm3cuDHm52JnjMACAAAAAAAdyptvvqnNmzfXi48ZM0ZVVVX63e9+p9mzZ2vq1KmSav964dChQ3XllVfqxRdfDHtPTk6OTj75ZM2ZM0d79uzRgw8+qD59+uinP/2ppNrG1BNPPKEzzzxTAwcO1Jw5c9StWzft3LlTK1euVGZmphYvXixJmj9/vpYuXapTTjlFl19+ufr376/du3dr0aJFevfdd5Wdna2hQ4fK6XTqrrvuktvtVlJSkk477TTl5eXpscce0yWXXKJhw4Zp5syZys3N1ddff63XX39dJ510kh555BFJ0oIFC3TWWWfp5JNP1o9//GMVFxfr4Ycf1sCBAyM22doDGlgAAAAAAKBD+f3vfx8x/sQTT+gvf/mLOnfurAcffDAQ79u3rxYsWKBrr71WL774ombMmBF47ZZbbtEnn3yiBQsWqLS0VKeffroeffRRpaamBqY59dRT9d577+mOO+7QI488orKyMnXp0kUnnHCCrrjiisB03bp10wcffKDf/e53eu6551RSUqJu3brpzDPPDMyvS5cu+vOf/6wFCxbosssuk9fr1cqVK5WXl6eLLrpIXbt21Z133ql77rlHVVVV6tatm8aOHas5c+YEljN58mQtWrRIv/3tb3XzzTerd+/eevLJJ/XPf/5Tq1ataqFPuW1Zxj9GrR0pKSlRVlaW3G534Cn7AAAAQEfW3h6K3t7yBQ4XlZWV2rZtm3r27Knk5OR4p2Nrq1at0vjx47Vo0SJNnz493unYXkPbVnN7OTwDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtsZD3AEAAAAAAOo49dRT1Q4fG95hMQILAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAB0CAsXLpRlWUpOTtbOnTvrvX7qqadq0KBBccgMzeWKdwIAAAAAAMAG3nor3hnUmjy52bOoqqrSnXfeqYcffrgFEoIdMAILAAAAAAB0KEOHDtVf//pX7dq1K96poIUwAgsAAADAYW3phnhnEDSRO5uAFnHLLbfooosu0p133qk//vGPUafzeDxasGCBFi5cqB07dig/P18XXXSR5s6dq6SkJEnS9ddfr6eeekpFRUWyLEuSdPXVV+uRRx7RQw89pGuuuUaStGfPHnXp0kWPPvqofv7zn7d+kYcZRmABAAAAAIAOpWfPnrr00ksbHIX1k5/8RL///e81bNgwPfDAAzrllFO0YMECzZw5MzDN2LFjVVxcrM8++ywQW716tRwOh1avXh0Wk6Rx48a1QkWggQUAAAAAADqcW2+9VR6PR3fddVfE19evX6+nnnpKP/nJT7Ro0SJdeeWVeuqpp3TjjTfq1Vdf1cqVKyVJJ598sqRgg8rtduvTTz/VeeedV6+BlZOTowEDBrRyZYcnGlgAAAAAAKDD6dWrly655BI9/vjj2r17d73X33jjDUm1twiGuuGGGyRJr7/+uiQpNzdX/fr107/+9S9J0r///W85nU796le/0p49e/TFF19Iqm1gnXzyyYHbDNGyaGABAAAAAIAO6be//a08Ho/uvPPOeq9t375dDodDffr0CYt36dJF2dnZ2r59eyA2duzYwGir1atXa8SIERoxYoRycnK0evVqlZSUaP369Ro7dmzrFnQYo4EFAAAAAAA6pF69euniiy+OOgpLUqNGTJ188snauXOntm7dqtWrV2vs2LGyLEsnn3yyVq9erTVr1sjn89HAakU0sAAAAAAAQIflH4VV91lYRx11lHw+X+AWQL89e/bowIEDOuqoowIxf2Nq2bJl+vDDDwM/jxs3TqtXr9bq1auVlpam4cOHt3I1hy9XvBMAAAAA4mXphnhnEDRxULwzAICOqXfv3rr44ov1l7/8RUcddZRcrtpWyJQpU3TLLbfowQcf1F/+8pfA9Pfff78k6ayzzgrEevbsqW7duumBBx5QTU2NTjrpJEm1ja0bb7xRL730kk488cTAvNHyGIEFAAAAAAA6tFtvvVU1NTX6/PPPA7EhQ4Zo1qxZevzxx3XBBRfo0Ucf1ezZs3X33XfrBz/4gcaPHx82j7Fjx+rzzz/XoEGDdMQRR0iShg0bprS0NG3ZsoXbB1tZsxtYn332mc4//3z16tVLqamp6ty5s8aNG6fFixeHTTd79mxZllXvv379+jU3BQAAAAAAgKj69Omjiy++uF78iSee0Lx58/Thhx/quuuu09tvv62bb75ZL7zwQr1p/Q2qk08+ORBzuVwaPXp02OtoHZYxxjRnBm+88Yb++Mc/avTo0eratasOHjyof/zjH1q9erX+8pe/6PLLL5dU28B64YUX9MQTT4S9PysrS1OnTm3SMktKSpSVlSW3263MzMzmpA8AAIDDWHu6hbA95Sq1r3zbU65Ac1VWVmrbtm3q2bOnkpOT450OOpCGtq3m9nKafXPmlClTNGXKlLDYL37xCw0fPlz3339/oIEl1XYmI3U8AQAAAAAAgGha5RlYTqdTBQUFOnDgQL3XvF6vSkpKWmOxAAAAAAAA6IBarIFVXl6uoqIiffnll3rggQf05ptv6vTTTw+b5uDBg8rMzFRWVpZycnJ01VVXqaysrKVSAAAAAAAAQAfUYn/f8YYbbgj82UmHw6Fp06bpkUceCbyen5+vm266ScOGDZPP59Nbb72lRx99VOvXr9eqVati/qnJqqoqVVVVBX72j+DyeDzyeDyBZTocDvl8Pvl8vsC0/rjX61Xo476ixZ1OpyzLCsw3NC7VjiBrTNzlcskYExa3LEtOp7NejtHi1ERN1ERN1ERN1ERN1NS6NZngbCSrNneZ8NyjxS1HbU3hcUuWwyljfKoz88hxyyHLcsgYnzye2DUZX8j0Pq+kkEfZWrU1GV/4emqtmjyehtdT1Frr5d42NcXa9oJpNryeWrum0F2tve1PoTrKMaIj1uTxeGSMCfzXFJZlRXyP3eJNYbfc23NNkmSMCevV1N32mqPFGljXXXedpk+frl27dunFF1+U1+tVdXV14PUFCxaETT9z5kwdc8wxuvXWW/XSSy9p5syZUee9YMECzZs3r1583bp1SktLkyTl5uaqd+/e2rZtm7777rvANN27d1f37t21ZcsWud3uQLxXr17Ky8vThg0bVFFREYj369dP2dnZWrduXdiBZvDgwUpMTFRhYWFYDiNGjFB1dbU++eSTQMzpdGrkyJFyu93avHlzIJ6SkqIhQ4aoqKhIW7duDcSzsrLUv39/7dq1Szt27AjEqYmaqImaqImaqImaqKl1a6o+EKwpofNgWc5EVe8JrynxyBEy3mrVFAVrsiynEruMlKl2q6Y4WJPlSlFi7hD5KorkcQdrciRlKSGnv7xlu+QtC9bkTMmVK7u3vO5tKiyMXVN1qeTK6iVnap5q9m2Q8QRrSsjpJyspWzV718mY1q+p8GDD68nr3iZvRbAmZ3p3uTK6y3Ngi3xVwfXUFjU1tO1VlzZ+PbV2TYUHgzW1t/2pIx4jOmpNycnJOnjwoBITE+VwOFReXh5WU1pamnw+X9g8LMtSWlqavF6vKisrA3GHw6HU1FR5PJ6wgSdOp1MpKSmqqakJ6w24XC4lJyerqqoqrKGRmJioxMREVVZWhn3uSUlJSkhIUEVFRVgTLzk5WS6XSwcPHgxrpqSkpFBTnGqSpJqaGm3YEPzLGKHbXnMfJ9Xsv0IYzcSJE3XgwAF98MEHsiwr4jQVFRVKT0/XnDlz6v11wlCRRmAVFBRo3759gSfX022nJmqiJmqiJmqiJmqipqbWtGJjSJJxHoF1ev/YNa3YGDJ9nEdgnT6g4fW05FP7jMA6Y2DsbS+4HcR/BNbpA4Lh9rY/heoox4iOWFNlZaW+/vrrQ/orhHYbldSeRyt1xJqqqqq0detW9ejRI7BthW57JSUl6tSpU/z+CmE006dP1xVXXKEtW7bo2GOPjThNSkqKOnXqpOLi4pjzSkpKCnTzQrlcrnq3Hvp32Lr8B5XGxqPd0tiUuGVZEePRcmxqnJqoKVqcmqhJoqZoOTY1Tk3UJFFTtBybGrdjTVakJ8JaUS6RI8Qty4oSdyjSzGPFXa7YNYW+zXJErslyND73aPHG1BS6GqOtj6i1Rs29dWuKte3VTbPJ668Fa4q0S7WX/am5cWpqm5pcLpcsywr811TR3mO3eFPYLff2XlOkXk2kWFO1yl8hlBQYwhY6nLGu0tJSFRUVKTc3t7XSAAAAAAAAQDvX7AbW3r1768Vqamr09NNPKyUlRQMGDFBlZaVKS0vrTXfHHXfIGKPJkyc3Nw0AAAAAAAB0UM2+hfCKK65QSUmJxo0bp27duunbb7/Vc889p82bN+u+++5Tenq6vvrqKx1//PG68MIL1a9fP0nSkiVL9MYbb2jy5Mk699xzm10IAAAAAAAAOqZmN7AuuOAC/e1vf9Njjz2mffv2KSMjQ8OHD9ddd92lc845R5KUnZ2ts88+W8uWLdNTTz0lr9erPn36aP78+brxxhsj3ssLAAAAAAAASC3QwJo5c6ZmzpwZc5rs7Gw988wzzV0UAAAAAABAXFiWpblz5+q2226LdyqHJYY+AQAAAACAdi30LyvG+m/VqlXxThWHqNkjsAAAAAAAQAfw3//GO4Naffo0+S117/p6+umntWzZsnrx/v37Nys1xA8NLAAAAAAA0K5dfPHFYT+///77WrZsWb042i9uIQQAAAAAAB1eeXm5brjhBhUUFCgpKUnHHnus7r33XhljwqarqqrSL3/5S+Xm5iojI0PnnHOOduzYUW9+27dv15VXXqljjz1WKSkp6tSpk84//3x99dVXgWm2bt0qy7L0wAMP1Hv/mjVrZFmW/t//+38tXmtHxAgsAAAAAC0uY6dNbkWSpEFNvx0JQMdijNE555yjlStX6rLLLtPQoUO1ZMkS/epXv9LOnTvDGkw/+clP9Oyzz+qiiy7SmDFj9Pbbb+uss86qN88PP/xQa9as0cyZM9W9e3d99dVXeuyxx3Tqqadq48aNSk1NVa9evXTSSSfpueee0y9/+cuw9z/33HPKyMjQueee2+r1dwQ0sAAAAAAAQIf22muv6e2339b//M//6NZbb5UkXXXVVTr//PP10EMP6Re/+IV69+6t9evX69lnn9WVV16pP/3pT4HpfvSjH+mTTz4Jm+dZZ52l6dOnh8WmTp2q0aNH6x//+IcuueQSSdKll16qK664Qps3b1a/fv0kSTU1NXrxxRc1bdo0paamtnb5HQK3EAIAAAAAgA7tjTfekNPp1DXXXBMWv+GGG2SM0ZtvvhmYTlK96a677rp680xJSQn8u6amRvv27VOfPn2UnZ2t//znP4HXZsyYoeTkZD333HOB2JIlS1RUVMQzupqAEVgAAAAA0I4s3RDvDIImDop3BkDjbN++XV27dlVGRkZY3P9XCbdv3x74v8PhUO/evcOmO/bYY+vNs6KiQgsWLNCTTz6pnTt3hj1Ly+12B/6dnZ2tqVOn6vnnn9cdd9whqfb2wW7duum0005rmQIPA4zAAgAAAAAAaKKrr75af/jDHzRjxgy9+OKLWrp0qZYtW6ZOnTrJ5/OFTXvppZdq69atWrNmjUpLS/Xaa6/pwgsvlMNBW6axGIEFAAAAAAA6tKOOOkrLly9XaWlp2CiszZs3B173/9/n8+nLL78MG3X1+eef15vnSy+9pFmzZum+++4LxCorK3XgwIF6006ePFm5ubl67rnndMIJJ+jgwYOBZ2ShcWj1AQAAAACADm3KlCnyer165JFHwuIPPPCALMvSmWeeKUmB///xj38Mm+7BBx+sN0+n0xl226AkPfzww/J6vfWmdblcuvDCC/Xiiy9q4cKFOu644zR48ODmlHTYYQQWAAAAAADo0KZOnarx48fr1ltv1VdffaUhQ4Zo6dKl+uc//6nrrrsu8MyroUOH6sILL9Sjjz4qt9utMWPGaMWKFfrvf/9bb55nn322nnnmGWVlZWnAgAF67733tHz5cnXq1CliDpdeeqn++Mc/auXKlbrrrrtatd6OiAYWAAAAAADo0BwOh1577TX9/ve/19///nc9+eSTOvroo3XPPffohhtuCJv2f//3fwO3+7366qs67bTT9Prrr6ugoCBsuoceekhOp1PPPfecKisrddJJJ2n58uWaNGlSxByGDx+ugQMHatOmTfrRj37UarV2VJapO96tHSgpKVFWVpbcbrcyMzPjnQ4AAADaqfb019zaU66S9N6S+qMV4mX0pD4xX29vn217yxf2UllZqW3btqlnz55KTk6OdzqHneOPP145OTlasWJFvFNpcQ1tW83t5fAMLAAAAAAAgFZWWFiojz/+WJdeemm8U2mXuIUQAAAAAACglWzYsEEfffSR7rvvPuXn5+uCCy6Id0rtEiOwAAAAAAAAWslLL72kOXPmqKamRv/v//0/bt08RDSwAAAAAAAAWsltt90mn8+nTZs26ZRTTol3Ou0WDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAARGVZlm677ba45kADCwAAAAAAdAgLFy6UZVkR//vNb34T7/Ra1fPPP68HH3ww3mm0Gle8EwAAAAAAAGhJt99+u3r27BkWGzRoUJyyaRvPP/+8NmzYoOuuuy7eqbQKGlgAAAAAAEAvb3o53ilIkqb1n9bseZx55pkaMWJEC2QTVF5errS0tBadJxqPWwgBAAAAAMBh4+2339bYsWOVlpam7OxsnXvuudq0aVPYNLfddpssy9LGjRt10UUX6YgjjtDJJ58ceP3ZZ5/V8OHDlZKSopycHM2cOVPffPNNvWV98MEHmjJlio444gilpaVp8ODBeuihhwKvf/LJJ5o9e7Z69eql5ORkdenSRT/+8Y+1b9++sPmUlpbquuuu09FHH62kpCTl5eXpjDPO0H/+8x9J0qmnnqrXX39d27dvD9wyefTRRwfeX1VVpblz56pPnz5KSkpSQUGBbrrpJlVVVYUtp6qqSr/85S+Vm5urjIwMnXPOOdqxY8chf9YtiRFYAAAAAACgQ3G73SoqKgqLde7cWcuXL9eZZ56pXr166bbbblNFRYUefvhhnXTSSfrPf/4T1vSRpPPPP199+/bV/PnzZYyRJP3hD3/Q7373O82YMUM/+clP9N133+nhhx/WuHHjtG7dOmVnZ0uSli1bprPPPlv5+fm69tpr1aVLF23atEn/93//p2uvvTYwzdatWzVnzhx16dJFn332mR5//HF99tlnev/992VZliTpZz/7mV566SX94he/0IABA7Rv3z69++672rRpk4YNG6Zbb71VbrdbO3bs0AMPPCBJSk9PlyT5fD6dc845evfdd3X55Zerf//++vTTT/XAAw9oy5YtevXVVwP1/uQnP9Gzzz6riy66SGPGjNHbb7+ts846q6VXzyGhgQUAAAAAADqUCRMm1IsZY/SrX/1KOTk5eu+995STkyNJ+sEPfqDjjz9ec+fO1VNPPRX2niFDhuj5558P/Lx9+3bNnTtX//M//6NbbrklEJ82bZqOP/54Pfroo7rlllvk9Xp1xRVXKD8/Xx9//HGgqeXPw+/KK6/UDTfcELbME088URdeeKHeffddjR07VpL0+uuv66c//anuu+++wHQ33XRT4N9nnHGGunXrpv379+viiy8Om9/zzz+v5cuX65133gkbRTZo0CD97Gc/05o1azRmzBitX79ezz77rK688kr96U9/kiRdddVV+tGPfqRPPvkkyifddriFEAAAAAAAdCh/+tOftGzZsrD/du/erY8//lizZ88ONK8kafDgwTrjjDP0xhtv1JvPz372s7CfX375Zfl8Ps2YMUNFRUWB/7p06aK+fftq5cqVkqR169Zp27Ztuu6668KaV5ICo6okKSUlJfDvyspKFRUV6cQTT5SkwO2BkpSdna0PPvhAu3btavJnsWjRIvXv31/9+vULy/m0006TpEDO/vqvueaasPfb5aHwjMACAABAi1m6Id4ZBE3s2H9sCgAQw6hRo+o9xP3999+XJB177LH1pu/fv7+WLFlS70Htdf+S4RdffCFjjPr27RtxuQkJCZKkL7/8UlLDf/mwuLhY8+bN0wsvvKC9e/eGveZ2uwP/vvvuuzVr1iwVFBRo+PDhmjJlii699FL16tUr5vz9OW/atEm5ubkRX/cvd/v27XI4HOrdu3fY65E+r3iggQUAAAAAABBB6AgpqfZ5UpZl6c0335TT6aw3vf+5U401Y8YMrVmzRr/61a80dOhQpaeny+fzafLkyfL5fGHTjR07Vq+88oqWLl2qe+65R3fddZdefvllnXnmmTGX4fP5dNxxx+n++++P+HpBQUGTco4XGlgAAAAAgFbBqEzYyVFHHSVJ+vzzz+u9tnnzZnXu3Dls9FUkvXv3ljFGPXv21DHHHBNzOknasGFDxOdxSdL+/fu1YsUKzZs3T7///e8D8S+++CLi9Pn5+bryyit15ZVXau/evRo2bJj+8Ic/BBpYobcm1s1l/fr1Ov3006NOI9V+Pj6fT19++WXYqKtIn1c88AwsAAAAAADQ4eXn52vo0KF66qmndODAgUB8w4YNWrp0qaZMmdLgPKZNmyan06l58+aFPYxdqn04+759+yRJw4YNU8+ePfXggw+GLcs/naTACK6683nwwQfDfvZ6vWG3E0pSXl6eunbtqqqqqkAsLS2t3nRS7eitnTt36q9//Wu91yoqKlReXi5JgUbYH//4x5j5xAsjsAAAAAAAwGHhnnvu0ZlnnqnRo0frsssuU0VFhR5++GFlZWXptttua/D9vXv31v/8z//o5ptv1ldffaUf/OAHysjI0LZt2/TKK6/o8ssv14033iiHw6HHHntMU6dO1dChQzVnzhzl5+dr8+bN+uyzz7RkyRJlZmZq3Lhxuvvuu1VTU6Nu3bpp6dKl2rZtW9gyS0tL1b17d02fPl1DhgxRenq6li9frg8//DDsrxIOHz5cf//733X99ddr5MiRSk9P19SpU3XJJZfoxRdf1M9+9jOtXLlSJ510krxerzZv3qwXX3xRS5Ys0YgRIzR06FBdeOGFevTRR+V2uzVmzBitWLFC//3vf1t6NRwSGlgAAAAAAOCwMGHCBL311luaO3eufv/73yshIUGnnHKK7rrrrnoPbI/mN7/5jY455hg98MADmjdvnqTa50hNnDhR55xzTmC6SZMmaeXKlZo3b57uu+8++Xw+9e7dWz/96U8D0zz//PO6+uqr9ac//UnGGE2cOFFvvvmmunbtGpgmNTVVV155pZYuXRr4K4h9+vTRo48+qp///OeB6a688kp9/PHHevLJJ/XAAw/oqKOO0tSpU+VwOPTqq6/qgQce0NNPP61XXnlFqamp6tWrl6699tqwWyH/93//V7m5uXruuef06quv6rTTTtPrr79ui+dkWabuWLV2oKSkRFlZWXK73crMzIx3OgAAAPhee3veTXvKtz3lKknvLbHHb+wlafSkPjFfb2+fbXvKtz3leriorKzUtm3b1LNnTyUnJ8c7HXQgDW1bze3l8AwsAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAADjPGmHingA6mtbepZjewPvvsM51//vnq1auXUlNT1blzZ40bN06LFy+uN+2mTZs0efJkpaenKycnR5dccom+++675qYAAAAAAAAaISEhQZJ08ODBOGeCjqa8vFyWZQW2sZbmau4Mtm/frtLSUs2aNUtdu3bVwYMH9Y9//EPnnHOO/vKXv+jyyy+XJO3YsUPjxo1TVlaW5s+fr7KyMt1777369NNPtXbtWiUmJja7GAAAAAAAEJ3T6VR2drb27t0rSUpNTZVlWXHOCu2VMUYej0clJSUqKSlRdna2nE5nqyyr2Q2sKVOmaMqUKWGxX/ziFxo+fLjuv//+QANr/vz5Ki8v10cffaQePXpIkkaNGqUzzjhDCxcuDEwHAAAAAABaT5cuXSQp0MQCmsvpdCo/P19ZWVmttoxmN7AicTqdKigo0IcffhiI/eMf/9DZZ58daF5J0oQJE3TMMcfoxRdfpIEFAAAAAEAbsCxL+fn5ysvLU01NTbzTQTvncrnkdDpbfSRfizWwysvLVVFRIbfbrddee01vvvmmLrjgAknSzp07tXfvXo0YMaLe+0aNGqU33nijpdIAAAAAAACN4HQ6W+12L6CltVgD64YbbtBf/vIXSZLD4dC0adP0yCOPSJJ2794tScrPz6/3vvz8fBUXF6uqqkpJSUkR511VVaWqqqrAzyUlJZIkj8cjj8cTWKbD4ZDP55PP5wtM6497vd6wJ+JHi/u7hv75hsYlyev1NirucrlkjAmLW5Ylp9NZL8docWqiJmqiJmqiJmqipvZWkzHffxEy4XHLUVtTeNyS5XDKGJ9kfA3HLYcsyxE97vNKCubu8zVcU/hiI+ceLd7SNXk8sdeT8UWvVVZtTcYXvp5aqyaPp+Ftz4TV//18LKtF4t8n36h47ecbe38KLqJltr3mrKfQXS3afia1/f4ULW5M7GNE7fSRaw0Lt8ExgmM5NVFTfGuqW1dTtVgD67rrrtP06dO1a9cuvfjii/J6vaqurpYkVVRUSFLEBlVycnJgmmgNrAULFmjevHn14uvWrVNaWpokKTc3V71799a2bdvC/rJh9+7d1b17d23ZskVutzsQ79Wrl/Ly8rRhw4ZAfpLUr18/ZWdna926dWEre/DgwUpMTFRhYWFYDiNGjFB1dbU++eSTQMzpdGrkyJFyu93avHlzIJ6SkqIhQ4aoqKhIW7duDcSzsrLUv39/7dq1Szt27AjEqYmaqImaqImaqIma2ltNSh0h461WTVGwJstyKrHLSJlqt2qKgzVZrhQl5g6Rr6JIHnewJkdSlhJy+stbtkvesmBNzpRcubJ7y+veJm9FsCZnene5MrrLc2CLfFXBmoq6NFxT9YFgTQmdB8tyJqp6T3hNiUe2TU2FhbHXU3Wp5MrqJWdqnmr2bZDxBGtKyOknKylbNXvXyZjWr6nwYMPbXoV3v6p9ZYF4sjNLyc5slXuK5DHB3FOcnZTkTFeZ51t5TfBWpjRXnhKsFJXU7JRR8MtTRkK+HHLJXfNNWE1ZCQXyyaPSmt3B3OVQVmJBg/uT77tySZLLSlF6Qp4qvQdU6Q1uS4mOdKW6OumgZ1/Emspq9kasqbRmV/2aHClyV38TtabCg2mBeLRjREbxEarxVajcE3x+kdNKUEZCV1V5y1Th3ReIt3ZN7h7DYx4j4rU/RTpGcCynJmqKb03+wUiHyjKhrbEWNHHiRB04cEAffPCBPvroI40cOVJPP/20LrnkkrDpbrrpJt1zzz2qrKxs0gisgoIC7du3T5mZmZLoeFITNVETNVETNVETNdmhphWb7DMC64xBDde0YmPoYuM7Auv0/rHX04qN0Wtt6xFYpw9oeNtb89aW8GXGcQTWiRN7x9yf1i7fGjZ97WceaSRX648qGzWhVyAabT/7cMVXMXJsarx5uY+e1DfmMWLpp/YZgXV6f47l1ERN8ayppKREnTp1ktvtDvRymqJVHuIuSdOnT9cVV1yhLVu2BG4d9N9KGGr37t3KycmJ2rySakduRXrd5XLJ5Qovwf+h1eVfsY2N153vocQty4oYj5ZjU+PURE3R4tRETRI1RcuxqXFqoiaJmqLlGCkeeH6rFbmmyHGHZNXPsclxR3ju/rJj1RRhNhFzjBZvyZpcrtjrKfRtdWsNxhufe7R4Y2oKXe3RtjEr4ofbcvFg06fheEP7U91lWJYVZT6tX1OkPKMdI6LV2rR483K3vt/pox0jmrJNtvYxgmM5NUWLU1Pb1BQt/8aKduRsNv+QMbfbrW7duik3N7f+EHNJa9eu1dChQ1srDQAAAAAAALRzzR6BtXfvXuXl5YXFampq9PTTTyslJUUDBgyQJJ133nl66qmn9M0336igoECStGLFCm3ZskW//OUvm5sGAAAAAADNsnRDvDMImjgo3hkA9tLsBtYVV1yhkpISjRs3Tt26ddO3336r5557Tps3b9Z9992n9PR0SdItt9yiRYsWafz48br22mtVVlame+65R8cdd5zmzJnT7EIAAAAAAADQMTW7gXXBBRfob3/7mx577DHt27dPGRkZGj58uO666y6dc845gekKCgr0zjvv6Prrr9dvfvMbJSYm6qyzztJ9990X8/lXAAAAAAAAOLw1u4E1c+ZMzZw5s1HTDhw4UEuWLGnuIgEAAAAAAHAYabWHuAMAAAAAAAAtgQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsrdkPcQcAAADQ+jJ2/jfeKQQN6hPvDAAAhxlGYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWXPFOAAAAAAAANM3SDfHOIGjioHhngMMBI7AAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrrngnAAAAgNiWboh3BkETB8U7AwAAcDhiBBYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABszRXvBAAAAAAAQMe2dEO8MwiaOCjeGeBQMAILAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALbmincCAAAAAAAAdrF0Q7wzCJo4KN4Z2AcjsAAAAAAAAGBrjMCyCTq8AAAAAAAAkTV7BNaHH36oX/ziFxo4cKDS0tLUo0cPzZgxQ1u2bAmbbvbs2bIsq95//fr1a24KAAAAAAAA6MCaPQLrrrvu0r///W+df/75Gjx4sL799ls98sgjGjZsmN5//30NGhQczpOUlKQnnngi7P1ZWVnNTQEAAAAAAAAdWLMbWNdff72ef/55JSYmBmIXXHCBjjvuON1555169tlngwtzuXTxxRc3d5EAAAAAAAA4jDS7gTVmzJh6sb59+2rgwIHatGlTvde8Xq/Ky8uVmZnZ3EUjTnheFwAAAAAAaEut8lcIjTHas2ePOnfuHBY/ePCgMjMzlZWVpZycHF111VUqKytrjRQAAAAAAADQQbTKXyF87rnntHPnTt1+++2BWH5+vm666SYNGzZMPp9Pb731lh599FGtX79eq1atkssVPZWqqipVVVUFfi4pKZEkeTweeTweSZLD4ZDD4ZDP55PP5wtM6497vV4ZYxqMO51OWZYVmG9oXKodQdaYuMvlkjEmLG5ZlpxOZ70cLcuS5JQxPskE47IcsixH9LjPK8k0Il5bk/GF1ySrNneZ8NyNiV1T7fwDM5HliJB7tHgL19TW6ylSvL1ve9RETdRETdRk/5pqT5nxPef6ryP8pUXL3X8dUff6wnLU1hQeb92afL6G11P4YiPnHi3e0jV5PLG3PWN8tfOxrO//rfD5R4l/n3yj4rW5mAbjHo+nwf2pKTm2RU2xjhGhy4j9GbR+TaHHj2j7maRGrae2qMkYE/O4F/7dQW22P0WKN+ZYXrubNe37U2vV5PHEPj9JrfedsKk1SQ2fcwPlxul7bmg8dHONdB1hfPY450q120FHuTaqe5xoqhZvYG3evFlXXXWVRo8erVmzZgXiCxYsCJtu5syZOuaYY3TrrbfqpZde0syZM6POc8GCBZo3b169+Lp165SWliZJys3NVe/evbVt2zZ99913gWm6d++u7t27a8uWLXK73YF4r169lJeXpw0bNqiioiIQ79evn7Kzs7Vu3bqwlT148GAlJiaqsLAwLIcRI0aourpan3zySSDmdDo1cuRIud1ubd68ORBPSUnRkCFDVFRUpK1btwbitQ+y7y9v2S55y3YE55OSK1d2b3nd2+StCNbkTO8uV0Z3eQ5ska8qWJMrq5ecqXmq2bdBxhOsKSGnn6ykbNXsXScTshMndB4sy5mo6j3hNXkHxK6pek+wJsuVosTcIfJVFMnjDtbkSMpSQk7r19TW66l///7atWuXduwI1tTetz1qoiZqoiZqsn9N1aXxP+f6ryMKD8auKeNAjnzyqLRmdyBmyaHMxALV+CpU7tkbzMVKUEZCV1V5y1Th3RfMxUpRekKeKr0HVOkN5pjoSFeqq5MOevap2hccxZ/szFKyM1tlNXvlMcHci7oc1+B6qj7Q8LVR4pEjZLzVqikKrifLciqxy0iZardqilvm2qiwMPa2564pV4qzk5Kc6SrzfCuvqQlMn+bKU4KVopKanTIKftHISMiXQy65a74JqykroSDiespKLJDHVEZcT9W+8sB6KiwsbnB/qvDuj7ieyj1FYeupLWpq6BjhrimXFNz2qnzuiNteW9RUWFgciEc7RkhHNGo9tUVNbndezONevPanSMe9xhzLq0ub/v2ptWoqPBj7/CS13nfCptYkNXzOrS5t3Hpqi5r857Jo1xE1FfY450q120FHuTbyD0Y6VJYJbY0107fffquTTjpJNTU1ev/999W1a9eY01dUVCg9PV1z5syp99cJQ0UagVVQUKB9+/YFnqVl99+cSrE7nis22WcE1sTjYte09FP7jMA6rR+/tacmaqImaqKmjl/Tio1SvM+5/uuI0wfEzn3t8m3f/6slRoY0b8TIiRP7NLieaj/bYK21qcdnxMjp/WNve2uXb41aa1uPwBo1oVeD+9Oat7Y0OsfWrunEib1jHiNqP9vGfAatPwJr1IRegWi0/ezDFV/ZZgTW6El9Yx73wr87KK4jsE7v3/CxfMVG2WYE1ukDYp+flm+0zwisSYMbPucGjrc2GIHlP5dJka8jVmy0xzlXqt0OOsq1UUlJiTp16iS3231Iz0VvsRFYbrdbZ555pg4cOKDVq1c32LySajuAnTp1UnFxcczpkpKSlJSUVC/ucrnq3Xro/9Dq8q/Yxsaj3dLYlLhlWRHj0XK0LIdkNSHuiJx79HiU1W2Fx63vz5/Raoo0nybn3kI1xWM9NTXeHrY9aqKmaDk2NU5N1CRRU7QcmxoPrSn0lBmvc67//F831bq5W/4LicAX8rqvtUQ88mNc68b96zLWeoo4KyvyeooUtywrSrzp68nlir3thdbX2M8g5JVGxxuzPkLXe8xr2ybk2No1xTpG1F1Gc7e9Q41LkfOMdoxoy/0pWty/z0c7vjX2O0hgXi20P0WKN+ZYHna8bULu0eLNqSn0I426n7XSd8JY8Wg1NXRurVtuW3/PDY3X3VzrHiP8acX7nCuFbwft/doo1qOjGqNFGliVlZWaOnWqtmzZouXLl2vAgAENv0lSaWmpioqKlJub2xJpAAAAAAAAoANqdgPL6/Xqggsu0Hvvvad//vOfGj16dL1pKisrVVNTo4yMjLD4HXfcIWOMJk+e3Nw0AAAAAAAA0EE1u4F1ww036LXXXtPUqVNVXFysZ599Nuz1iy++WN9++62OP/54XXjhherXr58kacmSJXrjjTc0efJknXvuuc1NAwAAAAAAAB1UsxtYH3/8sSRp8eLFWrx4cb3XL774YmVnZ+vss8/WsmXL9NRTT8nr9apPnz6aP3++brzxxoj3UwIAAAAAAABSCzSwVq1a1eA02dnZeuaZZ5q7KAAAAAAAAByGGPoEAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW2v2Q9wBu1u6Id4ZBE0cFO8MAABAqIyd/413CkGD+sQ7AwAAbIsGFgAAOOzwyw0AAID2hVsIAQAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABga654JwAgaOmGeGcQNHFQvDMAAAAAAKAWDSwAANAiaMIDAACgtXALIQAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyt2Q2sDz/8UL/4xS80cOBApaWlqUePHpoxY4a2bNlSb9pNmzZp8uTJSk9PV05Oji655BJ99913zU0BAAAAAAAAHZiruTO466679O9//1vnn3++Bg8erG+//VaPPPKIhg0bpvfff1+DBg2SJO3YsUPjxo1TVlaW5s+fr7KyMt1777369NNPtXbtWiUmJja7GAAAAAAAAHQ8zW5gXX/99Xr++efDGlAXXHCBjjvuON1555169tlnJUnz589XeXm5PvroI/Xo0UOSNGrUKJ1xxhlauHChLr/88uamAgAAAAAAgA6o2bcQjhkzpt7oqb59+2rgwIHatGlTIPaPf/xDZ599dqB5JUkTJkzQMcccoxdffLG5aQAAAAAAAKCDapWHuBtjtGfPHnXu3FmStHPnTu3du1cjRoyoN+2oUaO0bt261kgDAAAAAAAAHUCzbyGM5LnnntPOnTt1++23S5J2794tScrPz683bX5+voqLi1VVVaWkpKSI86uqqlJVVVXg55KSEkmSx+ORx+ORJDkcDjkcDvl8Pvl8vsC0/rjX65UxpsG40+mUZVmB+YbGJcnr9TYq7nK5ZIwJi1uWJafTWS9Hy7IkOWWMTzLBuCyHLMsRPe7zSjKNiNfWZHzhNcmqzV0mPHdjYtdUO//ATGQ5IuQeLd7CNTVmPRlf9FotR21N4fHWq8njib3tSY1fT61dk9R+96dI8fZ+jKAmamoPNRnTuuenphz3vN7YNdnlnCvLKWMaXk+1KcX3nOuvyb8JRtvGgtutCYvX5mJaKO5TOKs2xzpxn8/X4P5k6nyWkXKPFm/pmkL370jHgtpcI9caK94aNXk8ngaPEU3JsS1qinXcC11GS2x7zakpdDuItp9JavP9KVrcGBPz/BT+3UFxvS5vzDnX/92htc5PTakp9LtDpP1Mssc5t3b7bfg6IlBuHM+5/njo5hrp2sj47HHOlWq3Aztd7zXnGrbucaKpWryBtXnzZl111VUaPXq0Zs2aJUmqqKiQpIgNquTk5MA00RpYCxYs0Lx58+rF161bp7S0NElSbm6uevfurW3btoX9ZcPu3bure/fu2rJli9xudyDeq1cv5eXlacOGDYH8JKlfv37Kzs7WunXrwlb24MGDlZiYqMLCwrAcRowYoerqan3yySeBmNPp1MiRI+V2u7V58+ZAPCUlRUOGDFFRUZG2bt0aiGdlZUnqL2/ZLnnLdgTnk5IrV3Zved3b5K0I1uRM7y5XRnd5DmyRrypYkyurl5ypearZt0HGE6wpIaefrKRs1exdJxOyEyd0HizLmajqPeE1eQfErql6T7Amy5WixNwh8lUUyeMO1uRIylJCTuvX1Jj1VF0qJR45QsZbrZqiYE2W5VRil5Ey1W7VFLdNTYUHY297UuPXU2vXJLXf/al///7atWuXduwI1tTejxHURE3toSavad3zU1OOextM7Jrscs5NPHKEKioaXk/VpfE/5/prKjxYG4+27Uk58smj0prdgYglh7ISC+QxlSr37A3mYiUoI6Grqn3lqvDuC+ZipSg9IU9VPrcqvcEcEx3pSnV1UoV3v6p9ZYF4sjNLyc5slXuK5DHB3IuKshvcn9w1JYF4RkK+HHLJXfNNWEVZCQVtUlPoZxnpGOGuKVeKs5OSnOkq83wrr6kJTJ/mylOClaKSmp0yCn7RaK2aCguLGzxGNHY9tUVNDR333DXljV5PrV1TYWFxIB7tWC4d0eb7U7Sa3O68mOcn3/Z3GrWeMhMLVOOriFhTlbcsYk2V3gMRazro2Rexpi3OmgbPuQlbdyivuFIp1T59fWSKjGUFps8vqpDLa/TNkalhNRXsOSiP09LuzinBmoxRjz0Vqkh0aG9OciCe4PGpa1GlSlNcKs4KPoonucqrI/dX6UB6gtzpCZKkwoPdY15HSPY451quFEkNX0dUl9bG43nO9dfkP5dFuzaqqbDHOVeq/Q5pp+u95lzD+gcjHSrLhLbGmunbb7/VSSedpJqaGr3//vvq2rWrJKmwsFAjR47U008/rUsuuSTsPTfddJPuueceVVZWNmkEVkFBgfbt26fMzExJ7f833Cs22ee3wROPi13T0k/tMwLrtH4Nr6cVG6PX2tYjsE4fEHvbW/ZZ/H/T48990nHtd3863EfBUBM1xaumFZvsMwJrwsDYNS351B7nXFlOTRzU8HpasVGK9znXX9PpA2rD0baxtcu3ff+v+I/AOnFinwb3p7XLt4bNJ1LuzR2t1NiaRk3oFYhFOhbU5mqPEVijJvRq8Bix5q0tjc6xtWs6cWLvmMe90O0g3iOwQreDaPvZhyu+ss0IrNGT+sY8P7235IuotTY/96bVNGpCzwbPudsefl6Wqc3SZ9WZy/dvNY2MO0xtdoca73n1RTGvI5ZvtMc5V7I0aXDD1xG157KQHOM4Ast/LpMiXxut2GiPc65Ue9610/Vec65hS0pK1KlTJ7nd7kAvpylabASW2+3WmWeeqQMHDmj16tWB5pUUvHXQfythqN27dysnJydq80qqHbkV6XWXyyWXK7wE/4dWl3/FNjZed76HErcsK2I8Wo6W5VDtrVuNjDsi5x49HmV1W+Fx/y8ZotUUaT5Nzr2FamrM+ghbjBW5psjxlq8pNN1o215j11OseEvV1J73p6bGqYmaosWpqfFx//mjtc5PseJ1j3v+j8/u59zaZTa8nkJTitc5119T3VTr5m4FRivU+WYWeK0l4pEf41o37l/3sfanyPOqv8xo8ZasKdJ2EJp7aK6N/QxCXml0vDG5h+Yacz9rQo6tXVOs417dZTR32zvUuBQ5z2jHiLbcn6LF/ft8tPNQU9Zfa9fUmHOuI6SX4DARJpYCDavGxK1mxBu1n9ngnNtQjoH9rM5L8Tjn+uN1N9e6xwh/WvE+50rh5107XO/5Hco1bLT8G6tFGliVlZWaOnWqtmzZouXLl2vAgAFhr3fr1k25ubkRhphLa9eu1dChQ1siDQAAAAAADgvv7nw53ikETBw0Ld4p4DDQ7AaW1+vVBRdcoPfee0///Oc/NXr06IjTnXfeeXrqqaf0zTffqKCgQJK0YsUKbdmyRb/85S+bmwYAAB3O0g3xziBo4qB4ZwAAAIDDWbMbWDfccINee+01TZ06VcXFxXr22WfDXr/44oslSbfccosWLVqk8ePH69prr1VZWZnuueceHXfccZozZ05z0wAAAAAAAEAH1ewG1scffyxJWrx4sRYvXlzvdX8Dq6CgQO+8846uv/56/eY3v1FiYqLOOuss3XfffTGffwUAAAAAAIDDW7MbWKtWrWr0tAMHDtSSJUuau0gAAAAAAAAcRqL9SQgAAAAAAADAFmhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZc8U4AQPu1dEO8MwiaOCjeGQAAAAAAWgsjsAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrPMTdJjJ2/jfeKQQN6hPvDAAAAAAAAAIYgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABb4yHuAIDDytIN8c4gaOKgeGcAAAAAtA+MwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK254p0AAAAAAADo2D7euzLeKQRM1Ph4p4BDwAgsAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYmiveCaD9ydj533inEDSoT7wzAACg1XHuBQAAhztGYAEAAAAAAMDWGIEF4LCwdEO8MwiaOCjeGQAAAABA+8IILAAAAAAAANgaI7AAAM3C6DYAAAAArY0RWAAAAAAAALC1FmlglZWVae7cuZo8ebJycnJkWZYWLlxYb7rZs2fLsqx6//Xr168l0gAAAAAAAEAH1CK3EBYVFen2229Xjx49NGTIEK1atSrqtElJSXriiSfCYllZWS2RBgAAAAAAADqgFmlg5efna/fu3erSpYsKCws1cuTI6At0uXTxxRe3xGIBAAAAAABa1Jb9hfFOIWCiRsQ7BdtokVsIk5KS1KVLl0ZP7/V6VVJS0hKLBgAAAAAAQAfX5g9xP3jwoDIzM5WVlaWcnBxdddVVKisra+s0AAAAAAAA0E60yC2EjZWfn6+bbrpJw4YNk8/n01tvvaVHH31U69ev16pVq+RyRU6nqqpKVVVVgZ/9o7c8Ho88Ho8kyeFwyOFwyOfzyefzBab1x71er4wxDcadTqcsywrMNzQu1Y4ea0zc5XLJGBMWtyxLTqezXo6WZUnS93mYsPlYlkPG+BSu9uH3LRGvFb5M/+cRraa686nNMVrurVtTY9aT8UmynN//EF6T5aitKTxuyXI4a5cZttwoccsRrClS3OcNfAYeT+xtT7JkfOE1Rcu9tWuSGt6fAm+JUKs/R8tqm5r8m0K0/cyYxq+n1q7J42n6MSJS3C7HPf/H2db7U6S4v4RYNdUeltp2f4pWk9TAevLFZ3+KFPd4Gt72AvtZG+5P0WryemPvTy297TWnJmMavo7wnwfjec71x/37VbRjRHB7bkqOrVOTz+dr8Lhn6mzzkXKPFm/pmkKPWZGO2bW5tsz1XnNr8ng8DZ6f2voatqGaYp1zQ5fRlvtTpNxDt4No+5kU67tD2x4jjDExryMau/7a4hjRmGsjnyVZpjZLn1VnLt+/1TQy7jC12R1q3OPxxLzeC122n6ktt2lxBddKg3Gr9sW6cUkNXsNa/mNZ7YuSMWHz8cctE57kIcUbqCl0e410XS5jQnI0IfOw2iRuhWzDHo+n1fsRbfVdo+5xoqnatIG1YMGCsJ9nzpypY445RrfeeqteeuklzZw5M+r75s2bVy++bt06paWlSZJyc3PVu3dvbdu2Td99911gmu7du6t79+7asmWL3G53IN6rVy/l5eVpw4YNqqioCMT79eun7OxsrVu3LmxlDx48WImJiSosDL8XdsSIEaqurtYnn3wSiDmdTo0cOVJut1ubN28OxFNSUjRkyBAVFRVp69atgXjtQ+wTVOVzq9IbzDHRka5UVydVePer2hccpZbszFKyM1vlniJ5TDD3FGcnJTnTVeb5Vl5TE4inufKUYKWopGanjIIbXkZCvhxyyV3zTVhNXm+vmDWFTu+0EpSR0FXVvnJVePcF4i4rRekJea1eU2PWk++7cmUlFMgnj0prdgfilhzKTCxQja9C5Z699Wqq8pZFrKnSeyBiTQc9+yLWVFazN1BT4cG0mNuelK2avetkQr7gJHQeLMuZqOo94dte4pEjZLzVqikKrifLciqxy0iZardqioPbnuVKUWLuEPkqiuRxB7c9R1KWEnL6y1u2S96yHcHPICVXUsP7U3Xp959NVi85U/NUs2+DjCdYU0JOP1lJbVNT4cHaeFZWlvr3769du3Zpx45gTV5PrlzZveV1b5O3IliTM727XBnd5TmwRb6q4HptzZrWVTX9GBGpJrsc96pLW3bba8568m8HsWqSafv9KVpNUuz1VL03PvtTpJoKCxve9rym7fenaDVtMLH3p5be9ppTU0VFw9cR7pryuJ9z/dcRhYXFkqIfI6SciOfcrMQCeUxlxHNua9VUVJTd4HHPXRN8rEW0a6No1xEtXVPoZxnpWO6uKW+x673m1lRYWNzg+amtr2Fj1dTQOdddU97o9dTaNfn3MSn6dw3piDbfn6LV5HbnxbyOiNf+FKmmxlwbHTwyVXnFlUqp9mlHXoqMFWyD5BdVyOU1+ubI1LCaCvYclMdpaXfnlGBNxqjHngpVJjq0Nyc5EE/w+NS1qFJlKS4VZyUGc6zy6sj9VXKnJ8idniBJ2ldYGPN6T5K6eCylhnTC9jp9KnVK3T2WEkPiu1w+VVjS0TWWHCGtna8TfPJI6lUTfnPW1gSfXJJ6hMR9MtqWaJRipK6eYLz6+65YQ9ewXb//jMtdTh1ITFJ2TbXSPMFtpiQhQaUJCcqprlKyN7h/7E9M1EGXS7lVlUoI+eVeUVKSqpxOdamskCOkh7UnOVleywosL/AZpKTIaYyOrKwMHG+jfXc/4mCZ9qdlK8lTpYzK8mCtzgSVpGYqtbpCqdXB+VcmJKksOV3pVeVKrgkOvjmYmKKDSanKrChVoje435Qmp6kqIVlHHHTL6Qt+Bu6UDNW4EpVTfiDQmCssLGz1fkRbfddo7qOkLGPqtCubyf8Q9yeffFKzZ89ucPqKigqlp6drzpw59f46oV+kEVgFBQXat2+fMjMzJdlnJIJfUzuea5dvs80IrNGT+sas6b0</t>
+  </si>
+  <si>
+    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACTOElEQVR4nOzdeXhU5fn/8c+ZmWwQEgwEWRKQfV9UQMEFUGRTsLIIbizSn3WlVqtWbWuxFbRS99pq/RZcsBbButWFpWCpG0ZRQMBoWcqOITIhkG1mnt8fcSaZZGYyIcucwffrurg095w5577n7HeeObGMMUYAAAAAAACATTlinQAAAAAAAAAQCQ0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAGpp+vTpsixL06ZNi2r6hx9+WJZlqVevXg2cWc2GDx8uy7K0Zs2amCx/5syZsixLixYtisny60usP8cfklNOOUWWZWnHjh2xTgUAAMQQDSwAAGpp9uzZkqRXX31V3333XY3TL1y4MOh9DeU3v/mNLMvSb37zmwZdzokunj7HxmykrVmzRpZlafjw4Q2+LAAAgKpoYAEAUEvnnnuuunTpopKSEi1evDjitJ988ok2btyohIQEXXXVVY2UYXjPPfectmzZosGDB8c6lbjG5wgAANC4aGABAFBLlmXp6quvllQxuioc/+sXXXSRWrVq1eC51aR9+/bq0aOHmjRpEutU4hqfIwAAQOOigQUAwHGYOXOmnE6nPvvsM23YsCHkNMXFxfrb3/4mqfrXBz/99FNdccUVat++vZKSkpSRkaHRo0frrbfeCjmvys8Beu2113TeeecpIyMj8PUxy7I0d+5cSdLcuXNlWVbg38yZMwPzqekrZ//61780ZcoUZWVlKSkpSZmZmRo0aJDuueceHTp0KDBdWVmZXnjhBV1xxRXq0aOH0tLSlJKSou7du2vOnDnau3dvtB9ljRYtWhSo49ChQ7rhhhsCn1uHDh30s5/9LOxXOV955RX9+Mc/Vp8+fXTSSScpOTlZHTt21NVXX62vvvqq2vT19TmuWrVKEydOVJs2bZSYmKhWrVrpkksu0Ycffhhyev8yJGnZsmU6++yzlZaWpqZNm+qss86qtl341/l7770nSRoxYkRQrpWfMfbpp59q6tSpysrKUmJiotLS0tSpUydNmjRJr732Wsh8qho+fLhGjBghSXrvvfeClnXKKacETevxePTnP/9ZQ4cOVXp6upKTk9W1a1fNmTNHe/bsiWp54fzjH/8IfDbNmjXT8OHDw+4zfkuXLtWYMWOUmZmpxMREtWvXTldeeaU2b95c6+V//fXXuvrqq9WxY0clJSUpNTVVHTp00IUXXhi2mZ2bm6uf/OQn6ty5s5KTk5Wenq5zzz1XL7zwQr3lvWPHjsC6MMbo6aef1umnn66mTZsqPT1do0aNCrvtAQAQNwwAADgu48ePN5LMnDlzQr6+ePFiI8m0bdvWeDyeQPyRRx4xDofDSDIDBgwwkydPNmeffbZJTEw0kszcuXOrzatDhw5GkrnxxhuNJDNw4EBz2WWXmWHDhpl///vfZsaMGaZ///5Gkunfv7+ZMWNG4N9f/vKXwHyGDRtmJJnVq1dXW8ZNN91kJAXymjZtmhk7dqzp1KlTtffs2rXLSDLp6enmzDPPNFOmTDHjxo0zbdu2NZJMZmam+frrr6stY8aMGUaSWbhwYdSf88KFC40kM2HCBNO5c2fTvHlz86Mf/chccskl5qSTTjKSTPfu3c3BgwervdfpdJomTZqYgQMHmokTJ5oJEyYE6mnatKl5//33q+VX18/x1ltvNZKMw+EwgwcPNlOmTDFnnHGGsSzLOJ1O89e//rXae/yf+69//WtjWZY566yzzNSpUwO5WJZlXnnllcD0W7ZsMTNmzDAnn3yykWRGjx4dlOvatWuNMcasXLnSJCQkBOqZPHmyueSSS8zgwYNNUlKSufjii6NaB/PnzzejR482kszJJ58ctKxbb701MF1xcbEZOXKkkWSSk5PN2LFjzdSpU012draRZFq2bGk+/fTTqJbp59/2f/aznwVt+4MHDw58bo899li195WVlZlLL73USDJJSUlm6NChZsqUKYHPNCUlxbz99ttR57Fx40aTlpYW2N4mTpxopkyZYoYMGWJSU1NN//79q71nyZIlJjk52UgyPXr0MJdccok577zzTNOmTY0kM2vWrHrJe/v27UaS6dChg5kxY4ZJSEgw5513nrn00ktNt27dAvP66KOPoq4XAAC7oYEFAMBxevXVV40k06JFC1NSUlLtdf+N/F133RWIvfPOO8ayLNOyZUvz3nvvBU2/YcMGk5WVZSSZNWvWBL3mv4l3Op3mtddeC5nPPffcYySZe+65J2zO4Rovjz32WKCWf/3rX9Xe9/HHH5v//e9/gZ8LCgrMa6+9Vq3u0tJSc+eddxpJZty4cdXmU5cGliRz5plnmkOHDgVe++6778zQoUONJDNt2rRq733ppZdMYWFhUMzn85k//vGPRpLp3bu38fl8Qa/X5XN8+umnjSTTpUsX88UXXwS99t5775lmzZqZxMREk5ubG/Sav77mzZtXazL48+nWrVvUefiNGDHCSDIvvPBCtdcOHz5sPvzww7A1VrV69WojyQwbNizsNHfccYeRZDp37my2b98eiJeWlprZs2cbSaZjx44h95dw/Nu+ZVnV6njppZeMZVnG5XKZjRs3Br121113GUnmjDPOMNu2bQt67eWXXzZOp9OcdNJJ5rvvvosqj1mzZhlJ5ne/+121144dOxZyf05KSjLJyclm2bJlQa/t2LHD9O3b10gyzz77bJ3z9jew/E2sr776KvCax+MxV199tZFkRo0aFVWtAADYEQ0sAACOU1lZmWndurWRZF5++eWg13bu3BkYZVV5JNIZZ5xhJJmlS5eGnOeSJUuMJDNp0qSguP8m/uqrrw6bz/E2XsrKykxmZqaRVO1G+3i1bdvWOBwOU1BQEBSvawNr/fr11V7fsGGDsSzLOBwOs2vXrqjnO2TIECPJfPnll0Hx4/0cvV5vYARaTk5OyPf9/ve/N5KCRi0ZU9HACjWSqLi42KSnpxtJQU3EcHlU1qtXLyPJ5Ofnh60lWjU1sIqKikxqaqqRZF5//fVqrx89ejQwYmzx4sVRL9e/7f/oRz8K+fqkSZOMJPP//t//C8QOHTpkUlJSTHJystm9e3fI911//fVGknn88cejymPcuHFGkvnss8+imn7q1KlGklmwYEHI19etW2ckmdNPP73OeVduYIX67Pft2xcYhVVaWhpV/gAA2A3PwAIA4Di5XC7NmDFDkvTXv/416LWFCxfK5/Np2LBh6tKliyQpLy9P69atU0pKisaPHx9ynsOHD5ckffDBByFfnzx5cj1lX+HTTz/Vt99+q5YtW+qSSy6p1Xu/+OILPfTQQ7rpppt09dVXa+bMmZo5c6Y8Ho98Pp+++eabesuzf//+GjBgQLV43759deqpp8rn8+nf//53tde/+eYbPfHEE7r55ps1e/bsQI4HDhyQpJDPwjoe69ev1969e9W5c2edfvrpIaepaf2G2i6SkpLUqVMnSar1M6T8fyXxiiuu0H/+8x95PJ5avb82cnJyVFhYqIyMjJB1NGnSRNOmTZMkrV69utbz9+9r4eKVn0e2evVqFRUV6ayzzlK7du1Cvq+mdVGV/7O87rrr9O6776q4uDjstD6fT2+//bYkaerUqSGnGThwoFJTU7V+/frAvOqat8vl0pgxY6rFW7durZNOOkklJSVBz7IDACCeuGKdAAAA8ezqq6/WAw88oOXLl2vPnj1q166djDGBh2hXfnj79u3bZYxRUVGRkpKSIs7322+/DRmv+sDs+rBz505JUvfu3QMPEq/J0aNHddVVV+kf//hHxOkKCgrqnJ9fx44dI7722Wefaffu3YGY1+vVjTfeqKeeekrGmAbPcdu2bZKk//73vzV+juHWb/v27UPG09LSJCli0ySU+fPna8OGDXr77bf19ttvKyUlRaeddpqGDx+uK664Qj179qzV/CLxN9cirafOnTsHTVsb4ebrj1de9/51sWrVquNeF1Xddttt+s9//qOVK1dqzJgxSkhIUP/+/XXuuedq2rRpGjRoUGDaQ4cOBbar7OzsGud96NAhtWvXrs55t2nTRgkJCSGnT0tL03fffVfrbQgAALuggQUAQB1069ZN55xzjtauXavnnntOd955p1avXq0dO3YoPT09aMSUz+eTJKWmpmrSpEnHtbyUlJR6ybuu7rzzTv3jH/9Qjx49dP/992vQoEFq2bKlEhMTJUlDhw7Vhx9+GLFx1BAqL+/RRx/Vn//8Z7Vu3VoPPfSQhg4dqpNPPlnJycmSpMsvv1x/+9vf6i1H//pt3bq1Ro8eHXHali1bhow7HPU7OL5169bKycnRe++9p5UrV+r999/Xxx9/rPfff1/z5s3T/Pnzdccdd9TrMmOl8nr0r4suXbrorLPOivi+Hj16RDX/Jk2aaMWKFfrkk0/0zjvv6IMPPtAHH3ygnJwcPfTQQ7r++uv1xz/+MWj5UviRY5X5G9p1zbu+tx8AAOyEBhYAAHU0e/ZsrV27VgsXLtSdd94Z+DrhtGnTghpO/pEYlmXpr3/9q21uNv2jfnJzc2WMiWoU1pIlSyRJf//739WvX79qr3/99df1m6TKR7CFs2PHDklSVlZWIObP8amnntKECROqvae+c/Sv3xYtWgRG4NmBZVkaPnx44KtnxcXFWrRokW644Qbdddddmjx5cmBkVF34v/IWaT35RxiF+3pcJNu3b1f//v2rxUOte/+66N69e72vi0GDBgVGW3k8Hr366quaPn26nnzySU2ePFkjRoxQy5YtlZKSoqKiIi1YsCBsw7KqhswbAIB4Z48rZwAA4tiUKVOUlpamr7/+Wm+++aZeeeUVScFfH5Sktm3bql+/fjpy5Ijeeeedes/DP/qpts85GjhwoFq2bKlvv/1Wr776alTvyc/PlyR16NCh2mvvvvuu8vLyapVDNDZs2KANGzZUi3/55Zf67LPP5HA4dO6550aV45dffqnPP/885HKO93P0j0LbvHmzvvzyy1q993gdT67Jycm69tpr1a9fP/l8vpCf6fEsy/9Mp/z8fL3++uvVXi8qKtJLL70kSRoxYkTU+fo9//zzIePPPfecpIpnQ0nS+eefr8TERK1Zs0YHDx6s9bKi5XK5NHny5MCIO/825XQ6dcEFF0iqaKRGo7HyBgAgHtHAAgCgjpo0aaLLLrtMUvkzsYqKitS3b9+gZ+L4/e53v5MkzZo1S2+88Ua1140x+vjjj7V8+fJa5+EfgVLb5onL5dLdd98tSbrmmmtCPgj9k08+CXrGkP/ZSY8//njQdF999ZWuvfbaWi0/WsYYXXfddfruu+8CMbfbreuuu07GGE2aNCnoeUP+HP/4xz8GfaVr3759mj59ethGzPF+jgkJCbrnnntkjNEll1yi//znP9Wm8Xq9+te//qWPPvqoVvMOp6ZcFyxYoP/973/V4lu3bg2MQAvV4Iu0rK+//lplZWXVXk9OTtYNN9wgSbr11lsDz1aTpLKyMv30pz/V/v371bFjx+P6YwT/+Mc/Ag0wv6VLl2rZsmVyuVy66aabAvGTTz5ZN910k44eParx48dr48aN1eZXUlKi119/XVu3bo1q+U8++WTIB/7v379fOTk5koI/y3vuuUeJiYm67bbb9OyzzwZtg36bNm0KNLwbKm8AAE4YsfnjhwAAnFjWrVsX+DP2kswjjzwSdtpHH33UuFwuI8l06dLFXHjhhebyyy83F1xwgWnVqpWRZO64446g93To0MFIMtu3bw873/3795umTZsaSeass84yM2fONLNnzzZ//etfA9MMGzbMSDKrV68Oeq/P5zPXXnttIP9TTz3VTJs2zYwbN8506tSp2nuWLVtmLMsykkzfvn3NtGnTzHnnnWcSEhLMeeedZ4YOHRpyOTNmzDCSzMKFC2v6SAMWLlxoJJkJEyaYTp06mebNm5tLLrnETJw40WRkZBhJpmvXrubAgQNB7/voo49MYmJi4HO+9NJLzZgxY0xKSorp3bu3ueSSS0LmUpfP0RhjbrvttsDn2Lt3b3PxxRebadOmmeHDh5vmzZsbSeZPf/pT0Hv804cTbnlvvvmmkWQSExPNRRddZK6++moze/Zs8/777xtjjElPTzeSTI8ePcwll1xiLr/8cjN8+PDA9jd9+vQo1kCFgQMHGkmme/fu5oorrjCzZ88O2laLi4vN+eefbySZlJQUM27cODN16lTTvn17I8m0aNHC5OTk1GqZ/m3/5ptvNpLMoEGDzOWXX27OOOOMwOf20EMPVXtfWVmZufzyy40k43A4zKmnnmomTZpkpk6das4666zAOn777bejyqN///5GkunYsaMZP368ueKKK8yoUaNMSkqKkWTOO+88U1ZWFvSeJUuWmCZNmhhJJisry4waNcpcccUVZuzYsSYrK8tIMlOnTq1z3tu3bzeSTIcOHWr8HCMdQwAAsDMaWAAA1JO+ffsGmgl5eXkRp924caO55pprTNeuXU1ycrJp0qSJ6dSpkxk9erR57LHHzJ49e4Kmj/bm89///rcZOXKkOemkk4zD4TCSzIwZMwKvR2q8GGPM22+/bS6++GJz8sknm4SEBJOZmWkGDx5s5s6daw4dOlRtWeeff75p2bKladKkienTp4+57777TElJSdjl1KWBNWPGDHPw4EHzk5/8xGRlZZnExESTnZ1t5syZUy03vw0bNpgJEyaYNm3amOTkZNO1a1dz++23m4KCgoi51PVzfP/9980VV1xhOnToYJKSkkyzZs1Mt27dzI9+9CPzzDPPmPz8/KDpj7eBZYwxf/nLX8xpp50WaJRUrumFF14ws2bNMn369DEZGRkmKSnJdOjQwYwdO9b84x//MD6fL+wyQ9m5c6e5/PLLTZs2bQJNsKpNk7KyMvPkk0+aM8880zRr1swkJiaazp07m5tuusns3r27VsszJnjbX7JkiRkyZIhJTU01TZs2Neecc4554403Ir7/rbfeMhMnTjTt2rUzCQkJpnnz5qZnz55m2rRp5sUXXzRHjx6NKo8333zTXHfddebUU081mZmZJjEx0WRlZZnhw4ebZ5991pSWloZ83/bt283PfvYz06dPH9O0aVOTnJxsOnToYIYPH27uv/9+880339Q5bxpYAIAfAsuYRv7zQAAAALWwaNEizZo1SzNmzODB1gAAAD9QPAMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2xjOwAAAAAAAAYGuMwAIAAAAAAICt0cACAAAAAACArblincDx8Pl82rt3r5o1aybLsmKdDgAAAAAAACIwxujIkSNq27atHI7aj6eKywbW3r17lZ2dHes0AAAAAAAAUAu7du1SVlZWrd8Xlw2sZs2aSSovOi0tLcbZAAAAAAAAIJKCggJlZ2cHejq1FZcNLP/XBtPS0mhgAQAAAAAAxInjfRQUD3EHAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3F5V8hBAAAAAAAjc8YI6/XK4/HE+tUYBMul0tOp/O4/7pg1Mtp0LkDAAAAAIC4Z4zR4cOH9e2338rr9cY6HdiM0+lUq1atlJ6e3mCNLBpYAAAAAAAgov379+vw4cNKS0tTWlqaXC5Xg4+4gf0ZY+TxeFRQUKB9+/apqKhIbdq0aZBl0cACAAAAAABheb1eud1uZWZmqmXLlrFOBzbUrFkzJSUlKS8vT61atZLT6az3ZfAQdwAAAAAAEFZZWZmMMWratGmsU4GNNW3aVMYYlZWVNcj8aWABAAAAAIAa8ZVBRNLQ2wcNLAAAAAAAANgaDSwAAAAAAACENHPmTJ1yyimxToMGFgAAAAAA+OFatGiRLMsK+++jjz6KdYo12rx5s37zm99ox44dsU6lwfBXCAEAAAAAwA/evffeq44dO1aLd+nSJQbZ1M7mzZs1d+5cDR8+3BajpRoCDSwAAAAAAHDclm+KdQbSqD51n8fYsWM1cODAus8IDYKvEAIAAAAAAERwzz33yOFwaNWqVUHxa665RomJifriiy8kSWvWrJFlWfr73/+uu+66S61bt1bTpk01YcIE7dq1q9p8P/74Y40ZM0bp6elq0qSJhg0bpvfff7/adHv27NHs2bPVtm1bJSUlqWPHjrruuutUWlqqRYsWacqUKZKkESNGBL76uGbNmsD73377bZ1zzjlq2rSpmjVrpgsvvFBffvllteW8+uqr6tOnj5KTk9WnTx/94x//qMvHVq8YgQUAAAAAAH7w3G638vLygmKWZalFixb65S9/qTfeeEOzZ8/Wxo0b1axZM7377rv6y1/+ot/+9rfq379/0Pvuu+8+WZalO+64QwcPHtQjjzyikSNH6vPPP1dKSook6V//+pfGjh2r008/PdAgW7hwoc477zytXbtWgwcPliTt3btXgwcP1uHDh3XNNdeoR48e2rNnj5YuXapjx47p3HPP1Zw5c/TYY4/prrvuUs+ePSUp8N/nn39eM2bM0OjRo/XAAw/o2LFj+tOf/qSzzz5b69evD3zlcPny5Zo0aZJ69eql+fPn69ChQ5o1a5aysrIa8mOPmmWMMbFOorYKCgqUnp4ut9uttLS0WKcDAAAAAMAJq7i4WNu3b1fHjh2VnJxc7fV4/wrhokWLNGvWrJCvJSUlqbi4WJK0adMmnX766Zo+fboefPBB9enTR23atNGHH34ol6t8fNCaNWs0YsQItWvXTlu2bFGzZs0kSS+//LIuvfRSPfroo5ozZ46MMerevbs6deqkt99+W5ZlSZKKiorUu3dvdenSRcuXL5ckzZgxQy+88II+/vjjal9xNMbIsiwtXbpUU6ZM0erVqzV8+PDA64WFhcrOztaUKVP09NNPB+IHDhxQ9+7ddemllwbip556qg4cOKAtW7YoPT1dkrRixQqNGjVKHTp0qPEB8TVtJ3Xt5TACCwAAAAAA/OD98Y9/VLdu3YJiTqcz8P99+vTR3Llzdeedd2rDhg3Ky8vT8uXLA82ryqZPnx5oXknS5MmT1aZNG7311luaM2eOPv/8c3399df65S9/qUOHDgW99/zzz9fzzz8vn88nqfxrfePHjw/5fC5/4yucFStW6PDhw7rsssuCRpc5nU6dccYZWr16tSRp3759+vzzz/WLX/wi0LySpAsuuEC9evXS0aNHIy6nMdDAAgAAAAAAP3iDBw+u8SHut912m1566SWtW7dO8+bNU69evUJO17Vr16CfLctSly5dAqOYvv76a0nlo6vCcbvdKi0tVUFBgfr0Ob4hZv7lnHfeeSFf94+E2rlzZ8i8Jal79+767LPPjmv59YkGFgAAABAH7PAVHb9ovqoTb/kCQDS2bdsWaApt3LjxuOfjH1314IMPasCAASGnSU1NVX5+/nEvo/Jynn/+ebVu3bra66FGj9lV/GQKAAAAAAAQIz6fTzNnzlRaWppuvvlmzZs3T5MnT9bEiROrTetvcvkZY/TNN9+oX79+kqTOnTtLKh8BNXLkyLDLzMzMVFpamjZtivxbgXBfJfQvp1WrVhGX06FDh5B5S9JXX30VcdmNxRHrBAAAAAAAAOzuoYce0gcffKCnn35av/3tbzV06FBdd9111f5yoSQ999xzOnLkSODnpUuXat++fRo7dqwk6fTTT1fnzp21YMECFRYWVnv/t99+K0lyOBz60Y9+pDfeeEM5OTnVpvP/Xb6mTZtKkg4fPhz0+ujRo5WWlqZ58+aprKws7HLatGmjAQMG6Nlnn5Xb7Q68vmLFCm3evDni59JYGIEFAAAAAAB+8N5++21t3bq1Wnzo0KEqKSnRr371K82cOVPjx4+XVP7XCwcMGKDrr79eS5YsCXpPRkaGzj77bM2aNUsHDhzQI488oi5duuj//b//J6m8MfXMM89o7Nix6t27t2bNmqV27dppz549Wr16tdLS0vTGG29IkubNm6fly5dr2LBhuuaaa9SzZ0/t27dPL7/8sv7zn/+oefPmGjBggJxOpx544AG53W4lJSXpvPPOU6tWrfSnP/1JV111lU477TRNmzZNmZmZ+t///qd//vOfOuuss/TEE09IkubPn68LL7xQZ599tq6++mrl5+fr8ccfV+/evUM22RobDSwAAAAAAPCD9+tf/zpk/JlnntFTTz2lli1b6pFHHgnEu3btqvnz5+unP/2plixZoksvvTTw2l133aUNGzZo/vz5OnLkiM4//3w9+eSTatKkSWCa4cOH68MPP9Rvf/tbPfHEEyosLFTr1q11xhln6Cc/+Ulgunbt2unjjz/Wr371Ky1evFgFBQVq166dxo4dG5hf69at9ec//1nz58/X7Nmz5fV6tXr1arVq1UqXX3652rZtq/vvv18PPvigSkpK1K5dO51zzjmaNWtWYDljxozRyy+/rF/+8pe688471blzZy1cuFCvvfaa1qxZU0+f8vGzjH+82XH68ssv9Zvf/Eaffvqp9u/fryZNmqhXr1667bbbAl1Jvy1btuhnP/uZ/vOf/ygxMVEXXnihHnroIWVmZtZqmQUFBUpPT5fb7Q48MR8AAAA4kcXbQ9HjLV8A4RUXF2v79u3q2LGjkpOTY52Ora1Zs0YjRozQyy+/rMmTJ8c6nUZV03ZS115OnUdg7dy5U0eOHNGMGTPUtm1bHTt2TMuWLdOECRP01FNP6ZprrpEk7d69W+eee67S09M1b948FRYWasGCBdq4caPWrVunxMTEuqYCAAAAAACAE1CdG1jjxo3TuHHjgmI33nijTj/9dD300EOBBta8efN09OhRffrpp2rfvr0kafDgwbrgggu0aNGiwHQAAAAAAABAZQ3yVwidTqeys7ODnn6/bNkyXXTRRYHmlSSNHDlS3bp1q/awMwAAAAAAAMCv3h7ifvToURUVFcntduv111/X22+/ralTp0qS9uzZo4MHD2rgwIHV3jd48GC99dZb9ZUGAAAAAABATAwfPlx1fNQ4wqi3Btatt96qp556SlL5n4OcOHFi4E8x7tu3T5LUpk2bau9r06aN8vPzVVJSoqSkpJDzLikpUUlJSeDngoICSZLH45HH4wks0+FwyOfzyefzBab1x71eb9BGFC7udDplWVZgvpXjkuT1eqOKu1wuGWOC4pZlyel0VssxXJyaqImaqImaqImaqImaqMmfu/FJshyyLIeMzyup0g2SVV6T8QXXJKs8dxlvVHHLUV5TcNyS5XDKGN/3SUgeT801VZ7++5mHyb1xamLboyZqOv6aPB5PxbEoRHPGsixbxWvDbrnHc01S+fZRuVdTeduruv3VVr01sG6++WZNnjxZe/fu1ZIlS+T1elVaWipJKioqkqSQDSr/k+mLiorCNrDmz5+vuXPnVouvX79eTZs2lSRlZmaqc+fO2r59u7799tvANFlZWcrKylJubq7cbncg3qlTJ7Vq1UqbNm0K5CdJPXr0UPPmzbV+/fqgnbhfv35KTExUTk5OUA4DBw5UaWmpNmzYEIg5nU4NGjRIbrdbW7duDcRTUlLUv39/5eXladu2bYF4enq6evbsqb1792r37t2BODVREzVREzVREzVREzVRk7+m0iOSK72TnE1aqezQJhlPRU0JGT1kJTVX2cH1MpUaOAkt+8lyJqr0QHBNiScPlPGWqiyvoibLciqx9SCZUrfK8itqslwpSszsL19Rnjzu8ppyjtVck9e9Xd6iipqcqVlyNcuS53CufCUV66kxamLboyZqqntN/nt3r9er4uLiQNzhcKhJkybyeDxBA0+cTqdSUlJUVlYW6A1I5Y295ORklZSUBDU0EhMTlZiYqOLi4qAck5KSlJCQoKKioqAmXnJyslwul44dOxbUTElJSZHD4dDRo0eDamratKl8Pl/Q52JZlpo2bUpN9VSTJJWVlWnTpoo/Q1t52/MPRjpelmmgsW2jRo3S4cOH9fHHH+vTTz/VoEGD9Nxzz+mqq64Kmu7222/Xgw8+qOLi4lqNwMrOztahQ4cCf3rRLp1pvxOp205N1ERN1ERN1ERN1ERNsa9p1WbZZgTW+b1qrundjfYZgXVBb7Y9aqKmutRUXFys//3vf+rUqVPI+3ZGK1GTVN672bZtm9q3bx9oeFbe9goKCtSiRQu53e5AL6c26m0EVlWTJ0/WT37yE+Xm5ga+Ouj/KmFl+/btU0ZGRtjmlVTeyQv1usvlkssVXIJ/h63KvwNGG6863+OJW5YVMh4ux9rGqYmawsWpiZokagqXY23j1ERNEjWFy7G2cWqqW01WpZctR+iaLEeYy3sr+rhlWWHijkASlUsOl3vl6YNzDJd7w9bEtkdN1HT8NblcrvJjgxT4b1V2i9eG3XKP95pC9WpCxWqrQf4KoVTxtUG326127dopMzOz2rBESVq3bp0GDBjQUGkAAAAAAAAgztW5gXXw4MFqsbKyMj333HNKSUlRr169JEmTJk3Sm2++qV27dgWmW7VqlXJzczVlypS6pgEAAAAAAIATVJ2/QviTn/xEBQUFOvfcc9WuXTvt379fixcv1tatW/WHP/xBqampkqS77rpLL7/8skaMGKGf/vSnKiws1IMPPqi+fftq1qxZdS4EAAAAAAAAJ6Y6N7CmTp2q//u//9Of/vQnHTp0SM2aNdPpp5+uBx54QBMmTAhMl52drffee0+33HKLfvGLXygxMVEXXnih/vCHP0R8/hUAAAAAAAB+2OrcwJo2bZqmTZsW1bS9e/fWu+++W9dFAgAAAAAA4AekwR7iDgAAAAAAYHeLFi2SZVlKTk7Wnj17qr0+fPhw9enTJwaZobI6j8ACAAAAAAA/YO+8E+sMpDFj6jyLkpIS3X///Xr88cfrISHUN0ZgAQAAAACAH7wBAwboL3/5i/bu3RvrVBACI7AAAAAA/KAt3xTrDCqM4ltKQMzcdddduvzyy3X//ffrscceCzudx+PR/PnztWjRIu3evVtt2rTR5ZdfrnvuuSfwR+puueUWPfvss8rLy5NlWZKkm266SU888YQeffRRzZkzR5J04MABtW7dWk8++aSuu+66hi8yjjECCwAAAAAA/OB17NhR06dPr3EU1o9//GP9+te/1mmnnaaHH35Yw4YN0/z584P+wN0555yj/Px8ffnll4HY2rVr5XA4tHbt2qCYJJ177rkNUNGJhQYWAAAAAACApLvvvlsej0cPPPBAyNe/+OILPfvss/rxj3+sl19+Wddff72effZZ/fznP9err76q1atXS5LOPvtsSRUNKrfbrY0bN2rSpEnVGlgZGRnq1atXA1cW/2hgAQAAAAAASOrUqZOuuuoqPf3009q3b1+119966y1J5V8RrOzWW2+VJP3zn/+UJGVmZqpHjx7697//LUl6//335XQ6ddttt+nAgQP6+uuvJZU3sM4+++zA1wwRHg0sAAAAAACA7/3yl7+Ux+PR/fffX+21nTt3yuFwqEuXLkHx1q1bq3nz5tq5c2cgds455wRGW61du1YDBw7UwIEDlZGRobVr16qgoEBffPGFzjnnnIYt6ARBAwsAAAAAAOB7nTp10pVXXhl2FJakqEZMnX322dqzZ4+2bdumtWvX6pxzzpFlWTr77LO1du1affDBB/L5fDSwokQDCwAAAAAAoBL/KKyqz8Lq0KGDfD5f4CuAfgcOHNDhw4fVoUOHQMzfmFqxYoU++eSTwM/nnnuu1q5dq7Vr16pp06Y6/fTTG7iaE4Mr1gkAAAAAsbJ8U6wzqDCqT6wzAAD4de7cWVdeeaWeeuopdejQQS5Xeftk3Lhxuuuuu/TII4/oqaeeCkz/0EMPSZIuvPDCQKxjx45q166dHn74YZWVlemss86SVN7Y+vnPf66lS5fqzDPPDMwbkTECCwAAAAAAoIq7775bZWVl+uqrrwKx/v37a8aMGXr66ac1depUPfnkk5o5c6Z+//vf60c/+pFGjBgRNI9zzjlHX331lfr06aOTTjpJknTaaaepadOmys3N5euDtUADCwAAAAAAoIouXbroyiuvrBZ/5plnNHfuXH3yySe6+eab9a9//Ut33nmnXnrppWrT+htUZ599diDmcrk0ZMiQoNdRM8sYY2KdRG0VFBQoPT1dbrdbaWlpsU4HAAAAcSqevkIYT7lK8ZVvPOUKxEJxcbG2b9+ujh07Kjk5OdbpwKZq2k7q2sthBBYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAQAOxLEu/+c1vYp1G3KOBBQAAAAAAfpAsy4rq35o1a2Kd6g+eK9YJAAAAAACAOPbNN7HOQOrS5bje9vzzzwf9/Nxzz2nFihXV4j179jzu1FA/aGABAAAAAIAfpCuvvDLo548++kgrVqyoFkfs8RVCAAAAAACAMI4ePapbb71V2dnZSkpKUvfu3bVgwQIZY4KmKykp0c9+9jNlZmaqWbNmmjBhgnbv3l1tfjt37tT111+v7t27KyUlRS1atNCUKVO0Y8eOwDTbtm2TZVl6+OGHq73/gw8+kGVZ+tvf/lbvtdoZDSwAAAAAAIAQjDGaMGGCHn74YY0ZM0YPPfSQunfvrttuu0233HJL0LQ//vGP9cgjj2jUqFG6//77lZCQoAsvvLDaPD/55BN98MEHmjZtmh577DFde+21WrVqlYYPH65jx45Jkjp16qSzzjpLixcvrvb+xYsXq1mzZrr44osbpmib4iuEAAAAAAAAIbz++uv617/+pd/97ne6++67JUk33HCDpkyZokcffVQ33nijOnfurC+++EIvvPCCrr/+ev3xj38MTHfFFVdow4YNQfO88MILNXny5KDY+PHjNWTIEC1btkxXXXWVJGn69On6yU9+oq1bt6pHjx6SpLKyMi1ZskQTJ05UkyZNGrp8W2EEFgAAAAAAQAhvvfWWnE6n5syZExS/9dZbZYzR22+/HZhOUrXpbr755mrzTElJCfx/WVmZDh06pC5duqh58+b67LPPAq9deumlSk5ODhqF9e677yovL+8H+YwuGlgAAAAAAAAh7Ny5U23btlWzZs2C4v6/Srhz587Afx0Ohzp37hw0Xffu3avNs6ioSL/+9a8Dz9Rq2bKlMjMzdfjwYbnd7sB0zZs31/jx4/Xiiy8GYosXL1a7du103nnn1VuN8YKvEAIAAABAHFm+KdYZVBjVJ9YZAPHnpptu0sKFC3XzzTdryJAhSk9Pl2VZmjZtmnw+X9C006dP18svv6wPPvhAffv21euvv67rr79eDscPbzwSDSwAAAAAAIAQOnTooJUrV+rIkSNBo7C2bt0aeN3/X5/Pp//+979Bo66++uqravNcunSpZsyYoT/84Q+BWHFxsQ4fPlxt2jFjxigzM1OLFy/WGWecoWPHjgWekfVD88Nr2QEAAAAAAERh3Lhx8nq9euKJJ4LiDz/8sCzL0tixYyUp8N/HHnssaLpHHnmk2jydTqeMMUGxxx9/XF6vt9q0LpdLl112mZYsWaJFixapb9++6tevX11KiluMwAIAAABQ75rt+SbWKVTo0yXWGQCIU+PHj9eIESN09913a8eOHerfv7+WL1+u1157TTfffHPgmVcDBgzQZZddpieffFJut1tDhw7VqlWr9M031Y+FF110kZ5//nmlp6erV69e+vDDD7Vy5Uq1aNEiZA7Tp0/XY489ptWrV+uBBx5o0HrtjAYWAAAAAABACA6HQ6+//rp+/etf6+9//7sWLlyoU045RQ8++KBuvfXWoGn/+te/Br7u9+qrr+q8887TP//5T2VnZwdN9+ijj8rpdGrx4sUqLi7WWWedpZUrV2r06NEhczj99NPVu3dvbdmyRVdccUWD1Wp3lqk6bi0OFBQUKD09XW63W2lpabFOBwAAAHEqnh6GHU+5StKH79pnBNaQ0ZFHYMXbZxtv+SL+FRcXa/v27erYsaOSk5Njnc4P0qmnnqqMjAytWrUq1qmEVdN2UtdeDs/AAgAAAAAAsKmcnBx9/vnnmj59eqxTiSm+QggAAAAAAGAzmzZt0qeffqo//OEPatOmjaZOnRrrlGKKEVgAAAAAAAA2s3TpUs2aNUtlZWX629/+9oP/+iYNLAAAAAAAAJv5zW9+I5/Ppy1btmjYsGGxTifmaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAgBoZY2KdAmysobcPGlgAAAAAACAsp9MpSSorK4txJrAz//bh317qGw0sAAAAAAAQVkJCgpKSkuR2uxmFhZCMMXK73UpKSlJCQkKDLMPVIHMFAAAAAAAnjJYtW2rPnj3avXu30tPTlZCQIMuyYp0WYswYo7KyMrndbhUWFqpdu3YNtiwaWAAAAAAAIKK0tDRJUl5envbs2RPjbGA3SUlJateuXWA7aQg0sAAAAAAAQI3S0tKUlpamsrIyeb3eWKcDm3A6nQ32tcHKaGABAAAAAICoJSQkNErDAqiMh7gDAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1lyxTgAAAAAnjuWbYp1BhVF9Yp0BAACoL4zAAgAAAAAAgK3VuYH1ySef6MYbb1Tv3r3VtGlTtW/fXpdeeqlyc3ODpps5c6Ysy6r2r0ePHnVNAQAAAAAAACewOn+F8IEHHtD777+vKVOmqF+/ftq/f7+eeOIJnXbaafroo4/Up0/F2O2kpCQ988wzQe9PT0+vawoAAAAAABvia8UA6kudG1i33HKLXnzxRSUmJgZiU6dOVd++fXX//ffrhRdeqFiYy6Urr7yyrosEAAAAAADAD0idv0I4dOjQoOaVJHXt2lW9e/fWli1bqk3v9XpVUFBQ18UCAAAAAADgB6JBHuJujNGBAwfUsmXLoPixY8eUlpam9PR0ZWRk6IYbblBhYWFDpAAAAAAAAIATRJ2/QhjK4sWLtWfPHt17772BWJs2bXT77bfrtNNOk8/n0zvvvKMnn3xSX3zxhdasWSOXK3wqJSUlKikpCfzsH8Hl8Xjk8XgkSQ6HQw6HQz6fTz6fLzCtP+71emWMqTHudDplWVZgvpXjUvkIsmjiLpdLxpiguGVZcjqd1XIMF6cmaqImaqImaqImaoq3moxxfv8/wXHLUV5TcNyS5XDKGJ9kfDXHLYcsyxE+7vNKqsjd56u5puDFhs49XLy+a/J4Iq8n4wtfq6zymowveD01VE0eT83bngmq//v5WFa9xL9PPqp4+ecbeX+qWET9bHt1WU+Vd7Vw+5nU+PtTuLgxkY8R5dOHrjUo3AjHCI7l1ERNsa2pal21Ve8NrK1bt+qGG27QkCFDNGPGjEB8/vz5QdNNmzZN3bp10913362lS5dq2rRpYec5f/58zZ07t1p8/fr1atq0qSQpMzNTnTt31vbt2/Xtt98GpsnKylJWVpZyc3PldrsD8U6dOqlVq1batGmTioqKAvEePXqoefPmWr9+fdDK7tevnxITE5WTkxOUw8CBA1VaWqoNGzYEYk6nU4MGDZLb7dbWrVsD8ZSUFPXv3195eXnatm1bIJ6enq6ePXtq79692r17dyBOTdRETdRETdRETdQUbzWpyUAZb6nK8ipqsiynElsPkil1qyy/oibLlaLEzP7yFeXJ466oyZGUroSMnvIW7pW3sKImZ0qmXM07y+veLm9RRU3O1Cy5mmXJczhXvpKKmvJa11xT6eGKmhJa9pPlTFTpgeCaEk9unJpyciKvp9Ijkiu9k5xNWqns0CYZT0VNCRk9ZCU1V9nB9TKm4WvKOVbztlfk/U6lvopvWyQ705XsbK6jnjx5TEXuKc4WSnKmqtCzX15TFog3dbVSgpWigrI9Mqq4eWqW0EYOueQu2xVUU3pCtnzy6EjZvorc5VB6YnaN+1PpkejXUzTbXl3WU86xiprCHSOa5Z+kMl+RjnoOVsStBDVLaKsSb6GKvIcqcrFSlJrQSsXewyr2VuSY6EhVE1cLHfMcCrmeCssOhlxPR8r2Bq0nd/vTIx4jYrU/hVpPHMupiZpiW1NdHydlmcqtsTrav3+/zjrrLJWVlemjjz5S27ZtI05fVFSk1NRUzZo1q9pfJ6ws1Ais7OxsHTp0SGlpaZLoeFITNVETNVETNVETNdmhplVb7DMC64I+Nde0anPlxcZ2BNb5PSOvp1Wbw9fa2COwzu9V87b3wTu5wcuM4QisM0d1jrg/VWwHsR+BdX6vinC4/eyTVTu+3y5CjzarXbxu62PI6K4RjxHLN9pnBNb5PTmWUxM1xbKmgoICtWjRQm63O9DLqY16G4Hldrs1duxYHT58WGvXrq2xeSWVdwBbtGih/Pz8iNMlJSUpKSmpWtzlclX76qH/Q6vKv2KjjYf7SmNt4pZlhYyHy7G2cWqipnBxaqImiZrC5VjbODVRk0RN4XIMFbf8PQQrdE2h4w7Jqp5jreOO4Nz9ZUeqKcRsQuYYLl6fNblckddT5bdVrbUiHn3u4eLR1FR5tYfbxqyQH279xSsaVjXHa9qfqi6irttezfHw6yPUrhbuGBGu1trF67Y+rO93+nDHiNpskw19jOBYTk3h4tTUODVFenRUNOqlgVVcXKzx48crNzdXK1euVK9evWp+k6QjR44oLy9PmZmZ9ZEGAAAAAAAATkB1bmB5vV5NnTpVH374oV577TUNGTKk2jTFxcUqKytTs2bNguK//e1vZYzRmDFj6poGAAAAAAAATlB1bmDdeuutev311zV+/Hjl5+frhRdeCHr9yiuv1P79+3XqqafqsssuU48ePSRJ7777rt566y2NGTNGF198cV3TAAAAAAAAwAmqzg2szz//XJL0xhtv6I033qj2+pVXXqnmzZvroosu0ooVK/Tss8/K6/WqS5cumjdvnn7+85+H/D4lAAAAAAAAINVDA2vNmjU1TtO8eXM9//zzdV0UAAAAAAAAfoAY+gQAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW6OBBQAAAAAAAFujgQUAAAAAAABbc8U6AQAAAJw4mu35JtYpVOjTJdYZAACAesIILAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BrPwAIAAAAAQNLyTbHOoMKoPrHOALAXRmABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZcsU4AAAAAAGKp2Z5vYp1ChT5dYp0BANgSI7AAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABga65YJwAAAAAAAGpn+aZYZ1BhVJ9YZ4AfAhpYAAAANsdNCgAA+KHjK4QAAAAAAACwNRpYAAAAAAAAsDW+QggAAIAfrGZ7vol1ChX6dIn4cjzlCgBAfWMEFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGzNFesEEH+Wb4p1BhVG9Yl1BgAAAAAAoKExAgsAAAAAAAC2xggsAAAAAADQoPgmD+qKEVgAAAAAAACwNUZg2QTdaAAAAAAAgNAYgQUAAAAAAABbo4EFAAAAAAAAW+MrhDjh8fVMAAAAAADiGyOwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABga3VuYH3yySe68cYb1bt3bzVt2lTt27fXpZdeqtzc3GrTbtmyRWPGjFFqaqoyMjJ01VVX6dtvv61rCgAAAAAAADiB1fkh7g888IDef/99TZkyRf369dP+/fv1xBNP6LTTTtNHH32kPn3Kn1q9e/dunXvuuUpPT9e8efNUWFioBQsWaOPGjVq3bp0SExPrXAwAAAAAAABOPHVuYN1yyy168cUXgxpQU6dOVd++fXX//ffrhRdekCTNmzdPR48e1aeffqr27dtLkgYPHqwLLrhAixYt0jXXXFPXVAAAAAAAAOqEv2RvT3X+CuHQoUOrjZ7q2rWrevfurS1btgRiy5Yt00UXXRRoXknSyJEj1a1bNy1ZsqSuaQAAAAAAAOAE1SAPcTfG6MCBA2rZsqUkac+ePTp48KAGDhxYbdrBgwdr/fr1DZEGAAAAAAAATgB1/gphKIsXL9aePXt07733SpL27dsnSWrTpk21adu0aaP8/HyVlJQoKSkp5PxKSkpUUlIS+LmgoECS5PF45PF4JEkOh0MOh0M+n08+ny8wrT/u9XpljKkx7nQ6ZVlWYL6V45Lk9XqjirtcLhljguKWZcnpdFbL0bIsSU4Z45NMRVyWQ5blCB/3eSWZKOLlNRlfcE2yynOXCc7dmMg1lc8/MBNZjhC5h4vXc03RrCfjC1+r5SivKTjecDV5PPbb9kLF431/oiZqoiZqOtFqKj+9xPac67+O8JcWLveKz8MExctzMfUU9ymYVZ5jlbjP56txPZkqn2Wo3MPF67umyttNqG2sPNfQtUaKN0RNHo+nxv2pNjk2Rk2RjhGVl1Ef215daqq8HYTbzyQ1+v4ULm6MiXjcC753UEyvy6M5lvvvHWpz/9RQNVW+dwi1n0kNd09Y25qkms+5gXJjdJ9bOV55cw11HWF89jjnSuXbwYlybVT1OFFb9d7A2rp1q2644QYNGTJEM2bMkCQVFRVJUsgGVXJycmCacA2s+fPna+7cudXi69evV9OmTSVJmZmZ6ty5s7Zv3x70lw2zsrKUlZWl3Nxcud3uQLxTp05q1aqVNm3aFMhPknr06KHmzZtr/fr1QSu7X79+SkxMVE5OTlAOAwcOVGlpqTZs2BCIOZ1ODRo0SG63W1u3bg3EU1JS1L9/f+Xl5Wnbtm2BeHp6uqSe8hbulbdwd8V8UjLlat5ZXvd2eYsqanKmZsnVLEuew7nylVTU5ErvJGeTVio7tEnGU1FTQkYPWUnNVXZwvUylnTihZT9ZzkSVHgiuydsrck2lBypqslwpSszsL19RnjzuipocSelKyGj4mqJZT6VHpMSTB8p4S1WWV1GTZTmV2HqQTKlbZfmNU1POMfttez179tTevXu1e3dFTfG+P1ETNVETNZ1oNZUeif05138dkXMsck1Shnzy6EjZvkDEkkPpidnymGId9RysyMVKULOEtir1HVWR91BFLlaKUhNaqcTnVrG3IsdER6qauFqoyPudSn2FgXiyM13JzuY66smTx1TknpfXvMb15C4rCMSbJbSRQy65y3YFVZSekN0oNVX+LENte+6yo0pxtlCSM1WFnv3ymrLA9E1drZRgpaigbI+MKm40GqqmnJz8GvenaNdTY9RU0zHCXXY06vXU0DXl5OQH4uGOEdJJjb4/havJ7W4V8bhX9V4jltfl0RzLS4/U/v6poWrKORb5/CQ13D1hbWuSaj7nlh6Jbj01Rk3+c1m464iyInucc6Xy7eBEuTbyD0Y6Xpap3Bqro/379+uss85SWVmZPvroI7Vt21aSlJOTo0GDBum5557TVVddFfSe22+/XQ8++KCKi4trNQIrOztbhw4dUlpamiT7/+ZUitzxXLXFPiOwRvWNXNPyjfYZgXVej5rX06rN4Wtt7BFY5/ey37YXjyMRqImaqImafmg1rdosxfqc67+OOL9X5NzXrdz+/f/FfgTWmaO61Lie1q3cFjSfULk31giswSM7BWKhtrHyXO0xAmvwyE417k8fvJMbdY4NXdOZozpHPEZU3g5iPQKr8nYQbj/7ZNUO24zAGjK6a8TjXvC9g2J6XX5+z5qP5f57BzuMwKp87xBqP1u52T4jsEb3q/mcW34uU43rqTFq8p/LpNDXEas22+OcK5VvByfKtVFBQYFatGght9sd6OXURr2NwHK73Ro7dqwOHz6stWvXBppXUsVXB/1fJaxs3759ysjICNu8kspHboV63eVyyeUKLsH/oVXlX7HRxqvO93jilmWFjIfL0bIcklWLuCN07uHjYVa3FRy3vj9/hqsp1HxqnXs91RTN+ghajBW6ptDx+q+pcrp22vZqG4+H/YmaqClcjrWNUxM1SbGvqfLpJVbnXP/5v2qqVXO3/BcSgRvyqq/VRzz0Y1yrxv3rMtJ6Cj2v6ssMF6/PmkJtB5Vzr5xrtJ9BpVeijkeTe+VcI17b1iLHhq4p0jGi6jLquu0db1wKnWe4Y0Rj7k/h4v59PtzxLdp7kMC8GvC6PJpjedDxtha5h4vXpabKH2nY/ayB7gkjxcPVVNO5tWq5jX2fWzledXOteozwpxXrc64UvB3E+7VRuPyjVS8NrOLiYo0fP165ublauXKlevXqFfR6u3btlJmZGWKIubRu3ToNGDCgPtIAAAAAAADACajODSyv16upU6fqww8/1GuvvaYhQ4aEnG7SpEl69tlntWvXLmVnZ0uSVq1apdzcXP3sZz+raxoAAABRW74p1hlUGNUn1hkAAADYX50bWLfeeqtef/11jR8/Xvn5+XrhhReCXr/yyislSXfddZdefvlljRgxQj/96U9VWFioBx98UH379tWsWbPqmgYAAAAAAABOUHVuYH3++eeSpDfeeENvvPFGtdf9Dazs7Gy99957uuWWW/SLX/xCiYmJuvDCC/WHP/wh4vOvAAAAAAAA8MNW5wbWmjVrop62d+/eevfdd+u6SAAAAAAAAPyAhPvzFwAAAAAAAIAt0MACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICtuWKdAAAAAADgxNRszzexTqFCny6xzgBAHTACCwAAAAAAALbGCCzARpZvinUGFUb1iXUGAAAAAACUYwQWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbM0V6wQAAMCJYfmmWGdQYVSfWGcAAACA+sQILAAAAAAAANgaI7AAAAAAAJDUeflzsU6hQp/psc4AsBVGYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZcsU4AAACEtnxTrDOoMKpPrDMAAADADxkjsAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGuuWCcAIH4t3xTrDCqM6hPrDAAAAAAADYURWAAAAAAAALA1RmABAADYXLM938Q6hQp9usQ6AwAA8APECCwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2Fq9NLAKCwt1zz33aMyYMcrIyJBlWVq0aFG16WbOnCnLsqr969GjR32kAQAAAAAAgBOQqz5mkpeXp3vvvVft27dX//79tWbNmrDTJiUl6ZlnngmKpaen10caAAAAAAAAOAHVSwOrTZs22rdvn1q3bq2cnBwNGjQo/AJdLl155ZX1sVgAAAAAAAD8ANTLVwiTkpLUunXrqKf3er0qKCioj0UDAAAAAADgBFcvI7Bq49ixY0pLS9OxY8d00kkn6bLLLtMDDzyg1NTUxk4FAPADtHxTrDOoMKpPrDMAAAAA4kOjNrDatGmj22+/Xaeddpp8Pp/eeecdPfnkk/riiy+0Zs0auVyh0ykpKVFJSUngZ//oLY/HI4/HI0lyOBxyOBzy+Xzy+XyBaf1xr9crY0yNcafTKcuyAvOtHJfKR49FE3e5XDLGBMUty5LT6ayWo2VZkpwyxieZirgshyzLET7u80oyUcTLazK+4JpklecuE5y7MZFrKp9/YCayHCFyDxev55qiWU/GF75Wy1FeU3C84WryeCJve1L066mha5Jq3p8Cb6mnba8uNfk3hXD7WbwfI6ip/moyRo2+P4U7Rkg11OSLzf4UKu7x1LyejGnY81NtavJ6I297djnnyirfJmvan8z3OZXnaIKXWWPcp2Dlf0TneOP+/SrcsaBie65Njg1Tk8/nq/EYYaps86FyDxev75oqH7NCHd/Kc639+muImjweT43H8vre9upaU6TzU+VlNOb+FCr3yttBuP1MUqPvT+HixpiI1xHRrr/GOEZEcx3hsyTLlGfps6rM5fu3mijjDlOe3fHGPR5PxGsjyR7n3PJPq+brvWr3DjE45/rjlTfXUNewxhfb+9zKNXk8J851edXjRG01agNr/vz5QT9PmzZN3bp10913362lS5dq2rRpYd83d+7cavH169eradOmkqTMzEx17txZ27dv17fffhuYJisrS1lZWcrNzZXb7Q7EO3XqpFatWmnTpk0qKioKxHv06KHmzZtr/fr1QSu7X79+SkxMVE5OTlAOAwcOVGlpqTZs2BCIOZ1ODRo0SG63W1u3bg3EU1JS1L9/f+Xl5Wnbtm2BePlD7HvKW7hX3sLdFfNJyZSreWd53dvlLaqoyZmaJVezLHkO58pXUlGTK72TnE1aqezQJhlPRU0JGT1kJTVX2cH1MpV24oSW/WQ5E1V6ILgmb6/INZUeqKjJcqUoMbO/fEV58rgranIkpSsho+FrimY9lR6REk8eKOMtVVleRU2W5VRi60EypW6V5TdOTTnHIm97UvTrqaFrkmren0qPRLeeGqOmnGPl8fT0dPXs2VN79+7V7t0VNcX7MYKa6q8mmcbfn8IdI6TINZUejM3+FKqmnJya15PXNOz5qTY1bTKRtz27nHMTTx6ooqKa9yd32VE5rQQ1S2irUt9RFXkPVeRipSg1oZVKfG4VeytyTHSkqomrhYq836nUVxiIJzvTlexsrqOePHlMRe4pzhZKcqaq0LNfXlMWiDd1tVKClaKCsj0y8iknJ19S+GOElCGfPDpStq9iPcmh9MRseUyxjnoOVtTawDXl5TWv8RjhLqt4rEWzhDZyyCV32a6gitITshulpsqfZajjnrvsaNTrqaFrysnJr/FYXt/bXl1qqun85C47GvV6auia/PuYFP6cK53U6PtTuJrc7lYRryNitT+Fqima64hjJzdRq/xipZT6tLtVioxV0WVqk1ckl9do18lNgmrKPnBMHqelfS1TKmoyRu0PFKk40aGDGcmBeILHp7Z5xSpMcSk/PbEixxKvTv6uRO7UBLlTEyRJh3JyIl4bSfY451quFEk1X+/57x1iec711+S/dwh3DVtWFNv73Mo15Rw7ca7L6/ooKctUbo3VA/9D3BcuXKiZM2fWOH1RUZFSU1M1a9asan+d0C/UCKzs7GwdOnRIaWlpkuJ/JMKqLfb5bfCovpFrWr7RPiOwzutR83patTl8rY09Auv8XpG3vRVf2mcE1ui+Ne9PqzaHr9WfY2ONGDm/1/dRRitRUw01Ld8k24zAGt03ck0rv7TPCKzze9a8nlZtsc8IrJG9I2977260xzlXllOj+tS8P61bue37/GM/AmvwyE6Swh8L1q3c/v3/xX4E1pmjutR4jPB/tv75hMq9sUaM+D9bKfTxrTxXe4zAGjyyU43H8g/eyY06x4au6cxRnSOenypvB7EegVV5Owi3n32yaodtRmANGd014nXEh+9+HbbWuudeu5oGj+xY43XE9sdftM0IrI43XR7x2mjlZnuccyVLo/vVfL1X7d4hhiOw/PcOUuhr2FWb7TMC6/xeJ851eUFBgVq0aCG32x3o5dRGoz8Dq6qUlBS1aNFC+fn5YadJSkpSUlJStbjL5ar2tUP/h1aVf8VGGw/3dcbaxC3LChkPl6NlOVT+lZIo447QuYePh1ndVnDc/0uGcDWFmk+tc6+nmqJZH0GLsULXFDpe/zVVTjfcthfteooUr6+aatqfqr6lrttepHhNNVXdFMLlHs/HCGqqn5osSzHZn8LFI9UUYvKYHSNcrprXk//80VDnp0jxqjX5P1a7n3PLl1nz/mRZjqB4xQ2gooiH/ps9xxuvmmvVn63AaIXa5NgwNfnXfaRjROh5VV9muHh91hRqO6ice/B2ULv1V981Vc414n5WixwbuqZI56eqy2is/SnEKyHzDHeMaMz9KVzcv8+Hu16ozfpr6JqiuY5wVOolOEyIiaVAwyqauFWHeFT7mQ3OuTXlGNjPqt47xOCc649X3VyrHiP8acXqPrdyTZVzjffr8nD5R6te/gphXRw5ckR5eXnKzMyMdSoAAAAAAACwoUZrYBUXF+vIkSPV4r/97W9ljNGYMWMaKxUAAAAAAADEkXr7CuETTzyhw4cPa+/evZKkN954I/AAsJtuuknfffedTj31VF122WXfP6xaevfdd/XWW29pzJgxuvjii+srFQAAAAAAAJxA6q2BtWDBAu3cuTPw8yuvvKJXXnlFknTllVeqefPmuuiii7RixQo9++yz8nq96tKli+bNm6ef//znIb9TCQAAAAAAANRbA2vHjh01TvP888/X1+IAAAAAAADwA8GwJwAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2Jor1gkAQGNYvinWGVQY1SfWGQAAAABAfGEEFgAAAAAAAGyNBhYAAAAAAABsja8QAgDqhK9nAgAAAGhojMACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArblinQDKNdvzTaxTqNCnS6wz+MFiOwAAAAAAoDpGYAEAAAAAAMDWaGABAAAAAADA1vgKIQDY0PJNsc6gwqg+sc4AAAAAwA8dI7AAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGuuWCeA+NNszzexTqFCny41ThJv+QIAAAAAgGCMwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArdHAAgAAAAAAgK3VSwOrsLBQ99xzj8aMGaOMjAxZlqVFixaFnHbLli0aM2aMUlNTlZGRoauuukrffvttfaQBAAAAAACAE5CrPmaSl5ene++9V+3bt1f//v21Zs2akNPt3r1b5557rtLT0zVv3jwVFhZqwYIF2rhxo9atW6fExMT6SAcAAAAAAAAnkHppYLVp00b79u1T69atlZOTo0GDBoWcbt68eTp69Kg+/fRTtW/fXpI0ePBgXXDBBVq0aJGuueaa+kgHAAAAAAAAJ5B6+QphUlKSWrduXeN0y5Yt00UXXRRoXknSyJEj1a1bNy1ZsqQ+UgEAAAAAAMAJptEe4r5nzx4dPHhQAwcOrPba4MGDtX79+sZKBQAAAAAAAHGkXr5CGI19+/ZJKv+6YVVt2rRRfn6+SkpKlJSUVO31kpISlZSUBH4uKCiQJHk8Hnk8HkmSw+GQw+GQz+eTz+cLTOuPe71eGWNqjDudTlmWFZhv5bgkeb3eqOIul0vGmKC4ZVlyOp3VcrQsS5K+z8MEzceyHDLGp2CWLMuql3i54GX6P49wNVWdT3mO4XJv2JqiWU/l7w1d6/Hlfvw1eTyeiNteRb7B8wmVe0PXJKnG/SmQquUon4/PGzwfq3x/Mr7g9STL+X3q3qjilqN82wuOW7IczvLPy/jk3xTC7WfGOCrWU+XPOGzuDVeTx1PzMcL4Km8HwbVWy7GBa/J4Ih/3/IuOZj01dE3+7SDSsbx8c6+/ba8uNUk1nJ98sdmfQsU9nurHgrD7WSPuT+Fq8nrDn3PLt4PY7E+hajKm5usI/7khludcf9y/X4W7BqrYnmN7zpXKz2M1Xe+ZKtt8qNwb6zqi8jEr1PWC/5qmPq736lqTx+MJe871597Y17A11RTpurzyMhpzfwqVe+XtINx+JkW6d2jcY4QxJuJ1ebTrrzGOEdHcE/osyTLlWfqsKnP5/q0myrjDlGd3vPHK9w6h9jPJHufc8k8r/Dk3sJ9VvXeI4XV55c011HW58TXuNWykmjyehu9HRDqW12ePpepxorYarYFVVFQkSSEbVMnJyYFpQr0+f/58zZ07t1p8/fr1atq0qSQpMzNTnTt31vbt24P+qmFWVpaysrKUm5srt9sdiHfq1EmtWrXSpk2bArlJUo8ePdS8eXOtX78+aGX369dPiYmJysnJCcph4MCBKi0t1YYNGwIxp9OpQYMGye12a+vWrYF4SkqK+vfvr7y8PG3bti0QT09Pl5SgEp9bxd6KHBMdqWriaqEi73cq9RVWfF7OdCU7m+uoJ08eU5F7irOFkpypKvTsl9eUBeJNXa2UYKWooGyPjCo2vGYJbeSQS+6yXUE1eb2dItZUeXqnlaBmCW1V6juqIu+hQNxlpSg1oVWD1xTNenKXHVV6QrZ88uhI2b5A3JJD6YnZ8phiHfUcbJSacnLyI257kqJeTw1dk6Qa96fSI9/PJ72TnE1aqezQJhlPRU0JGT1kJTVX2cH1MpVOIAkt+8lyJqr0QPD+lHjyQBlvqcryKrY9y3IqsfUgmVK3yvIr9ifLlaLEzP7yFeXJ496mnGPffy7p6erZs6f27t2r3bt3B6b3ejLlat5ZXvd2eYsqanKmZsnVLEuew7nylVR8Bg1Z0/qSmo8RpQcqjhGOpHQlZPSUt3CvvIUVNTlTGqemmo57pUeiX08NXZN/O4h0LJep322vLjVJkc9PpQdjsz+Fqiknp6KmcOdcr2n8/SlcTZtM+HNuz56x259C1VRUVPN1hLvsaMzPuf7zU05OvqTw10ZShi3OuZKUl9e8xus9d1lBIB6rc66/psqfZahrWHfZ0Xq73qtrTTk5+WHPuf5jRGNfw0aqqabrcnfZ0ajXU0PX5N/HpPD3GtJJjb4/havJ7W4V8f4pVvtTqJqiuSc8dnITtcovVkqpT7tbpchYFV2mNnlFcnmNdp3cJKim7APH5HFa2tcypaImY9T+QJGKEx06mJEciCd4fGqbV6zCFJfy0yv+iFlyiVcnf1cid2qC3KkJkqRDOTkR73Mle5xzLVeKpPDnXP8xwn/vEMtzrr8m/zVjuHv3sqLGvYaNVFPOsYbvR0Q6ltdnj8U/GOl4WaZya6we+B/ivnDhQs2cObNa/LnnntNVV10V9J7bb79dDz74oIqLi6MegZWdna1Dhw4pLS1NUvyPwFq3crttRmANGd01Yk0fvvt1iBxj89vgQeefEhQNtT7WrdwWttbG/m3w4JGdIm57Hy3/r21GYA0d063G/WnVZv9MYj8C6/xe/npC72ertsT+Nz1+5/eq+RixYpN9RmCd3zPycc+/HdhhBJZ/O4h0LF++SbYZgTW6b+Tz08ov7TMC6/yeNf9GLrCf2eC3wSN7R/4t47sb7TMCa1Sfmq8jys9lsT3n+uODR3aSFP4aaN3K7d//X+xHYJ05qkuN13v+z9Y/n1C5N9Z1hP+zlUJfq/qvaewwAmvwyE41/tb+g3dyo86xoWs6c1TniNfllbeDWI/AqrwdhNvPPlm1wzYjsIaM7hrx/qnqvUMsr8sHj+xY4z3h9sdftM0IrI43XR7xPnflZnuccyVLo/vVPLKn2r1DDK/L/deMUujr8lWb7TMC6/xeJ84IrIKCArVo0UJutzvQy6mNRhuB5f/qoP+rhJXt27dPGRkZIZtXUvmorVCvuVwuuVzBJfg/tKr8KzbaeNX5Hk/csqyQ8XA5ln+V0AoRD/2osvqKV12m/yuN4WoKNZ/wuTdsTdGsj+D31ibH+q+pcl7htr1o11OkeH3VVNP+VDVVyxGmJkeYQ40VfdyyrDBxh2Q5VHVTqJq7/5dn/umr5xgu9/qvyZ9rpGOEFfIYESb3Bq6ppv2s8qJrWk91jtdQU9VUQx/HVK/bXl3jkc5PoQ4HjbE/hYq7XNXjYfezRtyfKpYdXJP/Yw1/zo3N/hQ695qvIyqfG2J1zvXHq+Za9Wf/dUSsz7mSAus+0vVe6Hk1/jm3fD+rvh1Uzj14O6jb9V6keDS5V8414n5WixwbuqZI1+VVlxHL6/JQeYY7RjTm/hQuHuneIdJ8YnGMiOae0FGpl+AwISaWAg2raOJWHeJR7Wc2OOfWlGNgP6t67xDD6/Kqm2vVY4Q/rca6hq0er37vUP7/DdePqG38eHos4fKPVqM9xL1du3bKzMwMMcxcWrdunQYMGNBYqQAAAAAAACCONFoDS5ImTZqkN998U7t2VXwPetWqVcrNzdWUKVMaMxUAAAAAAADEiXr7CuETTzyhw4cPa+/evZKkN954I/AAsJtuuknp6em666679PLLL2vEiBH66U9/qsLCQj344IPq27evZs2aVV+pAAAAAAAA4ARSbw2sBQsWaOfOnYGfX3nlFb3yyiuSpCuvvFLp6enKzs7We++9p1tuuUW/+MUvlJiYqAsvvFB/+MMfwj7/CgAAAAAAAD9s9dbA2rFjR1TT9e7dW++++259LRYAAAAAAAAnuEZ9BhYAAAAAAABQWzSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABga65YJwAgfjXb802sU6jQp0usMwAAAAAANBBGYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZcsU4AAACgsTXb802sU6jQp0usMwAAALA9RmABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWGrWBtWbNGlmWFfLfRx991JipAAAAAAAAIE64YrHQOXPmaNCgQUGxLl26xCIVAAAAAAAA2FxMGljnnHOOJk+eHItFAwAAAAAAIM7E7BlYR44ckcfjidXiAQAAAAAAECdi0sCaNWuW0tLSlJycrBEjRignJycWaQAAAAAAACAONOpXCBMTEzVp0iSNGzdOLVu21ObNm7VgwQKdc845+uCDD3TqqaeGfF9JSYlKSkoCPxcUFEiSPB5</t>
+  </si>
+  <si>
+    <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACRsUlEQVR4nOzdeXhU5fn/8c+ZmWwkJEggbAlCAFkFlE1QBIUioGBVEK0KUvt1q1J/Wtu6ixvaWve61VasYhVRK9aNRahUWUyNLAJiJVAgCCSQyb7MzPn9EWeSSWYyEzLJHMj7dV1eLffMnLnvsz1n7jxzxjBN0xQAAAAAAABgUbZoJwAAAAAAAAA0hAYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAFHSo0cPGYbh919cXJy6d++uWbNmac2aNS2Sx5VXXinDMLRw4cIWeb/m4l2fu3btinYqxz3v/goAANBSaGABABBlp59+uubMmaM5c+ZoypQp8ng8Wrx4scaNG6fHHnss2ulZwrHUZGvJRtrChQtlGIauvPLKZn8vAACAaHJEOwEAAFq7X/ziF34NiPLycl1zzTX629/+pt/85jc677zzdNJJJ0UvwWPEypUrVVVVpW7dukU7FQAAAEQYM7AAALCY+Ph4/elPf1JiYqLcbrfeeeedaKd0TOjVq5f69eunmJiYaKcCAACACKOBBQCABSUlJalv376SVO+raJ988onOO+88paWlKTY2Vl27dtWsWbOUlZUVdHmHDx/WTTfdpBNPPNF3n60bbrhBhw8fPqr87r33XhmGoXvvvVe7d+/W7Nmz1aVLF8XHx+ukk07Svffeq7Kysnqvq6qq0muvvabLLrtM/fr1U3JyshISEtS3b1/NmzdPubm5fs/ftWuXDMPQK6+8IkmaO3eu3z3D7r33Xt9zQ311b8mSJZo8ebI6duyo2NhYdevWTZdffrm2bt1a77ne9+3Ro4dM09SLL76oYcOGKTExUSkpKZo0aZLWrl3r9xrv1/l2794tSerZs6dfrqtXr/Y9d8WKFZo2bZo6deqkmJgYnXDCCerTp48uv/xyffbZZ+FsAvXo0UNz586VJL3yyit+7zV+/Hi/55aWlurhhx/WqaeeqrZt26pNmzYaOHCg7rzzTh05ciSs9wvmz3/+s2/dtGvXTlOnTtW6deuCPt/lcumll17S+PHj1b59e8XFxalnz5667rrrtGfPnka//3/+8x/NmjVL6enpio2NVXJysjIzM3XRRRfpvffeC/qayy67TN27d1dcXJzat2+vc845Rx9++GHE8l69erVvW1RVVemRRx7RwIEDlZCQoNTUVF144YXatm1bo+sFAKC14iuEAABYVGFhoSQpLi7OF7vrrrv0wAMPyDAMjRkzRt27d9e2bdu0ePFivf3223rxxRf185//3G85Bw4c0NixY/Xdd9/phBNO0HnnnSePx6NFixbp448/1sCBA486x5ycHA0bNkwOh0NnnnmmysrKtGrVKs2fP18rVqzQihUrFB8f75fLFVdcoZSUFPXv31+DBw9WSUmJvv76az399NN644039MUXX6h3796Sqht5c+bM0b///W99//33Ov30032PSdLQoUND5uhyuXTZZZdp8eLFiouL07Bhw9StWzft2LFDixYt0jvvvKN33nlHkydPDvj6uXPn6vXXX9fYsWN13nnn6euvv9by5cv12Wef6V//+pdGjRolSerdu7fmzJmjJUuWqKSkRBdddJGSkpJ8y+ncubOk6maTt/E0cuRInXXWWSorK9PevXv1xhtvqEOHDjrzzDND1jVjxgytW7dOn3/+uXr16qUzzjjD91i/fv18///w4cOaMGGCvv76ayUnJ+vss89WTEyM/vWvf+nBBx/U66+/rk8//VQ9evQI+Z513XzzzXriiSd0+umn6/zzz9fmzZv10Ucfafny5Vq8eLEuuOACv+cXFRVp+vTpWr16tZKSkjRs2DB17NhRmzdv1vPPP6+33npLy5cv1ymnnBLW+69cuVJTpkxRVVWVhgwZotGjR8vtdmvfvn364IMP5Ha7df755/u95sknn9TNN98sj8ejoUOHatSoUfrhhx+0evVqLVu2TPPnz9fdd98dsbyrqqo0depUffHFFzrzzDPVv39/bdiwQe+++65WrVql7Ozso1r3AAC0OiYAAIiKE0880ZRkvvzyy/Ue27hxo2mz2UxJ5l//+lfTNE3zo48+MiWZ8fHx5rJly/ye/9JLL5mSzJiYGHPLli1+j82YMcOUZI4dO9YsKCjwxfPz881Ro0aZkoLmEcw999zje935559vlpaW+h7bs2ePedJJJ5mSzN/97nd+ryssLDTfe+89s6Kiwi9eWVlp3nbbbaYkc+rUqfXeb86cOSFz9K7PnJwcv/jtt99uSjJHjRpl7ty50++xt956y7Tb7eYJJ5xgHjlyxBfPycnx1XfiiSea3377re8xl8tl/vznPzclmZMmTQo7D6+ePXuaksw1a9bUe+zAgQPmV199FbTGul5++WVTkjlnzpygz5k1a5av/ry8PF+8qKjInDJliinJHDNmTNjvaZqmb90kJCSYK1eu9Hvs97//vSnJTElJMQ8cOOD32M9+9jNTknneeefVe+zxxx83JZl9+vQxXS5XWHmcddZZpiTztddeq/dYQUGBuXbtWr/Yxx9/bBqGYXbo0MH817/+5ffYpk2bzPT0dFOSuXr16ibnvWrVKt96OuWUU8z9+/f7HisrKzPPOeccU5J59dVXh1UrAACtHQ0sAACiJFADq6CgwPzggw/MXr16mZLMrl27msXFxaZpmuaECRNMSebNN98ccHnnnXeeKcn8v//7P1/sf//7n2mz2UzDMMxvvvmm3muys7Ob1MBKSEjw+2Du9f7775uSzOTkZLOsrCzs5Xbt2tW02WxmYWGhX/xoG1j5+flmQkKCGR8fb+7duzfg666//npTkvn000/7YrUbWEuXLq33mv3795uSzLi4OLOysjJkHrW1adPGTElJCVpHY4RqYO3evdu3/Tdu3Fjv8b1795rx8fGmJPPzzz8P+3296+amm24K+Pjw4cNNSeaDDz7oi23dutU0DMPs2rVrve3rNXXqVFOS+f7774eVx4ABA0xJ5uHDh8N6vrdhu2TJkoCPL1682JRkXnTRRU3O29vAMgzD/Prrr+u9Zt26daYkMzMzM6zcAQBo7bgHFgAAUVb7vk7t2rXTueeeq++//169evXShx9+qMTERLlcLn3++eeS5PeLhbVdddVVkqRVq1b5Yp999pk8Ho9OPfVUDRgwoN5rhg4dqsGDBx917pMmTfJ9Na628847T6mpqSosLNRXX31V7/GNGzfqscce04033qif//znuvLKK3XllVfK5XLJ4/Hov//971HnVNuqVatUVlam008/PeivE3rvF/XFF1/Ue8zhcAT8amHnzp11wgknqKKiQvn5+Y3KaeTIkXI6nZo9e7b+85//yOPxNOr1jeHd/qecckrA7dytWzedc845kvz3m3DNmTMnYHz27NmS5Hffrw8//FCmaWrKlClq27ZtwNc1tC0CGTlypCTpsssu07///W+5XK6gz83Ly9OGDRuUkJCgadOmhf3+Tc27e/fuGjJkSL14//79JUn79u0LmjMAAKjBPbAAAIiy2vd1io2NVVpamk477TRNnjxZDkf1UJ2fn6/y8nJJ1TcHD6RXr16S/D8Q7927t8HXeB/btGnTUeXe0HJ79Oih/Px8Xw6SVFJSoiuuuELvvvtug8v13v+rqXbu3Cmp+l5JhmE0+NxDhw7Vi3Xp0iXorxomJyfryJEjvu0SrmeffVbnnXeeXn31Vb366qtq27atRowYobPPPltXXHGFunfv3qjlNcS7LzS0nQLtN+EKtlxvvPa2926Lv/zlL/rLX/7S4HIDbYtAFixYoE2bNumjjz7SRx99pISEBJ166qkaP368LrvsMl+TSKq+X5tpmiorK/O7r1yo929q3sG2Z3JysiSpoqKiwWUCAIBqNLAAAIiyX/ziF0FnVR0PTNP0/f/bbrtN7777rvr166eHH35YI0aMUIcOHRQbGytJGjNmjNauXev3mqbwzm7q3bu3Tj/99AafW/vG5142W+Qnq/fv31/ffvutli1bpk8//VRffPGF1qxZo08//VT33Xef/vKXv+jyyy+P+PtGQ+3t6N0WQ4cODTgjqTbvjfFD6dy5s7KysvSvf/1LK1as0Oeff67169fr888/10MPPaQFCxbot7/9rd/7JyUl6aKLLgq7hqbm3Rz7EAAArRENLAAAjgGpqamKi4tTRUWFdu7cGfDrYN6ZIrW/Kuf9/7t27Qq67IYeCyUnJyfkctPT032xxYsXS5LefPPNgDV89913R51LIBkZGZKkvn37auHChRFddlM4HA5NnTpVU6dOlVQ94+yxxx7T/Pnzdc011+iCCy5QYmJik9/Hu/29+0YggfabcOXk5AT8JchA2967LU4//XQ988wzjX6vYAzD0Pjx431f4ysvL9fChQv1y1/+UrfffrtmzJihXr16+d7fMAz99a9/Dbux1Fx5AwCAxuFPQgAAHAMcDofOOOMMSQraiPnrX/8qSTrrrLN8sTPPPFOGYeirr77S9u3b671m48aNR/31QUlatmyZDh48WC/+4YcfKj8/X23bttWwYcN88cOHD0uSTjzxxHqv+eSTT5SXlxfwfbwztBq6x1EgEyZMUGxsrFavXh0wz+ZwNLkmJyfr3nvvVbt27VRaWqodO3ZE5L3OPPNM2Ww2ff3119q4cWO9x/fv36+PP/5Ykv9+E65XX321wbi3qSRJU6ZMkSQtXbq00V+7bIz4+Hhde+21Gjx4sDwej2//7tq1qwYPHqyioiJfzeFoqbwBAEDDaGABAHCMuOWWWyRJzz33nFauXOn32MKFC7V06VLFxMToV7/6lS/evXt3XXDBBfJ4PLruuuv87i115MgRXX/99U36ul5ZWZmuu+46lZWV+WK5ubm+XK+99lrFx8f7HvPek+jpp5/2W863336ra6+9Nuj7eGfyfPPNN43Kr1OnTrrxxhtVUlKiadOmafPmzfWeU1FRoaVLlwZs8B2NhnItLS3VY489FvBeSWvWrFFBQYHsdrvfzKVw3mvr1q0BH+/evbtmzpwp0zR1zTXX+N1wvqSkRFdffbXKy8s1ZswYjRkzJqz3rO25557zu1G7JD3++OPasGGD2rZt6/thAUk65ZRTdNFFF2nPnj268MILA878Kykp0aJFi3TgwIGw3v/RRx/V//73v3rx7du3+2bz1W6WPvDAA5Kqfzjh/fffr/c60zS1fv16LVu2rFnzBgAAjcdXCAEAOEZMmTJFd955px544AH95Cc/0emnn67u3btr+/bt+uqrr2S32/X8889r4MCBfq/705/+pI0bN2r16tXq2bOnxo8fL9M0tWrVKqWmpmr69OlaunTpUeU0e/Zs/fOf/1RmZqbGjh2r8vJyffrppyopKdHo0aM1f/58v+ffc889mjFjhu666y4tXrxYAwcO1MGDB7VmzRqNHTtWXbt2DfhLbj/96U81f/58PfXUU9qyZYsyMjJks9k0ffp0TZ8+vcEcH374Ye3fv1+vv/667z5GmZmZcjgc2rt3r77++muVlJToo48+CngfrMa66KKLtGrVKl1++eWaNGmSTjjhBEnSrbfeqk6dOumWW27RrbfeqpNPPll9+vRRTEyMdu3apXXr1kmS7rjjDnXs2DGs9zrttNPUtWtXZWdn69RTT9XJJ5+smJgY9e3bV7feequk6u2/fft2rV+/Xr169dJZZ50lh8Ohf/3rXzp06JB69uypRYsWHVWt11xzjc4++2yNHTtW3bp105YtW7R582bZ7Xb99a9/rfcLlS+//LIKCgr00UcfqW/fvhoyZIh69uwp0zS1a9cubdy4UZWVldq2bZs6deoU8v0feOAB3XrrrerXr5/69++vhIQE5ebm+n6RcPbs2Tr11FN9z582bZqefPJJ3XLLLZo+fbp69+6tvn37KiUlRYcOHdLGjRt18OBB/fa3v9WkSZOaLW8AAHAUTAAAEBUnnniiKcl8+eWXG/W6jz76yJw6daqZmppqOhwOs3PnzubMmTPN9evXB31NXl6eeeONN5rp6elmbGysmZ6ebl577bXmoUOHzDlz5jQ6j3vuuceUZN5zzz3mzp07zUsvvdTs1KmTGRsba/bu3du8++67zZKSkoCv/eyzz8wJEyaYHTp0MNu0aWMOGjTIfPDBB82Kigpz3LhxpiRz1apV9V737rvvmqeffrrZtm1b0zAM3/t7eddnTk5OwPf98MMPzQsvvNDs1q2bGRMTY7Zr187s37+/eckll5ivv/66X745OTmmJPPEE08Mug6CvZ/b7TYXLFhgDhw40IyPjzcl+Wqqqqoyn3/+efPSSy81+/XrZ6akpJgJCQlmr169zIsuushcuXJl0PcLZvPmzeb06dPNjh07mjabzZRkjhs3zu85JSUl5oIFC8yhQ4eabdq0MePj483+/fubt99+u3n48OFGv6e3JtM0zeeee84cOnSomZCQYCYnJ5uTJ082P//886Cvdbvd5uuvv25OnTrV7NSpkxkTE2OmpqaagwYNMufOnWu+++67ZmVlZVh5vPbaa+bcuXPNQYMGme3btzfj4uLME0880ZwyZYr57rvvmh6PJ+DrNm/ebF599dVmnz59zPj4eLNNmzZmZmamec4555hPPfWUuW/fvibnvWrVqoDbIth6BAAADTNMM0I/8wMAAFqNe++9V/Pnz9c999yje++9N9rpAAAA4DjHPbAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBp3AMLAAAAAAAAlsYMLAAAAAAAAFgaDSwAAAAAAABYmiPaCXh5PB7l5uaqbdu2Mgwj2ukAAAAAAAAgQkzTVFFRkbp27SqbrfHzqSzTwMrNzVVGRka00wAAAAAAAEAz2bNnj9LT0xv9Oss0sNq2bSupupDk5OQoZwMAAAAAAIBIKSwsVEZGhq//01iWaWB5vzaYnJxMAwsAAAAAAOA4dLS3jeIm7gAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNMv8CiEAAAAAALA20zTldrvlcrminQoswuFwyG63H/WvC4b9Ps26dAAAAAAAcMwzTVMFBQU6dOiQ3G53tNOBxdjtdqWlpSklJaXZGlk0sAAAAAAAQIN++OEHFRQUKDk5WcnJyXI4HM0+4wbWZ5qmXC6XCgsLtX//fpWVlalLly7N8l40sAAAAAAAQFBut1tOp1MdO3ZUhw4dop0OLKht27aKi4tTXl6e0tLSZLfbI/4e3MQdAAAAAAAEVVVVJdM0lZiYGO1UYGGJiYkyTVNVVVXNsnwaWAAAAAAAICS+MoiGNPf+QQMLAAAAAAAAlkYDCwAAAAAAAAFdeeWV6tGjR7TToIEFAAAAAABar4ULF8owjKD/rVu3LtophrR161bde++92rVrV7RTaTb8CiEAAAAAAGj17rvvPvXs2bNevHfv3lHIpnG2bt2q+fPna/z48ZaYLdUcaGABAAAAAICjtmxLtDOQJg1q+jKmTJmi4cOHN31BaBZ8hRAAAAAAAKAB99xzj2w2m1auXOkXv/rqqxUbG6uNGzdKklavXi3DMPTmm2/q9ttvV+fOnZWYmKjp06drz5499Za7fv16TZ48WSkpKWrTpo3GjRunzz//vN7z9u3bp6uuukpdu3ZVXFycevbsqeuuu06VlZVauHChZs6cKUk666yzfF99XL16te/1H330kcaOHavExES1bdtW5557rr755pt67/OPf/xDgwYNUnx8vAYNGqR33323KastopiBBQAAAAAAWj2n06m8vDy/mGEYSk1N1Z133qn3339fV111lTZv3qy2bdvqk08+0Z///Gfdf//9GjJkiN/rHnzwQRmGod/+9rc6ePCgnnjiCU2cOFFff/21EhISJEmffvqppkyZomHDhvkaZC+//LLOPvtsrVmzRiNHjpQk5ebmauTIkSooKNDVV1+tfv36ad++fVqyZIlKS0t15plnat68eXrqqad0++23q3///pLk+99XX31Vc+bM0TnnnKNHHnlEpaWleu6553TGGWcoOzvb95XDZcuW6aKLLtKAAQO0YMEC5efna+7cuUpPT2/O1R42wzRNM9pJSFJhYaFSUlLkdDqVnJwc7XQAAAAAAICk8vJy5eTkqGfPnoqPj6/3+LH+FcKFCxdq7ty5AR+Li4tTeXm5JGnLli0aNmyYZs+erT/84Q8aNGiQunTporVr18rhqJ4ftHr1ap111lnq1q2btm3bprZt20qS3nrrLV188cV68sknNW/ePJmmqb59+yozM1MfffSRDMOQJJWVlWngwIHq3bu3li1bJkmaM2eOXnvtNa1fv77eVxxN05RhGFqyZIlmzpypVatWafz48b7Hi4uLlZGRoZkzZ+rFF1/0xQ8cOKC+ffvq4osv9sVPOeUUHThwQNu2bVNKSookafny5Zo0aZJOPPHEkDeID7WfNLXvwwwsAAAAAADQ6v3pT3/SSSed5Bez2+2+/z9o0CDNnz9ft912mzZt2qS8vDwtW7bM17yqbfbs2b7mlSTNmDFDXbp00Ycffqh58+bp66+/1nfffac777xT+fn5fq+dMGGCXn31VXk8HknVX+ubNm1awPtzeRtfwSxfvlwFBQW69NJL/WaX2e12jRo1SqtWrZIk7d+/X19//bV+97vf+ZpXkvSTn/xEAwYMUElJSYPv0xJoYAEAAAAAgFZv5MiRIW/ifuutt+qNN97Qhg0b9NBDD2nAgAEBn9enTx+/fxuGod69e/tmMX333XeSqmdXBeN0OlVZWanCwkINGnR0U8y873P22WcHfNw7E2r37t0B85akvn376quvvjqq948kGlgAAACABVnhKzle4Xw151jLFwCOxs6dO31Noc2bNx/1cryzq/7whz9o6NChAZ+TlJSkw4cPH/V71H6fV199VZ07d673eKDZY1Z17GQKAAAAAAAQJR6PR1deeaWSk5N100036aGHHtKMGTN04YUX1nuut8nlZZqm/vvf/2rw4MGSpF69ekmqngE1ceLEoO/ZsWNHJScna8uWhv9KEOyrhN73SUtLa/B9TjzxxIB5S9K3337b4Hu3FFu0EwAAAAAAALC6xx57TF988YVefPFF3X///RozZoyuu+66er9cKEl/+9vfVFRU5Pv3kiVLtH//fk2ZMkWSNGzYMPXq1UuPPvqoiouL673+0KFDkiSbzaaf/vSnev/995WVlVXved7f5UtMTJQkFRQU+D1+zjnnKDk5WQ899JCqqqqCvk+XLl00dOhQvfLKK3I6nb7Hly9frq1btza4XloKM7AAAAAAAECr99FHH2n79u314mPGjFFFRYXuuusuXXnllZo2bZqk6l8vHDp0qK6//notXrzY7zXt27fXGWecoblz5+rAgQN64okn1Lt3b/3f//2fpOrG1EsvvaQpU6Zo4MCBmjt3rrp166Z9+/Zp1apVSk5O1vvvvy9Jeuihh7Rs2TKNGzdOV199tfr376/9+/frrbfe0r///W+1a9dOQ4cOld1u1yOPPCKn06m4uDidffbZSktL03PPPacrrrhCp556qi655BJ17NhR//vf//TBBx/o9NNP1zPPPCNJWrBggc4991ydccYZ+vnPf67Dhw/r6aef1sCBAwM22VoaDSwAAAAAANDq3X333QHjL730kl544QV16NBBTzzxhC/ep08fLViwQL/61a+0ePFiXXzxxb7Hbr/9dm3atEkLFixQUVGRJkyYoGeffVZt2rTxPWf8+PFau3at7r//fj3zzDMqLi5W586dNWrUKF1zzTW+53Xr1k3r16/XXXfdpUWLFqmwsFDdunXTlClTfMvr3Lmznn/+eS1YsEBXXXWV3G63Vq1apbS0NP3sZz9T165d9fDDD+sPf/iDKioq1K1bN40dO1Zz5871vc/kyZP11ltv6c4779Rtt92mXr166eWXX9Z7772n1atXR2gtHz3D9M43a4Irr7xSr7zyStDH9+7dq27dujW4jMLCQqWkpMjpdPrugg8AAAC0VsfaTdGPtXwBhK+8vFw5OTnq2bOn4uPjo52Opa1evVpnnXWW3nrrLc2YMSPa6bSoUPtJU/s+EZmBdc0119S7GZhpmrr22mvVo0ePkM0rAAAAAAAAIJiINLBGjx6t0aNH+8X+/e9/q7S0VJdddlkk3gIAAAAAAACtVLP9CuHrr78uwzD0s5/9rLneAgAAAAAAAK1As9zEvaqqSosXL9aYMWPUo0eP5ngLAAAAAAAASxk/frwicKtxBNAsDaxPPvlE+fn5DX59sKKiQhUVFb5/FxYWSpJcLpdcLpek6p+VtNls8ng88ng8vud6426322/HCBa32+0yDMO33NpxSXK73WHFHQ6HTNP0ixuGIbvdXi/HYHFqoiZqoiZqoiZqoiZqoqZwajLN6ppMj39NMuw/PsEdVtywVdfkHzdk2OwyTY9kekLGPZ4wavLU+sBm2GQYNpket6Ta8ZapyeVi36MmaopkTS6XS6Zp+t4/UIPGMIxmjTdGc+dCTYHj3n/X7utINfte3X21sZqlgfX6668rJibG7yck61qwYIHmz59fL56dna3ExERJUseOHdWrVy/l5OTo0KFDvuekp6crPT1dO3bskNPp9MUzMzOVlpamLVu2qKyszBfv16+f2rVrp+zsbL+DcvDgwYqNjVVWVpZfDsOHD1dlZaU2bdrki9ntdo0YMUJOp1Pbt2/3xRMSEjRkyBDl5eVp586dvnhKSor69++v3Nxc7d271xenJmqiJmqiJmqiJmqiJmoKp6aEI4mKsSXIWblHpmo+5LaN6SKbHHJW7fGrKSUmQx65VFS13xczZFNybIaqPGUqcR2sqdWIUduYrqpwF6vMne+LO4wEJcWkqdxdoHJ3TY45iT1C1uTZnVuTuz1VcfYkFVXlym1W+eKJjrQWqSmrpLxmGcG2k2GoV2qqcvLzdai4uKamlBSlt2unHQcPyllre2SmpiotKUlbcnNVVlVTU7+0NLVLSFD2nj1y12pGDO7SRbEOh7L2+Nc0PCNDlS6XNu2vqcmenGypfe94PJ6oqek1xcfHq6KiQgkJCaqqqlJlZaXv+Q6Hw/d47SZFbGysYmNjVV5e7pdjXFycYmJiVFZW5tfEi4+Pl8PhUGlpqV9zJCEhQTabTSUlJX41JSYmyuPx+K0XwzCUmJgot9ut8vKac4HNZlObNm3kcrn8JtPY7XZqilBN3qbWli3+P0vr3feys7PVFIYZ4bltxcXF6tSpk84++2y9//77QZ8XaAZWRkaG8vPzfT+neCx2pkPFqYmaqImaqImaqImaqImawqlpw4qcHz8M1J4hJUnGj/9b9zI+cNwwbD8u9+jjp03qHbKm9cu/98slWO4tUdPIiT1rxYJsp507a2qqtQybYchmGHJ7PH5LDxa3G9U1uTz+NdmN6tzddT5uBYxnZlpq3zsejydqalpN5eXl+t///qeePXsqISGB2UrUFDBeXl6uXbt2KSMjQ/Hx8b64d987cuSIUlNT5XQ6fX2fxoj4DKx//OMfYf36YFxcnOLi4uon5HDI4fBPy3vA1uVdCeHG6y73aOKGYQSMB8uxsXFqoqZgcWqiJomaguXY2Dg1UZNETcFybGycmpqvJuPHRodhBPvdJSPsePWyjj7uraOhmgLlGSz35q4prO1Xu6YA72gPUGdDcUewuBG4Jr/4j/laZd+rSev4OZ4ayrGx8dZYk8PhkPFjs9b7/ECaO94Y0cqxNdfk/Xegvo433hQR/xXCRYsWKSkpSdOnT4/0ogEAAAAAANAKRbSBdejQIa1YsUIXXHCB2rRpE8lFAwAAAAAAoJWKaAPrzTfflMvlCvn1QQAAAAAAACBcEW1gLVq0SGlpaZo4cWIkFwsAAAAAAIBWLKI3cV+7dm0kFwcAAAAAAABE/ibuAAAAAAAAx4qFCxfKMAzFx8dr37599R4fP368Bg0aFIXMUFtEZ2ABAAAAAIBW5uOPo52BNHlykxdRUVGhhx9+WE8//XQEEkKk0cACAAAA0Oqs/T7aGdQY3TvaGQCQpKFDh+rPf/6zbrvtNnXt2jXa6aAOvkIIAAAAAABavdtvv11ut1sPP/xwg89zuVy6//771atXL8XFxalHjx66/fbbVVFR4XvOzTffrNTUVJmm6YvdeOONMgxDTz31lC924MABGYah5557LvIFHWdoYAEAAAAAgFavZ8+emj17tv785z8rNzc36PN+8Ytf6O6779app56qxx9/XOPGjdOCBQt0ySWX+J4zduxYHT58WN98840vtmbNGtlsNq1Zs8YvJklnnnlmM1R0fKGBBQAAAAAAIOmOO+6Qy+XSI488EvDxjRs36pVXXtEvfvELvfXWW7r++uv1yiuv6Ne//rX+8Y9/aNWqVZKkM844Q1JNg8rpdGrz5s266KKL6jWw2rdvrwEDBjRzZcc+GlgAAAAAAACSMjMzdcUVV+jFF1/U/v376z3+4YcfSqr+imBtt9xyiyTpgw8+kCR17NhR/fr102effSZJ+vzzz2W323XrrbfqwIED+u677yRVN7DOOOMMGYbRbDUdL2hgAQAAAAAA/OjOO++Uy+UKeC+s3bt3y2azqXdv/19f6Ny5s9q1a6fdu3f7YmPHjvXNtlqzZo2GDx+u4cOHq3379lqzZo0KCwu1ceNGjR07tnkLOk7QwAIAAAAAAPhRZmamLr/88qCzsCSFNWPqjDPO0L59+7Rz506tWbNGY8eOlWEYOuOMM7RmzRp98cUX8ng8NLDC5Ih2AgAAAEBLWLYl2hn4mzQo2hkAAIK588479dprr9W7F9aJJ54oj8ej7777Tv379/fFDxw4oIKCAp144om+mLcxtXz5cn355Zf63e9+J6n6hu3PPfecunbtqsTERA0bNqwFKjr2MQMLAAAAAACgll69eunyyy/XCy+8oB9++MEXnzp1qiTpiSee8Hv+Y489Jkk699xzfbGePXuqW7duevzxx1VVVaXTTz9dUnVj6/vvv9eSJUt02mmnyeFgblE4aGABAAAAAADUcccdd6iqqkrffvutLzZkyBDNmTNHL774ombNmqVnn31WV155pX7/+9/rpz/9qc466yy/ZYwdO1bffvutBg0apBNOOEGSdOqppyoxMVE7duzg64ONQAMLAAAAAACgjt69e+vyyy+vF3/ppZc0f/58ffnll7rpppv06aef6rbbbtMbb7xR77neBtUZZ5zhizkcDo0ePdrvcYRmmKZpRjsJSSosLFRKSoqcTqeSk5OjnQ4AAACOM8faPbDWfvLflkkkDKPP6R3yOeR79MLJF4im8vJy5eTkqGfPnoqPj492OrCoUPtJU/s+zMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAGgmhmHo3nvvjXYaxzwaWAAAAAAAoFUyDCOs/1avXh3tVFs9R7QTAAAAAAAAx7D//jfaGUi9ex/Vy1599VW/f//tb3/T8uXL68X79+9/1KkhMmhgAQAAAACAVunyyy/3+/e6deu0fPnyenFEH18hBAAAAAAACKKkpES33HKLMjIyFBcXp759++rRRx+VaZp+z6uoqND/+3//Tx07dlTbtm01ffp07d27t97ydu/ereuvv159+/ZVQkKCUlNTNXPmTO3atcv3nJ07d8owDD3++OP1Xv/FF1/IMAz9/e9/j3itVkYDCwAAAAAAIADTNDV9+nQ9/vjjmjx5sh577DH17dtXt956q26++Wa/5/7iF7/QE088oUmTJunhhx9WTEyMzj333HrL/PLLL/XFF1/okksu0VNPPaVrr71WK1eu1Pjx41VaWipJyszM1Omnn65FixbVe/2iRYvUtm1bnX/++c1TtEXxFUIAAAAAsLhlW6KdQY1Jg6KdAdByli5dqk8//VQPPPCA7rjjDknSL3/5S82cOVNPPvmkbrjhBvXq1UsbN27Ua6+9puuvv15/+tOffM+77LLLtGnTJr9lnnvuuZoxY4ZfbNq0aRo9erTefvttXXHFFZKk2bNn65prrtH27dvVr18/SVJVVZUWL16sCy+8UG3atGnu8i2FGVgAAAAAAAABfPjhh7Lb7Zo3b55f/JZbbpFpmvroo498z5NU73k33XRTvWUmJCT4/n9VVZXy8/PVu3dvtWvXTl999ZXvsYsvvljx8fF+s7A++eQT5eXltcp7dNHAAgAAAAAACGD37t3q2rWr2rZt6xf3/irh7t27ff9rs9nUq1cvv+f17du33jLLysp09913++6p1aFDB3Xs2FEFBQVyOp2+57Vr107Tpk3T66+/7ostWrRI3bp109lnnx2xGo8VNLAAAAAAAABayI033qgHH3xQF198sRYvXqxly5Zp+fLlSk1Nlcfj8Xvu7NmztXPnTn3xxRcqKirS0qVLdemll8pma33tHO6BBQAAAAAAEMCJJ56oFStWqKioyG8W1vbt232Pe//X4/Ho+++/95t19e2339Zb5pIlSzRnzhz98Y9/9MXKy8tVUFBQ77mTJ09Wx44dtWjRIo0aNUqlpaW+e2S1Nq2vZQcAAAAAABCGqVOnyu1265lnnvGLP/744zIMQ1OmTJEk3/8+9dRTfs974okn6i3TbrfLNE2/2NNPPy23213vuQ6HQ5deeqkWL16shQsX6uSTT9bgwYObUtIxixlYAAAAAAAAAUybNk1nnXWW7rjjDu3atUtDhgzRsmXL9N577+mmm27y3fNq6NChuvTSS/Xss8/K6XRqzJgxWrlypf773//WW+Z5552nV199VSkpKRowYIDWrl2rFStWKDU1NWAOs2fP1lNPPaVVq1bpkUceadZ6rYwGFgAAAAAAQAA2m01Lly7V3XffrTfffFMvv/yyevTooT/84Q+65ZZb/J7717/+1fd1v3/84x86++yz9cEHHygjI8PveU8++aTsdrsWLVqk8vJynX766VqxYoXOOeecgDkMGzZMAwcO1LZt23TZZZc1W61WZ5h1561FSWFhoVJSUuR0OpWcnBztdAAAAHCcWbYl2hn4mzSo4cfXflL/r/bRMvqc3iGfQ75HL5x8rbT/htp3cfwpLy9XTk6Oevbsqfj4+Gin0yqdcsopat++vVauXBntVIIKtZ80te/DPbAAAAAAAAAsKisrS19//bVmz54d7VSiiq8QAgAAAAAAWMyWLVv0n//8R3/84x/VpUsXzZo1K9opRRUzsAAAAAAAACxmyZIlmjt3rqqqqvT3v/+91X99kwYWAAAAAACAxdx7773yeDzatm2bxo0bF+10oo4GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAIyTTNaKcAC2vu/YMGFgAAAAAACMput0uSqqqqopwJrMy7f3j3l0ijgQUAAAAAAIKKiYlRXFycnE4ns7AQkGmacjqdiouLU0xMTLO8h6NZlgoAAAAAAI4bHTp00L59+7R3716lpKQoJiZGhmFEOy1EmWmaqqqqktPpVHFxsbp169Zs70UDCwAAAAAANCg5OVmSlJeXp3379kU5G1hNXFycunXr5ttPmgMNLAAAAAAAEFJycrKSk5NVVVUlt9sd7XRgEXa7vdm+NlhbxBpYX331le699179+9//Vnl5uTIzM3X11Vdr3rx5kXoLAAAAAAAQZTExMS3SsABqi0gDa9myZZo2bZpOOeUU3XXXXUpKStL333+vvXv3RmLxAAAAAAAAaMWa3MAqLCzU7Nmzde6552rJkiWy2fhhQwAAAAAAAEROkxtYr7/+ug4cOKAHH3xQNptNJSUlSkhIoJEFAAAAAK3Usi3RzqDGpEHRzgBAJDS5y7RixQolJydr37596tu3r5KSkpScnKzrrrtO5eXlkcgRAAAAAAAArViTZ2B99913crlcOv/883XVVVdpwYIFWr16tZ5++mkVFBTo73//e8DXVVRUqKKiwvfvwsJCSZLL5ZLL5ZIk2Ww22Ww2eTweeTwe33O9cbfbLdM0Q8btdrsMw/Att3ZcUr1fTwgWdzgcMk3TL24Yhux2e70cg8WpiZqoiZqoiZqoiZqoKTo1mZ5aDxjVcZn+NRm26pr844YMm12m6VGdhQSOGzYZhi143OOWZMqbarCaTNOUYRjVy/HP0vuMsOLVuZhNins8njC2U511EyT3lqip9n4QbN8zTU/Ndgozx+aqyeVyhTyeTE/k9r3Q8erjyfT4H0/e48blCn2OMD0tezw1FHe5Wu95j5qoyUo11X1+YzW5gVVcXKzS0lJde+21euqppyRJF154oSorK/XCCy/ovvvuU58+feq9bsGCBZo/f369eHZ2thITEyVJHTt2VK9evZSTk6NDhw75npOenq709HTt2LFDTqfTF8/MzFRaWpq2bNmisrIyX7xfv35q166dsrOz/Vbk4MGDFRsbq6ysLL8chg8frsrKSm3atMkXs9vtGjFihJxOp7Zv3+6LJyQkaMiQIcrLy9POnTt98ZSUFPXv31+5ubl+N7OnJmqiJmqiJmqiJmqipujUVFlUU1Nsp+Ey3ZWqyqupyTDsiu08QmalU1WHa2oyHAmK7ThEnrI8uZw1NdniUhTTvr/cxblyF9fUZE/oKEe7XnI7c+Quq6nJnpQuR9t0uQp2yFPhVFZpwzW5zETFGAkqrNonUzUfNNrGdJFNDjmr9vhtp5SYDHnkUlHV/prcZVNKbIZcZrlKXAdrcjFi1Damqyo9JSpz5/viDiNBSTFpqvA4Ve6uWe85OfbQ26kq1xdPsKcqzp6kYtcPcptVvniiI61Faqq9Dwfb98rchto4UlXmPqJKT7EvHm9PUby9nUpceXKZNdujOWvKznaGPJ4qD0Ru3/NypGTK3iZNVflbZLpqao1p309GXDtVHcyWWav5FNNhsAx7eOeIquKWPZ4aqimrtPWe96iJmqxUU3Z2tprCMGu30Y7CoEGD9M033+hf//qXzjzzTF/8s88+07hx4/TKK69o9uzZ9V4XaAZWRkaG8vPzlZycLCn63cHjseNJTdRETdRETdRETdQUyZo+2Rz92RXVcbvOObnhmlZuld/zJUV1BtaEAdXhYNtpw4ocy8zAOm1S75D73vrl3/uvmyjOwBo5sWetWODjacOKnZaZgTVyYmbIc8TyLdaZgTWhf+hzxMqt1pmBNWEA53JqoiYr1HTkyBGlpqbK6XT6+j6N0eQZWF27dtU333yjTp06+cXT0tJ8CQYSFxenuLi4+gk5HHI4/NPyrrS6vCsh3Hjd5R5N3DCMgPFgOTY2Tk3UFCxOTdQkUVOwHBsbpyZqkqgpWI6NjRuGIRmB4jbJqJ9jo+O2wLkHizeUe4DFB8m9ZWqqm2rd7WQYRs1yAjLCjlcv6+jj3v2toX0vUJ7Bcm/umsI5zrw5NDbH5qjJm29DuRsB1ntzH0+G7ejPEd63t8I5ona6nMupiZqsVVNjNPkm7sOGDZMk7du3zy+em1s9hbhjx45NfQsAAAAAAAC0Yk1uYF188cWSpL/85S9+8ZdeekkOh0Pjx49v6lsAAAAAAACgFWvyVwhPOeUU/fznP9df//pXuVwujRs3TqtXr9Zbb72l2267TV27do1EngAAAAAAAGilmtzAkqTnn39e3bt318svv6x3331XJ554oh5//HHddNNNkVg8AAAAAAAAWrGINLBiYmJ0zz336J577onE4gAAAAAAAACfJt8DCwAAAAAAAGhONLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpEbmJOwAAAAAAx6plW6KdQY1Jg6KdAWBNzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXxK4QAAAAAABxD+NVEtEbMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAIClOaKdAAAAAAAAOH4t2xLtDGpMGhTtDHC0mIEFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLc0Q7AQAAAAAAAKtYtiXaGdSYNCjaGVgHM7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaU1uYK1evVqGYQT8b926dZHIEQAAAAAAAK2YI1ILmjdvnkaMGOEX6927d6QWDwAAAAAAgFYqYg2ssWPHasaMGZFaHAAAAAAAACApwvfAKioqksvliuQiAQAAAAAA0MpFrIE1d+5cJScnKz4+XmeddZaysrIitWgAAAAAAAC0Yk3+CmFsbKwuuugiTZ06VR06dNDWrVv16KOPauzYsfriiy90yimnBHxdRUWFKioqfP8uLCyUJLlcLt8sLpvNJpvNJo/HI4/H43uuN+52u2WaZsi43W6XYRj1ZofZ7XZJktvtDivucDhkmqZf3DAM2e32ejkGi1MTNVETNVETNVETNTWU+8qtkmTIsNllmh7JrMldhk2GYQse97glmWHEq2syPXVmzhvVucusznHCgPBq8j7/x4UEzr0FapIa3k7+6fjXWrP4lqvJm2qwfc80zert5Pee1e/74zPCilfnYjYp7vF4wjie6qybILm3RE2194Ng5wjT9NRspzBzbK6aXC5XyHOE6WnZ46mhc4TLFfq8Z3pa9nhqKO5yhT6XVz+/fq3ROEeEMz6ZHoV9Lm/umlyu0GNupMenptQUznVE9fpt2TE3WNy7yx4P10ZN/cZekxtYY8aM0ZgxY3z/nj59umbMmKHBgwfrtttu08cffxzwdQsWLND8+fPrxbOzs5WYmChJ6tixo3r16qWcnBwdOnTI95z09HSlp6drx44dcjqdvnhmZqbS0tK0ZcsWlZWV+eL9+vVTu3btlJ2d7bciBw8erNjY2HqzxYYPH67Kykpt2rTJF7Pb7RoxYoScTqe2b9/uiyckJGjIkCHKy8vTzp07ffGUlBT1799fuV99pb21cuyYlKReqanKyc/XoeLimppSUpTerp12HDwoZ63cM1NTlZaUpC25uSqrqqqpKS1N7RISlL1nj9y1drzBXboo1uFQ1p49/jVlZKgyPT0yNeXmau/evTU1HQ/biZqoiZqoiZqoySI1VRZJtrgUxbTvL3dxrtzFNTXZEzrK0a6X3M4cuctqarInpcvRNl2ugh3yVNTU5EjJlL1Nmqryt8h01dQU076fjLh2qjqYLbPWhXNMh8Ey7LGqPFBdU1Zp6JrMSqeqDtfUZDgSFNtxiDxleXI5a7ZTS9QkNbydKotqtlNsp+Ey3ZWqyqupyTDsiu3ccjV512+wfc9lJirGSFBh1T6ZqrneaxvTRTY55Kzyv95LicmQRy4VVe2vyV02pcRmyGWWq8R1sCYXI0ZtY7qq0lOiMnd+zfo1EpQUk6YKj1Pl7pr1npNjD308VeX64gn2VMXZk1Ts+kFus+YaNtGR1iI11T4ug50jytyG2jhSVeY+okpPzXV5vD1F8fZ2KnHlyWXWbI/mrCk72xnyHOHZvdkX926ncneB33aKtSWpjSNVpa78gDUVVx0MWFNRVW79mmwJclbuCVhTVslhv5oCnSOqilv2ePKtmwDniKzS0Ody73nPty6jeI4IZ3yqLAr/XN7cNWWVhh5zIz0+NaWmcK4jKotafswNVlNW6fFzbZSdna2mMMzabbQIuvTSS/XOO++otLTU122rLdAMrIyMDOXn5ys5OVlS9LuDEflr8HffyVM7xx/z9Hg8tYYCyWYYshmG3B6P399ogsXtRvVfelx+f4mpjkuSu85mtRuG1Ls3f+GmJmqiJmqiJmqyeE3H2gysTzZHf3aFN/dzTm54O1Wv28C11iy+5WaMeNdvsH1vw4ocy8zAOm1S75DH0/rl3/uvmyjOwBo5sWetWOBzxIYVOy0zA2vkxMyQ54h1y/7biHXQvDXVXr9S4HPEyq3WmYE1YUDoc/myzdaZgTWhf+jxaeVWWWYG1oQBocfcTzZZZwbWxAGhryOq1681ZmB5x4rj4droyJEjSk1NldPp9PV9GiNiv0JYV0ZGhiorK1VSUhIwsbi4OMXFxdVPyOGQw+Gflnel1RWoMdZQvO5yjyZuGEbAeLAcvQ2ogM8P8J72AMtoKO4IFg/wngqSe6NramT8mNhO1ERNQXJsbJyaqEmipmA5NjbeWmsybLWfb/MPhIrbAucePB7kUtCojtdNNVhN3ueHlWMz19TQ9giw+CC5t0xNdVOtu+8ZP17PGQETl2oaIaHj1cs6+rh3/2zoeAqUZ7Dcm7umcM4d3hwam2Nz1OTNt6HcA6/fYOugeWsK57znfakVzhG10w2We6jzoX8uzVtTOOOT31jRiNyDxZtSU+1VGuwcEenxKZx4sJrCuV4IayxuoZpqr9/j8dqoMSL6K4S17dy5U/Hx8UpKSmqutwAAAAAAAEAr0OQGVu3vTXpt3LhRS5cu1aRJkwJ29QAAAAAAAIBwNfkrhLNmzVJCQoLGjBmjtLQ0bd26VS+++KLatGmjhx9+OBI5AgAAAAAAoBVrcgPrpz/9qRYtWqTHHntMhYWF6tixoy688ELdc8896t27dyRyBAAAAAAAQCvW5AbWvHnzNG/evEjkAgAAAAAAANTDDaoAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaY5oJ3C8W/t9tDOoMbp3tDMAAAAAAABoPGZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNIc0U4AAACgOS3bEu0MakwaFO0MAAAAjk3NMgPrwQcflGEYGjSIqzQAAAAAAAA0TcQbWHv37tVDDz2kxMTESC8aAAAAAAAArVDEv0L461//Wqeddprcbrfy8vIivXgAAAAAAAC0MhGdgfXZZ59pyZIleuKJJyK5WAAAAAAAALRiEWtgud1u3XjjjfrFL36hk08+OVKLBQAAAAAAQCsXsa8QPv/889q9e7dWrFgR1vMrKipUUVHh+3dhYaEkyeVyyeVySZJsNptsNps8Ho88Ho/vud642+2WaZoh43a7XYZh+JZbOy5VN9/CiTscDpmm6Rc3DEN2u71ejt54dR6m33IMwybT9MifIcMwIhKvZtaL1839aGsKtj2O5e1ETdRETdRETcdvTabpkWqPl4ateiz2uOU3XgaNV9dkevxrklGdu0x3WHHDFl5N1akaMmz24Lm3UE3ezRhqO/nXGiT3FqhJanjf80+n4e3UEjV5Uw12PJmm2ejrvUDx6lyCXZOGF/d4PGGcI+qsmwhdwx5NTbX3g2DnCNP0RO26vG7c5XKFPO/VXX7D66B5awrnHG96WvZ4aijucoUen6qfXzud6J0jwhlzTY8iPj4dbU0uV+jriGiNuYFqCuc6onr9tuyYGyzu3WWPh+u9us9vrIg0sPLz83X33XfrrrvuUseOHcN6zYIFCzR//vx68ezsbN8N4Dt27KhevXopJydHhw4d8j0nPT1d6enp2rFjh5xOpy+emZmptLQ0bdmyRWVlZb54v3791K5dO2VnZ/utyMGDBys2NlZZWVl+OQwfPlyVlZXatGmTL2a32zVixAg5nU5t377dF09ISNCQIUOUl5ennTt3+uIpKSnq37+/KjxOlbtrcoy1JamNI1Vl7iOq9BT74vH2FMXb26nElSeXWZN7gj1VcfYkFbt+kNus8sUTHWmKMRJUWLVPpmp2vLYxXWSTQ86qPX41pcRkqKysLHRNJSVKiInRkK5dlVdcrJ35+TXLSEhQ/7Q05RYUaG+t9d4xKUm9UlOVk5+vQ8U1NaWnpCi9XTvtOHhQzlrbIzM1VWlJSdqSm6uyqpqa+qWlqV1CgrL37JHb45F+3A9aYjvl5uZq7969NTUdB/seNVETNVETNVXX5HbmyF1WU5M9KV2OtulyFeyQp6KmJkdKpuxt0lSVv0Wmq6ammPb9ZMS1U9XBbJm1LjJjOgyWYY9V5QH/mmI7DZfprlRVXk1NhmFXbOfwaqoskmxxKYpp31/u4ly5i2tqsid0lKNdy9WUVRp6O5mVTlUdrqnJcCQotuMQecry5HLWbKeWqElqeN+rLApvO7VUTd71G+x4cpmJjb7e88iloqr9NbnLppTYDLnMcpW4DtbkYsSobUxXVXpKVOauud5zGAlKikmrdw2bk2MPfY6oyvXFI3kNezQ11T7XBDtHlLmNqF2X160pO9sZ8rxXeznBtlNLfdYI51xeVdyyx5Nv3QQ4R2SVhh6fGnMub+6awhlzK4siOz41paas0tDXEdEYc4PVFM51RGVRy4+5wWrKKj1+rveys7PVFIZZu412lK677jqtWLFC33zzjWJjYyVJ48ePV15enrZs2RLwNYFmYGVkZCg/P1/JycmSot8djMRfg7/4+DtZZQbW6HN6h65p504Zkuw2mzymKU+t9RgsbpNqtlOtZdsMQzbDkNvj8csmWNxuVNfk8q7HzMzqODMRqImaqImaqKkJNX2y2TozsH4yMHRNK7dKVpmBNWFA9T8b2k6fbI7+7Apv7uec3PC+V71uA9das/iWmzHiXb/BjqcNK3IsMwPrtEm9Q54j1i//3n/dRHEG1siJPWvFAp8jNqzYaZkZWCMnZoY8761b9t9GrIPmran2+pUCnyNWbrXODKwJA0KPT8s2W2cG1oT+ocfclVtlmRlYEwaEvo74ZJN1ZmBNHBD6OqJ6/VpjBpZ3rDgerveOHDmi1NRUOZ1OX9+nMZo8A+u7777Tiy++qCeeeEK5uTV/dSkvL1dVVZV27dql5ORktW/f3u91cXFxiouLq5+QwyGHwz8t70qry7sSwo3XXe7RxA3DCBgPlqNhGKoZpGrHA99+LFLxwO8ZOPfa8bU5tZcXOPfg8WC5HF189En+uTbndmps/FjY96iJmoLl2Ng4NVGTdGzXZBg2KcB4adgC5x48HuSyyQg/Hk5NtVMNmnsL1VQ31WDbKXCtjcw9QjU1tI8FvGwKsp1aoqa6qdY9nqqvIxt3vRcsHvyaNLy4d/9s6BwRKM9IXMMGizeUezjnDm8O0bgurxv35ttQ7oHXb3Q+a4RzLve+1ArniNrpBsu9Mef45q4pnDHXb6yI0Ph0tDXVXqVBx+IojbmB4uFcR4Q1FrdQTbXX7/F4vdcYTb6J+759++TxeDRv3jz17NnT99/69eu1Y8cO9ezZU/fdd19T3wYAAAAAAACtVJNnYA0aNEjvvvtuvfidd96poqIiPfnkk+rVq1dT3wYAAAAAAACtVJMbWB06dNBPf/rTevEnnnhCkgI+BgAAAAAAAISryV8hBAAAAAAAAJpTk2dgBbN69ermWjQAAAAAAABaEWZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0hzRTgAAABxblm2JdgY1Jg2KdgYAAABoCczAAgAAAAAAgKUxAwvHLCvNAJCYBQAAAAAAQHNhBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACytyQ2sb775RjNnzlRmZqbatGmjDh066Mwzz9T7778fifwAAAAAAADQyjmauoDdu3erqKhIc+bMUdeuXVVaWqq3335b06dP1wsvvKCrr746EnkCAAAAAACglWpyA2vq1KmaOnWqX+yGG27QsGHD9Nhjj9HAAgAAAAAAQJM0yz2w7Ha7MjIyVFBQ0ByLBwAAAAAAQCvS5BlYXiUlJSorK5PT6dTSpUv10UcfadasWZFaPAAAAAAAAFqpiDWwbrnlFr3wwguSJJvNpgsvvFDPPPNM0OdXVFSooqLC9+/CwkJJksvlksvl8i3HZrPJ4/HI4/H4nuuNu91umaYZMm6322UYhm+5teOS5Ha7w4o7HA6ZpukXNwxDdru9Xo7eeHUept9yDMMm0/TInyHDMCISr2bWi9fNPVBN3uVV5xgs95apybu9gm0P07T/+H/844atuib/uCHDZq9ett/7BokbtpqaAsU9bv91YNgkWWvfC3bcHMvHEzVREzVZoybTowbOh9U1mR7/mmQEPmcHi4d7Lne5QtfUmHN5S9QUajtVpxq58akpNXl3zVD7XkuPucFqkho+nvzTif51hDfVYOcI0zQbfb0XKH5013X+cY/HE8Y5os66idA17NHUVHs/CHaOME1P1K7L68ZdLlfIc3nd5bfkdXnd3MMZt0xP9K7L68ZdrtBjbvXza6cTvXNEONcR1WNxy465weIuV+jriGiNuYFqCufayO9aJ8rXEd5d9ni4hq37/MaKWAPrpptu0owZM5Sbm6vFixfL7XarsrIy6PMXLFig+fPn14tnZ2crMTFRktSxY0f16tVLOTk5OnTokO856enpSk9P144dO+R0On3xzMxMpaWlacuWLSorK/PF+/Xrp3bt2ik7O9tvRQ4ePFixsbHKysryy2H48OGqrKzUpk2bfDG73a4RI0bI6XRq+/btvnhCQoKGDBmivLw87dy50xdPSUlR//79VeFxqtxdk2OsLUltHKkqcx9RpafYF4+3pyje3k4lrjy5zJrcE+ypirMnqdj1g9xmlS+e6EhTjJGgwqp9MlWz47WN6SKbHHJW7fGrKSUmQ2VlZSFrclaVyG7EqG1MV1V6SlTmzvc932EkKCkmrcVqyso63OB2alvQXh65VFS13xczZFNybIaqPGUqcR2sqfXHmircxQFrKncXBKyp1JUfsKbiqoP1atLJQy217+Xm5mrv3r2++PFwPFETNVGTNWqqLJIcKZmyt0lTVf4Wma6ammLa95MR105VB7Nl1rogi+kwWIY9VpUH/GuK7TRcprtSVXk1NRmGXbGdR8isdKrqcE1NhiNBsR2HyFOWJ5ezuqas0tA1uZ05cpfV1GRPSpejbbpcBTvkqajZTi1RUzjbqbJIssWlKKZ9f7mLc+UurqnJntBRjnYtV1NWaXW8oX0vnO0ktUxNUsPHU2VReNuppWryrt9g5wiXmdjo671A10YpsRlymeUBr43Cvd7LybGHPkdU5frikbyGPZqaap8/g50jytxG1K7L69aUne0MeS6vvZyWvi6vW1M441NVccseT751E+AckVUaesyN9PjUlJrCuY6oLGr5MTdYTVmloa8jojHmBqspnGujyqKWH3OD1ZRVevxcw2ZnZ6spDLN2Gy2CJk2apIKCAq1fv16GYdR7PNAMrIyMDOXn5ys5OVlS9LuDkfgL9xcffyerzMAafU7vkDVtWLGzVo7RnYE1cmKmpODbY8OKnIC1RuKvjEdT05jJfSy171mt205N1ERNx09NK7cqqn85rf2X0AkDQtf0yWbrzMD6ycDQ22nl1sC1+uXYQn8NnjCg+p8N7XufbI7+7Apv7uec3PDxVL1uA9das/iWmzHiXb/BzhEbVuRYZgbWaZN6hzxHrF/+vf+6ieIMrJETe9aKBT5HbFix0zIzsEZOzAx5Ll+37L+NWAfNW1Pt9SsFPkes3Nqyx1ND8QkDQo+5yzZbZwbWhP6hryOqx2JrzMCaMCD0dcQnm6wzA2vigNDXRn7XOlGegeUdK46Ha9gjR44oNTVVTqfT1/dpjIjNwKprxowZuuaaa7Rjxw717du33uNxcXGKi4urn5DDIYfDPy3vSqvLuxLCjddd7tHEDcMIGA+WY3Xzrn4DzzAC3z8/UvHA7xk499rx2ssLnnvL1FQ317r/rmmMNibH5q3JSvteY+PHwvFETdQULMfGxqmpaTXVPgUatsA1GbYglxhG+HHDMILEbb4kapccfCy2+SftyzFY7s1bU6jt5Ld+g+XeQjXVTTXYvhdqOzUp3siaGjpuAg7fR7nvNSn+Y+51U617jvBe6zTmei9YvKnXRt79s6FzRKA8I3ENGyzeUO7hnA+9OUTjurxuvOZaPHjugddvdD5rhDM+eV9qhXNE7XSD5d6Yc3xz1xTOdYT/WNwyY26weFhjcZTG3EDxcK6BwhqLW6im2uv3eLyGbYxm+RVCSb7pZbWnnwEAAAAAAACN1eQG1sGDB+vFqqqq9Le//U0JCQkaMGBAU98CAAAAAAAArViTv0J4zTXXqLCwUGeeeaa6deumH374QYsWLdL27dv1xz/+UUlJSZHIEwAAAAAAAK1UkxtYs2bN0l/+8hc999xzys/PV9u2bTVs2DA98sgjmj59eiRyBAAAAAAAQCvW5AbWJZdcoksuuSQSuQAAAAAAAAD1NNtN3AEAAAAAAIBIoIEFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEtzRDsBAABau2Vbop1BjUmDop0BAAAAUB8zsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBp3MQdaCFWukmzxI2aAQAAAADHDmZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0hzRTgAAgEhbtiXaGdSYNCjaGQAAAADHPmZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNIc0U4AgDUt2xLtDGpMGhTtDAAAAAAA0cQMLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFhakxtYX375pW644QYNHDhQiYmJ6t69uy6++GLt2LEjEvkBAAAAAACglXM0dQGPPPKIPv/8c82cOVODBw/WDz/8oGeeeUannnqq1q1bp0GDBkUiTwAAAAAAALRSTW5g3XzzzXr99dcVGxvri82aNUsnn3yyHn74Yb322mtNfQsAQJQt2xLtDGpM4u8iAAAAQKvT5AbWmDFj6sX69OmjgQMHatu2bU1dPAAAAAAAAFq5ZrmJu2maOnDggDp06NAciwcAAAAAAEAr0uQZWIEsWrRI+/bt03333Rf0ORUVFaqoqPD9u7CwUJLkcrnkcrkkSTabTTabTR6PRx6Px/dcb9ztdss0zZBxu90uwzB8y60dlyS32x1W3OFwyDRNv7hhGLLb7fVy9Mar8zD9lmMYNpmmR/4MGYYRkXg1s168bu6BavIurzrHYLm3TE3e7RVse9Rs48bk2Hw1eXMMtu/5vcSw/5i6f03B4oatejv5xw0ZNnt1Lv4LDxw3bDU1mR55D4dgx41p/vh8j9t/3RjVNZke/+OpOWtyuwMfZ8fDOeJYqal6P/Bl36R9r1683j7W8L4XTk2mRy16PDWUu8sVeju15PEUqqZw9r3q9WuNc4TLFfp4itS+F6maQp0jqlNtmeMpVE3ewy3UOaKljqdQNUkNnyPCGYtb8hwReiw2G329FygeiWsjj8cTxvhUZ91E6Br2aGqqvR8EO0eYpidq1+V14y6XK+R1RN3lt+R1ed3cwx2LW3rMDRZ3uUJfG/lf6yiq54hwrve81zpWuI6ofa0TdCyO0pgbqKZwrsv9rnWifB3h3WWPh88adZ/fWBFvYG3fvl2//OUvNXr0aM2ZMyfo8xYsWKD58+fXi2dnZysxMVGS1LFjR/Xq1Us5OTk6dOiQ7znp6elKT0/Xjh075HQ6ffHMzEylpaVpy5YtKisr88X79eundu3aKTs7229FDh48WLGxscrKyvLLYfjw4aqsrNSmTZt8MbvdrhEjRsjpdGr79u2+eEJCgoYMGaK8vDzt3LnTF09JSVH//v1V4XGq3F2TY6wtSW0cqSpzH1Glp9gXj7enKN7eTiWuPLnMmtwT7KmKsyep2PWD3GaVL57oSFOMkaDCqn0yVbPjtY3pIpscclbt8aspJSZDZWVlIWtyVpXIbsSobUxXVXpKVObO9z3fYSQoKSatxWrKyjrc4HaS2ssjl4qq9vsihmxKic2QyyxXietgTa0tUJOkBve9yoKafS+mw2AZ9lhVHvCvKbbTcJnuSlXl1Wwnw7ArtvMImZVOVR2u2fcMR4JiOw6RpyxPLmfNvmeLS1FM+/5yF+fKXby3Zh0kdJSjXS+5nTlylx1SVml1PNjx5LFlyt4mTVX5W2S6amqKad9PRlw7VR3Mlmm2TE07YqqPp9zcXO3dW1PT8XCOOFZqqjwQuX3PF09Kl6NtulwFO+SpqKnJkdLwvhdOTZVFLXs8NVRTVmno7dSSx1OomsLZ9zyHSnzn8qKq3PrncluCnJV7wh6fAp3Lk2MzVOUpC3gur3AX+87lWaWJIY+nSO17kdhO4ZwjKota7ngKVZN3rGjoHNGSx1OomqSGzxGeQyW+eFP3PanmOqLcXRDwOqLUlR/wOqK46qBcZpmySquveYOdI1xmYqOv95rr2ignxx56fKrK9cUjeQ17NDXVHhOCnSPK3EbUrsvr1pSd7Qx5HVF7OS19XV63pnCuI6qKW37MlQKfI7JKQ18bxWz5h19NGQdK5bIb2t8hoSZ301T3A2Uqi7XpYPt4XzzG5VHXvHIVJTh0OKXm3tDxFW51OlKhgqQYOZNifPGkMpdSnZXKT4lVcULNR/KU4iq1K67SDvuIkNd7lUXRuS4PtJ2ySkNfw0ZjzA1WUzjX5ZVFLT/mBqspq/T4+ayRnZ2tpjDM2m20Jvrhhx90+umnq6qqSuvWrVPXrl2DPjfQDKyMjAzl5+crOTlZUvS7g5GYXfHFx9/JKjOwRp/TO2RNG1bsrJVjdGdgjZyYKSn49tiwIidgrdGagTVmcp8G972VW2s/PfozsCYMqA4HO25WbrPG7ApJmjjQmn9BaE0zsJZttsbsCsMwdHa/0DWt3CpLzK6QpAkDQm+nTzZZZwbWxAGh973qsSK6syu88ZETM0MeT59sju5fTmsW79BPBoY+R1SPF9aYgeUdKxo6R3yyOfqzK7y5n3Nyw+c973WON58fi/VfBS14HeG91gl2jtiwIscyM7BOm9Q75Pi0fvn3QWsNJx7JmkZO7FkrFvgcsWHFTsvMwBo5MTPkdcS6Zf9txDpo3ppqr18p+FhslRlYEwaEvjb67xOv+lf64yJNwy8sm1m91CbFzep7+Xiqy/Z7T0NSj19dFvJ6z3utY4UZWLWvdYKOxZusMwOr7rVO0LHYIjOwvGPx8fBZ48iRI0pNTZXT6fT1fRojYjOwnE6npkyZooKCAq1Zs6bB5pUkxcXFKS4urn5CDoccDv+0vCutLu9KCDded7lHEzcMI2A8WI6GYcjvrOSLB779WKTigd8zcO6147WXFzz3lqmpbq51/12dhxqZY/PW1NC+F/AlRpBDMEDcMIwgcZsCLTxUvO6uUDd37+o1bIFrMmzh5x4sHm5N3tSCHWfH8jniWKkp0PY+2n2vXjzoPnb0Nfm9TQscT/XitXKvnW6w7dSSx1OoeDj7nv9Y0fTxKVg8nHN27e0efCyOzL4Xqe0U6hxRO9XmPp5C1VQ31WDniJY6nsKJN3SOCLxfRu86om6u9cdio8HlRPp4aiju3T8bOkcEyjNa54hwxmJvDtG4Lq8br7kWD5574PUbnc8ajRmLrXCOqJ1usNxtQaZ1GAHiRoTiNql+f1PhXe/5jRVRvo6ovUqDjsVRGnMDxcO5/g5rLG6hmmqv3+Pxs0ZjRKSBVV5ermnTpmnHjh1asWKFBgwYEInFAkDYlm2JdgY1Jg2KdgYAAAAAcHxpcgPL7XZr1qxZWrt2rd577z2NHj06EnkBAAAAAAAAkiLQwLrlllu0dOlSTZs2TYcPH9Zrr73m9/jll1/e1LcAgOMOM8YAAAAAIHxNbmB9/fXXkqT3339f77//fr3HaWABAAAAAACgKZrcwFq9enUE0gAAAAAAAAACC/ZTGQAAAAAAAIAl0MACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAIClRaSBVVxcrHvuuUeTJ09W+/btZRiGFi5cGIlFAwAAAAAAoJWLSAMrLy9P9913n7Zt26YhQ4ZEYpEAAAAAAACAJMkRiYV06dJF+/fvV+fOnZWVlaURI0ZEYrEAAAAAAABAZGZgxcXFqXPnzpFYFAAAAAAAAOCHm7gDAAAAAADA0iLyFcKjUVFRoYqKCt+/CwsLJUkul0sul0uSZLPZZLPZ5PF45PF4fM/1xt1ut0zTDBm32+0yDMO33NpxSXK73WHFHQ6HTNP0ixuGIbvdXi9Hb7w6D9NvOYZhk2l65M+</t>
   </si>
 </sst>
 </file>
@@ -478,25 +478,25 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>45687</v>
+        <v>45707.83333333334</v>
       </c>
       <c r="E2">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>37.64114853713622</v>
+        <v>46.35577462242414</v>
       </c>
       <c r="G2" s="2">
-        <v>45687</v>
+        <v>45707.83333333334</v>
       </c>
       <c r="H2">
-        <v>22.07845885499383</v>
+        <v>29.68336716628981</v>
       </c>
       <c r="I2">
-        <v>5.412539116244487</v>
+        <v>12.9926758235007</v>
       </c>
       <c r="J2">
-        <v>37.64114853713622</v>
+        <v>46.35577462242414</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
@@ -513,25 +513,25 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>45687</v>
+        <v>45707.83333333334</v>
       </c>
       <c r="E3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3">
-        <v>32.66228956634455</v>
+        <v>39.68514855679198</v>
       </c>
       <c r="G3" s="2">
-        <v>45687</v>
+        <v>45707.83333333334</v>
       </c>
       <c r="H3">
-        <v>17.51022447277154</v>
+        <v>23.75127184224192</v>
       </c>
       <c r="I3">
-        <v>2.338072152989103</v>
+        <v>9.450090826054085</v>
       </c>
       <c r="J3">
-        <v>32.66228956634455</v>
+        <v>39.68514855679198</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
@@ -545,28 +545,28 @@
         <v>13</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>45687</v>
+        <v>45707.83333333334</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>9.16309809196412</v>
+        <v>10.42752596367906</v>
       </c>
       <c r="G4" s="2">
-        <v>45687</v>
+        <v>45707.83333333334</v>
       </c>
       <c r="H4">
-        <v>4.348516376332625</v>
+        <v>5.81888767865089</v>
       </c>
       <c r="I4">
-        <v>-0.6612457159234781</v>
+        <v>0.9822851101156052</v>
       </c>
       <c r="J4">
-        <v>9.16309809196412</v>
+        <v>10.42752596367906</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>

</xml_diff>